<commit_message>
[Fonds de solidarite] Add classe effectif to published data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -22,12 +22,12 @@
     <t>volet</t>
   </si>
   <si>
-    <t>sum</t>
-  </si>
-  <si>
     <t>nombre_aides</t>
   </si>
   <si>
+    <t>montant_total</t>
+  </si>
+  <si>
     <t>reg</t>
   </si>
   <si>
@@ -40,7 +40,7 @@
     <t>libelle_categorie_juridique</t>
   </si>
   <si>
-    <t>Fonds de solidarit??</t>
+    <t>Fonds de solidarité</t>
   </si>
   <si>
     <t>VOLET1</t>
@@ -657,10 +657,10 @@
         <v>9</v>
       </c>
       <c r="C2">
+        <v>178404</v>
+      </c>
+      <c r="D2">
         <v>230501752</v>
-      </c>
-      <c r="D2">
-        <v>178404</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -683,10 +683,10 @@
         <v>9</v>
       </c>
       <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="D3">
         <v>160901</v>
-      </c>
-      <c r="D3">
-        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -709,10 +709,10 @@
         <v>9</v>
       </c>
       <c r="C4">
+        <v>172</v>
+      </c>
+      <c r="D4">
         <v>249378</v>
-      </c>
-      <c r="D4">
-        <v>172</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -735,10 +735,10 @@
         <v>9</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>6000</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -761,10 +761,10 @@
         <v>9</v>
       </c>
       <c r="C6">
+        <v>461</v>
+      </c>
+      <c r="D6">
         <v>685592</v>
-      </c>
-      <c r="D6">
-        <v>461</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -787,10 +787,10 @@
         <v>9</v>
       </c>
       <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>14820</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -813,10 +813,10 @@
         <v>9</v>
       </c>
       <c r="C8">
+        <v>73157</v>
+      </c>
+      <c r="D8">
         <v>108028359</v>
-      </c>
-      <c r="D8">
-        <v>73157</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -839,10 +839,10 @@
         <v>9</v>
       </c>
       <c r="C9">
+        <v>85</v>
+      </c>
+      <c r="D9">
         <v>127290</v>
-      </c>
-      <c r="D9">
-        <v>85</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -865,10 +865,10 @@
         <v>9</v>
       </c>
       <c r="C10">
+        <v>34456</v>
+      </c>
+      <c r="D10">
         <v>50085144</v>
-      </c>
-      <c r="D10">
-        <v>34456</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -891,10 +891,10 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11">
         <v>36210</v>
-      </c>
-      <c r="D11">
-        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -917,10 +917,10 @@
         <v>9</v>
       </c>
       <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
         <v>4500</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -943,10 +943,10 @@
         <v>9</v>
       </c>
       <c r="C13">
+        <v>1942</v>
+      </c>
+      <c r="D13">
         <v>2766423</v>
-      </c>
-      <c r="D13">
-        <v>1942</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -969,10 +969,10 @@
         <v>9</v>
       </c>
       <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
         <v>6000</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -995,10 +995,10 @@
         <v>9</v>
       </c>
       <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
         <v>33100</v>
-      </c>
-      <c r="D15">
-        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1021,10 +1021,10 @@
         <v>9</v>
       </c>
       <c r="C16">
+        <v>2104</v>
+      </c>
+      <c r="D16">
         <v>2969784</v>
-      </c>
-      <c r="D16">
-        <v>2104</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1047,10 +1047,10 @@
         <v>9</v>
       </c>
       <c r="C17">
+        <v>45335</v>
+      </c>
+      <c r="D17">
         <v>57796564</v>
-      </c>
-      <c r="D17">
-        <v>45335</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1073,10 +1073,10 @@
         <v>9</v>
       </c>
       <c r="C18">
+        <v>31</v>
+      </c>
+      <c r="D18">
         <v>42140</v>
-      </c>
-      <c r="D18">
-        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1099,10 +1099,10 @@
         <v>9</v>
       </c>
       <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
         <v>30000</v>
-      </c>
-      <c r="D19">
-        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1125,10 +1125,10 @@
         <v>9</v>
       </c>
       <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
         <v>4500</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1151,10 +1151,10 @@
         <v>9</v>
       </c>
       <c r="C21">
+        <v>157</v>
+      </c>
+      <c r="D21">
         <v>229241</v>
-      </c>
-      <c r="D21">
-        <v>157</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1177,10 +1177,10 @@
         <v>9</v>
       </c>
       <c r="C22">
+        <v>20658</v>
+      </c>
+      <c r="D22">
         <v>30468460</v>
-      </c>
-      <c r="D22">
-        <v>20658</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1203,10 +1203,10 @@
         <v>9</v>
       </c>
       <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23">
         <v>24654</v>
-      </c>
-      <c r="D23">
-        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1229,10 +1229,10 @@
         <v>9</v>
       </c>
       <c r="C24">
+        <v>6842</v>
+      </c>
+      <c r="D24">
         <v>9935763</v>
-      </c>
-      <c r="D24">
-        <v>6842</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1255,10 +1255,10 @@
         <v>9</v>
       </c>
       <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
         <v>12000</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1281,10 +1281,10 @@
         <v>9</v>
       </c>
       <c r="C26">
+        <v>797</v>
+      </c>
+      <c r="D26">
         <v>1123007</v>
-      </c>
-      <c r="D26">
-        <v>797</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1307,10 +1307,10 @@
         <v>9</v>
       </c>
       <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
         <v>7500</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1333,10 +1333,10 @@
         <v>9</v>
       </c>
       <c r="C28">
+        <v>657</v>
+      </c>
+      <c r="D28">
         <v>933668</v>
-      </c>
-      <c r="D28">
-        <v>657</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1359,10 +1359,10 @@
         <v>9</v>
       </c>
       <c r="C29">
+        <v>57904</v>
+      </c>
+      <c r="D29">
         <v>74489084</v>
-      </c>
-      <c r="D29">
-        <v>57904</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1385,10 +1385,10 @@
         <v>9</v>
       </c>
       <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30">
         <v>33638</v>
-      </c>
-      <c r="D30">
-        <v>29</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -1411,10 +1411,10 @@
         <v>9</v>
       </c>
       <c r="C31">
+        <v>51</v>
+      </c>
+      <c r="D31">
         <v>73044</v>
-      </c>
-      <c r="D31">
-        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1437,10 +1437,10 @@
         <v>9</v>
       </c>
       <c r="C32">
+        <v>458</v>
+      </c>
+      <c r="D32">
         <v>680235</v>
-      </c>
-      <c r="D32">
-        <v>458</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1463,10 +1463,10 @@
         <v>9</v>
       </c>
       <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
         <v>4500</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -1489,10 +1489,10 @@
         <v>9</v>
       </c>
       <c r="C34">
+        <v>28565</v>
+      </c>
+      <c r="D34">
         <v>42188920</v>
-      </c>
-      <c r="D34">
-        <v>28565</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1515,10 +1515,10 @@
         <v>9</v>
       </c>
       <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35">
         <v>17950</v>
-      </c>
-      <c r="D35">
-        <v>12</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -1541,10 +1541,10 @@
         <v>9</v>
       </c>
       <c r="C36">
+        <v>5488</v>
+      </c>
+      <c r="D36">
         <v>7916150</v>
-      </c>
-      <c r="D36">
-        <v>5488</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1567,10 +1567,10 @@
         <v>9</v>
       </c>
       <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
         <v>6000</v>
-      </c>
-      <c r="D37">
-        <v>4</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1593,10 +1593,10 @@
         <v>9</v>
       </c>
       <c r="C38">
+        <v>702</v>
+      </c>
+      <c r="D38">
         <v>984892</v>
-      </c>
-      <c r="D38">
-        <v>702</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1619,10 +1619,10 @@
         <v>9</v>
       </c>
       <c r="C39">
+        <v>682</v>
+      </c>
+      <c r="D39">
         <v>963029</v>
-      </c>
-      <c r="D39">
-        <v>682</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1645,10 +1645,10 @@
         <v>9</v>
       </c>
       <c r="C40">
+        <v>39994</v>
+      </c>
+      <c r="D40">
         <v>50905481</v>
-      </c>
-      <c r="D40">
-        <v>39994</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1671,10 +1671,10 @@
         <v>9</v>
       </c>
       <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41">
         <v>13095</v>
-      </c>
-      <c r="D41">
-        <v>14</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -1697,10 +1697,10 @@
         <v>9</v>
       </c>
       <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42">
         <v>33472</v>
-      </c>
-      <c r="D42">
-        <v>25</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -1723,10 +1723,10 @@
         <v>9</v>
       </c>
       <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
         <v>4500</v>
-      </c>
-      <c r="D43">
-        <v>3</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -1749,10 +1749,10 @@
         <v>9</v>
       </c>
       <c r="C44">
+        <v>190</v>
+      </c>
+      <c r="D44">
         <v>281581</v>
-      </c>
-      <c r="D44">
-        <v>190</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1775,10 +1775,10 @@
         <v>9</v>
       </c>
       <c r="C45">
+        <v>17789</v>
+      </c>
+      <c r="D45">
         <v>26249060</v>
-      </c>
-      <c r="D45">
-        <v>17789</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1801,10 +1801,10 @@
         <v>9</v>
       </c>
       <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
         <v>15000</v>
-      </c>
-      <c r="D46">
-        <v>10</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -1827,10 +1827,10 @@
         <v>9</v>
       </c>
       <c r="C47">
+        <v>6532</v>
+      </c>
+      <c r="D47">
         <v>9491231</v>
-      </c>
-      <c r="D47">
-        <v>6532</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1853,10 +1853,10 @@
         <v>9</v>
       </c>
       <c r="C48">
+        <v>726</v>
+      </c>
+      <c r="D48">
         <v>1020035</v>
-      </c>
-      <c r="D48">
-        <v>726</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1879,10 +1879,10 @@
         <v>9</v>
       </c>
       <c r="C49">
+        <v>415</v>
+      </c>
+      <c r="D49">
         <v>588085</v>
-      </c>
-      <c r="D49">
-        <v>415</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -1905,10 +1905,10 @@
         <v>9</v>
       </c>
       <c r="C50">
+        <v>11024</v>
+      </c>
+      <c r="D50">
         <v>14460780</v>
-      </c>
-      <c r="D50">
-        <v>11024</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -1931,10 +1931,10 @@
         <v>9</v>
       </c>
       <c r="C51">
+        <v>14</v>
+      </c>
+      <c r="D51">
         <v>17827</v>
-      </c>
-      <c r="D51">
-        <v>14</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -1957,10 +1957,10 @@
         <v>9</v>
       </c>
       <c r="C52">
+        <v>12</v>
+      </c>
+      <c r="D52">
         <v>16725</v>
-      </c>
-      <c r="D52">
-        <v>12</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
@@ -1983,10 +1983,10 @@
         <v>9</v>
       </c>
       <c r="C53">
+        <v>27</v>
+      </c>
+      <c r="D53">
         <v>39202</v>
-      </c>
-      <c r="D53">
-        <v>27</v>
       </c>
       <c r="E53" t="s">
         <v>14</v>
@@ -2009,10 +2009,10 @@
         <v>9</v>
       </c>
       <c r="C54">
+        <v>4088</v>
+      </c>
+      <c r="D54">
         <v>6008751</v>
-      </c>
-      <c r="D54">
-        <v>4088</v>
       </c>
       <c r="E54" t="s">
         <v>14</v>
@@ -2035,10 +2035,10 @@
         <v>9</v>
       </c>
       <c r="C55">
+        <v>2763</v>
+      </c>
+      <c r="D55">
         <v>4030173</v>
-      </c>
-      <c r="D55">
-        <v>2763</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2061,10 +2061,10 @@
         <v>9</v>
       </c>
       <c r="C56">
+        <v>226</v>
+      </c>
+      <c r="D56">
         <v>314357</v>
-      </c>
-      <c r="D56">
-        <v>226</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2087,10 +2087,10 @@
         <v>9</v>
       </c>
       <c r="C57">
+        <v>91</v>
+      </c>
+      <c r="D57">
         <v>127184</v>
-      </c>
-      <c r="D57">
-        <v>91</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2113,10 +2113,10 @@
         <v>9</v>
       </c>
       <c r="C58">
+        <v>81173</v>
+      </c>
+      <c r="D58">
         <v>102788081</v>
-      </c>
-      <c r="D58">
-        <v>81173</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2139,10 +2139,10 @@
         <v>9</v>
       </c>
       <c r="C59">
+        <v>23</v>
+      </c>
+      <c r="D59">
         <v>26464</v>
-      </c>
-      <c r="D59">
-        <v>23</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2165,10 +2165,10 @@
         <v>9</v>
       </c>
       <c r="C60">
+        <v>49</v>
+      </c>
+      <c r="D60">
         <v>69932</v>
-      </c>
-      <c r="D60">
-        <v>49</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2191,10 +2191,10 @@
         <v>9</v>
       </c>
       <c r="C61">
+        <v>9</v>
+      </c>
+      <c r="D61">
         <v>13500</v>
-      </c>
-      <c r="D61">
-        <v>9</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2217,10 +2217,10 @@
         <v>9</v>
       </c>
       <c r="C62">
+        <v>220</v>
+      </c>
+      <c r="D62">
         <v>323293</v>
-      </c>
-      <c r="D62">
-        <v>220</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2243,10 +2243,10 @@
         <v>9</v>
       </c>
       <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63">
         <v>8947</v>
-      </c>
-      <c r="D63">
-        <v>7</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2269,10 +2269,10 @@
         <v>9</v>
       </c>
       <c r="C64">
+        <v>40051</v>
+      </c>
+      <c r="D64">
         <v>59182969</v>
-      </c>
-      <c r="D64">
-        <v>40051</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
@@ -2295,10 +2295,10 @@
         <v>9</v>
       </c>
       <c r="C65">
+        <v>46</v>
+      </c>
+      <c r="D65">
         <v>68174</v>
-      </c>
-      <c r="D65">
-        <v>46</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2321,10 +2321,10 @@
         <v>9</v>
       </c>
       <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
         <v>6000</v>
-      </c>
-      <c r="D66">
-        <v>4</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2347,10 +2347,10 @@
         <v>9</v>
       </c>
       <c r="C67">
+        <v>17761</v>
+      </c>
+      <c r="D67">
         <v>25858690</v>
-      </c>
-      <c r="D67">
-        <v>17761</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2373,10 +2373,10 @@
         <v>9</v>
       </c>
       <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68">
         <v>7570</v>
-      </c>
-      <c r="D68">
-        <v>6</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2399,10 +2399,10 @@
         <v>9</v>
       </c>
       <c r="C69">
+        <v>1256</v>
+      </c>
+      <c r="D69">
         <v>1811135</v>
-      </c>
-      <c r="D69">
-        <v>1256</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2425,10 +2425,10 @@
         <v>9</v>
       </c>
       <c r="C70">
+        <v>941</v>
+      </c>
+      <c r="D70">
         <v>1333604</v>
-      </c>
-      <c r="D70">
-        <v>941</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2451,10 +2451,10 @@
         <v>9</v>
       </c>
       <c r="C71">
+        <v>12648</v>
+      </c>
+      <c r="D71">
         <v>17143001</v>
-      </c>
-      <c r="D71">
-        <v>12648</v>
       </c>
       <c r="E71" t="s">
         <v>16</v>
@@ -2477,10 +2477,10 @@
         <v>9</v>
       </c>
       <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
         <v>6000</v>
-      </c>
-      <c r="D72">
-        <v>4</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2503,10 +2503,10 @@
         <v>9</v>
       </c>
       <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73">
         <v>9000</v>
-      </c>
-      <c r="D73">
-        <v>6</v>
       </c>
       <c r="E73" t="s">
         <v>16</v>
@@ -2529,10 +2529,10 @@
         <v>9</v>
       </c>
       <c r="C74">
+        <v>14</v>
+      </c>
+      <c r="D74">
         <v>20256</v>
-      </c>
-      <c r="D74">
-        <v>14</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2555,10 +2555,10 @@
         <v>9</v>
       </c>
       <c r="C75">
+        <v>4052</v>
+      </c>
+      <c r="D75">
         <v>5977759</v>
-      </c>
-      <c r="D75">
-        <v>4052</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2581,10 +2581,10 @@
         <v>9</v>
       </c>
       <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
         <v>4500</v>
-      </c>
-      <c r="D76">
-        <v>3</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2607,10 +2607,10 @@
         <v>9</v>
       </c>
       <c r="C77">
+        <v>3179</v>
+      </c>
+      <c r="D77">
         <v>4592705</v>
-      </c>
-      <c r="D77">
-        <v>3179</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -2633,10 +2633,10 @@
         <v>9</v>
       </c>
       <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
         <v>4500</v>
-      </c>
-      <c r="D78">
-        <v>3</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2659,10 +2659,10 @@
         <v>9</v>
       </c>
       <c r="C79">
+        <v>176</v>
+      </c>
+      <c r="D79">
         <v>252311</v>
-      </c>
-      <c r="D79">
-        <v>176</v>
       </c>
       <c r="E79" t="s">
         <v>16</v>
@@ -2685,10 +2685,10 @@
         <v>9</v>
       </c>
       <c r="C80">
+        <v>138</v>
+      </c>
+      <c r="D80">
         <v>199962</v>
-      </c>
-      <c r="D80">
-        <v>138</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2711,10 +2711,10 @@
         <v>9</v>
       </c>
       <c r="C81">
+        <v>2637</v>
+      </c>
+      <c r="D81">
         <v>3632992</v>
-      </c>
-      <c r="D81">
-        <v>2637</v>
       </c>
       <c r="E81" t="s">
         <v>17</v>
@@ -2737,10 +2737,10 @@
         <v>9</v>
       </c>
       <c r="C82">
+        <v>796</v>
+      </c>
+      <c r="D82">
         <v>1170854</v>
-      </c>
-      <c r="D82">
-        <v>796</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2763,10 +2763,10 @@
         <v>9</v>
       </c>
       <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
         <v>4500</v>
-      </c>
-      <c r="D83">
-        <v>3</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2789,10 +2789,10 @@
         <v>9</v>
       </c>
       <c r="C84">
+        <v>954</v>
+      </c>
+      <c r="D84">
         <v>1388291</v>
-      </c>
-      <c r="D84">
-        <v>954</v>
       </c>
       <c r="E84" t="s">
         <v>17</v>
@@ -2815,10 +2815,10 @@
         <v>9</v>
       </c>
       <c r="C85">
+        <v>24</v>
+      </c>
+      <c r="D85">
         <v>35318</v>
-      </c>
-      <c r="D85">
-        <v>24</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2841,10 +2841,10 @@
         <v>9</v>
       </c>
       <c r="C86">
+        <v>32</v>
+      </c>
+      <c r="D86">
         <v>45950</v>
-      </c>
-      <c r="D86">
-        <v>32</v>
       </c>
       <c r="E86" t="s">
         <v>17</v>
@@ -2867,10 +2867,10 @@
         <v>9</v>
       </c>
       <c r="C87">
+        <v>83351</v>
+      </c>
+      <c r="D87">
         <v>104215155</v>
-      </c>
-      <c r="D87">
-        <v>83351</v>
       </c>
       <c r="E87" t="s">
         <v>18</v>
@@ -2893,10 +2893,10 @@
         <v>9</v>
       </c>
       <c r="C88">
+        <v>21</v>
+      </c>
+      <c r="D88">
         <v>25249</v>
-      </c>
-      <c r="D88">
-        <v>21</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -2919,10 +2919,10 @@
         <v>9</v>
       </c>
       <c r="C89">
+        <v>39</v>
+      </c>
+      <c r="D89">
         <v>57561</v>
-      </c>
-      <c r="D89">
-        <v>39</v>
       </c>
       <c r="E89" t="s">
         <v>18</v>
@@ -2945,10 +2945,10 @@
         <v>9</v>
       </c>
       <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90">
         <v>5895</v>
-      </c>
-      <c r="D90">
-        <v>4</v>
       </c>
       <c r="E90" t="s">
         <v>18</v>
@@ -2971,10 +2971,10 @@
         <v>9</v>
       </c>
       <c r="C91">
+        <v>490</v>
+      </c>
+      <c r="D91">
         <v>726323</v>
-      </c>
-      <c r="D91">
-        <v>490</v>
       </c>
       <c r="E91" t="s">
         <v>18</v>
@@ -2997,10 +2997,10 @@
         <v>9</v>
       </c>
       <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92">
         <v>5600</v>
-      </c>
-      <c r="D92">
-        <v>4</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3023,10 +3023,10 @@
         <v>9</v>
       </c>
       <c r="C93">
+        <v>34108</v>
+      </c>
+      <c r="D93">
         <v>50303448</v>
-      </c>
-      <c r="D93">
-        <v>34108</v>
       </c>
       <c r="E93" t="s">
         <v>18</v>
@@ -3049,10 +3049,10 @@
         <v>9</v>
       </c>
       <c r="C94">
+        <v>51</v>
+      </c>
+      <c r="D94">
         <v>76500</v>
-      </c>
-      <c r="D94">
-        <v>51</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3075,10 +3075,10 @@
         <v>9</v>
       </c>
       <c r="C95">
+        <v>16056</v>
+      </c>
+      <c r="D95">
         <v>23364937</v>
-      </c>
-      <c r="D95">
-        <v>16056</v>
       </c>
       <c r="E95" t="s">
         <v>18</v>
@@ -3101,10 +3101,10 @@
         <v>9</v>
       </c>
       <c r="C96">
+        <v>620</v>
+      </c>
+      <c r="D96">
         <v>850913</v>
-      </c>
-      <c r="D96">
-        <v>620</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3127,10 +3127,10 @@
         <v>9</v>
       </c>
       <c r="C97">
+        <v>732</v>
+      </c>
+      <c r="D97">
         <v>1032815</v>
-      </c>
-      <c r="D97">
-        <v>732</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3153,10 +3153,10 @@
         <v>9</v>
       </c>
       <c r="C98">
+        <v>7</v>
+      </c>
+      <c r="D98">
         <v>10500</v>
-      </c>
-      <c r="D98">
-        <v>7</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3179,10 +3179,10 @@
         <v>9</v>
       </c>
       <c r="C99">
+        <v>23648</v>
+      </c>
+      <c r="D99">
         <v>31942778</v>
-      </c>
-      <c r="D99">
-        <v>23648</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
@@ -3205,10 +3205,10 @@
         <v>9</v>
       </c>
       <c r="C100">
+        <v>11</v>
+      </c>
+      <c r="D100">
         <v>14653</v>
-      </c>
-      <c r="D100">
-        <v>11</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3231,10 +3231,10 @@
         <v>9</v>
       </c>
       <c r="C101">
+        <v>13</v>
+      </c>
+      <c r="D101">
         <v>18423</v>
-      </c>
-      <c r="D101">
-        <v>13</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -3257,10 +3257,10 @@
         <v>9</v>
       </c>
       <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102">
         <v>4500</v>
-      </c>
-      <c r="D102">
-        <v>3</v>
       </c>
       <c r="E102" t="s">
         <v>19</v>
@@ -3283,10 +3283,10 @@
         <v>9</v>
       </c>
       <c r="C103">
+        <v>315</v>
+      </c>
+      <c r="D103">
         <v>472500</v>
-      </c>
-      <c r="D103">
-        <v>315</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
@@ -3309,10 +3309,10 @@
         <v>9</v>
       </c>
       <c r="C104">
+        <v>8698</v>
+      </c>
+      <c r="D104">
         <v>12827778</v>
-      </c>
-      <c r="D104">
-        <v>8698</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -3335,10 +3335,10 @@
         <v>9</v>
       </c>
       <c r="C105">
+        <v>2217</v>
+      </c>
+      <c r="D105">
         <v>3213092</v>
-      </c>
-      <c r="D105">
-        <v>2217</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3361,10 +3361,10 @@
         <v>9</v>
       </c>
       <c r="C106">
+        <v>6</v>
+      </c>
+      <c r="D106">
         <v>9000</v>
-      </c>
-      <c r="D106">
-        <v>6</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3387,10 +3387,10 @@
         <v>9</v>
       </c>
       <c r="C107">
+        <v>192</v>
+      </c>
+      <c r="D107">
         <v>277230</v>
-      </c>
-      <c r="D107">
-        <v>192</v>
       </c>
       <c r="E107" t="s">
         <v>19</v>
@@ -3413,10 +3413,10 @@
         <v>9</v>
       </c>
       <c r="C108">
+        <v>130</v>
+      </c>
+      <c r="D108">
         <v>179066</v>
-      </c>
-      <c r="D108">
-        <v>130</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -3439,10 +3439,10 @@
         <v>9</v>
       </c>
       <c r="C109">
+        <v>8563</v>
+      </c>
+      <c r="D109">
         <v>11423258</v>
-      </c>
-      <c r="D109">
-        <v>8563</v>
       </c>
       <c r="E109" t="s">
         <v>20</v>
@@ -3465,10 +3465,10 @@
         <v>9</v>
       </c>
       <c r="C110">
+        <v>35</v>
+      </c>
+      <c r="D110">
         <v>50906</v>
-      </c>
-      <c r="D110">
-        <v>35</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3491,10 +3491,10 @@
         <v>9</v>
       </c>
       <c r="C111">
+        <v>3958</v>
+      </c>
+      <c r="D111">
         <v>5794672</v>
-      </c>
-      <c r="D111">
-        <v>3958</v>
       </c>
       <c r="E111" t="s">
         <v>20</v>
@@ -3517,10 +3517,10 @@
         <v>9</v>
       </c>
       <c r="C112">
+        <v>2445</v>
+      </c>
+      <c r="D112">
         <v>3536367</v>
-      </c>
-      <c r="D112">
-        <v>2445</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3543,10 +3543,10 @@
         <v>9</v>
       </c>
       <c r="C113">
+        <v>121</v>
+      </c>
+      <c r="D113">
         <v>169262</v>
-      </c>
-      <c r="D113">
-        <v>121</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3569,10 +3569,10 @@
         <v>9</v>
       </c>
       <c r="C114">
+        <v>62</v>
+      </c>
+      <c r="D114">
         <v>88518</v>
-      </c>
-      <c r="D114">
-        <v>62</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3595,10 +3595,10 @@
         <v>9</v>
       </c>
       <c r="C115">
+        <v>2393</v>
+      </c>
+      <c r="D115">
         <v>3383012</v>
-      </c>
-      <c r="D115">
-        <v>2393</v>
       </c>
       <c r="E115" t="s">
         <v>21</v>
@@ -3621,10 +3621,10 @@
         <v>9</v>
       </c>
       <c r="C116">
+        <v>690</v>
+      </c>
+      <c r="D116">
         <v>1021993</v>
-      </c>
-      <c r="D116">
-        <v>690</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3647,10 +3647,10 @@
         <v>9</v>
       </c>
       <c r="C117">
+        <v>90</v>
+      </c>
+      <c r="D117">
         <v>132600</v>
-      </c>
-      <c r="D117">
-        <v>90</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3673,10 +3673,10 @@
         <v>9</v>
       </c>
       <c r="C118">
+        <v>12</v>
+      </c>
+      <c r="D118">
         <v>18000</v>
-      </c>
-      <c r="D118">
-        <v>12</v>
       </c>
       <c r="E118" t="s">
         <v>21</v>
@@ -3699,10 +3699,10 @@
         <v>9</v>
       </c>
       <c r="C119">
+        <v>11</v>
+      </c>
+      <c r="D119">
         <v>16500</v>
-      </c>
-      <c r="D119">
-        <v>11</v>
       </c>
       <c r="E119" t="s">
         <v>21</v>
@@ -3725,10 +3725,10 @@
         <v>9</v>
       </c>
       <c r="C120">
+        <v>52350</v>
+      </c>
+      <c r="D120">
         <v>66568785</v>
-      </c>
-      <c r="D120">
-        <v>52350</v>
       </c>
       <c r="E120" t="s">
         <v>22</v>
@@ -3751,10 +3751,10 @@
         <v>9</v>
       </c>
       <c r="C121">
+        <v>15</v>
+      </c>
+      <c r="D121">
         <v>20095</v>
-      </c>
-      <c r="D121">
-        <v>15</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3777,10 +3777,10 @@
         <v>9</v>
       </c>
       <c r="C122">
+        <v>55</v>
+      </c>
+      <c r="D122">
         <v>80699</v>
-      </c>
-      <c r="D122">
-        <v>55</v>
       </c>
       <c r="E122" t="s">
         <v>22</v>
@@ -3803,10 +3803,10 @@
         <v>9</v>
       </c>
       <c r="C123">
+        <v>4</v>
+      </c>
+      <c r="D123">
         <v>5830</v>
-      </c>
-      <c r="D123">
-        <v>4</v>
       </c>
       <c r="E123" t="s">
         <v>22</v>
@@ -3829,10 +3829,10 @@
         <v>9</v>
       </c>
       <c r="C124">
+        <v>334</v>
+      </c>
+      <c r="D124">
         <v>491762</v>
-      </c>
-      <c r="D124">
-        <v>334</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
@@ -3855,10 +3855,10 @@
         <v>9</v>
       </c>
       <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125">
         <v>4500</v>
-      </c>
-      <c r="D125">
-        <v>3</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3881,10 +3881,10 @@
         <v>9</v>
       </c>
       <c r="C126">
+        <v>21994</v>
+      </c>
+      <c r="D126">
         <v>32447763</v>
-      </c>
-      <c r="D126">
-        <v>21994</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
@@ -3907,10 +3907,10 @@
         <v>9</v>
       </c>
       <c r="C127">
+        <v>14</v>
+      </c>
+      <c r="D127">
         <v>21000</v>
-      </c>
-      <c r="D127">
-        <v>14</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3933,10 +3933,10 @@
         <v>9</v>
       </c>
       <c r="C128">
+        <v>7732</v>
+      </c>
+      <c r="D128">
         <v>11238814</v>
-      </c>
-      <c r="D128">
-        <v>7732</v>
       </c>
       <c r="E128" t="s">
         <v>22</v>
@@ -3959,10 +3959,10 @@
         <v>9</v>
       </c>
       <c r="C129">
+        <v>5</v>
+      </c>
+      <c r="D129">
         <v>6419</v>
-      </c>
-      <c r="D129">
-        <v>5</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -3985,10 +3985,10 @@
         <v>9</v>
       </c>
       <c r="C130">
+        <v>646</v>
+      </c>
+      <c r="D130">
         <v>908322</v>
-      </c>
-      <c r="D130">
-        <v>646</v>
       </c>
       <c r="E130" t="s">
         <v>22</v>
@@ -4011,10 +4011,10 @@
         <v>9</v>
       </c>
       <c r="C131">
+        <v>609</v>
+      </c>
+      <c r="D131">
         <v>869447</v>
-      </c>
-      <c r="D131">
-        <v>609</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4037,10 +4037,10 @@
         <v>9</v>
       </c>
       <c r="C132">
+        <v>138747</v>
+      </c>
+      <c r="D132">
         <v>175088042</v>
-      </c>
-      <c r="D132">
-        <v>138747</v>
       </c>
       <c r="E132" t="s">
         <v>23</v>
@@ -4063,10 +4063,10 @@
         <v>9</v>
       </c>
       <c r="C133">
+        <v>59</v>
+      </c>
+      <c r="D133">
         <v>64536</v>
-      </c>
-      <c r="D133">
-        <v>59</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4089,10 +4089,10 @@
         <v>9</v>
       </c>
       <c r="C134">
+        <v>98</v>
+      </c>
+      <c r="D134">
         <v>141375</v>
-      </c>
-      <c r="D134">
-        <v>98</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4115,10 +4115,10 @@
         <v>9</v>
       </c>
       <c r="C135">
+        <v>6</v>
+      </c>
+      <c r="D135">
         <v>8230</v>
-      </c>
-      <c r="D135">
-        <v>6</v>
       </c>
       <c r="E135" t="s">
         <v>23</v>
@@ -4141,10 +4141,10 @@
         <v>9</v>
       </c>
       <c r="C136">
+        <v>491</v>
+      </c>
+      <c r="D136">
         <v>722809</v>
-      </c>
-      <c r="D136">
-        <v>491</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
@@ -4167,10 +4167,10 @@
         <v>9</v>
       </c>
       <c r="C137">
+        <v>3</v>
+      </c>
+      <c r="D137">
         <v>4500</v>
-      </c>
-      <c r="D137">
-        <v>3</v>
       </c>
       <c r="E137" t="s">
         <v>23</v>
@@ -4193,10 +4193,10 @@
         <v>9</v>
       </c>
       <c r="C138">
+        <v>55809</v>
+      </c>
+      <c r="D138">
         <v>82223809</v>
-      </c>
-      <c r="D138">
-        <v>55809</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4219,10 +4219,10 @@
         <v>9</v>
       </c>
       <c r="C139">
+        <v>60</v>
+      </c>
+      <c r="D139">
         <v>87295</v>
-      </c>
-      <c r="D139">
-        <v>60</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -4245,10 +4245,10 @@
         <v>9</v>
       </c>
       <c r="C140">
+        <v>19846</v>
+      </c>
+      <c r="D140">
         <v>28723269</v>
-      </c>
-      <c r="D140">
-        <v>19846</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4271,10 +4271,10 @@
         <v>9</v>
       </c>
       <c r="C141">
+        <v>17</v>
+      </c>
+      <c r="D141">
         <v>25500</v>
-      </c>
-      <c r="D141">
-        <v>17</v>
       </c>
       <c r="E141" t="s">
         <v>23</v>
@@ -4297,10 +4297,10 @@
         <v>9</v>
       </c>
       <c r="C142">
+        <v>6</v>
+      </c>
+      <c r="D142">
         <v>9000</v>
-      </c>
-      <c r="D142">
-        <v>6</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
@@ -4323,10 +4323,10 @@
         <v>9</v>
       </c>
       <c r="C143">
+        <v>2623</v>
+      </c>
+      <c r="D143">
         <v>3751218</v>
-      </c>
-      <c r="D143">
-        <v>2623</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4349,10 +4349,10 @@
         <v>9</v>
       </c>
       <c r="C144">
+        <v>6</v>
+      </c>
+      <c r="D144">
         <v>9000</v>
-      </c>
-      <c r="D144">
-        <v>6</v>
       </c>
       <c r="E144" t="s">
         <v>23</v>
@@ -4375,10 +4375,10 @@
         <v>9</v>
       </c>
       <c r="C145">
+        <v>1702</v>
+      </c>
+      <c r="D145">
         <v>2362376</v>
-      </c>
-      <c r="D145">
-        <v>1702</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -4401,10 +4401,10 @@
         <v>9</v>
       </c>
       <c r="C146">
+        <v>149100</v>
+      </c>
+      <c r="D146">
         <v>186484314</v>
-      </c>
-      <c r="D146">
-        <v>149100</v>
       </c>
       <c r="E146" t="s">
         <v>24</v>
@@ -4427,10 +4427,10 @@
         <v>9</v>
       </c>
       <c r="C147">
+        <v>77</v>
+      </c>
+      <c r="D147">
         <v>77934</v>
-      </c>
-      <c r="D147">
-        <v>77</v>
       </c>
       <c r="E147" t="s">
         <v>24</v>
@@ -4453,10 +4453,10 @@
         <v>9</v>
       </c>
       <c r="C148">
+        <v>137</v>
+      </c>
+      <c r="D148">
         <v>197049</v>
-      </c>
-      <c r="D148">
-        <v>137</v>
       </c>
       <c r="E148" t="s">
         <v>24</v>
@@ -4479,10 +4479,10 @@
         <v>9</v>
       </c>
       <c r="C149">
+        <v>9</v>
+      </c>
+      <c r="D149">
         <v>12825</v>
-      </c>
-      <c r="D149">
-        <v>9</v>
       </c>
       <c r="E149" t="s">
         <v>24</v>
@@ -4505,10 +4505,10 @@
         <v>9</v>
       </c>
       <c r="C150">
+        <v>5</v>
+      </c>
+      <c r="D150">
         <v>6378</v>
-      </c>
-      <c r="D150">
-        <v>5</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -4531,10 +4531,10 @@
         <v>9</v>
       </c>
       <c r="C151">
+        <v>337</v>
+      </c>
+      <c r="D151">
         <v>497546</v>
-      </c>
-      <c r="D151">
-        <v>337</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4557,10 +4557,10 @@
         <v>9</v>
       </c>
       <c r="C152">
+        <v>59244</v>
+      </c>
+      <c r="D152">
         <v>87189802</v>
-      </c>
-      <c r="D152">
-        <v>59244</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -4583,10 +4583,10 @@
         <v>9</v>
       </c>
       <c r="C153">
+        <v>47</v>
+      </c>
+      <c r="D153">
         <v>69699</v>
-      </c>
-      <c r="D153">
-        <v>47</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
@@ -4609,10 +4609,10 @@
         <v>9</v>
       </c>
       <c r="C154">
+        <v>6</v>
+      </c>
+      <c r="D154">
         <v>9000</v>
-      </c>
-      <c r="D154">
-        <v>6</v>
       </c>
       <c r="E154" t="s">
         <v>24</v>
@@ -4635,10 +4635,10 @@
         <v>9</v>
       </c>
       <c r="C155">
+        <v>30190</v>
+      </c>
+      <c r="D155">
         <v>43862088</v>
-      </c>
-      <c r="D155">
-        <v>30190</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4661,10 +4661,10 @@
         <v>9</v>
       </c>
       <c r="C156">
+        <v>17</v>
+      </c>
+      <c r="D156">
         <v>24857</v>
-      </c>
-      <c r="D156">
-        <v>17</v>
       </c>
       <c r="E156" t="s">
         <v>24</v>
@@ -4687,10 +4687,10 @@
         <v>9</v>
       </c>
       <c r="C157">
+        <v>9</v>
+      </c>
+      <c r="D157">
         <v>12160</v>
-      </c>
-      <c r="D157">
-        <v>9</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4713,10 +4713,10 @@
         <v>9</v>
       </c>
       <c r="C158">
+        <v>2388</v>
+      </c>
+      <c r="D158">
         <v>3374019</v>
-      </c>
-      <c r="D158">
-        <v>2388</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4739,10 +4739,10 @@
         <v>9</v>
       </c>
       <c r="C159">
+        <v>4</v>
+      </c>
+      <c r="D159">
         <v>6000</v>
-      </c>
-      <c r="D159">
-        <v>4</v>
       </c>
       <c r="E159" t="s">
         <v>24</v>
@@ -4765,10 +4765,10 @@
         <v>9</v>
       </c>
       <c r="C160">
+        <v>7</v>
+      </c>
+      <c r="D160">
         <v>10500</v>
-      </c>
-      <c r="D160">
-        <v>7</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4791,10 +4791,10 @@
         <v>9</v>
       </c>
       <c r="C161">
+        <v>2019</v>
+      </c>
+      <c r="D161">
         <v>2818213</v>
-      </c>
-      <c r="D161">
-        <v>2019</v>
       </c>
       <c r="E161" t="s">
         <v>24</v>
@@ -4817,10 +4817,10 @@
         <v>9</v>
       </c>
       <c r="C162">
+        <v>4</v>
+      </c>
+      <c r="D162">
         <v>6000</v>
-      </c>
-      <c r="D162">
-        <v>4</v>
       </c>
       <c r="E162" t="s">
         <v>24</v>
@@ -4843,10 +4843,10 @@
         <v>9</v>
       </c>
       <c r="C163">
+        <v>5</v>
+      </c>
+      <c r="D163">
         <v>7500</v>
-      </c>
-      <c r="D163">
-        <v>5</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4869,10 +4869,10 @@
         <v>9</v>
       </c>
       <c r="C164">
+        <v>61848</v>
+      </c>
+      <c r="D164">
         <v>78940393</v>
-      </c>
-      <c r="D164">
-        <v>61848</v>
       </c>
       <c r="E164" t="s">
         <v>25</v>
@@ -4895,10 +4895,10 @@
         <v>9</v>
       </c>
       <c r="C165">
+        <v>37</v>
+      </c>
+      <c r="D165">
         <v>38600</v>
-      </c>
-      <c r="D165">
-        <v>37</v>
       </c>
       <c r="E165" t="s">
         <v>25</v>
@@ -4921,10 +4921,10 @@
         <v>9</v>
       </c>
       <c r="C166">
+        <v>40</v>
+      </c>
+      <c r="D166">
         <v>57365</v>
-      </c>
-      <c r="D166">
-        <v>40</v>
       </c>
       <c r="E166" t="s">
         <v>25</v>
@@ -4947,10 +4947,10 @@
         <v>9</v>
       </c>
       <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167">
         <v>4900</v>
-      </c>
-      <c r="D167">
-        <v>4</v>
       </c>
       <c r="E167" t="s">
         <v>25</v>
@@ -4973,10 +4973,10 @@
         <v>9</v>
       </c>
       <c r="C168">
+        <v>286</v>
+      </c>
+      <c r="D168">
         <v>416129</v>
-      </c>
-      <c r="D168">
-        <v>286</v>
       </c>
       <c r="E168" t="s">
         <v>25</v>
@@ -4999,10 +4999,10 @@
         <v>9</v>
       </c>
       <c r="C169">
+        <v>32117</v>
+      </c>
+      <c r="D169">
         <v>47362674</v>
-      </c>
-      <c r="D169">
-        <v>32117</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5025,10 +5025,10 @@
         <v>9</v>
       </c>
       <c r="C170">
+        <v>18</v>
+      </c>
+      <c r="D170">
         <v>25649</v>
-      </c>
-      <c r="D170">
-        <v>18</v>
       </c>
       <c r="E170" t="s">
         <v>25</v>
@@ -5051,10 +5051,10 @@
         <v>9</v>
       </c>
       <c r="C171">
+        <v>7269</v>
+      </c>
+      <c r="D171">
         <v>10494625</v>
-      </c>
-      <c r="D171">
-        <v>7269</v>
       </c>
       <c r="E171" t="s">
         <v>25</v>
@@ -5077,10 +5077,10 @@
         <v>9</v>
       </c>
       <c r="C172">
+        <v>4</v>
+      </c>
+      <c r="D172">
         <v>4390</v>
-      </c>
-      <c r="D172">
-        <v>4</v>
       </c>
       <c r="E172" t="s">
         <v>25</v>
@@ -5103,10 +5103,10 @@
         <v>9</v>
       </c>
       <c r="C173">
+        <v>1070</v>
+      </c>
+      <c r="D173">
         <v>1541997</v>
-      </c>
-      <c r="D173">
-        <v>1070</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5129,10 +5129,10 @@
         <v>9</v>
       </c>
       <c r="C174">
+        <v>933</v>
+      </c>
+      <c r="D174">
         <v>1305177</v>
-      </c>
-      <c r="D174">
-        <v>933</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5155,10 +5155,10 @@
         <v>9</v>
       </c>
       <c r="C175">
+        <v>146810</v>
+      </c>
+      <c r="D175">
         <v>187091159</v>
-      </c>
-      <c r="D175">
-        <v>146810</v>
       </c>
       <c r="E175" t="s">
         <v>26</v>
@@ -5181,10 +5181,10 @@
         <v>9</v>
       </c>
       <c r="C176">
+        <v>80</v>
+      </c>
+      <c r="D176">
         <v>97997</v>
-      </c>
-      <c r="D176">
-        <v>80</v>
       </c>
       <c r="E176" t="s">
         <v>26</v>
@@ -5207,10 +5207,10 @@
         <v>9</v>
       </c>
       <c r="C177">
+        <v>139</v>
+      </c>
+      <c r="D177">
         <v>205062</v>
-      </c>
-      <c r="D177">
-        <v>139</v>
       </c>
       <c r="E177" t="s">
         <v>26</v>
@@ -5233,10 +5233,10 @@
         <v>9</v>
       </c>
       <c r="C178">
+        <v>6</v>
+      </c>
+      <c r="D178">
         <v>9000</v>
-      </c>
-      <c r="D178">
-        <v>6</v>
       </c>
       <c r="E178" t="s">
         <v>26</v>
@@ -5259,10 +5259,10 @@
         <v>9</v>
       </c>
       <c r="C179">
+        <v>4</v>
+      </c>
+      <c r="D179">
         <v>6000</v>
-      </c>
-      <c r="D179">
-        <v>4</v>
       </c>
       <c r="E179" t="s">
         <v>26</v>
@@ -5285,10 +5285,10 @@
         <v>9</v>
       </c>
       <c r="C180">
+        <v>7</v>
+      </c>
+      <c r="D180">
         <v>9981</v>
-      </c>
-      <c r="D180">
-        <v>7</v>
       </c>
       <c r="E180" t="s">
         <v>26</v>
@@ -5311,10 +5311,10 @@
         <v>9</v>
       </c>
       <c r="C181">
+        <v>451</v>
+      </c>
+      <c r="D181">
         <v>672838</v>
-      </c>
-      <c r="D181">
-        <v>451</v>
       </c>
       <c r="E181" t="s">
         <v>26</v>
@@ -5337,10 +5337,10 @@
         <v>9</v>
       </c>
       <c r="C182">
+        <v>7</v>
+      </c>
+      <c r="D182">
         <v>10500</v>
-      </c>
-      <c r="D182">
-        <v>7</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5363,10 +5363,10 @@
         <v>9</v>
       </c>
       <c r="C183">
+        <v>59645</v>
+      </c>
+      <c r="D183">
         <v>87959330</v>
-      </c>
-      <c r="D183">
-        <v>59645</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5389,10 +5389,10 @@
         <v>9</v>
       </c>
       <c r="C184">
+        <v>51</v>
+      </c>
+      <c r="D184">
         <v>74192</v>
-      </c>
-      <c r="D184">
-        <v>51</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5415,10 +5415,10 @@
         <v>9</v>
       </c>
       <c r="C185">
+        <v>37884</v>
+      </c>
+      <c r="D185">
         <v>55133550</v>
-      </c>
-      <c r="D185">
-        <v>37884</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5441,10 +5441,10 @@
         <v>9</v>
       </c>
       <c r="C186">
+        <v>7</v>
+      </c>
+      <c r="D186">
         <v>10489</v>
-      </c>
-      <c r="D186">
-        <v>7</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5467,10 +5467,10 @@
         <v>9</v>
       </c>
       <c r="C187">
+        <v>1232</v>
+      </c>
+      <c r="D187">
         <v>1754656</v>
-      </c>
-      <c r="D187">
-        <v>1232</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5493,10 +5493,10 @@
         <v>9</v>
       </c>
       <c r="C188">
+        <v>8</v>
+      </c>
+      <c r="D188">
         <v>12000</v>
-      </c>
-      <c r="D188">
-        <v>8</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5519,10 +5519,10 @@
         <v>9</v>
       </c>
       <c r="C189">
+        <v>1618</v>
+      </c>
+      <c r="D189">
         <v>2269633</v>
-      </c>
-      <c r="D189">
-        <v>1618</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5545,10 +5545,10 @@
         <v>9</v>
       </c>
       <c r="C190">
+        <v>228216</v>
+      </c>
+      <c r="D190">
         <v>301766402</v>
-      </c>
-      <c r="D190">
-        <v>228216</v>
       </c>
       <c r="E190" t="s">
         <v>27</v>
@@ -5571,10 +5571,10 @@
         <v>9</v>
       </c>
       <c r="C191">
+        <v>38</v>
+      </c>
+      <c r="D191">
         <v>47989</v>
-      </c>
-      <c r="D191">
-        <v>38</v>
       </c>
       <c r="E191" t="s">
         <v>27</v>
@@ -5597,10 +5597,10 @@
         <v>9</v>
       </c>
       <c r="C192">
+        <v>110</v>
+      </c>
+      <c r="D192">
         <v>163537</v>
-      </c>
-      <c r="D192">
-        <v>110</v>
       </c>
       <c r="E192" t="s">
         <v>27</v>
@@ -5623,10 +5623,10 @@
         <v>9</v>
       </c>
       <c r="C193">
+        <v>4</v>
+      </c>
+      <c r="D193">
         <v>6000</v>
-      </c>
-      <c r="D193">
-        <v>4</v>
       </c>
       <c r="E193" t="s">
         <v>27</v>
@@ -5649,10 +5649,10 @@
         <v>9</v>
       </c>
       <c r="C194">
+        <v>10</v>
+      </c>
+      <c r="D194">
         <v>14998</v>
-      </c>
-      <c r="D194">
-        <v>10</v>
       </c>
       <c r="E194" t="s">
         <v>27</v>
@@ -5675,10 +5675,10 @@
         <v>9</v>
       </c>
       <c r="C195">
+        <v>697</v>
+      </c>
+      <c r="D195">
         <v>1038074</v>
-      </c>
-      <c r="D195">
-        <v>697</v>
       </c>
       <c r="E195" t="s">
         <v>27</v>
@@ -5701,10 +5701,10 @@
         <v>9</v>
       </c>
       <c r="C196">
+        <v>11</v>
+      </c>
+      <c r="D196">
         <v>15716</v>
-      </c>
-      <c r="D196">
-        <v>11</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>
@@ -5727,10 +5727,10 @@
         <v>9</v>
       </c>
       <c r="C197">
+        <v>119034</v>
+      </c>
+      <c r="D197">
         <v>175934984</v>
-      </c>
-      <c r="D197">
-        <v>119034</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5753,10 +5753,10 @@
         <v>9</v>
       </c>
       <c r="C198">
+        <v>206</v>
+      </c>
+      <c r="D198">
         <v>306880</v>
-      </c>
-      <c r="D198">
-        <v>206</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5779,10 +5779,10 @@
         <v>9</v>
       </c>
       <c r="C199">
+        <v>6</v>
+      </c>
+      <c r="D199">
         <v>9000</v>
-      </c>
-      <c r="D199">
-        <v>6</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5805,10 +5805,10 @@
         <v>9</v>
       </c>
       <c r="C200">
+        <v>94616</v>
+      </c>
+      <c r="D200">
         <v>137968317</v>
-      </c>
-      <c r="D200">
-        <v>94616</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5831,10 +5831,10 @@
         <v>9</v>
       </c>
       <c r="C201">
+        <v>20</v>
+      </c>
+      <c r="D201">
         <v>28832</v>
-      </c>
-      <c r="D201">
-        <v>20</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5857,10 +5857,10 @@
         <v>9</v>
       </c>
       <c r="C202">
+        <v>1120</v>
+      </c>
+      <c r="D202">
         <v>1579179</v>
-      </c>
-      <c r="D202">
-        <v>1120</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5883,10 +5883,10 @@
         <v>9</v>
       </c>
       <c r="C203">
+        <v>3</v>
+      </c>
+      <c r="D203">
         <v>4222</v>
-      </c>
-      <c r="D203">
-        <v>3</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5909,10 +5909,10 @@
         <v>9</v>
       </c>
       <c r="C204">
+        <v>2083</v>
+      </c>
+      <c r="D204">
         <v>2959734</v>
-      </c>
-      <c r="D204">
-        <v>2083</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5935,10 +5935,10 @@
         <v>9</v>
       </c>
       <c r="C205">
+        <v>10</v>
+      </c>
+      <c r="D205">
         <v>15000</v>
-      </c>
-      <c r="D205">
-        <v>10</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-18 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="82">
   <si>
     <t>dispositif</t>
   </si>
@@ -617,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H205"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,10 +657,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>178404</v>
+        <v>179773</v>
       </c>
       <c r="D2">
-        <v>230501752</v>
+        <v>232204240</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -683,10 +683,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D3">
-        <v>160901</v>
+        <v>164021</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -709,10 +709,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D4">
-        <v>249378</v>
+        <v>253878</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -761,10 +761,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="D6">
-        <v>685592</v>
+        <v>700592</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -813,10 +813,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>73157</v>
+        <v>73921</v>
       </c>
       <c r="D8">
-        <v>108028359</v>
+        <v>109138199</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -865,10 +865,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>34456</v>
+        <v>34789</v>
       </c>
       <c r="D10">
-        <v>50085144</v>
+        <v>50560760</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -943,10 +943,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>1942</v>
+        <v>1968</v>
       </c>
       <c r="D13">
-        <v>2766423</v>
+        <v>2801844</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1021,10 +1021,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2104</v>
+        <v>2140</v>
       </c>
       <c r="D16">
-        <v>2969784</v>
+        <v>3021980</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1047,10 +1047,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>45335</v>
+        <v>45754</v>
       </c>
       <c r="D17">
-        <v>57796564</v>
+        <v>58309546</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1151,10 +1151,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D21">
-        <v>229241</v>
+        <v>232241</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1177,10 +1177,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>20658</v>
+        <v>20872</v>
       </c>
       <c r="D22">
-        <v>30468460</v>
+        <v>30781240</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1229,10 +1229,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>6842</v>
+        <v>6896</v>
       </c>
       <c r="D24">
-        <v>9935763</v>
+        <v>10012662</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1281,10 +1281,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>797</v>
+        <v>810</v>
       </c>
       <c r="D26">
-        <v>1123007</v>
+        <v>1139793</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1333,10 +1333,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>657</v>
+        <v>673</v>
       </c>
       <c r="D28">
-        <v>933668</v>
+        <v>954883</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1359,10 +1359,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>57904</v>
+        <v>58442</v>
       </c>
       <c r="D29">
-        <v>74489084</v>
+        <v>75147814</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1385,10 +1385,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30">
-        <v>33638</v>
+        <v>34462</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -1437,10 +1437,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="D32">
-        <v>680235</v>
+        <v>690735</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1489,10 +1489,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>28565</v>
+        <v>28827</v>
       </c>
       <c r="D34">
-        <v>42188920</v>
+        <v>42575136</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1541,10 +1541,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5488</v>
+        <v>5515</v>
       </c>
       <c r="D36">
-        <v>7916150</v>
+        <v>7954547</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1593,10 +1593,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="D38">
-        <v>984892</v>
+        <v>1003779</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1619,10 +1619,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>682</v>
+        <v>697</v>
       </c>
       <c r="D39">
-        <v>963029</v>
+        <v>983691</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1645,10 +1645,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>39994</v>
+        <v>40301</v>
       </c>
       <c r="D40">
-        <v>50905481</v>
+        <v>51270363</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1749,10 +1749,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D44">
-        <v>281581</v>
+        <v>283708</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1775,10 +1775,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>17789</v>
+        <v>17965</v>
       </c>
       <c r="D45">
-        <v>26249060</v>
+        <v>26503749</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1827,10 +1827,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6532</v>
+        <v>6593</v>
       </c>
       <c r="D47">
-        <v>9491231</v>
+        <v>9577109</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1853,10 +1853,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="D48">
-        <v>1020035</v>
+        <v>1041132</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1879,10 +1879,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>415</v>
+        <v>435</v>
       </c>
       <c r="D49">
-        <v>588085</v>
+        <v>614644</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -1905,10 +1905,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>11024</v>
+        <v>11113</v>
       </c>
       <c r="D50">
-        <v>14460780</v>
+        <v>14572870</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -2009,10 +2009,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>4088</v>
+        <v>4123</v>
       </c>
       <c r="D54">
-        <v>6008751</v>
+        <v>6059950</v>
       </c>
       <c r="E54" t="s">
         <v>14</v>
@@ -2035,10 +2035,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>2763</v>
+        <v>2793</v>
       </c>
       <c r="D55">
-        <v>4030173</v>
+        <v>4074350</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2061,10 +2061,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D56">
-        <v>314357</v>
+        <v>318857</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2087,10 +2087,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D57">
-        <v>127184</v>
+        <v>133184</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2113,10 +2113,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>81173</v>
+        <v>81832</v>
       </c>
       <c r="D58">
-        <v>102788081</v>
+        <v>103601543</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2139,10 +2139,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D59">
-        <v>26464</v>
+        <v>29464</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2165,10 +2165,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D60">
-        <v>69932</v>
+        <v>72932</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2217,10 +2217,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D62">
-        <v>323293</v>
+        <v>323826</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2269,10 +2269,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>40051</v>
+        <v>40461</v>
       </c>
       <c r="D64">
-        <v>59182969</v>
+        <v>59783343</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
@@ -2347,10 +2347,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>17761</v>
+        <v>17949</v>
       </c>
       <c r="D67">
-        <v>25858690</v>
+        <v>26126672</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2399,10 +2399,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>1256</v>
+        <v>1281</v>
       </c>
       <c r="D69">
-        <v>1811135</v>
+        <v>1847050</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2425,10 +2425,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>941</v>
+        <v>961</v>
       </c>
       <c r="D70">
-        <v>1333604</v>
+        <v>1362311</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2451,10 +2451,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>12648</v>
+        <v>12795</v>
       </c>
       <c r="D71">
-        <v>17143001</v>
+        <v>17341953</v>
       </c>
       <c r="E71" t="s">
         <v>16</v>
@@ -2555,10 +2555,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>4052</v>
+        <v>4092</v>
       </c>
       <c r="D75">
-        <v>5977759</v>
+        <v>6036649</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2607,10 +2607,10 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>3179</v>
+        <v>3219</v>
       </c>
       <c r="D77">
-        <v>4592705</v>
+        <v>4651595</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -2659,10 +2659,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D79">
-        <v>252311</v>
+        <v>254311</v>
       </c>
       <c r="E79" t="s">
         <v>16</v>
@@ -2685,10 +2685,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D80">
-        <v>199962</v>
+        <v>205962</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2711,10 +2711,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>2637</v>
+        <v>2673</v>
       </c>
       <c r="D81">
-        <v>3632992</v>
+        <v>3684513</v>
       </c>
       <c r="E81" t="s">
         <v>17</v>
@@ -2737,10 +2737,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="D82">
-        <v>1170854</v>
+        <v>1186864</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2789,10 +2789,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>954</v>
+        <v>965</v>
       </c>
       <c r="D84">
-        <v>1388291</v>
+        <v>1404791</v>
       </c>
       <c r="E84" t="s">
         <v>17</v>
@@ -2815,10 +2815,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D85">
-        <v>35318</v>
+        <v>38110</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2841,10 +2841,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D86">
-        <v>45950</v>
+        <v>48950</v>
       </c>
       <c r="E86" t="s">
         <v>17</v>
@@ -2867,10 +2867,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>83351</v>
+        <v>83934</v>
       </c>
       <c r="D87">
-        <v>104215155</v>
+        <v>104942677</v>
       </c>
       <c r="E87" t="s">
         <v>18</v>
@@ -2971,10 +2971,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="D91">
-        <v>726323</v>
+        <v>740777</v>
       </c>
       <c r="E91" t="s">
         <v>18</v>
@@ -3023,10 +3023,10 @@
         <v>9</v>
       </c>
       <c r="C93">
-        <v>34108</v>
+        <v>34413</v>
       </c>
       <c r="D93">
-        <v>50303448</v>
+        <v>50746408</v>
       </c>
       <c r="E93" t="s">
         <v>18</v>
@@ -3049,10 +3049,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D94">
-        <v>76500</v>
+        <v>78000</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3075,10 +3075,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>16056</v>
+        <v>16199</v>
       </c>
       <c r="D95">
-        <v>23364937</v>
+        <v>23572681</v>
       </c>
       <c r="E95" t="s">
         <v>18</v>
@@ -3101,10 +3101,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="D96">
-        <v>850913</v>
+        <v>866468</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3127,10 +3127,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>732</v>
+        <v>761</v>
       </c>
       <c r="D97">
-        <v>1032815</v>
+        <v>1074844</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3179,10 +3179,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>23648</v>
+        <v>23855</v>
       </c>
       <c r="D99">
-        <v>31942778</v>
+        <v>32210850</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
@@ -3309,10 +3309,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>8698</v>
+        <v>8755</v>
       </c>
       <c r="D104">
-        <v>12827778</v>
+        <v>12911566</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -3335,10 +3335,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>2217</v>
+        <v>2234</v>
       </c>
       <c r="D105">
-        <v>3213092</v>
+        <v>3237992</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3387,10 +3387,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D107">
-        <v>277230</v>
+        <v>280230</v>
       </c>
       <c r="E107" t="s">
         <v>19</v>
@@ -3413,10 +3413,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D108">
-        <v>179066</v>
+        <v>191066</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -3439,10 +3439,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>8563</v>
+        <v>8675</v>
       </c>
       <c r="D109">
-        <v>11423258</v>
+        <v>11574954</v>
       </c>
       <c r="E109" t="s">
         <v>20</v>
@@ -3491,10 +3491,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>3958</v>
+        <v>4008</v>
       </c>
       <c r="D111">
-        <v>5794672</v>
+        <v>5868292</v>
       </c>
       <c r="E111" t="s">
         <v>20</v>
@@ -3517,10 +3517,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>2445</v>
+        <v>2473</v>
       </c>
       <c r="D112">
-        <v>3536367</v>
+        <v>3578367</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3595,10 +3595,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>2393</v>
+        <v>2442</v>
       </c>
       <c r="D115">
-        <v>3383012</v>
+        <v>3450906</v>
       </c>
       <c r="E115" t="s">
         <v>21</v>
@@ -3621,10 +3621,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="D116">
-        <v>1021993</v>
+        <v>1035463</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3647,10 +3647,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D117">
-        <v>132600</v>
+        <v>137100</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3725,10 +3725,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>52350</v>
+        <v>52763</v>
       </c>
       <c r="D120">
-        <v>66568785</v>
+        <v>67085064</v>
       </c>
       <c r="E120" t="s">
         <v>22</v>
@@ -3829,10 +3829,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D124">
-        <v>491762</v>
+        <v>496262</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
@@ -3881,10 +3881,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>21994</v>
+        <v>22206</v>
       </c>
       <c r="D126">
-        <v>32447763</v>
+        <v>32756705</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
@@ -3933,10 +3933,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>7732</v>
+        <v>7808</v>
       </c>
       <c r="D128">
-        <v>11238814</v>
+        <v>11347732</v>
       </c>
       <c r="E128" t="s">
         <v>22</v>
@@ -3985,10 +3985,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>646</v>
+        <v>661</v>
       </c>
       <c r="D130">
-        <v>908322</v>
+        <v>929922</v>
       </c>
       <c r="E130" t="s">
         <v>22</v>
@@ -4011,10 +4011,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="D131">
-        <v>869447</v>
+        <v>898625</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4037,10 +4037,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>138747</v>
+        <v>139835</v>
       </c>
       <c r="D132">
-        <v>175088042</v>
+        <v>176409395</v>
       </c>
       <c r="E132" t="s">
         <v>23</v>
@@ -4063,10 +4063,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D133">
-        <v>64536</v>
+        <v>65576</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4089,10 +4089,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D134">
-        <v>141375</v>
+        <v>145875</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4141,10 +4141,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="D136">
-        <v>722809</v>
+        <v>728809</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
@@ -4193,10 +4193,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>55809</v>
+        <v>56345</v>
       </c>
       <c r="D138">
-        <v>82223809</v>
+        <v>83008400</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4245,10 +4245,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>19846</v>
+        <v>20024</v>
       </c>
       <c r="D140">
-        <v>28723269</v>
+        <v>28977912</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4323,10 +4323,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>2623</v>
+        <v>2658</v>
       </c>
       <c r="D143">
-        <v>3751218</v>
+        <v>3799905</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4375,10 +4375,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>1702</v>
+        <v>1746</v>
       </c>
       <c r="D145">
-        <v>2362376</v>
+        <v>2425286</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -4401,10 +4401,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>149100</v>
+        <v>150372</v>
       </c>
       <c r="D146">
-        <v>186484314</v>
+        <v>188079928</v>
       </c>
       <c r="E146" t="s">
         <v>24</v>
@@ -4453,10 +4453,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D148">
-        <v>197049</v>
+        <v>198549</v>
       </c>
       <c r="E148" t="s">
         <v>24</v>
@@ -4531,10 +4531,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D151">
-        <v>497546</v>
+        <v>500546</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4557,10 +4557,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>59244</v>
+        <v>59836</v>
       </c>
       <c r="D152">
-        <v>87189802</v>
+        <v>88051993</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -4635,10 +4635,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>30190</v>
+        <v>30460</v>
       </c>
       <c r="D155">
-        <v>43862088</v>
+        <v>44250591</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4713,10 +4713,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>2388</v>
+        <v>2421</v>
       </c>
       <c r="D158">
-        <v>3374019</v>
+        <v>3413447</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4791,10 +4791,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>2019</v>
+        <v>2063</v>
       </c>
       <c r="D161">
-        <v>2818213</v>
+        <v>2879493</v>
       </c>
       <c r="E161" t="s">
         <v>24</v>
@@ -4869,10 +4869,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>61848</v>
+        <v>62325</v>
       </c>
       <c r="D164">
-        <v>78940393</v>
+        <v>79531223</v>
       </c>
       <c r="E164" t="s">
         <v>25</v>
@@ -4973,10 +4973,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D168">
-        <v>416129</v>
+        <v>426629</v>
       </c>
       <c r="E168" t="s">
         <v>25</v>
@@ -4999,10 +4999,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>32117</v>
+        <v>32379</v>
       </c>
       <c r="D169">
-        <v>47362674</v>
+        <v>47746578</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5051,10 +5051,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>7269</v>
+        <v>7330</v>
       </c>
       <c r="D171">
-        <v>10494625</v>
+        <v>10582581</v>
       </c>
       <c r="E171" t="s">
         <v>25</v>
@@ -5103,10 +5103,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>1070</v>
+        <v>1088</v>
       </c>
       <c r="D173">
-        <v>1541997</v>
+        <v>1568407</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5129,10 +5129,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>933</v>
+        <v>3</v>
       </c>
       <c r="D174">
-        <v>1305177</v>
+        <v>2596</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5141,10 +5141,10 @@
         <v>43</v>
       </c>
       <c r="G174" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H174" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5155,22 +5155,22 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>146810</v>
+        <v>950</v>
       </c>
       <c r="D175">
-        <v>187091159</v>
+        <v>1328503</v>
       </c>
       <c r="E175" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F175" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G175" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H175" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5181,10 +5181,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>80</v>
+        <v>147901</v>
       </c>
       <c r="D176">
-        <v>97997</v>
+        <v>188436887</v>
       </c>
       <c r="E176" t="s">
         <v>26</v>
@@ -5193,10 +5193,10 @@
         <v>44</v>
       </c>
       <c r="G176" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H176" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5207,10 +5207,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="D177">
-        <v>205062</v>
+        <v>99497</v>
       </c>
       <c r="E177" t="s">
         <v>26</v>
@@ -5219,10 +5219,10 @@
         <v>44</v>
       </c>
       <c r="G177" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H177" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5233,10 +5233,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="D178">
-        <v>9000</v>
+        <v>205062</v>
       </c>
       <c r="E178" t="s">
         <v>26</v>
@@ -5245,10 +5245,10 @@
         <v>44</v>
       </c>
       <c r="G178" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H178" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5259,10 +5259,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D179">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E179" t="s">
         <v>26</v>
@@ -5271,10 +5271,10 @@
         <v>44</v>
       </c>
       <c r="G179" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H179" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5285,10 +5285,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D180">
-        <v>9981</v>
+        <v>6000</v>
       </c>
       <c r="E180" t="s">
         <v>26</v>
@@ -5297,10 +5297,10 @@
         <v>44</v>
       </c>
       <c r="G180" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H180" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5311,10 +5311,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>451</v>
+        <v>7</v>
       </c>
       <c r="D181">
-        <v>672838</v>
+        <v>9981</v>
       </c>
       <c r="E181" t="s">
         <v>26</v>
@@ -5323,10 +5323,10 @@
         <v>44</v>
       </c>
       <c r="G181" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H181" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5337,10 +5337,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>7</v>
+        <v>459</v>
       </c>
       <c r="D182">
-        <v>10500</v>
+        <v>684838</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5349,10 +5349,10 @@
         <v>44</v>
       </c>
       <c r="G182" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H182" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5363,10 +5363,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>59645</v>
+        <v>7</v>
       </c>
       <c r="D183">
-        <v>87959330</v>
+        <v>10500</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5375,10 +5375,10 @@
         <v>44</v>
       </c>
       <c r="G183" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H183" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5389,10 +5389,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>51</v>
+        <v>60209</v>
       </c>
       <c r="D184">
-        <v>74192</v>
+        <v>88780540</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5401,10 +5401,10 @@
         <v>44</v>
       </c>
       <c r="G184" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H184" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5415,10 +5415,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>37884</v>
+        <v>53</v>
       </c>
       <c r="D185">
-        <v>55133550</v>
+        <v>77192</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5427,10 +5427,10 @@
         <v>44</v>
       </c>
       <c r="G185" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H185" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5441,10 +5441,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>7</v>
+        <v>38206</v>
       </c>
       <c r="D186">
-        <v>10489</v>
+        <v>55598565</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5453,10 +5453,10 @@
         <v>44</v>
       </c>
       <c r="G186" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H186" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5467,10 +5467,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>1232</v>
+        <v>7</v>
       </c>
       <c r="D187">
-        <v>1754656</v>
+        <v>10489</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5479,10 +5479,10 @@
         <v>44</v>
       </c>
       <c r="G187" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H187" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5493,10 +5493,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>8</v>
+        <v>1246</v>
       </c>
       <c r="D188">
-        <v>12000</v>
+        <v>1775656</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5505,10 +5505,10 @@
         <v>44</v>
       </c>
       <c r="G188" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H188" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5519,10 +5519,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>1618</v>
+        <v>8</v>
       </c>
       <c r="D189">
-        <v>2269633</v>
+        <v>12000</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5531,10 +5531,10 @@
         <v>44</v>
       </c>
       <c r="G189" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H189" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5545,22 +5545,22 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>228216</v>
+        <v>1646</v>
       </c>
       <c r="D190">
-        <v>301766402</v>
+        <v>2308424</v>
       </c>
       <c r="E190" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F190" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G190" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H190" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5571,10 +5571,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>38</v>
+        <v>230296</v>
       </c>
       <c r="D191">
-        <v>47989</v>
+        <v>304381763</v>
       </c>
       <c r="E191" t="s">
         <v>27</v>
@@ -5583,10 +5583,10 @@
         <v>45</v>
       </c>
       <c r="G191" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H191" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5597,10 +5597,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="D192">
-        <v>163537</v>
+        <v>50389</v>
       </c>
       <c r="E192" t="s">
         <v>27</v>
@@ -5609,10 +5609,10 @@
         <v>45</v>
       </c>
       <c r="G192" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H192" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5623,10 +5623,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="D193">
-        <v>6000</v>
+        <v>166537</v>
       </c>
       <c r="E193" t="s">
         <v>27</v>
@@ -5635,10 +5635,10 @@
         <v>45</v>
       </c>
       <c r="G193" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H193" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5649,10 +5649,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D194">
-        <v>14998</v>
+        <v>6000</v>
       </c>
       <c r="E194" t="s">
         <v>27</v>
@@ -5661,10 +5661,10 @@
         <v>45</v>
       </c>
       <c r="G194" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H194" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5675,10 +5675,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>697</v>
+        <v>10</v>
       </c>
       <c r="D195">
-        <v>1038074</v>
+        <v>14998</v>
       </c>
       <c r="E195" t="s">
         <v>27</v>
@@ -5687,10 +5687,10 @@
         <v>45</v>
       </c>
       <c r="G195" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H195" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5701,10 +5701,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>11</v>
+        <v>708</v>
       </c>
       <c r="D196">
-        <v>15716</v>
+        <v>1054574</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>
@@ -5713,10 +5713,10 @@
         <v>45</v>
       </c>
       <c r="G196" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H196" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5727,10 +5727,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>119034</v>
+        <v>11</v>
       </c>
       <c r="D197">
-        <v>175934984</v>
+        <v>15716</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5739,10 +5739,10 @@
         <v>45</v>
       </c>
       <c r="G197" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H197" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5753,10 +5753,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>206</v>
+        <v>120270</v>
       </c>
       <c r="D198">
-        <v>306880</v>
+        <v>177739387</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5765,10 +5765,10 @@
         <v>45</v>
       </c>
       <c r="G198" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H198" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5779,10 +5779,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>6</v>
+        <v>210</v>
       </c>
       <c r="D199">
-        <v>9000</v>
+        <v>312880</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5791,10 +5791,10 @@
         <v>45</v>
       </c>
       <c r="G199" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H199" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5805,10 +5805,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>94616</v>
+        <v>6</v>
       </c>
       <c r="D200">
-        <v>137968317</v>
+        <v>9000</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5817,10 +5817,10 @@
         <v>45</v>
       </c>
       <c r="G200" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H200" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5831,10 +5831,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>20</v>
+        <v>95574</v>
       </c>
       <c r="D201">
-        <v>28832</v>
+        <v>139347112</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5843,10 +5843,10 @@
         <v>45</v>
       </c>
       <c r="G201" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H201" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5857,10 +5857,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>1120</v>
+        <v>20</v>
       </c>
       <c r="D202">
-        <v>1579179</v>
+        <v>28832</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5869,10 +5869,10 @@
         <v>45</v>
       </c>
       <c r="G202" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H202" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5883,10 +5883,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>3</v>
+        <v>1146</v>
       </c>
       <c r="D203">
-        <v>4222</v>
+        <v>1613313</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5895,10 +5895,10 @@
         <v>45</v>
       </c>
       <c r="G203" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H203" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5909,10 +5909,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>2083</v>
+        <v>3</v>
       </c>
       <c r="D204">
-        <v>2959734</v>
+        <v>4222</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5921,10 +5921,10 @@
         <v>45</v>
       </c>
       <c r="G204" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H204" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5935,10 +5935,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>10</v>
+        <v>2129</v>
       </c>
       <c r="D205">
-        <v>15000</v>
+        <v>3023825</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5947,9 +5947,35 @@
         <v>45</v>
       </c>
       <c r="G205" t="s">
+        <v>57</v>
+      </c>
+      <c r="H205" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8">
+      <c r="A206" t="s">
+        <v>8</v>
+      </c>
+      <c r="B206" t="s">
+        <v>9</v>
+      </c>
+      <c r="C206">
+        <v>10</v>
+      </c>
+      <c r="D206">
+        <v>15000</v>
+      </c>
+      <c r="E206" t="s">
+        <v>27</v>
+      </c>
+      <c r="F206" t="s">
+        <v>45</v>
+      </c>
+      <c r="G206" t="s">
         <v>60</v>
       </c>
-      <c r="H205" t="s">
+      <c r="H206" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-19 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="83">
   <si>
     <t>dispositif</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Autre personne morale de droit privé</t>
+  </si>
+  <si>
+    <t>Paroisse hors zone concordataire</t>
   </si>
   <si>
     <t>Fondation</t>
@@ -617,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H206"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>179773</v>
+        <v>182003</v>
       </c>
       <c r="D2">
-        <v>232204240</v>
+        <v>234932654</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -683,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D3">
-        <v>164021</v>
+        <v>166051</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -709,10 +712,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D4">
-        <v>253878</v>
+        <v>258378</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -761,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="D6">
-        <v>700592</v>
+        <v>715592</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -813,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>73921</v>
+        <v>74874</v>
       </c>
       <c r="D8">
-        <v>109138199</v>
+        <v>110518434</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -839,10 +842,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D9">
-        <v>127290</v>
+        <v>131790</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -865,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>34789</v>
+        <v>35272</v>
       </c>
       <c r="D10">
-        <v>50560760</v>
+        <v>51237215</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -891,10 +894,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>36210</v>
+        <v>37710</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -943,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>1968</v>
+        <v>2008</v>
       </c>
       <c r="D13">
-        <v>2801844</v>
+        <v>2859476</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1021,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2140</v>
+        <v>2251</v>
       </c>
       <c r="D16">
-        <v>3021980</v>
+        <v>3178112</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1047,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>45754</v>
+        <v>46266</v>
       </c>
       <c r="D17">
-        <v>58309546</v>
+        <v>58931553</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1073,10 +1076,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18">
-        <v>42140</v>
+        <v>43640</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1151,10 +1154,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D21">
-        <v>232241</v>
+        <v>244241</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1177,10 +1180,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>20872</v>
+        <v>21158</v>
       </c>
       <c r="D22">
-        <v>30781240</v>
+        <v>31193416</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1229,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>6896</v>
+        <v>6991</v>
       </c>
       <c r="D24">
-        <v>10012662</v>
+        <v>10148656</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1255,10 +1258,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>12000</v>
+        <v>12638</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1281,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>810</v>
+        <v>822</v>
       </c>
       <c r="D26">
-        <v>1139793</v>
+        <v>1156893</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1333,10 +1336,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>673</v>
+        <v>691</v>
       </c>
       <c r="D28">
-        <v>954883</v>
+        <v>978983</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1359,10 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>58442</v>
+        <v>59026</v>
       </c>
       <c r="D29">
-        <v>75147814</v>
+        <v>75869204</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1411,10 +1414,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D31">
-        <v>73044</v>
+        <v>74544</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1437,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="D32">
-        <v>690735</v>
+        <v>709471</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1489,10 +1492,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>28827</v>
+        <v>29145</v>
       </c>
       <c r="D34">
-        <v>42575136</v>
+        <v>43033177</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1541,10 +1544,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5515</v>
+        <v>5577</v>
       </c>
       <c r="D36">
-        <v>7954547</v>
+        <v>8040824</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1593,10 +1596,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>715</v>
+        <v>726</v>
       </c>
       <c r="D38">
-        <v>1003779</v>
+        <v>1016541</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1619,10 +1622,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>697</v>
+        <v>737</v>
       </c>
       <c r="D39">
-        <v>983691</v>
+        <v>1038582</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1645,10 +1648,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>40301</v>
+        <v>40771</v>
       </c>
       <c r="D40">
-        <v>51270363</v>
+        <v>51832508</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1749,10 +1752,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D44">
-        <v>283708</v>
+        <v>289708</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1775,10 +1778,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>17965</v>
+        <v>18214</v>
       </c>
       <c r="D45">
-        <v>26503749</v>
+        <v>26869264</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1827,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6593</v>
+        <v>6680</v>
       </c>
       <c r="D47">
-        <v>9577109</v>
+        <v>9697552</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1853,10 +1856,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="D48">
-        <v>1041132</v>
+        <v>1056110</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1879,10 +1882,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>435</v>
+        <v>4</v>
       </c>
       <c r="D49">
-        <v>614644</v>
+        <v>5400</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -1891,10 +1894,10 @@
         <v>31</v>
       </c>
       <c r="G49" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1905,22 +1908,22 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>11113</v>
+        <v>471</v>
       </c>
       <c r="D50">
-        <v>14572870</v>
+        <v>666968</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G50" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H50" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1931,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>14</v>
+        <v>11322</v>
       </c>
       <c r="D51">
-        <v>17827</v>
+        <v>14835194</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -1943,10 +1946,10 @@
         <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1957,10 +1960,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D52">
-        <v>16725</v>
+        <v>17827</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
@@ -1969,10 +1972,10 @@
         <v>32</v>
       </c>
       <c r="G52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1983,10 +1986,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D53">
-        <v>39202</v>
+        <v>16725</v>
       </c>
       <c r="E53" t="s">
         <v>14</v>
@@ -1995,10 +1998,10 @@
         <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2009,10 +2012,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>4123</v>
+        <v>27</v>
       </c>
       <c r="D54">
-        <v>6059950</v>
+        <v>39202</v>
       </c>
       <c r="E54" t="s">
         <v>14</v>
@@ -2021,10 +2024,10 @@
         <v>32</v>
       </c>
       <c r="G54" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2035,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>2793</v>
+        <v>4187</v>
       </c>
       <c r="D55">
-        <v>4074350</v>
+        <v>6151385</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2047,10 +2050,10 @@
         <v>32</v>
       </c>
       <c r="G55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H55" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2061,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>229</v>
+        <v>2843</v>
       </c>
       <c r="D56">
-        <v>318857</v>
+        <v>4146955</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2073,10 +2076,10 @@
         <v>32</v>
       </c>
       <c r="G56" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2087,10 +2090,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>95</v>
+        <v>236</v>
       </c>
       <c r="D57">
-        <v>133184</v>
+        <v>327824</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2099,10 +2102,10 @@
         <v>32</v>
       </c>
       <c r="G57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2113,22 +2116,22 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>81832</v>
+        <v>99</v>
       </c>
       <c r="D58">
-        <v>103601543</v>
+        <v>137023</v>
       </c>
       <c r="E58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G58" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H58" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2139,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>25</v>
+        <v>82780</v>
       </c>
       <c r="D59">
-        <v>29464</v>
+        <v>104763489</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2151,10 +2154,10 @@
         <v>33</v>
       </c>
       <c r="G59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2165,10 +2168,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D60">
-        <v>72932</v>
+        <v>31611</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2177,10 +2180,10 @@
         <v>33</v>
       </c>
       <c r="G60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2191,10 +2194,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D61">
-        <v>13500</v>
+        <v>72932</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2203,10 +2206,10 @@
         <v>33</v>
       </c>
       <c r="G61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2217,10 +2220,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="D62">
-        <v>323826</v>
+        <v>13500</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2229,10 +2232,10 @@
         <v>33</v>
       </c>
       <c r="G62" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2243,10 +2246,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>7</v>
+        <v>225</v>
       </c>
       <c r="D63">
-        <v>8947</v>
+        <v>329826</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2255,10 +2258,10 @@
         <v>33</v>
       </c>
       <c r="G63" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2269,10 +2272,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>40461</v>
+        <v>7</v>
       </c>
       <c r="D64">
-        <v>59783343</v>
+        <v>8947</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
@@ -2281,10 +2284,10 @@
         <v>33</v>
       </c>
       <c r="G64" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2295,10 +2298,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>46</v>
+        <v>40984</v>
       </c>
       <c r="D65">
-        <v>68174</v>
+        <v>60544867</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2307,10 +2310,10 @@
         <v>33</v>
       </c>
       <c r="G65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2321,10 +2324,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D66">
-        <v>6000</v>
+        <v>68174</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2333,10 +2336,10 @@
         <v>33</v>
       </c>
       <c r="G66" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H66" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2347,10 +2350,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>17949</v>
+        <v>4</v>
       </c>
       <c r="D67">
-        <v>26126672</v>
+        <v>6000</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2359,10 +2362,10 @@
         <v>33</v>
       </c>
       <c r="G67" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H67" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2373,10 +2376,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>6</v>
+        <v>18177</v>
       </c>
       <c r="D68">
-        <v>7570</v>
+        <v>26447389</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2385,10 +2388,10 @@
         <v>33</v>
       </c>
       <c r="G68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2399,10 +2402,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>1281</v>
+        <v>6</v>
       </c>
       <c r="D69">
-        <v>1847050</v>
+        <v>7570</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2411,10 +2414,10 @@
         <v>33</v>
       </c>
       <c r="G69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2425,10 +2428,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>961</v>
+        <v>1311</v>
       </c>
       <c r="D70">
-        <v>1362311</v>
+        <v>1890741</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2437,10 +2440,10 @@
         <v>33</v>
       </c>
       <c r="G70" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H70" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2451,22 +2454,22 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>12795</v>
+        <v>990</v>
       </c>
       <c r="D71">
-        <v>17341953</v>
+        <v>1403661</v>
       </c>
       <c r="E71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G71" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H71" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2477,10 +2480,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>13127</v>
       </c>
       <c r="D72">
-        <v>6000</v>
+        <v>17799604</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2489,10 +2492,10 @@
         <v>34</v>
       </c>
       <c r="G72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H72" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2503,10 +2506,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D73">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="E73" t="s">
         <v>16</v>
@@ -2515,10 +2518,10 @@
         <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H73" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2529,10 +2532,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D74">
-        <v>20256</v>
+        <v>10500</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2541,10 +2544,10 @@
         <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="H74" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2555,10 +2558,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>4092</v>
+        <v>14</v>
       </c>
       <c r="D75">
-        <v>6036649</v>
+        <v>20256</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2567,10 +2570,10 @@
         <v>34</v>
       </c>
       <c r="G75" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H75" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2581,10 +2584,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>4166</v>
       </c>
       <c r="D76">
-        <v>4500</v>
+        <v>6144846</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2593,10 +2596,10 @@
         <v>34</v>
       </c>
       <c r="G76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2607,10 +2610,10 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>3219</v>
+        <v>3</v>
       </c>
       <c r="D77">
-        <v>4651595</v>
+        <v>4500</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -2619,10 +2622,10 @@
         <v>34</v>
       </c>
       <c r="G77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2633,10 +2636,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>3273</v>
       </c>
       <c r="D78">
-        <v>4500</v>
+        <v>4730106</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2645,10 +2648,10 @@
         <v>34</v>
       </c>
       <c r="G78" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2659,10 +2662,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>178</v>
+        <v>3</v>
       </c>
       <c r="D79">
-        <v>254311</v>
+        <v>4500</v>
       </c>
       <c r="E79" t="s">
         <v>16</v>
@@ -2671,10 +2674,10 @@
         <v>34</v>
       </c>
       <c r="G79" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H79" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2685,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="D80">
-        <v>205962</v>
+        <v>261811</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2697,10 +2700,10 @@
         <v>34</v>
       </c>
       <c r="G80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H80" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2711,22 +2714,22 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>2673</v>
+        <v>145</v>
       </c>
       <c r="D81">
-        <v>3684513</v>
+        <v>209982</v>
       </c>
       <c r="E81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G81" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H81" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2737,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>808</v>
+        <v>2779</v>
       </c>
       <c r="D82">
-        <v>1186864</v>
+        <v>3828885</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2749,10 +2752,10 @@
         <v>35</v>
       </c>
       <c r="G82" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H82" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2763,10 +2766,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>3</v>
+        <v>826</v>
       </c>
       <c r="D83">
-        <v>4500</v>
+        <v>1213864</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2775,10 +2778,10 @@
         <v>35</v>
       </c>
       <c r="G83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2789,10 +2792,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>965</v>
+        <v>4</v>
       </c>
       <c r="D84">
-        <v>1404791</v>
+        <v>6000</v>
       </c>
       <c r="E84" t="s">
         <v>17</v>
@@ -2801,10 +2804,10 @@
         <v>35</v>
       </c>
       <c r="G84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2815,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>26</v>
+        <v>997</v>
       </c>
       <c r="D85">
-        <v>38110</v>
+        <v>1450871</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2827,10 +2830,10 @@
         <v>35</v>
       </c>
       <c r="G85" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H85" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2841,10 +2844,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D86">
-        <v>48950</v>
+        <v>38110</v>
       </c>
       <c r="E86" t="s">
         <v>17</v>
@@ -2853,10 +2856,10 @@
         <v>35</v>
       </c>
       <c r="G86" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H86" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2867,22 +2870,22 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>83934</v>
+        <v>36</v>
       </c>
       <c r="D87">
-        <v>104942677</v>
+        <v>51950</v>
       </c>
       <c r="E87" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G87" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H87" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2893,10 +2896,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>21</v>
+        <v>84899</v>
       </c>
       <c r="D88">
-        <v>25249</v>
+        <v>106104076</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -2905,10 +2908,10 @@
         <v>36</v>
       </c>
       <c r="G88" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H88" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2919,10 +2922,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D89">
-        <v>57561</v>
+        <v>28249</v>
       </c>
       <c r="E89" t="s">
         <v>18</v>
@@ -2931,10 +2934,10 @@
         <v>36</v>
       </c>
       <c r="G89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H89" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2945,10 +2948,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="D90">
-        <v>5895</v>
+        <v>57561</v>
       </c>
       <c r="E90" t="s">
         <v>18</v>
@@ -2957,10 +2960,10 @@
         <v>36</v>
       </c>
       <c r="G90" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2971,10 +2974,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>500</v>
+        <v>4</v>
       </c>
       <c r="D91">
-        <v>740777</v>
+        <v>5895</v>
       </c>
       <c r="E91" t="s">
         <v>18</v>
@@ -2983,10 +2986,10 @@
         <v>36</v>
       </c>
       <c r="G91" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2997,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>4</v>
+        <v>512</v>
       </c>
       <c r="D92">
-        <v>5600</v>
+        <v>758777</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3009,10 +3012,10 @@
         <v>36</v>
       </c>
       <c r="G92" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3023,10 +3026,10 @@
         <v>9</v>
       </c>
       <c r="C93">
-        <v>34413</v>
+        <v>4</v>
       </c>
       <c r="D93">
-        <v>50746408</v>
+        <v>5600</v>
       </c>
       <c r="E93" t="s">
         <v>18</v>
@@ -3035,10 +3038,10 @@
         <v>36</v>
       </c>
       <c r="G93" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3049,10 +3052,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>52</v>
+        <v>34865</v>
       </c>
       <c r="D94">
-        <v>78000</v>
+        <v>51399230</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3061,10 +3064,10 @@
         <v>36</v>
       </c>
       <c r="G94" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3075,10 +3078,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>16199</v>
+        <v>55</v>
       </c>
       <c r="D95">
-        <v>23572681</v>
+        <v>81659</v>
       </c>
       <c r="E95" t="s">
         <v>18</v>
@@ -3087,10 +3090,10 @@
         <v>36</v>
       </c>
       <c r="G95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3101,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>632</v>
+        <v>16409</v>
       </c>
       <c r="D96">
-        <v>866468</v>
+        <v>23870543</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3113,10 +3116,10 @@
         <v>36</v>
       </c>
       <c r="G96" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H96" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3127,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>761</v>
+        <v>646</v>
       </c>
       <c r="D97">
-        <v>1074844</v>
+        <v>884720</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3139,10 +3142,10 @@
         <v>36</v>
       </c>
       <c r="G97" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3153,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>7</v>
+        <v>799</v>
       </c>
       <c r="D98">
-        <v>10500</v>
+        <v>1124279</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3165,10 +3168,10 @@
         <v>36</v>
       </c>
       <c r="G98" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H98" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3179,22 +3182,22 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>23855</v>
+        <v>7</v>
       </c>
       <c r="D99">
-        <v>32210850</v>
+        <v>10500</v>
       </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F99" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G99" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H99" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3205,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>11</v>
+        <v>24182</v>
       </c>
       <c r="D100">
-        <v>14653</v>
+        <v>32646600</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3217,10 +3220,10 @@
         <v>37</v>
       </c>
       <c r="G100" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3231,10 +3234,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D101">
-        <v>18423</v>
+        <v>14653</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -3243,10 +3246,10 @@
         <v>37</v>
       </c>
       <c r="G101" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H101" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3257,10 +3260,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D102">
-        <v>4500</v>
+        <v>18423</v>
       </c>
       <c r="E102" t="s">
         <v>19</v>
@@ -3269,10 +3272,10 @@
         <v>37</v>
       </c>
       <c r="G102" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H102" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3283,10 +3286,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>315</v>
+        <v>3</v>
       </c>
       <c r="D103">
-        <v>472500</v>
+        <v>4500</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
@@ -3295,10 +3298,10 @@
         <v>37</v>
       </c>
       <c r="G103" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="H103" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3309,10 +3312,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>8755</v>
+        <v>315</v>
       </c>
       <c r="D104">
-        <v>12911566</v>
+        <v>472500</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -3321,10 +3324,10 @@
         <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H104" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3335,10 +3338,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>2234</v>
+        <v>8851</v>
       </c>
       <c r="D105">
-        <v>3237992</v>
+        <v>13052936</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3347,10 +3350,10 @@
         <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H105" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3361,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>6</v>
+        <v>2265</v>
       </c>
       <c r="D106">
-        <v>9000</v>
+        <v>3283169</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3373,10 +3376,10 @@
         <v>37</v>
       </c>
       <c r="G106" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H106" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3387,10 +3390,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>194</v>
+        <v>6</v>
       </c>
       <c r="D107">
-        <v>280230</v>
+        <v>9000</v>
       </c>
       <c r="E107" t="s">
         <v>19</v>
@@ -3399,10 +3402,10 @@
         <v>37</v>
       </c>
       <c r="G107" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H107" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3413,10 +3416,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="D108">
-        <v>191066</v>
+        <v>294215</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -3425,10 +3428,10 @@
         <v>37</v>
       </c>
       <c r="G108" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H108" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3439,22 +3442,22 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>8675</v>
+        <v>152</v>
       </c>
       <c r="D109">
-        <v>11574954</v>
+        <v>212066</v>
       </c>
       <c r="E109" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F109" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G109" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H109" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3465,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>35</v>
+        <v>8806</v>
       </c>
       <c r="D110">
-        <v>50906</v>
+        <v>11742320</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3477,10 +3480,10 @@
         <v>38</v>
       </c>
       <c r="G110" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H110" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3491,10 +3494,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>4008</v>
+        <v>35</v>
       </c>
       <c r="D111">
-        <v>5868292</v>
+        <v>50906</v>
       </c>
       <c r="E111" t="s">
         <v>20</v>
@@ -3503,10 +3506,10 @@
         <v>38</v>
       </c>
       <c r="G111" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H111" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3517,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>2473</v>
+        <v>4067</v>
       </c>
       <c r="D112">
-        <v>3578367</v>
+        <v>5951726</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3529,10 +3532,10 @@
         <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H112" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3543,10 +3546,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>121</v>
+        <v>2521</v>
       </c>
       <c r="D113">
-        <v>169262</v>
+        <v>3647288</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3555,10 +3558,10 @@
         <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H113" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3569,10 +3572,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="D114">
-        <v>88518</v>
+        <v>173762</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3581,10 +3584,10 @@
         <v>38</v>
       </c>
       <c r="G114" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H114" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3595,22 +3598,22 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>2442</v>
+        <v>67</v>
       </c>
       <c r="D115">
-        <v>3450906</v>
+        <v>96018</v>
       </c>
       <c r="E115" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F115" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G115" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H115" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3621,10 +3624,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>699</v>
+        <v>2760</v>
       </c>
       <c r="D116">
-        <v>1035463</v>
+        <v>3902662</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3633,10 +3636,10 @@
         <v>39</v>
       </c>
       <c r="G116" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H116" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3647,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>93</v>
+        <v>733</v>
       </c>
       <c r="D117">
-        <v>137100</v>
+        <v>1086463</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3659,10 +3662,10 @@
         <v>39</v>
       </c>
       <c r="G117" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H117" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3673,10 +3676,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D118">
-        <v>18000</v>
+        <v>138600</v>
       </c>
       <c r="E118" t="s">
         <v>21</v>
@@ -3685,10 +3688,10 @@
         <v>39</v>
       </c>
       <c r="G118" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H118" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -3699,10 +3702,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D119">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E119" t="s">
         <v>21</v>
@@ -3711,10 +3714,10 @@
         <v>39</v>
       </c>
       <c r="G119" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H119" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3725,22 +3728,22 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>52763</v>
+        <v>16</v>
       </c>
       <c r="D120">
-        <v>67085064</v>
+        <v>23949</v>
       </c>
       <c r="E120" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F120" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G120" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H120" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3751,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>15</v>
+        <v>53337</v>
       </c>
       <c r="D121">
-        <v>20095</v>
+        <v>67790347</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3763,10 +3766,10 @@
         <v>40</v>
       </c>
       <c r="G121" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H121" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3777,10 +3780,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D122">
-        <v>80699</v>
+        <v>20095</v>
       </c>
       <c r="E122" t="s">
         <v>22</v>
@@ -3789,10 +3792,10 @@
         <v>40</v>
       </c>
       <c r="G122" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H122" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -3803,10 +3806,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="D123">
-        <v>5830</v>
+        <v>80699</v>
       </c>
       <c r="E123" t="s">
         <v>22</v>
@@ -3815,10 +3818,10 @@
         <v>40</v>
       </c>
       <c r="G123" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H123" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3829,10 +3832,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>337</v>
+        <v>5</v>
       </c>
       <c r="D124">
-        <v>496262</v>
+        <v>7330</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
@@ -3841,10 +3844,10 @@
         <v>40</v>
       </c>
       <c r="G124" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H124" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3855,10 +3858,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>3</v>
+        <v>343</v>
       </c>
       <c r="D125">
-        <v>4500</v>
+        <v>505262</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3867,10 +3870,10 @@
         <v>40</v>
       </c>
       <c r="G125" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H125" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3881,10 +3884,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>22206</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>32756705</v>
+        <v>4500</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
@@ -3893,10 +3896,10 @@
         <v>40</v>
       </c>
       <c r="G126" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H126" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -3907,10 +3910,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>14</v>
+        <v>22472</v>
       </c>
       <c r="D127">
-        <v>21000</v>
+        <v>33143865</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3919,10 +3922,10 @@
         <v>40</v>
       </c>
       <c r="G127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H127" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -3933,10 +3936,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>7808</v>
+        <v>14</v>
       </c>
       <c r="D128">
-        <v>11347732</v>
+        <v>21000</v>
       </c>
       <c r="E128" t="s">
         <v>22</v>
@@ -3945,10 +3948,10 @@
         <v>40</v>
       </c>
       <c r="G128" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H128" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3959,10 +3962,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>5</v>
+        <v>7914</v>
       </c>
       <c r="D129">
-        <v>6419</v>
+        <v>11495024</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -3971,10 +3974,10 @@
         <v>40</v>
       </c>
       <c r="G129" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H129" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -3985,10 +3988,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>661</v>
+        <v>5</v>
       </c>
       <c r="D130">
-        <v>929922</v>
+        <v>6419</v>
       </c>
       <c r="E130" t="s">
         <v>22</v>
@@ -3997,10 +4000,10 @@
         <v>40</v>
       </c>
       <c r="G130" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H130" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4011,10 +4014,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>629</v>
+        <v>676</v>
       </c>
       <c r="D131">
-        <v>898625</v>
+        <v>951906</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4023,10 +4026,10 @@
         <v>40</v>
       </c>
       <c r="G131" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H131" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -4037,22 +4040,22 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>139835</v>
+        <v>653</v>
       </c>
       <c r="D132">
-        <v>176409395</v>
+        <v>932216</v>
       </c>
       <c r="E132" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F132" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G132" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H132" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4063,10 +4066,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>60</v>
+        <v>141356</v>
       </c>
       <c r="D133">
-        <v>65576</v>
+        <v>178245911</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4075,10 +4078,10 @@
         <v>41</v>
       </c>
       <c r="G133" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H133" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -4089,10 +4092,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D134">
-        <v>145875</v>
+        <v>66504</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4101,10 +4104,10 @@
         <v>41</v>
       </c>
       <c r="G134" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H134" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -4115,10 +4118,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="D135">
-        <v>8230</v>
+        <v>147375</v>
       </c>
       <c r="E135" t="s">
         <v>23</v>
@@ -4127,10 +4130,10 @@
         <v>41</v>
       </c>
       <c r="G135" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H135" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -4141,10 +4144,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>495</v>
+        <v>3</v>
       </c>
       <c r="D136">
-        <v>728809</v>
+        <v>4500</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
@@ -4153,10 +4156,10 @@
         <v>41</v>
       </c>
       <c r="G136" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="H136" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4167,10 +4170,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D137">
-        <v>4500</v>
+        <v>8230</v>
       </c>
       <c r="E137" t="s">
         <v>23</v>
@@ -4179,10 +4182,10 @@
         <v>41</v>
       </c>
       <c r="G137" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="H137" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4193,10 +4196,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>56345</v>
+        <v>505</v>
       </c>
       <c r="D138">
-        <v>83008400</v>
+        <v>743809</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4205,10 +4208,10 @@
         <v>41</v>
       </c>
       <c r="G138" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H138" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4219,10 +4222,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D139">
-        <v>87295</v>
+        <v>6000</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -4231,10 +4234,10 @@
         <v>41</v>
       </c>
       <c r="G139" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="H139" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4245,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>20024</v>
+        <v>56971</v>
       </c>
       <c r="D140">
-        <v>28977912</v>
+        <v>83919212</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4257,10 +4260,10 @@
         <v>41</v>
       </c>
       <c r="G140" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H140" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4271,10 +4274,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D141">
-        <v>25500</v>
+        <v>87295</v>
       </c>
       <c r="E141" t="s">
         <v>23</v>
@@ -4283,10 +4286,10 @@
         <v>41</v>
       </c>
       <c r="G141" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H141" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4297,10 +4300,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>6</v>
+        <v>20257</v>
       </c>
       <c r="D142">
-        <v>9000</v>
+        <v>29307907</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
@@ -4309,10 +4312,10 @@
         <v>41</v>
       </c>
       <c r="G142" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H142" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4323,10 +4326,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>2658</v>
+        <v>17</v>
       </c>
       <c r="D143">
-        <v>3799905</v>
+        <v>25500</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4335,10 +4338,10 @@
         <v>41</v>
       </c>
       <c r="G143" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H143" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4361,10 +4364,10 @@
         <v>41</v>
       </c>
       <c r="G144" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="H144" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4375,10 +4378,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>1746</v>
+        <v>2718</v>
       </c>
       <c r="D145">
-        <v>2425286</v>
+        <v>3886252</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -4387,10 +4390,10 @@
         <v>41</v>
       </c>
       <c r="G145" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H145" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4401,22 +4404,22 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>150372</v>
+        <v>6</v>
       </c>
       <c r="D146">
-        <v>188079928</v>
+        <v>9000</v>
       </c>
       <c r="E146" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F146" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G146" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H146" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4427,22 +4430,22 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>77</v>
+        <v>1812</v>
       </c>
       <c r="D147">
-        <v>77934</v>
+        <v>2515088</v>
       </c>
       <c r="E147" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F147" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G147" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H147" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4453,22 +4456,22 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="D148">
-        <v>198549</v>
+        <v>3715</v>
       </c>
       <c r="E148" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F148" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G148" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H148" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4479,10 +4482,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>9</v>
+        <v>152054</v>
       </c>
       <c r="D149">
-        <v>12825</v>
+        <v>190109811</v>
       </c>
       <c r="E149" t="s">
         <v>24</v>
@@ -4491,10 +4494,10 @@
         <v>42</v>
       </c>
       <c r="G149" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H149" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4505,10 +4508,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D150">
-        <v>6378</v>
+        <v>77934</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -4517,10 +4520,10 @@
         <v>42</v>
       </c>
       <c r="G150" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H150" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4531,10 +4534,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>339</v>
+        <v>142</v>
       </c>
       <c r="D151">
-        <v>500546</v>
+        <v>203230</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4543,10 +4546,10 @@
         <v>42</v>
       </c>
       <c r="G151" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H151" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4557,10 +4560,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>59836</v>
+        <v>9</v>
       </c>
       <c r="D152">
-        <v>88051993</v>
+        <v>12825</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -4569,10 +4572,10 @@
         <v>42</v>
       </c>
       <c r="G152" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H152" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4583,10 +4586,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D153">
-        <v>69699</v>
+        <v>6378</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
@@ -4595,10 +4598,10 @@
         <v>42</v>
       </c>
       <c r="G153" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H153" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4609,10 +4612,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>6</v>
+        <v>345</v>
       </c>
       <c r="D154">
-        <v>9000</v>
+        <v>509546</v>
       </c>
       <c r="E154" t="s">
         <v>24</v>
@@ -4621,10 +4624,10 @@
         <v>42</v>
       </c>
       <c r="G154" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="H154" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -4635,10 +4638,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>30460</v>
+        <v>4</v>
       </c>
       <c r="D155">
-        <v>44250591</v>
+        <v>6000</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4647,10 +4650,10 @@
         <v>42</v>
       </c>
       <c r="G155" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H155" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4661,10 +4664,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>17</v>
+        <v>60588</v>
       </c>
       <c r="D156">
-        <v>24857</v>
+        <v>89137372</v>
       </c>
       <c r="E156" t="s">
         <v>24</v>
@@ -4673,10 +4676,10 @@
         <v>42</v>
       </c>
       <c r="G156" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H156" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4687,10 +4690,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D157">
-        <v>12160</v>
+        <v>69699</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4699,10 +4702,10 @@
         <v>42</v>
       </c>
       <c r="G157" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H157" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4713,10 +4716,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>2421</v>
+        <v>6</v>
       </c>
       <c r="D158">
-        <v>3413447</v>
+        <v>9000</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4725,10 +4728,10 @@
         <v>42</v>
       </c>
       <c r="G158" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H158" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4739,10 +4742,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>4</v>
+        <v>30839</v>
       </c>
       <c r="D159">
-        <v>6000</v>
+        <v>44796602</v>
       </c>
       <c r="E159" t="s">
         <v>24</v>
@@ -4751,10 +4754,10 @@
         <v>42</v>
       </c>
       <c r="G159" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H159" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -4765,10 +4768,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D160">
-        <v>10500</v>
+        <v>24857</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4777,10 +4780,10 @@
         <v>42</v>
       </c>
       <c r="G160" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="H160" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -4791,10 +4794,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>2063</v>
+        <v>9</v>
       </c>
       <c r="D161">
-        <v>2879493</v>
+        <v>12160</v>
       </c>
       <c r="E161" t="s">
         <v>24</v>
@@ -4803,10 +4806,10 @@
         <v>42</v>
       </c>
       <c r="G161" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H161" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -4817,10 +4820,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>4</v>
+        <v>2467</v>
       </c>
       <c r="D162">
-        <v>6000</v>
+        <v>3479071</v>
       </c>
       <c r="E162" t="s">
         <v>24</v>
@@ -4829,10 +4832,10 @@
         <v>42</v>
       </c>
       <c r="G162" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="H162" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -4843,10 +4846,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D163">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4855,10 +4858,10 @@
         <v>42</v>
       </c>
       <c r="G163" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H163" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -4869,22 +4872,22 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>62325</v>
+        <v>7</v>
       </c>
       <c r="D164">
-        <v>79531223</v>
+        <v>10500</v>
       </c>
       <c r="E164" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F164" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G164" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H164" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -4895,22 +4898,22 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>37</v>
+        <v>2109</v>
       </c>
       <c r="D165">
-        <v>38600</v>
+        <v>2944010</v>
       </c>
       <c r="E165" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F165" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G165" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H165" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -4921,22 +4924,22 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D166">
-        <v>57365</v>
+        <v>6000</v>
       </c>
       <c r="E166" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F166" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G166" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="H166" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -4947,22 +4950,22 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D167">
-        <v>4900</v>
+        <v>7500</v>
       </c>
       <c r="E167" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F167" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G167" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H167" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -4973,10 +4976,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>293</v>
+        <v>62956</v>
       </c>
       <c r="D168">
-        <v>426629</v>
+        <v>80267950</v>
       </c>
       <c r="E168" t="s">
         <v>25</v>
@@ -4985,10 +4988,10 @@
         <v>43</v>
       </c>
       <c r="G168" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H168" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -4999,10 +5002,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>32379</v>
+        <v>37</v>
       </c>
       <c r="D169">
-        <v>47746578</v>
+        <v>38600</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5011,10 +5014,10 @@
         <v>43</v>
       </c>
       <c r="G169" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H169" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -5025,10 +5028,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D170">
-        <v>25649</v>
+        <v>58865</v>
       </c>
       <c r="E170" t="s">
         <v>25</v>
@@ -5037,10 +5040,10 @@
         <v>43</v>
       </c>
       <c r="G170" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H170" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -5051,10 +5054,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>7330</v>
+        <v>4</v>
       </c>
       <c r="D171">
-        <v>10582581</v>
+        <v>4900</v>
       </c>
       <c r="E171" t="s">
         <v>25</v>
@@ -5063,10 +5066,10 @@
         <v>43</v>
       </c>
       <c r="G171" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H171" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -5077,10 +5080,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>4</v>
+        <v>299</v>
       </c>
       <c r="D172">
-        <v>4390</v>
+        <v>435629</v>
       </c>
       <c r="E172" t="s">
         <v>25</v>
@@ -5089,10 +5092,10 @@
         <v>43</v>
       </c>
       <c r="G172" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="H172" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5103,10 +5106,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>1088</v>
+        <v>32788</v>
       </c>
       <c r="D173">
-        <v>1568407</v>
+        <v>48341368</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5115,10 +5118,10 @@
         <v>43</v>
       </c>
       <c r="G173" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H173" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -5129,10 +5132,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D174">
-        <v>2596</v>
+        <v>25649</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5141,10 +5144,10 @@
         <v>43</v>
       </c>
       <c r="G174" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="H174" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5155,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>950</v>
+        <v>7419</v>
       </c>
       <c r="D175">
-        <v>1328503</v>
+        <v>10707063</v>
       </c>
       <c r="E175" t="s">
         <v>25</v>
@@ -5167,10 +5170,10 @@
         <v>43</v>
       </c>
       <c r="G175" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H175" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5181,22 +5184,22 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>147901</v>
+        <v>4</v>
       </c>
       <c r="D176">
-        <v>188436887</v>
+        <v>4390</v>
       </c>
       <c r="E176" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F176" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G176" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H176" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5207,22 +5210,22 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>81</v>
+        <v>1106</v>
       </c>
       <c r="D177">
-        <v>99497</v>
+        <v>1594757</v>
       </c>
       <c r="E177" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F177" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G177" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H177" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5233,22 +5236,22 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>139</v>
+        <v>4</v>
       </c>
       <c r="D178">
-        <v>205062</v>
+        <v>4096</v>
       </c>
       <c r="E178" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F178" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G178" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="H178" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5259,22 +5262,22 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>6</v>
+        <v>981</v>
       </c>
       <c r="D179">
-        <v>9000</v>
+        <v>1372353</v>
       </c>
       <c r="E179" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F179" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G179" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H179" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5285,10 +5288,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>4</v>
+        <v>149708</v>
       </c>
       <c r="D180">
-        <v>6000</v>
+        <v>190661875</v>
       </c>
       <c r="E180" t="s">
         <v>26</v>
@@ -5297,10 +5300,10 @@
         <v>44</v>
       </c>
       <c r="G180" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H180" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5311,10 +5314,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="D181">
-        <v>9981</v>
+        <v>103997</v>
       </c>
       <c r="E181" t="s">
         <v>26</v>
@@ -5323,10 +5326,10 @@
         <v>44</v>
       </c>
       <c r="G181" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="H181" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5337,10 +5340,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>459</v>
+        <v>141</v>
       </c>
       <c r="D182">
-        <v>684838</v>
+        <v>208062</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5349,10 +5352,10 @@
         <v>44</v>
       </c>
       <c r="G182" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H182" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5363,10 +5366,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D183">
-        <v>10500</v>
+        <v>9000</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5375,10 +5378,10 @@
         <v>44</v>
       </c>
       <c r="G183" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H183" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5389,10 +5392,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>60209</v>
+        <v>4</v>
       </c>
       <c r="D184">
-        <v>88780540</v>
+        <v>6000</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5401,10 +5404,10 @@
         <v>44</v>
       </c>
       <c r="G184" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H184" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5415,10 +5418,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D185">
-        <v>77192</v>
+        <v>9981</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5427,10 +5430,10 @@
         <v>44</v>
       </c>
       <c r="G185" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H185" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5441,10 +5444,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>38206</v>
+        <v>471</v>
       </c>
       <c r="D186">
-        <v>55598565</v>
+        <v>701367</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5453,10 +5456,10 @@
         <v>44</v>
       </c>
       <c r="G186" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="H186" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5470,7 +5473,7 @@
         <v>7</v>
       </c>
       <c r="D187">
-        <v>10489</v>
+        <v>10500</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5479,10 +5482,10 @@
         <v>44</v>
       </c>
       <c r="G187" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="H187" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5493,10 +5496,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>1246</v>
+        <v>60988</v>
       </c>
       <c r="D188">
-        <v>1775656</v>
+        <v>89905983</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5505,10 +5508,10 @@
         <v>44</v>
       </c>
       <c r="G188" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H188" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5519,10 +5522,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D189">
-        <v>12000</v>
+        <v>81692</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5531,10 +5534,10 @@
         <v>44</v>
       </c>
       <c r="G189" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="H189" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5545,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>1646</v>
+        <v>38690</v>
       </c>
       <c r="D190">
-        <v>2308424</v>
+        <v>56299016</v>
       </c>
       <c r="E190" t="s">
         <v>26</v>
@@ -5557,10 +5560,10 @@
         <v>44</v>
       </c>
       <c r="G190" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H190" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5571,22 +5574,22 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>230296</v>
+        <v>7</v>
       </c>
       <c r="D191">
-        <v>304381763</v>
+        <v>10489</v>
       </c>
       <c r="E191" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F191" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G191" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H191" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5597,22 +5600,22 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>40</v>
+        <v>1287</v>
       </c>
       <c r="D192">
-        <v>50389</v>
+        <v>1832737</v>
       </c>
       <c r="E192" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F192" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G192" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H192" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5623,22 +5626,22 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="D193">
-        <v>166537</v>
+        <v>12000</v>
       </c>
       <c r="E193" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F193" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G193" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="H193" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5649,22 +5652,22 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>4</v>
+        <v>1729</v>
       </c>
       <c r="D194">
-        <v>6000</v>
+        <v>2427420</v>
       </c>
       <c r="E194" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F194" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G194" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H194" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5675,10 +5678,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>10</v>
+        <v>233290</v>
       </c>
       <c r="D195">
-        <v>14998</v>
+        <v>308134293</v>
       </c>
       <c r="E195" t="s">
         <v>27</v>
@@ -5687,10 +5690,10 @@
         <v>45</v>
       </c>
       <c r="G195" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H195" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5701,10 +5704,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>708</v>
+        <v>40</v>
       </c>
       <c r="D196">
-        <v>1054574</v>
+        <v>50389</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>
@@ -5713,10 +5716,10 @@
         <v>45</v>
       </c>
       <c r="G196" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H196" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5727,10 +5730,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="D197">
-        <v>15716</v>
+        <v>173368</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5739,10 +5742,10 @@
         <v>45</v>
       </c>
       <c r="G197" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="H197" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5753,10 +5756,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>120270</v>
+        <v>4</v>
       </c>
       <c r="D198">
-        <v>177739387</v>
+        <v>6000</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5765,10 +5768,10 @@
         <v>45</v>
       </c>
       <c r="G198" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H198" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5779,10 +5782,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="D199">
-        <v>312880</v>
+        <v>14998</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5791,10 +5794,10 @@
         <v>45</v>
       </c>
       <c r="G199" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H199" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5805,10 +5808,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>6</v>
+        <v>729</v>
       </c>
       <c r="D200">
-        <v>9000</v>
+        <v>1085718</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5817,10 +5820,10 @@
         <v>45</v>
       </c>
       <c r="G200" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="H200" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5831,10 +5834,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>95574</v>
+        <v>11</v>
       </c>
       <c r="D201">
-        <v>139347112</v>
+        <v>15716</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5843,10 +5846,10 @@
         <v>45</v>
       </c>
       <c r="G201" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H201" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5857,10 +5860,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>20</v>
+        <v>121858</v>
       </c>
       <c r="D202">
-        <v>28832</v>
+        <v>180070143</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5869,10 +5872,10 @@
         <v>45</v>
       </c>
       <c r="G202" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H202" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5883,10 +5886,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>1146</v>
+        <v>214</v>
       </c>
       <c r="D203">
-        <v>1613313</v>
+        <v>318880</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5895,10 +5898,10 @@
         <v>45</v>
       </c>
       <c r="G203" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H203" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5909,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D204">
-        <v>4222</v>
+        <v>9000</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5921,10 +5924,10 @@
         <v>45</v>
       </c>
       <c r="G204" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="H204" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5935,10 +5938,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>2129</v>
+        <v>96871</v>
       </c>
       <c r="D205">
-        <v>3023825</v>
+        <v>141225393</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5947,10 +5950,10 @@
         <v>45</v>
       </c>
       <c r="G205" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H205" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5961,10 +5964,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D206">
-        <v>15000</v>
+        <v>28832</v>
       </c>
       <c r="E206" t="s">
         <v>27</v>
@@ -5973,9 +5976,113 @@
         <v>45</v>
       </c>
       <c r="G206" t="s">
+        <v>53</v>
+      </c>
+      <c r="H206" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8">
+      <c r="A207" t="s">
+        <v>8</v>
+      </c>
+      <c r="B207" t="s">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <v>1184</v>
+      </c>
+      <c r="D207">
+        <v>1668054</v>
+      </c>
+      <c r="E207" t="s">
+        <v>27</v>
+      </c>
+      <c r="F207" t="s">
+        <v>45</v>
+      </c>
+      <c r="G207" t="s">
+        <v>55</v>
+      </c>
+      <c r="H207" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208" t="s">
+        <v>8</v>
+      </c>
+      <c r="B208" t="s">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+      <c r="D208">
+        <v>4222</v>
+      </c>
+      <c r="E208" t="s">
+        <v>27</v>
+      </c>
+      <c r="F208" t="s">
+        <v>45</v>
+      </c>
+      <c r="G208" t="s">
+        <v>10</v>
+      </c>
+      <c r="H208" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209">
+        <v>2196</v>
+      </c>
+      <c r="D209">
+        <v>3119516</v>
+      </c>
+      <c r="E209" t="s">
+        <v>27</v>
+      </c>
+      <c r="F209" t="s">
+        <v>45</v>
+      </c>
+      <c r="G209" t="s">
+        <v>57</v>
+      </c>
+      <c r="H209" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
+      <c r="A210" t="s">
+        <v>8</v>
+      </c>
+      <c r="B210" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <v>10</v>
+      </c>
+      <c r="D210">
+        <v>15000</v>
+      </c>
+      <c r="E210" t="s">
+        <v>27</v>
+      </c>
+      <c r="F210" t="s">
+        <v>45</v>
+      </c>
+      <c r="G210" t="s">
         <v>60</v>
       </c>
-      <c r="H206" t="s">
+      <c r="H210" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-20 data (and add past wallis et futuna data)
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="83">
   <si>
     <t>dispositif</t>
   </si>
@@ -620,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>182003</v>
+        <v>183429</v>
       </c>
       <c r="D2">
-        <v>234932654</v>
+        <v>236685431</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -686,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3">
-        <v>166051</v>
+        <v>167551</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -712,10 +712,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D4">
-        <v>258378</v>
+        <v>262878</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -764,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="D6">
-        <v>715592</v>
+        <v>732092</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -816,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>74874</v>
+        <v>75729</v>
       </c>
       <c r="D8">
-        <v>110518434</v>
+        <v>111763182</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -842,10 +842,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9">
-        <v>131790</v>
+        <v>134790</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -868,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>35272</v>
+        <v>35659</v>
       </c>
       <c r="D10">
-        <v>51237215</v>
+        <v>51785123</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -946,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>2008</v>
+        <v>2041</v>
       </c>
       <c r="D13">
-        <v>2859476</v>
+        <v>2908891</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -998,10 +998,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>33100</v>
+        <v>36100</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1024,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2251</v>
+        <v>2329</v>
       </c>
       <c r="D16">
-        <v>3178112</v>
+        <v>3285697</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1050,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>46266</v>
+        <v>46630</v>
       </c>
       <c r="D17">
-        <v>58931553</v>
+        <v>59369943</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1154,10 +1154,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D21">
-        <v>244241</v>
+        <v>245741</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1180,10 +1180,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>21158</v>
+        <v>21415</v>
       </c>
       <c r="D22">
-        <v>31193416</v>
+        <v>31571022</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1232,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>6991</v>
+        <v>7065</v>
       </c>
       <c r="D24">
-        <v>10148656</v>
+        <v>10252818</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1258,10 +1258,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>12638</v>
+        <v>14138</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1284,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>822</v>
+        <v>837</v>
       </c>
       <c r="D26">
-        <v>1156893</v>
+        <v>1178018</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1336,10 +1336,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>691</v>
+        <v>708</v>
       </c>
       <c r="D28">
-        <v>978983</v>
+        <v>1004483</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1362,10 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>59026</v>
+        <v>59481</v>
       </c>
       <c r="D29">
-        <v>75869204</v>
+        <v>76425904</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1414,10 +1414,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31">
-        <v>74544</v>
+        <v>76044</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1440,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="D32">
-        <v>709471</v>
+        <v>743971</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1492,10 +1492,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>29145</v>
+        <v>29467</v>
       </c>
       <c r="D34">
-        <v>43033177</v>
+        <v>43488533</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1544,10 +1544,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5577</v>
+        <v>5619</v>
       </c>
       <c r="D36">
-        <v>8040824</v>
+        <v>8099752</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1596,10 +1596,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>726</v>
+        <v>744</v>
       </c>
       <c r="D38">
-        <v>1016541</v>
+        <v>1040901</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1622,10 +1622,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>737</v>
+        <v>773</v>
       </c>
       <c r="D39">
-        <v>1038582</v>
+        <v>1087853</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1648,10 +1648,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>40771</v>
+        <v>41079</v>
       </c>
       <c r="D40">
-        <v>51832508</v>
+        <v>52210680</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1752,10 +1752,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="D44">
-        <v>289708</v>
+        <v>300208</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1778,10 +1778,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>18214</v>
+        <v>18429</v>
       </c>
       <c r="D45">
-        <v>26869264</v>
+        <v>27183100</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1804,10 +1804,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D46">
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -1830,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6680</v>
+        <v>6748</v>
       </c>
       <c r="D47">
-        <v>9697552</v>
+        <v>9795356</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1856,10 +1856,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="D48">
-        <v>1056110</v>
+        <v>1073906</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1908,10 +1908,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>471</v>
+        <v>500</v>
       </c>
       <c r="D50">
-        <v>666968</v>
+        <v>709848</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -1934,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>11322</v>
+        <v>11432</v>
       </c>
       <c r="D51">
-        <v>14835194</v>
+        <v>14982577</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -2012,10 +2012,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D54">
-        <v>39202</v>
+        <v>40702</v>
       </c>
       <c r="E54" t="s">
         <v>14</v>
@@ -2038,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>4187</v>
+        <v>4219</v>
       </c>
       <c r="D55">
-        <v>6151385</v>
+        <v>6198168</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2064,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2843</v>
+        <v>2874</v>
       </c>
       <c r="D56">
-        <v>4146955</v>
+        <v>4190202</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2090,10 +2090,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D57">
-        <v>327824</v>
+        <v>329324</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2116,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D58">
-        <v>137023</v>
+        <v>141523</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -2142,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>82780</v>
+        <v>83391</v>
       </c>
       <c r="D59">
-        <v>104763489</v>
+        <v>105493501</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2168,10 +2168,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D60">
-        <v>31611</v>
+        <v>33181</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2220,10 +2220,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D62">
-        <v>13500</v>
+        <v>15000</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2246,10 +2246,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D63">
-        <v>329826</v>
+        <v>338636</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2298,10 +2298,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>40984</v>
+        <v>41420</v>
       </c>
       <c r="D65">
-        <v>60544867</v>
+        <v>61179039</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2376,10 +2376,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>18177</v>
+        <v>18331</v>
       </c>
       <c r="D68">
-        <v>26447389</v>
+        <v>26663832</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2428,10 +2428,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1311</v>
+        <v>1339</v>
       </c>
       <c r="D70">
-        <v>1890741</v>
+        <v>1929469</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2454,10 +2454,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>990</v>
+        <v>1019</v>
       </c>
       <c r="D71">
-        <v>1403661</v>
+        <v>1446666</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2480,10 +2480,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>13127</v>
+        <v>13329</v>
       </c>
       <c r="D72">
-        <v>17799604</v>
+        <v>18070819</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2584,10 +2584,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>4166</v>
+        <v>4226</v>
       </c>
       <c r="D76">
-        <v>6144846</v>
+        <v>6234522</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2636,10 +2636,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>3273</v>
+        <v>3311</v>
       </c>
       <c r="D78">
-        <v>4730106</v>
+        <v>4781059</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2688,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D80">
-        <v>261811</v>
+        <v>270811</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2714,10 +2714,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D81">
-        <v>209982</v>
+        <v>211482</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
@@ -2740,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>2779</v>
+        <v>2818</v>
       </c>
       <c r="D82">
-        <v>3828885</v>
+        <v>3879363</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2766,10 +2766,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>826</v>
+        <v>844</v>
       </c>
       <c r="D83">
-        <v>1213864</v>
+        <v>1240864</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2818,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>997</v>
+        <v>1015</v>
       </c>
       <c r="D85">
-        <v>1450871</v>
+        <v>1474516</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2870,10 +2870,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D87">
-        <v>51950</v>
+        <v>53450</v>
       </c>
       <c r="E87" t="s">
         <v>17</v>
@@ -2896,10 +2896,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>84899</v>
+        <v>85485</v>
       </c>
       <c r="D88">
-        <v>106104076</v>
+        <v>106822002</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -3000,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>512</v>
+        <v>525</v>
       </c>
       <c r="D92">
-        <v>758777</v>
+        <v>778277</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3052,10 +3052,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>34865</v>
+        <v>35227</v>
       </c>
       <c r="D94">
-        <v>51399230</v>
+        <v>51929388</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3104,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>16409</v>
+        <v>16571</v>
       </c>
       <c r="D96">
-        <v>23870543</v>
+        <v>24102133</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3130,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>646</v>
+        <v>657</v>
       </c>
       <c r="D97">
-        <v>884720</v>
+        <v>894842</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3156,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>799</v>
+        <v>822</v>
       </c>
       <c r="D98">
-        <v>1124279</v>
+        <v>1157086</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3208,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>24182</v>
+        <v>24397</v>
       </c>
       <c r="D100">
-        <v>32646600</v>
+        <v>32933132</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3234,10 +3234,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D101">
-        <v>14653</v>
+        <v>16153</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -3338,10 +3338,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>8851</v>
+        <v>8933</v>
       </c>
       <c r="D105">
-        <v>13052936</v>
+        <v>13174729</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3364,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>2265</v>
+        <v>2280</v>
       </c>
       <c r="D106">
-        <v>3283169</v>
+        <v>3304566</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3468,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>8806</v>
+        <v>8914</v>
       </c>
       <c r="D110">
-        <v>11742320</v>
+        <v>11883524</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3520,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>4067</v>
+        <v>4104</v>
       </c>
       <c r="D112">
-        <v>5951726</v>
+        <v>6006964</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3546,10 +3546,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>2521</v>
+        <v>2555</v>
       </c>
       <c r="D113">
-        <v>3647288</v>
+        <v>3696231</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3572,10 +3572,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D114">
-        <v>173762</v>
+        <v>175262</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3598,10 +3598,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D115">
-        <v>96018</v>
+        <v>101361</v>
       </c>
       <c r="E115" t="s">
         <v>20</v>
@@ -3624,10 +3624,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>2760</v>
+        <v>2912</v>
       </c>
       <c r="D116">
-        <v>3902662</v>
+        <v>4123230</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3650,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>733</v>
+        <v>752</v>
       </c>
       <c r="D117">
-        <v>1086463</v>
+        <v>1114963</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3676,10 +3676,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D118">
-        <v>138600</v>
+        <v>150600</v>
       </c>
       <c r="E118" t="s">
         <v>21</v>
@@ -3702,10 +3702,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D119">
-        <v>18000</v>
+        <v>19500</v>
       </c>
       <c r="E119" t="s">
         <v>21</v>
@@ -3754,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>53337</v>
+        <v>53705</v>
       </c>
       <c r="D121">
-        <v>67790347</v>
+        <v>68249261</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3858,10 +3858,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="D125">
-        <v>505262</v>
+        <v>526262</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3910,10 +3910,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>22472</v>
+        <v>22712</v>
       </c>
       <c r="D127">
-        <v>33143865</v>
+        <v>33494224</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3936,10 +3936,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D128">
-        <v>21000</v>
+        <v>22500</v>
       </c>
       <c r="E128" t="s">
         <v>22</v>
@@ -3962,10 +3962,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>7914</v>
+        <v>7993</v>
       </c>
       <c r="D129">
-        <v>11495024</v>
+        <v>11606500</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -4014,10 +4014,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="D131">
-        <v>951906</v>
+        <v>966516</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4040,10 +4040,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="D132">
-        <v>932216</v>
+        <v>944216</v>
       </c>
       <c r="E132" t="s">
         <v>22</v>
@@ -4066,10 +4066,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>141356</v>
+        <v>142358</v>
       </c>
       <c r="D133">
-        <v>178245911</v>
+        <v>179459461</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4092,10 +4092,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D134">
-        <v>66504</v>
+        <v>67502</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4196,10 +4196,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="D138">
-        <v>743809</v>
+        <v>755809</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4222,10 +4222,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D139">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -4248,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>56971</v>
+        <v>57534</v>
       </c>
       <c r="D140">
-        <v>83919212</v>
+        <v>84734381</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4300,10 +4300,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>20257</v>
+        <v>3</v>
       </c>
       <c r="D142">
-        <v>29307907</v>
+        <v>4500</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
@@ -4312,10 +4312,10 @@
         <v>41</v>
       </c>
       <c r="G142" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H142" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4326,10 +4326,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>17</v>
+        <v>20424</v>
       </c>
       <c r="D143">
-        <v>25500</v>
+        <v>29543766</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4338,10 +4338,10 @@
         <v>41</v>
       </c>
       <c r="G143" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H143" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4352,10 +4352,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D144">
-        <v>9000</v>
+        <v>25500</v>
       </c>
       <c r="E144" t="s">
         <v>23</v>
@@ -4364,10 +4364,10 @@
         <v>41</v>
       </c>
       <c r="G144" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H144" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4378,10 +4378,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>2718</v>
+        <v>6</v>
       </c>
       <c r="D145">
-        <v>3886252</v>
+        <v>9000</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -4390,10 +4390,10 @@
         <v>41</v>
       </c>
       <c r="G145" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H145" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4404,10 +4404,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>6</v>
+        <v>2765</v>
       </c>
       <c r="D146">
-        <v>9000</v>
+        <v>3955320</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -4416,10 +4416,10 @@
         <v>41</v>
       </c>
       <c r="G146" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H146" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4430,10 +4430,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>1812</v>
+        <v>6</v>
       </c>
       <c r="D147">
-        <v>2515088</v>
+        <v>9000</v>
       </c>
       <c r="E147" t="s">
         <v>23</v>
@@ -4442,10 +4442,10 @@
         <v>41</v>
       </c>
       <c r="G147" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H147" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4456,10 +4456,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>3</v>
+        <v>1875</v>
       </c>
       <c r="D148">
-        <v>3715</v>
+        <v>2604313</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -4468,10 +4468,10 @@
         <v>41</v>
       </c>
       <c r="G148" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H148" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4482,22 +4482,22 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>152054</v>
+        <v>3</v>
       </c>
       <c r="D149">
-        <v>190109811</v>
+        <v>3715</v>
       </c>
       <c r="E149" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F149" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G149" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H149" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4508,10 +4508,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>77</v>
+        <v>153117</v>
       </c>
       <c r="D150">
-        <v>77934</v>
+        <v>191402603</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -4520,10 +4520,10 @@
         <v>42</v>
       </c>
       <c r="G150" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H150" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4534,10 +4534,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="D151">
-        <v>203230</v>
+        <v>77934</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4546,10 +4546,10 @@
         <v>42</v>
       </c>
       <c r="G151" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H151" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4560,10 +4560,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>9</v>
+        <v>143</v>
       </c>
       <c r="D152">
-        <v>12825</v>
+        <v>204730</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -4572,10 +4572,10 @@
         <v>42</v>
       </c>
       <c r="G152" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H152" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4586,10 +4586,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D153">
-        <v>6378</v>
+        <v>12825</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
@@ -4598,10 +4598,10 @@
         <v>42</v>
       </c>
       <c r="G153" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H153" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4612,10 +4612,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>345</v>
+        <v>5</v>
       </c>
       <c r="D154">
-        <v>509546</v>
+        <v>6378</v>
       </c>
       <c r="E154" t="s">
         <v>24</v>
@@ -4624,10 +4624,10 @@
         <v>42</v>
       </c>
       <c r="G154" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H154" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -4638,10 +4638,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>4</v>
+        <v>352</v>
       </c>
       <c r="D155">
-        <v>6000</v>
+        <v>518558</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4650,10 +4650,10 @@
         <v>42</v>
       </c>
       <c r="G155" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H155" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4664,10 +4664,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>60588</v>
+        <v>4</v>
       </c>
       <c r="D156">
-        <v>89137372</v>
+        <v>6000</v>
       </c>
       <c r="E156" t="s">
         <v>24</v>
@@ -4676,10 +4676,10 @@
         <v>42</v>
       </c>
       <c r="G156" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H156" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4690,10 +4690,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>47</v>
+        <v>61310</v>
       </c>
       <c r="D157">
-        <v>69699</v>
+        <v>90188494</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4702,10 +4702,10 @@
         <v>42</v>
       </c>
       <c r="G157" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H157" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4716,10 +4716,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D158">
-        <v>9000</v>
+        <v>71199</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4728,10 +4728,10 @@
         <v>42</v>
       </c>
       <c r="G158" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H158" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4742,10 +4742,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>30839</v>
+        <v>6</v>
       </c>
       <c r="D159">
-        <v>44796602</v>
+        <v>9000</v>
       </c>
       <c r="E159" t="s">
         <v>24</v>
@@ -4754,10 +4754,10 @@
         <v>42</v>
       </c>
       <c r="G159" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H159" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -4768,10 +4768,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>17</v>
+        <v>31120</v>
       </c>
       <c r="D160">
-        <v>24857</v>
+        <v>45201445</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4780,10 +4780,10 @@
         <v>42</v>
       </c>
       <c r="G160" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H160" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -4794,10 +4794,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D161">
-        <v>12160</v>
+        <v>24857</v>
       </c>
       <c r="E161" t="s">
         <v>24</v>
@@ -4806,10 +4806,10 @@
         <v>42</v>
       </c>
       <c r="G161" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H161" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -4820,10 +4820,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>2467</v>
+        <v>9</v>
       </c>
       <c r="D162">
-        <v>3479071</v>
+        <v>12160</v>
       </c>
       <c r="E162" t="s">
         <v>24</v>
@@ -4832,10 +4832,10 @@
         <v>42</v>
       </c>
       <c r="G162" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H162" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -4846,10 +4846,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>4</v>
+        <v>2500</v>
       </c>
       <c r="D163">
-        <v>6000</v>
+        <v>3526819</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4858,10 +4858,10 @@
         <v>42</v>
       </c>
       <c r="G163" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H163" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -4872,10 +4872,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D164">
-        <v>10500</v>
+        <v>6000</v>
       </c>
       <c r="E164" t="s">
         <v>24</v>
@@ -4884,10 +4884,10 @@
         <v>42</v>
       </c>
       <c r="G164" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="H164" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -4898,10 +4898,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>2109</v>
+        <v>7</v>
       </c>
       <c r="D165">
-        <v>2944010</v>
+        <v>10500</v>
       </c>
       <c r="E165" t="s">
         <v>24</v>
@@ -4910,10 +4910,10 @@
         <v>42</v>
       </c>
       <c r="G165" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H165" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -4924,10 +4924,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>4</v>
+        <v>2175</v>
       </c>
       <c r="D166">
-        <v>6000</v>
+        <v>3035042</v>
       </c>
       <c r="E166" t="s">
         <v>24</v>
@@ -4936,10 +4936,10 @@
         <v>42</v>
       </c>
       <c r="G166" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="H166" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -4950,10 +4950,10 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D167">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E167" t="s">
         <v>24</v>
@@ -4962,10 +4962,10 @@
         <v>42</v>
       </c>
       <c r="G167" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="H167" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -4976,22 +4976,22 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>62956</v>
+        <v>5</v>
       </c>
       <c r="D168">
-        <v>80267950</v>
+        <v>7500</v>
       </c>
       <c r="E168" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F168" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G168" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H168" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -5002,10 +5002,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>37</v>
+        <v>63390</v>
       </c>
       <c r="D169">
-        <v>38600</v>
+        <v>80798787</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5014,10 +5014,10 @@
         <v>43</v>
       </c>
       <c r="G169" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H169" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -5028,10 +5028,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D170">
-        <v>58865</v>
+        <v>39470</v>
       </c>
       <c r="E170" t="s">
         <v>25</v>
@@ -5040,10 +5040,10 @@
         <v>43</v>
       </c>
       <c r="G170" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H170" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -5054,10 +5054,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="D171">
-        <v>4900</v>
+        <v>58865</v>
       </c>
       <c r="E171" t="s">
         <v>25</v>
@@ -5066,10 +5066,10 @@
         <v>43</v>
       </c>
       <c r="G171" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H171" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -5080,10 +5080,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>299</v>
+        <v>4</v>
       </c>
       <c r="D172">
-        <v>435629</v>
+        <v>4900</v>
       </c>
       <c r="E172" t="s">
         <v>25</v>
@@ -5092,10 +5092,10 @@
         <v>43</v>
       </c>
       <c r="G172" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="H172" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5106,10 +5106,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>32788</v>
+        <v>305</v>
       </c>
       <c r="D173">
-        <v>48341368</v>
+        <v>444629</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5118,10 +5118,10 @@
         <v>43</v>
       </c>
       <c r="G173" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H173" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -5132,10 +5132,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>18</v>
+        <v>33113</v>
       </c>
       <c r="D174">
-        <v>25649</v>
+        <v>48812855</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5144,10 +5144,10 @@
         <v>43</v>
       </c>
       <c r="G174" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H174" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5158,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>7419</v>
+        <v>18</v>
       </c>
       <c r="D175">
-        <v>10707063</v>
+        <v>25649</v>
       </c>
       <c r="E175" t="s">
         <v>25</v>
@@ -5170,10 +5170,10 @@
         <v>43</v>
       </c>
       <c r="G175" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H175" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5184,10 +5184,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>4</v>
+        <v>7473</v>
       </c>
       <c r="D176">
-        <v>4390</v>
+        <v>10784454</v>
       </c>
       <c r="E176" t="s">
         <v>25</v>
@@ -5196,10 +5196,10 @@
         <v>43</v>
       </c>
       <c r="G176" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H176" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5210,10 +5210,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>1106</v>
+        <v>5</v>
       </c>
       <c r="D177">
-        <v>1594757</v>
+        <v>4798</v>
       </c>
       <c r="E177" t="s">
         <v>25</v>
@@ -5222,10 +5222,10 @@
         <v>43</v>
       </c>
       <c r="G177" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H177" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5236,10 +5236,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>4</v>
+        <v>1131</v>
       </c>
       <c r="D178">
-        <v>4096</v>
+        <v>1629383</v>
       </c>
       <c r="E178" t="s">
         <v>25</v>
@@ -5248,10 +5248,10 @@
         <v>43</v>
       </c>
       <c r="G178" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H178" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5262,10 +5262,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>981</v>
+        <v>4</v>
       </c>
       <c r="D179">
-        <v>1372353</v>
+        <v>4096</v>
       </c>
       <c r="E179" t="s">
         <v>25</v>
@@ -5274,10 +5274,10 @@
         <v>43</v>
       </c>
       <c r="G179" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H179" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5288,22 +5288,22 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>149708</v>
+        <v>1006</v>
       </c>
       <c r="D180">
-        <v>190661875</v>
+        <v>1406651</v>
       </c>
       <c r="E180" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F180" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G180" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H180" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5314,10 +5314,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>84</v>
+        <v>150718</v>
       </c>
       <c r="D181">
-        <v>103997</v>
+        <v>191900396</v>
       </c>
       <c r="E181" t="s">
         <v>26</v>
@@ -5326,10 +5326,10 @@
         <v>44</v>
       </c>
       <c r="G181" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H181" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5340,10 +5340,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="D182">
-        <v>208062</v>
+        <v>112032</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5352,10 +5352,10 @@
         <v>44</v>
       </c>
       <c r="G182" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H182" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5366,10 +5366,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="D183">
-        <v>9000</v>
+        <v>213409</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5378,10 +5378,10 @@
         <v>44</v>
       </c>
       <c r="G183" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H183" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5392,10 +5392,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D184">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5404,10 +5404,10 @@
         <v>44</v>
       </c>
       <c r="G184" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H184" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5418,10 +5418,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D185">
-        <v>9981</v>
+        <v>6000</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5430,10 +5430,10 @@
         <v>44</v>
       </c>
       <c r="G185" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H185" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5444,10 +5444,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>471</v>
+        <v>7</v>
       </c>
       <c r="D186">
-        <v>701367</v>
+        <v>9981</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5456,10 +5456,10 @@
         <v>44</v>
       </c>
       <c r="G186" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H186" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5470,10 +5470,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>480</v>
       </c>
       <c r="D187">
-        <v>10500</v>
+        <v>713799</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5482,10 +5482,10 @@
         <v>44</v>
       </c>
       <c r="G187" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H187" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5496,10 +5496,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>60988</v>
+        <v>7</v>
       </c>
       <c r="D188">
-        <v>89905983</v>
+        <v>10500</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5508,10 +5508,10 @@
         <v>44</v>
       </c>
       <c r="G188" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H188" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5522,10 +5522,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>56</v>
+        <v>61554</v>
       </c>
       <c r="D189">
-        <v>81692</v>
+        <v>90723742</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5534,10 +5534,10 @@
         <v>44</v>
       </c>
       <c r="G189" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H189" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5548,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>38690</v>
+        <v>58</v>
       </c>
       <c r="D190">
-        <v>56299016</v>
+        <v>84692</v>
       </c>
       <c r="E190" t="s">
         <v>26</v>
@@ -5560,10 +5560,10 @@
         <v>44</v>
       </c>
       <c r="G190" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H190" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5574,10 +5574,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>7</v>
+        <v>39061</v>
       </c>
       <c r="D191">
-        <v>10489</v>
+        <v>56829299</v>
       </c>
       <c r="E191" t="s">
         <v>26</v>
@@ -5586,10 +5586,10 @@
         <v>44</v>
       </c>
       <c r="G191" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H191" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5600,10 +5600,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>1287</v>
+        <v>9</v>
       </c>
       <c r="D192">
-        <v>1832737</v>
+        <v>13489</v>
       </c>
       <c r="E192" t="s">
         <v>26</v>
@@ -5612,10 +5612,10 @@
         <v>44</v>
       </c>
       <c r="G192" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H192" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5626,10 +5626,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>8</v>
+        <v>1320</v>
       </c>
       <c r="D193">
-        <v>12000</v>
+        <v>1879971</v>
       </c>
       <c r="E193" t="s">
         <v>26</v>
@@ -5638,10 +5638,10 @@
         <v>44</v>
       </c>
       <c r="G193" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H193" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5652,10 +5652,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>1729</v>
+        <v>8</v>
       </c>
       <c r="D194">
-        <v>2427420</v>
+        <v>12000</v>
       </c>
       <c r="E194" t="s">
         <v>26</v>
@@ -5664,10 +5664,10 @@
         <v>44</v>
       </c>
       <c r="G194" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H194" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5678,22 +5678,22 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>233290</v>
+        <v>1780</v>
       </c>
       <c r="D195">
-        <v>308134293</v>
+        <v>2498956</v>
       </c>
       <c r="E195" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F195" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G195" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H195" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5704,10 +5704,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>40</v>
+        <v>235265</v>
       </c>
       <c r="D196">
-        <v>50389</v>
+        <v>310590722</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>
@@ -5716,10 +5716,10 @@
         <v>45</v>
       </c>
       <c r="G196" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H196" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5730,10 +5730,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="D197">
-        <v>173368</v>
+        <v>51889</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5742,10 +5742,10 @@
         <v>45</v>
       </c>
       <c r="G197" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H197" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5756,10 +5756,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="D198">
-        <v>6000</v>
+        <v>179368</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5768,10 +5768,10 @@
         <v>45</v>
       </c>
       <c r="G198" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H198" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5782,10 +5782,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D199">
-        <v>14998</v>
+        <v>7500</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5794,10 +5794,10 @@
         <v>45</v>
       </c>
       <c r="G199" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H199" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5808,10 +5808,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>729</v>
+        <v>10</v>
       </c>
       <c r="D200">
-        <v>1085718</v>
+        <v>14998</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5820,10 +5820,10 @@
         <v>45</v>
       </c>
       <c r="G200" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H200" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5834,10 +5834,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>11</v>
+        <v>737</v>
       </c>
       <c r="D201">
-        <v>15716</v>
+        <v>1097718</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5846,10 +5846,10 @@
         <v>45</v>
       </c>
       <c r="G201" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H201" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5860,10 +5860,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>121858</v>
+        <v>11</v>
       </c>
       <c r="D202">
-        <v>180070143</v>
+        <v>15716</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5872,10 +5872,10 @@
         <v>45</v>
       </c>
       <c r="G202" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H202" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5886,10 +5886,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>214</v>
+        <v>123162</v>
       </c>
       <c r="D203">
-        <v>318880</v>
+        <v>181973178</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5898,10 +5898,10 @@
         <v>45</v>
       </c>
       <c r="G203" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H203" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5912,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>6</v>
+        <v>214</v>
       </c>
       <c r="D204">
-        <v>9000</v>
+        <v>318880</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5924,10 +5924,10 @@
         <v>45</v>
       </c>
       <c r="G204" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H204" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5938,10 +5938,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>96871</v>
+        <v>7</v>
       </c>
       <c r="D205">
-        <v>141225393</v>
+        <v>10500</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5950,10 +5950,10 @@
         <v>45</v>
       </c>
       <c r="G205" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H205" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5964,10 +5964,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>20</v>
+        <v>97925</v>
       </c>
       <c r="D206">
-        <v>28832</v>
+        <v>142747895</v>
       </c>
       <c r="E206" t="s">
         <v>27</v>
@@ -5976,10 +5976,10 @@
         <v>45</v>
       </c>
       <c r="G206" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H206" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5990,10 +5990,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>1184</v>
+        <v>20</v>
       </c>
       <c r="D207">
-        <v>1668054</v>
+        <v>28832</v>
       </c>
       <c r="E207" t="s">
         <v>27</v>
@@ -6002,10 +6002,10 @@
         <v>45</v>
       </c>
       <c r="G207" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H207" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -6016,10 +6016,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>3</v>
+        <v>1231</v>
       </c>
       <c r="D208">
-        <v>4222</v>
+        <v>1736240</v>
       </c>
       <c r="E208" t="s">
         <v>27</v>
@@ -6028,10 +6028,10 @@
         <v>45</v>
       </c>
       <c r="G208" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H208" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -6042,10 +6042,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>2196</v>
+        <v>3</v>
       </c>
       <c r="D209">
-        <v>3119516</v>
+        <v>4222</v>
       </c>
       <c r="E209" t="s">
         <v>27</v>
@@ -6054,10 +6054,10 @@
         <v>45</v>
       </c>
       <c r="G209" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H209" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -6068,10 +6068,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>10</v>
+        <v>2261</v>
       </c>
       <c r="D210">
-        <v>15000</v>
+        <v>3209569</v>
       </c>
       <c r="E210" t="s">
         <v>27</v>
@@ -6080,9 +6080,35 @@
         <v>45</v>
       </c>
       <c r="G210" t="s">
+        <v>57</v>
+      </c>
+      <c r="H210" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
+      <c r="A211" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <v>10</v>
+      </c>
+      <c r="D211">
+        <v>15000</v>
+      </c>
+      <c r="E211" t="s">
+        <v>27</v>
+      </c>
+      <c r="F211" t="s">
+        <v>45</v>
+      </c>
+      <c r="G211" t="s">
         <v>60</v>
       </c>
-      <c r="H210" t="s">
+      <c r="H211" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-21 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="83">
   <si>
     <t>dispositif</t>
   </si>
@@ -620,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>183429</v>
+        <v>184293</v>
       </c>
       <c r="D2">
-        <v>236685431</v>
+        <v>237729068</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -764,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D6">
-        <v>732092</v>
+        <v>733592</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -816,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>75729</v>
+        <v>76008</v>
       </c>
       <c r="D8">
-        <v>111763182</v>
+        <v>112165093</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -842,10 +842,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9">
-        <v>134790</v>
+        <v>136290</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -868,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>35659</v>
+        <v>35830</v>
       </c>
       <c r="D10">
-        <v>51785123</v>
+        <v>52030243</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -946,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>2041</v>
+        <v>2049</v>
       </c>
       <c r="D13">
-        <v>2908891</v>
+        <v>2920191</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1024,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2329</v>
+        <v>2350</v>
       </c>
       <c r="D16">
-        <v>3285697</v>
+        <v>3313213</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1050,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>46630</v>
+        <v>46792</v>
       </c>
       <c r="D17">
-        <v>59369943</v>
+        <v>59555967</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1180,10 +1180,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>21415</v>
+        <v>21493</v>
       </c>
       <c r="D22">
-        <v>31571022</v>
+        <v>31679878</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1232,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>7065</v>
+        <v>7106</v>
       </c>
       <c r="D24">
-        <v>10252818</v>
+        <v>10311308</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1284,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="D26">
-        <v>1178018</v>
+        <v>1184491</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1336,10 +1336,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="D28">
-        <v>1004483</v>
+        <v>1008983</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1362,10 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>59481</v>
+        <v>59685</v>
       </c>
       <c r="D29">
-        <v>76425904</v>
+        <v>76661880</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1440,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D32">
-        <v>743971</v>
+        <v>746971</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1492,10 +1492,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>29467</v>
+        <v>29569</v>
       </c>
       <c r="D34">
-        <v>43488533</v>
+        <v>43637478</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1518,10 +1518,10 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35">
-        <v>17950</v>
+        <v>19450</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -1544,10 +1544,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5619</v>
+        <v>5634</v>
       </c>
       <c r="D36">
-        <v>8099752</v>
+        <v>8121407</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1596,10 +1596,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="D38">
-        <v>1040901</v>
+        <v>1048530</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1622,10 +1622,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>773</v>
+        <v>784</v>
       </c>
       <c r="D39">
-        <v>1087853</v>
+        <v>1104353</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1648,10 +1648,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>41079</v>
+        <v>41251</v>
       </c>
       <c r="D40">
-        <v>52210680</v>
+        <v>52417648</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1700,10 +1700,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D42">
-        <v>33472</v>
+        <v>34972</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -1778,10 +1778,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>18429</v>
+        <v>18522</v>
       </c>
       <c r="D45">
-        <v>27183100</v>
+        <v>27317010</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1830,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6748</v>
+        <v>6770</v>
       </c>
       <c r="D47">
-        <v>9795356</v>
+        <v>9827790</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1856,10 +1856,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="D48">
-        <v>1073906</v>
+        <v>1079756</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1908,10 +1908,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="D50">
-        <v>709848</v>
+        <v>719568</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -1934,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>11432</v>
+        <v>11492</v>
       </c>
       <c r="D51">
-        <v>14982577</v>
+        <v>15055669</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -1960,10 +1960,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>17827</v>
+        <v>19327</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
@@ -2038,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>4219</v>
+        <v>4231</v>
       </c>
       <c r="D55">
-        <v>6198168</v>
+        <v>6215560</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2064,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2874</v>
+        <v>2896</v>
       </c>
       <c r="D56">
-        <v>4190202</v>
+        <v>4221047</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2116,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D58">
-        <v>141523</v>
+        <v>143023</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -2142,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>83391</v>
+        <v>83746</v>
       </c>
       <c r="D59">
-        <v>105493501</v>
+        <v>105917268</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2298,10 +2298,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>41420</v>
+        <v>41558</v>
       </c>
       <c r="D65">
-        <v>61179039</v>
+        <v>61381053</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2376,10 +2376,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>18331</v>
+        <v>18403</v>
       </c>
       <c r="D68">
-        <v>26663832</v>
+        <v>26763784</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2428,10 +2428,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1339</v>
+        <v>1348</v>
       </c>
       <c r="D70">
-        <v>1929469</v>
+        <v>1942969</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2454,10 +2454,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>1019</v>
+        <v>1028</v>
       </c>
       <c r="D71">
-        <v>1446666</v>
+        <v>1457852</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2480,10 +2480,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>13329</v>
+        <v>13542</v>
       </c>
       <c r="D72">
-        <v>18070819</v>
+        <v>18358361</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2584,10 +2584,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>4226</v>
+        <v>4259</v>
       </c>
       <c r="D76">
-        <v>6234522</v>
+        <v>6282442</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2636,10 +2636,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>3311</v>
+        <v>3333</v>
       </c>
       <c r="D78">
-        <v>4781059</v>
+        <v>4813815</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2688,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D80">
-        <v>270811</v>
+        <v>278311</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2714,10 +2714,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D81">
-        <v>211482</v>
+        <v>217482</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
@@ -2740,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>2818</v>
+        <v>2873</v>
       </c>
       <c r="D82">
-        <v>3879363</v>
+        <v>3953810</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2766,10 +2766,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="D83">
-        <v>1240864</v>
+        <v>1247754</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2818,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>1015</v>
+        <v>1026</v>
       </c>
       <c r="D85">
-        <v>1474516</v>
+        <v>1491016</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2870,10 +2870,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D87">
-        <v>53450</v>
+        <v>54950</v>
       </c>
       <c r="E87" t="s">
         <v>17</v>
@@ -2896,10 +2896,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>85485</v>
+        <v>85819</v>
       </c>
       <c r="D88">
-        <v>106822002</v>
+        <v>107204519</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -3000,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D92">
-        <v>778277</v>
+        <v>782777</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3052,10 +3052,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>35227</v>
+        <v>35336</v>
       </c>
       <c r="D94">
-        <v>51929388</v>
+        <v>52089582</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3104,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>16571</v>
+        <v>16629</v>
       </c>
       <c r="D96">
-        <v>24102133</v>
+        <v>24188093</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3130,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D97">
-        <v>894842</v>
+        <v>899342</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3156,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="D98">
-        <v>1157086</v>
+        <v>1166892</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3208,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>24397</v>
+        <v>24545</v>
       </c>
       <c r="D100">
-        <v>32933132</v>
+        <v>33130177</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3338,10 +3338,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>8933</v>
+        <v>8976</v>
       </c>
       <c r="D105">
-        <v>13174729</v>
+        <v>13236125</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3364,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>2280</v>
+        <v>2291</v>
       </c>
       <c r="D106">
-        <v>3304566</v>
+        <v>3320096</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3442,10 +3442,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D109">
-        <v>212066</v>
+        <v>215066</v>
       </c>
       <c r="E109" t="s">
         <v>19</v>
@@ -3468,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>8914</v>
+        <v>8997</v>
       </c>
       <c r="D110">
-        <v>11883524</v>
+        <v>11988811</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3520,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>4104</v>
+        <v>4137</v>
       </c>
       <c r="D112">
-        <v>6006964</v>
+        <v>6054347</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3546,10 +3546,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>2555</v>
+        <v>2581</v>
       </c>
       <c r="D113">
-        <v>3696231</v>
+        <v>3734785</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3572,10 +3572,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D114">
-        <v>175262</v>
+        <v>176762</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3624,10 +3624,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>2912</v>
+        <v>3012</v>
       </c>
       <c r="D116">
-        <v>4123230</v>
+        <v>4265629</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3650,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>752</v>
+        <v>763</v>
       </c>
       <c r="D117">
-        <v>1114963</v>
+        <v>1130943</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3754,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>53705</v>
+        <v>53911</v>
       </c>
       <c r="D121">
-        <v>68249261</v>
+        <v>68495760</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3858,10 +3858,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D125">
-        <v>526262</v>
+        <v>530762</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3910,10 +3910,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>22712</v>
+        <v>22792</v>
       </c>
       <c r="D127">
-        <v>33494224</v>
+        <v>33611301</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3962,10 +3962,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>7993</v>
+        <v>8027</v>
       </c>
       <c r="D129">
-        <v>11606500</v>
+        <v>11654882</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -4014,10 +4014,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D131">
-        <v>966516</v>
+        <v>970931</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4040,10 +4040,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="D132">
-        <v>944216</v>
+        <v>950640</v>
       </c>
       <c r="E132" t="s">
         <v>22</v>
@@ -4066,10 +4066,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>142358</v>
+        <v>143019</v>
       </c>
       <c r="D133">
-        <v>179459461</v>
+        <v>180237543</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4196,10 +4196,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D138">
-        <v>755809</v>
+        <v>757559</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4248,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>57534</v>
+        <v>57744</v>
       </c>
       <c r="D140">
-        <v>84734381</v>
+        <v>85035460</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4326,10 +4326,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>20424</v>
+        <v>20510</v>
       </c>
       <c r="D143">
-        <v>29543766</v>
+        <v>29662868</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4404,10 +4404,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>2765</v>
+        <v>2785</v>
       </c>
       <c r="D146">
-        <v>3955320</v>
+        <v>3983212</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -4456,10 +4456,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>1875</v>
+        <v>1891</v>
       </c>
       <c r="D148">
-        <v>2604313</v>
+        <v>2627926</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -4508,10 +4508,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>153117</v>
+        <v>153693</v>
       </c>
       <c r="D150">
-        <v>191402603</v>
+        <v>192065911</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -4534,10 +4534,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D151">
-        <v>77934</v>
+        <v>78412</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4638,10 +4638,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D155">
-        <v>518558</v>
+        <v>521558</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4690,10 +4690,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>61310</v>
+        <v>61563</v>
       </c>
       <c r="D157">
-        <v>90188494</v>
+        <v>90556873</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4716,10 +4716,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D158">
-        <v>71199</v>
+        <v>74199</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4768,10 +4768,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>31120</v>
+        <v>31252</v>
       </c>
       <c r="D160">
-        <v>45201445</v>
+        <v>45387390</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4846,10 +4846,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>2500</v>
+        <v>2506</v>
       </c>
       <c r="D163">
-        <v>3526819</v>
+        <v>3534722</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4924,10 +4924,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>2175</v>
+        <v>2188</v>
       </c>
       <c r="D166">
-        <v>3035042</v>
+        <v>3052267</v>
       </c>
       <c r="E166" t="s">
         <v>24</v>
@@ -5002,10 +5002,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>63390</v>
+        <v>63608</v>
       </c>
       <c r="D169">
-        <v>80798787</v>
+        <v>81046127</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5106,10 +5106,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="D173">
-        <v>444629</v>
+        <v>453629</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5132,10 +5132,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>33113</v>
+        <v>3</v>
       </c>
       <c r="D174">
-        <v>48812855</v>
+        <v>2113</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5144,10 +5144,10 @@
         <v>43</v>
       </c>
       <c r="G174" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H174" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5158,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>18</v>
+        <v>33217</v>
       </c>
       <c r="D175">
-        <v>25649</v>
+        <v>48963243</v>
       </c>
       <c r="E175" t="s">
         <v>25</v>
@@ -5170,10 +5170,10 @@
         <v>43</v>
       </c>
       <c r="G175" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H175" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5184,10 +5184,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>7473</v>
+        <v>18</v>
       </c>
       <c r="D176">
-        <v>10784454</v>
+        <v>25649</v>
       </c>
       <c r="E176" t="s">
         <v>25</v>
@@ -5196,10 +5196,10 @@
         <v>43</v>
       </c>
       <c r="G176" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H176" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5210,10 +5210,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>5</v>
+        <v>7501</v>
       </c>
       <c r="D177">
-        <v>4798</v>
+        <v>10823309</v>
       </c>
       <c r="E177" t="s">
         <v>25</v>
@@ -5222,10 +5222,10 @@
         <v>43</v>
       </c>
       <c r="G177" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H177" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5236,10 +5236,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>1131</v>
+        <v>5</v>
       </c>
       <c r="D178">
-        <v>1629383</v>
+        <v>4798</v>
       </c>
       <c r="E178" t="s">
         <v>25</v>
@@ -5248,10 +5248,10 @@
         <v>43</v>
       </c>
       <c r="G178" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H178" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5262,10 +5262,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>4</v>
+        <v>1135</v>
       </c>
       <c r="D179">
-        <v>4096</v>
+        <v>1635383</v>
       </c>
       <c r="E179" t="s">
         <v>25</v>
@@ -5274,10 +5274,10 @@
         <v>43</v>
       </c>
       <c r="G179" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H179" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5288,10 +5288,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>1006</v>
+        <v>4</v>
       </c>
       <c r="D180">
-        <v>1406651</v>
+        <v>4096</v>
       </c>
       <c r="E180" t="s">
         <v>25</v>
@@ -5300,10 +5300,10 @@
         <v>43</v>
       </c>
       <c r="G180" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H180" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5314,22 +5314,22 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>150718</v>
+        <v>1010</v>
       </c>
       <c r="D181">
-        <v>191900396</v>
+        <v>1412651</v>
       </c>
       <c r="E181" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F181" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G181" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H181" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5340,10 +5340,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>91</v>
+        <v>151445</v>
       </c>
       <c r="D182">
-        <v>112032</v>
+        <v>192764493</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5352,10 +5352,10 @@
         <v>44</v>
       </c>
       <c r="G182" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H182" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5366,10 +5366,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D183">
-        <v>213409</v>
+        <v>112032</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5378,10 +5378,10 @@
         <v>44</v>
       </c>
       <c r="G183" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H183" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5392,10 +5392,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="D184">
-        <v>9000</v>
+        <v>213409</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5404,10 +5404,10 @@
         <v>44</v>
       </c>
       <c r="G184" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H184" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5418,10 +5418,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D185">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5430,10 +5430,10 @@
         <v>44</v>
       </c>
       <c r="G185" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H185" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5444,10 +5444,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D186">
-        <v>9981</v>
+        <v>6000</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5456,10 +5456,10 @@
         <v>44</v>
       </c>
       <c r="G186" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H186" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5470,10 +5470,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>480</v>
+        <v>7</v>
       </c>
       <c r="D187">
-        <v>713799</v>
+        <v>9981</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5482,10 +5482,10 @@
         <v>44</v>
       </c>
       <c r="G187" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H187" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5496,10 +5496,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>7</v>
+        <v>485</v>
       </c>
       <c r="D188">
-        <v>10500</v>
+        <v>721299</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5508,10 +5508,10 @@
         <v>44</v>
       </c>
       <c r="G188" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H188" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5522,10 +5522,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>61554</v>
+        <v>7</v>
       </c>
       <c r="D189">
-        <v>90723742</v>
+        <v>10500</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5534,10 +5534,10 @@
         <v>44</v>
       </c>
       <c r="G189" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H189" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5548,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>58</v>
+        <v>61822</v>
       </c>
       <c r="D190">
-        <v>84692</v>
+        <v>91109826</v>
       </c>
       <c r="E190" t="s">
         <v>26</v>
@@ -5560,10 +5560,10 @@
         <v>44</v>
       </c>
       <c r="G190" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H190" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5574,10 +5574,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>39061</v>
+        <v>58</v>
       </c>
       <c r="D191">
-        <v>56829299</v>
+        <v>84692</v>
       </c>
       <c r="E191" t="s">
         <v>26</v>
@@ -5586,10 +5586,10 @@
         <v>44</v>
       </c>
       <c r="G191" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H191" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5600,10 +5600,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>9</v>
+        <v>39234</v>
       </c>
       <c r="D192">
-        <v>13489</v>
+        <v>57069535</v>
       </c>
       <c r="E192" t="s">
         <v>26</v>
@@ -5612,10 +5612,10 @@
         <v>44</v>
       </c>
       <c r="G192" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H192" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5626,10 +5626,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>1320</v>
+        <v>9</v>
       </c>
       <c r="D193">
-        <v>1879971</v>
+        <v>13489</v>
       </c>
       <c r="E193" t="s">
         <v>26</v>
@@ -5638,10 +5638,10 @@
         <v>44</v>
       </c>
       <c r="G193" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H193" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5652,10 +5652,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>8</v>
+        <v>1326</v>
       </c>
       <c r="D194">
-        <v>12000</v>
+        <v>1888321</v>
       </c>
       <c r="E194" t="s">
         <v>26</v>
@@ -5664,10 +5664,10 @@
         <v>44</v>
       </c>
       <c r="G194" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H194" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5678,10 +5678,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>1780</v>
+        <v>8</v>
       </c>
       <c r="D195">
-        <v>2498956</v>
+        <v>12000</v>
       </c>
       <c r="E195" t="s">
         <v>26</v>
@@ -5690,10 +5690,10 @@
         <v>44</v>
       </c>
       <c r="G195" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H195" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5704,22 +5704,22 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>235265</v>
+        <v>1800</v>
       </c>
       <c r="D196">
-        <v>310590722</v>
+        <v>2528117</v>
       </c>
       <c r="E196" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F196" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G196" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H196" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5730,10 +5730,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>41</v>
+        <v>236745</v>
       </c>
       <c r="D197">
-        <v>51889</v>
+        <v>312445967</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5742,10 +5742,10 @@
         <v>45</v>
       </c>
       <c r="G197" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H197" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5756,10 +5756,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="D198">
-        <v>179368</v>
+        <v>51889</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5768,10 +5768,10 @@
         <v>45</v>
       </c>
       <c r="G198" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H198" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5782,10 +5782,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="D199">
-        <v>7500</v>
+        <v>179818</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5794,10 +5794,10 @@
         <v>45</v>
       </c>
       <c r="G199" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H199" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5808,10 +5808,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D200">
-        <v>14998</v>
+        <v>7500</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5820,10 +5820,10 @@
         <v>45</v>
       </c>
       <c r="G200" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H200" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5834,10 +5834,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>737</v>
+        <v>10</v>
       </c>
       <c r="D201">
-        <v>1097718</v>
+        <v>14998</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5846,10 +5846,10 @@
         <v>45</v>
       </c>
       <c r="G201" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H201" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5860,10 +5860,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>11</v>
+        <v>739</v>
       </c>
       <c r="D202">
-        <v>15716</v>
+        <v>1100718</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5872,10 +5872,10 @@
         <v>45</v>
       </c>
       <c r="G202" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H202" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5886,10 +5886,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>123162</v>
+        <v>11</v>
       </c>
       <c r="D203">
-        <v>181973178</v>
+        <v>15716</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5898,10 +5898,10 @@
         <v>45</v>
       </c>
       <c r="G203" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H203" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5912,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>214</v>
+        <v>123841</v>
       </c>
       <c r="D204">
-        <v>318880</v>
+        <v>182959971</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5924,10 +5924,10 @@
         <v>45</v>
       </c>
       <c r="G204" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H204" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5938,10 +5938,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D205">
-        <v>10500</v>
+        <v>320380</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5950,10 +5950,10 @@
         <v>45</v>
       </c>
       <c r="G205" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H205" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5964,10 +5964,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>97925</v>
+        <v>7</v>
       </c>
       <c r="D206">
-        <v>142747895</v>
+        <v>10500</v>
       </c>
       <c r="E206" t="s">
         <v>27</v>
@@ -5976,10 +5976,10 @@
         <v>45</v>
       </c>
       <c r="G206" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H206" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5990,10 +5990,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>20</v>
+        <v>98550</v>
       </c>
       <c r="D207">
-        <v>28832</v>
+        <v>143653418</v>
       </c>
       <c r="E207" t="s">
         <v>27</v>
@@ -6002,10 +6002,10 @@
         <v>45</v>
       </c>
       <c r="G207" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H207" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -6016,10 +6016,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>1231</v>
+        <v>20</v>
       </c>
       <c r="D208">
-        <v>1736240</v>
+        <v>28832</v>
       </c>
       <c r="E208" t="s">
         <v>27</v>
@@ -6028,10 +6028,10 @@
         <v>45</v>
       </c>
       <c r="G208" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H208" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -6042,10 +6042,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>3</v>
+        <v>1240</v>
       </c>
       <c r="D209">
-        <v>4222</v>
+        <v>1749099</v>
       </c>
       <c r="E209" t="s">
         <v>27</v>
@@ -6054,10 +6054,10 @@
         <v>45</v>
       </c>
       <c r="G209" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H209" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -6068,10 +6068,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>2261</v>
+        <v>3</v>
       </c>
       <c r="D210">
-        <v>3209569</v>
+        <v>4222</v>
       </c>
       <c r="E210" t="s">
         <v>27</v>
@@ -6080,10 +6080,10 @@
         <v>45</v>
       </c>
       <c r="G210" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H210" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -6094,10 +6094,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>10</v>
+        <v>2291</v>
       </c>
       <c r="D211">
-        <v>15000</v>
+        <v>3248922</v>
       </c>
       <c r="E211" t="s">
         <v>27</v>
@@ -6106,9 +6106,35 @@
         <v>45</v>
       </c>
       <c r="G211" t="s">
+        <v>57</v>
+      </c>
+      <c r="H211" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8">
+      <c r="A212" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212" t="s">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <v>10</v>
+      </c>
+      <c r="D212">
+        <v>15000</v>
+      </c>
+      <c r="E212" t="s">
+        <v>27</v>
+      </c>
+      <c r="F212" t="s">
+        <v>45</v>
+      </c>
+      <c r="G212" t="s">
         <v>60</v>
       </c>
-      <c r="H211" t="s">
+      <c r="H212" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-23 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -660,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>184639</v>
+        <v>185295</v>
       </c>
       <c r="D2">
-        <v>238151732</v>
+        <v>238956444</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -764,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="D6">
-        <v>737537</v>
+        <v>744414</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -816,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>76163</v>
+        <v>76513</v>
       </c>
       <c r="D8">
-        <v>112389534</v>
+        <v>112899229</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -868,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>35910</v>
+        <v>36118</v>
       </c>
       <c r="D10">
-        <v>52144147</v>
+        <v>52445295</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -946,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>2054</v>
+        <v>2069</v>
       </c>
       <c r="D13">
-        <v>2926526</v>
+        <v>2948472</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1024,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2355</v>
+        <v>2380</v>
       </c>
       <c r="D16">
-        <v>3319813</v>
+        <v>3353634</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1050,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>46861</v>
+        <v>47038</v>
       </c>
       <c r="D17">
-        <v>59639843</v>
+        <v>59832863</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1102,10 +1102,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>30000</v>
+        <v>30563</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1154,10 +1154,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D21">
-        <v>245741</v>
+        <v>247241</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1180,10 +1180,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>21548</v>
+        <v>21669</v>
       </c>
       <c r="D22">
-        <v>31758151</v>
+        <v>31935155</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1232,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>7124</v>
+        <v>7162</v>
       </c>
       <c r="D24">
-        <v>10338308</v>
+        <v>10391888</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1284,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D26">
-        <v>1187491</v>
+        <v>1188028</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1336,10 +1336,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="D28">
-        <v>1011983</v>
+        <v>1023983</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1362,10 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>59785</v>
+        <v>60009</v>
       </c>
       <c r="D29">
-        <v>76794305</v>
+        <v>77058224</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1388,10 +1388,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D30">
-        <v>34462</v>
+        <v>37462</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -1440,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="D32">
-        <v>751471</v>
+        <v>758971</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1492,10 +1492,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>29637</v>
+        <v>29765</v>
       </c>
       <c r="D34">
-        <v>43736700</v>
+        <v>43921013</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1544,10 +1544,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5641</v>
+        <v>5661</v>
       </c>
       <c r="D36">
-        <v>8131907</v>
+        <v>8159694</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1596,10 +1596,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>753</v>
+        <v>761</v>
       </c>
       <c r="D38">
-        <v>1050945</v>
+        <v>1062945</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1622,10 +1622,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="D39">
-        <v>1108671</v>
+        <v>1114671</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1648,10 +1648,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>41307</v>
+        <v>41449</v>
       </c>
       <c r="D40">
-        <v>52487377</v>
+        <v>52652896</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1674,10 +1674,10 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D41">
-        <v>13095</v>
+        <v>14595</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -1752,10 +1752,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D44">
-        <v>300208</v>
+        <v>303208</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1778,10 +1778,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>18563</v>
+        <v>18661</v>
       </c>
       <c r="D45">
-        <v>27375187</v>
+        <v>27516106</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1830,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6785</v>
+        <v>6809</v>
       </c>
       <c r="D47">
-        <v>9849141</v>
+        <v>9883782</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1856,10 +1856,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>770</v>
+        <v>775</v>
       </c>
       <c r="D48">
-        <v>1079756</v>
+        <v>1086606</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1908,10 +1908,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="D50">
-        <v>723768</v>
+        <v>729983</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -1934,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>11514</v>
+        <v>11565</v>
       </c>
       <c r="D51">
-        <v>15085946</v>
+        <v>15154115</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -2038,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>4247</v>
+        <v>4280</v>
       </c>
       <c r="D55">
-        <v>6235424</v>
+        <v>6282849</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2064,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2899</v>
+        <v>2907</v>
       </c>
       <c r="D56">
-        <v>4225547</v>
+        <v>4236301</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2090,10 +2090,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D57">
-        <v>329324</v>
+        <v>339625</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2116,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D58">
-        <v>143023</v>
+        <v>146116</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -2142,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>83903</v>
+        <v>84258</v>
       </c>
       <c r="D59">
-        <v>106100949</v>
+        <v>106517955</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2246,10 +2246,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D63">
-        <v>338636</v>
+        <v>341636</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2298,10 +2298,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>41677</v>
+        <v>41983</v>
       </c>
       <c r="D65">
-        <v>61547988</v>
+        <v>61986095</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2324,10 +2324,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D66">
-        <v>68174</v>
+        <v>69674</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2376,10 +2376,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>18463</v>
+        <v>18578</v>
       </c>
       <c r="D68">
-        <v>26847621</v>
+        <v>27013388</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2428,10 +2428,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1351</v>
+        <v>1363</v>
       </c>
       <c r="D70">
-        <v>1946279</v>
+        <v>1962434</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2454,10 +2454,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="D71">
-        <v>1466852</v>
+        <v>1472682</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2480,10 +2480,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>13636</v>
+        <v>13769</v>
       </c>
       <c r="D72">
-        <v>18487120</v>
+        <v>18660209</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2584,10 +2584,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>4266</v>
+        <v>4303</v>
       </c>
       <c r="D76">
-        <v>6291862</v>
+        <v>6346768</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2636,10 +2636,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>3354</v>
+        <v>3385</v>
       </c>
       <c r="D78">
-        <v>4844868</v>
+        <v>4887719</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2688,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D80">
-        <v>281311</v>
+        <v>284311</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2714,10 +2714,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D81">
-        <v>217482</v>
+        <v>230982</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
@@ -2740,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>2884</v>
+        <v>2915</v>
       </c>
       <c r="D82">
-        <v>3970010</v>
+        <v>4012786</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2766,10 +2766,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>853</v>
+        <v>862</v>
       </c>
       <c r="D83">
-        <v>1253754</v>
+        <v>1267254</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2818,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>1034</v>
+        <v>1049</v>
       </c>
       <c r="D85">
-        <v>1503016</v>
+        <v>1524552</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2896,10 +2896,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>85964</v>
+        <v>86277</v>
       </c>
       <c r="D88">
-        <v>107396946</v>
+        <v>107763342</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -2948,10 +2948,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D90">
-        <v>57561</v>
+        <v>59061</v>
       </c>
       <c r="E90" t="s">
         <v>18</v>
@@ -3000,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="D92">
-        <v>787277</v>
+        <v>796277</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3052,10 +3052,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>35420</v>
+        <v>35613</v>
       </c>
       <c r="D94">
-        <v>52209709</v>
+        <v>52491684</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3104,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>16664</v>
+        <v>16760</v>
       </c>
       <c r="D96">
-        <v>24235235</v>
+        <v>24370536</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3130,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D97">
-        <v>906842</v>
+        <v>910382</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3156,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>836</v>
+        <v>847</v>
       </c>
       <c r="D98">
-        <v>1176491</v>
+        <v>1191872</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3208,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>24638</v>
+        <v>24768</v>
       </c>
       <c r="D100">
-        <v>33256848</v>
+        <v>33430461</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3312,10 +3312,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D104">
-        <v>472500</v>
+        <v>474000</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -3338,10 +3338,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>9009</v>
+        <v>9047</v>
       </c>
       <c r="D105">
-        <v>13284682</v>
+        <v>13340314</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3364,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>2300</v>
+        <v>2304</v>
       </c>
       <c r="D106">
-        <v>3333482</v>
+        <v>3338722</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3416,10 +3416,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D108">
-        <v>297215</v>
+        <v>300215</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -3442,10 +3442,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D109">
-        <v>216566</v>
+        <v>217288</v>
       </c>
       <c r="E109" t="s">
         <v>19</v>
@@ -3468,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>9016</v>
+        <v>9062</v>
       </c>
       <c r="D110">
-        <v>12014981</v>
+        <v>12078830</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3520,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>4147</v>
+        <v>4156</v>
       </c>
       <c r="D112">
-        <v>6069347</v>
+        <v>6082127</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3546,10 +3546,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>2588</v>
+        <v>2599</v>
       </c>
       <c r="D113">
-        <v>3743585</v>
+        <v>3757705</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3572,10 +3572,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D114">
-        <v>176762</v>
+        <v>180513</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3624,10 +3624,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>3036</v>
+        <v>3045</v>
       </c>
       <c r="D116">
-        <v>4300309</v>
+        <v>4313809</v>
       </c>
       <c r="E116" t="s">
         <v>21</v>
@@ -3650,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>767</v>
+        <v>775</v>
       </c>
       <c r="D117">
-        <v>1136943</v>
+        <v>1148943</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3676,10 +3676,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D118">
-        <v>150600</v>
+        <v>156600</v>
       </c>
       <c r="E118" t="s">
         <v>21</v>
@@ -3728,10 +3728,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D120">
-        <v>23949</v>
+        <v>26949</v>
       </c>
       <c r="E120" t="s">
         <v>21</v>
@@ -3754,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>54001</v>
+        <v>54210</v>
       </c>
       <c r="D121">
-        <v>68611480</v>
+        <v>68863412</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3858,10 +3858,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D125">
-        <v>532262</v>
+        <v>536762</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3910,10 +3910,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>22844</v>
+        <v>22993</v>
       </c>
       <c r="D127">
-        <v>33687139</v>
+        <v>33905865</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3962,10 +3962,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>8046</v>
+        <v>8095</v>
       </c>
       <c r="D129">
-        <v>11681847</v>
+        <v>11753126</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -4014,10 +4014,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D131">
-        <v>973931</v>
+        <v>976931</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4040,10 +4040,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="D132">
-        <v>952140</v>
+        <v>959426</v>
       </c>
       <c r="E132" t="s">
         <v>22</v>
@@ -4066,10 +4066,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>143252</v>
+        <v>143767</v>
       </c>
       <c r="D133">
-        <v>180513755</v>
+        <v>181133519</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -4092,10 +4092,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D134">
-        <v>67502</v>
+        <v>68835</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4196,10 +4196,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D138">
-        <v>759059</v>
+        <v>762059</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4222,10 +4222,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D139">
-        <v>7500</v>
+        <v>8383</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -4248,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>57854</v>
+        <v>58174</v>
       </c>
       <c r="D140">
-        <v>85192235</v>
+        <v>85661375</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4326,10 +4326,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>20549</v>
+        <v>20639</v>
       </c>
       <c r="D143">
-        <v>29718867</v>
+        <v>29846607</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4404,10 +4404,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>2800</v>
+        <v>2817</v>
       </c>
       <c r="D146">
-        <v>4004977</v>
+        <v>4029106</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -4456,10 +4456,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>1901</v>
+        <v>1918</v>
       </c>
       <c r="D148">
-        <v>2642617</v>
+        <v>2667013</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -4482,10 +4482,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D149">
-        <v>3715</v>
+        <v>5215</v>
       </c>
       <c r="E149" t="s">
         <v>23</v>
@@ -4508,10 +4508,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>153939</v>
+        <v>154413</v>
       </c>
       <c r="D150">
-        <v>192368073</v>
+        <v>192931258</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -4534,10 +4534,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D151">
-        <v>78412</v>
+        <v>78978</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4638,10 +4638,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D155">
-        <v>521558</v>
+        <v>524558</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4690,10 +4690,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>61678</v>
+        <v>61970</v>
       </c>
       <c r="D157">
-        <v>90725037</v>
+        <v>91147484</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4768,10 +4768,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>31307</v>
+        <v>31443</v>
       </c>
       <c r="D160">
-        <v>45463696</v>
+        <v>45658010</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4846,10 +4846,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>2518</v>
+        <v>2532</v>
       </c>
       <c r="D163">
-        <v>3552328</v>
+        <v>3572234</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4924,10 +4924,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>2196</v>
+        <v>2213</v>
       </c>
       <c r="D166">
-        <v>3063300</v>
+        <v>3087613</v>
       </c>
       <c r="E166" t="s">
         <v>24</v>
@@ -5002,10 +5002,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>63720</v>
+        <v>63961</v>
       </c>
       <c r="D169">
-        <v>81182093</v>
+        <v>81452743</v>
       </c>
       <c r="E169" t="s">
         <v>25</v>
@@ -5106,10 +5106,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D173">
-        <v>453629</v>
+        <v>456629</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5158,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>33263</v>
+        <v>33397</v>
       </c>
       <c r="D175">
-        <v>49029406</v>
+        <v>49223407</v>
       </c>
       <c r="E175" t="s">
         <v>25</v>
@@ -5210,10 +5210,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>7515</v>
+        <v>7552</v>
       </c>
       <c r="D177">
-        <v>10843394</v>
+        <v>10897644</v>
       </c>
       <c r="E177" t="s">
         <v>25</v>
@@ -5262,10 +5262,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>1136</v>
+        <v>1145</v>
       </c>
       <c r="D179">
-        <v>1636883</v>
+        <v>1649505</v>
       </c>
       <c r="E179" t="s">
         <v>25</v>
@@ -5314,10 +5314,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>1017</v>
+        <v>1020</v>
       </c>
       <c r="D181">
-        <v>1423151</v>
+        <v>1425577</v>
       </c>
       <c r="E181" t="s">
         <v>25</v>
@@ -5340,10 +5340,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>151726</v>
+        <v>152302</v>
       </c>
       <c r="D182">
-        <v>193113869</v>
+        <v>193821304</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
@@ -5496,10 +5496,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="D188">
-        <v>721299</v>
+        <v>729450</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5548,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>61972</v>
+        <v>62297</v>
       </c>
       <c r="D190">
-        <v>91327866</v>
+        <v>91799253</v>
       </c>
       <c r="E190" t="s">
         <v>26</v>
@@ -5600,10 +5600,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>39317</v>
+        <v>39510</v>
       </c>
       <c r="D192">
-        <v>57185302</v>
+        <v>57466904</v>
       </c>
       <c r="E192" t="s">
         <v>26</v>
@@ -5652,10 +5652,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>1328</v>
+        <v>1345</v>
       </c>
       <c r="D194">
-        <v>1891321</v>
+        <v>1916481</v>
       </c>
       <c r="E194" t="s">
         <v>26</v>
@@ -5704,10 +5704,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>1804</v>
+        <v>1825</v>
       </c>
       <c r="D196">
-        <v>2530519</v>
+        <v>2560669</v>
       </c>
       <c r="E196" t="s">
         <v>26</v>
@@ -5730,10 +5730,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>237205</v>
+        <v>238382</v>
       </c>
       <c r="D197">
-        <v>313038457</v>
+        <v>314501238</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
@@ -5860,10 +5860,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="D202">
-        <v>1105218</v>
+        <v>1123218</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5912,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>124156</v>
+        <v>125019</v>
       </c>
       <c r="D204">
-        <v>183419377</v>
+        <v>184669180</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5938,10 +5938,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D205">
-        <v>321880</v>
+        <v>323380</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5990,10 +5990,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>98794</v>
+        <v>99414</v>
       </c>
       <c r="D207">
-        <v>144006525</v>
+        <v>144909790</v>
       </c>
       <c r="E207" t="s">
         <v>27</v>
@@ -6042,10 +6042,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>1245</v>
+        <v>1250</v>
       </c>
       <c r="D209">
-        <v>1756599</v>
+        <v>1763849</v>
       </c>
       <c r="E209" t="s">
         <v>27</v>
@@ -6094,10 +6094,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>2297</v>
+        <v>2336</v>
       </c>
       <c r="D211">
-        <v>3257922</v>
+        <v>3310012</v>
       </c>
       <c r="E211" t="s">
         <v>27</v>
@@ -6120,10 +6120,10 @@
         <v>9</v>
       </c>
       <c r="C212">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D212">
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="E212" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="83">
   <si>
     <t>dispositif</t>
   </si>
@@ -620,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>185295</v>
+        <v>185917</v>
       </c>
       <c r="D2">
-        <v>238956444</v>
+        <v>239697024</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -686,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D3">
-        <v>167551</v>
+        <v>170551</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -764,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D6">
-        <v>744414</v>
+        <v>745914</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -816,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>76513</v>
+        <v>76684</v>
       </c>
       <c r="D8">
-        <v>112899229</v>
+        <v>113144985</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -868,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>36118</v>
+        <v>36221</v>
       </c>
       <c r="D10">
-        <v>52445295</v>
+        <v>52590363</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -946,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>2069</v>
+        <v>2076</v>
       </c>
       <c r="D13">
-        <v>2948472</v>
+        <v>2957689</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -998,10 +998,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>36100</v>
+        <v>37600</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1024,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>2380</v>
+        <v>2404</v>
       </c>
       <c r="D16">
-        <v>3353634</v>
+        <v>3387794</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1050,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>47038</v>
+        <v>47194</v>
       </c>
       <c r="D17">
-        <v>59832863</v>
+        <v>60012159</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1180,10 +1180,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>21669</v>
+        <v>21718</v>
       </c>
       <c r="D22">
-        <v>31935155</v>
+        <v>32005366</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1232,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>7162</v>
+        <v>7183</v>
       </c>
       <c r="D24">
-        <v>10391888</v>
+        <v>10422244</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1284,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="D26">
-        <v>1188028</v>
+        <v>1193880</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1336,10 +1336,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>722</v>
+        <v>730</v>
       </c>
       <c r="D28">
-        <v>1023983</v>
+        <v>1035523</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1362,10 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>60009</v>
+        <v>60162</v>
       </c>
       <c r="D29">
-        <v>77058224</v>
+        <v>77234004</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1440,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D32">
-        <v>758971</v>
+        <v>760471</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1492,10 +1492,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>29765</v>
+        <v>29807</v>
       </c>
       <c r="D34">
-        <v>43921013</v>
+        <v>43981926</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1544,10 +1544,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>5661</v>
+        <v>5675</v>
       </c>
       <c r="D36">
-        <v>8159694</v>
+        <v>8180322</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1596,10 +1596,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="D38">
-        <v>1062945</v>
+        <v>1066486</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1622,10 +1622,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="D39">
-        <v>1114671</v>
+        <v>1121882</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1648,10 +1648,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>41449</v>
+        <v>41556</v>
       </c>
       <c r="D40">
-        <v>52652896</v>
+        <v>52778122</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1778,10 +1778,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>18661</v>
+        <v>18700</v>
       </c>
       <c r="D45">
-        <v>27516106</v>
+        <v>27570812</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -1830,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>6809</v>
+        <v>6822</v>
       </c>
       <c r="D47">
-        <v>9883782</v>
+        <v>9902602</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -1856,10 +1856,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="D48">
-        <v>1086606</v>
+        <v>1088106</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -1908,10 +1908,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="D50">
-        <v>729983</v>
+        <v>733161</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -1934,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>11565</v>
+        <v>11596</v>
       </c>
       <c r="D51">
-        <v>15154115</v>
+        <v>15196538</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -2038,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>4280</v>
+        <v>4286</v>
       </c>
       <c r="D55">
-        <v>6282849</v>
+        <v>6290839</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2064,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2907</v>
+        <v>2908</v>
       </c>
       <c r="D56">
-        <v>4236301</v>
+        <v>4237801</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2090,10 +2090,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D57">
-        <v>339625</v>
+        <v>341125</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -2116,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D58">
-        <v>146116</v>
+        <v>147326</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -2142,10 +2142,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>84258</v>
+        <v>84525</v>
       </c>
       <c r="D59">
-        <v>106517955</v>
+        <v>106822917</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2246,10 +2246,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D63">
-        <v>341636</v>
+        <v>344570</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2298,10 +2298,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>41983</v>
+        <v>42111</v>
       </c>
       <c r="D65">
-        <v>61986095</v>
+        <v>62164449</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2376,10 +2376,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>18578</v>
+        <v>18642</v>
       </c>
       <c r="D68">
-        <v>27013388</v>
+        <v>27099312</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2428,10 +2428,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1363</v>
+        <v>1367</v>
       </c>
       <c r="D70">
-        <v>1962434</v>
+        <v>1968434</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2454,10 +2454,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>1038</v>
+        <v>1051</v>
       </c>
       <c r="D71">
-        <v>1472682</v>
+        <v>1488760</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2480,10 +2480,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>13769</v>
+        <v>13851</v>
       </c>
       <c r="D72">
-        <v>18660209</v>
+        <v>18771693</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2584,10 +2584,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>4303</v>
+        <v>4317</v>
       </c>
       <c r="D76">
-        <v>6346768</v>
+        <v>6367768</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2636,10 +2636,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>3385</v>
+        <v>3395</v>
       </c>
       <c r="D78">
-        <v>4887719</v>
+        <v>4900931</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2688,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D80">
-        <v>284311</v>
+        <v>287311</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
@@ -2740,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>2915</v>
+        <v>2926</v>
       </c>
       <c r="D82">
-        <v>4012786</v>
+        <v>4026392</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
@@ -2766,10 +2766,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="D83">
-        <v>1267254</v>
+        <v>1270254</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
@@ -2818,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="D85">
-        <v>1524552</v>
+        <v>1527552</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
@@ -2896,10 +2896,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>86277</v>
+        <v>86493</v>
       </c>
       <c r="D88">
-        <v>107763342</v>
+        <v>108005370</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -3000,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D92">
-        <v>796277</v>
+        <v>796397</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -3052,10 +3052,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>35613</v>
+        <v>35676</v>
       </c>
       <c r="D94">
-        <v>52491684</v>
+        <v>52579873</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -3104,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>16760</v>
+        <v>16793</v>
       </c>
       <c r="D96">
-        <v>24370536</v>
+        <v>24418915</v>
       </c>
       <c r="E96" t="s">
         <v>18</v>
@@ -3130,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="D97">
-        <v>910382</v>
+        <v>915482</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -3156,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="D98">
-        <v>1191872</v>
+        <v>1197386</v>
       </c>
       <c r="E98" t="s">
         <v>18</v>
@@ -3208,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>24768</v>
+        <v>24854</v>
       </c>
       <c r="D100">
-        <v>33430461</v>
+        <v>33541193</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -3338,10 +3338,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>9047</v>
+        <v>9068</v>
       </c>
       <c r="D105">
-        <v>13340314</v>
+        <v>13367178</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -3364,10 +3364,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>2304</v>
+        <v>2306</v>
       </c>
       <c r="D106">
-        <v>3338722</v>
+        <v>3341722</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3416,10 +3416,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D108">
-        <v>300215</v>
+        <v>301715</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -3442,10 +3442,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D109">
-        <v>217288</v>
+        <v>223903</v>
       </c>
       <c r="E109" t="s">
         <v>19</v>
@@ -3468,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>9062</v>
+        <v>9102</v>
       </c>
       <c r="D110">
-        <v>12078830</v>
+        <v>12132153</v>
       </c>
       <c r="E110" t="s">
         <v>20</v>
@@ -3494,10 +3494,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D111">
-        <v>50906</v>
+        <v>6126</v>
       </c>
       <c r="E111" t="s">
         <v>20</v>
@@ -3506,10 +3506,10 @@
         <v>38</v>
       </c>
       <c r="G111" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H111" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3520,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>4156</v>
+        <v>35</v>
       </c>
       <c r="D112">
-        <v>6082127</v>
+        <v>50906</v>
       </c>
       <c r="E112" t="s">
         <v>20</v>
@@ -3532,10 +3532,10 @@
         <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H112" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3546,10 +3546,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>2599</v>
+        <v>4164</v>
       </c>
       <c r="D113">
-        <v>3757705</v>
+        <v>6094127</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3558,10 +3558,10 @@
         <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H113" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3572,10 +3572,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>129</v>
+        <v>2607</v>
       </c>
       <c r="D114">
-        <v>180513</v>
+        <v>3768413</v>
       </c>
       <c r="E114" t="s">
         <v>20</v>
@@ -3584,10 +3584,10 @@
         <v>38</v>
       </c>
       <c r="G114" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H114" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3598,10 +3598,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="D115">
-        <v>101361</v>
+        <v>183513</v>
       </c>
       <c r="E115" t="s">
         <v>20</v>
@@ -3610,10 +3610,10 @@
         <v>38</v>
       </c>
       <c r="G115" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H115" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3624,22 +3624,22 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>3045</v>
+        <v>71</v>
       </c>
       <c r="D116">
-        <v>4313809</v>
+        <v>101361</v>
       </c>
       <c r="E116" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F116" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G116" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H116" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3650,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>775</v>
+        <v>3079</v>
       </c>
       <c r="D117">
-        <v>1148943</v>
+        <v>4360249</v>
       </c>
       <c r="E117" t="s">
         <v>21</v>
@@ -3662,10 +3662,10 @@
         <v>39</v>
       </c>
       <c r="G117" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H117" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3676,10 +3676,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>106</v>
+        <v>775</v>
       </c>
       <c r="D118">
-        <v>156600</v>
+        <v>1148943</v>
       </c>
       <c r="E118" t="s">
         <v>21</v>
@@ -3688,10 +3688,10 @@
         <v>39</v>
       </c>
       <c r="G118" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H118" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -3702,10 +3702,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="D119">
-        <v>19500</v>
+        <v>158100</v>
       </c>
       <c r="E119" t="s">
         <v>21</v>
@@ -3714,10 +3714,10 @@
         <v>39</v>
       </c>
       <c r="G119" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H119" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3728,10 +3728,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D120">
-        <v>26949</v>
+        <v>19500</v>
       </c>
       <c r="E120" t="s">
         <v>21</v>
@@ -3740,10 +3740,10 @@
         <v>39</v>
       </c>
       <c r="G120" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H120" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3754,22 +3754,22 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>54210</v>
+        <v>20</v>
       </c>
       <c r="D121">
-        <v>68863412</v>
+        <v>29949</v>
       </c>
       <c r="E121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F121" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G121" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H121" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3780,10 +3780,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>15</v>
+        <v>54353</v>
       </c>
       <c r="D122">
-        <v>20095</v>
+        <v>69033227</v>
       </c>
       <c r="E122" t="s">
         <v>22</v>
@@ -3792,10 +3792,10 @@
         <v>40</v>
       </c>
       <c r="G122" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H122" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -3806,10 +3806,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D123">
-        <v>80699</v>
+        <v>20095</v>
       </c>
       <c r="E123" t="s">
         <v>22</v>
@@ -3818,10 +3818,10 @@
         <v>40</v>
       </c>
       <c r="G123" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H123" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3832,10 +3832,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D124">
-        <v>7330</v>
+        <v>82199</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
@@ -3844,10 +3844,10 @@
         <v>40</v>
       </c>
       <c r="G124" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H124" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3858,10 +3858,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>364</v>
+        <v>5</v>
       </c>
       <c r="D125">
-        <v>536762</v>
+        <v>7330</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3870,10 +3870,10 @@
         <v>40</v>
       </c>
       <c r="G125" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H125" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3884,10 +3884,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>365</v>
       </c>
       <c r="D126">
-        <v>4500</v>
+        <v>538262</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
@@ -3896,10 +3896,10 @@
         <v>40</v>
       </c>
       <c r="G126" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H126" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -3910,10 +3910,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>22993</v>
+        <v>3</v>
       </c>
       <c r="D127">
-        <v>33905865</v>
+        <v>4500</v>
       </c>
       <c r="E127" t="s">
         <v>22</v>
@@ -3922,10 +3922,10 @@
         <v>40</v>
       </c>
       <c r="G127" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H127" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -3936,10 +3936,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>15</v>
+        <v>23038</v>
       </c>
       <c r="D128">
-        <v>22500</v>
+        <v>33971008</v>
       </c>
       <c r="E128" t="s">
         <v>22</v>
@@ -3948,10 +3948,10 @@
         <v>40</v>
       </c>
       <c r="G128" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H128" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3962,10 +3962,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>8095</v>
+        <v>15</v>
       </c>
       <c r="D129">
-        <v>11753126</v>
+        <v>22500</v>
       </c>
       <c r="E129" t="s">
         <v>22</v>
@@ -3974,10 +3974,10 @@
         <v>40</v>
       </c>
       <c r="G129" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H129" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -3988,10 +3988,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>5</v>
+        <v>8109</v>
       </c>
       <c r="D130">
-        <v>6419</v>
+        <v>11773535</v>
       </c>
       <c r="E130" t="s">
         <v>22</v>
@@ -4000,10 +4000,10 @@
         <v>40</v>
       </c>
       <c r="G130" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4014,10 +4014,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>693</v>
+        <v>5</v>
       </c>
       <c r="D131">
-        <v>976931</v>
+        <v>6419</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4026,10 +4026,10 @@
         <v>40</v>
       </c>
       <c r="G131" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H131" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -4040,10 +4040,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>673</v>
+        <v>699</v>
       </c>
       <c r="D132">
-        <v>959426</v>
+        <v>985345</v>
       </c>
       <c r="E132" t="s">
         <v>22</v>
@@ -4052,10 +4052,10 @@
         <v>40</v>
       </c>
       <c r="G132" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H132" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4066,22 +4066,22 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>143767</v>
+        <v>678</v>
       </c>
       <c r="D133">
-        <v>181133519</v>
+        <v>965594</v>
       </c>
       <c r="E133" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G133" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H133" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -4092,10 +4092,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>64</v>
+        <v>144148</v>
       </c>
       <c r="D134">
-        <v>68835</v>
+        <v>181578013</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
@@ -4104,10 +4104,10 @@
         <v>41</v>
       </c>
       <c r="G134" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H134" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -4118,10 +4118,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D135">
-        <v>147375</v>
+        <v>69745</v>
       </c>
       <c r="E135" t="s">
         <v>23</v>
@@ -4130,10 +4130,10 @@
         <v>41</v>
       </c>
       <c r="G135" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H135" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -4144,10 +4144,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="D136">
-        <v>4500</v>
+        <v>147375</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
@@ -4156,10 +4156,10 @@
         <v>41</v>
       </c>
       <c r="G136" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="H136" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4170,10 +4170,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D137">
-        <v>8230</v>
+        <v>4500</v>
       </c>
       <c r="E137" t="s">
         <v>23</v>
@@ -4182,10 +4182,10 @@
         <v>41</v>
       </c>
       <c r="G137" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="H137" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4196,10 +4196,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>518</v>
+        <v>6</v>
       </c>
       <c r="D138">
-        <v>762059</v>
+        <v>8230</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
@@ -4208,10 +4208,10 @@
         <v>41</v>
       </c>
       <c r="G138" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H138" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4222,10 +4222,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>6</v>
+        <v>518</v>
       </c>
       <c r="D139">
-        <v>8383</v>
+        <v>762059</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -4234,10 +4234,10 @@
         <v>41</v>
       </c>
       <c r="G139" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H139" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4248,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>58174</v>
+        <v>6</v>
       </c>
       <c r="D140">
-        <v>85661375</v>
+        <v>8383</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -4260,10 +4260,10 @@
         <v>41</v>
       </c>
       <c r="G140" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H140" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4274,10 +4274,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>60</v>
+        <v>58282</v>
       </c>
       <c r="D141">
-        <v>87295</v>
+        <v>85816416</v>
       </c>
       <c r="E141" t="s">
         <v>23</v>
@@ -4286,10 +4286,10 @@
         <v>41</v>
       </c>
       <c r="G141" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H141" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4300,10 +4300,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D142">
-        <v>4500</v>
+        <v>87295</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
@@ -4312,10 +4312,10 @@
         <v>41</v>
       </c>
       <c r="G142" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H142" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4326,10 +4326,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>20639</v>
+        <v>3</v>
       </c>
       <c r="D143">
-        <v>29846607</v>
+        <v>4500</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -4338,10 +4338,10 @@
         <v>41</v>
       </c>
       <c r="G143" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H143" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4352,10 +4352,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>17</v>
+        <v>20671</v>
       </c>
       <c r="D144">
-        <v>25500</v>
+        <v>29893513</v>
       </c>
       <c r="E144" t="s">
         <v>23</v>
@@ -4364,10 +4364,10 @@
         <v>41</v>
       </c>
       <c r="G144" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H144" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4378,10 +4378,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D145">
-        <v>9000</v>
+        <v>25500</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -4390,10 +4390,10 @@
         <v>41</v>
       </c>
       <c r="G145" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H145" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4404,10 +4404,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>2817</v>
+        <v>7</v>
       </c>
       <c r="D146">
-        <v>4029106</v>
+        <v>9554</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -4416,10 +4416,10 @@
         <v>41</v>
       </c>
       <c r="G146" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H146" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4430,10 +4430,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>6</v>
+        <v>2830</v>
       </c>
       <c r="D147">
-        <v>9000</v>
+        <v>4048171</v>
       </c>
       <c r="E147" t="s">
         <v>23</v>
@@ -4442,10 +4442,10 @@
         <v>41</v>
       </c>
       <c r="G147" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H147" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4456,10 +4456,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>1918</v>
+        <v>6</v>
       </c>
       <c r="D148">
-        <v>2667013</v>
+        <v>9000</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -4468,10 +4468,10 @@
         <v>41</v>
       </c>
       <c r="G148" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H148" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4482,10 +4482,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>4</v>
+        <v>1934</v>
       </c>
       <c r="D149">
-        <v>5215</v>
+        <v>2688649</v>
       </c>
       <c r="E149" t="s">
         <v>23</v>
@@ -4494,10 +4494,10 @@
         <v>41</v>
       </c>
       <c r="G149" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H149" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4508,22 +4508,22 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>154413</v>
+        <v>4</v>
       </c>
       <c r="D150">
-        <v>192931258</v>
+        <v>5215</v>
       </c>
       <c r="E150" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F150" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G150" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H150" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4534,10 +4534,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>79</v>
+        <v>154827</v>
       </c>
       <c r="D151">
-        <v>78978</v>
+        <v>193400302</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -4546,10 +4546,10 @@
         <v>42</v>
       </c>
       <c r="G151" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H151" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4560,10 +4560,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="D152">
-        <v>204730</v>
+        <v>80478</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -4572,10 +4572,10 @@
         <v>42</v>
       </c>
       <c r="G152" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H152" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4586,10 +4586,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>9</v>
+        <v>143</v>
       </c>
       <c r="D153">
-        <v>12825</v>
+        <v>204730</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
@@ -4598,10 +4598,10 @@
         <v>42</v>
       </c>
       <c r="G153" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H153" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4612,10 +4612,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D154">
-        <v>6378</v>
+        <v>12825</v>
       </c>
       <c r="E154" t="s">
         <v>24</v>
@@ -4624,10 +4624,10 @@
         <v>42</v>
       </c>
       <c r="G154" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H154" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -4638,10 +4638,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>356</v>
+        <v>5</v>
       </c>
       <c r="D155">
-        <v>524558</v>
+        <v>6378</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -4650,10 +4650,10 @@
         <v>42</v>
       </c>
       <c r="G155" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H155" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4664,10 +4664,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>4</v>
+        <v>358</v>
       </c>
       <c r="D156">
-        <v>6000</v>
+        <v>527558</v>
       </c>
       <c r="E156" t="s">
         <v>24</v>
@@ -4676,10 +4676,10 @@
         <v>42</v>
       </c>
       <c r="G156" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H156" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4690,10 +4690,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>61970</v>
+        <v>4</v>
       </c>
       <c r="D157">
-        <v>91147484</v>
+        <v>6000</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -4702,10 +4702,10 @@
         <v>42</v>
       </c>
       <c r="G157" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H157" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4716,10 +4716,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>50</v>
+        <v>62068</v>
       </c>
       <c r="D158">
-        <v>74199</v>
+        <v>91291665</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -4728,10 +4728,10 @@
         <v>42</v>
       </c>
       <c r="G158" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H158" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4742,10 +4742,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D159">
-        <v>9000</v>
+        <v>74199</v>
       </c>
       <c r="E159" t="s">
         <v>24</v>
@@ -4754,10 +4754,10 @@
         <v>42</v>
       </c>
       <c r="G159" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H159" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -4768,10 +4768,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>31443</v>
+        <v>6</v>
       </c>
       <c r="D160">
-        <v>45658010</v>
+        <v>9000</v>
       </c>
       <c r="E160" t="s">
         <v>24</v>
@@ -4780,10 +4780,10 @@
         <v>42</v>
       </c>
       <c r="G160" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H160" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -4794,10 +4794,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>17</v>
+        <v>31498</v>
       </c>
       <c r="D161">
-        <v>24857</v>
+        <v>45738723</v>
       </c>
       <c r="E161" t="s">
         <v>24</v>
@@ -4806,10 +4806,10 @@
         <v>42</v>
       </c>
       <c r="G161" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H161" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -4820,10 +4820,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D162">
-        <v>12160</v>
+        <v>24857</v>
       </c>
       <c r="E162" t="s">
         <v>24</v>
@@ -4832,10 +4832,10 @@
         <v>42</v>
       </c>
       <c r="G162" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H162" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -4846,10 +4846,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>2532</v>
+        <v>9</v>
       </c>
       <c r="D163">
-        <v>3572234</v>
+        <v>12160</v>
       </c>
       <c r="E163" t="s">
         <v>24</v>
@@ -4858,10 +4858,10 @@
         <v>42</v>
       </c>
       <c r="G163" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H163" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -4872,10 +4872,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>4</v>
+        <v>2545</v>
       </c>
       <c r="D164">
-        <v>6000</v>
+        <v>3590076</v>
       </c>
       <c r="E164" t="s">
         <v>24</v>
@@ -4884,10 +4884,10 @@
         <v>42</v>
       </c>
       <c r="G164" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H164" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -4898,10 +4898,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D165">
-        <v>10500</v>
+        <v>6000</v>
       </c>
       <c r="E165" t="s">
         <v>24</v>
@@ -4910,10 +4910,10 @@
         <v>42</v>
       </c>
       <c r="G165" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="H165" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -4924,10 +4924,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>2213</v>
+        <v>7</v>
       </c>
       <c r="D166">
-        <v>3087613</v>
+        <v>10500</v>
       </c>
       <c r="E166" t="s">
         <v>24</v>
@@ -4936,10 +4936,10 @@
         <v>42</v>
       </c>
       <c r="G166" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H166" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -4950,10 +4950,10 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>4</v>
+        <v>2225</v>
       </c>
       <c r="D167">
-        <v>6000</v>
+        <v>3102641</v>
       </c>
       <c r="E167" t="s">
         <v>24</v>
@@ -4962,10 +4962,10 @@
         <v>42</v>
       </c>
       <c r="G167" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="H167" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -4976,10 +4976,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D168">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E168" t="s">
         <v>24</v>
@@ -4988,10 +4988,10 @@
         <v>42</v>
       </c>
       <c r="G168" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="H168" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -5002,22 +5002,22 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>63961</v>
+        <v>5</v>
       </c>
       <c r="D169">
-        <v>81452743</v>
+        <v>7500</v>
       </c>
       <c r="E169" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F169" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G169" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H169" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -5028,10 +5028,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>38</v>
+        <v>64134</v>
       </c>
       <c r="D170">
-        <v>39470</v>
+        <v>81655627</v>
       </c>
       <c r="E170" t="s">
         <v>25</v>
@@ -5040,10 +5040,10 @@
         <v>43</v>
       </c>
       <c r="G170" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H170" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -5054,10 +5054,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D171">
-        <v>58865</v>
+        <v>39470</v>
       </c>
       <c r="E171" t="s">
         <v>25</v>
@@ -5066,10 +5066,10 @@
         <v>43</v>
       </c>
       <c r="G171" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H171" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -5080,10 +5080,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D172">
-        <v>4900</v>
+        <v>59665</v>
       </c>
       <c r="E172" t="s">
         <v>25</v>
@@ -5092,10 +5092,10 @@
         <v>43</v>
       </c>
       <c r="G172" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H172" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5106,10 +5106,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>313</v>
+        <v>4</v>
       </c>
       <c r="D173">
-        <v>456629</v>
+        <v>4900</v>
       </c>
       <c r="E173" t="s">
         <v>25</v>
@@ -5118,10 +5118,10 @@
         <v>43</v>
       </c>
       <c r="G173" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="H173" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -5132,10 +5132,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>3</v>
+        <v>314</v>
       </c>
       <c r="D174">
-        <v>2113</v>
+        <v>458129</v>
       </c>
       <c r="E174" t="s">
         <v>25</v>
@@ -5144,10 +5144,10 @@
         <v>43</v>
       </c>
       <c r="G174" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H174" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5158,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>33397</v>
+        <v>3</v>
       </c>
       <c r="D175">
-        <v>49223407</v>
+        <v>2113</v>
       </c>
       <c r="E175" t="s">
         <v>25</v>
@@ -5170,10 +5170,10 @@
         <v>43</v>
       </c>
       <c r="G175" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H175" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5184,10 +5184,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>18</v>
+        <v>33453</v>
       </c>
       <c r="D176">
-        <v>25649</v>
+        <v>49305385</v>
       </c>
       <c r="E176" t="s">
         <v>25</v>
@@ -5196,10 +5196,10 @@
         <v>43</v>
       </c>
       <c r="G176" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H176" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5210,10 +5210,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>7552</v>
+        <v>18</v>
       </c>
       <c r="D177">
-        <v>10897644</v>
+        <v>25649</v>
       </c>
       <c r="E177" t="s">
         <v>25</v>
@@ -5222,10 +5222,10 @@
         <v>43</v>
       </c>
       <c r="G177" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H177" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5236,10 +5236,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>5</v>
+        <v>7564</v>
       </c>
       <c r="D178">
-        <v>4798</v>
+        <v>10915644</v>
       </c>
       <c r="E178" t="s">
         <v>25</v>
@@ -5248,10 +5248,10 @@
         <v>43</v>
       </c>
       <c r="G178" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H178" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5262,10 +5262,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>1145</v>
+        <v>5</v>
       </c>
       <c r="D179">
-        <v>1649505</v>
+        <v>4798</v>
       </c>
       <c r="E179" t="s">
         <v>25</v>
@@ -5274,10 +5274,10 @@
         <v>43</v>
       </c>
       <c r="G179" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H179" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5288,10 +5288,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>4</v>
+        <v>1151</v>
       </c>
       <c r="D180">
-        <v>4096</v>
+        <v>1658505</v>
       </c>
       <c r="E180" t="s">
         <v>25</v>
@@ -5300,10 +5300,10 @@
         <v>43</v>
       </c>
       <c r="G180" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H180" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5314,10 +5314,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>1020</v>
+        <v>4</v>
       </c>
       <c r="D181">
-        <v>1425577</v>
+        <v>4096</v>
       </c>
       <c r="E181" t="s">
         <v>25</v>
@@ -5326,10 +5326,10 @@
         <v>43</v>
       </c>
       <c r="G181" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H181" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5340,22 +5340,22 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>152302</v>
+        <v>1031</v>
       </c>
       <c r="D182">
-        <v>193821304</v>
+        <v>1439449</v>
       </c>
       <c r="E182" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F182" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G182" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H182" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5366,10 +5366,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>91</v>
+        <v>152660</v>
       </c>
       <c r="D183">
-        <v>112032</v>
+        <v>194246277</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
@@ -5378,10 +5378,10 @@
         <v>44</v>
       </c>
       <c r="G183" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H183" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5392,10 +5392,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D184">
-        <v>214399</v>
+        <v>113532</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
@@ -5404,10 +5404,10 @@
         <v>44</v>
       </c>
       <c r="G184" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H184" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5418,10 +5418,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="D185">
-        <v>9000</v>
+        <v>214399</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
@@ -5430,10 +5430,10 @@
         <v>44</v>
       </c>
       <c r="G185" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H185" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5444,10 +5444,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D186">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -5456,10 +5456,10 @@
         <v>44</v>
       </c>
       <c r="G186" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H186" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5470,10 +5470,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D187">
-        <v>9981</v>
+        <v>6000</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
@@ -5482,10 +5482,10 @@
         <v>44</v>
       </c>
       <c r="G187" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H187" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5496,10 +5496,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>491</v>
+        <v>7</v>
       </c>
       <c r="D188">
-        <v>729450</v>
+        <v>9981</v>
       </c>
       <c r="E188" t="s">
         <v>26</v>
@@ -5508,10 +5508,10 @@
         <v>44</v>
       </c>
       <c r="G188" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H188" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5522,10 +5522,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>7</v>
+        <v>491</v>
       </c>
       <c r="D189">
-        <v>10500</v>
+        <v>729450</v>
       </c>
       <c r="E189" t="s">
         <v>26</v>
@@ -5534,10 +5534,10 @@
         <v>44</v>
       </c>
       <c r="G189" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H189" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5548,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>62297</v>
+        <v>7</v>
       </c>
       <c r="D190">
-        <v>91799253</v>
+        <v>10500</v>
       </c>
       <c r="E190" t="s">
         <v>26</v>
@@ -5560,10 +5560,10 @@
         <v>44</v>
       </c>
       <c r="G190" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H190" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5574,10 +5574,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>58</v>
+        <v>62395</v>
       </c>
       <c r="D191">
-        <v>84692</v>
+        <v>91938824</v>
       </c>
       <c r="E191" t="s">
         <v>26</v>
@@ -5586,10 +5586,10 @@
         <v>44</v>
       </c>
       <c r="G191" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H191" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5600,10 +5600,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>39510</v>
+        <v>60</v>
       </c>
       <c r="D192">
-        <v>57466904</v>
+        <v>87692</v>
       </c>
       <c r="E192" t="s">
         <v>26</v>
@@ -5612,10 +5612,10 @@
         <v>44</v>
       </c>
       <c r="G192" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H192" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5626,10 +5626,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>9</v>
+        <v>39611</v>
       </c>
       <c r="D193">
-        <v>13489</v>
+        <v>57610341</v>
       </c>
       <c r="E193" t="s">
         <v>26</v>
@@ -5638,10 +5638,10 @@
         <v>44</v>
       </c>
       <c r="G193" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H193" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5652,10 +5652,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>1345</v>
+        <v>9</v>
       </c>
       <c r="D194">
-        <v>1916481</v>
+        <v>13489</v>
       </c>
       <c r="E194" t="s">
         <v>26</v>
@@ -5664,10 +5664,10 @@
         <v>44</v>
       </c>
       <c r="G194" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H194" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5678,10 +5678,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>8</v>
+        <v>1350</v>
       </c>
       <c r="D195">
-        <v>12000</v>
+        <v>1923981</v>
       </c>
       <c r="E195" t="s">
         <v>26</v>
@@ -5690,10 +5690,10 @@
         <v>44</v>
       </c>
       <c r="G195" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H195" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5704,10 +5704,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>1825</v>
+        <v>8</v>
       </c>
       <c r="D196">
-        <v>2560669</v>
+        <v>12000</v>
       </c>
       <c r="E196" t="s">
         <v>26</v>
@@ -5716,10 +5716,10 @@
         <v>44</v>
       </c>
       <c r="G196" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H196" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5730,22 +5730,22 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>238382</v>
+        <v>1840</v>
       </c>
       <c r="D197">
-        <v>314501238</v>
+        <v>2582297</v>
       </c>
       <c r="E197" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F197" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G197" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H197" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5756,10 +5756,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>41</v>
+        <v>239178</v>
       </c>
       <c r="D198">
-        <v>51889</v>
+        <v>315482856</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
@@ -5768,10 +5768,10 @@
         <v>45</v>
       </c>
       <c r="G198" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H198" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5782,10 +5782,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="D199">
-        <v>179818</v>
+        <v>51889</v>
       </c>
       <c r="E199" t="s">
         <v>27</v>
@@ -5794,10 +5794,10 @@
         <v>45</v>
       </c>
       <c r="G199" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H199" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5808,10 +5808,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="D200">
-        <v>7500</v>
+        <v>181318</v>
       </c>
       <c r="E200" t="s">
         <v>27</v>
@@ -5820,10 +5820,10 @@
         <v>45</v>
       </c>
       <c r="G200" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H200" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5834,10 +5834,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D201">
-        <v>14998</v>
+        <v>7500</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -5846,10 +5846,10 @@
         <v>45</v>
       </c>
       <c r="G201" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H201" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5860,10 +5860,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>754</v>
+        <v>10</v>
       </c>
       <c r="D202">
-        <v>1123218</v>
+        <v>14998</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -5872,10 +5872,10 @@
         <v>45</v>
       </c>
       <c r="G202" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H202" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5886,10 +5886,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>11</v>
+        <v>756</v>
       </c>
       <c r="D203">
-        <v>15716</v>
+        <v>1126218</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
@@ -5898,10 +5898,10 @@
         <v>45</v>
       </c>
       <c r="G203" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H203" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5912,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>125019</v>
+        <v>11</v>
       </c>
       <c r="D204">
-        <v>184669180</v>
+        <v>15716</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -5924,10 +5924,10 @@
         <v>45</v>
       </c>
       <c r="G204" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H204" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5938,10 +5938,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>217</v>
+        <v>125373</v>
       </c>
       <c r="D205">
-        <v>323380</v>
+        <v>185185183</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -5950,10 +5950,10 @@
         <v>45</v>
       </c>
       <c r="G205" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H205" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5964,10 +5964,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>7</v>
+        <v>218</v>
       </c>
       <c r="D206">
-        <v>10500</v>
+        <v>324880</v>
       </c>
       <c r="E206" t="s">
         <v>27</v>
@@ -5976,10 +5976,10 @@
         <v>45</v>
       </c>
       <c r="G206" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H206" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5990,10 +5990,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>99414</v>
+        <v>7</v>
       </c>
       <c r="D207">
-        <v>144909790</v>
+        <v>10500</v>
       </c>
       <c r="E207" t="s">
         <v>27</v>
@@ -6002,10 +6002,10 @@
         <v>45</v>
       </c>
       <c r="G207" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H207" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -6016,10 +6016,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>20</v>
+        <v>99710</v>
       </c>
       <c r="D208">
-        <v>28832</v>
+        <v>145338630</v>
       </c>
       <c r="E208" t="s">
         <v>27</v>
@@ -6028,10 +6028,10 @@
         <v>45</v>
       </c>
       <c r="G208" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H208" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -6042,10 +6042,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>1250</v>
+        <v>20</v>
       </c>
       <c r="D209">
-        <v>1763849</v>
+        <v>28832</v>
       </c>
       <c r="E209" t="s">
         <v>27</v>
@@ -6054,10 +6054,10 @@
         <v>45</v>
       </c>
       <c r="G209" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H209" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -6068,10 +6068,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>3</v>
+        <v>1256</v>
       </c>
       <c r="D210">
-        <v>4222</v>
+        <v>1772842</v>
       </c>
       <c r="E210" t="s">
         <v>27</v>
@@ -6080,10 +6080,10 @@
         <v>45</v>
       </c>
       <c r="G210" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H210" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -6094,10 +6094,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>2336</v>
+        <v>3</v>
       </c>
       <c r="D211">
-        <v>3310012</v>
+        <v>4222</v>
       </c>
       <c r="E211" t="s">
         <v>27</v>
@@ -6106,10 +6106,10 @@
         <v>45</v>
       </c>
       <c r="G211" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="H211" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -6120,10 +6120,10 @@
         <v>9</v>
       </c>
       <c r="C212">
-        <v>11</v>
+        <v>2362</v>
       </c>
       <c r="D212">
-        <v>16500</v>
+        <v>3345604</v>
       </c>
       <c r="E212" t="s">
         <v>27</v>
@@ -6132,9 +6132,35 @@
         <v>45</v>
       </c>
       <c r="G212" t="s">
+        <v>57</v>
+      </c>
+      <c r="H212" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8">
+      <c r="A213" t="s">
+        <v>8</v>
+      </c>
+      <c r="B213" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213">
+        <v>11</v>
+      </c>
+      <c r="D213">
+        <v>16500</v>
+      </c>
+      <c r="E213" t="s">
+        <v>27</v>
+      </c>
+      <c r="F213" t="s">
+        <v>45</v>
+      </c>
+      <c r="G213" t="s">
         <v>60</v>
       </c>
-      <c r="H212" t="s">
+      <c r="H213" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-06-25 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -711,10 +711,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>276819</v>
+        <v>277715</v>
       </c>
       <c r="D2">
-        <v>353962708</v>
+        <v>355121162</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -867,10 +867,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="D8">
-        <v>1127894</v>
+        <v>1135394</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -919,10 +919,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>105567</v>
+        <v>105988</v>
       </c>
       <c r="D10">
-        <v>154969929</v>
+        <v>155584022</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -971,10 +971,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>51968</v>
+        <v>52214</v>
       </c>
       <c r="D12">
-        <v>75122450</v>
+        <v>75473447</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1075,10 +1075,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>3406</v>
+        <v>3429</v>
       </c>
       <c r="D16">
-        <v>4841315</v>
+        <v>4874603</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1179,10 +1179,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>4863</v>
+        <v>4908</v>
       </c>
       <c r="D20">
-        <v>6812479</v>
+        <v>6874088</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1231,10 +1231,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>68666</v>
+        <v>68858</v>
       </c>
       <c r="D22">
-        <v>86244128</v>
+        <v>86478690</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1335,10 +1335,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1361,10 +1361,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D27">
-        <v>367718</v>
+        <v>370718</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1387,10 +1387,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>29534</v>
+        <v>29640</v>
       </c>
       <c r="D28">
-        <v>43297234</v>
+        <v>43449773</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1439,10 +1439,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>10138</v>
+        <v>10179</v>
       </c>
       <c r="D30">
-        <v>14628620</v>
+        <v>14687443</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1517,10 +1517,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>1340</v>
+        <v>1351</v>
       </c>
       <c r="D33">
-        <v>1884586</v>
+        <v>1900715</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1569,10 +1569,10 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>1388</v>
+        <v>1404</v>
       </c>
       <c r="D35">
-        <v>1955703</v>
+        <v>1979703</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -1595,10 +1595,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>86944</v>
+        <v>87144</v>
       </c>
       <c r="D36">
-        <v>110249062</v>
+        <v>110495459</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1621,10 +1621,10 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D37">
-        <v>64493</v>
+        <v>65593</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1647,10 +1647,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38">
-        <v>102653</v>
+        <v>104153</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1751,10 +1751,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="D42">
-        <v>1174158</v>
+        <v>1183958</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1777,10 +1777,10 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1803,10 +1803,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>40664</v>
+        <v>40775</v>
       </c>
       <c r="D44">
-        <v>59717937</v>
+        <v>59878093</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1855,10 +1855,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>8125</v>
+        <v>8155</v>
       </c>
       <c r="D46">
-        <v>11668027</v>
+        <v>11713027</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1907,10 +1907,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="D48">
-        <v>1644017</v>
+        <v>1647017</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1985,10 +1985,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>1708</v>
+        <v>1729</v>
       </c>
       <c r="D51">
-        <v>2380883</v>
+        <v>2411827</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2011,10 +2011,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>60395</v>
+        <v>60536</v>
       </c>
       <c r="D52">
-        <v>76049596</v>
+        <v>76225032</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -2115,10 +2115,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D56">
-        <v>497909</v>
+        <v>500909</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -2167,10 +2167,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>25563</v>
+        <v>25644</v>
       </c>
       <c r="D58">
-        <v>37535790</v>
+        <v>37651295</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -2245,10 +2245,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>9798</v>
+        <v>9837</v>
       </c>
       <c r="D61">
-        <v>14188915</v>
+        <v>14243937</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2271,10 +2271,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="D62">
-        <v>1672219</v>
+        <v>1674607</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2349,10 +2349,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>1108</v>
+        <v>1115</v>
       </c>
       <c r="D65">
-        <v>1556609</v>
+        <v>1566576</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -2401,10 +2401,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>17693</v>
+        <v>17776</v>
       </c>
       <c r="D67">
-        <v>23163968</v>
+        <v>23270436</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
@@ -2505,10 +2505,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>6441</v>
+        <v>6465</v>
       </c>
       <c r="D71">
-        <v>9425651</v>
+        <v>9459992</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
@@ -2531,10 +2531,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>4389</v>
+        <v>4407</v>
       </c>
       <c r="D72">
-        <v>6379811</v>
+        <v>6405710</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
@@ -2557,10 +2557,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D73">
-        <v>567258</v>
+        <v>568758</v>
       </c>
       <c r="E73" t="s">
         <v>14</v>
@@ -2583,10 +2583,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D74">
-        <v>299056</v>
+        <v>308056</v>
       </c>
       <c r="E74" t="s">
         <v>14</v>
@@ -2609,10 +2609,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>123524</v>
+        <v>123920</v>
       </c>
       <c r="D75">
-        <v>154680612</v>
+        <v>155152951</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -2687,10 +2687,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D78">
-        <v>25500</v>
+        <v>27000</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
@@ -2713,10 +2713,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D79">
-        <v>533282</v>
+        <v>534782</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
@@ -2765,10 +2765,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>57431</v>
+        <v>57653</v>
       </c>
       <c r="D81">
-        <v>84325364</v>
+        <v>84645609</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -2791,10 +2791,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D82">
-        <v>99082</v>
+        <v>102082</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -2843,10 +2843,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>26286</v>
+        <v>26414</v>
       </c>
       <c r="D84">
-        <v>38063058</v>
+        <v>38250161</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -2895,10 +2895,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>2292</v>
+        <v>2305</v>
       </c>
       <c r="D86">
-        <v>3304938</v>
+        <v>3324328</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -2921,10 +2921,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>2072</v>
+        <v>2100</v>
       </c>
       <c r="D87">
-        <v>2918175</v>
+        <v>2956207</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -2947,10 +2947,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>23612</v>
+        <v>23784</v>
       </c>
       <c r="D88">
-        <v>32069750</v>
+        <v>32297817</v>
       </c>
       <c r="E88" t="s">
         <v>16</v>
@@ -3051,10 +3051,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>6328</v>
+        <v>6356</v>
       </c>
       <c r="D92">
-        <v>9329839</v>
+        <v>9368176</v>
       </c>
       <c r="E92" t="s">
         <v>16</v>
@@ -3103,10 +3103,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>5483</v>
+        <v>5523</v>
       </c>
       <c r="D94">
-        <v>7947196</v>
+        <v>8006034</v>
       </c>
       <c r="E94" t="s">
         <v>16</v>
@@ -3155,10 +3155,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D96">
-        <v>542159</v>
+        <v>545809</v>
       </c>
       <c r="E96" t="s">
         <v>16</v>
@@ -3181,10 +3181,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D97">
-        <v>461161</v>
+        <v>464161</v>
       </c>
       <c r="E97" t="s">
         <v>16</v>
@@ -3207,10 +3207,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>5345</v>
+        <v>5394</v>
       </c>
       <c r="D98">
-        <v>7403181</v>
+        <v>7473286</v>
       </c>
       <c r="E98" t="s">
         <v>17</v>
@@ -3259,10 +3259,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>1358</v>
+        <v>1368</v>
       </c>
       <c r="D100">
-        <v>1999062</v>
+        <v>2014062</v>
       </c>
       <c r="E100" t="s">
         <v>17</v>
@@ -3311,10 +3311,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>1859</v>
+        <v>1871</v>
       </c>
       <c r="D102">
-        <v>2712626</v>
+        <v>2730601</v>
       </c>
       <c r="E102" t="s">
         <v>17</v>
@@ -3363,10 +3363,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D104">
-        <v>91520</v>
+        <v>93020</v>
       </c>
       <c r="E104" t="s">
         <v>17</v>
@@ -3389,10 +3389,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D105">
-        <v>128412</v>
+        <v>133789</v>
       </c>
       <c r="E105" t="s">
         <v>17</v>
@@ -3415,10 +3415,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>124874</v>
+        <v>125128</v>
       </c>
       <c r="D106">
-        <v>154846524</v>
+        <v>155153237</v>
       </c>
       <c r="E106" t="s">
         <v>18</v>
@@ -3519,10 +3519,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="D110">
-        <v>1260132</v>
+        <v>1270632</v>
       </c>
       <c r="E110" t="s">
         <v>18</v>
@@ -3571,10 +3571,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>48113</v>
+        <v>48250</v>
       </c>
       <c r="D112">
-        <v>70622941</v>
+        <v>70826657</v>
       </c>
       <c r="E112" t="s">
         <v>18</v>
@@ -3597,10 +3597,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D113">
-        <v>116159</v>
+        <v>117659</v>
       </c>
       <c r="E113" t="s">
         <v>18</v>
@@ -3623,10 +3623,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>23739</v>
+        <v>23819</v>
       </c>
       <c r="D114">
-        <v>34420806</v>
+        <v>34533935</v>
       </c>
       <c r="E114" t="s">
         <v>18</v>
@@ -3649,10 +3649,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>1095</v>
+        <v>1102</v>
       </c>
       <c r="D115">
-        <v>1494420</v>
+        <v>1502832</v>
       </c>
       <c r="E115" t="s">
         <v>18</v>
@@ -3727,10 +3727,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>1696</v>
+        <v>1709</v>
       </c>
       <c r="D118">
-        <v>2385850</v>
+        <v>2404872</v>
       </c>
       <c r="E118" t="s">
         <v>18</v>
@@ -3779,10 +3779,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>37300</v>
+        <v>37421</v>
       </c>
       <c r="D120">
-        <v>50054497</v>
+        <v>50207259</v>
       </c>
       <c r="E120" t="s">
         <v>19</v>
@@ -3805,10 +3805,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D121">
-        <v>31153</v>
+        <v>32653</v>
       </c>
       <c r="E121" t="s">
         <v>19</v>
@@ -3935,10 +3935,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>12397</v>
+        <v>12429</v>
       </c>
       <c r="D126">
-        <v>18225420</v>
+        <v>18273127</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -3961,10 +3961,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>3239</v>
+        <v>3247</v>
       </c>
       <c r="D127">
-        <v>4677466</v>
+        <v>4688941</v>
       </c>
       <c r="E127" t="s">
         <v>19</v>
@@ -4039,10 +4039,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D130">
-        <v>470536</v>
+        <v>472036</v>
       </c>
       <c r="E130" t="s">
         <v>19</v>
@@ -4091,10 +4091,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D132">
-        <v>408690</v>
+        <v>413190</v>
       </c>
       <c r="E132" t="s">
         <v>19</v>
@@ -4117,10 +4117,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>14080</v>
+        <v>14150</v>
       </c>
       <c r="D133">
-        <v>18686782</v>
+        <v>18777683</v>
       </c>
       <c r="E133" t="s">
         <v>20</v>
@@ -4221,10 +4221,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>6039</v>
+        <v>6071</v>
       </c>
       <c r="D137">
-        <v>8800752</v>
+        <v>8848752</v>
       </c>
       <c r="E137" t="s">
         <v>20</v>
@@ -4273,10 +4273,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>3999</v>
+        <v>4020</v>
       </c>
       <c r="D139">
-        <v>5772169</v>
+        <v>5799615</v>
       </c>
       <c r="E139" t="s">
         <v>20</v>
@@ -4325,10 +4325,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D141">
-        <v>287933</v>
+        <v>289433</v>
       </c>
       <c r="E141" t="s">
         <v>20</v>
@@ -4351,10 +4351,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D142">
-        <v>243164</v>
+        <v>250664</v>
       </c>
       <c r="E142" t="s">
         <v>20</v>
@@ -4403,10 +4403,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>8745</v>
+        <v>8872</v>
       </c>
       <c r="D144">
-        <v>12619681</v>
+        <v>12805026</v>
       </c>
       <c r="E144" t="s">
         <v>21</v>
@@ -4429,10 +4429,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>1306</v>
+        <v>1309</v>
       </c>
       <c r="D145">
-        <v>1940578</v>
+        <v>1945078</v>
       </c>
       <c r="E145" t="s">
         <v>21</v>
@@ -4455,10 +4455,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D146">
-        <v>261171</v>
+        <v>265671</v>
       </c>
       <c r="E146" t="s">
         <v>21</v>
@@ -4481,10 +4481,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D147">
-        <v>37190</v>
+        <v>38690</v>
       </c>
       <c r="E147" t="s">
         <v>21</v>
@@ -4533,10 +4533,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>77416</v>
+        <v>77620</v>
       </c>
       <c r="D149">
-        <v>97268604</v>
+        <v>97513434</v>
       </c>
       <c r="E149" t="s">
         <v>22</v>
@@ -4663,10 +4663,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="D154">
-        <v>865537</v>
+        <v>870037</v>
       </c>
       <c r="E154" t="s">
         <v>22</v>
@@ -4715,10 +4715,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>30951</v>
+        <v>31064</v>
       </c>
       <c r="D156">
-        <v>45444614</v>
+        <v>45606600</v>
       </c>
       <c r="E156" t="s">
         <v>22</v>
@@ -4767,10 +4767,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>11458</v>
+        <v>11501</v>
       </c>
       <c r="D158">
-        <v>16573763</v>
+        <v>16637592</v>
       </c>
       <c r="E158" t="s">
         <v>22</v>
@@ -4819,10 +4819,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="D160">
-        <v>1480896</v>
+        <v>1482396</v>
       </c>
       <c r="E160" t="s">
         <v>22</v>
@@ -4871,10 +4871,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>1248</v>
+        <v>1253</v>
       </c>
       <c r="D162">
-        <v>1766726</v>
+        <v>1774226</v>
       </c>
       <c r="E162" t="s">
         <v>22</v>
@@ -4923,10 +4923,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>209512</v>
+        <v>209991</v>
       </c>
       <c r="D164">
-        <v>261354864</v>
+        <v>261928662</v>
       </c>
       <c r="E164" t="s">
         <v>23</v>
@@ -4975,10 +4975,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D166">
-        <v>216953</v>
+        <v>218453</v>
       </c>
       <c r="E166" t="s">
         <v>23</v>
@@ -5079,10 +5079,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D170">
-        <v>1157290</v>
+        <v>1158790</v>
       </c>
       <c r="E170" t="s">
         <v>23</v>
@@ -5131,10 +5131,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>78971</v>
+        <v>79169</v>
       </c>
       <c r="D172">
-        <v>115874839</v>
+        <v>116157136</v>
       </c>
       <c r="E172" t="s">
         <v>23</v>
@@ -5209,10 +5209,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>29276</v>
+        <v>29377</v>
       </c>
       <c r="D175">
-        <v>42174908</v>
+        <v>42316015</v>
       </c>
       <c r="E175" t="s">
         <v>23</v>
@@ -5287,10 +5287,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>4399</v>
+        <v>4418</v>
       </c>
       <c r="D178">
-        <v>6281886</v>
+        <v>6310386</v>
       </c>
       <c r="E178" t="s">
         <v>23</v>
@@ -5365,10 +5365,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>3694</v>
+        <v>3722</v>
       </c>
       <c r="D181">
-        <v>5138237</v>
+        <v>5178659</v>
       </c>
       <c r="E181" t="s">
         <v>23</v>
@@ -5443,10 +5443,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>228302</v>
+        <v>229021</v>
       </c>
       <c r="D184">
-        <v>283315736</v>
+        <v>284180113</v>
       </c>
       <c r="E184" t="s">
         <v>24</v>
@@ -5469,10 +5469,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D185">
-        <v>148352</v>
+        <v>151352</v>
       </c>
       <c r="E185" t="s">
         <v>24</v>
@@ -5495,10 +5495,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D186">
-        <v>310411</v>
+        <v>311911</v>
       </c>
       <c r="E186" t="s">
         <v>24</v>
@@ -5599,10 +5599,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="D190">
-        <v>804627</v>
+        <v>809382</v>
       </c>
       <c r="E190" t="s">
         <v>24</v>
@@ -5651,10 +5651,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>85561</v>
+        <v>85888</v>
       </c>
       <c r="D192">
-        <v>125321137</v>
+        <v>125786042</v>
       </c>
       <c r="E192" t="s">
         <v>24</v>
@@ -5729,10 +5729,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>45116</v>
+        <v>45307</v>
       </c>
       <c r="D195">
-        <v>65300593</v>
+        <v>65569267</v>
       </c>
       <c r="E195" t="s">
         <v>24</v>
@@ -5807,10 +5807,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>3997</v>
+        <v>4019</v>
       </c>
       <c r="D198">
-        <v>5622948</v>
+        <v>5654667</v>
       </c>
       <c r="E198" t="s">
         <v>24</v>
@@ -5885,10 +5885,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>4282</v>
+        <v>4320</v>
       </c>
       <c r="D201">
-        <v>5931648</v>
+        <v>5981557</v>
       </c>
       <c r="E201" t="s">
         <v>24</v>
@@ -5963,10 +5963,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>93852</v>
+        <v>94085</v>
       </c>
       <c r="D204">
-        <v>118138010</v>
+        <v>118431412</v>
       </c>
       <c r="E204" t="s">
         <v>25</v>
@@ -5989,10 +5989,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D205">
-        <v>67042</v>
+        <v>70104</v>
       </c>
       <c r="E205" t="s">
         <v>25</v>
@@ -6093,10 +6093,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="D209">
-        <v>737912</v>
+        <v>742412</v>
       </c>
       <c r="E209" t="s">
         <v>25</v>
@@ -6145,10 +6145,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>45351</v>
+        <v>45479</v>
       </c>
       <c r="D211">
-        <v>66511046</v>
+        <v>66697294</v>
       </c>
       <c r="E211" t="s">
         <v>25</v>
@@ -6197,10 +6197,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>10900</v>
+        <v>10945</v>
       </c>
       <c r="D213">
-        <v>15687311</v>
+        <v>15750706</v>
       </c>
       <c r="E213" t="s">
         <v>25</v>
@@ -6249,10 +6249,10 @@
         <v>9</v>
       </c>
       <c r="C215">
-        <v>1678</v>
+        <v>1687</v>
       </c>
       <c r="D215">
-        <v>2404945</v>
+        <v>2417347</v>
       </c>
       <c r="E215" t="s">
         <v>25</v>
@@ -6275,10 +6275,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D216">
-        <v>8596</v>
+        <v>10096</v>
       </c>
       <c r="E216" t="s">
         <v>25</v>
@@ -6301,10 +6301,10 @@
         <v>9</v>
       </c>
       <c r="C217">
-        <v>1929</v>
+        <v>1948</v>
       </c>
       <c r="D217">
-        <v>2692450</v>
+        <v>2719580</v>
       </c>
       <c r="E217" t="s">
         <v>25</v>
@@ -6327,10 +6327,10 @@
         <v>9</v>
       </c>
       <c r="C218">
-        <v>224591</v>
+        <v>225212</v>
       </c>
       <c r="D218">
-        <v>284284291</v>
+        <v>285059174</v>
       </c>
       <c r="E218" t="s">
         <v>26</v>
@@ -6353,10 +6353,10 @@
         <v>9</v>
       </c>
       <c r="C219">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D219">
-        <v>183856</v>
+        <v>185356</v>
       </c>
       <c r="E219" t="s">
         <v>26</v>
@@ -6379,10 +6379,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D220">
-        <v>323332</v>
+        <v>324832</v>
       </c>
       <c r="E220" t="s">
         <v>26</v>
@@ -6483,10 +6483,10 @@
         <v>9</v>
       </c>
       <c r="C224">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="D224">
-        <v>1074810</v>
+        <v>1080810</v>
       </c>
       <c r="E224" t="s">
         <v>26</v>
@@ -6535,10 +6535,10 @@
         <v>9</v>
       </c>
       <c r="C226">
-        <v>86153</v>
+        <v>86433</v>
       </c>
       <c r="D226">
-        <v>126404267</v>
+        <v>126808751</v>
       </c>
       <c r="E226" t="s">
         <v>26</v>
@@ -6613,10 +6613,10 @@
         <v>9</v>
       </c>
       <c r="C229">
-        <v>56916</v>
+        <v>57138</v>
       </c>
       <c r="D229">
-        <v>82597270</v>
+        <v>82914285</v>
       </c>
       <c r="E229" t="s">
         <v>26</v>
@@ -6665,10 +6665,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>2072</v>
+        <v>2082</v>
       </c>
       <c r="D231">
-        <v>2927670</v>
+        <v>2942645</v>
       </c>
       <c r="E231" t="s">
         <v>26</v>
@@ -6743,10 +6743,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>3524</v>
+        <v>3542</v>
       </c>
       <c r="D234">
-        <v>4949026</v>
+        <v>4972531</v>
       </c>
       <c r="E234" t="s">
         <v>26</v>
@@ -6769,10 +6769,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>386084</v>
+        <v>387829</v>
       </c>
       <c r="D235">
-        <v>507180829</v>
+        <v>509494954</v>
       </c>
       <c r="E235" t="s">
         <v>27</v>
@@ -6795,10 +6795,10 @@
         <v>9</v>
       </c>
       <c r="C236">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D236">
-        <v>89497</v>
+        <v>90997</v>
       </c>
       <c r="E236" t="s">
         <v>27</v>
@@ -6899,10 +6899,10 @@
         <v>9</v>
       </c>
       <c r="C240">
-        <v>1147</v>
+        <v>1152</v>
       </c>
       <c r="D240">
-        <v>1702051</v>
+        <v>1709551</v>
       </c>
       <c r="E240" t="s">
         <v>27</v>
@@ -6951,10 +6951,10 @@
         <v>9</v>
       </c>
       <c r="C242">
-        <v>178530</v>
+        <v>179221</v>
       </c>
       <c r="D242">
-        <v>262867411</v>
+        <v>263875195</v>
       </c>
       <c r="E242" t="s">
         <v>27</v>
@@ -6977,10 +6977,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D243">
-        <v>470790</v>
+        <v>473790</v>
       </c>
       <c r="E243" t="s">
         <v>27</v>
@@ -7029,10 +7029,10 @@
         <v>9</v>
       </c>
       <c r="C245">
-        <v>148988</v>
+        <v>149596</v>
       </c>
       <c r="D245">
-        <v>216735606</v>
+        <v>217607407</v>
       </c>
       <c r="E245" t="s">
         <v>27</v>
@@ -7081,10 +7081,10 @@
         <v>9</v>
       </c>
       <c r="C247">
-        <v>2214</v>
+        <v>2239</v>
       </c>
       <c r="D247">
-        <v>3109699</v>
+        <v>3141648</v>
       </c>
       <c r="E247" t="s">
         <v>27</v>
@@ -7133,10 +7133,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>4552</v>
+        <v>4586</v>
       </c>
       <c r="D249">
-        <v>6422629</v>
+        <v>6471254</v>
       </c>
       <c r="E249" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:H257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>293035</v>
+        <v>297586</v>
       </c>
       <c r="D2" t="n">
-        <v>374198026</v>
+        <v>379984986</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D3" t="n">
-        <v>285154</v>
+        <v>296174</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D4" t="n">
-        <v>417366</v>
+        <v>423366</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>798</v>
+        <v>810</v>
       </c>
       <c r="D8" t="n">
-        <v>1175544</v>
+        <v>1193544</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>109905</v>
+        <v>111136</v>
       </c>
       <c r="D10" t="n">
-        <v>161174934</v>
+        <v>162971547</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D11" t="n">
-        <v>195328</v>
+        <v>196828</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>54497</v>
+        <v>55292</v>
       </c>
       <c r="D12" t="n">
-        <v>78712845</v>
+        <v>79858373</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3638</v>
+        <v>3671</v>
       </c>
       <c r="D16" t="n">
-        <v>5168439</v>
+        <v>5213366</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" t="n">
-        <v>91274</v>
+        <v>92774</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5509</v>
+        <v>5700</v>
       </c>
       <c r="D20" t="n">
-        <v>7705250</v>
+        <v>7972734</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>71786</v>
+        <v>72786</v>
       </c>
       <c r="D22" t="n">
-        <v>89915303</v>
+        <v>91119379</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24" t="n">
-        <v>51234</v>
+        <v>52734</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D27" t="n">
-        <v>390218</v>
+        <v>396647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30699</v>
+        <v>31029</v>
       </c>
       <c r="D28" t="n">
-        <v>44962641</v>
+        <v>45442692</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" t="n">
-        <v>35654</v>
+        <v>37154</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>10651</v>
+        <v>10780</v>
       </c>
       <c r="D30" t="n">
-        <v>15341793</v>
+        <v>15527971</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1424</v>
+        <v>1446</v>
       </c>
       <c r="D33" t="n">
-        <v>2000572</v>
+        <v>2032002</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1549</v>
+        <v>1580</v>
       </c>
       <c r="D35" t="n">
-        <v>2185879</v>
+        <v>2229864</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>90657</v>
+        <v>91898</v>
       </c>
       <c r="D36" t="n">
-        <v>114609822</v>
+        <v>116115033</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D37" t="n">
-        <v>64493</v>
+        <v>66723</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="D42" t="n">
-        <v>1276961</v>
+        <v>1287461</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42115</v>
+        <v>42551</v>
       </c>
       <c r="D44" t="n">
-        <v>61789186</v>
+        <v>62419576</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D45" t="n">
-        <v>31450</v>
+        <v>32950</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8469</v>
+        <v>8585</v>
       </c>
       <c r="D46" t="n">
-        <v>12165144</v>
+        <v>12331259</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1284</v>
+        <v>1299</v>
       </c>
       <c r="D48" t="n">
-        <v>1781396</v>
+        <v>1801507</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1937</v>
+        <v>2000</v>
       </c>
       <c r="D51" t="n">
-        <v>2695242</v>
+        <v>2785383</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>63741</v>
+        <v>64613</v>
       </c>
       <c r="D52" t="n">
-        <v>80173214</v>
+        <v>81260422</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D53" t="n">
-        <v>35383</v>
+        <v>36883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D56" t="n">
-        <v>534039</v>
+        <v>539844</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>26522</v>
+        <v>26836</v>
       </c>
       <c r="D58" t="n">
-        <v>38916646</v>
+        <v>39372084</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D59" t="n">
-        <v>30000</v>
+        <v>33000</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10244</v>
+        <v>10382</v>
       </c>
       <c r="D61" t="n">
-        <v>14819735</v>
+        <v>15014976</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1263</v>
+        <v>1282</v>
       </c>
       <c r="D63" t="n">
-        <v>1762334</v>
+        <v>1787997</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1241</v>
+        <v>1289</v>
       </c>
       <c r="D67" t="n">
-        <v>1734539</v>
+        <v>1801568</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>18540</v>
+        <v>18936</v>
       </c>
       <c r="D69" t="n">
-        <v>24250742</v>
+        <v>24773881</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D70" t="n">
-        <v>34821</v>
+        <v>37140</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D71" t="n">
-        <v>30225</v>
+        <v>31725</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D72" t="n">
-        <v>75573</v>
+        <v>77073</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>6732</v>
+        <v>6917</v>
       </c>
       <c r="D73" t="n">
-        <v>9850926</v>
+        <v>10121609</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D74" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4597</v>
+        <v>4695</v>
       </c>
       <c r="D75" t="n">
-        <v>6678522</v>
+        <v>6817953</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="D76" t="n">
-        <v>612205</v>
+        <v>624189</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D77" t="n">
-        <v>324608</v>
+        <v>336608</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>130128</v>
+        <v>131945</v>
       </c>
       <c r="D78" t="n">
-        <v>162634338</v>
+        <v>164832494</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D79" t="n">
-        <v>68960</v>
+        <v>74960</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D80" t="n">
-        <v>115879</v>
+        <v>117379</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="D82" t="n">
-        <v>566355</v>
+        <v>580975</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>59860</v>
+        <v>60465</v>
       </c>
       <c r="D84" t="n">
-        <v>87811589</v>
+        <v>88690243</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D85" t="n">
-        <v>109582</v>
+        <v>112582</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>27623</v>
+        <v>27923</v>
       </c>
       <c r="D87" t="n">
-        <v>39980487</v>
+        <v>40416523</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2480</v>
+        <v>2502</v>
       </c>
       <c r="D89" t="n">
-        <v>3573501</v>
+        <v>3605058</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2362</v>
+        <v>2407</v>
       </c>
       <c r="D90" t="n">
-        <v>3333596</v>
+        <v>3396557</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>27298</v>
+        <v>27864</v>
       </c>
       <c r="D91" t="n">
-        <v>37024834</v>
+        <v>37803679</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
-        <v>8302</v>
+        <v>9802</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D93" t="n">
-        <v>12825</v>
+        <v>17325</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6952</v>
+        <v>7049</v>
       </c>
       <c r="D95" t="n">
-        <v>10243035</v>
+        <v>10386856</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6140</v>
+        <v>6270</v>
       </c>
       <c r="D97" t="n">
-        <v>8899126</v>
+        <v>9090688</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D99" t="n">
-        <v>607667</v>
+        <v>613667</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="D100" t="n">
-        <v>597329</v>
+        <v>611752</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>6694</v>
+        <v>6909</v>
       </c>
       <c r="D101" t="n">
-        <v>9286497</v>
+        <v>9588403</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1690</v>
+        <v>1744</v>
       </c>
       <c r="D103" t="n">
-        <v>2485456</v>
+        <v>2564779</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D104" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2256</v>
+        <v>2330</v>
       </c>
       <c r="D105" t="n">
-        <v>3285962</v>
+        <v>3396667</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D107" t="n">
-        <v>125390</v>
+        <v>140390</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D108" t="n">
-        <v>156189</v>
+        <v>159189</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>130862</v>
+        <v>132634</v>
       </c>
       <c r="D109" t="n">
-        <v>162026521</v>
+        <v>164218537</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D111" t="n">
-        <v>92374</v>
+        <v>95374</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="D113" t="n">
-        <v>1332805</v>
+        <v>1343763</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>49884</v>
+        <v>50402</v>
       </c>
       <c r="D115" t="n">
-        <v>73178708</v>
+        <v>73928290</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D116" t="n">
-        <v>119159</v>
+        <v>120659</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>24943</v>
+        <v>25268</v>
       </c>
       <c r="D117" t="n">
-        <v>36139237</v>
+        <v>36615551</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1192</v>
+        <v>1208</v>
       </c>
       <c r="D118" t="n">
-        <v>1628010</v>
+        <v>1648815</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1917</v>
+        <v>1958</v>
       </c>
       <c r="D121" t="n">
-        <v>2691247</v>
+        <v>2750038</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>432650</v>
+        <v>444074</v>
       </c>
       <c r="D123" t="n">
-        <v>569677194</v>
+        <v>584966139</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D124" t="n">
-        <v>102117</v>
+        <v>105117</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D125" t="n">
-        <v>287743</v>
+        <v>289243</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1243</v>
+        <v>1253</v>
       </c>
       <c r="D128" t="n">
-        <v>1843976</v>
+        <v>1858976</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D129" t="n">
-        <v>30773</v>
+        <v>32273</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>189206</v>
+        <v>192091</v>
       </c>
       <c r="D130" t="n">
-        <v>278341082</v>
+        <v>282566342</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="D131" t="n">
-        <v>508290</v>
+        <v>524790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D132" t="n">
-        <v>18000</v>
+        <v>19500</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>160240</v>
+        <v>163626</v>
       </c>
       <c r="D133" t="n">
-        <v>232978981</v>
+        <v>237907270</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2436</v>
+        <v>2513</v>
       </c>
       <c r="D136" t="n">
-        <v>3412324</v>
+        <v>3522827</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5127</v>
+        <v>5292</v>
       </c>
       <c r="D138" t="n">
-        <v>7231379</v>
+        <v>7468266</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>39656</v>
+        <v>40642</v>
       </c>
       <c r="D141" t="n">
-        <v>53087681</v>
+        <v>54410493</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D142" t="n">
-        <v>32653</v>
+        <v>33791</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13008</v>
+        <v>13246</v>
       </c>
       <c r="D147" t="n">
-        <v>19106021</v>
+        <v>19451396</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3399</v>
+        <v>3469</v>
       </c>
       <c r="D148" t="n">
-        <v>4909250</v>
+        <v>5005490</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D151" t="n">
-        <v>501648</v>
+        <v>510648</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D153" t="n">
-        <v>471309</v>
+        <v>472809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>15400</v>
+        <v>15713</v>
       </c>
       <c r="D154" t="n">
-        <v>20419852</v>
+        <v>20829410</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6455</v>
+        <v>6558</v>
       </c>
       <c r="D158" t="n">
-        <v>9405859</v>
+        <v>9548386</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4365</v>
+        <v>4449</v>
       </c>
       <c r="D160" t="n">
-        <v>6294090</v>
+        <v>6414779</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D162" t="n">
-        <v>332078</v>
+        <v>337960</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D163" t="n">
-        <v>305545</v>
+        <v>315096</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>11425</v>
+        <v>12126</v>
       </c>
       <c r="D165" t="n">
-        <v>16527440</v>
+        <v>17555372</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1456</v>
+        <v>1518</v>
       </c>
       <c r="D166" t="n">
-        <v>2165478</v>
+        <v>2257798</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D167" t="n">
-        <v>295671</v>
+        <v>299302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D168" t="n">
-        <v>43190</v>
+        <v>6000</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6745,12 +6745,12 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="D169" t="n">
-        <v>106449</v>
+        <v>44690</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6783,12 +6783,12 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6804,29 +6804,29 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>81364</v>
+        <v>72</v>
       </c>
       <c r="D170" t="n">
-        <v>102054471</v>
+        <v>107949</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>06</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Normandie</t>
+          <t>Mayotte</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>26</v>
+        <v>82445</v>
       </c>
       <c r="D171" t="n">
-        <v>31729</v>
+        <v>103360445</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6859,12 +6859,12 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="D172" t="n">
-        <v>120144</v>
+        <v>33229</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6897,12 +6897,12 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="D173" t="n">
-        <v>3961</v>
+        <v>120144</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6935,12 +6935,12 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D174" t="n">
-        <v>17820</v>
+        <v>3961</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6973,12 +6973,12 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>617</v>
+        <v>12</v>
       </c>
       <c r="D175" t="n">
-        <v>910426</v>
+        <v>17820</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7011,12 +7011,12 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>4</v>
+        <v>620</v>
       </c>
       <c r="D176" t="n">
-        <v>6000</v>
+        <v>914844</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7049,12 +7049,12 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>32083</v>
+        <v>4</v>
       </c>
       <c r="D177" t="n">
-        <v>47076175</v>
+        <v>6000</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7087,12 +7087,12 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>22</v>
+        <v>32396</v>
       </c>
       <c r="D178" t="n">
-        <v>33000</v>
+        <v>47529252</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7125,12 +7125,12 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>12050</v>
+        <v>22</v>
       </c>
       <c r="D179" t="n">
-        <v>17423946</v>
+        <v>33000</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7163,12 +7163,12 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>9</v>
+        <v>12208</v>
       </c>
       <c r="D180" t="n">
-        <v>12419</v>
+        <v>17654514</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7201,12 +7201,12 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1144</v>
+        <v>9</v>
       </c>
       <c r="D181" t="n">
-        <v>1600691</v>
+        <v>12419</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7239,12 +7239,12 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>3</v>
+        <v>1152</v>
       </c>
       <c r="D182" t="n">
-        <v>4500</v>
+        <v>1610129</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7277,12 +7277,12 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1392</v>
+        <v>4</v>
       </c>
       <c r="D183" t="n">
-        <v>1954051</v>
+        <v>5839</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7315,12 +7315,12 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>3</v>
+        <v>1427</v>
       </c>
       <c r="D184" t="n">
-        <v>4500</v>
+        <v>2003236</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7353,12 +7353,12 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -7374,29 +7374,29 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>219646</v>
+        <v>3</v>
       </c>
       <c r="D185" t="n">
-        <v>273562852</v>
+        <v>4500</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Nouvelle-Aquitaine</t>
+          <t>Normandie</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>124</v>
+        <v>222862</v>
       </c>
       <c r="D186" t="n">
-        <v>132870</v>
+        <v>277484626</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7429,12 +7429,12 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="D187" t="n">
-        <v>231736</v>
+        <v>136670</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7467,12 +7467,12 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="D188" t="n">
-        <v>6741</v>
+        <v>231736</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7505,12 +7505,12 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D189" t="n">
-        <v>13500</v>
+        <v>6741</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7543,12 +7543,12 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>Paroisse hors zone concordataire</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D190" t="n">
-        <v>10795</v>
+        <v>13500</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7581,12 +7581,12 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Paroisse hors zone concordataire</t>
         </is>
       </c>
     </row>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>827</v>
+        <v>10</v>
       </c>
       <c r="D191" t="n">
-        <v>1216284</v>
+        <v>10795</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7619,12 +7619,12 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>7</v>
+        <v>836</v>
       </c>
       <c r="D192" t="n">
-        <v>9883</v>
+        <v>1229784</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7657,12 +7657,12 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>81896</v>
+        <v>7</v>
       </c>
       <c r="D193" t="n">
-        <v>120099898</v>
+        <v>9883</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7695,12 +7695,12 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>89</v>
+        <v>82811</v>
       </c>
       <c r="D194" t="n">
-        <v>129127</v>
+        <v>121425956</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7733,12 +7733,12 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="D195" t="n">
-        <v>6000</v>
+        <v>129127</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7771,12 +7771,12 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>30618</v>
+        <v>4</v>
       </c>
       <c r="D196" t="n">
-        <v>44083003</v>
+        <v>6000</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7809,12 +7809,12 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>24</v>
+        <v>31039</v>
       </c>
       <c r="D197" t="n">
-        <v>36000</v>
+        <v>44687424</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7847,12 +7847,12 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D198" t="n">
-        <v>17608</v>
+        <v>36000</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7885,12 +7885,12 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>4639</v>
+        <v>13</v>
       </c>
       <c r="D199" t="n">
-        <v>6610350</v>
+        <v>17608</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7923,12 +7923,12 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>3</v>
+        <v>4690</v>
       </c>
       <c r="D200" t="n">
-        <v>4500</v>
+        <v>6682601</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7961,12 +7961,12 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Comité d'entreprise</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D201" t="n">
-        <v>15000</v>
+        <v>4500</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -7999,12 +7999,12 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Comité d'entreprise</t>
         </is>
       </c>
     </row>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>4081</v>
+        <v>10</v>
       </c>
       <c r="D202" t="n">
-        <v>5661348</v>
+        <v>15000</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8037,12 +8037,12 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>3</v>
+        <v>4193</v>
       </c>
       <c r="D203" t="n">
-        <v>4500</v>
+        <v>5813179</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8075,12 +8075,12 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D204" t="n">
-        <v>10447</v>
+        <v>6000</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8113,12 +8113,12 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -8134,29 +8134,29 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>240633</v>
+        <v>9</v>
       </c>
       <c r="D205" t="n">
-        <v>298249915</v>
+        <v>11947</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Occitanie</t>
+          <t>Nouvelle-Aquitaine</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>145</v>
+        <v>244437</v>
       </c>
       <c r="D206" t="n">
-        <v>157190</v>
+        <v>302855013</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8189,12 +8189,12 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>233</v>
+        <v>147</v>
       </c>
       <c r="D207" t="n">
-        <v>332911</v>
+        <v>160190</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8227,12 +8227,12 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>13</v>
+        <v>236</v>
       </c>
       <c r="D208" t="n">
-        <v>18100</v>
+        <v>337411</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8265,12 +8265,12 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D209" t="n">
-        <v>10552</v>
+        <v>19435</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8303,12 +8303,12 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D210" t="n">
-        <v>4500</v>
+        <v>10552</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8341,12 +8341,12 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -8379,12 +8379,12 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>577</v>
+        <v>3</v>
       </c>
       <c r="D212" t="n">
-        <v>842127</v>
+        <v>4500</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8417,12 +8417,12 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>5</v>
+        <v>585</v>
       </c>
       <c r="D213" t="n">
-        <v>7500</v>
+        <v>853140</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8455,12 +8455,12 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>89012</v>
+        <v>5</v>
       </c>
       <c r="D214" t="n">
-        <v>130295849</v>
+        <v>7500</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8493,12 +8493,12 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>79</v>
+        <v>90035</v>
       </c>
       <c r="D215" t="n">
-        <v>117699</v>
+        <v>131789259</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8531,12 +8531,12 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="D216" t="n">
-        <v>10500</v>
+        <v>120699</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8569,12 +8569,12 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>47382</v>
+        <v>7</v>
       </c>
       <c r="D217" t="n">
-        <v>68536813</v>
+        <v>10500</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8607,12 +8607,12 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>27</v>
+        <v>48031</v>
       </c>
       <c r="D218" t="n">
-        <v>39075</v>
+        <v>69476033</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8645,12 +8645,12 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D219" t="n">
-        <v>24160</v>
+        <v>39075</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8683,12 +8683,12 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>4263</v>
+        <v>17</v>
       </c>
       <c r="D220" t="n">
-        <v>5982934</v>
+        <v>24160</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8721,12 +8721,12 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>6</v>
+        <v>4307</v>
       </c>
       <c r="D221" t="n">
-        <v>9000</v>
+        <v>6045215</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8759,12 +8759,12 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D222" t="n">
-        <v>22212</v>
+        <v>9000</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8797,12 +8797,12 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>69</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
         </is>
       </c>
     </row>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4733</v>
+        <v>17</v>
       </c>
       <c r="D223" t="n">
-        <v>6537275</v>
+        <v>25212</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8835,12 +8835,12 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>6</v>
+        <v>4876</v>
       </c>
       <c r="D224" t="n">
-        <v>9000</v>
+        <v>6734619</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8873,12 +8873,12 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -8911,12 +8911,12 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -8932,29 +8932,29 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>98118</v>
+        <v>6</v>
       </c>
       <c r="D226" t="n">
-        <v>123197706</v>
+        <v>9000</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>76</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>Pays de la Loire</t>
+          <t>Occitanie</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>67</v>
+        <v>99539</v>
       </c>
       <c r="D227" t="n">
-        <v>69152</v>
+        <v>124921906</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -8987,12 +8987,12 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D228" t="n">
-        <v>94477</v>
+        <v>73652</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9025,12 +9025,12 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="D229" t="n">
-        <v>11147</v>
+        <v>98945</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9063,12 +9063,12 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D230" t="n">
-        <v>3655</v>
+        <v>11147</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9101,12 +9101,12 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>537</v>
+        <v>3</v>
       </c>
       <c r="D231" t="n">
-        <v>785235</v>
+        <v>3655</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9139,12 +9139,12 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>4</v>
+        <v>540</v>
       </c>
       <c r="D232" t="n">
-        <v>2563</v>
+        <v>789735</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9177,12 +9177,12 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>46868</v>
+        <v>4</v>
       </c>
       <c r="D233" t="n">
-        <v>68700415</v>
+        <v>2563</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9215,12 +9215,12 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>29</v>
+        <v>47375</v>
       </c>
       <c r="D234" t="n">
-        <v>41211</v>
+        <v>69440364</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9253,12 +9253,12 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>11423</v>
+        <v>31</v>
       </c>
       <c r="D235" t="n">
-        <v>16429999</v>
+        <v>44211</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9291,12 +9291,12 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12</v>
+        <v>11578</v>
       </c>
       <c r="D236" t="n">
-        <v>12204</v>
+        <v>16654580</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9329,12 +9329,12 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>1780</v>
+        <v>12</v>
       </c>
       <c r="D237" t="n">
-        <v>2553013</v>
+        <v>12204</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9367,12 +9367,12 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>7</v>
+        <v>1791</v>
       </c>
       <c r="D238" t="n">
-        <v>8596</v>
+        <v>2569013</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9405,12 +9405,12 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>2178</v>
+        <v>7</v>
       </c>
       <c r="D239" t="n">
-        <v>3035140</v>
+        <v>8596</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9443,12 +9443,12 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -9464,29 +9464,29 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>235860</v>
+        <v>2225</v>
       </c>
       <c r="D240" t="n">
-        <v>298233852</v>
+        <v>3102944</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>156</v>
+        <v>239500</v>
       </c>
       <c r="D241" t="n">
-        <v>193801</v>
+        <v>302814010</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9519,12 +9519,12 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="D242" t="n">
-        <v>334092</v>
+        <v>199801</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9557,12 +9557,12 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="D243" t="n">
-        <v>19500</v>
+        <v>337947</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9595,12 +9595,12 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D244" t="n">
-        <v>22500</v>
+        <v>19500</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9633,12 +9633,12 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D245" t="n">
-        <v>15980</v>
+        <v>22500</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9671,12 +9671,12 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>766</v>
+        <v>11</v>
       </c>
       <c r="D246" t="n">
-        <v>1127064</v>
+        <v>15980</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9709,12 +9709,12 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>9</v>
+        <v>781</v>
       </c>
       <c r="D247" t="n">
-        <v>13500</v>
+        <v>1149564</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9747,12 +9747,12 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>89683</v>
+        <v>9</v>
       </c>
       <c r="D248" t="n">
-        <v>131489248</v>
+        <v>13500</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9785,12 +9785,12 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>73</v>
+        <v>90785</v>
       </c>
       <c r="D249" t="n">
-        <v>106661</v>
+        <v>133109323</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9823,12 +9823,12 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D250" t="n">
-        <v>6000</v>
+        <v>106661</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9861,12 +9861,12 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>59677</v>
+        <v>4</v>
       </c>
       <c r="D251" t="n">
-        <v>86547365</v>
+        <v>6000</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9899,12 +9899,12 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>15</v>
+        <v>60529</v>
       </c>
       <c r="D252" t="n">
-        <v>22489</v>
+        <v>87777601</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9937,12 +9937,12 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>2208</v>
+        <v>15</v>
       </c>
       <c r="D253" t="n">
-        <v>3113382</v>
+        <v>22489</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9975,12 +9975,12 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>10</v>
+        <v>2239</v>
       </c>
       <c r="D254" t="n">
-        <v>15000</v>
+        <v>3156292</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10013,12 +10013,12 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D255" t="n">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10051,12 +10051,12 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>3880</v>
+        <v>6</v>
       </c>
       <c r="D256" t="n">
-        <v>5445171</v>
+        <v>9000</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10089,10 +10089,48 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>Syndicat de propriétaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>3994</v>
+      </c>
+      <c r="D257" t="n">
+        <v>5602412</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
           <t>92</t>
         </is>
       </c>
-      <c r="H256" t="inlineStr">
+      <c r="H257" t="inlineStr">
         <is>
           <t>Association loi 1901 ou assimilé</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-23 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>297586</v>
+        <v>300912</v>
       </c>
       <c r="D2" t="n">
-        <v>379984986</v>
+        <v>384142141</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D3" t="n">
-        <v>296174</v>
+        <v>296759</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="D4" t="n">
-        <v>423366</v>
+        <v>430843</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>6977</v>
+        <v>12977</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>810</v>
+        <v>819</v>
       </c>
       <c r="D8" t="n">
-        <v>1193544</v>
+        <v>1207044</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>111136</v>
+        <v>112087</v>
       </c>
       <c r="D10" t="n">
-        <v>162971547</v>
+        <v>164355739</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>55292</v>
+        <v>55901</v>
       </c>
       <c r="D12" t="n">
-        <v>79858373</v>
+        <v>80731063</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3671</v>
+        <v>3727</v>
       </c>
       <c r="D16" t="n">
-        <v>5213366</v>
+        <v>5294333</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D19" t="n">
-        <v>92774</v>
+        <v>97035</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5700</v>
+        <v>5831</v>
       </c>
       <c r="D20" t="n">
-        <v>7972734</v>
+        <v>8154995</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>72786</v>
+        <v>73450</v>
       </c>
       <c r="D22" t="n">
-        <v>91119379</v>
+        <v>91938622</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24" t="n">
-        <v>52734</v>
+        <v>54234</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D27" t="n">
-        <v>396647</v>
+        <v>402647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31029</v>
+        <v>31261</v>
       </c>
       <c r="D28" t="n">
-        <v>45442692</v>
+        <v>45780683</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>37154</v>
+        <v>37404</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>10780</v>
+        <v>10902</v>
       </c>
       <c r="D30" t="n">
-        <v>15527971</v>
+        <v>15701622</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1446</v>
+        <v>1456</v>
       </c>
       <c r="D33" t="n">
-        <v>2032002</v>
+        <v>2047002</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1580</v>
+        <v>1614</v>
       </c>
       <c r="D35" t="n">
-        <v>2229864</v>
+        <v>2278504</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>91898</v>
+        <v>92685</v>
       </c>
       <c r="D36" t="n">
-        <v>116115033</v>
+        <v>117046485</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="D42" t="n">
-        <v>1287461</v>
+        <v>1296509</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42551</v>
+        <v>42891</v>
       </c>
       <c r="D44" t="n">
-        <v>62419576</v>
+        <v>62912290</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D45" t="n">
-        <v>32950</v>
+        <v>34450</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8585</v>
+        <v>8677</v>
       </c>
       <c r="D46" t="n">
-        <v>12331259</v>
+        <v>12461416</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1299</v>
+        <v>1312</v>
       </c>
       <c r="D48" t="n">
-        <v>1801507</v>
+        <v>1819204</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2000</v>
+        <v>2046</v>
       </c>
       <c r="D51" t="n">
-        <v>2785383</v>
+        <v>2849071</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>64613</v>
+        <v>65280</v>
       </c>
       <c r="D52" t="n">
-        <v>81260422</v>
+        <v>82052579</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="D56" t="n">
-        <v>539844</v>
+        <v>550344</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>26836</v>
+        <v>27034</v>
       </c>
       <c r="D58" t="n">
-        <v>39372084</v>
+        <v>39660962</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10382</v>
+        <v>10465</v>
       </c>
       <c r="D61" t="n">
-        <v>15014976</v>
+        <v>15136817</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1282</v>
+        <v>1289</v>
       </c>
       <c r="D63" t="n">
-        <v>1787997</v>
+        <v>1798080</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1289</v>
+        <v>1316</v>
       </c>
       <c r="D67" t="n">
-        <v>1801568</v>
+        <v>1838451</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>18936</v>
+        <v>19189</v>
       </c>
       <c r="D69" t="n">
-        <v>24773881</v>
+        <v>25115648</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D70" t="n">
-        <v>37140</v>
+        <v>38640</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D71" t="n">
-        <v>31725</v>
+        <v>34725</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>6917</v>
+        <v>7038</v>
       </c>
       <c r="D73" t="n">
-        <v>10121609</v>
+        <v>10299944</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4695</v>
+        <v>4778</v>
       </c>
       <c r="D75" t="n">
-        <v>6817953</v>
+        <v>6937281</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="D76" t="n">
-        <v>624189</v>
+        <v>634689</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D77" t="n">
-        <v>336608</v>
+        <v>341108</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>131945</v>
+        <v>133228</v>
       </c>
       <c r="D78" t="n">
-        <v>164832494</v>
+        <v>166410907</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D79" t="n">
-        <v>74960</v>
+        <v>76460</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D80" t="n">
-        <v>117379</v>
+        <v>118186</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D82" t="n">
-        <v>580975</v>
+        <v>588475</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>60465</v>
+        <v>61011</v>
       </c>
       <c r="D84" t="n">
-        <v>88690243</v>
+        <v>89478666</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>27923</v>
+        <v>28183</v>
       </c>
       <c r="D87" t="n">
-        <v>40416523</v>
+        <v>40801618</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2502</v>
+        <v>2524</v>
       </c>
       <c r="D89" t="n">
-        <v>3605058</v>
+        <v>3637425</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2407</v>
+        <v>2477</v>
       </c>
       <c r="D90" t="n">
-        <v>3396557</v>
+        <v>3494448</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>27864</v>
+        <v>28496</v>
       </c>
       <c r="D91" t="n">
-        <v>37803679</v>
+        <v>38669069</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D94" t="n">
-        <v>32099</v>
+        <v>35814</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7049</v>
+        <v>7178</v>
       </c>
       <c r="D95" t="n">
-        <v>10386856</v>
+        <v>10575520</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6270</v>
+        <v>6389</v>
       </c>
       <c r="D97" t="n">
-        <v>9090688</v>
+        <v>9260975</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>433</v>
+        <v>455</v>
       </c>
       <c r="D99" t="n">
-        <v>613667</v>
+        <v>645943</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="D100" t="n">
-        <v>611752</v>
+        <v>632481</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>6909</v>
+        <v>7134</v>
       </c>
       <c r="D101" t="n">
-        <v>9588403</v>
+        <v>9903273</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1744</v>
+        <v>1812</v>
       </c>
       <c r="D103" t="n">
-        <v>2564779</v>
+        <v>2666618</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D104" t="n">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2330</v>
+        <v>2462</v>
       </c>
       <c r="D105" t="n">
-        <v>3396667</v>
+        <v>3593112</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D107" t="n">
-        <v>140390</v>
+        <v>142690</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D108" t="n">
-        <v>159189</v>
+        <v>172689</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>132634</v>
+        <v>133871</v>
       </c>
       <c r="D109" t="n">
-        <v>164218537</v>
+        <v>165707896</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D110" t="n">
-        <v>41717</v>
+        <v>43217</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D111" t="n">
-        <v>95374</v>
+        <v>96874</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D112" t="n">
-        <v>7395</v>
+        <v>8895</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>50402</v>
+        <v>50805</v>
       </c>
       <c r="D115" t="n">
-        <v>73928290</v>
+        <v>74505951</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D116" t="n">
-        <v>120659</v>
+        <v>122159</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25268</v>
+        <v>25525</v>
       </c>
       <c r="D117" t="n">
-        <v>36615551</v>
+        <v>36985505</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1208</v>
+        <v>1214</v>
       </c>
       <c r="D118" t="n">
-        <v>1648815</v>
+        <v>1656952</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1958</v>
+        <v>2002</v>
       </c>
       <c r="D121" t="n">
-        <v>2750038</v>
+        <v>2813844</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>444074</v>
+        <v>453008</v>
       </c>
       <c r="D123" t="n">
-        <v>584966139</v>
+        <v>596918027</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D124" t="n">
-        <v>105117</v>
+        <v>108117</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D125" t="n">
-        <v>289243</v>
+        <v>290743</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1253</v>
+        <v>1276</v>
       </c>
       <c r="D128" t="n">
-        <v>1858976</v>
+        <v>1893155</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D129" t="n">
-        <v>32273</v>
+        <v>36773</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>192091</v>
+        <v>194577</v>
       </c>
       <c r="D130" t="n">
-        <v>282566342</v>
+        <v>286210199</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D131" t="n">
-        <v>524790</v>
+        <v>527790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>163626</v>
+        <v>166199</v>
       </c>
       <c r="D133" t="n">
-        <v>237907270</v>
+        <v>241661406</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2513</v>
+        <v>2572</v>
       </c>
       <c r="D136" t="n">
-        <v>3522827</v>
+        <v>3607067</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D137" t="n">
-        <v>14722</v>
+        <v>16222</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5292</v>
+        <v>5418</v>
       </c>
       <c r="D138" t="n">
-        <v>7468266</v>
+        <v>7650963</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D140" t="n">
-        <v>22500</v>
+        <v>24000</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>40642</v>
+        <v>41266</v>
       </c>
       <c r="D141" t="n">
-        <v>54410493</v>
+        <v>55223901</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D142" t="n">
-        <v>33791</v>
+        <v>35291</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>322</v>
+        <v>355</v>
       </c>
       <c r="D146" t="n">
-        <v>482665</v>
+        <v>532165</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13246</v>
+        <v>13379</v>
       </c>
       <c r="D147" t="n">
-        <v>19451396</v>
+        <v>19643189</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3469</v>
+        <v>3511</v>
       </c>
       <c r="D148" t="n">
-        <v>5005490</v>
+        <v>5066464</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D151" t="n">
-        <v>510648</v>
+        <v>516519</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D153" t="n">
-        <v>472809</v>
+        <v>475809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>15713</v>
+        <v>15952</v>
       </c>
       <c r="D154" t="n">
-        <v>20829410</v>
+        <v>21135979</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6558</v>
+        <v>6628</v>
       </c>
       <c r="D158" t="n">
-        <v>9548386</v>
+        <v>9651353</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4449</v>
+        <v>4517</v>
       </c>
       <c r="D160" t="n">
-        <v>6414779</v>
+        <v>6510041</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D162" t="n">
-        <v>337960</v>
+        <v>343960</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>12126</v>
+        <v>12718</v>
       </c>
       <c r="D165" t="n">
-        <v>17555372</v>
+        <v>18420635</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1518</v>
+        <v>1572</v>
       </c>
       <c r="D166" t="n">
-        <v>2257798</v>
+        <v>2338038</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D167" t="n">
-        <v>299302</v>
+        <v>308302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D169" t="n">
-        <v>44690</v>
+        <v>49190</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D170" t="n">
-        <v>107949</v>
+        <v>110949</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>82445</v>
+        <v>83238</v>
       </c>
       <c r="D171" t="n">
-        <v>103360445</v>
+        <v>104298393</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D176" t="n">
-        <v>914844</v>
+        <v>919146</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32396</v>
+        <v>32625</v>
       </c>
       <c r="D178" t="n">
-        <v>47529252</v>
+        <v>47861104</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D179" t="n">
-        <v>33000</v>
+        <v>37500</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12208</v>
+        <v>12346</v>
       </c>
       <c r="D180" t="n">
-        <v>17654514</v>
+        <v>17848959</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1152</v>
+        <v>1163</v>
       </c>
       <c r="D182" t="n">
-        <v>1610129</v>
+        <v>1625980</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1427</v>
+        <v>1454</v>
       </c>
       <c r="D184" t="n">
-        <v>2003236</v>
+        <v>2043172</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>222862</v>
+        <v>225192</v>
       </c>
       <c r="D186" t="n">
-        <v>277484626</v>
+        <v>280296424</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D187" t="n">
-        <v>136670</v>
+        <v>138170</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D188" t="n">
-        <v>231736</v>
+        <v>233236</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="D192" t="n">
-        <v>1229784</v>
+        <v>1237997</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>82811</v>
+        <v>83459</v>
       </c>
       <c r="D194" t="n">
-        <v>121425956</v>
+        <v>122371239</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31039</v>
+        <v>31332</v>
       </c>
       <c r="D197" t="n">
-        <v>44687424</v>
+        <v>45113705</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D198" t="n">
-        <v>36000</v>
+        <v>37500</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4690</v>
+        <v>4736</v>
       </c>
       <c r="D200" t="n">
-        <v>6682601</v>
+        <v>6746743</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4193</v>
+        <v>4292</v>
       </c>
       <c r="D203" t="n">
-        <v>5813179</v>
+        <v>5950644</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>244437</v>
+        <v>247267</v>
       </c>
       <c r="D206" t="n">
-        <v>302855013</v>
+        <v>306283472</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D207" t="n">
-        <v>160190</v>
+        <v>161690</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D209" t="n">
-        <v>19435</v>
+        <v>20935</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D210" t="n">
-        <v>10552</v>
+        <v>12052</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="D213" t="n">
-        <v>853140</v>
+        <v>859356</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>90035</v>
+        <v>90827</v>
       </c>
       <c r="D215" t="n">
-        <v>131789259</v>
+        <v>132938878</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>48031</v>
+        <v>48547</v>
       </c>
       <c r="D218" t="n">
-        <v>69476033</v>
+        <v>70220470</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4307</v>
+        <v>4343</v>
       </c>
       <c r="D221" t="n">
-        <v>6045215</v>
+        <v>6096509</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>4876</v>
+        <v>5003</v>
       </c>
       <c r="D224" t="n">
-        <v>6734619</v>
+        <v>6915375</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>99539</v>
+        <v>100615</v>
       </c>
       <c r="D227" t="n">
-        <v>124921906</v>
+        <v>126188976</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D228" t="n">
-        <v>73652</v>
+        <v>75152</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D232" t="n">
-        <v>789735</v>
+        <v>792339</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>47375</v>
+        <v>47756</v>
       </c>
       <c r="D234" t="n">
-        <v>69440364</v>
+        <v>69990328</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D235" t="n">
-        <v>44211</v>
+        <v>45711</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11578</v>
+        <v>11716</v>
       </c>
       <c r="D236" t="n">
-        <v>16654580</v>
+        <v>16852847</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1791</v>
+        <v>1798</v>
       </c>
       <c r="D238" t="n">
-        <v>2569013</v>
+        <v>2579513</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2225</v>
+        <v>2271</v>
       </c>
       <c r="D240" t="n">
-        <v>3102944</v>
+        <v>3167473</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>239500</v>
+        <v>242305</v>
       </c>
       <c r="D241" t="n">
-        <v>302814010</v>
+        <v>306370821</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D243" t="n">
-        <v>337947</v>
+        <v>341457</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="D247" t="n">
-        <v>1149564</v>
+        <v>1157064</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>90785</v>
+        <v>91658</v>
       </c>
       <c r="D249" t="n">
-        <v>133109323</v>
+        <v>134381634</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>60529</v>
+        <v>61227</v>
       </c>
       <c r="D252" t="n">
-        <v>87777601</v>
+        <v>88782246</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D253" t="n">
-        <v>22489</v>
+        <v>23989</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2239</v>
+        <v>2271</v>
       </c>
       <c r="D254" t="n">
-        <v>3156292</v>
+        <v>3204242</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>3994</v>
+        <v>4074</v>
       </c>
       <c r="D257" t="n">
-        <v>5602412</v>
+        <v>5714907</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>300912</v>
+        <v>302841</v>
       </c>
       <c r="D2" t="n">
-        <v>384142141</v>
+        <v>386545519</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D3" t="n">
-        <v>296759</v>
+        <v>297311</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D8" t="n">
-        <v>1207044</v>
+        <v>1208544</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>112087</v>
+        <v>112538</v>
       </c>
       <c r="D10" t="n">
-        <v>164355739</v>
+        <v>165002681</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>55901</v>
+        <v>56281</v>
       </c>
       <c r="D12" t="n">
-        <v>80731063</v>
+        <v>81278020</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" t="n">
-        <v>62059</v>
+        <v>63559</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3727</v>
+        <v>3739</v>
       </c>
       <c r="D16" t="n">
-        <v>5294333</v>
+        <v>5309577</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5831</v>
+        <v>5886</v>
       </c>
       <c r="D20" t="n">
-        <v>8154995</v>
+        <v>8231054</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>73450</v>
+        <v>73846</v>
       </c>
       <c r="D22" t="n">
-        <v>91938622</v>
+        <v>92392725</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D27" t="n">
-        <v>402647</v>
+        <v>404147</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31261</v>
+        <v>31365</v>
       </c>
       <c r="D28" t="n">
-        <v>45780683</v>
+        <v>45934396</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>10902</v>
+        <v>10956</v>
       </c>
       <c r="D30" t="n">
-        <v>15701622</v>
+        <v>15779222</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1456</v>
+        <v>1464</v>
       </c>
       <c r="D33" t="n">
-        <v>2047002</v>
+        <v>2056887</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1614</v>
+        <v>1624</v>
       </c>
       <c r="D35" t="n">
-        <v>2278504</v>
+        <v>2291538</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>92685</v>
+        <v>93146</v>
       </c>
       <c r="D36" t="n">
-        <v>117046485</v>
+        <v>117574866</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D37" t="n">
-        <v>66723</v>
+        <v>69477</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D38" t="n">
-        <v>102653</v>
+        <v>105528</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="D42" t="n">
-        <v>1296509</v>
+        <v>1303772</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42891</v>
+        <v>43068</v>
       </c>
       <c r="D44" t="n">
-        <v>62912290</v>
+        <v>63163909</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8677</v>
+        <v>8728</v>
       </c>
       <c r="D46" t="n">
-        <v>12461416</v>
+        <v>12532183</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1312</v>
+        <v>1322</v>
       </c>
       <c r="D48" t="n">
-        <v>1819204</v>
+        <v>1830857</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2046</v>
+        <v>2063</v>
       </c>
       <c r="D51" t="n">
-        <v>2849071</v>
+        <v>2873497</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>65280</v>
+        <v>65657</v>
       </c>
       <c r="D52" t="n">
-        <v>82052579</v>
+        <v>82496390</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D56" t="n">
-        <v>550344</v>
+        <v>551844</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27034</v>
+        <v>27155</v>
       </c>
       <c r="D58" t="n">
-        <v>39660962</v>
+        <v>39833781</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10465</v>
+        <v>10535</v>
       </c>
       <c r="D61" t="n">
-        <v>15136817</v>
+        <v>15241201</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1289</v>
+        <v>1299</v>
       </c>
       <c r="D63" t="n">
-        <v>1798080</v>
+        <v>1810872</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1316</v>
+        <v>1332</v>
       </c>
       <c r="D67" t="n">
-        <v>1838451</v>
+        <v>1860599</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19189</v>
+        <v>19329</v>
       </c>
       <c r="D69" t="n">
-        <v>25115648</v>
+        <v>25305578</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7038</v>
+        <v>7100</v>
       </c>
       <c r="D73" t="n">
-        <v>10299944</v>
+        <v>10392921</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4778</v>
+        <v>4809</v>
       </c>
       <c r="D75" t="n">
-        <v>6937281</v>
+        <v>6982002</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="D76" t="n">
-        <v>634689</v>
+        <v>643689</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D77" t="n">
-        <v>341108</v>
+        <v>342608</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>133228</v>
+        <v>133934</v>
       </c>
       <c r="D78" t="n">
-        <v>166410907</v>
+        <v>167260783</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D82" t="n">
-        <v>588475</v>
+        <v>591475</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D83" t="n">
-        <v>14438</v>
+        <v>15938</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61011</v>
+        <v>61249</v>
       </c>
       <c r="D84" t="n">
-        <v>89478666</v>
+        <v>89823059</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D85" t="n">
-        <v>112582</v>
+        <v>114082</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28183</v>
+        <v>28300</v>
       </c>
       <c r="D87" t="n">
-        <v>40801618</v>
+        <v>40970415</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2524</v>
+        <v>2545</v>
       </c>
       <c r="D89" t="n">
-        <v>3637425</v>
+        <v>3666197</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2477</v>
+        <v>2505</v>
       </c>
       <c r="D90" t="n">
-        <v>3494448</v>
+        <v>3533428</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>28496</v>
+        <v>28967</v>
       </c>
       <c r="D91" t="n">
-        <v>38669069</v>
+        <v>39301571</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7178</v>
+        <v>7301</v>
       </c>
       <c r="D95" t="n">
-        <v>10575520</v>
+        <v>10752256</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6389</v>
+        <v>6516</v>
       </c>
       <c r="D97" t="n">
-        <v>9260975</v>
+        <v>9445503</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="D99" t="n">
-        <v>645943</v>
+        <v>660905</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D100" t="n">
-        <v>632481</v>
+        <v>638407</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7134</v>
+        <v>7387</v>
       </c>
       <c r="D101" t="n">
-        <v>9903273</v>
+        <v>10246285</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1812</v>
+        <v>1862</v>
       </c>
       <c r="D103" t="n">
-        <v>2666618</v>
+        <v>2740613</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2462</v>
+        <v>2517</v>
       </c>
       <c r="D105" t="n">
-        <v>3593112</v>
+        <v>3673883</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D106" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D107" t="n">
-        <v>142690</v>
+        <v>145620</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D108" t="n">
-        <v>172689</v>
+        <v>178689</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>133871</v>
+        <v>134579</v>
       </c>
       <c r="D109" t="n">
-        <v>165707896</v>
+        <v>166569120</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="D113" t="n">
-        <v>1343763</v>
+        <v>1349856</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>50805</v>
+        <v>51010</v>
       </c>
       <c r="D115" t="n">
-        <v>74505951</v>
+        <v>74805173</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25525</v>
+        <v>25674</v>
       </c>
       <c r="D117" t="n">
-        <v>36985505</v>
+        <v>37201793</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1214</v>
+        <v>1221</v>
       </c>
       <c r="D118" t="n">
-        <v>1656952</v>
+        <v>1667352</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2002</v>
+        <v>2021</v>
       </c>
       <c r="D121" t="n">
-        <v>2813844</v>
+        <v>2838827</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>453008</v>
+        <v>458504</v>
       </c>
       <c r="D123" t="n">
-        <v>596918027</v>
+        <v>604369121</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1276</v>
+        <v>1288</v>
       </c>
       <c r="D128" t="n">
-        <v>1893155</v>
+        <v>1910238</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D129" t="n">
-        <v>36773</v>
+        <v>38273</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>194577</v>
+        <v>195893</v>
       </c>
       <c r="D130" t="n">
-        <v>286210199</v>
+        <v>288137566</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="D131" t="n">
-        <v>527790</v>
+        <v>536790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>166199</v>
+        <v>167471</v>
       </c>
       <c r="D133" t="n">
-        <v>241661406</v>
+        <v>243509062</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2572</v>
+        <v>2598</v>
       </c>
       <c r="D136" t="n">
-        <v>3607067</v>
+        <v>3645233</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D137" t="n">
-        <v>16222</v>
+        <v>17722</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5418</v>
+        <v>5494</v>
       </c>
       <c r="D138" t="n">
-        <v>7650963</v>
+        <v>7758783</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>41266</v>
+        <v>41562</v>
       </c>
       <c r="D141" t="n">
-        <v>55223901</v>
+        <v>55606820</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D142" t="n">
-        <v>35291</v>
+        <v>36791</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D144" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13379</v>
+        <v>13430</v>
       </c>
       <c r="D147" t="n">
-        <v>19643189</v>
+        <v>19717097</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3511</v>
+        <v>3544</v>
       </c>
       <c r="D148" t="n">
-        <v>5066464</v>
+        <v>5112511</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D151" t="n">
-        <v>516519</v>
+        <v>520222</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D153" t="n">
-        <v>475809</v>
+        <v>481809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>15952</v>
+        <v>16118</v>
       </c>
       <c r="D154" t="n">
-        <v>21135979</v>
+        <v>21353642</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D155" t="n">
-        <v>9126</v>
+        <v>10626</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6628</v>
+        <v>6699</v>
       </c>
       <c r="D158" t="n">
-        <v>9651353</v>
+        <v>9750622</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4517</v>
+        <v>4569</v>
       </c>
       <c r="D160" t="n">
-        <v>6510041</v>
+        <v>6584361</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D162" t="n">
-        <v>343960</v>
+        <v>352535</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D163" t="n">
-        <v>315096</v>
+        <v>325433</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>12718</v>
+        <v>13077</v>
       </c>
       <c r="D165" t="n">
-        <v>18420635</v>
+        <v>18949397</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1572</v>
+        <v>1605</v>
       </c>
       <c r="D166" t="n">
-        <v>2338038</v>
+        <v>2387538</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D170" t="n">
-        <v>110949</v>
+        <v>112449</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>83238</v>
+        <v>83783</v>
       </c>
       <c r="D171" t="n">
-        <v>104298393</v>
+        <v>104955896</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D172" t="n">
-        <v>33229</v>
+        <v>34729</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D173" t="n">
-        <v>120144</v>
+        <v>121521</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D176" t="n">
-        <v>919146</v>
+        <v>922146</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32625</v>
+        <v>32726</v>
       </c>
       <c r="D178" t="n">
-        <v>47861104</v>
+        <v>48005314</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D179" t="n">
-        <v>37500</v>
+        <v>39000</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12346</v>
+        <v>12409</v>
       </c>
       <c r="D180" t="n">
-        <v>17848959</v>
+        <v>17938735</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="D182" t="n">
-        <v>1625980</v>
+        <v>1637980</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1454</v>
+        <v>1467</v>
       </c>
       <c r="D184" t="n">
-        <v>2043172</v>
+        <v>2061283</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>225192</v>
+        <v>226506</v>
       </c>
       <c r="D186" t="n">
-        <v>280296424</v>
+        <v>281902505</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D187" t="n">
-        <v>138170</v>
+        <v>140030</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="D192" t="n">
-        <v>1237997</v>
+        <v>1242497</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>83459</v>
+        <v>83779</v>
       </c>
       <c r="D194" t="n">
-        <v>122371239</v>
+        <v>122840009</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D195" t="n">
-        <v>129127</v>
+        <v>130627</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31332</v>
+        <v>31512</v>
       </c>
       <c r="D197" t="n">
-        <v>45113705</v>
+        <v>45368995</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4736</v>
+        <v>4767</v>
       </c>
       <c r="D200" t="n">
-        <v>6746743</v>
+        <v>6793198</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4292</v>
+        <v>4339</v>
       </c>
       <c r="D203" t="n">
-        <v>5950644</v>
+        <v>6017376</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>247267</v>
+        <v>248879</v>
       </c>
       <c r="D206" t="n">
-        <v>306283472</v>
+        <v>308244337</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D207" t="n">
-        <v>161690</v>
+        <v>163190</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D208" t="n">
-        <v>337411</v>
+        <v>338911</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="D213" t="n">
-        <v>859356</v>
+        <v>863856</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>90827</v>
+        <v>91276</v>
       </c>
       <c r="D215" t="n">
-        <v>132938878</v>
+        <v>133587280</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>48547</v>
+        <v>48798</v>
       </c>
       <c r="D218" t="n">
-        <v>70220470</v>
+        <v>70576815</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4343</v>
+        <v>4372</v>
       </c>
       <c r="D221" t="n">
-        <v>6096509</v>
+        <v>6134805</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5003</v>
+        <v>5080</v>
       </c>
       <c r="D224" t="n">
-        <v>6915375</v>
+        <v>7021076</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>100615</v>
+        <v>101174</v>
       </c>
       <c r="D227" t="n">
-        <v>126188976</v>
+        <v>126869863</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D228" t="n">
-        <v>75152</v>
+        <v>76136</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="D232" t="n">
-        <v>792339</v>
+        <v>799839</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>47756</v>
+        <v>47917</v>
       </c>
       <c r="D234" t="n">
-        <v>69990328</v>
+        <v>70225506</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11716</v>
+        <v>11784</v>
       </c>
       <c r="D236" t="n">
-        <v>16852847</v>
+        <v>16951795</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1798</v>
+        <v>1806</v>
       </c>
       <c r="D238" t="n">
-        <v>2579513</v>
+        <v>2591513</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2271</v>
+        <v>2299</v>
       </c>
       <c r="D240" t="n">
-        <v>3167473</v>
+        <v>3209473</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>242305</v>
+        <v>243785</v>
       </c>
       <c r="D241" t="n">
-        <v>306370821</v>
+        <v>308222188</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="D247" t="n">
-        <v>1157064</v>
+        <v>1166064</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>91658</v>
+        <v>92066</v>
       </c>
       <c r="D249" t="n">
-        <v>134381634</v>
+        <v>134981151</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>61227</v>
+        <v>61612</v>
       </c>
       <c r="D252" t="n">
-        <v>88782246</v>
+        <v>89328757</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2271</v>
+        <v>2283</v>
       </c>
       <c r="D254" t="n">
-        <v>3204242</v>
+        <v>3222242</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4074</v>
+        <v>4122</v>
       </c>
       <c r="D257" t="n">
-        <v>5714907</v>
+        <v>5781853</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-26 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>302841</v>
+        <v>306385</v>
       </c>
       <c r="D2" t="n">
-        <v>386545519</v>
+        <v>390931793</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D3" t="n">
-        <v>297311</v>
+        <v>301099</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D4" t="n">
-        <v>430843</v>
+        <v>436843</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D8" t="n">
-        <v>1208544</v>
+        <v>1211544</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>112538</v>
+        <v>113104</v>
       </c>
       <c r="D10" t="n">
-        <v>165002681</v>
+        <v>165823559</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56281</v>
+        <v>56673</v>
       </c>
       <c r="D12" t="n">
-        <v>81278020</v>
+        <v>81836194</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3739</v>
+        <v>3755</v>
       </c>
       <c r="D16" t="n">
-        <v>5309577</v>
+        <v>5331173</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5886</v>
+        <v>6006</v>
       </c>
       <c r="D20" t="n">
-        <v>8231054</v>
+        <v>8392260</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>73846</v>
+        <v>74514</v>
       </c>
       <c r="D22" t="n">
-        <v>92392725</v>
+        <v>93161583</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31365</v>
+        <v>31511</v>
       </c>
       <c r="D28" t="n">
-        <v>45934396</v>
+        <v>46145854</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>10956</v>
+        <v>11044</v>
       </c>
       <c r="D30" t="n">
-        <v>15779222</v>
+        <v>15911020</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1464</v>
+        <v>1478</v>
       </c>
       <c r="D33" t="n">
-        <v>2056887</v>
+        <v>2076871</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1624</v>
+        <v>1648</v>
       </c>
       <c r="D35" t="n">
-        <v>2291538</v>
+        <v>2323974</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>93146</v>
+        <v>94012</v>
       </c>
       <c r="D36" t="n">
-        <v>117574866</v>
+        <v>118609288</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D37" t="n">
-        <v>69477</v>
+        <v>75477</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D38" t="n">
-        <v>105528</v>
+        <v>112488</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43068</v>
+        <v>43264</v>
       </c>
       <c r="D44" t="n">
-        <v>63163909</v>
+        <v>63439607</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8728</v>
+        <v>8802</v>
       </c>
       <c r="D46" t="n">
-        <v>12532183</v>
+        <v>12634147</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1322</v>
+        <v>1336</v>
       </c>
       <c r="D48" t="n">
-        <v>1830857</v>
+        <v>1851857</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2063</v>
+        <v>2103</v>
       </c>
       <c r="D51" t="n">
-        <v>2873497</v>
+        <v>2928539</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>65657</v>
+        <v>66325</v>
       </c>
       <c r="D52" t="n">
-        <v>82496390</v>
+        <v>83312356</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D53" t="n">
-        <v>36883</v>
+        <v>39883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D54" t="n">
-        <v>54866</v>
+        <v>57866</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27155</v>
+        <v>27317</v>
       </c>
       <c r="D58" t="n">
-        <v>39833781</v>
+        <v>40066703</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D59" t="n">
-        <v>33000</v>
+        <v>36000</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10535</v>
+        <v>10623</v>
       </c>
       <c r="D61" t="n">
-        <v>15241201</v>
+        <v>15364049</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1299</v>
+        <v>1309</v>
       </c>
       <c r="D63" t="n">
-        <v>1810872</v>
+        <v>1825706</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1332</v>
+        <v>1358</v>
       </c>
       <c r="D67" t="n">
-        <v>1860599</v>
+        <v>1897181</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19329</v>
+        <v>19541</v>
       </c>
       <c r="D69" t="n">
-        <v>25305578</v>
+        <v>25579770</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7100</v>
+        <v>7174</v>
       </c>
       <c r="D73" t="n">
-        <v>10392921</v>
+        <v>10503921</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4809</v>
+        <v>4843</v>
       </c>
       <c r="D75" t="n">
-        <v>6982002</v>
+        <v>7032802</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D76" t="n">
-        <v>643689</v>
+        <v>649689</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D77" t="n">
-        <v>342608</v>
+        <v>349904</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>133934</v>
+        <v>135230</v>
       </c>
       <c r="D78" t="n">
-        <v>167260783</v>
+        <v>168823155</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D79" t="n">
-        <v>76460</v>
+        <v>78110</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D82" t="n">
-        <v>591475</v>
+        <v>597475</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61249</v>
+        <v>61513</v>
       </c>
       <c r="D84" t="n">
-        <v>89823059</v>
+        <v>90202951</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28300</v>
+        <v>28480</v>
       </c>
       <c r="D87" t="n">
-        <v>40970415</v>
+        <v>41225419</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2545</v>
+        <v>2553</v>
       </c>
       <c r="D89" t="n">
-        <v>3666197</v>
+        <v>3676471</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2505</v>
+        <v>2541</v>
       </c>
       <c r="D90" t="n">
-        <v>3533428</v>
+        <v>3583312</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>28967</v>
+        <v>29757</v>
       </c>
       <c r="D91" t="n">
-        <v>39301571</v>
+        <v>40326921</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7301</v>
+        <v>7451</v>
       </c>
       <c r="D95" t="n">
-        <v>10752256</v>
+        <v>10973440</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6516</v>
+        <v>6706</v>
       </c>
       <c r="D97" t="n">
-        <v>9445503</v>
+        <v>9717049</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="D99" t="n">
-        <v>660905</v>
+        <v>672805</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D100" t="n">
-        <v>638407</v>
+        <v>653139</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7387</v>
+        <v>7605</v>
       </c>
       <c r="D101" t="n">
-        <v>10246285</v>
+        <v>10535403</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1862</v>
+        <v>1932</v>
       </c>
       <c r="D103" t="n">
-        <v>2740613</v>
+        <v>2842255</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2517</v>
+        <v>2621</v>
       </c>
       <c r="D105" t="n">
-        <v>3673883</v>
+        <v>3827867</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D107" t="n">
-        <v>145620</v>
+        <v>157620</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D108" t="n">
-        <v>178689</v>
+        <v>181689</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>134579</v>
+        <v>135891</v>
       </c>
       <c r="D109" t="n">
-        <v>166569120</v>
+        <v>168168386</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="D113" t="n">
-        <v>1349856</v>
+        <v>1355856</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51010</v>
+        <v>51270</v>
       </c>
       <c r="D115" t="n">
-        <v>74805173</v>
+        <v>75187817</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25674</v>
+        <v>25916</v>
       </c>
       <c r="D117" t="n">
-        <v>37201793</v>
+        <v>37553759</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1221</v>
+        <v>1233</v>
       </c>
       <c r="D118" t="n">
-        <v>1667352</v>
+        <v>1685352</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2021</v>
+        <v>2055</v>
       </c>
       <c r="D121" t="n">
-        <v>2838827</v>
+        <v>2887981</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>458504</v>
+        <v>468356</v>
       </c>
       <c r="D123" t="n">
-        <v>604369121</v>
+        <v>617507011</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D124" t="n">
-        <v>108117</v>
+        <v>114117</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1288</v>
+        <v>1306</v>
       </c>
       <c r="D128" t="n">
-        <v>1910238</v>
+        <v>1937238</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>195893</v>
+        <v>198029</v>
       </c>
       <c r="D130" t="n">
-        <v>288137566</v>
+        <v>291240890</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="D131" t="n">
-        <v>536790</v>
+        <v>545790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>167471</v>
+        <v>169855</v>
       </c>
       <c r="D133" t="n">
-        <v>243509062</v>
+        <v>246993802</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2598</v>
+        <v>2648</v>
       </c>
       <c r="D136" t="n">
-        <v>3645233</v>
+        <v>3718731</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5494</v>
+        <v>5652</v>
       </c>
       <c r="D138" t="n">
-        <v>7758783</v>
+        <v>7980217</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>41562</v>
+        <v>42126</v>
       </c>
       <c r="D141" t="n">
-        <v>55606820</v>
+        <v>56330028</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D145" t="n">
-        <v>4500</v>
+        <v>7500</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13430</v>
+        <v>13530</v>
       </c>
       <c r="D147" t="n">
-        <v>19717097</v>
+        <v>19860035</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3544</v>
+        <v>3564</v>
       </c>
       <c r="D148" t="n">
-        <v>5112511</v>
+        <v>5141043</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="D151" t="n">
-        <v>520222</v>
+        <v>532222</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D153" t="n">
-        <v>481809</v>
+        <v>487809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16118</v>
+        <v>16412</v>
       </c>
       <c r="D154" t="n">
-        <v>21353642</v>
+        <v>21742798</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6699</v>
+        <v>6791</v>
       </c>
       <c r="D158" t="n">
-        <v>9750622</v>
+        <v>9885802</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4569</v>
+        <v>4625</v>
       </c>
       <c r="D160" t="n">
-        <v>6584361</v>
+        <v>6657989</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="D163" t="n">
-        <v>325433</v>
+        <v>355433</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>13077</v>
+        <v>13659</v>
       </c>
       <c r="D165" t="n">
-        <v>18949397</v>
+        <v>19817831</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1605</v>
+        <v>1633</v>
       </c>
       <c r="D166" t="n">
-        <v>2387538</v>
+        <v>2429138</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D167" t="n">
-        <v>308302</v>
+        <v>317302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D170" t="n">
-        <v>112449</v>
+        <v>118449</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>83783</v>
+        <v>84607</v>
       </c>
       <c r="D171" t="n">
-        <v>104955896</v>
+        <v>105900308</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D176" t="n">
-        <v>922146</v>
+        <v>924346</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32726</v>
+        <v>32890</v>
       </c>
       <c r="D178" t="n">
-        <v>48005314</v>
+        <v>48249164</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12409</v>
+        <v>12475</v>
       </c>
       <c r="D180" t="n">
-        <v>17938735</v>
+        <v>18035889</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1171</v>
+        <v>1181</v>
       </c>
       <c r="D182" t="n">
-        <v>1637980</v>
+        <v>1652676</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1467</v>
+        <v>1497</v>
       </c>
       <c r="D184" t="n">
-        <v>2061283</v>
+        <v>2106283</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>226506</v>
+        <v>228722</v>
       </c>
       <c r="D186" t="n">
-        <v>281902505</v>
+        <v>284573779</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>83779</v>
+        <v>84161</v>
       </c>
       <c r="D194" t="n">
-        <v>122840009</v>
+        <v>123393817</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31512</v>
+        <v>31726</v>
       </c>
       <c r="D197" t="n">
-        <v>45368995</v>
+        <v>45670091</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4767</v>
+        <v>4793</v>
       </c>
       <c r="D200" t="n">
-        <v>6793198</v>
+        <v>6827260</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4339</v>
+        <v>4413</v>
       </c>
       <c r="D203" t="n">
-        <v>6017376</v>
+        <v>6121390</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D205" t="n">
-        <v>11947</v>
+        <v>13411</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>248879</v>
+        <v>251765</v>
       </c>
       <c r="D206" t="n">
-        <v>308244337</v>
+        <v>311746683</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="D213" t="n">
-        <v>863856</v>
+        <v>875856</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>91276</v>
+        <v>91760</v>
       </c>
       <c r="D215" t="n">
-        <v>133587280</v>
+        <v>134293926</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>48798</v>
+        <v>49134</v>
       </c>
       <c r="D218" t="n">
-        <v>70576815</v>
+        <v>71060029</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D219" t="n">
-        <v>39075</v>
+        <v>40769</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4372</v>
+        <v>4424</v>
       </c>
       <c r="D221" t="n">
-        <v>6134805</v>
+        <v>6206721</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5080</v>
+        <v>5206</v>
       </c>
       <c r="D224" t="n">
-        <v>7021076</v>
+        <v>7194064</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>101174</v>
+        <v>102198</v>
       </c>
       <c r="D227" t="n">
-        <v>126869863</v>
+        <v>128113851</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="D232" t="n">
-        <v>799839</v>
+        <v>808839</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>47917</v>
+        <v>48151</v>
       </c>
       <c r="D234" t="n">
-        <v>70225506</v>
+        <v>70568176</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11784</v>
+        <v>11878</v>
       </c>
       <c r="D236" t="n">
-        <v>16951795</v>
+        <v>17079547</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1806</v>
+        <v>1812</v>
       </c>
       <c r="D238" t="n">
-        <v>2591513</v>
+        <v>2600513</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2299</v>
+        <v>2335</v>
       </c>
       <c r="D240" t="n">
-        <v>3209473</v>
+        <v>3263033</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>243785</v>
+        <v>246297</v>
       </c>
       <c r="D241" t="n">
-        <v>308222188</v>
+        <v>311307350</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D242" t="n">
-        <v>199801</v>
+        <v>201831</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D243" t="n">
-        <v>341457</v>
+        <v>344457</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>92066</v>
+        <v>92580</v>
       </c>
       <c r="D249" t="n">
-        <v>134981151</v>
+        <v>135705975</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>61612</v>
+        <v>62106</v>
       </c>
       <c r="D252" t="n">
-        <v>89328757</v>
+        <v>90050353</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2283</v>
+        <v>2305</v>
       </c>
       <c r="D254" t="n">
-        <v>3222242</v>
+        <v>3254042</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4122</v>
+        <v>4186</v>
       </c>
       <c r="D257" t="n">
-        <v>5781853</v>
+        <v>5874601</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Deduplicate 2020-07-26 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -66,6 +66,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,10 +488,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>306385</v>
+        <v>304613</v>
       </c>
       <c r="D2" t="n">
-        <v>390931793</v>
+        <v>388738656</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +526,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D3" t="n">
-        <v>301099</v>
+        <v>299205</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +564,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D4" t="n">
-        <v>436843</v>
+        <v>433843</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +716,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D8" t="n">
-        <v>1211544</v>
+        <v>1210044</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +792,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>113104</v>
+        <v>112821</v>
       </c>
       <c r="D10" t="n">
-        <v>165823559</v>
+        <v>165413120</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +868,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56673</v>
+        <v>56477</v>
       </c>
       <c r="D12" t="n">
-        <v>81836194</v>
+        <v>81557107</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +1020,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3755</v>
+        <v>3747</v>
       </c>
       <c r="D16" t="n">
-        <v>5331173</v>
+        <v>5320375</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1172,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6006</v>
+        <v>5946</v>
       </c>
       <c r="D20" t="n">
-        <v>8392260</v>
+        <v>8311657</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1248,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74514</v>
+        <v>74180</v>
       </c>
       <c r="D22" t="n">
-        <v>93161583</v>
+        <v>92777154</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1476,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31511</v>
+        <v>31438</v>
       </c>
       <c r="D28" t="n">
-        <v>46145854</v>
+        <v>46040125</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1552,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11044</v>
+        <v>11000</v>
       </c>
       <c r="D30" t="n">
-        <v>15911020</v>
+        <v>15845121</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1666,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1478</v>
+        <v>1471</v>
       </c>
       <c r="D33" t="n">
-        <v>2076871</v>
+        <v>2066879</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1742,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1648</v>
+        <v>1636</v>
       </c>
       <c r="D35" t="n">
-        <v>2323974</v>
+        <v>2307756</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1780,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>94012</v>
+        <v>93579</v>
       </c>
       <c r="D36" t="n">
-        <v>118609288</v>
+        <v>118092077</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1818,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" t="n">
-        <v>75477</v>
+        <v>72477</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1856,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D38" t="n">
-        <v>112488</v>
+        <v>109008</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2016,10 +2084,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43264</v>
+        <v>43166</v>
       </c>
       <c r="D44" t="n">
-        <v>63439607</v>
+        <v>63301758</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2160,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8802</v>
+        <v>8765</v>
       </c>
       <c r="D46" t="n">
-        <v>12634147</v>
+        <v>12583165</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2236,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1336</v>
+        <v>1329</v>
       </c>
       <c r="D48" t="n">
-        <v>1851857</v>
+        <v>1841357</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2350,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2103</v>
+        <v>2083</v>
       </c>
       <c r="D51" t="n">
-        <v>2928539</v>
+        <v>2901018</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2388,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>66325</v>
+        <v>65991</v>
       </c>
       <c r="D52" t="n">
-        <v>83312356</v>
+        <v>82904373</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2426,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D53" t="n">
-        <v>39883</v>
+        <v>38383</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2464,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D54" t="n">
-        <v>57866</v>
+        <v>56366</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2548,10 +2616,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27317</v>
+        <v>27236</v>
       </c>
       <c r="D58" t="n">
-        <v>40066703</v>
+        <v>39950242</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2654,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D59" t="n">
-        <v>36000</v>
+        <v>34500</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2730,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10623</v>
+        <v>10579</v>
       </c>
       <c r="D61" t="n">
-        <v>15364049</v>
+        <v>15302625</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2806,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1309</v>
+        <v>1304</v>
       </c>
       <c r="D63" t="n">
-        <v>1825706</v>
+        <v>1818289</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2958,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1358</v>
+        <v>1345</v>
       </c>
       <c r="D67" t="n">
-        <v>1897181</v>
+        <v>1878890</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +3034,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19541</v>
+        <v>19435</v>
       </c>
       <c r="D69" t="n">
-        <v>25579770</v>
+        <v>25442674</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3186,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7174</v>
+        <v>7137</v>
       </c>
       <c r="D73" t="n">
-        <v>10503921</v>
+        <v>10448421</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3262,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4843</v>
+        <v>4826</v>
       </c>
       <c r="D75" t="n">
-        <v>7032802</v>
+        <v>7007402</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3300,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D76" t="n">
-        <v>649689</v>
+        <v>646689</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3338,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D77" t="n">
-        <v>349904</v>
+        <v>346256</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3376,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>135230</v>
+        <v>134582</v>
       </c>
       <c r="D78" t="n">
-        <v>168823155</v>
+        <v>168041969</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3414,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D79" t="n">
-        <v>78110</v>
+        <v>77285</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3460,10 +3528,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D82" t="n">
-        <v>597475</v>
+        <v>594475</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3604,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61513</v>
+        <v>61381</v>
       </c>
       <c r="D84" t="n">
-        <v>90202951</v>
+        <v>90013005</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3718,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28480</v>
+        <v>28390</v>
       </c>
       <c r="D87" t="n">
-        <v>41225419</v>
+        <v>41097917</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3794,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2553</v>
+        <v>2549</v>
       </c>
       <c r="D89" t="n">
-        <v>3676471</v>
+        <v>3671334</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3832,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2541</v>
+        <v>2523</v>
       </c>
       <c r="D90" t="n">
-        <v>3583312</v>
+        <v>3558370</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3870,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>29757</v>
+        <v>29362</v>
       </c>
       <c r="D91" t="n">
-        <v>40326921</v>
+        <v>39814246</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +4022,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7451</v>
+        <v>7376</v>
       </c>
       <c r="D95" t="n">
-        <v>10973440</v>
+        <v>10862848</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4098,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6706</v>
+        <v>6611</v>
       </c>
       <c r="D97" t="n">
-        <v>9717049</v>
+        <v>9581276</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4174,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D99" t="n">
-        <v>672805</v>
+        <v>666855</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4212,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D100" t="n">
-        <v>653139</v>
+        <v>645773</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4250,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7605</v>
+        <v>7496</v>
       </c>
       <c r="D101" t="n">
-        <v>10535403</v>
+        <v>10390844</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4326,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1932</v>
+        <v>1897</v>
       </c>
       <c r="D103" t="n">
-        <v>2842255</v>
+        <v>2791434</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4402,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2621</v>
+        <v>2569</v>
       </c>
       <c r="D105" t="n">
-        <v>3827867</v>
+        <v>3750875</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4478,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D107" t="n">
-        <v>157620</v>
+        <v>151620</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4516,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D108" t="n">
-        <v>181689</v>
+        <v>180189</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4554,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>135891</v>
+        <v>135235</v>
       </c>
       <c r="D109" t="n">
-        <v>168168386</v>
+        <v>167368753</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4706,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D113" t="n">
-        <v>1355856</v>
+        <v>1352856</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4782,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51270</v>
+        <v>51140</v>
       </c>
       <c r="D115" t="n">
-        <v>75187817</v>
+        <v>74996495</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4858,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25916</v>
+        <v>25795</v>
       </c>
       <c r="D117" t="n">
-        <v>37553759</v>
+        <v>37377776</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4896,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1233</v>
+        <v>1227</v>
       </c>
       <c r="D118" t="n">
-        <v>1685352</v>
+        <v>1676352</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +5010,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2055</v>
+        <v>2038</v>
       </c>
       <c r="D121" t="n">
-        <v>2887981</v>
+        <v>2863404</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5086,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>468356</v>
+        <v>463430</v>
       </c>
       <c r="D123" t="n">
-        <v>617507011</v>
+        <v>610938066</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5124,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D124" t="n">
-        <v>114117</v>
+        <v>111117</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5208,10 +5276,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1306</v>
+        <v>1297</v>
       </c>
       <c r="D128" t="n">
-        <v>1937238</v>
+        <v>1923738</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5352,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>198029</v>
+        <v>196961</v>
       </c>
       <c r="D130" t="n">
-        <v>291240890</v>
+        <v>289689228</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5390,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D131" t="n">
-        <v>545790</v>
+        <v>541290</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5466,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>169855</v>
+        <v>168663</v>
       </c>
       <c r="D133" t="n">
-        <v>246993802</v>
+        <v>245251432</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5580,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2648</v>
+        <v>2623</v>
       </c>
       <c r="D136" t="n">
-        <v>3718731</v>
+        <v>3681982</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5656,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5652</v>
+        <v>5573</v>
       </c>
       <c r="D138" t="n">
-        <v>7980217</v>
+        <v>7869500</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5770,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>42126</v>
+        <v>41844</v>
       </c>
       <c r="D141" t="n">
-        <v>56330028</v>
+        <v>55968424</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5854,10 +5922,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D145" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5930,10 +5998,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13530</v>
+        <v>13480</v>
       </c>
       <c r="D147" t="n">
-        <v>19860035</v>
+        <v>19788566</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +6036,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3564</v>
+        <v>3554</v>
       </c>
       <c r="D148" t="n">
-        <v>5141043</v>
+        <v>5126777</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6150,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D151" t="n">
-        <v>532222</v>
+        <v>526222</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6226,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D153" t="n">
-        <v>487809</v>
+        <v>484809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6264,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16412</v>
+        <v>16265</v>
       </c>
       <c r="D154" t="n">
-        <v>21742798</v>
+        <v>21548220</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6416,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6791</v>
+        <v>6745</v>
       </c>
       <c r="D158" t="n">
-        <v>9885802</v>
+        <v>9818212</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6492,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4625</v>
+        <v>4597</v>
       </c>
       <c r="D160" t="n">
-        <v>6657989</v>
+        <v>6621175</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6538,10 +6606,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D163" t="n">
-        <v>355433</v>
+        <v>340433</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6682,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>13659</v>
+        <v>13368</v>
       </c>
       <c r="D165" t="n">
-        <v>19817831</v>
+        <v>19383614</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6720,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1633</v>
+        <v>1619</v>
       </c>
       <c r="D166" t="n">
-        <v>2429138</v>
+        <v>2408338</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6758,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D167" t="n">
-        <v>317302</v>
+        <v>312802</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6872,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D170" t="n">
-        <v>118449</v>
+        <v>115449</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6910,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>84607</v>
+        <v>84195</v>
       </c>
       <c r="D171" t="n">
-        <v>105900308</v>
+        <v>105428102</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7100,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D176" t="n">
-        <v>924346</v>
+        <v>923246</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7176,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32890</v>
+        <v>32808</v>
       </c>
       <c r="D178" t="n">
-        <v>48249164</v>
+        <v>48127239</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7252,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12475</v>
+        <v>12442</v>
       </c>
       <c r="D180" t="n">
-        <v>18035889</v>
+        <v>17987312</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7328,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="D182" t="n">
-        <v>1652676</v>
+        <v>1645328</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7404,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1497</v>
+        <v>1482</v>
       </c>
       <c r="D184" t="n">
-        <v>2106283</v>
+        <v>2083783</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7480,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>228722</v>
+        <v>227614</v>
       </c>
       <c r="D186" t="n">
-        <v>284573779</v>
+        <v>283238142</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7716,10 +7784,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>84161</v>
+        <v>83970</v>
       </c>
       <c r="D194" t="n">
-        <v>123393817</v>
+        <v>123116913</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7898,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31726</v>
+        <v>31619</v>
       </c>
       <c r="D197" t="n">
-        <v>45670091</v>
+        <v>45519543</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +8012,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4793</v>
+        <v>4780</v>
       </c>
       <c r="D200" t="n">
-        <v>6827260</v>
+        <v>6810229</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8126,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4413</v>
+        <v>4376</v>
       </c>
       <c r="D203" t="n">
-        <v>6121390</v>
+        <v>6069383</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8134,10 +8202,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D205" t="n">
-        <v>13411</v>
+        <v>12679</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8172,10 +8240,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>251765</v>
+        <v>250322</v>
       </c>
       <c r="D206" t="n">
-        <v>311746683</v>
+        <v>309995510</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8438,10 +8506,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D213" t="n">
-        <v>875856</v>
+        <v>869856</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8582,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>91760</v>
+        <v>91518</v>
       </c>
       <c r="D215" t="n">
-        <v>134293926</v>
+        <v>133940603</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8696,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>49134</v>
+        <v>48966</v>
       </c>
       <c r="D218" t="n">
-        <v>71060029</v>
+        <v>70818422</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8666,10 +8734,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D219" t="n">
-        <v>40769</v>
+        <v>39922</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8742,10 +8810,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4424</v>
+        <v>4398</v>
       </c>
       <c r="D221" t="n">
-        <v>6206721</v>
+        <v>6170763</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8924,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5206</v>
+        <v>5143</v>
       </c>
       <c r="D224" t="n">
-        <v>7194064</v>
+        <v>7107570</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +9038,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>102198</v>
+        <v>101686</v>
       </c>
       <c r="D227" t="n">
-        <v>128113851</v>
+        <v>127491857</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9160,10 +9228,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D232" t="n">
-        <v>808839</v>
+        <v>804339</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9304,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48151</v>
+        <v>48034</v>
       </c>
       <c r="D234" t="n">
-        <v>70568176</v>
+        <v>70396841</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9380,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11878</v>
+        <v>11831</v>
       </c>
       <c r="D236" t="n">
-        <v>17079547</v>
+        <v>17015671</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9456,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="D238" t="n">
-        <v>2600513</v>
+        <v>2596013</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9532,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2335</v>
+        <v>2317</v>
       </c>
       <c r="D240" t="n">
-        <v>3263033</v>
+        <v>3236253</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9570,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>246297</v>
+        <v>245041</v>
       </c>
       <c r="D241" t="n">
-        <v>311307350</v>
+        <v>309764769</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9608,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D242" t="n">
-        <v>201831</v>
+        <v>200816</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9646,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D243" t="n">
-        <v>344457</v>
+        <v>342957</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9874,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>92580</v>
+        <v>92323</v>
       </c>
       <c r="D249" t="n">
-        <v>135705975</v>
+        <v>135343563</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9988,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>62106</v>
+        <v>61859</v>
       </c>
       <c r="D252" t="n">
-        <v>90050353</v>
+        <v>89689555</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +10064,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2305</v>
+        <v>2294</v>
       </c>
       <c r="D254" t="n">
-        <v>3254042</v>
+        <v>3238142</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10178,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4186</v>
+        <v>4154</v>
       </c>
       <c r="D257" t="n">
-        <v>5874601</v>
+        <v>5828227</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-27 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -66,74 +66,6 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -488,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>304613</v>
+        <v>306223</v>
       </c>
       <c r="D2" t="n">
-        <v>388738656</v>
+        <v>390783556</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -564,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D4" t="n">
-        <v>433843</v>
+        <v>436843</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -716,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="D8" t="n">
-        <v>1210044</v>
+        <v>1212315</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -792,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>112821</v>
+        <v>113334</v>
       </c>
       <c r="D10" t="n">
-        <v>165413120</v>
+        <v>166149096</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -830,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" t="n">
-        <v>196828</v>
+        <v>198013</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -868,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56477</v>
+        <v>56771</v>
       </c>
       <c r="D12" t="n">
-        <v>81557107</v>
+        <v>81971061</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -944,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="n">
-        <v>63559</v>
+        <v>64543</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1020,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3747</v>
+        <v>3767</v>
       </c>
       <c r="D16" t="n">
-        <v>5320375</v>
+        <v>5348624</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1172,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5946</v>
+        <v>6007</v>
       </c>
       <c r="D20" t="n">
-        <v>8311657</v>
+        <v>8399136</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1248,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74180</v>
+        <v>74529</v>
       </c>
       <c r="D22" t="n">
-        <v>92777154</v>
+        <v>93183159</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1438,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D27" t="n">
-        <v>404147</v>
+        <v>405647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1476,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31438</v>
+        <v>31555</v>
       </c>
       <c r="D28" t="n">
-        <v>46040125</v>
+        <v>46208147</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1552,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11000</v>
+        <v>11049</v>
       </c>
       <c r="D30" t="n">
-        <v>15845121</v>
+        <v>15914009</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1666,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1471</v>
+        <v>1477</v>
       </c>
       <c r="D33" t="n">
-        <v>2066879</v>
+        <v>2075879</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1742,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1636</v>
+        <v>1661</v>
       </c>
       <c r="D35" t="n">
-        <v>2307756</v>
+        <v>2339428</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1780,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>93579</v>
+        <v>93915</v>
       </c>
       <c r="D36" t="n">
-        <v>118092077</v>
+        <v>118490606</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1818,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D37" t="n">
-        <v>72477</v>
+        <v>73613</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2008,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D42" t="n">
-        <v>1303772</v>
+        <v>1305272</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2084,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43166</v>
+        <v>43319</v>
       </c>
       <c r="D44" t="n">
-        <v>63301758</v>
+        <v>63522241</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2160,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8765</v>
+        <v>8806</v>
       </c>
       <c r="D46" t="n">
-        <v>12583165</v>
+        <v>12643049</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2236,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1329</v>
+        <v>1346</v>
       </c>
       <c r="D48" t="n">
-        <v>1841357</v>
+        <v>1866279</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2350,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2083</v>
+        <v>2114</v>
       </c>
       <c r="D51" t="n">
-        <v>2901018</v>
+        <v>2945288</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2388,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>65991</v>
+        <v>66295</v>
       </c>
       <c r="D52" t="n">
-        <v>82904373</v>
+        <v>83265579</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2540,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D56" t="n">
-        <v>551844</v>
+        <v>554844</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2616,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27236</v>
+        <v>27334</v>
       </c>
       <c r="D58" t="n">
-        <v>39950242</v>
+        <v>40092325</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2730,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10579</v>
+        <v>10626</v>
       </c>
       <c r="D61" t="n">
-        <v>15302625</v>
+        <v>15369479</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2806,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="D63" t="n">
-        <v>1818289</v>
+        <v>1821289</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2958,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1345</v>
+        <v>1359</v>
       </c>
       <c r="D67" t="n">
-        <v>1878890</v>
+        <v>1898921</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3034,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19435</v>
+        <v>19528</v>
       </c>
       <c r="D69" t="n">
-        <v>25442674</v>
+        <v>25565413</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3072,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D70" t="n">
-        <v>38640</v>
+        <v>39736</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3186,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7137</v>
+        <v>7178</v>
       </c>
       <c r="D73" t="n">
-        <v>10448421</v>
+        <v>10509608</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3262,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4826</v>
+        <v>4869</v>
       </c>
       <c r="D75" t="n">
-        <v>7007402</v>
+        <v>7070974</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3300,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D76" t="n">
-        <v>646689</v>
+        <v>649689</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3338,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D77" t="n">
-        <v>346256</v>
+        <v>347756</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3376,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>134582</v>
+        <v>135181</v>
       </c>
       <c r="D78" t="n">
-        <v>168041969</v>
+        <v>168767915</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3452,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D80" t="n">
-        <v>118186</v>
+        <v>119686</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3528,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D82" t="n">
-        <v>594475</v>
+        <v>595975</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3604,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61381</v>
+        <v>61631</v>
       </c>
       <c r="D84" t="n">
-        <v>90013005</v>
+        <v>90372225</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3642,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D85" t="n">
-        <v>114082</v>
+        <v>115582</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3718,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28390</v>
+        <v>28501</v>
       </c>
       <c r="D87" t="n">
-        <v>41097917</v>
+        <v>41258785</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3794,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2549</v>
+        <v>2559</v>
       </c>
       <c r="D89" t="n">
-        <v>3671334</v>
+        <v>3684605</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3832,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2523</v>
+        <v>2557</v>
       </c>
       <c r="D90" t="n">
-        <v>3558370</v>
+        <v>3607895</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3870,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>29362</v>
+        <v>29622</v>
       </c>
       <c r="D91" t="n">
-        <v>39814246</v>
+        <v>40156045</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4022,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7376</v>
+        <v>7403</v>
       </c>
       <c r="D95" t="n">
-        <v>10862848</v>
+        <v>10901229</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4098,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6611</v>
+        <v>6649</v>
       </c>
       <c r="D97" t="n">
-        <v>9581276</v>
+        <v>9637508</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4174,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="D99" t="n">
-        <v>666855</v>
+        <v>673905</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4212,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D100" t="n">
-        <v>645773</v>
+        <v>648773</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4250,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7496</v>
+        <v>7597</v>
       </c>
       <c r="D101" t="n">
-        <v>10390844</v>
+        <v>10532585</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4326,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1897</v>
+        <v>1925</v>
       </c>
       <c r="D103" t="n">
-        <v>2791434</v>
+        <v>2833434</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4402,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2569</v>
+        <v>2622</v>
       </c>
       <c r="D105" t="n">
-        <v>3750875</v>
+        <v>3829013</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4478,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D107" t="n">
-        <v>151620</v>
+        <v>154620</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4554,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>135235</v>
+        <v>135844</v>
       </c>
       <c r="D109" t="n">
-        <v>167368753</v>
+        <v>168093341</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4706,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="D113" t="n">
-        <v>1352856</v>
+        <v>1356382</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4782,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51140</v>
+        <v>51303</v>
       </c>
       <c r="D115" t="n">
-        <v>74996495</v>
+        <v>75233018</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4858,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25795</v>
+        <v>25924</v>
       </c>
       <c r="D117" t="n">
-        <v>37377776</v>
+        <v>37567039</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4896,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1227</v>
+        <v>1237</v>
       </c>
       <c r="D118" t="n">
-        <v>1676352</v>
+        <v>1691352</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -5010,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2038</v>
+        <v>2070</v>
       </c>
       <c r="D121" t="n">
-        <v>2863404</v>
+        <v>2908075</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5086,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>463430</v>
+        <v>467557</v>
       </c>
       <c r="D123" t="n">
-        <v>610938066</v>
+        <v>616426843</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5124,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D124" t="n">
-        <v>111117</v>
+        <v>116947</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5276,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1297</v>
+        <v>1306</v>
       </c>
       <c r="D128" t="n">
-        <v>1923738</v>
+        <v>1936292</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5352,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>196961</v>
+        <v>198065</v>
       </c>
       <c r="D130" t="n">
-        <v>289689228</v>
+        <v>291297788</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5390,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D131" t="n">
-        <v>541290</v>
+        <v>544290</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5466,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>168663</v>
+        <v>169832</v>
       </c>
       <c r="D133" t="n">
-        <v>245251432</v>
+        <v>246944610</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5580,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2623</v>
+        <v>2650</v>
       </c>
       <c r="D136" t="n">
-        <v>3681982</v>
+        <v>3721234</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5656,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5573</v>
+        <v>5645</v>
       </c>
       <c r="D138" t="n">
-        <v>7869500</v>
+        <v>7974747</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5770,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>41844</v>
+        <v>42146</v>
       </c>
       <c r="D141" t="n">
-        <v>55968424</v>
+        <v>56358870</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5998,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13480</v>
+        <v>13530</v>
       </c>
       <c r="D147" t="n">
-        <v>19788566</v>
+        <v>19861386</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6036,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3554</v>
+        <v>3575</v>
       </c>
       <c r="D148" t="n">
-        <v>5126777</v>
+        <v>5156127</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6150,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D151" t="n">
-        <v>526222</v>
+        <v>530722</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6226,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D153" t="n">
-        <v>484809</v>
+        <v>487809</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6264,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16265</v>
+        <v>16371</v>
       </c>
       <c r="D154" t="n">
-        <v>21548220</v>
+        <v>21674871</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6416,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6745</v>
+        <v>6776</v>
       </c>
       <c r="D158" t="n">
-        <v>9818212</v>
+        <v>9862788</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6492,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4597</v>
+        <v>4628</v>
       </c>
       <c r="D160" t="n">
-        <v>6621175</v>
+        <v>6666674</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6606,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D163" t="n">
-        <v>340433</v>
+        <v>341933</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6682,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>13368</v>
+        <v>13577</v>
       </c>
       <c r="D165" t="n">
-        <v>19383614</v>
+        <v>19691075</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6720,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1619</v>
+        <v>1629</v>
       </c>
       <c r="D166" t="n">
-        <v>2408338</v>
+        <v>2422130</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6758,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D167" t="n">
-        <v>312802</v>
+        <v>317302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6910,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>84195</v>
+        <v>84578</v>
       </c>
       <c r="D171" t="n">
-        <v>105428102</v>
+        <v>105885872</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6986,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D173" t="n">
-        <v>121521</v>
+        <v>123021</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7100,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D176" t="n">
-        <v>923246</v>
+        <v>926246</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7176,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32808</v>
+        <v>32923</v>
       </c>
       <c r="D178" t="n">
-        <v>48127239</v>
+        <v>48297457</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7252,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12442</v>
+        <v>12508</v>
       </c>
       <c r="D180" t="n">
-        <v>17987312</v>
+        <v>18082085</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7328,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1176</v>
+        <v>1186</v>
       </c>
       <c r="D182" t="n">
-        <v>1645328</v>
+        <v>1660166</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7404,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1482</v>
+        <v>1503</v>
       </c>
       <c r="D184" t="n">
-        <v>2083783</v>
+        <v>2113595</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7480,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>227614</v>
+        <v>228673</v>
       </c>
       <c r="D186" t="n">
-        <v>283238142</v>
+        <v>284539741</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7708,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="D192" t="n">
-        <v>1242497</v>
+        <v>1249997</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7784,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>83970</v>
+        <v>84246</v>
       </c>
       <c r="D194" t="n">
-        <v>123116913</v>
+        <v>123519133</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7898,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31619</v>
+        <v>31778</v>
       </c>
       <c r="D197" t="n">
-        <v>45519543</v>
+        <v>45745080</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -8012,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4780</v>
+        <v>4813</v>
       </c>
       <c r="D200" t="n">
-        <v>6810229</v>
+        <v>6855829</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8126,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4376</v>
+        <v>4422</v>
       </c>
       <c r="D203" t="n">
-        <v>6069383</v>
+        <v>6126829</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8240,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>250322</v>
+        <v>251679</v>
       </c>
       <c r="D206" t="n">
-        <v>309995510</v>
+        <v>311630975</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8316,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D208" t="n">
-        <v>338911</v>
+        <v>340064</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8582,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>91518</v>
+        <v>91917</v>
       </c>
       <c r="D215" t="n">
-        <v>133940603</v>
+        <v>134513892</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8620,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D216" t="n">
-        <v>120699</v>
+        <v>125199</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8696,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>48966</v>
+        <v>49205</v>
       </c>
       <c r="D218" t="n">
-        <v>70818422</v>
+        <v>71158042</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8734,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D219" t="n">
-        <v>39922</v>
+        <v>41422</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8810,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4398</v>
+        <v>4416</v>
       </c>
       <c r="D221" t="n">
-        <v>6170763</v>
+        <v>6197013</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8924,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5143</v>
+        <v>5203</v>
       </c>
       <c r="D224" t="n">
-        <v>7107570</v>
+        <v>7192711</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8962,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D225" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9038,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>101686</v>
+        <v>102186</v>
       </c>
       <c r="D227" t="n">
-        <v>127491857</v>
+        <v>128077389</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9228,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D232" t="n">
-        <v>804339</v>
+        <v>805839</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9304,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48034</v>
+        <v>48207</v>
       </c>
       <c r="D234" t="n">
-        <v>70396841</v>
+        <v>70648215</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9380,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11831</v>
+        <v>11889</v>
       </c>
       <c r="D236" t="n">
-        <v>17015671</v>
+        <v>17099217</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9456,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1809</v>
+        <v>1817</v>
       </c>
       <c r="D238" t="n">
-        <v>2596013</v>
+        <v>2606722</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9532,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2317</v>
+        <v>2329</v>
       </c>
       <c r="D240" t="n">
-        <v>3236253</v>
+        <v>3254253</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9570,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>245041</v>
+        <v>246342</v>
       </c>
       <c r="D241" t="n">
-        <v>309764769</v>
+        <v>311360917</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9798,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D247" t="n">
-        <v>1166064</v>
+        <v>1167564</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9874,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>92323</v>
+        <v>92708</v>
       </c>
       <c r="D249" t="n">
-        <v>135343563</v>
+        <v>135898468</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9988,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>61859</v>
+        <v>62216</v>
       </c>
       <c r="D252" t="n">
-        <v>89689555</v>
+        <v>90192928</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -10064,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2294</v>
+        <v>2300</v>
       </c>
       <c r="D254" t="n">
-        <v>3238142</v>
+        <v>3246380</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10178,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4154</v>
+        <v>4195</v>
       </c>
       <c r="D257" t="n">
-        <v>5828227</v>
+        <v>5888436</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-28 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>306223</v>
+        <v>308068</v>
       </c>
       <c r="D2" t="n">
-        <v>390783556</v>
+        <v>393057646</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D4" t="n">
-        <v>436843</v>
+        <v>437418</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="D8" t="n">
-        <v>1212315</v>
+        <v>1222607</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>23820</v>
+        <v>25256</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>113334</v>
+        <v>113827</v>
       </c>
       <c r="D10" t="n">
-        <v>166149096</v>
+        <v>166863750</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D11" t="n">
-        <v>198013</v>
+        <v>199513</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56771</v>
+        <v>57139</v>
       </c>
       <c r="D12" t="n">
-        <v>81971061</v>
+        <v>82493241</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3767</v>
+        <v>3795</v>
       </c>
       <c r="D16" t="n">
-        <v>5348624</v>
+        <v>5387842</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6007</v>
+        <v>6070</v>
       </c>
       <c r="D20" t="n">
-        <v>8399136</v>
+        <v>8486980</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74529</v>
+        <v>74863</v>
       </c>
       <c r="D22" t="n">
-        <v>93183159</v>
+        <v>93567941</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" t="n">
-        <v>64509</v>
+        <v>66009</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" t="n">
-        <v>18000</v>
+        <v>19500</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31555</v>
+        <v>31651</v>
       </c>
       <c r="D28" t="n">
-        <v>46208147</v>
+        <v>46346023</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11049</v>
+        <v>11096</v>
       </c>
       <c r="D30" t="n">
-        <v>15914009</v>
+        <v>15979554</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" t="n">
-        <v>21513</v>
+        <v>23013</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1477</v>
+        <v>1485</v>
       </c>
       <c r="D33" t="n">
-        <v>2075879</v>
+        <v>2087494</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1661</v>
+        <v>1681</v>
       </c>
       <c r="D35" t="n">
-        <v>2339428</v>
+        <v>2368314</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>93915</v>
+        <v>94351</v>
       </c>
       <c r="D36" t="n">
-        <v>118490606</v>
+        <v>118995861</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="D42" t="n">
-        <v>1305272</v>
+        <v>1306772</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43319</v>
+        <v>43465</v>
       </c>
       <c r="D44" t="n">
-        <v>63522241</v>
+        <v>63728927</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8806</v>
+        <v>8853</v>
       </c>
       <c r="D46" t="n">
-        <v>12643049</v>
+        <v>12711902</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1346</v>
+        <v>1350</v>
       </c>
       <c r="D48" t="n">
-        <v>1866279</v>
+        <v>1871519</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2114</v>
+        <v>2131</v>
       </c>
       <c r="D51" t="n">
-        <v>2945288</v>
+        <v>2970229</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>66295</v>
+        <v>66654</v>
       </c>
       <c r="D52" t="n">
-        <v>83265579</v>
+        <v>83701739</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D53" t="n">
-        <v>38383</v>
+        <v>39883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D54" t="n">
-        <v>56366</v>
+        <v>57866</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27334</v>
+        <v>27431</v>
       </c>
       <c r="D58" t="n">
-        <v>40092325</v>
+        <v>40235764</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10626</v>
+        <v>10684</v>
       </c>
       <c r="D61" t="n">
-        <v>15369479</v>
+        <v>15453344</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1306</v>
+        <v>1311</v>
       </c>
       <c r="D63" t="n">
-        <v>1821289</v>
+        <v>1828789</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D65" t="n">
-        <v>20400</v>
+        <v>21900</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1359</v>
+        <v>1372</v>
       </c>
       <c r="D67" t="n">
-        <v>1898921</v>
+        <v>1918421</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19528</v>
+        <v>19658</v>
       </c>
       <c r="D69" t="n">
-        <v>25565413</v>
+        <v>25746018</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D72" t="n">
-        <v>77073</v>
+        <v>78573</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7178</v>
+        <v>7259</v>
       </c>
       <c r="D73" t="n">
-        <v>10509608</v>
+        <v>10626165</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4869</v>
+        <v>4897</v>
       </c>
       <c r="D75" t="n">
-        <v>7070974</v>
+        <v>7112039</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="D76" t="n">
-        <v>649689</v>
+        <v>653239</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D77" t="n">
-        <v>347756</v>
+        <v>358713</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>135181</v>
+        <v>135823</v>
       </c>
       <c r="D78" t="n">
-        <v>168767915</v>
+        <v>169536804</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D80" t="n">
-        <v>119686</v>
+        <v>121186</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D82" t="n">
-        <v>595975</v>
+        <v>598975</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61631</v>
+        <v>61892</v>
       </c>
       <c r="D84" t="n">
-        <v>90372225</v>
+        <v>90743012</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28501</v>
+        <v>28647</v>
       </c>
       <c r="D87" t="n">
-        <v>41258785</v>
+        <v>41465744</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2559</v>
+        <v>2585</v>
       </c>
       <c r="D89" t="n">
-        <v>3684605</v>
+        <v>3722163</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2557</v>
+        <v>2588</v>
       </c>
       <c r="D90" t="n">
-        <v>3607895</v>
+        <v>3653384</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>29622</v>
+        <v>30030</v>
       </c>
       <c r="D91" t="n">
-        <v>40156045</v>
+        <v>40703157</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7403</v>
+        <v>7464</v>
       </c>
       <c r="D95" t="n">
-        <v>10901229</v>
+        <v>10988116</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6649</v>
+        <v>6737</v>
       </c>
       <c r="D97" t="n">
-        <v>9637508</v>
+        <v>9767443</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="D99" t="n">
-        <v>673905</v>
+        <v>679905</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D100" t="n">
-        <v>648773</v>
+        <v>650273</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7597</v>
+        <v>7809</v>
       </c>
       <c r="D101" t="n">
-        <v>10532585</v>
+        <v>10834993</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D102" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1925</v>
+        <v>1977</v>
       </c>
       <c r="D103" t="n">
-        <v>2833434</v>
+        <v>2910510</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2622</v>
+        <v>2683</v>
       </c>
       <c r="D105" t="n">
-        <v>3829013</v>
+        <v>3919379</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D107" t="n">
-        <v>154620</v>
+        <v>156120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D108" t="n">
-        <v>180189</v>
+        <v>189189</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>135844</v>
+        <v>136492</v>
       </c>
       <c r="D109" t="n">
-        <v>168093341</v>
+        <v>168886541</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D111" t="n">
-        <v>96874</v>
+        <v>101374</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="D113" t="n">
-        <v>1356382</v>
+        <v>1368382</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51303</v>
+        <v>51475</v>
       </c>
       <c r="D115" t="n">
-        <v>75233018</v>
+        <v>75485365</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D116" t="n">
-        <v>122159</v>
+        <v>124459</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>25924</v>
+        <v>26046</v>
       </c>
       <c r="D117" t="n">
-        <v>37567039</v>
+        <v>37741831</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1237</v>
+        <v>1252</v>
       </c>
       <c r="D118" t="n">
-        <v>1691352</v>
+        <v>1713298</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2070</v>
+        <v>2096</v>
       </c>
       <c r="D121" t="n">
-        <v>2908075</v>
+        <v>2941579</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>467557</v>
+        <v>472808</v>
       </c>
       <c r="D123" t="n">
-        <v>616426843</v>
+        <v>623479950</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D125" t="n">
-        <v>290743</v>
+        <v>293743</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1306</v>
+        <v>1316</v>
       </c>
       <c r="D128" t="n">
-        <v>1936292</v>
+        <v>1950311</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>198065</v>
+        <v>199200</v>
       </c>
       <c r="D130" t="n">
-        <v>291297788</v>
+        <v>292953351</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D131" t="n">
-        <v>544290</v>
+        <v>548790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>169832</v>
+        <v>171093</v>
       </c>
       <c r="D133" t="n">
-        <v>246944610</v>
+        <v>248758722</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D135" t="n">
-        <v>43832</v>
+        <v>45332</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2650</v>
+        <v>2664</v>
       </c>
       <c r="D136" t="n">
-        <v>3721234</v>
+        <v>3742234</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5645</v>
+        <v>5731</v>
       </c>
       <c r="D138" t="n">
-        <v>7974747</v>
+        <v>8098695</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>42146</v>
+        <v>42433</v>
       </c>
       <c r="D141" t="n">
-        <v>56358870</v>
+        <v>56729600</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D142" t="n">
-        <v>36791</v>
+        <v>38291</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D143" t="n">
-        <v>28730</v>
+        <v>33230</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13530</v>
+        <v>13588</v>
       </c>
       <c r="D147" t="n">
-        <v>19861386</v>
+        <v>19945063</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3575</v>
+        <v>3596</v>
       </c>
       <c r="D148" t="n">
-        <v>5156127</v>
+        <v>5187077</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D151" t="n">
-        <v>530722</v>
+        <v>533202</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D153" t="n">
-        <v>487809</v>
+        <v>492010</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16371</v>
+        <v>16532</v>
       </c>
       <c r="D154" t="n">
-        <v>21674871</v>
+        <v>21880036</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6776</v>
+        <v>6820</v>
       </c>
       <c r="D158" t="n">
-        <v>9862788</v>
+        <v>9926404</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4628</v>
+        <v>4687</v>
       </c>
       <c r="D160" t="n">
-        <v>6666674</v>
+        <v>6751040</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D162" t="n">
-        <v>352535</v>
+        <v>359559</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D163" t="n">
-        <v>341933</v>
+        <v>352433</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>13577</v>
+        <v>13909</v>
       </c>
       <c r="D165" t="n">
-        <v>19691075</v>
+        <v>20173710</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1629</v>
+        <v>1653</v>
       </c>
       <c r="D166" t="n">
-        <v>2422130</v>
+        <v>2458130</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D167" t="n">
-        <v>317302</v>
+        <v>327802</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D169" t="n">
-        <v>49190</v>
+        <v>50690</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>84578</v>
+        <v>84988</v>
       </c>
       <c r="D171" t="n">
-        <v>105885872</v>
+        <v>106388195</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D176" t="n">
-        <v>926246</v>
+        <v>927746</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>32923</v>
+        <v>33061</v>
       </c>
       <c r="D178" t="n">
-        <v>48297457</v>
+        <v>48498631</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12508</v>
+        <v>12546</v>
       </c>
       <c r="D180" t="n">
-        <v>18082085</v>
+        <v>18134434</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D181" t="n">
-        <v>12419</v>
+        <v>13919</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1186</v>
+        <v>1196</v>
       </c>
       <c r="D182" t="n">
-        <v>1660166</v>
+        <v>1673931</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1503</v>
+        <v>1520</v>
       </c>
       <c r="D184" t="n">
-        <v>2113595</v>
+        <v>2138367</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>228673</v>
+        <v>229910</v>
       </c>
       <c r="D186" t="n">
-        <v>284539741</v>
+        <v>286028511</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="D192" t="n">
-        <v>1249997</v>
+        <v>1254497</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>84246</v>
+        <v>84558</v>
       </c>
       <c r="D194" t="n">
-        <v>123519133</v>
+        <v>123978884</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31778</v>
+        <v>31925</v>
       </c>
       <c r="D197" t="n">
-        <v>45745080</v>
+        <v>45954766</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D199" t="n">
-        <v>17608</v>
+        <v>20608</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4813</v>
+        <v>4855</v>
       </c>
       <c r="D200" t="n">
-        <v>6855829</v>
+        <v>6916210</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4422</v>
+        <v>4480</v>
       </c>
       <c r="D203" t="n">
-        <v>6126829</v>
+        <v>6195842</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>251679</v>
+        <v>253109</v>
       </c>
       <c r="D206" t="n">
-        <v>311630975</v>
+        <v>313350987</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D207" t="n">
-        <v>163190</v>
+        <v>165408</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D208" t="n">
-        <v>340064</v>
+        <v>347564</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D209" t="n">
-        <v>20935</v>
+        <v>22435</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D213" t="n">
-        <v>869856</v>
+        <v>873906</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>91917</v>
+        <v>92325</v>
       </c>
       <c r="D215" t="n">
-        <v>134513892</v>
+        <v>135110335</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>49205</v>
+        <v>49483</v>
       </c>
       <c r="D218" t="n">
-        <v>71158042</v>
+        <v>71554867</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4416</v>
+        <v>4443</v>
       </c>
       <c r="D221" t="n">
-        <v>6197013</v>
+        <v>6233214</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D222" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5203</v>
+        <v>5262</v>
       </c>
       <c r="D224" t="n">
-        <v>7192711</v>
+        <v>7275165</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>102186</v>
+        <v>102649</v>
       </c>
       <c r="D227" t="n">
-        <v>128077389</v>
+        <v>128627483</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D229" t="n">
-        <v>98945</v>
+        <v>100445</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D232" t="n">
-        <v>805839</v>
+        <v>811839</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48207</v>
+        <v>48363</v>
       </c>
       <c r="D234" t="n">
-        <v>70648215</v>
+        <v>70869826</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11889</v>
+        <v>11950</v>
       </c>
       <c r="D236" t="n">
-        <v>17099217</v>
+        <v>17182461</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1817</v>
+        <v>1828</v>
       </c>
       <c r="D238" t="n">
-        <v>2606722</v>
+        <v>2621159</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2329</v>
+        <v>2345</v>
       </c>
       <c r="D240" t="n">
-        <v>3254253</v>
+        <v>3275374</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>246342</v>
+        <v>247671</v>
       </c>
       <c r="D241" t="n">
-        <v>311360917</v>
+        <v>313011444</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D243" t="n">
-        <v>342957</v>
+        <v>347457</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="D247" t="n">
-        <v>1167564</v>
+        <v>1168396</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>92708</v>
+        <v>93159</v>
       </c>
       <c r="D249" t="n">
-        <v>135898468</v>
+        <v>136553276</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D250" t="n">
-        <v>106661</v>
+        <v>108161</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>62216</v>
+        <v>62534</v>
       </c>
       <c r="D252" t="n">
-        <v>90192928</v>
+        <v>90645181</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2300</v>
+        <v>2317</v>
       </c>
       <c r="D254" t="n">
-        <v>3246380</v>
+        <v>3269549</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4195</v>
+        <v>4237</v>
       </c>
       <c r="D257" t="n">
-        <v>5888436</v>
+        <v>5946510</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-29 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>308068</v>
+        <v>309473</v>
       </c>
       <c r="D2" t="n">
-        <v>393057646</v>
+        <v>394789073</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D3" t="n">
-        <v>299205</v>
+        <v>300350</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D4" t="n">
-        <v>437418</v>
+        <v>441918</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D8" t="n">
-        <v>1222607</v>
+        <v>1224107</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>113827</v>
+        <v>114254</v>
       </c>
       <c r="D10" t="n">
-        <v>166863750</v>
+        <v>167482684</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D11" t="n">
-        <v>199513</v>
+        <v>207013</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>57139</v>
+        <v>57400</v>
       </c>
       <c r="D12" t="n">
-        <v>82493241</v>
+        <v>82868470</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3795</v>
+        <v>3818</v>
       </c>
       <c r="D16" t="n">
-        <v>5387842</v>
+        <v>5421792</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" t="n">
-        <v>97035</v>
+        <v>98535</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6070</v>
+        <v>6162</v>
       </c>
       <c r="D20" t="n">
-        <v>8486980</v>
+        <v>8610222</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74863</v>
+        <v>75148</v>
       </c>
       <c r="D22" t="n">
-        <v>93567941</v>
+        <v>93902311</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23" t="n">
-        <v>66009</v>
+        <v>66709</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D27" t="n">
-        <v>405647</v>
+        <v>407147</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31651</v>
+        <v>31771</v>
       </c>
       <c r="D28" t="n">
-        <v>46346023</v>
+        <v>46522351</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11096</v>
+        <v>11143</v>
       </c>
       <c r="D30" t="n">
-        <v>15979554</v>
+        <v>16045328</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1485</v>
+        <v>1490</v>
       </c>
       <c r="D33" t="n">
-        <v>2087494</v>
+        <v>2094294</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1681</v>
+        <v>1692</v>
       </c>
       <c r="D35" t="n">
-        <v>2368314</v>
+        <v>2383549</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>94351</v>
+        <v>94611</v>
       </c>
       <c r="D36" t="n">
-        <v>118995861</v>
+        <v>119292982</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" t="n">
-        <v>73613</v>
+        <v>74727</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D42" t="n">
-        <v>1306772</v>
+        <v>1308272</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43465</v>
+        <v>43573</v>
       </c>
       <c r="D44" t="n">
-        <v>63728927</v>
+        <v>63883540</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8853</v>
+        <v>8889</v>
       </c>
       <c r="D46" t="n">
-        <v>12711902</v>
+        <v>12763932</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1350</v>
+        <v>1359</v>
       </c>
       <c r="D48" t="n">
-        <v>1871519</v>
+        <v>1885019</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2131</v>
+        <v>2146</v>
       </c>
       <c r="D51" t="n">
-        <v>2970229</v>
+        <v>2990888</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>66654</v>
+        <v>66919</v>
       </c>
       <c r="D52" t="n">
-        <v>83701739</v>
+        <v>84020499</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27431</v>
+        <v>27521</v>
       </c>
       <c r="D58" t="n">
-        <v>40235764</v>
+        <v>40366157</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10684</v>
+        <v>10731</v>
       </c>
       <c r="D61" t="n">
-        <v>15453344</v>
+        <v>15521011</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1311</v>
+        <v>1323</v>
       </c>
       <c r="D63" t="n">
-        <v>1828789</v>
+        <v>1846789</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1372</v>
+        <v>1379</v>
       </c>
       <c r="D67" t="n">
-        <v>1918421</v>
+        <v>1927403</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19658</v>
+        <v>19780</v>
       </c>
       <c r="D69" t="n">
-        <v>25746018</v>
+        <v>25906320</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D70" t="n">
-        <v>39736</v>
+        <v>41126</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D72" t="n">
-        <v>78573</v>
+        <v>80073</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7259</v>
+        <v>7311</v>
       </c>
       <c r="D73" t="n">
-        <v>10626165</v>
+        <v>10703227</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4897</v>
+        <v>4925</v>
       </c>
       <c r="D75" t="n">
-        <v>7112039</v>
+        <v>7153369</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D76" t="n">
-        <v>653239</v>
+        <v>656239</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D77" t="n">
-        <v>358713</v>
+        <v>363213</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>135823</v>
+        <v>136395</v>
       </c>
       <c r="D78" t="n">
-        <v>169536804</v>
+        <v>170213634</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D83" t="n">
-        <v>15938</v>
+        <v>17438</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>61892</v>
+        <v>62144</v>
       </c>
       <c r="D84" t="n">
-        <v>90743012</v>
+        <v>91106030</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28647</v>
+        <v>28778</v>
       </c>
       <c r="D87" t="n">
-        <v>41465744</v>
+        <v>41657015</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2585</v>
+        <v>2611</v>
       </c>
       <c r="D89" t="n">
-        <v>3722163</v>
+        <v>3758692</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2588</v>
+        <v>2609</v>
       </c>
       <c r="D90" t="n">
-        <v>3653384</v>
+        <v>3683347</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>30030</v>
+        <v>30328</v>
       </c>
       <c r="D91" t="n">
-        <v>40703157</v>
+        <v>41098166</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7464</v>
+        <v>7521</v>
       </c>
       <c r="D95" t="n">
-        <v>10988116</v>
+        <v>11071620</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6737</v>
+        <v>6789</v>
       </c>
       <c r="D97" t="n">
-        <v>9767443</v>
+        <v>9841716</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="D99" t="n">
-        <v>679905</v>
+        <v>687405</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D100" t="n">
-        <v>650273</v>
+        <v>653273</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7809</v>
+        <v>7940</v>
       </c>
       <c r="D101" t="n">
-        <v>10834993</v>
+        <v>11019065</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1977</v>
+        <v>2021</v>
       </c>
       <c r="D103" t="n">
-        <v>2910510</v>
+        <v>2975415</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2683</v>
+        <v>2737</v>
       </c>
       <c r="D105" t="n">
-        <v>3919379</v>
+        <v>3996373</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D108" t="n">
-        <v>189189</v>
+        <v>196689</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>136492</v>
+        <v>137023</v>
       </c>
       <c r="D109" t="n">
-        <v>168886541</v>
+        <v>169528862</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>932</v>
+        <v>937</v>
       </c>
       <c r="D113" t="n">
-        <v>1368382</v>
+        <v>1375882</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51475</v>
+        <v>51605</v>
       </c>
       <c r="D115" t="n">
-        <v>75485365</v>
+        <v>75672727</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26046</v>
+        <v>26138</v>
       </c>
       <c r="D117" t="n">
-        <v>37741831</v>
+        <v>37871454</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1252</v>
+        <v>1259</v>
       </c>
       <c r="D118" t="n">
-        <v>1713298</v>
+        <v>1723356</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2096</v>
+        <v>2119</v>
       </c>
       <c r="D121" t="n">
-        <v>2941579</v>
+        <v>2973107</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>472808</v>
+        <v>476606</v>
       </c>
       <c r="D123" t="n">
-        <v>623479950</v>
+        <v>628508024</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1316</v>
+        <v>1324</v>
       </c>
       <c r="D128" t="n">
-        <v>1950311</v>
+        <v>1962311</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D129" t="n">
-        <v>38273</v>
+        <v>39010</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>199200</v>
+        <v>200279</v>
       </c>
       <c r="D130" t="n">
-        <v>292953351</v>
+        <v>294512507</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D131" t="n">
-        <v>548790</v>
+        <v>554790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>171093</v>
+        <v>172270</v>
       </c>
       <c r="D133" t="n">
-        <v>248758722</v>
+        <v>250457545</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2664</v>
+        <v>2686</v>
       </c>
       <c r="D136" t="n">
-        <v>3742234</v>
+        <v>3771597</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5731</v>
+        <v>5826</v>
       </c>
       <c r="D138" t="n">
-        <v>8098695</v>
+        <v>8232797</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>42433</v>
+        <v>42695</v>
       </c>
       <c r="D141" t="n">
-        <v>56729600</v>
+        <v>57074279</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13588</v>
+        <v>13637</v>
       </c>
       <c r="D147" t="n">
-        <v>19945063</v>
+        <v>20010076</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3596</v>
+        <v>3623</v>
       </c>
       <c r="D148" t="n">
-        <v>5187077</v>
+        <v>5227267</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D151" t="n">
-        <v>533202</v>
+        <v>536202</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D153" t="n">
-        <v>492010</v>
+        <v>495010</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16532</v>
+        <v>16651</v>
       </c>
       <c r="D154" t="n">
-        <v>21880036</v>
+        <v>22024026</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D157" t="n">
-        <v>55406</v>
+        <v>56906</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6820</v>
+        <v>6866</v>
       </c>
       <c r="D158" t="n">
-        <v>9926404</v>
+        <v>9993822</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4687</v>
+        <v>4727</v>
       </c>
       <c r="D160" t="n">
-        <v>6751040</v>
+        <v>6808755</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D162" t="n">
-        <v>359559</v>
+        <v>365559</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D163" t="n">
-        <v>352433</v>
+        <v>353933</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>13909</v>
+        <v>14071</v>
       </c>
       <c r="D165" t="n">
-        <v>20173710</v>
+        <v>20410134</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1653</v>
+        <v>1671</v>
       </c>
       <c r="D166" t="n">
-        <v>2458130</v>
+        <v>2485130</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D167" t="n">
-        <v>327802</v>
+        <v>330802</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>84988</v>
+        <v>85305</v>
       </c>
       <c r="D171" t="n">
-        <v>106388195</v>
+        <v>106773857</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D172" t="n">
-        <v>34729</v>
+        <v>36229</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="D176" t="n">
-        <v>927746</v>
+        <v>931348</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33061</v>
+        <v>33156</v>
       </c>
       <c r="D178" t="n">
-        <v>48498631</v>
+        <v>48635526</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12546</v>
+        <v>12605</v>
       </c>
       <c r="D180" t="n">
-        <v>18134434</v>
+        <v>18215592</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1196</v>
+        <v>1199</v>
       </c>
       <c r="D182" t="n">
-        <v>1673931</v>
+        <v>1678257</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1520</v>
+        <v>1540</v>
       </c>
       <c r="D184" t="n">
-        <v>2138367</v>
+        <v>2165709</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>229910</v>
+        <v>230824</v>
       </c>
       <c r="D186" t="n">
-        <v>286028511</v>
+        <v>287152057</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D188" t="n">
-        <v>233236</v>
+        <v>234736</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>853</v>
+        <v>859</v>
       </c>
       <c r="D192" t="n">
-        <v>1254497</v>
+        <v>1263497</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>84558</v>
+        <v>84783</v>
       </c>
       <c r="D194" t="n">
-        <v>123978884</v>
+        <v>124306984</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D195" t="n">
-        <v>130627</v>
+        <v>133627</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>31925</v>
+        <v>32046</v>
       </c>
       <c r="D197" t="n">
-        <v>45954766</v>
+        <v>46127048</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4855</v>
+        <v>4888</v>
       </c>
       <c r="D200" t="n">
-        <v>6916210</v>
+        <v>6964365</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4480</v>
+        <v>4522</v>
       </c>
       <c r="D203" t="n">
-        <v>6195842</v>
+        <v>6255652</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>253109</v>
+        <v>254361</v>
       </c>
       <c r="D206" t="n">
-        <v>313350987</v>
+        <v>314916624</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D207" t="n">
-        <v>165408</v>
+        <v>166518</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D208" t="n">
-        <v>347564</v>
+        <v>349064</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D213" t="n">
-        <v>873906</v>
+        <v>876906</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>92325</v>
+        <v>92676</v>
       </c>
       <c r="D215" t="n">
-        <v>135110335</v>
+        <v>135622863</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>49483</v>
+        <v>49743</v>
       </c>
       <c r="D218" t="n">
-        <v>71554867</v>
+        <v>71927879</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4443</v>
+        <v>4489</v>
       </c>
       <c r="D221" t="n">
-        <v>6233214</v>
+        <v>6298404</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5262</v>
+        <v>5313</v>
       </c>
       <c r="D224" t="n">
-        <v>7275165</v>
+        <v>7345090</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>102649</v>
+        <v>103072</v>
       </c>
       <c r="D227" t="n">
-        <v>128627483</v>
+        <v>129145086</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D229" t="n">
-        <v>100445</v>
+        <v>101945</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D232" t="n">
-        <v>811839</v>
+        <v>816339</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48363</v>
+        <v>48498</v>
       </c>
       <c r="D234" t="n">
-        <v>70869826</v>
+        <v>71066993</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11950</v>
+        <v>11987</v>
       </c>
       <c r="D236" t="n">
-        <v>17182461</v>
+        <v>17235823</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1828</v>
+        <v>1837</v>
       </c>
       <c r="D238" t="n">
-        <v>2621159</v>
+        <v>2634659</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2345</v>
+        <v>2366</v>
       </c>
       <c r="D240" t="n">
-        <v>3275374</v>
+        <v>3304968</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>247671</v>
+        <v>248729</v>
       </c>
       <c r="D241" t="n">
-        <v>313011444</v>
+        <v>314298908</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D242" t="n">
-        <v>200816</v>
+        <v>204290</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D243" t="n">
-        <v>347457</v>
+        <v>348957</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D247" t="n">
-        <v>1168396</v>
+        <v>1169896</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>93159</v>
+        <v>93512</v>
       </c>
       <c r="D249" t="n">
-        <v>136553276</v>
+        <v>137060782</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>62534</v>
+        <v>62766</v>
       </c>
       <c r="D252" t="n">
-        <v>90645181</v>
+        <v>90973646</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2317</v>
+        <v>2328</v>
       </c>
       <c r="D254" t="n">
-        <v>3269549</v>
+        <v>3286049</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4237</v>
+        <v>4277</v>
       </c>
       <c r="D257" t="n">
-        <v>5946510</v>
+        <v>6005261</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>309473</v>
+        <v>310991</v>
       </c>
       <c r="D2" t="n">
-        <v>394789073</v>
+        <v>396647845</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D4" t="n">
-        <v>441918</v>
+        <v>444918</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="D8" t="n">
-        <v>1224107</v>
+        <v>1230107</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>114254</v>
+        <v>114713</v>
       </c>
       <c r="D10" t="n">
-        <v>167482684</v>
+        <v>168138944</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D11" t="n">
-        <v>207013</v>
+        <v>208513</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>57400</v>
+        <v>57638</v>
       </c>
       <c r="D12" t="n">
-        <v>82868470</v>
+        <v>83212065</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3818</v>
+        <v>3853</v>
       </c>
       <c r="D16" t="n">
-        <v>5421792</v>
+        <v>5472028</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6162</v>
+        <v>6253</v>
       </c>
       <c r="D20" t="n">
-        <v>8610222</v>
+        <v>8733268</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>75148</v>
+        <v>75443</v>
       </c>
       <c r="D22" t="n">
-        <v>93902311</v>
+        <v>94243622</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" t="n">
-        <v>66709</v>
+        <v>68209</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D27" t="n">
-        <v>407147</v>
+        <v>408647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31771</v>
+        <v>31880</v>
       </c>
       <c r="D28" t="n">
-        <v>46522351</v>
+        <v>46677875</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11143</v>
+        <v>11195</v>
       </c>
       <c r="D30" t="n">
-        <v>16045328</v>
+        <v>16118429</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1490</v>
+        <v>1510</v>
       </c>
       <c r="D33" t="n">
-        <v>2094294</v>
+        <v>2122793</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1692</v>
+        <v>1703</v>
       </c>
       <c r="D35" t="n">
-        <v>2383549</v>
+        <v>2399215</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>94611</v>
+        <v>94910</v>
       </c>
       <c r="D36" t="n">
-        <v>119292982</v>
+        <v>119657547</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D38" t="n">
-        <v>109008</v>
+        <v>110508</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="D42" t="n">
-        <v>1308272</v>
+        <v>1312902</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43573</v>
+        <v>43705</v>
       </c>
       <c r="D44" t="n">
-        <v>63883540</v>
+        <v>64077770</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8889</v>
+        <v>8919</v>
       </c>
       <c r="D46" t="n">
-        <v>12763932</v>
+        <v>12806979</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1359</v>
+        <v>1366</v>
       </c>
       <c r="D48" t="n">
-        <v>1885019</v>
+        <v>1895519</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2146</v>
+        <v>2169</v>
       </c>
       <c r="D51" t="n">
-        <v>2990888</v>
+        <v>3021365</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>66919</v>
+        <v>67175</v>
       </c>
       <c r="D52" t="n">
-        <v>84020499</v>
+        <v>84344191</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D56" t="n">
-        <v>554844</v>
+        <v>556965</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27521</v>
+        <v>27616</v>
       </c>
       <c r="D58" t="n">
-        <v>40366157</v>
+        <v>40504618</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10731</v>
+        <v>10794</v>
       </c>
       <c r="D61" t="n">
-        <v>15521011</v>
+        <v>15610878</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1323</v>
+        <v>1334</v>
       </c>
       <c r="D63" t="n">
-        <v>1846789</v>
+        <v>1863289</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1379</v>
+        <v>1393</v>
       </c>
       <c r="D67" t="n">
-        <v>1927403</v>
+        <v>1946818</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19780</v>
+        <v>19869</v>
       </c>
       <c r="D69" t="n">
-        <v>25906320</v>
+        <v>26027863</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D70" t="n">
-        <v>41126</v>
+        <v>42626</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D72" t="n">
-        <v>80073</v>
+        <v>83073</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7311</v>
+        <v>7355</v>
       </c>
       <c r="D73" t="n">
-        <v>10703227</v>
+        <v>10768145</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4925</v>
+        <v>4954</v>
       </c>
       <c r="D75" t="n">
-        <v>7153369</v>
+        <v>7191516</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D76" t="n">
-        <v>656239</v>
+        <v>657739</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D77" t="n">
-        <v>363213</v>
+        <v>369673</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>136395</v>
+        <v>136961</v>
       </c>
       <c r="D78" t="n">
-        <v>170213634</v>
+        <v>170905244</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D81" t="n">
-        <v>26650</v>
+        <v>29650</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="D82" t="n">
-        <v>598975</v>
+        <v>607416</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62144</v>
+        <v>62370</v>
       </c>
       <c r="D84" t="n">
-        <v>91106030</v>
+        <v>91425250</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28778</v>
+        <v>28928</v>
       </c>
       <c r="D87" t="n">
-        <v>41657015</v>
+        <v>41859716</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2611</v>
+        <v>2636</v>
       </c>
       <c r="D89" t="n">
-        <v>3758692</v>
+        <v>3794012</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2609</v>
+        <v>2638</v>
       </c>
       <c r="D90" t="n">
-        <v>3683347</v>
+        <v>3725197</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>30328</v>
+        <v>30697</v>
       </c>
       <c r="D91" t="n">
-        <v>41098166</v>
+        <v>41606096</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7521</v>
+        <v>7581</v>
       </c>
       <c r="D95" t="n">
-        <v>11071620</v>
+        <v>11160262</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6789</v>
+        <v>6841</v>
       </c>
       <c r="D97" t="n">
-        <v>9841716</v>
+        <v>9915655</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="D99" t="n">
-        <v>687405</v>
+        <v>708405</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D100" t="n">
-        <v>653273</v>
+        <v>654088</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7940</v>
+        <v>8076</v>
       </c>
       <c r="D101" t="n">
-        <v>11019065</v>
+        <v>11206558</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2021</v>
+        <v>2069</v>
       </c>
       <c r="D103" t="n">
-        <v>2975415</v>
+        <v>3045507</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D104" t="n">
-        <v>12000</v>
+        <v>13500</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2737</v>
+        <v>2763</v>
       </c>
       <c r="D105" t="n">
-        <v>3996373</v>
+        <v>4034212</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D107" t="n">
-        <v>156120</v>
+        <v>162120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D108" t="n">
-        <v>196689</v>
+        <v>212265</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>137023</v>
+        <v>137537</v>
       </c>
       <c r="D109" t="n">
-        <v>169528862</v>
+        <v>170164377</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c r="D113" t="n">
-        <v>1375882</v>
+        <v>1380382</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51605</v>
+        <v>51756</v>
       </c>
       <c r="D115" t="n">
-        <v>75672727</v>
+        <v>75887829</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26138</v>
+        <v>26251</v>
       </c>
       <c r="D117" t="n">
-        <v>37871454</v>
+        <v>38035618</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1259</v>
+        <v>1271</v>
       </c>
       <c r="D118" t="n">
-        <v>1723356</v>
+        <v>1738865</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2119</v>
+        <v>2138</v>
       </c>
       <c r="D121" t="n">
-        <v>2973107</v>
+        <v>3000581</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>476606</v>
+        <v>480323</v>
       </c>
       <c r="D123" t="n">
-        <v>628508024</v>
+        <v>633427410</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D125" t="n">
-        <v>293743</v>
+        <v>297996</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D127" t="n">
-        <v>31498</v>
+        <v>32998</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1324</v>
+        <v>1342</v>
       </c>
       <c r="D128" t="n">
-        <v>1962311</v>
+        <v>1989311</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>200279</v>
+        <v>201359</v>
       </c>
       <c r="D130" t="n">
-        <v>294512507</v>
+        <v>296073399</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="D131" t="n">
-        <v>554790</v>
+        <v>565290</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>172270</v>
+        <v>173419</v>
       </c>
       <c r="D133" t="n">
-        <v>250457545</v>
+        <v>252106243</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2686</v>
+        <v>2714</v>
       </c>
       <c r="D136" t="n">
-        <v>3771597</v>
+        <v>3811489</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5826</v>
+        <v>5945</v>
       </c>
       <c r="D138" t="n">
-        <v>8232797</v>
+        <v>8397513</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>42695</v>
+        <v>42936</v>
       </c>
       <c r="D141" t="n">
-        <v>57074279</v>
+        <v>57378945</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D142" t="n">
-        <v>38291</v>
+        <v>39791</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>355</v>
+        <v>385</v>
       </c>
       <c r="D146" t="n">
-        <v>532165</v>
+        <v>577165</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13637</v>
+        <v>13694</v>
       </c>
       <c r="D147" t="n">
-        <v>20010076</v>
+        <v>20093699</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3623</v>
+        <v>3639</v>
       </c>
       <c r="D148" t="n">
-        <v>5227267</v>
+        <v>5249824</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="D151" t="n">
-        <v>536202</v>
+        <v>549702</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D153" t="n">
-        <v>495010</v>
+        <v>498010</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16651</v>
+        <v>16764</v>
       </c>
       <c r="D154" t="n">
-        <v>22024026</v>
+        <v>22163201</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6866</v>
+        <v>6904</v>
       </c>
       <c r="D158" t="n">
-        <v>9993822</v>
+        <v>10047146</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4727</v>
+        <v>4768</v>
       </c>
       <c r="D160" t="n">
-        <v>6808755</v>
+        <v>6868125</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D162" t="n">
-        <v>365559</v>
+        <v>368559</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D163" t="n">
-        <v>353933</v>
+        <v>356933</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14071</v>
+        <v>14186</v>
       </c>
       <c r="D165" t="n">
-        <v>20410134</v>
+        <v>20572820</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1671</v>
+        <v>1678</v>
       </c>
       <c r="D166" t="n">
-        <v>2485130</v>
+        <v>2495630</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D167" t="n">
-        <v>330802</v>
+        <v>332302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D169" t="n">
-        <v>50690</v>
+        <v>59690</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>85305</v>
+        <v>85548</v>
       </c>
       <c r="D171" t="n">
-        <v>106773857</v>
+        <v>107065121</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D172" t="n">
-        <v>36229</v>
+        <v>36655</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D176" t="n">
-        <v>931348</v>
+        <v>932848</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33156</v>
+        <v>33256</v>
       </c>
       <c r="D178" t="n">
-        <v>48635526</v>
+        <v>48782438</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D179" t="n">
-        <v>39000</v>
+        <v>40500</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12605</v>
+        <v>12671</v>
       </c>
       <c r="D180" t="n">
-        <v>18215592</v>
+        <v>18311606</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1199</v>
+        <v>1206</v>
       </c>
       <c r="D182" t="n">
-        <v>1678257</v>
+        <v>1687223</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1540</v>
+        <v>1564</v>
       </c>
       <c r="D184" t="n">
-        <v>2165709</v>
+        <v>2201709</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>230824</v>
+        <v>231717</v>
       </c>
       <c r="D186" t="n">
-        <v>287152057</v>
+        <v>288209196</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D187" t="n">
-        <v>140030</v>
+        <v>141530</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="D192" t="n">
-        <v>1263497</v>
+        <v>1266497</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>84783</v>
+        <v>85065</v>
       </c>
       <c r="D194" t="n">
-        <v>124306984</v>
+        <v>124718468</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D195" t="n">
-        <v>133627</v>
+        <v>135127</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32046</v>
+        <v>32189</v>
       </c>
       <c r="D197" t="n">
-        <v>46127048</v>
+        <v>46332744</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4888</v>
+        <v>4931</v>
       </c>
       <c r="D200" t="n">
-        <v>6964365</v>
+        <v>7026228</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4522</v>
+        <v>4557</v>
       </c>
       <c r="D203" t="n">
-        <v>6255652</v>
+        <v>6306114</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>254361</v>
+        <v>255607</v>
       </c>
       <c r="D206" t="n">
-        <v>314916624</v>
+        <v>316464521</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D208" t="n">
-        <v>349064</v>
+        <v>350564</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D213" t="n">
-        <v>876906</v>
+        <v>878406</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>92676</v>
+        <v>93112</v>
       </c>
       <c r="D215" t="n">
-        <v>135622863</v>
+        <v>136244812</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>49743</v>
+        <v>50006</v>
       </c>
       <c r="D218" t="n">
-        <v>71927879</v>
+        <v>72291084</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D219" t="n">
-        <v>41422</v>
+        <v>42922</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4489</v>
+        <v>4511</v>
       </c>
       <c r="D221" t="n">
-        <v>6298404</v>
+        <v>6327023</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5313</v>
+        <v>5362</v>
       </c>
       <c r="D224" t="n">
-        <v>7345090</v>
+        <v>7414480</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>103072</v>
+        <v>103453</v>
       </c>
       <c r="D227" t="n">
-        <v>129145086</v>
+        <v>129570862</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D229" t="n">
-        <v>101945</v>
+        <v>103445</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D232" t="n">
-        <v>816339</v>
+        <v>819339</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48498</v>
+        <v>48640</v>
       </c>
       <c r="D234" t="n">
-        <v>71066993</v>
+        <v>71270549</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>11987</v>
+        <v>12040</v>
       </c>
       <c r="D236" t="n">
-        <v>17235823</v>
+        <v>17310351</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1837</v>
+        <v>1850</v>
       </c>
       <c r="D238" t="n">
-        <v>2634659</v>
+        <v>2654159</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2366</v>
+        <v>2389</v>
       </c>
       <c r="D240" t="n">
-        <v>3304968</v>
+        <v>3337538</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>248729</v>
+        <v>249895</v>
       </c>
       <c r="D241" t="n">
-        <v>314298908</v>
+        <v>315735112</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D242" t="n">
-        <v>204290</v>
+        <v>206936</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="D247" t="n">
-        <v>1169896</v>
+        <v>1178896</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>93512</v>
+        <v>93825</v>
       </c>
       <c r="D249" t="n">
-        <v>137060782</v>
+        <v>137509273</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D250" t="n">
-        <v>108161</v>
+        <v>111161</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>62766</v>
+        <v>63057</v>
       </c>
       <c r="D252" t="n">
-        <v>90973646</v>
+        <v>91386696</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2328</v>
+        <v>2344</v>
       </c>
       <c r="D254" t="n">
-        <v>3286049</v>
+        <v>3308589</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4277</v>
+        <v>4340</v>
       </c>
       <c r="D257" t="n">
-        <v>6005261</v>
+        <v>6092591</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-31 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>310991</v>
+        <v>312670</v>
       </c>
       <c r="D2" t="n">
-        <v>396647845</v>
+        <v>398708282</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="D8" t="n">
-        <v>1230107</v>
+        <v>1240607</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>114713</v>
+        <v>115236</v>
       </c>
       <c r="D10" t="n">
-        <v>168138944</v>
+        <v>168876720</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>57638</v>
+        <v>57972</v>
       </c>
       <c r="D12" t="n">
-        <v>83212065</v>
+        <v>83682410</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3853</v>
+        <v>3901</v>
       </c>
       <c r="D16" t="n">
-        <v>5472028</v>
+        <v>5541112</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6253</v>
+        <v>6328</v>
       </c>
       <c r="D20" t="n">
-        <v>8733268</v>
+        <v>8833021</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>75443</v>
+        <v>75750</v>
       </c>
       <c r="D22" t="n">
-        <v>94243622</v>
+        <v>94592520</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D23" t="n">
-        <v>68209</v>
+        <v>69709</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>31880</v>
+        <v>32025</v>
       </c>
       <c r="D28" t="n">
-        <v>46677875</v>
+        <v>46887378</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11195</v>
+        <v>11241</v>
       </c>
       <c r="D30" t="n">
-        <v>16118429</v>
+        <v>16176617</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1510</v>
+        <v>1538</v>
       </c>
       <c r="D33" t="n">
-        <v>2122793</v>
+        <v>2160632</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1703</v>
+        <v>1732</v>
       </c>
       <c r="D35" t="n">
-        <v>2399215</v>
+        <v>2442462</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>94910</v>
+        <v>95220</v>
       </c>
       <c r="D36" t="n">
-        <v>119657547</v>
+        <v>120020647</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D37" t="n">
-        <v>74727</v>
+        <v>75537</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D38" t="n">
-        <v>110508</v>
+        <v>113508</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="D42" t="n">
-        <v>1312902</v>
+        <v>1318685</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43705</v>
+        <v>43840</v>
       </c>
       <c r="D44" t="n">
-        <v>64077770</v>
+        <v>64265036</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D45" t="n">
-        <v>34450</v>
+        <v>35950</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8919</v>
+        <v>8951</v>
       </c>
       <c r="D46" t="n">
-        <v>12806979</v>
+        <v>12848358</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1366</v>
+        <v>1378</v>
       </c>
       <c r="D48" t="n">
-        <v>1895519</v>
+        <v>1913400</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2169</v>
+        <v>2205</v>
       </c>
       <c r="D51" t="n">
-        <v>3021365</v>
+        <v>3073244</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67175</v>
+        <v>67506</v>
       </c>
       <c r="D52" t="n">
-        <v>84344191</v>
+        <v>84750976</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D56" t="n">
-        <v>556965</v>
+        <v>558465</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27616</v>
+        <v>27715</v>
       </c>
       <c r="D58" t="n">
-        <v>40504618</v>
+        <v>40647682</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10794</v>
+        <v>10847</v>
       </c>
       <c r="D61" t="n">
-        <v>15610878</v>
+        <v>15685809</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1334</v>
+        <v>1338</v>
       </c>
       <c r="D63" t="n">
-        <v>1863289</v>
+        <v>1869289</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1393</v>
+        <v>1404</v>
       </c>
       <c r="D67" t="n">
-        <v>1946818</v>
+        <v>1963318</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19869</v>
+        <v>19980</v>
       </c>
       <c r="D69" t="n">
-        <v>26027863</v>
+        <v>26168565</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7355</v>
+        <v>7415</v>
       </c>
       <c r="D73" t="n">
-        <v>10768145</v>
+        <v>10856094</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4954</v>
+        <v>4973</v>
       </c>
       <c r="D75" t="n">
-        <v>7191516</v>
+        <v>7219515</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D76" t="n">
-        <v>657739</v>
+        <v>663739</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D77" t="n">
-        <v>369673</v>
+        <v>372673</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>136961</v>
+        <v>137547</v>
       </c>
       <c r="D78" t="n">
-        <v>170905244</v>
+        <v>171647175</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="D82" t="n">
-        <v>607416</v>
+        <v>616416</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62370</v>
+        <v>62603</v>
       </c>
       <c r="D84" t="n">
-        <v>91425250</v>
+        <v>91763728</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D85" t="n">
-        <v>115582</v>
+        <v>117082</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D86" t="n">
-        <v>10500</v>
+        <v>13500</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>28928</v>
+        <v>29066</v>
       </c>
       <c r="D87" t="n">
-        <v>41859716</v>
+        <v>42061809</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2636</v>
+        <v>2659</v>
       </c>
       <c r="D89" t="n">
-        <v>3794012</v>
+        <v>3827740</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2638</v>
+        <v>2689</v>
       </c>
       <c r="D90" t="n">
-        <v>3725197</v>
+        <v>3799740</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>30697</v>
+        <v>31158</v>
       </c>
       <c r="D91" t="n">
-        <v>41606096</v>
+        <v>42216821</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D94" t="n">
-        <v>35814</v>
+        <v>37314</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7581</v>
+        <v>7675</v>
       </c>
       <c r="D95" t="n">
-        <v>11160262</v>
+        <v>11288846</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6841</v>
+        <v>6917</v>
       </c>
       <c r="D97" t="n">
-        <v>9915655</v>
+        <v>10027028</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="D99" t="n">
-        <v>708405</v>
+        <v>721885</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="D100" t="n">
-        <v>654088</v>
+        <v>662524</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8076</v>
+        <v>8310</v>
       </c>
       <c r="D101" t="n">
-        <v>11206558</v>
+        <v>11537874</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2069</v>
+        <v>2120</v>
       </c>
       <c r="D103" t="n">
-        <v>3045507</v>
+        <v>3122007</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2763</v>
+        <v>2828</v>
       </c>
       <c r="D105" t="n">
-        <v>4034212</v>
+        <v>4131362</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D107" t="n">
-        <v>162120</v>
+        <v>168120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D108" t="n">
-        <v>212265</v>
+        <v>221265</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>137537</v>
+        <v>138085</v>
       </c>
       <c r="D109" t="n">
-        <v>170164377</v>
+        <v>170829419</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="D113" t="n">
-        <v>1380382</v>
+        <v>1384882</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51756</v>
+        <v>51919</v>
       </c>
       <c r="D115" t="n">
-        <v>75887829</v>
+        <v>76122301</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26251</v>
+        <v>26334</v>
       </c>
       <c r="D117" t="n">
-        <v>38035618</v>
+        <v>38153062</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1271</v>
+        <v>1283</v>
       </c>
       <c r="D118" t="n">
-        <v>1738865</v>
+        <v>1755065</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2138</v>
+        <v>2154</v>
       </c>
       <c r="D121" t="n">
-        <v>3000581</v>
+        <v>3024553</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>480323</v>
+        <v>485191</v>
       </c>
       <c r="D123" t="n">
-        <v>633427410</v>
+        <v>639993867</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D125" t="n">
-        <v>297996</v>
+        <v>302496</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1342</v>
+        <v>1349</v>
       </c>
       <c r="D128" t="n">
-        <v>1989311</v>
+        <v>1999811</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>201359</v>
+        <v>202363</v>
       </c>
       <c r="D130" t="n">
-        <v>296073399</v>
+        <v>297524598</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D131" t="n">
-        <v>565290</v>
+        <v>571290</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>173419</v>
+        <v>174505</v>
       </c>
       <c r="D133" t="n">
-        <v>252106243</v>
+        <v>253662759</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2714</v>
+        <v>2752</v>
       </c>
       <c r="D136" t="n">
-        <v>3811489</v>
+        <v>3864704</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5945</v>
+        <v>6039</v>
       </c>
       <c r="D138" t="n">
-        <v>8397513</v>
+        <v>8530294</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>42936</v>
+        <v>43177</v>
       </c>
       <c r="D141" t="n">
-        <v>57378945</v>
+        <v>57671497</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>385</v>
+        <v>424</v>
       </c>
       <c r="D146" t="n">
-        <v>577165</v>
+        <v>635665</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13694</v>
+        <v>13751</v>
       </c>
       <c r="D147" t="n">
-        <v>20093699</v>
+        <v>20177428</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3639</v>
+        <v>3652</v>
       </c>
       <c r="D148" t="n">
-        <v>5249824</v>
+        <v>5268267</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D150" t="n">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D151" t="n">
-        <v>549702</v>
+        <v>550502</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="D153" t="n">
-        <v>498010</v>
+        <v>505510</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16764</v>
+        <v>16916</v>
       </c>
       <c r="D154" t="n">
-        <v>22163201</v>
+        <v>22356351</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D157" t="n">
-        <v>56906</v>
+        <v>77906</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6904</v>
+        <v>6936</v>
       </c>
       <c r="D158" t="n">
-        <v>10047146</v>
+        <v>10091531</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4768</v>
+        <v>4818</v>
       </c>
       <c r="D160" t="n">
-        <v>6868125</v>
+        <v>6938965</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D162" t="n">
-        <v>368559</v>
+        <v>370035</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D163" t="n">
-        <v>356933</v>
+        <v>360783</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14186</v>
+        <v>14355</v>
       </c>
       <c r="D165" t="n">
-        <v>20572820</v>
+        <v>20817296</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1678</v>
+        <v>1689</v>
       </c>
       <c r="D166" t="n">
-        <v>2495630</v>
+        <v>2512130</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D167" t="n">
-        <v>332302</v>
+        <v>335302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D169" t="n">
-        <v>59690</v>
+        <v>64190</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>85548</v>
+        <v>85921</v>
       </c>
       <c r="D171" t="n">
-        <v>107065121</v>
+        <v>107518453</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D173" t="n">
-        <v>123021</v>
+        <v>124454</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D176" t="n">
-        <v>932848</v>
+        <v>937348</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33256</v>
+        <v>33376</v>
       </c>
       <c r="D178" t="n">
-        <v>48782438</v>
+        <v>48953841</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12671</v>
+        <v>12734</v>
       </c>
       <c r="D180" t="n">
-        <v>18311606</v>
+        <v>18398319</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1206</v>
+        <v>1218</v>
       </c>
       <c r="D182" t="n">
-        <v>1687223</v>
+        <v>1704817</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1564</v>
+        <v>1577</v>
       </c>
       <c r="D184" t="n">
-        <v>2201709</v>
+        <v>2219199</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>231717</v>
+        <v>232828</v>
       </c>
       <c r="D186" t="n">
-        <v>288209196</v>
+        <v>289564744</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85065</v>
+        <v>85353</v>
       </c>
       <c r="D194" t="n">
-        <v>124718468</v>
+        <v>125129958</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32189</v>
+        <v>32332</v>
       </c>
       <c r="D197" t="n">
-        <v>46332744</v>
+        <v>46537322</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4931</v>
+        <v>4976</v>
       </c>
       <c r="D200" t="n">
-        <v>7026228</v>
+        <v>7091639</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4557</v>
+        <v>4616</v>
       </c>
       <c r="D203" t="n">
-        <v>6306114</v>
+        <v>6387299</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>255607</v>
+        <v>256921</v>
       </c>
       <c r="D206" t="n">
-        <v>316464521</v>
+        <v>318073487</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D207" t="n">
-        <v>166518</v>
+        <v>168018</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D213" t="n">
-        <v>878406</v>
+        <v>881406</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>93112</v>
+        <v>93514</v>
       </c>
       <c r="D215" t="n">
-        <v>136244812</v>
+        <v>136827854</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D216" t="n">
-        <v>125199</v>
+        <v>126699</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50006</v>
+        <v>50262</v>
       </c>
       <c r="D218" t="n">
-        <v>72291084</v>
+        <v>72650140</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4511</v>
+        <v>4550</v>
       </c>
       <c r="D221" t="n">
-        <v>6327023</v>
+        <v>6384586</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5362</v>
+        <v>5435</v>
       </c>
       <c r="D224" t="n">
-        <v>7414480</v>
+        <v>7517354</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>103453</v>
+        <v>103880</v>
       </c>
       <c r="D227" t="n">
-        <v>129570862</v>
+        <v>130097755</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D228" t="n">
-        <v>76136</v>
+        <v>77405</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48640</v>
+        <v>48792</v>
       </c>
       <c r="D234" t="n">
-        <v>71270549</v>
+        <v>71487994</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12040</v>
+        <v>12101</v>
       </c>
       <c r="D236" t="n">
-        <v>17310351</v>
+        <v>17396509</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1850</v>
+        <v>1869</v>
       </c>
       <c r="D238" t="n">
-        <v>2654159</v>
+        <v>2678609</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2389</v>
+        <v>2401</v>
       </c>
       <c r="D240" t="n">
-        <v>3337538</v>
+        <v>3353096</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>249895</v>
+        <v>251034</v>
       </c>
       <c r="D241" t="n">
-        <v>315735112</v>
+        <v>317146423</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D242" t="n">
-        <v>206936</v>
+        <v>207959</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D244" t="n">
-        <v>19500</v>
+        <v>21000</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>802</v>
+        <v>814</v>
       </c>
       <c r="D247" t="n">
-        <v>1178896</v>
+        <v>1195550</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>93825</v>
+        <v>94160</v>
       </c>
       <c r="D249" t="n">
-        <v>137509273</v>
+        <v>137986579</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63057</v>
+        <v>63402</v>
       </c>
       <c r="D252" t="n">
-        <v>91386696</v>
+        <v>91886018</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2344</v>
+        <v>2350</v>
       </c>
       <c r="D254" t="n">
-        <v>3308589</v>
+        <v>3317589</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4340</v>
+        <v>4387</v>
       </c>
       <c r="D257" t="n">
-        <v>6092591</v>
+        <v>6156842</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-02 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>312670</v>
+        <v>313578</v>
       </c>
       <c r="D2" t="n">
-        <v>398708282</v>
+        <v>399833937</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D8" t="n">
-        <v>1240607</v>
+        <v>1242107</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>115236</v>
+        <v>115429</v>
       </c>
       <c r="D10" t="n">
-        <v>168876720</v>
+        <v>169154743</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D11" t="n">
-        <v>208513</v>
+        <v>210013</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>57972</v>
+        <v>58148</v>
       </c>
       <c r="D12" t="n">
-        <v>83682410</v>
+        <v>83931016</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3901</v>
+        <v>3914</v>
       </c>
       <c r="D16" t="n">
-        <v>5541112</v>
+        <v>5556730</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6328</v>
+        <v>6371</v>
       </c>
       <c r="D20" t="n">
-        <v>8833021</v>
+        <v>8894832</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>75750</v>
+        <v>75931</v>
       </c>
       <c r="D22" t="n">
-        <v>94592520</v>
+        <v>94801227</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32025</v>
+        <v>32067</v>
       </c>
       <c r="D28" t="n">
-        <v>46887378</v>
+        <v>46947793</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D29" t="n">
-        <v>37404</v>
+        <v>40404</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11241</v>
+        <v>11284</v>
       </c>
       <c r="D30" t="n">
-        <v>16176617</v>
+        <v>16234369</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1538</v>
+        <v>1543</v>
       </c>
       <c r="D33" t="n">
-        <v>2160632</v>
+        <v>2165807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1732</v>
+        <v>1746</v>
       </c>
       <c r="D35" t="n">
-        <v>2442462</v>
+        <v>2462260</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95220</v>
+        <v>95435</v>
       </c>
       <c r="D36" t="n">
-        <v>120020647</v>
+        <v>120259140</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43840</v>
+        <v>43889</v>
       </c>
       <c r="D44" t="n">
-        <v>64265036</v>
+        <v>64335532</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8951</v>
+        <v>8971</v>
       </c>
       <c r="D46" t="n">
-        <v>12848358</v>
+        <v>12876443</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1378</v>
+        <v>1381</v>
       </c>
       <c r="D48" t="n">
-        <v>1913400</v>
+        <v>1917900</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2205</v>
+        <v>2221</v>
       </c>
       <c r="D51" t="n">
-        <v>3073244</v>
+        <v>3096346</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67506</v>
+        <v>67659</v>
       </c>
       <c r="D52" t="n">
-        <v>84750976</v>
+        <v>84930576</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D53" t="n">
-        <v>39883</v>
+        <v>41883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27715</v>
+        <v>27758</v>
       </c>
       <c r="D58" t="n">
-        <v>40647682</v>
+        <v>40712181</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10847</v>
+        <v>10876</v>
       </c>
       <c r="D61" t="n">
-        <v>15685809</v>
+        <v>15725187</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="D63" t="n">
-        <v>1869289</v>
+        <v>1872289</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1404</v>
+        <v>1410</v>
       </c>
       <c r="D67" t="n">
-        <v>1963318</v>
+        <v>1972268</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19980</v>
+        <v>20048</v>
       </c>
       <c r="D69" t="n">
-        <v>26168565</v>
+        <v>26259215</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7415</v>
+        <v>7437</v>
       </c>
       <c r="D73" t="n">
-        <v>10856094</v>
+        <v>10887361</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4973</v>
+        <v>4999</v>
       </c>
       <c r="D75" t="n">
-        <v>7219515</v>
+        <v>7257616</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="D76" t="n">
-        <v>663739</v>
+        <v>669739</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>137547</v>
+        <v>137836</v>
       </c>
       <c r="D78" t="n">
-        <v>171647175</v>
+        <v>172000132</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D79" t="n">
-        <v>77285</v>
+        <v>78785</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D83" t="n">
-        <v>17438</v>
+        <v>18938</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62603</v>
+        <v>62704</v>
       </c>
       <c r="D84" t="n">
-        <v>91763728</v>
+        <v>91909689</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D85" t="n">
-        <v>117082</v>
+        <v>118582</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29066</v>
+        <v>29143</v>
       </c>
       <c r="D87" t="n">
-        <v>42061809</v>
+        <v>42173732</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2659</v>
+        <v>2672</v>
       </c>
       <c r="D89" t="n">
-        <v>3827740</v>
+        <v>3847200</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2689</v>
+        <v>2702</v>
       </c>
       <c r="D90" t="n">
-        <v>3799740</v>
+        <v>3817857</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>31158</v>
+        <v>31414</v>
       </c>
       <c r="D91" t="n">
-        <v>42216821</v>
+        <v>42563441</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7675</v>
+        <v>7717</v>
       </c>
       <c r="D95" t="n">
-        <v>11288846</v>
+        <v>11349394</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6917</v>
+        <v>6973</v>
       </c>
       <c r="D97" t="n">
-        <v>10027028</v>
+        <v>10106870</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="D99" t="n">
-        <v>721885</v>
+        <v>725575</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="D100" t="n">
-        <v>662524</v>
+        <v>683524</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8310</v>
+        <v>8386</v>
       </c>
       <c r="D101" t="n">
-        <v>11537874</v>
+        <v>11644525</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2120</v>
+        <v>2134</v>
       </c>
       <c r="D103" t="n">
-        <v>3122007</v>
+        <v>3142970</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2828</v>
+        <v>2870</v>
       </c>
       <c r="D105" t="n">
-        <v>4131362</v>
+        <v>4192919</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D108" t="n">
-        <v>221265</v>
+        <v>224265</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>138085</v>
+        <v>138376</v>
       </c>
       <c r="D109" t="n">
-        <v>170829419</v>
+        <v>171171340</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="D113" t="n">
-        <v>1384882</v>
+        <v>1387882</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>51919</v>
+        <v>52017</v>
       </c>
       <c r="D115" t="n">
-        <v>76122301</v>
+        <v>76266008</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26334</v>
+        <v>26401</v>
       </c>
       <c r="D117" t="n">
-        <v>38153062</v>
+        <v>38248391</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D118" t="n">
-        <v>1755065</v>
+        <v>1756565</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2154</v>
+        <v>2164</v>
       </c>
       <c r="D121" t="n">
-        <v>3024553</v>
+        <v>3037718</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>485191</v>
+        <v>487513</v>
       </c>
       <c r="D123" t="n">
-        <v>639993867</v>
+        <v>643030498</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D125" t="n">
-        <v>302496</v>
+        <v>303996</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D128" t="n">
-        <v>1999811</v>
+        <v>2001311</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>202363</v>
+        <v>203040</v>
       </c>
       <c r="D130" t="n">
-        <v>297524598</v>
+        <v>298497854</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>174505</v>
+        <v>175152</v>
       </c>
       <c r="D133" t="n">
-        <v>253662759</v>
+        <v>254595034</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2752</v>
+        <v>2767</v>
       </c>
       <c r="D136" t="n">
-        <v>3864704</v>
+        <v>3887204</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6039</v>
+        <v>6077</v>
       </c>
       <c r="D138" t="n">
-        <v>8530294</v>
+        <v>8583244</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>43177</v>
+        <v>43323</v>
       </c>
       <c r="D141" t="n">
-        <v>57671497</v>
+        <v>57861480</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>424</v>
+        <v>451</v>
       </c>
       <c r="D146" t="n">
-        <v>635665</v>
+        <v>676165</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13751</v>
+        <v>13780</v>
       </c>
       <c r="D147" t="n">
-        <v>20177428</v>
+        <v>20219830</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3652</v>
+        <v>3659</v>
       </c>
       <c r="D148" t="n">
-        <v>5268267</v>
+        <v>5278299</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D153" t="n">
-        <v>505510</v>
+        <v>511251</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>16916</v>
+        <v>17025</v>
       </c>
       <c r="D154" t="n">
-        <v>22356351</v>
+        <v>22500403</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6936</v>
+        <v>6969</v>
       </c>
       <c r="D158" t="n">
-        <v>10091531</v>
+        <v>10137638</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4818</v>
+        <v>4861</v>
       </c>
       <c r="D160" t="n">
-        <v>6938965</v>
+        <v>6995956</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D163" t="n">
-        <v>360783</v>
+        <v>366783</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14355</v>
+        <v>14409</v>
       </c>
       <c r="D165" t="n">
-        <v>20817296</v>
+        <v>20895860</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1689</v>
+        <v>1696</v>
       </c>
       <c r="D166" t="n">
-        <v>2512130</v>
+        <v>2522630</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D167" t="n">
-        <v>335302</v>
+        <v>339802</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D169" t="n">
-        <v>64190</v>
+        <v>70190</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>85921</v>
+        <v>86078</v>
       </c>
       <c r="D171" t="n">
-        <v>107518453</v>
+        <v>107709855</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33376</v>
+        <v>33421</v>
       </c>
       <c r="D178" t="n">
-        <v>48953841</v>
+        <v>49015645</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12734</v>
+        <v>12759</v>
       </c>
       <c r="D180" t="n">
-        <v>18398319</v>
+        <v>18433490</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1218</v>
+        <v>1226</v>
       </c>
       <c r="D182" t="n">
-        <v>1704817</v>
+        <v>1715196</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1577</v>
+        <v>1586</v>
       </c>
       <c r="D184" t="n">
-        <v>2219199</v>
+        <v>2232193</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>232828</v>
+        <v>233363</v>
       </c>
       <c r="D186" t="n">
-        <v>289564744</v>
+        <v>290195988</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D192" t="n">
-        <v>1266497</v>
+        <v>1267997</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85353</v>
+        <v>85482</v>
       </c>
       <c r="D194" t="n">
-        <v>125129958</v>
+        <v>125316381</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32332</v>
+        <v>32401</v>
       </c>
       <c r="D197" t="n">
-        <v>46537322</v>
+        <v>46632577</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4976</v>
+        <v>5000</v>
       </c>
       <c r="D200" t="n">
-        <v>7091639</v>
+        <v>7126548</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4616</v>
+        <v>4642</v>
       </c>
       <c r="D203" t="n">
-        <v>6387299</v>
+        <v>6421939</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>256921</v>
+        <v>257588</v>
       </c>
       <c r="D206" t="n">
-        <v>318073487</v>
+        <v>318882992</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D207" t="n">
-        <v>168018</v>
+        <v>168908</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D208" t="n">
-        <v>350564</v>
+        <v>352064</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>93514</v>
+        <v>93672</v>
       </c>
       <c r="D215" t="n">
-        <v>136827854</v>
+        <v>137054826</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50262</v>
+        <v>50381</v>
       </c>
       <c r="D218" t="n">
-        <v>72650140</v>
+        <v>72823112</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4550</v>
+        <v>4559</v>
       </c>
       <c r="D221" t="n">
-        <v>6384586</v>
+        <v>6397936</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5435</v>
+        <v>5475</v>
       </c>
       <c r="D224" t="n">
-        <v>7517354</v>
+        <v>7569668</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D225" t="n">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>103880</v>
+        <v>104149</v>
       </c>
       <c r="D227" t="n">
-        <v>130097755</v>
+        <v>130416965</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48792</v>
+        <v>48856</v>
       </c>
       <c r="D234" t="n">
-        <v>71487994</v>
+        <v>71582744</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D235" t="n">
-        <v>45711</v>
+        <v>47211</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12101</v>
+        <v>12131</v>
       </c>
       <c r="D236" t="n">
-        <v>17396509</v>
+        <v>17439437</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2401</v>
+        <v>2411</v>
       </c>
       <c r="D240" t="n">
-        <v>3353096</v>
+        <v>3368096</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>251034</v>
+        <v>251757</v>
       </c>
       <c r="D241" t="n">
-        <v>317146423</v>
+        <v>318026697</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c r="D247" t="n">
-        <v>1195550</v>
+        <v>1201550</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>94160</v>
+        <v>94329</v>
       </c>
       <c r="D249" t="n">
-        <v>137986579</v>
+        <v>138230379</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63402</v>
+        <v>63557</v>
       </c>
       <c r="D252" t="n">
-        <v>91886018</v>
+        <v>92108388</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2350</v>
+        <v>2357</v>
       </c>
       <c r="D254" t="n">
-        <v>3317589</v>
+        <v>3327089</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4387</v>
+        <v>4410</v>
       </c>
       <c r="D257" t="n">
-        <v>6156842</v>
+        <v>6190882</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-03 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>313578</v>
+        <v>314078</v>
       </c>
       <c r="D2" t="n">
-        <v>399833937</v>
+        <v>400449863</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D4" t="n">
-        <v>444918</v>
+        <v>446418</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D8" t="n">
-        <v>1242107</v>
+        <v>1243607</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>115429</v>
+        <v>115579</v>
       </c>
       <c r="D10" t="n">
-        <v>169154743</v>
+        <v>169373365</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58148</v>
+        <v>58255</v>
       </c>
       <c r="D12" t="n">
-        <v>83931016</v>
+        <v>84083724</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3914</v>
+        <v>3924</v>
       </c>
       <c r="D16" t="n">
-        <v>5556730</v>
+        <v>5570261</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6371</v>
+        <v>6397</v>
       </c>
       <c r="D20" t="n">
-        <v>8894832</v>
+        <v>8928807</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>75931</v>
+        <v>76031</v>
       </c>
       <c r="D22" t="n">
-        <v>94801227</v>
+        <v>94920236</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32067</v>
+        <v>32096</v>
       </c>
       <c r="D28" t="n">
-        <v>46947793</v>
+        <v>46990193</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11284</v>
+        <v>11298</v>
       </c>
       <c r="D30" t="n">
-        <v>16234369</v>
+        <v>16253953</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D33" t="n">
-        <v>2165807</v>
+        <v>2167307</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1746</v>
+        <v>1750</v>
       </c>
       <c r="D35" t="n">
-        <v>2462260</v>
+        <v>2468260</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95435</v>
+        <v>95569</v>
       </c>
       <c r="D36" t="n">
-        <v>120259140</v>
+        <v>120414056</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D38" t="n">
-        <v>113508</v>
+        <v>115008</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43889</v>
+        <v>43939</v>
       </c>
       <c r="D44" t="n">
-        <v>64335532</v>
+        <v>64406727</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8971</v>
+        <v>8987</v>
       </c>
       <c r="D46" t="n">
-        <v>12876443</v>
+        <v>12899920</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D48" t="n">
-        <v>1917900</v>
+        <v>1919400</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2221</v>
+        <v>2225</v>
       </c>
       <c r="D51" t="n">
-        <v>3096346</v>
+        <v>3102064</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67659</v>
+        <v>67752</v>
       </c>
       <c r="D52" t="n">
-        <v>84930576</v>
+        <v>85050831</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27758</v>
+        <v>27789</v>
       </c>
       <c r="D58" t="n">
-        <v>40712181</v>
+        <v>40757814</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10876</v>
+        <v>10891</v>
       </c>
       <c r="D61" t="n">
-        <v>15725187</v>
+        <v>15746434</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D63" t="n">
-        <v>1872289</v>
+        <v>1873789</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1410</v>
+        <v>1415</v>
       </c>
       <c r="D67" t="n">
-        <v>1972268</v>
+        <v>1979768</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>20048</v>
+        <v>20093</v>
       </c>
       <c r="D69" t="n">
-        <v>26259215</v>
+        <v>26320731</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D71" t="n">
-        <v>34725</v>
+        <v>36225</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7437</v>
+        <v>7458</v>
       </c>
       <c r="D73" t="n">
-        <v>10887361</v>
+        <v>10918861</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4999</v>
+        <v>5007</v>
       </c>
       <c r="D75" t="n">
-        <v>7257616</v>
+        <v>7269616</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>137836</v>
+        <v>138041</v>
       </c>
       <c r="D78" t="n">
-        <v>172000132</v>
+        <v>172238482</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D82" t="n">
-        <v>616416</v>
+        <v>619271</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62704</v>
+        <v>62780</v>
       </c>
       <c r="D84" t="n">
-        <v>91909689</v>
+        <v>92020516</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29143</v>
+        <v>29185</v>
       </c>
       <c r="D87" t="n">
-        <v>42173732</v>
+        <v>42230152</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2672</v>
+        <v>2684</v>
       </c>
       <c r="D89" t="n">
-        <v>3847200</v>
+        <v>3865020</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2702</v>
+        <v>2714</v>
       </c>
       <c r="D90" t="n">
-        <v>3817857</v>
+        <v>3834205</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>31414</v>
+        <v>31494</v>
       </c>
       <c r="D91" t="n">
-        <v>42563441</v>
+        <v>42669798</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7717</v>
+        <v>7725</v>
       </c>
       <c r="D95" t="n">
-        <v>11349394</v>
+        <v>11360101</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6973</v>
+        <v>7000</v>
       </c>
       <c r="D97" t="n">
-        <v>10106870</v>
+        <v>10146480</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8386</v>
+        <v>8439</v>
       </c>
       <c r="D101" t="n">
-        <v>11644525</v>
+        <v>11717672</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2134</v>
+        <v>2139</v>
       </c>
       <c r="D103" t="n">
-        <v>3142970</v>
+        <v>3150470</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2870</v>
+        <v>2882</v>
       </c>
       <c r="D105" t="n">
-        <v>4192919</v>
+        <v>4210919</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>138376</v>
+        <v>138608</v>
       </c>
       <c r="D109" t="n">
-        <v>171171340</v>
+        <v>171456720</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>52017</v>
+        <v>52065</v>
       </c>
       <c r="D115" t="n">
-        <v>76266008</v>
+        <v>76336116</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26401</v>
+        <v>26443</v>
       </c>
       <c r="D117" t="n">
-        <v>38248391</v>
+        <v>38310315</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1284</v>
+        <v>1288</v>
       </c>
       <c r="D118" t="n">
-        <v>1756565</v>
+        <v>1762565</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2164</v>
+        <v>2172</v>
       </c>
       <c r="D121" t="n">
-        <v>3037718</v>
+        <v>3049718</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>487513</v>
+        <v>488640</v>
       </c>
       <c r="D123" t="n">
-        <v>643030498</v>
+        <v>644473878</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D125" t="n">
-        <v>303996</v>
+        <v>305496</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1350</v>
+        <v>1353</v>
       </c>
       <c r="D128" t="n">
-        <v>2001311</v>
+        <v>2005811</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>203040</v>
+        <v>203418</v>
       </c>
       <c r="D130" t="n">
-        <v>298497854</v>
+        <v>299044164</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D131" t="n">
-        <v>571290</v>
+        <v>574290</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>175152</v>
+        <v>175532</v>
       </c>
       <c r="D133" t="n">
-        <v>254595034</v>
+        <v>255141397</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2767</v>
+        <v>2779</v>
       </c>
       <c r="D136" t="n">
-        <v>3887204</v>
+        <v>3904832</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6077</v>
+        <v>6104</v>
       </c>
       <c r="D138" t="n">
-        <v>8583244</v>
+        <v>8622701</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>43323</v>
+        <v>43450</v>
       </c>
       <c r="D141" t="n">
-        <v>57861480</v>
+        <v>58024573</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13780</v>
+        <v>13804</v>
       </c>
       <c r="D147" t="n">
-        <v>20219830</v>
+        <v>20255424</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3659</v>
+        <v>3672</v>
       </c>
       <c r="D148" t="n">
-        <v>5278299</v>
+        <v>5296465</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D151" t="n">
-        <v>550502</v>
+        <v>553431</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D153" t="n">
-        <v>511251</v>
+        <v>515751</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>17025</v>
+        <v>17061</v>
       </c>
       <c r="D154" t="n">
-        <v>22500403</v>
+        <v>22549202</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6969</v>
+        <v>6977</v>
       </c>
       <c r="D158" t="n">
-        <v>10137638</v>
+        <v>10149416</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4861</v>
+        <v>4866</v>
       </c>
       <c r="D160" t="n">
-        <v>6995956</v>
+        <v>7003456</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D163" t="n">
-        <v>366783</v>
+        <v>368283</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14409</v>
+        <v>14457</v>
       </c>
       <c r="D165" t="n">
-        <v>20895860</v>
+        <v>20964860</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1696</v>
+        <v>1702</v>
       </c>
       <c r="D166" t="n">
-        <v>2522630</v>
+        <v>2531630</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D167" t="n">
-        <v>339802</v>
+        <v>341302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>86078</v>
+        <v>86175</v>
       </c>
       <c r="D171" t="n">
-        <v>107709855</v>
+        <v>107828686</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D176" t="n">
-        <v>937348</v>
+        <v>938848</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33421</v>
+        <v>33451</v>
       </c>
       <c r="D178" t="n">
-        <v>49015645</v>
+        <v>49058394</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12759</v>
+        <v>12777</v>
       </c>
       <c r="D180" t="n">
-        <v>18433490</v>
+        <v>18460490</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D182" t="n">
-        <v>1715196</v>
+        <v>1716696</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1586</v>
+        <v>1589</v>
       </c>
       <c r="D184" t="n">
-        <v>2232193</v>
+        <v>2236693</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>233363</v>
+        <v>233736</v>
       </c>
       <c r="D186" t="n">
-        <v>290195988</v>
+        <v>290645864</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D188" t="n">
-        <v>234736</v>
+        <v>236236</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="D192" t="n">
-        <v>1267997</v>
+        <v>1270997</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85482</v>
+        <v>85577</v>
       </c>
       <c r="D194" t="n">
-        <v>125316381</v>
+        <v>125455104</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32401</v>
+        <v>32460</v>
       </c>
       <c r="D197" t="n">
-        <v>46632577</v>
+        <v>46718166</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5000</v>
+        <v>5010</v>
       </c>
       <c r="D200" t="n">
-        <v>7126548</v>
+        <v>7141248</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4642</v>
+        <v>4665</v>
       </c>
       <c r="D203" t="n">
-        <v>6421939</v>
+        <v>6452607</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>257588</v>
+        <v>258132</v>
       </c>
       <c r="D206" t="n">
-        <v>318882992</v>
+        <v>319543320</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D207" t="n">
-        <v>168908</v>
+        <v>169473</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D213" t="n">
-        <v>881406</v>
+        <v>882906</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>93672</v>
+        <v>93817</v>
       </c>
       <c r="D215" t="n">
-        <v>137054826</v>
+        <v>137262984</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50381</v>
+        <v>50470</v>
       </c>
       <c r="D218" t="n">
-        <v>72823112</v>
+        <v>72947143</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4559</v>
+        <v>4578</v>
       </c>
       <c r="D221" t="n">
-        <v>6397936</v>
+        <v>6424215</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5475</v>
+        <v>5503</v>
       </c>
       <c r="D224" t="n">
-        <v>7569668</v>
+        <v>7607738</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>104149</v>
+        <v>104292</v>
       </c>
       <c r="D227" t="n">
-        <v>130416965</v>
+        <v>130582634</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48856</v>
+        <v>48904</v>
       </c>
       <c r="D234" t="n">
-        <v>71582744</v>
+        <v>71652542</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12131</v>
+        <v>12156</v>
       </c>
       <c r="D236" t="n">
-        <v>17439437</v>
+        <v>17475692</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1869</v>
+        <v>1872</v>
       </c>
       <c r="D238" t="n">
-        <v>2678609</v>
+        <v>2683109</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2411</v>
+        <v>2416</v>
       </c>
       <c r="D240" t="n">
-        <v>3368096</v>
+        <v>3375596</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>251757</v>
+        <v>252184</v>
       </c>
       <c r="D241" t="n">
-        <v>318026697</v>
+        <v>318555526</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D242" t="n">
-        <v>207959</v>
+        <v>209459</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D243" t="n">
-        <v>348957</v>
+        <v>351957</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>94329</v>
+        <v>94443</v>
       </c>
       <c r="D249" t="n">
-        <v>138230379</v>
+        <v>138398849</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D250" t="n">
-        <v>111161</v>
+        <v>112661</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63557</v>
+        <v>63676</v>
       </c>
       <c r="D252" t="n">
-        <v>92108388</v>
+        <v>92279279</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2357</v>
+        <v>2361</v>
       </c>
       <c r="D254" t="n">
-        <v>3327089</v>
+        <v>3332247</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4410</v>
+        <v>4442</v>
       </c>
       <c r="D257" t="n">
-        <v>6190882</v>
+        <v>6234180</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-04 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>314078</v>
+        <v>314738</v>
       </c>
       <c r="D2" t="n">
-        <v>400449863</v>
+        <v>401280715</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D4" t="n">
-        <v>446418</v>
+        <v>447707</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>10500</v>
+        <v>11676</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D8" t="n">
-        <v>1243607</v>
+        <v>1245107</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>115579</v>
+        <v>115723</v>
       </c>
       <c r="D10" t="n">
-        <v>169373365</v>
+        <v>169581339</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58255</v>
+        <v>58345</v>
       </c>
       <c r="D12" t="n">
-        <v>84083724</v>
+        <v>84213662</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" t="n">
-        <v>64543</v>
+        <v>66043</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3924</v>
+        <v>3939</v>
       </c>
       <c r="D16" t="n">
-        <v>5570261</v>
+        <v>5592761</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6397</v>
+        <v>6414</v>
       </c>
       <c r="D20" t="n">
-        <v>8928807</v>
+        <v>8951081</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>76031</v>
+        <v>76141</v>
       </c>
       <c r="D22" t="n">
-        <v>94920236</v>
+        <v>95044030</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32096</v>
+        <v>32127</v>
       </c>
       <c r="D28" t="n">
-        <v>46990193</v>
+        <v>47036600</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11298</v>
+        <v>11315</v>
       </c>
       <c r="D30" t="n">
-        <v>16253953</v>
+        <v>16277294</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D33" t="n">
-        <v>2167307</v>
+        <v>2168807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1750</v>
+        <v>1763</v>
       </c>
       <c r="D35" t="n">
-        <v>2468260</v>
+        <v>2487523</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95569</v>
+        <v>95685</v>
       </c>
       <c r="D36" t="n">
-        <v>120414056</v>
+        <v>120561110</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D42" t="n">
-        <v>1318685</v>
+        <v>1320185</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43939</v>
+        <v>43970</v>
       </c>
       <c r="D44" t="n">
-        <v>64406727</v>
+        <v>64451538</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D45" t="n">
-        <v>35950</v>
+        <v>37450</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8987</v>
+        <v>8997</v>
       </c>
       <c r="D46" t="n">
-        <v>12899920</v>
+        <v>12914224</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D48" t="n">
-        <v>1919400</v>
+        <v>1920900</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2225</v>
+        <v>2233</v>
       </c>
       <c r="D51" t="n">
-        <v>3102064</v>
+        <v>3114064</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67752</v>
+        <v>67884</v>
       </c>
       <c r="D52" t="n">
-        <v>85050831</v>
+        <v>85214566</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27789</v>
+        <v>27826</v>
       </c>
       <c r="D58" t="n">
-        <v>40757814</v>
+        <v>40811711</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10891</v>
+        <v>10917</v>
       </c>
       <c r="D61" t="n">
-        <v>15746434</v>
+        <v>15784890</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1415</v>
+        <v>1420</v>
       </c>
       <c r="D67" t="n">
-        <v>1979768</v>
+        <v>1987268</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>20093</v>
+        <v>20144</v>
       </c>
       <c r="D69" t="n">
-        <v>26320731</v>
+        <v>26385968</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7458</v>
+        <v>7467</v>
       </c>
       <c r="D73" t="n">
-        <v>10918861</v>
+        <v>10932361</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5007</v>
+        <v>5023</v>
       </c>
       <c r="D75" t="n">
-        <v>7269616</v>
+        <v>7292706</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="D76" t="n">
-        <v>669739</v>
+        <v>675739</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>138041</v>
+        <v>138296</v>
       </c>
       <c r="D78" t="n">
-        <v>172238482</v>
+        <v>172530287</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62780</v>
+        <v>62830</v>
       </c>
       <c r="D84" t="n">
-        <v>92020516</v>
+        <v>92094575</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29185</v>
+        <v>29235</v>
       </c>
       <c r="D87" t="n">
-        <v>42230152</v>
+        <v>42298498</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2684</v>
+        <v>2689</v>
       </c>
       <c r="D89" t="n">
-        <v>3865020</v>
+        <v>3872520</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2714</v>
+        <v>2723</v>
       </c>
       <c r="D90" t="n">
-        <v>3834205</v>
+        <v>3847605</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>31494</v>
+        <v>31684</v>
       </c>
       <c r="D91" t="n">
-        <v>42669798</v>
+        <v>42935818</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7725</v>
+        <v>7732</v>
       </c>
       <c r="D95" t="n">
-        <v>11360101</v>
+        <v>11369567</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7000</v>
+        <v>7027</v>
       </c>
       <c r="D97" t="n">
-        <v>10146480</v>
+        <v>10186733</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D99" t="n">
-        <v>725575</v>
+        <v>728005</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="D100" t="n">
-        <v>683524</v>
+        <v>688443</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8439</v>
+        <v>8565</v>
       </c>
       <c r="D101" t="n">
-        <v>11717672</v>
+        <v>11884856</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2139</v>
+        <v>2155</v>
       </c>
       <c r="D103" t="n">
-        <v>3150470</v>
+        <v>3174470</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2882</v>
+        <v>2905</v>
       </c>
       <c r="D105" t="n">
-        <v>4210919</v>
+        <v>4241402</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D107" t="n">
-        <v>168120</v>
+        <v>171120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D108" t="n">
-        <v>224265</v>
+        <v>224586</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>138608</v>
+        <v>138837</v>
       </c>
       <c r="D109" t="n">
-        <v>171456720</v>
+        <v>171727843</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>52065</v>
+        <v>52110</v>
       </c>
       <c r="D115" t="n">
-        <v>76336116</v>
+        <v>76395826</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D116" t="n">
-        <v>124459</v>
+        <v>125959</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26443</v>
+        <v>26491</v>
       </c>
       <c r="D117" t="n">
-        <v>38310315</v>
+        <v>38379200</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1288</v>
+        <v>1294</v>
       </c>
       <c r="D118" t="n">
-        <v>1762565</v>
+        <v>1770551</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2172</v>
+        <v>2175</v>
       </c>
       <c r="D121" t="n">
-        <v>3049718</v>
+        <v>3054218</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>488640</v>
+        <v>490570</v>
       </c>
       <c r="D123" t="n">
-        <v>644473878</v>
+        <v>647008988</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D125" t="n">
-        <v>305496</v>
+        <v>306736</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="D128" t="n">
-        <v>2005811</v>
+        <v>2008811</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>203418</v>
+        <v>203791</v>
       </c>
       <c r="D130" t="n">
-        <v>299044164</v>
+        <v>299590510</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D131" t="n">
-        <v>574290</v>
+        <v>575790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>175532</v>
+        <v>175987</v>
       </c>
       <c r="D133" t="n">
-        <v>255141397</v>
+        <v>255802165</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2779</v>
+        <v>2793</v>
       </c>
       <c r="D136" t="n">
-        <v>3904832</v>
+        <v>3925444</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6104</v>
+        <v>6121</v>
       </c>
       <c r="D138" t="n">
-        <v>8622701</v>
+        <v>8647603</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>43450</v>
+        <v>43553</v>
       </c>
       <c r="D141" t="n">
-        <v>58024573</v>
+        <v>58160226</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13804</v>
+        <v>13836</v>
       </c>
       <c r="D147" t="n">
-        <v>20255424</v>
+        <v>20294557</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3672</v>
+        <v>3685</v>
       </c>
       <c r="D148" t="n">
-        <v>5296465</v>
+        <v>5315965</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D151" t="n">
-        <v>553431</v>
+        <v>559431</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>17061</v>
+        <v>17125</v>
       </c>
       <c r="D154" t="n">
-        <v>22549202</v>
+        <v>22633593</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6977</v>
+        <v>7001</v>
       </c>
       <c r="D158" t="n">
-        <v>10149416</v>
+        <v>10185416</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4866</v>
+        <v>4874</v>
       </c>
       <c r="D160" t="n">
-        <v>7003456</v>
+        <v>7015456</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D163" t="n">
-        <v>368283</v>
+        <v>369783</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14457</v>
+        <v>14796</v>
       </c>
       <c r="D165" t="n">
-        <v>20964860</v>
+        <v>21463720</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1702</v>
+        <v>1716</v>
       </c>
       <c r="D166" t="n">
-        <v>2531630</v>
+        <v>2552630</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D167" t="n">
-        <v>341302</v>
+        <v>342802</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D169" t="n">
-        <v>70190</v>
+        <v>71690</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>86175</v>
+        <v>86300</v>
       </c>
       <c r="D171" t="n">
-        <v>107828686</v>
+        <v>107985744</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D176" t="n">
-        <v>938848</v>
+        <v>940348</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33451</v>
+        <v>33473</v>
       </c>
       <c r="D178" t="n">
-        <v>49058394</v>
+        <v>49091394</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12777</v>
+        <v>12789</v>
       </c>
       <c r="D180" t="n">
-        <v>18460490</v>
+        <v>18478490</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1227</v>
+        <v>1231</v>
       </c>
       <c r="D182" t="n">
-        <v>1716696</v>
+        <v>1722396</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1589</v>
+        <v>1594</v>
       </c>
       <c r="D184" t="n">
-        <v>2236693</v>
+        <v>2244193</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>233736</v>
+        <v>234202</v>
       </c>
       <c r="D186" t="n">
-        <v>290645864</v>
+        <v>291214392</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85577</v>
+        <v>85668</v>
       </c>
       <c r="D194" t="n">
-        <v>125455104</v>
+        <v>125590329</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32460</v>
+        <v>32501</v>
       </c>
       <c r="D197" t="n">
-        <v>46718166</v>
+        <v>46776170</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5010</v>
+        <v>5022</v>
       </c>
       <c r="D200" t="n">
-        <v>7141248</v>
+        <v>7156762</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4665</v>
+        <v>4691</v>
       </c>
       <c r="D203" t="n">
-        <v>6452607</v>
+        <v>6487816</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>258132</v>
+        <v>258820</v>
       </c>
       <c r="D206" t="n">
-        <v>319543320</v>
+        <v>320397886</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D208" t="n">
-        <v>352064</v>
+        <v>353087</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>93817</v>
+        <v>93974</v>
       </c>
       <c r="D215" t="n">
-        <v>137262984</v>
+        <v>137494162</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50470</v>
+        <v>50574</v>
       </c>
       <c r="D218" t="n">
-        <v>72947143</v>
+        <v>73092217</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4578</v>
+        <v>4597</v>
       </c>
       <c r="D221" t="n">
-        <v>6424215</v>
+        <v>6452415</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5503</v>
+        <v>5525</v>
       </c>
       <c r="D224" t="n">
-        <v>7607738</v>
+        <v>7639436</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>104292</v>
+        <v>104441</v>
       </c>
       <c r="D227" t="n">
-        <v>130582634</v>
+        <v>130749202</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D232" t="n">
-        <v>819339</v>
+        <v>819439</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48904</v>
+        <v>48959</v>
       </c>
       <c r="D234" t="n">
-        <v>71652542</v>
+        <v>71731859</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12156</v>
+        <v>12173</v>
       </c>
       <c r="D236" t="n">
-        <v>17475692</v>
+        <v>17500151</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1872</v>
+        <v>1875</v>
       </c>
       <c r="D238" t="n">
-        <v>2683109</v>
+        <v>2687338</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2416</v>
+        <v>2421</v>
       </c>
       <c r="D240" t="n">
-        <v>3375596</v>
+        <v>3382219</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>252184</v>
+        <v>252635</v>
       </c>
       <c r="D241" t="n">
-        <v>318555526</v>
+        <v>319104043</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D244" t="n">
-        <v>21000</v>
+        <v>22500</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="D247" t="n">
-        <v>1201550</v>
+        <v>1203050</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>94443</v>
+        <v>94559</v>
       </c>
       <c r="D249" t="n">
-        <v>138398849</v>
+        <v>138570298</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63676</v>
+        <v>63786</v>
       </c>
       <c r="D252" t="n">
-        <v>92279279</v>
+        <v>92438746</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2361</v>
+        <v>2369</v>
       </c>
       <c r="D254" t="n">
-        <v>3332247</v>
+        <v>3343918</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4442</v>
+        <v>4453</v>
       </c>
       <c r="D257" t="n">
-        <v>6234180</v>
+        <v>6250224</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-05 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>314738</v>
+        <v>315122</v>
       </c>
       <c r="D2" t="n">
-        <v>401280715</v>
+        <v>401744408</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D4" t="n">
-        <v>447707</v>
+        <v>449207</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>11676</v>
+        <v>14676</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="D8" t="n">
-        <v>1245107</v>
+        <v>1245908</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>115723</v>
+        <v>115809</v>
       </c>
       <c r="D10" t="n">
-        <v>169581339</v>
+        <v>169704179</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58345</v>
+        <v>58409</v>
       </c>
       <c r="D12" t="n">
-        <v>84213662</v>
+        <v>84305345</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3939</v>
+        <v>3949</v>
       </c>
       <c r="D16" t="n">
-        <v>5592761</v>
+        <v>5605861</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6414</v>
+        <v>6433</v>
       </c>
       <c r="D20" t="n">
-        <v>8951081</v>
+        <v>8977335</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>76141</v>
+        <v>76223</v>
       </c>
       <c r="D22" t="n">
-        <v>95044030</v>
+        <v>95141217</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32127</v>
+        <v>32149</v>
       </c>
       <c r="D28" t="n">
-        <v>47036600</v>
+        <v>47069041</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11315</v>
+        <v>11329</v>
       </c>
       <c r="D30" t="n">
-        <v>16277294</v>
+        <v>16295486</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1545</v>
+        <v>1547</v>
       </c>
       <c r="D33" t="n">
-        <v>2168807</v>
+        <v>2171807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1763</v>
+        <v>1766</v>
       </c>
       <c r="D35" t="n">
-        <v>2487523</v>
+        <v>2492023</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95685</v>
+        <v>95788</v>
       </c>
       <c r="D36" t="n">
-        <v>120561110</v>
+        <v>120673422</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43970</v>
+        <v>44000</v>
       </c>
       <c r="D44" t="n">
-        <v>64451538</v>
+        <v>64490087</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8997</v>
+        <v>9003</v>
       </c>
       <c r="D46" t="n">
-        <v>12914224</v>
+        <v>12923224</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1383</v>
+        <v>1386</v>
       </c>
       <c r="D48" t="n">
-        <v>1920900</v>
+        <v>1925100</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2233</v>
+        <v>2241</v>
       </c>
       <c r="D51" t="n">
-        <v>3114064</v>
+        <v>3125564</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67884</v>
+        <v>67967</v>
       </c>
       <c r="D52" t="n">
-        <v>85214566</v>
+        <v>85310896</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27826</v>
+        <v>27852</v>
       </c>
       <c r="D58" t="n">
-        <v>40811711</v>
+        <v>40850210</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10917</v>
+        <v>10923</v>
       </c>
       <c r="D61" t="n">
-        <v>15784890</v>
+        <v>15793057</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1341</v>
+        <v>1343</v>
       </c>
       <c r="D63" t="n">
-        <v>1873789</v>
+        <v>1876789</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1420</v>
+        <v>1426</v>
       </c>
       <c r="D67" t="n">
-        <v>1987268</v>
+        <v>1995599</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>20144</v>
+        <v>20173</v>
       </c>
       <c r="D69" t="n">
-        <v>26385968</v>
+        <v>26423774</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7467</v>
+        <v>7486</v>
       </c>
       <c r="D73" t="n">
-        <v>10932361</v>
+        <v>10959496</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5023</v>
+        <v>5029</v>
       </c>
       <c r="D75" t="n">
-        <v>7292706</v>
+        <v>7301706</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="D76" t="n">
-        <v>675739</v>
+        <v>683239</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>138296</v>
+        <v>138462</v>
       </c>
       <c r="D78" t="n">
-        <v>172530287</v>
+        <v>172733006</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D79" t="n">
-        <v>78785</v>
+        <v>80285</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62830</v>
+        <v>62874</v>
       </c>
       <c r="D84" t="n">
-        <v>92094575</v>
+        <v>92157458</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86" t="n">
-        <v>13500</v>
+        <v>15000</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29235</v>
+        <v>29270</v>
       </c>
       <c r="D87" t="n">
-        <v>42298498</v>
+        <v>42346144</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2689</v>
+        <v>2699</v>
       </c>
       <c r="D89" t="n">
-        <v>3872520</v>
+        <v>3886643</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2723</v>
+        <v>2734</v>
       </c>
       <c r="D90" t="n">
-        <v>3847605</v>
+        <v>3862665</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>31684</v>
+        <v>31773</v>
       </c>
       <c r="D91" t="n">
-        <v>42935818</v>
+        <v>43055768</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7732</v>
+        <v>7746</v>
       </c>
       <c r="D95" t="n">
-        <v>11369567</v>
+        <v>11388970</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7027</v>
+        <v>7039</v>
       </c>
       <c r="D97" t="n">
-        <v>10186733</v>
+        <v>10204733</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="D99" t="n">
-        <v>728005</v>
+        <v>730405</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="D100" t="n">
-        <v>688443</v>
+        <v>692443</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8565</v>
+        <v>8618</v>
       </c>
       <c r="D101" t="n">
-        <v>11884856</v>
+        <v>11954383</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2155</v>
+        <v>2177</v>
       </c>
       <c r="D103" t="n">
-        <v>3174470</v>
+        <v>3207470</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2905</v>
+        <v>2921</v>
       </c>
       <c r="D105" t="n">
-        <v>4241402</v>
+        <v>4265402</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D107" t="n">
-        <v>171120</v>
+        <v>177120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D108" t="n">
-        <v>224586</v>
+        <v>230586</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>138837</v>
+        <v>138968</v>
       </c>
       <c r="D109" t="n">
-        <v>171727843</v>
+        <v>171882772</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>52110</v>
+        <v>52152</v>
       </c>
       <c r="D115" t="n">
-        <v>76395826</v>
+        <v>76458543</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26491</v>
+        <v>26529</v>
       </c>
       <c r="D117" t="n">
-        <v>38379200</v>
+        <v>38432803</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1294</v>
+        <v>1297</v>
       </c>
       <c r="D118" t="n">
-        <v>1770551</v>
+        <v>1775051</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2175</v>
+        <v>2184</v>
       </c>
       <c r="D121" t="n">
-        <v>3054218</v>
+        <v>3067697</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>490570</v>
+        <v>491420</v>
       </c>
       <c r="D123" t="n">
-        <v>647008988</v>
+        <v>648119682</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1355</v>
+        <v>1357</v>
       </c>
       <c r="D128" t="n">
-        <v>2008811</v>
+        <v>2011811</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D129" t="n">
-        <v>39010</v>
+        <v>40510</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>203791</v>
+        <v>204097</v>
       </c>
       <c r="D130" t="n">
-        <v>299590510</v>
+        <v>300042477</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>175987</v>
+        <v>176257</v>
       </c>
       <c r="D133" t="n">
-        <v>255802165</v>
+        <v>256200655</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2793</v>
+        <v>2799</v>
       </c>
       <c r="D136" t="n">
-        <v>3925444</v>
+        <v>3933784</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6121</v>
+        <v>6131</v>
       </c>
       <c r="D138" t="n">
-        <v>8647603</v>
+        <v>8661949</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>43553</v>
+        <v>43635</v>
       </c>
       <c r="D141" t="n">
-        <v>58160226</v>
+        <v>58269634</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D146" t="n">
-        <v>676165</v>
+        <v>677665</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13836</v>
+        <v>13859</v>
       </c>
       <c r="D147" t="n">
-        <v>20294557</v>
+        <v>20328132</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3685</v>
+        <v>3688</v>
       </c>
       <c r="D148" t="n">
-        <v>5315965</v>
+        <v>5319238</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D151" t="n">
-        <v>559431</v>
+        <v>563931</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="D153" t="n">
-        <v>515751</v>
+        <v>524751</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>17125</v>
+        <v>17170</v>
       </c>
       <c r="D154" t="n">
-        <v>22633593</v>
+        <v>22695489</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>7001</v>
+        <v>7026</v>
       </c>
       <c r="D158" t="n">
-        <v>10185416</v>
+        <v>10219841</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4874</v>
+        <v>4894</v>
       </c>
       <c r="D160" t="n">
-        <v>7015456</v>
+        <v>7044436</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D162" t="n">
-        <v>370035</v>
+        <v>371235</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D163" t="n">
-        <v>369783</v>
+        <v>370774</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>14796</v>
+        <v>15080</v>
       </c>
       <c r="D165" t="n">
-        <v>21463720</v>
+        <v>21883231</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1716</v>
+        <v>1724</v>
       </c>
       <c r="D166" t="n">
-        <v>2552630</v>
+        <v>2564530</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D167" t="n">
-        <v>342802</v>
+        <v>344302</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D170" t="n">
-        <v>115449</v>
+        <v>116949</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>86300</v>
+        <v>86386</v>
       </c>
       <c r="D171" t="n">
-        <v>107985744</v>
+        <v>108082934</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33473</v>
+        <v>33500</v>
       </c>
       <c r="D178" t="n">
-        <v>49091394</v>
+        <v>49130831</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12789</v>
+        <v>12807</v>
       </c>
       <c r="D180" t="n">
-        <v>18478490</v>
+        <v>18504388</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>1231</v>
+        <v>1236</v>
       </c>
       <c r="D182" t="n">
-        <v>1722396</v>
+        <v>1729896</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1594</v>
+        <v>1598</v>
       </c>
       <c r="D184" t="n">
-        <v>2244193</v>
+        <v>2249693</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>234202</v>
+        <v>234507</v>
       </c>
       <c r="D186" t="n">
-        <v>291214392</v>
+        <v>291585336</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D188" t="n">
-        <v>236236</v>
+        <v>237736</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85668</v>
+        <v>85725</v>
       </c>
       <c r="D194" t="n">
-        <v>125590329</v>
+        <v>125673111</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32501</v>
+        <v>32542</v>
       </c>
       <c r="D197" t="n">
-        <v>46776170</v>
+        <v>46835537</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5022</v>
+        <v>5027</v>
       </c>
       <c r="D200" t="n">
-        <v>7156762</v>
+        <v>7164262</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4691</v>
+        <v>4706</v>
       </c>
       <c r="D203" t="n">
-        <v>6487816</v>
+        <v>6509827</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>258820</v>
+        <v>259210</v>
       </c>
       <c r="D206" t="n">
-        <v>320397886</v>
+        <v>320863622</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D207" t="n">
-        <v>169473</v>
+        <v>170973</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D208" t="n">
-        <v>353087</v>
+        <v>356087</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D213" t="n">
-        <v>882906</v>
+        <v>884406</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>93974</v>
+        <v>94073</v>
       </c>
       <c r="D215" t="n">
-        <v>137494162</v>
+        <v>137637989</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50574</v>
+        <v>50635</v>
       </c>
       <c r="D218" t="n">
-        <v>73092217</v>
+        <v>73181166</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D219" t="n">
-        <v>42922</v>
+        <v>44422</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4597</v>
+        <v>4607</v>
       </c>
       <c r="D221" t="n">
-        <v>6452415</v>
+        <v>6467232</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5525</v>
+        <v>5545</v>
       </c>
       <c r="D224" t="n">
-        <v>7639436</v>
+        <v>7669273</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>104441</v>
+        <v>104548</v>
       </c>
       <c r="D227" t="n">
-        <v>130749202</v>
+        <v>130877892</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D232" t="n">
-        <v>819439</v>
+        <v>820939</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48959</v>
+        <v>48983</v>
       </c>
       <c r="D234" t="n">
-        <v>71731859</v>
+        <v>71766007</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12173</v>
+        <v>12184</v>
       </c>
       <c r="D236" t="n">
-        <v>17500151</v>
+        <v>17516277</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2421</v>
+        <v>2423</v>
       </c>
       <c r="D240" t="n">
-        <v>3382219</v>
+        <v>3385150</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>252635</v>
+        <v>252961</v>
       </c>
       <c r="D241" t="n">
-        <v>319104043</v>
+        <v>319495817</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D243" t="n">
-        <v>351957</v>
+        <v>353457</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>94559</v>
+        <v>94651</v>
       </c>
       <c r="D249" t="n">
-        <v>138570298</v>
+        <v>138705244</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63786</v>
+        <v>63858</v>
       </c>
       <c r="D252" t="n">
-        <v>92438746</v>
+        <v>92542620</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2369</v>
+        <v>2376</v>
       </c>
       <c r="D254" t="n">
-        <v>3343918</v>
+        <v>3353361</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4453</v>
+        <v>4472</v>
       </c>
       <c r="D257" t="n">
-        <v>6250224</v>
+        <v>6276892</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-06 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>315122</v>
+        <v>315448</v>
       </c>
       <c r="D2" t="n">
-        <v>401744408</v>
+        <v>402139651</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D3" t="n">
-        <v>300350</v>
+        <v>301350</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>115809</v>
+        <v>115909</v>
       </c>
       <c r="D10" t="n">
-        <v>169704179</v>
+        <v>169849856</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58409</v>
+        <v>58467</v>
       </c>
       <c r="D12" t="n">
-        <v>84305345</v>
+        <v>84384552</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3949</v>
+        <v>3956</v>
       </c>
       <c r="D16" t="n">
-        <v>5605861</v>
+        <v>5616361</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6433</v>
+        <v>6448</v>
       </c>
       <c r="D20" t="n">
-        <v>8977335</v>
+        <v>8999385</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>76223</v>
+        <v>76280</v>
       </c>
       <c r="D22" t="n">
-        <v>95141217</v>
+        <v>95204800</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32149</v>
+        <v>32168</v>
       </c>
       <c r="D28" t="n">
-        <v>47069041</v>
+        <v>47095912</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11329</v>
+        <v>11339</v>
       </c>
       <c r="D30" t="n">
-        <v>16295486</v>
+        <v>16309112</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1547</v>
+        <v>1553</v>
       </c>
       <c r="D33" t="n">
-        <v>2171807</v>
+        <v>2180807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1766</v>
+        <v>1775</v>
       </c>
       <c r="D35" t="n">
-        <v>2492023</v>
+        <v>2504333</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95788</v>
+        <v>95864</v>
       </c>
       <c r="D36" t="n">
-        <v>120673422</v>
+        <v>120758463</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44000</v>
+        <v>44017</v>
       </c>
       <c r="D44" t="n">
-        <v>64490087</v>
+        <v>64512773</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9003</v>
+        <v>9016</v>
       </c>
       <c r="D46" t="n">
-        <v>12923224</v>
+        <v>12939198</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D48" t="n">
-        <v>1925100</v>
+        <v>1926600</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2241</v>
+        <v>2245</v>
       </c>
       <c r="D51" t="n">
-        <v>3125564</v>
+        <v>3131499</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>67967</v>
+        <v>68030</v>
       </c>
       <c r="D52" t="n">
-        <v>85310896</v>
+        <v>85385228</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>27852</v>
+        <v>27872</v>
       </c>
       <c r="D58" t="n">
-        <v>40850210</v>
+        <v>40879369</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10923</v>
+        <v>10935</v>
       </c>
       <c r="D61" t="n">
-        <v>15793057</v>
+        <v>15811057</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1343</v>
+        <v>1347</v>
       </c>
       <c r="D63" t="n">
-        <v>1876789</v>
+        <v>1882789</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1426</v>
+        <v>1436</v>
       </c>
       <c r="D67" t="n">
-        <v>1995599</v>
+        <v>2010599</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>20173</v>
+        <v>20204</v>
       </c>
       <c r="D69" t="n">
-        <v>26423774</v>
+        <v>26462753</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D72" t="n">
-        <v>83073</v>
+        <v>84573</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7486</v>
+        <v>7498</v>
       </c>
       <c r="D73" t="n">
-        <v>10959496</v>
+        <v>10976590</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5029</v>
+        <v>5040</v>
       </c>
       <c r="D75" t="n">
-        <v>7301706</v>
+        <v>7318206</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D76" t="n">
-        <v>683239</v>
+        <v>684739</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>138462</v>
+        <v>138606</v>
       </c>
       <c r="D78" t="n">
-        <v>172733006</v>
+        <v>172907533</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D83" t="n">
-        <v>18938</v>
+        <v>19021</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>62874</v>
+        <v>62922</v>
       </c>
       <c r="D84" t="n">
-        <v>92157458</v>
+        <v>92228125</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29270</v>
+        <v>29304</v>
       </c>
       <c r="D87" t="n">
-        <v>42346144</v>
+        <v>42395157</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2699</v>
+        <v>2705</v>
       </c>
       <c r="D89" t="n">
-        <v>3886643</v>
+        <v>3895643</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2734</v>
+        <v>2743</v>
       </c>
       <c r="D90" t="n">
-        <v>3862665</v>
+        <v>3875850</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>31773</v>
+        <v>31902</v>
       </c>
       <c r="D91" t="n">
-        <v>43055768</v>
+        <v>43227975</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7746</v>
+        <v>7765</v>
       </c>
       <c r="D95" t="n">
-        <v>11388970</v>
+        <v>11417070</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7039</v>
+        <v>7058</v>
       </c>
       <c r="D97" t="n">
-        <v>10204733</v>
+        <v>10231955</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D99" t="n">
-        <v>730405</v>
+        <v>731905</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8618</v>
+        <v>8676</v>
       </c>
       <c r="D101" t="n">
-        <v>11954383</v>
+        <v>12035029</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2177</v>
+        <v>2185</v>
       </c>
       <c r="D103" t="n">
-        <v>3207470</v>
+        <v>3219470</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2921</v>
+        <v>2939</v>
       </c>
       <c r="D105" t="n">
-        <v>4265402</v>
+        <v>4292112</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D107" t="n">
-        <v>177120</v>
+        <v>183120</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D108" t="n">
-        <v>230586</v>
+        <v>233586</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>138968</v>
+        <v>139094</v>
       </c>
       <c r="D109" t="n">
-        <v>171882772</v>
+        <v>172037233</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>52152</v>
+        <v>52184</v>
       </c>
       <c r="D115" t="n">
-        <v>76458543</v>
+        <v>76503350</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>26529</v>
+        <v>26551</v>
       </c>
       <c r="D117" t="n">
-        <v>38432803</v>
+        <v>38465443</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2184</v>
+        <v>2194</v>
       </c>
       <c r="D121" t="n">
-        <v>3067697</v>
+        <v>3081996</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>491420</v>
+        <v>492219</v>
       </c>
       <c r="D123" t="n">
-        <v>648119682</v>
+        <v>649150254</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1357</v>
+        <v>1360</v>
       </c>
       <c r="D128" t="n">
-        <v>2011811</v>
+        <v>2016311</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>204097</v>
+        <v>204369</v>
       </c>
       <c r="D130" t="n">
-        <v>300042477</v>
+        <v>300440174</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D131" t="n">
-        <v>575790</v>
+        <v>578790</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>176257</v>
+        <v>176529</v>
       </c>
       <c r="D133" t="n">
-        <v>256200655</v>
+        <v>256593906</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2799</v>
+        <v>2803</v>
       </c>
       <c r="D136" t="n">
-        <v>3933784</v>
+        <v>3939784</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6131</v>
+        <v>6153</v>
       </c>
       <c r="D138" t="n">
-        <v>8661949</v>
+        <v>8693320</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>43635</v>
+        <v>43687</v>
       </c>
       <c r="D141" t="n">
-        <v>58269634</v>
+        <v>58340355</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>13859</v>
+        <v>13868</v>
       </c>
       <c r="D147" t="n">
-        <v>20328132</v>
+        <v>20341228</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3688</v>
+        <v>3692</v>
       </c>
       <c r="D148" t="n">
-        <v>5319238</v>
+        <v>5325211</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D150" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D151" t="n">
-        <v>563931</v>
+        <v>565431</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D153" t="n">
-        <v>524751</v>
+        <v>526251</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>17170</v>
+        <v>17200</v>
       </c>
       <c r="D154" t="n">
-        <v>22695489</v>
+        <v>22731008</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>7026</v>
+        <v>7037</v>
       </c>
       <c r="D158" t="n">
-        <v>10219841</v>
+        <v>10233981</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4894</v>
+        <v>4902</v>
       </c>
       <c r="D160" t="n">
-        <v>7044436</v>
+        <v>7056436</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D162" t="n">
-        <v>371235</v>
+        <v>377235</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D163" t="n">
-        <v>370774</v>
+        <v>372274</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>15080</v>
+        <v>15222</v>
       </c>
       <c r="D165" t="n">
-        <v>21883231</v>
+        <v>22087426</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1724</v>
+        <v>1732</v>
       </c>
       <c r="D166" t="n">
-        <v>2564530</v>
+        <v>2576530</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>86386</v>
+        <v>86453</v>
       </c>
       <c r="D171" t="n">
-        <v>108082934</v>
+        <v>108159819</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D176" t="n">
-        <v>940348</v>
+        <v>941848</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>33500</v>
+        <v>33519</v>
       </c>
       <c r="D178" t="n">
-        <v>49130831</v>
+        <v>49158950</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>12807</v>
+        <v>12815</v>
       </c>
       <c r="D180" t="n">
-        <v>18504388</v>
+        <v>18516388</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="D184" t="n">
-        <v>2249693</v>
+        <v>2252693</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>234507</v>
+        <v>234752</v>
       </c>
       <c r="D186" t="n">
-        <v>291585336</v>
+        <v>291895644</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D187" t="n">
-        <v>141530</v>
+        <v>143030</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="D192" t="n">
-        <v>1270997</v>
+        <v>1272497</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>85725</v>
+        <v>85781</v>
       </c>
       <c r="D194" t="n">
-        <v>125673111</v>
+        <v>125751202</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>32542</v>
+        <v>32573</v>
       </c>
       <c r="D197" t="n">
-        <v>46835537</v>
+        <v>46877087</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5027</v>
+        <v>5033</v>
       </c>
       <c r="D200" t="n">
-        <v>7164262</v>
+        <v>7172101</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4706</v>
+        <v>4720</v>
       </c>
       <c r="D203" t="n">
-        <v>6509827</v>
+        <v>6530827</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>259210</v>
+        <v>259536</v>
       </c>
       <c r="D206" t="n">
-        <v>320863622</v>
+        <v>321272342</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D213" t="n">
-        <v>884406</v>
+        <v>886378</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>94073</v>
+        <v>94170</v>
       </c>
       <c r="D215" t="n">
-        <v>137637989</v>
+        <v>137772400</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D216" t="n">
-        <v>126699</v>
+        <v>128199</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>50635</v>
+        <v>50689</v>
       </c>
       <c r="D218" t="n">
-        <v>73181166</v>
+        <v>73257624</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4607</v>
+        <v>4611</v>
       </c>
       <c r="D221" t="n">
-        <v>6467232</v>
+        <v>6472416</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5545</v>
+        <v>5568</v>
       </c>
       <c r="D224" t="n">
-        <v>7669273</v>
+        <v>7703381</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>104548</v>
+        <v>104619</v>
       </c>
       <c r="D227" t="n">
-        <v>130877892</v>
+        <v>130957186</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D228" t="n">
-        <v>77405</v>
+        <v>78905</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>48983</v>
+        <v>49010</v>
       </c>
       <c r="D234" t="n">
-        <v>71766007</v>
+        <v>71804122</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12184</v>
+        <v>12196</v>
       </c>
       <c r="D236" t="n">
-        <v>17516277</v>
+        <v>17532969</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="D238" t="n">
-        <v>2687338</v>
+        <v>2688838</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2423</v>
+        <v>2426</v>
       </c>
       <c r="D240" t="n">
-        <v>3385150</v>
+        <v>3389650</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>252961</v>
+        <v>253233</v>
       </c>
       <c r="D241" t="n">
-        <v>319495817</v>
+        <v>319826601</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D242" t="n">
-        <v>209459</v>
+        <v>210959</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>94651</v>
+        <v>94712</v>
       </c>
       <c r="D249" t="n">
-        <v>138705244</v>
+        <v>138787414</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>63858</v>
+        <v>63938</v>
       </c>
       <c r="D252" t="n">
-        <v>92542620</v>
+        <v>92653129</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2376</v>
+        <v>2379</v>
       </c>
       <c r="D254" t="n">
-        <v>3353361</v>
+        <v>3357861</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>4472</v>
+        <v>4485</v>
       </c>
       <c r="D257" t="n">
-        <v>6276892</v>
+        <v>6296392</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-18 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>317645</v>
+        <v>319245</v>
       </c>
       <c r="D2" t="n">
-        <v>404785147</v>
+        <v>406871348</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D4" t="n">
-        <v>449207</v>
+        <v>450707</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D8" t="n">
-        <v>1259408</v>
+        <v>1262408</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>116345</v>
+        <v>116637</v>
       </c>
       <c r="D10" t="n">
-        <v>170479391</v>
+        <v>170910039</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58834</v>
+        <v>59099</v>
       </c>
       <c r="D12" t="n">
-        <v>84905431</v>
+        <v>85293945</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3997</v>
+        <v>4000</v>
       </c>
       <c r="D16" t="n">
-        <v>5672075</v>
+        <v>5676575</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6548</v>
+        <v>6589</v>
       </c>
       <c r="D20" t="n">
-        <v>9131339</v>
+        <v>9192134</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>76719</v>
+        <v>77128</v>
       </c>
       <c r="D22" t="n">
-        <v>95695584</v>
+        <v>96191150</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32275</v>
+        <v>32352</v>
       </c>
       <c r="D28" t="n">
-        <v>47247553</v>
+        <v>47359432</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11386</v>
+        <v>11432</v>
       </c>
       <c r="D30" t="n">
-        <v>16374789</v>
+        <v>16441040</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D33" t="n">
-        <v>2188307</v>
+        <v>2189807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1800</v>
+        <v>1809</v>
       </c>
       <c r="D35" t="n">
-        <v>2540531</v>
+        <v>2553671</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>96353</v>
+        <v>96746</v>
       </c>
       <c r="D36" t="n">
-        <v>121305396</v>
+        <v>121789127</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D42" t="n">
-        <v>1324685</v>
+        <v>1326185</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44133</v>
+        <v>44251</v>
       </c>
       <c r="D44" t="n">
-        <v>64675603</v>
+        <v>64849724</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9056</v>
+        <v>9098</v>
       </c>
       <c r="D46" t="n">
-        <v>12996244</v>
+        <v>13054796</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="D48" t="n">
-        <v>1943109</v>
+        <v>1945010</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2272</v>
+        <v>2285</v>
       </c>
       <c r="D51" t="n">
-        <v>3169665</v>
+        <v>3188628</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>68448</v>
+        <v>68780</v>
       </c>
       <c r="D52" t="n">
-        <v>85870468</v>
+        <v>86282932</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D54" t="n">
-        <v>57866</v>
+        <v>60697</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>27977</v>
+        <v>28084</v>
       </c>
       <c r="D59" t="n">
-        <v>41029769</v>
+        <v>41189366</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>10989</v>
+        <v>11051</v>
       </c>
       <c r="D62" t="n">
-        <v>15890144</v>
+        <v>15979479</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1449</v>
+        <v>1457</v>
       </c>
       <c r="D68" t="n">
-        <v>2029565</v>
+        <v>2041565</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20316</v>
+        <v>20414</v>
       </c>
       <c r="D70" t="n">
-        <v>26606591</v>
+        <v>26742300</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D73" t="n">
-        <v>84573</v>
+        <v>86073</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7537</v>
+        <v>7560</v>
       </c>
       <c r="D74" t="n">
-        <v>11035021</v>
+        <v>11069064</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5079</v>
+        <v>5104</v>
       </c>
       <c r="D76" t="n">
-        <v>7374678</v>
+        <v>7409384</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D78" t="n">
-        <v>378673</v>
+        <v>380173</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>139548</v>
+        <v>140259</v>
       </c>
       <c r="D79" t="n">
-        <v>174004762</v>
+        <v>174919792</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D81" t="n">
-        <v>121884</v>
+        <v>123384</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D83" t="n">
-        <v>619271</v>
+        <v>620771</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63143</v>
+        <v>63333</v>
       </c>
       <c r="D85" t="n">
-        <v>92545516</v>
+        <v>92824331</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29463</v>
+        <v>29592</v>
       </c>
       <c r="D88" t="n">
-        <v>42619516</v>
+        <v>42808751</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2779</v>
+        <v>2803</v>
       </c>
       <c r="D91" t="n">
-        <v>3925445</v>
+        <v>3959864</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>32541</v>
+        <v>32726</v>
       </c>
       <c r="D92" t="n">
-        <v>44078095</v>
+        <v>44337200</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D95" t="n">
-        <v>37314</v>
+        <v>38814</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7863</v>
+        <v>7903</v>
       </c>
       <c r="D96" t="n">
-        <v>11560856</v>
+        <v>11619686</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7193</v>
+        <v>7243</v>
       </c>
       <c r="D98" t="n">
-        <v>10429452</v>
+        <v>10503011</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D100" t="n">
-        <v>751716</v>
+        <v>753216</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>8984</v>
+        <v>9207</v>
       </c>
       <c r="D102" t="n">
-        <v>12473374</v>
+        <v>13033754</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2266</v>
+        <v>2338</v>
       </c>
       <c r="D104" t="n">
-        <v>3339302</v>
+        <v>3545597</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3025</v>
+        <v>3113</v>
       </c>
       <c r="D106" t="n">
-        <v>4417834</v>
+        <v>4660982</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D108" t="n">
-        <v>190620</v>
+        <v>195120</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D109" t="n">
-        <v>253043</v>
+        <v>253843</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>139976</v>
+        <v>140868</v>
       </c>
       <c r="D110" t="n">
-        <v>173057560</v>
+        <v>174213229</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52359</v>
+        <v>52526</v>
       </c>
       <c r="D116" t="n">
-        <v>76751867</v>
+        <v>76996340</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>26720</v>
+        <v>26881</v>
       </c>
       <c r="D118" t="n">
-        <v>38706826</v>
+        <v>38943412</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="D119" t="n">
-        <v>1788004</v>
+        <v>1790634</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2220</v>
+        <v>2240</v>
       </c>
       <c r="D122" t="n">
-        <v>3117138</v>
+        <v>3144983</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>497154</v>
+        <v>504630</v>
       </c>
       <c r="D124" t="n">
-        <v>655542822</v>
+        <v>665993506</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D126" t="n">
-        <v>309736</v>
+        <v>312009</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1366</v>
+        <v>1371</v>
       </c>
       <c r="D129" t="n">
-        <v>2025311</v>
+        <v>2032811</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D130" t="n">
-        <v>40510</v>
+        <v>42010</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>205715</v>
+        <v>206643</v>
       </c>
       <c r="D131" t="n">
-        <v>302397374</v>
+        <v>303763413</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D132" t="n">
-        <v>581790</v>
+        <v>586250</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>177987</v>
+        <v>180157</v>
       </c>
       <c r="D134" t="n">
-        <v>258693003</v>
+        <v>261897201</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2844</v>
+        <v>2846</v>
       </c>
       <c r="D137" t="n">
-        <v>3996716</v>
+        <v>3998456</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6239</v>
+        <v>6295</v>
       </c>
       <c r="D139" t="n">
-        <v>8812722</v>
+        <v>8894620</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>44091</v>
+        <v>44349</v>
       </c>
       <c r="D142" t="n">
-        <v>58853334</v>
+        <v>59209720</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>13952</v>
+        <v>13996</v>
       </c>
       <c r="D148" t="n">
-        <v>20459287</v>
+        <v>20525287</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3718</v>
+        <v>3735</v>
       </c>
       <c r="D149" t="n">
-        <v>5360897</v>
+        <v>5386097</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D152" t="n">
-        <v>572511</v>
+        <v>575216</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D154" t="n">
-        <v>530751</v>
+        <v>533751</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17394</v>
+        <v>17472</v>
       </c>
       <c r="D155" t="n">
-        <v>22980924</v>
+        <v>23088912</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7094</v>
+        <v>7118</v>
       </c>
       <c r="D159" t="n">
-        <v>10316395</v>
+        <v>10352086</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4944</v>
+        <v>4960</v>
       </c>
       <c r="D161" t="n">
-        <v>7114863</v>
+        <v>7137333</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D163" t="n">
-        <v>380231</v>
+        <v>381431</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>15728</v>
+        <v>16323</v>
       </c>
       <c r="D166" t="n">
-        <v>22822012</v>
+        <v>24422175</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1777</v>
+        <v>1839</v>
       </c>
       <c r="D167" t="n">
-        <v>2643230</v>
+        <v>2812613</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D168" t="n">
-        <v>348802</v>
+        <v>366802</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D170" t="n">
-        <v>79190</v>
+        <v>85190</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D171" t="n">
-        <v>128949</v>
+        <v>154449</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>86915</v>
+        <v>87367</v>
       </c>
       <c r="D172" t="n">
-        <v>108707093</v>
+        <v>109273205</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D176" t="n">
-        <v>19320</v>
+        <v>20820</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>33634</v>
+        <v>33738</v>
       </c>
       <c r="D179" t="n">
-        <v>49322182</v>
+        <v>49476963</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>12882</v>
+        <v>12953</v>
       </c>
       <c r="D181" t="n">
-        <v>18610299</v>
+        <v>18715230</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D183" t="n">
-        <v>1740396</v>
+        <v>1741896</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1629</v>
+        <v>1633</v>
       </c>
       <c r="D185" t="n">
-        <v>2288635</v>
+        <v>2294635</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>236441</v>
+        <v>237683</v>
       </c>
       <c r="D187" t="n">
-        <v>293904050</v>
+        <v>295485117</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D189" t="n">
-        <v>239236</v>
+        <v>242236</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="D193" t="n">
-        <v>1277845</v>
+        <v>1283845</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86070</v>
+        <v>86314</v>
       </c>
       <c r="D195" t="n">
-        <v>126165518</v>
+        <v>126525712</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>32749</v>
+        <v>32893</v>
       </c>
       <c r="D198" t="n">
-        <v>47131040</v>
+        <v>47343968</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5096</v>
+        <v>5101</v>
       </c>
       <c r="D201" t="n">
-        <v>7256836</v>
+        <v>7261436</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4804</v>
+        <v>4835</v>
       </c>
       <c r="D204" t="n">
-        <v>6650353</v>
+        <v>6696033</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>261441</v>
+        <v>262816</v>
       </c>
       <c r="D207" t="n">
-        <v>323540114</v>
+        <v>325294041</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D214" t="n">
-        <v>889378</v>
+        <v>890878</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>94555</v>
+        <v>94829</v>
       </c>
       <c r="D216" t="n">
-        <v>138324414</v>
+        <v>138730121</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D217" t="n">
-        <v>129699</v>
+        <v>131199</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>50987</v>
+        <v>51221</v>
       </c>
       <c r="D219" t="n">
-        <v>73687242</v>
+        <v>74033583</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4661</v>
+        <v>4667</v>
       </c>
       <c r="D222" t="n">
-        <v>6544355</v>
+        <v>6553355</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5650</v>
+        <v>5698</v>
       </c>
       <c r="D225" t="n">
-        <v>7811237</v>
+        <v>7880764</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>105240</v>
+        <v>105830</v>
       </c>
       <c r="D228" t="n">
-        <v>131638155</v>
+        <v>132390997</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D231" t="n">
-        <v>11147</v>
+        <v>12647</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D233" t="n">
-        <v>822439</v>
+        <v>823939</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49177</v>
+        <v>49299</v>
       </c>
       <c r="D235" t="n">
-        <v>72039495</v>
+        <v>72217501</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12255</v>
+        <v>12340</v>
       </c>
       <c r="D237" t="n">
-        <v>17619577</v>
+        <v>17745369</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="D239" t="n">
-        <v>2707382</v>
+        <v>2708882</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2470</v>
+        <v>2492</v>
       </c>
       <c r="D241" t="n">
-        <v>3453065</v>
+        <v>3484565</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>254907</v>
+        <v>256350</v>
       </c>
       <c r="D242" t="n">
-        <v>321805729</v>
+        <v>323705322</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D244" t="n">
-        <v>356457</v>
+        <v>357957</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="D248" t="n">
-        <v>1205563</v>
+        <v>1211563</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D249" t="n">
-        <v>13500</v>
+        <v>15000</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>95089</v>
+        <v>95424</v>
       </c>
       <c r="D250" t="n">
-        <v>139326822</v>
+        <v>139818032</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>64307</v>
+        <v>64672</v>
       </c>
       <c r="D253" t="n">
-        <v>93183772</v>
+        <v>93718520</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2402</v>
+        <v>2408</v>
       </c>
       <c r="D255" t="n">
-        <v>3389701</v>
+        <v>3396674</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4534</v>
+        <v>4566</v>
       </c>
       <c r="D258" t="n">
-        <v>6365450</v>
+        <v>6411613</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-19 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>319245</v>
+        <v>320625</v>
       </c>
       <c r="D2" t="n">
-        <v>406871348</v>
+        <v>408622958</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>306979</v>
+        <v>308479</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D4" t="n">
-        <v>450707</v>
+        <v>452207</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="D8" t="n">
-        <v>1262408</v>
+        <v>1266295</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>116637</v>
+        <v>116962</v>
       </c>
       <c r="D10" t="n">
-        <v>170910039</v>
+        <v>171386841</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59099</v>
+        <v>59357</v>
       </c>
       <c r="D12" t="n">
-        <v>85293945</v>
+        <v>85669933</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" t="n">
-        <v>66043</v>
+        <v>67543</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4000</v>
+        <v>4003</v>
       </c>
       <c r="D16" t="n">
-        <v>5676575</v>
+        <v>5681075</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6589</v>
+        <v>6643</v>
       </c>
       <c r="D20" t="n">
-        <v>9192134</v>
+        <v>9270246</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77128</v>
+        <v>77447</v>
       </c>
       <c r="D22" t="n">
-        <v>96191150</v>
+        <v>96577884</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32352</v>
+        <v>32453</v>
       </c>
       <c r="D28" t="n">
-        <v>47359432</v>
+        <v>47508425</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11432</v>
+        <v>11472</v>
       </c>
       <c r="D30" t="n">
-        <v>16441040</v>
+        <v>16500815</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1809</v>
+        <v>1826</v>
       </c>
       <c r="D35" t="n">
-        <v>2553671</v>
+        <v>2578410</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>96746</v>
+        <v>97098</v>
       </c>
       <c r="D36" t="n">
-        <v>121789127</v>
+        <v>122215897</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="D42" t="n">
-        <v>1326185</v>
+        <v>1327685</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44251</v>
+        <v>44356</v>
       </c>
       <c r="D44" t="n">
-        <v>64849724</v>
+        <v>65003278</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9098</v>
+        <v>9141</v>
       </c>
       <c r="D46" t="n">
-        <v>13054796</v>
+        <v>13118353</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1401</v>
+        <v>1404</v>
       </c>
       <c r="D48" t="n">
-        <v>1945010</v>
+        <v>1948603</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2285</v>
+        <v>2299</v>
       </c>
       <c r="D51" t="n">
-        <v>3188628</v>
+        <v>3208415</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>68780</v>
+        <v>69041</v>
       </c>
       <c r="D52" t="n">
-        <v>86282932</v>
+        <v>86599294</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D57" t="n">
-        <v>559965</v>
+        <v>561230</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28084</v>
+        <v>28181</v>
       </c>
       <c r="D59" t="n">
-        <v>41189366</v>
+        <v>41332157</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11051</v>
+        <v>11114</v>
       </c>
       <c r="D62" t="n">
-        <v>15979479</v>
+        <v>16071291</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1352</v>
+        <v>1358</v>
       </c>
       <c r="D64" t="n">
-        <v>1890289</v>
+        <v>1899289</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1457</v>
+        <v>1468</v>
       </c>
       <c r="D68" t="n">
-        <v>2041565</v>
+        <v>2056882</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20414</v>
+        <v>20494</v>
       </c>
       <c r="D70" t="n">
-        <v>26742300</v>
+        <v>26844470</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D73" t="n">
-        <v>86073</v>
+        <v>87573</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7560</v>
+        <v>7580</v>
       </c>
       <c r="D74" t="n">
-        <v>11069064</v>
+        <v>11099008</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5104</v>
+        <v>5121</v>
       </c>
       <c r="D76" t="n">
-        <v>7409384</v>
+        <v>7434515</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D77" t="n">
-        <v>690739</v>
+        <v>692239</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="D78" t="n">
-        <v>380173</v>
+        <v>387673</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>140259</v>
+        <v>140830</v>
       </c>
       <c r="D79" t="n">
-        <v>174919792</v>
+        <v>175629798</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="D83" t="n">
-        <v>620771</v>
+        <v>624824</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63333</v>
+        <v>63497</v>
       </c>
       <c r="D85" t="n">
-        <v>92824331</v>
+        <v>93061232</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D86" t="n">
-        <v>118582</v>
+        <v>120082</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29592</v>
+        <v>29706</v>
       </c>
       <c r="D88" t="n">
-        <v>42808751</v>
+        <v>42973422</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2723</v>
+        <v>2732</v>
       </c>
       <c r="D90" t="n">
-        <v>3920852</v>
+        <v>3933357</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2803</v>
+        <v>2824</v>
       </c>
       <c r="D91" t="n">
-        <v>3959864</v>
+        <v>3992864</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>32726</v>
+        <v>33028</v>
       </c>
       <c r="D92" t="n">
-        <v>44337200</v>
+        <v>44748641</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7903</v>
+        <v>7980</v>
       </c>
       <c r="D96" t="n">
-        <v>11619686</v>
+        <v>11734288</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7243</v>
+        <v>7336</v>
       </c>
       <c r="D98" t="n">
-        <v>10503011</v>
+        <v>10640354</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D100" t="n">
-        <v>753216</v>
+        <v>754716</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="D101" t="n">
-        <v>701198</v>
+        <v>712391</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9207</v>
+        <v>9614</v>
       </c>
       <c r="D102" t="n">
-        <v>13033754</v>
+        <v>14050818</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2338</v>
+        <v>2431</v>
       </c>
       <c r="D104" t="n">
-        <v>3545597</v>
+        <v>3803558</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3113</v>
+        <v>3256</v>
       </c>
       <c r="D106" t="n">
-        <v>4660982</v>
+        <v>5074796</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D108" t="n">
-        <v>195120</v>
+        <v>223220</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D109" t="n">
-        <v>253843</v>
+        <v>264543</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>140868</v>
+        <v>141504</v>
       </c>
       <c r="D110" t="n">
-        <v>174213229</v>
+        <v>175002933</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="D114" t="n">
-        <v>1392288</v>
+        <v>1393788</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52526</v>
+        <v>52677</v>
       </c>
       <c r="D116" t="n">
-        <v>76996340</v>
+        <v>77216646</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>26881</v>
+        <v>27039</v>
       </c>
       <c r="D118" t="n">
-        <v>38943412</v>
+        <v>39173191</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="D119" t="n">
-        <v>1790634</v>
+        <v>1792784</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2240</v>
+        <v>2260</v>
       </c>
       <c r="D122" t="n">
-        <v>3144983</v>
+        <v>3174143</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>504630</v>
+        <v>510118</v>
       </c>
       <c r="D124" t="n">
-        <v>665993506</v>
+        <v>673555727</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D125" t="n">
-        <v>117789</v>
+        <v>120789</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1371</v>
+        <v>1375</v>
       </c>
       <c r="D129" t="n">
-        <v>2032811</v>
+        <v>2037986</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>206643</v>
+        <v>207662</v>
       </c>
       <c r="D131" t="n">
-        <v>303763413</v>
+        <v>305269947</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="D132" t="n">
-        <v>586250</v>
+        <v>598250</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>180157</v>
+        <v>182064</v>
       </c>
       <c r="D134" t="n">
-        <v>261897201</v>
+        <v>264716069</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D136" t="n">
-        <v>45332</v>
+        <v>46832</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2846</v>
+        <v>2850</v>
       </c>
       <c r="D137" t="n">
-        <v>3998456</v>
+        <v>4004236</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6295</v>
+        <v>6338</v>
       </c>
       <c r="D139" t="n">
-        <v>8894620</v>
+        <v>8955307</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>44349</v>
+        <v>44607</v>
       </c>
       <c r="D142" t="n">
-        <v>59209720</v>
+        <v>59553539</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D144" t="n">
-        <v>33230</v>
+        <v>34730</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>13996</v>
+        <v>14064</v>
       </c>
       <c r="D148" t="n">
-        <v>20525287</v>
+        <v>20625662</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3735</v>
+        <v>3755</v>
       </c>
       <c r="D149" t="n">
-        <v>5386097</v>
+        <v>5415751</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D152" t="n">
-        <v>575216</v>
+        <v>576716</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D154" t="n">
-        <v>533751</v>
+        <v>539663</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17472</v>
+        <v>17580</v>
       </c>
       <c r="D155" t="n">
-        <v>23088912</v>
+        <v>23237179</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7118</v>
+        <v>7162</v>
       </c>
       <c r="D159" t="n">
-        <v>10352086</v>
+        <v>10416985</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4960</v>
+        <v>4995</v>
       </c>
       <c r="D161" t="n">
-        <v>7137333</v>
+        <v>7188346</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D163" t="n">
-        <v>381431</v>
+        <v>384431</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D164" t="n">
-        <v>378864</v>
+        <v>380364</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>16323</v>
+        <v>17110</v>
       </c>
       <c r="D166" t="n">
-        <v>24422175</v>
+        <v>26570937</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1839</v>
+        <v>1924</v>
       </c>
       <c r="D167" t="n">
-        <v>2812613</v>
+        <v>3049172</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="D168" t="n">
-        <v>366802</v>
+        <v>396802</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D170" t="n">
-        <v>85190</v>
+        <v>94190</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>87367</v>
+        <v>87715</v>
       </c>
       <c r="D172" t="n">
-        <v>109273205</v>
+        <v>109698302</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D177" t="n">
-        <v>941848</v>
+        <v>944848</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>33738</v>
+        <v>33840</v>
       </c>
       <c r="D179" t="n">
-        <v>49476963</v>
+        <v>49626554</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>12953</v>
+        <v>13021</v>
       </c>
       <c r="D181" t="n">
-        <v>18715230</v>
+        <v>18815300</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D183" t="n">
-        <v>1741896</v>
+        <v>1742429</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1633</v>
+        <v>1648</v>
       </c>
       <c r="D185" t="n">
-        <v>2294635</v>
+        <v>2316234</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>237683</v>
+        <v>238563</v>
       </c>
       <c r="D187" t="n">
-        <v>295485117</v>
+        <v>296568415</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="D193" t="n">
-        <v>1283845</v>
+        <v>1289845</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86314</v>
+        <v>86537</v>
       </c>
       <c r="D195" t="n">
-        <v>126525712</v>
+        <v>126854185</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>32893</v>
+        <v>33026</v>
       </c>
       <c r="D198" t="n">
-        <v>47343968</v>
+        <v>47537691</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D200" t="n">
-        <v>20608</v>
+        <v>22108</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5101</v>
+        <v>5109</v>
       </c>
       <c r="D201" t="n">
-        <v>7261436</v>
+        <v>7273022</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4835</v>
+        <v>4867</v>
       </c>
       <c r="D204" t="n">
-        <v>6696033</v>
+        <v>6740856</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>262816</v>
+        <v>263853</v>
       </c>
       <c r="D207" t="n">
-        <v>325294041</v>
+        <v>326570180</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D209" t="n">
-        <v>362087</v>
+        <v>363587</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D214" t="n">
-        <v>890878</v>
+        <v>895378</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>94829</v>
+        <v>95085</v>
       </c>
       <c r="D216" t="n">
-        <v>138730121</v>
+        <v>139106486</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51221</v>
+        <v>51421</v>
       </c>
       <c r="D219" t="n">
-        <v>74033583</v>
+        <v>74326568</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D220" t="n">
-        <v>44422</v>
+        <v>45922</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4667</v>
+        <v>4672</v>
       </c>
       <c r="D222" t="n">
-        <v>6553355</v>
+        <v>6559305</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5698</v>
+        <v>5735</v>
       </c>
       <c r="D225" t="n">
-        <v>7880764</v>
+        <v>7933597</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>105830</v>
+        <v>106305</v>
       </c>
       <c r="D228" t="n">
-        <v>132390997</v>
+        <v>132956279</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D230" t="n">
-        <v>103445</v>
+        <v>106445</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D233" t="n">
-        <v>823939</v>
+        <v>825439</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49299</v>
+        <v>49444</v>
       </c>
       <c r="D235" t="n">
-        <v>72217501</v>
+        <v>72431671</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D236" t="n">
-        <v>47211</v>
+        <v>48711</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12340</v>
+        <v>12403</v>
       </c>
       <c r="D237" t="n">
-        <v>17745369</v>
+        <v>17836981</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1890</v>
+        <v>1894</v>
       </c>
       <c r="D239" t="n">
-        <v>2708882</v>
+        <v>2714882</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2492</v>
+        <v>2508</v>
       </c>
       <c r="D241" t="n">
-        <v>3484565</v>
+        <v>3508565</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>256350</v>
+        <v>257642</v>
       </c>
       <c r="D242" t="n">
-        <v>323705322</v>
+        <v>325349607</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D244" t="n">
-        <v>357957</v>
+        <v>359457</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c r="D248" t="n">
-        <v>1211563</v>
+        <v>1220563</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>95424</v>
+        <v>95746</v>
       </c>
       <c r="D250" t="n">
-        <v>139818032</v>
+        <v>140291814</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>64672</v>
+        <v>65033</v>
       </c>
       <c r="D253" t="n">
-        <v>93718520</v>
+        <v>94245369</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2408</v>
+        <v>2412</v>
       </c>
       <c r="D255" t="n">
-        <v>3396674</v>
+        <v>3402009</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4566</v>
+        <v>4595</v>
       </c>
       <c r="D258" t="n">
-        <v>6411613</v>
+        <v>6452982</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-20 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>320625</v>
+        <v>321335</v>
       </c>
       <c r="D2" t="n">
-        <v>408622958</v>
+        <v>409522759</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="D8" t="n">
-        <v>1266295</v>
+        <v>1269295</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>116962</v>
+        <v>117147</v>
       </c>
       <c r="D10" t="n">
-        <v>171386841</v>
+        <v>171657107</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59357</v>
+        <v>59516</v>
       </c>
       <c r="D12" t="n">
-        <v>85669933</v>
+        <v>85899912</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4003</v>
+        <v>4007</v>
       </c>
       <c r="D16" t="n">
-        <v>5681075</v>
+        <v>5685992</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6643</v>
+        <v>6668</v>
       </c>
       <c r="D20" t="n">
-        <v>9270246</v>
+        <v>9306076</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77447</v>
+        <v>77629</v>
       </c>
       <c r="D22" t="n">
-        <v>96577884</v>
+        <v>96800087</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D27" t="n">
-        <v>410147</v>
+        <v>411647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32453</v>
+        <v>32496</v>
       </c>
       <c r="D28" t="n">
-        <v>47508425</v>
+        <v>47572675</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11472</v>
+        <v>11504</v>
       </c>
       <c r="D30" t="n">
-        <v>16500815</v>
+        <v>16548031</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="D35" t="n">
-        <v>2578410</v>
+        <v>2583295</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>97098</v>
+        <v>97314</v>
       </c>
       <c r="D36" t="n">
-        <v>122215897</v>
+        <v>122468812</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44356</v>
+        <v>44412</v>
       </c>
       <c r="D44" t="n">
-        <v>65003278</v>
+        <v>65086668</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9141</v>
+        <v>9160</v>
       </c>
       <c r="D46" t="n">
-        <v>13118353</v>
+        <v>13145853</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1404</v>
+        <v>1407</v>
       </c>
       <c r="D48" t="n">
-        <v>1948603</v>
+        <v>1953103</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2299</v>
+        <v>2308</v>
       </c>
       <c r="D51" t="n">
-        <v>3208415</v>
+        <v>3221915</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69041</v>
+        <v>69166</v>
       </c>
       <c r="D52" t="n">
-        <v>86599294</v>
+        <v>86754877</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28181</v>
+        <v>28217</v>
       </c>
       <c r="D59" t="n">
-        <v>41332157</v>
+        <v>41380960</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11114</v>
+        <v>11144</v>
       </c>
       <c r="D62" t="n">
-        <v>16071291</v>
+        <v>16113338</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1468</v>
+        <v>1474</v>
       </c>
       <c r="D68" t="n">
-        <v>2056882</v>
+        <v>2064149</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20494</v>
+        <v>20537</v>
       </c>
       <c r="D70" t="n">
-        <v>26844470</v>
+        <v>26904948</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7580</v>
+        <v>7596</v>
       </c>
       <c r="D74" t="n">
-        <v>11099008</v>
+        <v>11123008</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5121</v>
+        <v>5133</v>
       </c>
       <c r="D76" t="n">
-        <v>7434515</v>
+        <v>7452515</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="D77" t="n">
-        <v>692239</v>
+        <v>696739</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D78" t="n">
-        <v>387673</v>
+        <v>392173</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>140830</v>
+        <v>141110</v>
       </c>
       <c r="D79" t="n">
-        <v>175629798</v>
+        <v>175974123</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D80" t="n">
-        <v>81785</v>
+        <v>83285</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D83" t="n">
-        <v>624824</v>
+        <v>626324</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63497</v>
+        <v>63596</v>
       </c>
       <c r="D85" t="n">
-        <v>93061232</v>
+        <v>93206179</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29706</v>
+        <v>29780</v>
       </c>
       <c r="D88" t="n">
-        <v>42973422</v>
+        <v>43080712</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2732</v>
+        <v>2737</v>
       </c>
       <c r="D90" t="n">
-        <v>3933357</v>
+        <v>3940857</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2824</v>
+        <v>2831</v>
       </c>
       <c r="D91" t="n">
-        <v>3992864</v>
+        <v>4002218</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33028</v>
+        <v>33168</v>
       </c>
       <c r="D92" t="n">
-        <v>44748641</v>
+        <v>44943381</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7980</v>
+        <v>8025</v>
       </c>
       <c r="D96" t="n">
-        <v>11734288</v>
+        <v>11800209</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7336</v>
+        <v>7380</v>
       </c>
       <c r="D98" t="n">
-        <v>10640354</v>
+        <v>10706154</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D100" t="n">
-        <v>754716</v>
+        <v>757716</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9614</v>
+        <v>9812</v>
       </c>
       <c r="D102" t="n">
-        <v>14050818</v>
+        <v>14545354</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D103" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2431</v>
+        <v>2478</v>
       </c>
       <c r="D104" t="n">
-        <v>3803558</v>
+        <v>3936378</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3256</v>
+        <v>3314</v>
       </c>
       <c r="D106" t="n">
-        <v>5074796</v>
+        <v>5232274</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D108" t="n">
-        <v>223220</v>
+        <v>228820</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D109" t="n">
-        <v>264543</v>
+        <v>275043</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>141504</v>
+        <v>141790</v>
       </c>
       <c r="D110" t="n">
-        <v>175002933</v>
+        <v>175350331</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="D114" t="n">
-        <v>1393788</v>
+        <v>1394036</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52677</v>
+        <v>52769</v>
       </c>
       <c r="D116" t="n">
-        <v>77216646</v>
+        <v>77349493</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27039</v>
+        <v>27117</v>
       </c>
       <c r="D118" t="n">
-        <v>39173191</v>
+        <v>39287777</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D119" t="n">
-        <v>1792784</v>
+        <v>1794284</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2260</v>
+        <v>2265</v>
       </c>
       <c r="D122" t="n">
-        <v>3174143</v>
+        <v>3181643</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>510118</v>
+        <v>512941</v>
       </c>
       <c r="D124" t="n">
-        <v>673555727</v>
+        <v>677422128</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1375</v>
+        <v>1378</v>
       </c>
       <c r="D129" t="n">
-        <v>2037986</v>
+        <v>2042486</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>207662</v>
+        <v>208249</v>
       </c>
       <c r="D131" t="n">
-        <v>305269947</v>
+        <v>306137580</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D132" t="n">
-        <v>598250</v>
+        <v>599750</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>182064</v>
+        <v>183058</v>
       </c>
       <c r="D134" t="n">
-        <v>264716069</v>
+        <v>266179685</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2850</v>
+        <v>2852</v>
       </c>
       <c r="D137" t="n">
-        <v>4004236</v>
+        <v>4007236</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6338</v>
+        <v>6363</v>
       </c>
       <c r="D139" t="n">
-        <v>8955307</v>
+        <v>8986191</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>44607</v>
+        <v>44773</v>
       </c>
       <c r="D142" t="n">
-        <v>59553539</v>
+        <v>59780360</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14064</v>
+        <v>14092</v>
       </c>
       <c r="D148" t="n">
-        <v>20625662</v>
+        <v>20664361</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3755</v>
+        <v>3761</v>
       </c>
       <c r="D149" t="n">
-        <v>5415751</v>
+        <v>5424751</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D152" t="n">
-        <v>576716</v>
+        <v>578216</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D154" t="n">
-        <v>539663</v>
+        <v>544163</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17580</v>
+        <v>17640</v>
       </c>
       <c r="D155" t="n">
-        <v>23237179</v>
+        <v>23319922</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7162</v>
+        <v>7189</v>
       </c>
       <c r="D159" t="n">
-        <v>10416985</v>
+        <v>10456701</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4995</v>
+        <v>5017</v>
       </c>
       <c r="D161" t="n">
-        <v>7188346</v>
+        <v>7220397</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D164" t="n">
-        <v>380364</v>
+        <v>381864</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>17110</v>
+        <v>17526</v>
       </c>
       <c r="D166" t="n">
-        <v>26570937</v>
+        <v>27658559</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1924</v>
+        <v>1945</v>
       </c>
       <c r="D167" t="n">
-        <v>3049172</v>
+        <v>3105649</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D168" t="n">
-        <v>396802</v>
+        <v>412433</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D170" t="n">
-        <v>94190</v>
+        <v>100190</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>87715</v>
+        <v>87893</v>
       </c>
       <c r="D172" t="n">
-        <v>109698302</v>
+        <v>109911146</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D177" t="n">
-        <v>944848</v>
+        <v>946348</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>33840</v>
+        <v>33903</v>
       </c>
       <c r="D179" t="n">
-        <v>49626554</v>
+        <v>49720524</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13021</v>
+        <v>13062</v>
       </c>
       <c r="D181" t="n">
-        <v>18815300</v>
+        <v>18873514</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="D183" t="n">
-        <v>1742429</v>
+        <v>1745429</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="D185" t="n">
-        <v>2316234</v>
+        <v>2322234</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D186" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>238563</v>
+        <v>239039</v>
       </c>
       <c r="D187" t="n">
-        <v>296568415</v>
+        <v>297152156</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="D193" t="n">
-        <v>1289845</v>
+        <v>1291345</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86537</v>
+        <v>86687</v>
       </c>
       <c r="D195" t="n">
-        <v>126854185</v>
+        <v>127073143</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D196" t="n">
-        <v>135127</v>
+        <v>136627</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33026</v>
+        <v>33105</v>
       </c>
       <c r="D198" t="n">
-        <v>47537691</v>
+        <v>47653114</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5109</v>
+        <v>5114</v>
       </c>
       <c r="D201" t="n">
-        <v>7273022</v>
+        <v>7279777</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4867</v>
+        <v>4880</v>
       </c>
       <c r="D204" t="n">
-        <v>6740856</v>
+        <v>6757428</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>263853</v>
+        <v>264478</v>
       </c>
       <c r="D207" t="n">
-        <v>326570180</v>
+        <v>327325610</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D214" t="n">
-        <v>895378</v>
+        <v>898378</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95085</v>
+        <v>95230</v>
       </c>
       <c r="D216" t="n">
-        <v>139106486</v>
+        <v>139321251</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D217" t="n">
-        <v>131199</v>
+        <v>132699</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51421</v>
+        <v>51568</v>
       </c>
       <c r="D219" t="n">
-        <v>74326568</v>
+        <v>74541518</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D220" t="n">
-        <v>45922</v>
+        <v>48922</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4672</v>
+        <v>4673</v>
       </c>
       <c r="D222" t="n">
-        <v>6559305</v>
+        <v>6560805</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5735</v>
+        <v>5771</v>
       </c>
       <c r="D225" t="n">
-        <v>7933597</v>
+        <v>7983779</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>106305</v>
+        <v>106574</v>
       </c>
       <c r="D228" t="n">
-        <v>132956279</v>
+        <v>133275394</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D233" t="n">
-        <v>825439</v>
+        <v>826939</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49444</v>
+        <v>49559</v>
       </c>
       <c r="D235" t="n">
-        <v>72431671</v>
+        <v>72599734</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12403</v>
+        <v>12443</v>
       </c>
       <c r="D237" t="n">
-        <v>17836981</v>
+        <v>17892635</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1894</v>
+        <v>1896</v>
       </c>
       <c r="D239" t="n">
-        <v>2714882</v>
+        <v>2717882</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2508</v>
+        <v>2515</v>
       </c>
       <c r="D241" t="n">
-        <v>3508565</v>
+        <v>3518971</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>257642</v>
+        <v>258296</v>
       </c>
       <c r="D242" t="n">
-        <v>325349607</v>
+        <v>326191127</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D248" t="n">
-        <v>1220563</v>
+        <v>1222063</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>95746</v>
+        <v>95917</v>
       </c>
       <c r="D250" t="n">
-        <v>140291814</v>
+        <v>140544736</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65033</v>
+        <v>65239</v>
       </c>
       <c r="D253" t="n">
-        <v>94245369</v>
+        <v>94546964</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2412</v>
+        <v>2413</v>
       </c>
       <c r="D255" t="n">
-        <v>3402009</v>
+        <v>3403509</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4595</v>
+        <v>4620</v>
       </c>
       <c r="D258" t="n">
-        <v>6452982</v>
+        <v>6489371</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-21 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>321335</v>
+        <v>322380</v>
       </c>
       <c r="D2" t="n">
-        <v>409522759</v>
+        <v>410843293</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D3" t="n">
-        <v>308479</v>
+        <v>309979</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D4" t="n">
-        <v>452207</v>
+        <v>453707</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="D8" t="n">
-        <v>1269295</v>
+        <v>1273795</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117147</v>
+        <v>117398</v>
       </c>
       <c r="D10" t="n">
-        <v>171657107</v>
+        <v>172022519</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D11" t="n">
-        <v>210013</v>
+        <v>211513</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59516</v>
+        <v>59711</v>
       </c>
       <c r="D12" t="n">
-        <v>85899912</v>
+        <v>86184648</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4007</v>
+        <v>4009</v>
       </c>
       <c r="D16" t="n">
-        <v>5685992</v>
+        <v>5688992</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" t="n">
-        <v>101535</v>
+        <v>103035</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6668</v>
+        <v>6725</v>
       </c>
       <c r="D20" t="n">
-        <v>9306076</v>
+        <v>9388533</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77629</v>
+        <v>77849</v>
       </c>
       <c r="D22" t="n">
-        <v>96800087</v>
+        <v>97046177</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D27" t="n">
-        <v>411647</v>
+        <v>413147</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32496</v>
+        <v>32564</v>
       </c>
       <c r="D28" t="n">
-        <v>47572675</v>
+        <v>47669242</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11504</v>
+        <v>11529</v>
       </c>
       <c r="D30" t="n">
-        <v>16548031</v>
+        <v>16584949</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D33" t="n">
-        <v>2189807</v>
+        <v>2191307</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1830</v>
+        <v>1844</v>
       </c>
       <c r="D35" t="n">
-        <v>2583295</v>
+        <v>2603270</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>97314</v>
+        <v>97589</v>
       </c>
       <c r="D36" t="n">
-        <v>122468812</v>
+        <v>122794547</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D37" t="n">
-        <v>77037</v>
+        <v>77868</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="D42" t="n">
-        <v>1327685</v>
+        <v>1329185</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44412</v>
+        <v>44481</v>
       </c>
       <c r="D44" t="n">
-        <v>65086668</v>
+        <v>65188847</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9160</v>
+        <v>9184</v>
       </c>
       <c r="D46" t="n">
-        <v>13145853</v>
+        <v>13178380</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D48" t="n">
-        <v>1953103</v>
+        <v>1954603</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2308</v>
+        <v>2325</v>
       </c>
       <c r="D51" t="n">
-        <v>3221915</v>
+        <v>3245929</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69166</v>
+        <v>69352</v>
       </c>
       <c r="D52" t="n">
-        <v>86754877</v>
+        <v>86989444</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D53" t="n">
-        <v>43383</v>
+        <v>47883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D57" t="n">
-        <v>561230</v>
+        <v>562730</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28217</v>
+        <v>28284</v>
       </c>
       <c r="D59" t="n">
-        <v>41380960</v>
+        <v>41479994</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11144</v>
+        <v>11178</v>
       </c>
       <c r="D62" t="n">
-        <v>16113338</v>
+        <v>16164170</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="D64" t="n">
-        <v>1899289</v>
+        <v>1902289</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1474</v>
+        <v>1487</v>
       </c>
       <c r="D68" t="n">
-        <v>2064149</v>
+        <v>2082584</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20537</v>
+        <v>20592</v>
       </c>
       <c r="D70" t="n">
-        <v>26904948</v>
+        <v>26975819</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7596</v>
+        <v>7616</v>
       </c>
       <c r="D74" t="n">
-        <v>11123008</v>
+        <v>11153008</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5133</v>
+        <v>5148</v>
       </c>
       <c r="D76" t="n">
-        <v>7452515</v>
+        <v>7474910</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D77" t="n">
-        <v>696739</v>
+        <v>699739</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D78" t="n">
-        <v>392173</v>
+        <v>393083</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>141110</v>
+        <v>141494</v>
       </c>
       <c r="D79" t="n">
-        <v>175974123</v>
+        <v>176410978</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D80" t="n">
-        <v>83285</v>
+        <v>84321</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63596</v>
+        <v>63711</v>
       </c>
       <c r="D85" t="n">
-        <v>93206179</v>
+        <v>93377216</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29780</v>
+        <v>29867</v>
       </c>
       <c r="D88" t="n">
-        <v>43080712</v>
+        <v>43207116</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2831</v>
+        <v>2855</v>
       </c>
       <c r="D91" t="n">
-        <v>4002218</v>
+        <v>4037318</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33168</v>
+        <v>33426</v>
       </c>
       <c r="D92" t="n">
-        <v>44943381</v>
+        <v>45305052</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D95" t="n">
-        <v>38814</v>
+        <v>40314</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8025</v>
+        <v>8086</v>
       </c>
       <c r="D96" t="n">
-        <v>11800209</v>
+        <v>11888715</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7380</v>
+        <v>7442</v>
       </c>
       <c r="D98" t="n">
-        <v>10706154</v>
+        <v>10798839</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="D100" t="n">
-        <v>757716</v>
+        <v>763651</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="D101" t="n">
-        <v>712391</v>
+        <v>719891</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9812</v>
+        <v>10098</v>
       </c>
       <c r="D102" t="n">
-        <v>14545354</v>
+        <v>15183364</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2478</v>
+        <v>2515</v>
       </c>
       <c r="D104" t="n">
-        <v>3936378</v>
+        <v>4043791</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3314</v>
+        <v>3380</v>
       </c>
       <c r="D106" t="n">
-        <v>5232274</v>
+        <v>5412425</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D108" t="n">
-        <v>228820</v>
+        <v>248320</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D109" t="n">
-        <v>275043</v>
+        <v>288468</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>141790</v>
+        <v>142213</v>
       </c>
       <c r="D110" t="n">
-        <v>175350331</v>
+        <v>175859022</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="D114" t="n">
-        <v>1394036</v>
+        <v>1395536</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52769</v>
+        <v>52884</v>
       </c>
       <c r="D116" t="n">
-        <v>77349493</v>
+        <v>77518194</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27117</v>
+        <v>27230</v>
       </c>
       <c r="D118" t="n">
-        <v>39287777</v>
+        <v>39452525</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D119" t="n">
-        <v>1794284</v>
+        <v>1795784</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2265</v>
+        <v>2282</v>
       </c>
       <c r="D122" t="n">
-        <v>3181643</v>
+        <v>3206569</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>512941</v>
+        <v>516974</v>
       </c>
       <c r="D124" t="n">
-        <v>677422128</v>
+        <v>682834769</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D126" t="n">
-        <v>312009</v>
+        <v>313509</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1378</v>
+        <v>1381</v>
       </c>
       <c r="D129" t="n">
-        <v>2042486</v>
+        <v>2046986</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>208249</v>
+        <v>209127</v>
       </c>
       <c r="D131" t="n">
-        <v>306137580</v>
+        <v>307433450</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D132" t="n">
-        <v>599750</v>
+        <v>604250</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>183058</v>
+        <v>184300</v>
       </c>
       <c r="D134" t="n">
-        <v>266179685</v>
+        <v>268004291</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D135" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2852</v>
+        <v>2854</v>
       </c>
       <c r="D137" t="n">
-        <v>4007236</v>
+        <v>4008969</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6363</v>
+        <v>6420</v>
       </c>
       <c r="D139" t="n">
-        <v>8986191</v>
+        <v>9069280</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>44773</v>
+        <v>44941</v>
       </c>
       <c r="D142" t="n">
-        <v>59780360</v>
+        <v>60005115</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D143" t="n">
-        <v>39791</v>
+        <v>40262</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D146" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14092</v>
+        <v>14137</v>
       </c>
       <c r="D148" t="n">
-        <v>20664361</v>
+        <v>20728558</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3761</v>
+        <v>3787</v>
       </c>
       <c r="D149" t="n">
-        <v>5424751</v>
+        <v>5461520</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D154" t="n">
-        <v>544163</v>
+        <v>547163</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17640</v>
+        <v>17730</v>
       </c>
       <c r="D155" t="n">
-        <v>23319922</v>
+        <v>23436553</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7189</v>
+        <v>7222</v>
       </c>
       <c r="D159" t="n">
-        <v>10456701</v>
+        <v>10505701</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5017</v>
+        <v>5047</v>
       </c>
       <c r="D161" t="n">
-        <v>7220397</v>
+        <v>7264413</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D163" t="n">
-        <v>384431</v>
+        <v>388931</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D164" t="n">
-        <v>381864</v>
+        <v>386364</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>17526</v>
+        <v>18005</v>
       </c>
       <c r="D166" t="n">
-        <v>27658559</v>
+        <v>28860627</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1945</v>
+        <v>1985</v>
       </c>
       <c r="D167" t="n">
-        <v>3105649</v>
+        <v>3214449</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D168" t="n">
-        <v>412433</v>
+        <v>425661</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D170" t="n">
-        <v>100190</v>
+        <v>107690</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D171" t="n">
-        <v>154449</v>
+        <v>160449</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>87893</v>
+        <v>88166</v>
       </c>
       <c r="D172" t="n">
-        <v>109911146</v>
+        <v>110225791</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>33903</v>
+        <v>33975</v>
       </c>
       <c r="D179" t="n">
-        <v>49720524</v>
+        <v>49824677</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13062</v>
+        <v>13097</v>
       </c>
       <c r="D181" t="n">
-        <v>18873514</v>
+        <v>18924462</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1652</v>
+        <v>1669</v>
       </c>
       <c r="D185" t="n">
-        <v>2322234</v>
+        <v>2346650</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>239039</v>
+        <v>239691</v>
       </c>
       <c r="D187" t="n">
-        <v>297152156</v>
+        <v>297920989</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D188" t="n">
-        <v>144587</v>
+        <v>146087</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="D193" t="n">
-        <v>1291345</v>
+        <v>1297345</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86687</v>
+        <v>86861</v>
       </c>
       <c r="D195" t="n">
-        <v>127073143</v>
+        <v>127329295</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33105</v>
+        <v>33198</v>
       </c>
       <c r="D198" t="n">
-        <v>47653114</v>
+        <v>47789043</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5114</v>
+        <v>5121</v>
       </c>
       <c r="D201" t="n">
-        <v>7279777</v>
+        <v>7290277</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4880</v>
+        <v>4926</v>
       </c>
       <c r="D204" t="n">
-        <v>6757428</v>
+        <v>6820989</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>264478</v>
+        <v>265303</v>
       </c>
       <c r="D207" t="n">
-        <v>327325610</v>
+        <v>328314392</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D209" t="n">
-        <v>363587</v>
+        <v>365087</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8362,10 +8362,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D211" t="n">
-        <v>12052</v>
+        <v>12731</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95230</v>
+        <v>95461</v>
       </c>
       <c r="D216" t="n">
-        <v>139321251</v>
+        <v>139656018</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D217" t="n">
-        <v>132699</v>
+        <v>134199</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51568</v>
+        <v>51710</v>
       </c>
       <c r="D219" t="n">
-        <v>74541518</v>
+        <v>74743148</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4673</v>
+        <v>4684</v>
       </c>
       <c r="D222" t="n">
-        <v>6560805</v>
+        <v>6577031</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5771</v>
+        <v>5824</v>
       </c>
       <c r="D225" t="n">
-        <v>7983779</v>
+        <v>8057434</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>106574</v>
+        <v>106890</v>
       </c>
       <c r="D228" t="n">
-        <v>133275394</v>
+        <v>133663492</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49559</v>
+        <v>49670</v>
       </c>
       <c r="D235" t="n">
-        <v>72599734</v>
+        <v>72762868</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12443</v>
+        <v>12494</v>
       </c>
       <c r="D237" t="n">
-        <v>17892635</v>
+        <v>17964997</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2515</v>
+        <v>2539</v>
       </c>
       <c r="D241" t="n">
-        <v>3518971</v>
+        <v>3552972</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>258296</v>
+        <v>259193</v>
       </c>
       <c r="D242" t="n">
-        <v>326191127</v>
+        <v>327300068</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D244" t="n">
-        <v>359457</v>
+        <v>360312</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="D248" t="n">
-        <v>1222063</v>
+        <v>1223563</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>95917</v>
+        <v>96169</v>
       </c>
       <c r="D250" t="n">
-        <v>140544736</v>
+        <v>140916287</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65239</v>
+        <v>65459</v>
       </c>
       <c r="D253" t="n">
-        <v>94546964</v>
+        <v>94866547</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2413</v>
+        <v>2417</v>
       </c>
       <c r="D255" t="n">
-        <v>3403509</v>
+        <v>3408238</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4620</v>
+        <v>4656</v>
       </c>
       <c r="D258" t="n">
-        <v>6489371</v>
+        <v>6541560</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>322380</v>
+        <v>322974</v>
       </c>
       <c r="D2" t="n">
-        <v>410843293</v>
+        <v>411573047</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D4" t="n">
-        <v>453707</v>
+        <v>456707</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117398</v>
+        <v>117562</v>
       </c>
       <c r="D10" t="n">
-        <v>172022519</v>
+        <v>172259949</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59711</v>
+        <v>59844</v>
       </c>
       <c r="D12" t="n">
-        <v>86184648</v>
+        <v>86375361</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4009</v>
+        <v>4012</v>
       </c>
       <c r="D16" t="n">
-        <v>5688992</v>
+        <v>5693492</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6725</v>
+        <v>6764</v>
       </c>
       <c r="D20" t="n">
-        <v>9388533</v>
+        <v>9440454</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77849</v>
+        <v>77998</v>
       </c>
       <c r="D22" t="n">
-        <v>97046177</v>
+        <v>97219735</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D27" t="n">
-        <v>413147</v>
+        <v>414647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32564</v>
+        <v>32613</v>
       </c>
       <c r="D28" t="n">
-        <v>47669242</v>
+        <v>47737942</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11529</v>
+        <v>11544</v>
       </c>
       <c r="D30" t="n">
-        <v>16584949</v>
+        <v>16607449</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D33" t="n">
-        <v>2191307</v>
+        <v>2192807</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1844</v>
+        <v>1852</v>
       </c>
       <c r="D35" t="n">
-        <v>2603270</v>
+        <v>2615179</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>97589</v>
+        <v>97732</v>
       </c>
       <c r="D36" t="n">
-        <v>122794547</v>
+        <v>122958638</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D42" t="n">
-        <v>1329185</v>
+        <v>1330685</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44481</v>
+        <v>44526</v>
       </c>
       <c r="D44" t="n">
-        <v>65188847</v>
+        <v>65254435</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9184</v>
+        <v>9197</v>
       </c>
       <c r="D46" t="n">
-        <v>13178380</v>
+        <v>13196716</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2325</v>
+        <v>2340</v>
       </c>
       <c r="D51" t="n">
-        <v>3245929</v>
+        <v>3268018</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69352</v>
+        <v>69450</v>
       </c>
       <c r="D52" t="n">
-        <v>86989444</v>
+        <v>87108726</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28284</v>
+        <v>28316</v>
       </c>
       <c r="D59" t="n">
-        <v>41479994</v>
+        <v>41525953</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11178</v>
+        <v>11200</v>
       </c>
       <c r="D62" t="n">
-        <v>16164170</v>
+        <v>16196623</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1360</v>
+        <v>1363</v>
       </c>
       <c r="D64" t="n">
-        <v>1902289</v>
+        <v>1904737</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1487</v>
+        <v>1494</v>
       </c>
       <c r="D68" t="n">
-        <v>2082584</v>
+        <v>2093084</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20592</v>
+        <v>20618</v>
       </c>
       <c r="D70" t="n">
-        <v>26975819</v>
+        <v>27008207</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7616</v>
+        <v>7624</v>
       </c>
       <c r="D74" t="n">
-        <v>11153008</v>
+        <v>11164724</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5148</v>
+        <v>5156</v>
       </c>
       <c r="D76" t="n">
-        <v>7474910</v>
+        <v>7486610</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>141494</v>
+        <v>141733</v>
       </c>
       <c r="D79" t="n">
-        <v>176410978</v>
+        <v>176687278</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D83" t="n">
-        <v>626324</v>
+        <v>627824</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63711</v>
+        <v>63803</v>
       </c>
       <c r="D85" t="n">
-        <v>93377216</v>
+        <v>93512484</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29867</v>
+        <v>29907</v>
       </c>
       <c r="D88" t="n">
-        <v>43207116</v>
+        <v>43265941</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2855</v>
+        <v>2868</v>
       </c>
       <c r="D91" t="n">
-        <v>4037318</v>
+        <v>4056084</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33426</v>
+        <v>33483</v>
       </c>
       <c r="D92" t="n">
-        <v>45305052</v>
+        <v>45379530</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8086</v>
+        <v>8106</v>
       </c>
       <c r="D96" t="n">
-        <v>11888715</v>
+        <v>11918050</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7442</v>
+        <v>7458</v>
       </c>
       <c r="D98" t="n">
-        <v>10798839</v>
+        <v>10822367</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10098</v>
+        <v>10197</v>
       </c>
       <c r="D102" t="n">
-        <v>15183364</v>
+        <v>15394555</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2515</v>
+        <v>2537</v>
       </c>
       <c r="D104" t="n">
-        <v>4043791</v>
+        <v>4100088</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3380</v>
+        <v>3413</v>
       </c>
       <c r="D106" t="n">
-        <v>5412425</v>
+        <v>5504979</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D108" t="n">
-        <v>248320</v>
+        <v>256445</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D109" t="n">
-        <v>288468</v>
+        <v>298032</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>142213</v>
+        <v>142418</v>
       </c>
       <c r="D110" t="n">
-        <v>175859022</v>
+        <v>176119579</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D112" t="n">
-        <v>102644</v>
+        <v>104144</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52884</v>
+        <v>52971</v>
       </c>
       <c r="D116" t="n">
-        <v>77518194</v>
+        <v>77645580</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27230</v>
+        <v>27303</v>
       </c>
       <c r="D118" t="n">
-        <v>39452525</v>
+        <v>39560507</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2282</v>
+        <v>2294</v>
       </c>
       <c r="D122" t="n">
-        <v>3206569</v>
+        <v>3222668</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>516974</v>
+        <v>518530</v>
       </c>
       <c r="D124" t="n">
-        <v>682834769</v>
+        <v>684872080</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D126" t="n">
-        <v>313509</v>
+        <v>316509</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D129" t="n">
-        <v>2046986</v>
+        <v>2048486</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>209127</v>
+        <v>209555</v>
       </c>
       <c r="D131" t="n">
-        <v>307433450</v>
+        <v>308059771</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>184300</v>
+        <v>184904</v>
       </c>
       <c r="D134" t="n">
-        <v>268004291</v>
+        <v>268890806</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2854</v>
+        <v>2856</v>
       </c>
       <c r="D137" t="n">
-        <v>4008969</v>
+        <v>4011969</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6420</v>
+        <v>6453</v>
       </c>
       <c r="D139" t="n">
-        <v>9069280</v>
+        <v>9117366</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>44941</v>
+        <v>45019</v>
       </c>
       <c r="D142" t="n">
-        <v>60005115</v>
+        <v>60106966</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14137</v>
+        <v>14162</v>
       </c>
       <c r="D148" t="n">
-        <v>20728558</v>
+        <v>20764513</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3787</v>
+        <v>3794</v>
       </c>
       <c r="D149" t="n">
-        <v>5461520</v>
+        <v>5471002</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="D154" t="n">
-        <v>547163</v>
+        <v>552263</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17730</v>
+        <v>17748</v>
       </c>
       <c r="D155" t="n">
-        <v>23436553</v>
+        <v>23460996</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7222</v>
+        <v>7236</v>
       </c>
       <c r="D159" t="n">
-        <v>10505701</v>
+        <v>10526263</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5047</v>
+        <v>5054</v>
       </c>
       <c r="D161" t="n">
-        <v>7264413</v>
+        <v>7274629</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18005</v>
+        <v>18252</v>
       </c>
       <c r="D166" t="n">
-        <v>28860627</v>
+        <v>29420621</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1985</v>
+        <v>1996</v>
       </c>
       <c r="D167" t="n">
-        <v>3214449</v>
+        <v>3244449</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D168" t="n">
-        <v>425661</v>
+        <v>430101</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88166</v>
+        <v>88331</v>
       </c>
       <c r="D172" t="n">
-        <v>110225791</v>
+        <v>110425175</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>33975</v>
+        <v>34007</v>
       </c>
       <c r="D179" t="n">
-        <v>49824677</v>
+        <v>49872577</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13097</v>
+        <v>13117</v>
       </c>
       <c r="D181" t="n">
-        <v>18924462</v>
+        <v>18954462</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1669</v>
+        <v>1677</v>
       </c>
       <c r="D185" t="n">
-        <v>2346650</v>
+        <v>2357296</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>239691</v>
+        <v>240028</v>
       </c>
       <c r="D187" t="n">
-        <v>297920989</v>
+        <v>298326830</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86861</v>
+        <v>86993</v>
       </c>
       <c r="D195" t="n">
-        <v>127329295</v>
+        <v>127522657</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33198</v>
+        <v>33246</v>
       </c>
       <c r="D198" t="n">
-        <v>47789043</v>
+        <v>47855799</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5121</v>
+        <v>5133</v>
       </c>
       <c r="D201" t="n">
-        <v>7290277</v>
+        <v>7308277</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4926</v>
+        <v>4954</v>
       </c>
       <c r="D204" t="n">
-        <v>6820989</v>
+        <v>6860923</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>265303</v>
+        <v>265735</v>
       </c>
       <c r="D207" t="n">
-        <v>328314392</v>
+        <v>328837164</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D210" t="n">
-        <v>22435</v>
+        <v>23935</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95461</v>
+        <v>95601</v>
       </c>
       <c r="D216" t="n">
-        <v>139656018</v>
+        <v>139859523</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51710</v>
+        <v>51798</v>
       </c>
       <c r="D219" t="n">
-        <v>74743148</v>
+        <v>74864968</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4684</v>
+        <v>4689</v>
       </c>
       <c r="D222" t="n">
-        <v>6577031</v>
+        <v>6584531</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5824</v>
+        <v>5866</v>
       </c>
       <c r="D225" t="n">
-        <v>8057434</v>
+        <v>8116077</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>106890</v>
+        <v>107072</v>
       </c>
       <c r="D228" t="n">
-        <v>133663492</v>
+        <v>133876653</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49670</v>
+        <v>49752</v>
       </c>
       <c r="D235" t="n">
-        <v>72762868</v>
+        <v>72882937</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12494</v>
+        <v>12534</v>
       </c>
       <c r="D237" t="n">
-        <v>17964997</v>
+        <v>18024997</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1896</v>
+        <v>1898</v>
       </c>
       <c r="D239" t="n">
-        <v>2717882</v>
+        <v>2720882</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2539</v>
+        <v>2555</v>
       </c>
       <c r="D241" t="n">
-        <v>3552972</v>
+        <v>3574909</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>259193</v>
+        <v>259630</v>
       </c>
       <c r="D242" t="n">
-        <v>327300068</v>
+        <v>327842062</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="D248" t="n">
-        <v>1223563</v>
+        <v>1226563</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96169</v>
+        <v>96316</v>
       </c>
       <c r="D250" t="n">
-        <v>140916287</v>
+        <v>141130937</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65459</v>
+        <v>65600</v>
       </c>
       <c r="D253" t="n">
-        <v>94866547</v>
+        <v>95068640</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2417</v>
+        <v>2419</v>
       </c>
       <c r="D255" t="n">
-        <v>3408238</v>
+        <v>3411238</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4656</v>
+        <v>4671</v>
       </c>
       <c r="D258" t="n">
-        <v>6541560</v>
+        <v>6563526</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-25 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>322974</v>
+        <v>323557</v>
       </c>
       <c r="D2" t="n">
-        <v>411573047</v>
+        <v>412295059</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D3" t="n">
-        <v>309979</v>
+        <v>311479</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D4" t="n">
-        <v>456707</v>
+        <v>461207</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="D8" t="n">
-        <v>1273795</v>
+        <v>1276795</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117562</v>
+        <v>117739</v>
       </c>
       <c r="D10" t="n">
-        <v>172259949</v>
+        <v>172518675</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59844</v>
+        <v>59972</v>
       </c>
       <c r="D12" t="n">
-        <v>86375361</v>
+        <v>86560844</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4012</v>
+        <v>4020</v>
       </c>
       <c r="D16" t="n">
-        <v>5693492</v>
+        <v>5704697</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6764</v>
+        <v>6799</v>
       </c>
       <c r="D20" t="n">
-        <v>9440454</v>
+        <v>9488900</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77998</v>
+        <v>78099</v>
       </c>
       <c r="D22" t="n">
-        <v>97219735</v>
+        <v>97341572</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D27" t="n">
-        <v>414647</v>
+        <v>416147</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32613</v>
+        <v>32646</v>
       </c>
       <c r="D28" t="n">
-        <v>47737942</v>
+        <v>47783310</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11544</v>
+        <v>11562</v>
       </c>
       <c r="D30" t="n">
-        <v>16607449</v>
+        <v>16630812</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1561</v>
+        <v>1563</v>
       </c>
       <c r="D33" t="n">
-        <v>2192807</v>
+        <v>2195781</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1852</v>
+        <v>1868</v>
       </c>
       <c r="D35" t="n">
-        <v>2615179</v>
+        <v>2637352</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>97732</v>
+        <v>97920</v>
       </c>
       <c r="D36" t="n">
-        <v>122958638</v>
+        <v>123186688</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44526</v>
+        <v>44579</v>
       </c>
       <c r="D44" t="n">
-        <v>65254435</v>
+        <v>65333498</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9197</v>
+        <v>9216</v>
       </c>
       <c r="D46" t="n">
-        <v>13196716</v>
+        <v>13223944</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="D48" t="n">
-        <v>1954603</v>
+        <v>1957603</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2340</v>
+        <v>2356</v>
       </c>
       <c r="D51" t="n">
-        <v>3268018</v>
+        <v>3291669</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69450</v>
+        <v>69580</v>
       </c>
       <c r="D52" t="n">
-        <v>87108726</v>
+        <v>87270642</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D54" t="n">
-        <v>60697</v>
+        <v>62197</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28316</v>
+        <v>28354</v>
       </c>
       <c r="D59" t="n">
-        <v>41525953</v>
+        <v>41582953</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11200</v>
+        <v>11218</v>
       </c>
       <c r="D62" t="n">
-        <v>16196623</v>
+        <v>16221284</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D64" t="n">
-        <v>1904737</v>
+        <v>1906237</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1494</v>
+        <v>1507</v>
       </c>
       <c r="D68" t="n">
-        <v>2093084</v>
+        <v>2112344</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20618</v>
+        <v>20657</v>
       </c>
       <c r="D70" t="n">
-        <v>27008207</v>
+        <v>27057267</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D71" t="n">
-        <v>42626</v>
+        <v>43781</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7624</v>
+        <v>7640</v>
       </c>
       <c r="D74" t="n">
-        <v>11164724</v>
+        <v>11187874</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5156</v>
+        <v>5161</v>
       </c>
       <c r="D76" t="n">
-        <v>7486610</v>
+        <v>7493563</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D78" t="n">
-        <v>393083</v>
+        <v>397583</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>141733</v>
+        <v>141957</v>
       </c>
       <c r="D79" t="n">
-        <v>176687278</v>
+        <v>176959291</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63803</v>
+        <v>63878</v>
       </c>
       <c r="D85" t="n">
-        <v>93512484</v>
+        <v>93622032</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29907</v>
+        <v>29961</v>
       </c>
       <c r="D88" t="n">
-        <v>43265941</v>
+        <v>43341861</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2737</v>
+        <v>2741</v>
       </c>
       <c r="D90" t="n">
-        <v>3940857</v>
+        <v>3945957</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2868</v>
+        <v>2883</v>
       </c>
       <c r="D91" t="n">
-        <v>4056084</v>
+        <v>4075360</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33483</v>
+        <v>33593</v>
       </c>
       <c r="D92" t="n">
-        <v>45379530</v>
+        <v>45527970</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D95" t="n">
-        <v>40314</v>
+        <v>43314</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8106</v>
+        <v>8135</v>
       </c>
       <c r="D96" t="n">
-        <v>11918050</v>
+        <v>11960834</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7458</v>
+        <v>7485</v>
       </c>
       <c r="D98" t="n">
-        <v>10822367</v>
+        <v>10862221</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D100" t="n">
-        <v>763651</v>
+        <v>765151</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D101" t="n">
-        <v>719891</v>
+        <v>721391</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10197</v>
+        <v>10343</v>
       </c>
       <c r="D102" t="n">
-        <v>15394555</v>
+        <v>15715707</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2537</v>
+        <v>2558</v>
       </c>
       <c r="D104" t="n">
-        <v>4100088</v>
+        <v>4157088</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3413</v>
+        <v>3455</v>
       </c>
       <c r="D106" t="n">
-        <v>5504979</v>
+        <v>5607959</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D108" t="n">
-        <v>256445</v>
+        <v>262445</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D109" t="n">
-        <v>298032</v>
+        <v>308030</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>142418</v>
+        <v>142655</v>
       </c>
       <c r="D110" t="n">
-        <v>176119579</v>
+        <v>176406032</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>52971</v>
+        <v>53045</v>
       </c>
       <c r="D116" t="n">
-        <v>77645580</v>
+        <v>77751453</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27303</v>
+        <v>27366</v>
       </c>
       <c r="D118" t="n">
-        <v>39560507</v>
+        <v>39650941</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="D119" t="n">
-        <v>1795784</v>
+        <v>1797981</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2294</v>
+        <v>2300</v>
       </c>
       <c r="D122" t="n">
-        <v>3222668</v>
+        <v>3231668</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>518530</v>
+        <v>520045</v>
       </c>
       <c r="D124" t="n">
-        <v>684872080</v>
+        <v>686874241</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D125" t="n">
-        <v>120789</v>
+        <v>122289</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D126" t="n">
-        <v>316509</v>
+        <v>318009</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1382</v>
+        <v>1385</v>
       </c>
       <c r="D129" t="n">
-        <v>2048486</v>
+        <v>2052682</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>209555</v>
+        <v>210034</v>
       </c>
       <c r="D131" t="n">
-        <v>308059771</v>
+        <v>308763592</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D132" t="n">
-        <v>604250</v>
+        <v>607250</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>184904</v>
+        <v>185500</v>
       </c>
       <c r="D134" t="n">
-        <v>268890806</v>
+        <v>269759855</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2856</v>
+        <v>2858</v>
       </c>
       <c r="D137" t="n">
-        <v>4011969</v>
+        <v>4014969</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6453</v>
+        <v>6487</v>
       </c>
       <c r="D139" t="n">
-        <v>9117366</v>
+        <v>9165314</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D140" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>45019</v>
+        <v>45125</v>
       </c>
       <c r="D142" t="n">
-        <v>60106966</v>
+        <v>60248831</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14162</v>
+        <v>14180</v>
       </c>
       <c r="D148" t="n">
-        <v>20764513</v>
+        <v>20790133</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3794</v>
+        <v>3800</v>
       </c>
       <c r="D149" t="n">
-        <v>5471002</v>
+        <v>5480002</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D152" t="n">
-        <v>578216</v>
+        <v>579716</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D154" t="n">
-        <v>552263</v>
+        <v>555263</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17748</v>
+        <v>17798</v>
       </c>
       <c r="D155" t="n">
-        <v>23460996</v>
+        <v>23523618</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7236</v>
+        <v>7255</v>
       </c>
       <c r="D159" t="n">
-        <v>10526263</v>
+        <v>10555975</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5054</v>
+        <v>5065</v>
       </c>
       <c r="D161" t="n">
-        <v>7274629</v>
+        <v>7289996</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D164" t="n">
-        <v>386364</v>
+        <v>387864</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18252</v>
+        <v>18440</v>
       </c>
       <c r="D166" t="n">
-        <v>29420621</v>
+        <v>29888219</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1996</v>
+        <v>2013</v>
       </c>
       <c r="D167" t="n">
-        <v>3244449</v>
+        <v>3283349</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D168" t="n">
-        <v>430101</v>
+        <v>448101</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D170" t="n">
-        <v>107690</v>
+        <v>110690</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88331</v>
+        <v>88486</v>
       </c>
       <c r="D172" t="n">
-        <v>110425175</v>
+        <v>110603462</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D177" t="n">
-        <v>946348</v>
+        <v>949348</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>34007</v>
+        <v>34081</v>
       </c>
       <c r="D179" t="n">
-        <v>49872577</v>
+        <v>49977954</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13117</v>
+        <v>13149</v>
       </c>
       <c r="D181" t="n">
-        <v>18954462</v>
+        <v>18998582</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1247</v>
+        <v>1250</v>
       </c>
       <c r="D183" t="n">
-        <v>1745429</v>
+        <v>1749929</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1677</v>
+        <v>1685</v>
       </c>
       <c r="D185" t="n">
-        <v>2357296</v>
+        <v>2368656</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>240028</v>
+        <v>240306</v>
       </c>
       <c r="D187" t="n">
-        <v>298326830</v>
+        <v>298655698</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>86993</v>
+        <v>87077</v>
       </c>
       <c r="D195" t="n">
-        <v>127522657</v>
+        <v>127641359</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D196" t="n">
-        <v>136627</v>
+        <v>139627</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33246</v>
+        <v>33297</v>
       </c>
       <c r="D198" t="n">
-        <v>47855799</v>
+        <v>47930691</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5133</v>
+        <v>5140</v>
       </c>
       <c r="D201" t="n">
-        <v>7308277</v>
+        <v>7318777</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4954</v>
+        <v>4977</v>
       </c>
       <c r="D204" t="n">
-        <v>6860923</v>
+        <v>6891752</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>265735</v>
+        <v>266156</v>
       </c>
       <c r="D207" t="n">
-        <v>328837164</v>
+        <v>329359127</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D214" t="n">
-        <v>898378</v>
+        <v>901378</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95601</v>
+        <v>95715</v>
       </c>
       <c r="D216" t="n">
-        <v>139859523</v>
+        <v>140026640</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51798</v>
+        <v>51899</v>
       </c>
       <c r="D219" t="n">
-        <v>74864968</v>
+        <v>75010453</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4689</v>
+        <v>4695</v>
       </c>
       <c r="D222" t="n">
-        <v>6584531</v>
+        <v>6592244</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5866</v>
+        <v>5887</v>
       </c>
       <c r="D225" t="n">
-        <v>8116077</v>
+        <v>8146147</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>107072</v>
+        <v>107233</v>
       </c>
       <c r="D228" t="n">
-        <v>133876653</v>
+        <v>134065891</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D229" t="n">
-        <v>79164</v>
+        <v>80550</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D233" t="n">
-        <v>826939</v>
+        <v>828439</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49752</v>
+        <v>49818</v>
       </c>
       <c r="D235" t="n">
-        <v>72882937</v>
+        <v>72980383</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D236" t="n">
-        <v>48711</v>
+        <v>50211</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12534</v>
+        <v>12554</v>
       </c>
       <c r="D237" t="n">
-        <v>18024997</v>
+        <v>18051518</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2555</v>
+        <v>2564</v>
       </c>
       <c r="D241" t="n">
-        <v>3574909</v>
+        <v>3586686</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>259630</v>
+        <v>260123</v>
       </c>
       <c r="D242" t="n">
-        <v>327842062</v>
+        <v>328463035</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D247" t="n">
-        <v>15980</v>
+        <v>17480</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96316</v>
+        <v>96443</v>
       </c>
       <c r="D250" t="n">
-        <v>141130937</v>
+        <v>141312865</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65600</v>
+        <v>65731</v>
       </c>
       <c r="D253" t="n">
-        <v>95068640</v>
+        <v>95259938</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2419</v>
+        <v>2422</v>
       </c>
       <c r="D255" t="n">
-        <v>3411238</v>
+        <v>3414819</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4671</v>
+        <v>4697</v>
       </c>
       <c r="D258" t="n">
-        <v>6563526</v>
+        <v>6600605</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-26 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>323557</v>
+        <v>324074</v>
       </c>
       <c r="D2" t="n">
-        <v>412295059</v>
+        <v>412922472</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D3" t="n">
-        <v>311479</v>
+        <v>311952</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D4" t="n">
-        <v>461207</v>
+        <v>464207</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D8" t="n">
-        <v>1276795</v>
+        <v>1278295</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117739</v>
+        <v>117874</v>
       </c>
       <c r="D10" t="n">
-        <v>172518675</v>
+        <v>172715765</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59972</v>
+        <v>60069</v>
       </c>
       <c r="D12" t="n">
-        <v>86560844</v>
+        <v>86696408</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4020</v>
+        <v>4025</v>
       </c>
       <c r="D16" t="n">
-        <v>5704697</v>
+        <v>5712197</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6799</v>
+        <v>6830</v>
       </c>
       <c r="D20" t="n">
-        <v>9488900</v>
+        <v>9533037</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78099</v>
+        <v>78190</v>
       </c>
       <c r="D22" t="n">
-        <v>97341572</v>
+        <v>97445489</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32646</v>
+        <v>32667</v>
       </c>
       <c r="D28" t="n">
-        <v>47783310</v>
+        <v>47814776</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11562</v>
+        <v>11577</v>
       </c>
       <c r="D30" t="n">
-        <v>16630812</v>
+        <v>16653312</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D33" t="n">
-        <v>2195781</v>
+        <v>2197281</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1868</v>
+        <v>1880</v>
       </c>
       <c r="D35" t="n">
-        <v>2637352</v>
+        <v>2655168</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>97920</v>
+        <v>98050</v>
       </c>
       <c r="D36" t="n">
-        <v>123186688</v>
+        <v>123337544</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44579</v>
+        <v>44611</v>
       </c>
       <c r="D44" t="n">
-        <v>65333498</v>
+        <v>65380019</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9216</v>
+        <v>9231</v>
       </c>
       <c r="D46" t="n">
-        <v>13223944</v>
+        <v>13243911</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1410</v>
+        <v>1414</v>
       </c>
       <c r="D48" t="n">
-        <v>1957603</v>
+        <v>1963603</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2356</v>
+        <v>2375</v>
       </c>
       <c r="D51" t="n">
-        <v>3291669</v>
+        <v>3317952</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69580</v>
+        <v>69681</v>
       </c>
       <c r="D52" t="n">
-        <v>87270642</v>
+        <v>87396051</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28354</v>
+        <v>28380</v>
       </c>
       <c r="D59" t="n">
-        <v>41582953</v>
+        <v>41621428</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11218</v>
+        <v>11236</v>
       </c>
       <c r="D62" t="n">
-        <v>16221284</v>
+        <v>16247212</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D64" t="n">
-        <v>1906237</v>
+        <v>1907737</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1507</v>
+        <v>1514</v>
       </c>
       <c r="D68" t="n">
-        <v>2112344</v>
+        <v>2122704</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20657</v>
+        <v>20678</v>
       </c>
       <c r="D70" t="n">
-        <v>27057267</v>
+        <v>27080493</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7640</v>
+        <v>7655</v>
       </c>
       <c r="D74" t="n">
-        <v>11187874</v>
+        <v>11210276</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5161</v>
+        <v>5168</v>
       </c>
       <c r="D76" t="n">
-        <v>7493563</v>
+        <v>7504063</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D78" t="n">
-        <v>397583</v>
+        <v>399083</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>141957</v>
+        <v>142179</v>
       </c>
       <c r="D79" t="n">
-        <v>176959291</v>
+        <v>177218222</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D83" t="n">
-        <v>627824</v>
+        <v>629324</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63878</v>
+        <v>63966</v>
       </c>
       <c r="D85" t="n">
-        <v>93622032</v>
+        <v>93751771</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>29961</v>
+        <v>30008</v>
       </c>
       <c r="D88" t="n">
-        <v>43341861</v>
+        <v>43406845</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2741</v>
+        <v>2746</v>
       </c>
       <c r="D90" t="n">
-        <v>3945957</v>
+        <v>3953457</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2883</v>
+        <v>2893</v>
       </c>
       <c r="D91" t="n">
-        <v>4075360</v>
+        <v>4090360</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33593</v>
+        <v>33679</v>
       </c>
       <c r="D92" t="n">
-        <v>45527970</v>
+        <v>45646991</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8135</v>
+        <v>8158</v>
       </c>
       <c r="D96" t="n">
-        <v>11960834</v>
+        <v>11994580</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7485</v>
+        <v>7509</v>
       </c>
       <c r="D98" t="n">
-        <v>10862221</v>
+        <v>10893587</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D101" t="n">
-        <v>721391</v>
+        <v>722891</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10343</v>
+        <v>10434</v>
       </c>
       <c r="D102" t="n">
-        <v>15715707</v>
+        <v>15915355</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2558</v>
+        <v>2573</v>
       </c>
       <c r="D104" t="n">
-        <v>4157088</v>
+        <v>4195321</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3455</v>
+        <v>3478</v>
       </c>
       <c r="D106" t="n">
-        <v>5607959</v>
+        <v>5664690</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>142655</v>
+        <v>142860</v>
       </c>
       <c r="D110" t="n">
-        <v>176406032</v>
+        <v>176655196</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53045</v>
+        <v>53104</v>
       </c>
       <c r="D116" t="n">
-        <v>77751453</v>
+        <v>77837043</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27366</v>
+        <v>27413</v>
       </c>
       <c r="D118" t="n">
-        <v>39650941</v>
+        <v>39719852</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="D119" t="n">
-        <v>1797981</v>
+        <v>1800981</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2300</v>
+        <v>2317</v>
       </c>
       <c r="D122" t="n">
-        <v>3231668</v>
+        <v>3257168</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>520045</v>
+        <v>521312</v>
       </c>
       <c r="D124" t="n">
-        <v>686874241</v>
+        <v>688532394</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D126" t="n">
-        <v>318009</v>
+        <v>321009</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D129" t="n">
-        <v>2052682</v>
+        <v>2054182</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>210034</v>
+        <v>210405</v>
       </c>
       <c r="D131" t="n">
-        <v>308763592</v>
+        <v>309309006</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>185500</v>
+        <v>185957</v>
       </c>
       <c r="D134" t="n">
-        <v>269759855</v>
+        <v>270422504</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2858</v>
+        <v>2863</v>
       </c>
       <c r="D137" t="n">
-        <v>4014969</v>
+        <v>4021893</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6487</v>
+        <v>6517</v>
       </c>
       <c r="D139" t="n">
-        <v>9165314</v>
+        <v>9208214</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>45125</v>
+        <v>45222</v>
       </c>
       <c r="D142" t="n">
-        <v>60248831</v>
+        <v>60373149</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14180</v>
+        <v>14209</v>
       </c>
       <c r="D148" t="n">
-        <v>20790133</v>
+        <v>20831928</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3800</v>
+        <v>3804</v>
       </c>
       <c r="D149" t="n">
-        <v>5480002</v>
+        <v>5485240</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D152" t="n">
-        <v>579716</v>
+        <v>581216</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D154" t="n">
-        <v>555263</v>
+        <v>558263</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17798</v>
+        <v>17825</v>
       </c>
       <c r="D155" t="n">
-        <v>23523618</v>
+        <v>23559950</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7255</v>
+        <v>7275</v>
       </c>
       <c r="D159" t="n">
-        <v>10555975</v>
+        <v>10585075</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5065</v>
+        <v>5074</v>
       </c>
       <c r="D161" t="n">
-        <v>7289996</v>
+        <v>7303496</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18440</v>
+        <v>18533</v>
       </c>
       <c r="D166" t="n">
-        <v>29888219</v>
+        <v>30115202</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2013</v>
+        <v>2030</v>
       </c>
       <c r="D167" t="n">
-        <v>3283349</v>
+        <v>3326572</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88486</v>
+        <v>88621</v>
       </c>
       <c r="D172" t="n">
-        <v>110603462</v>
+        <v>110760198</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>34081</v>
+        <v>34116</v>
       </c>
       <c r="D179" t="n">
-        <v>49977954</v>
+        <v>50026949</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13149</v>
+        <v>13168</v>
       </c>
       <c r="D181" t="n">
-        <v>18998582</v>
+        <v>19024845</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1685</v>
+        <v>1692</v>
       </c>
       <c r="D185" t="n">
-        <v>2368656</v>
+        <v>2378192</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>240306</v>
+        <v>240589</v>
       </c>
       <c r="D187" t="n">
-        <v>298655698</v>
+        <v>298985378</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D189" t="n">
-        <v>242236</v>
+        <v>243736</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>87077</v>
+        <v>87174</v>
       </c>
       <c r="D195" t="n">
-        <v>127641359</v>
+        <v>127783392</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33297</v>
+        <v>33330</v>
       </c>
       <c r="D198" t="n">
-        <v>47930691</v>
+        <v>47979310</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5140</v>
+        <v>5150</v>
       </c>
       <c r="D201" t="n">
-        <v>7318777</v>
+        <v>7333077</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>4977</v>
+        <v>5002</v>
       </c>
       <c r="D204" t="n">
-        <v>6891752</v>
+        <v>6927484</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>266156</v>
+        <v>266535</v>
       </c>
       <c r="D207" t="n">
-        <v>329359127</v>
+        <v>329806749</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D208" t="n">
-        <v>174913</v>
+        <v>176413</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D209" t="n">
-        <v>365087</v>
+        <v>365539</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D214" t="n">
-        <v>901378</v>
+        <v>902878</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95715</v>
+        <v>95808</v>
       </c>
       <c r="D216" t="n">
-        <v>140026640</v>
+        <v>140163257</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D217" t="n">
-        <v>134199</v>
+        <v>135699</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51899</v>
+        <v>51981</v>
       </c>
       <c r="D219" t="n">
-        <v>75010453</v>
+        <v>75127469</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4695</v>
+        <v>4702</v>
       </c>
       <c r="D222" t="n">
-        <v>6592244</v>
+        <v>6600691</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5887</v>
+        <v>5916</v>
       </c>
       <c r="D225" t="n">
-        <v>8146147</v>
+        <v>8189397</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>107233</v>
+        <v>107378</v>
       </c>
       <c r="D228" t="n">
-        <v>134065891</v>
+        <v>134233300</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49818</v>
+        <v>49860</v>
       </c>
       <c r="D235" t="n">
-        <v>72980383</v>
+        <v>73039747</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12554</v>
+        <v>12582</v>
       </c>
       <c r="D237" t="n">
-        <v>18051518</v>
+        <v>18089606</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1898</v>
+        <v>1901</v>
       </c>
       <c r="D239" t="n">
-        <v>2720882</v>
+        <v>2725382</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2564</v>
+        <v>2576</v>
       </c>
       <c r="D241" t="n">
-        <v>3586686</v>
+        <v>3604686</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>260123</v>
+        <v>260526</v>
       </c>
       <c r="D242" t="n">
-        <v>328463035</v>
+        <v>328954344</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="D248" t="n">
-        <v>1226563</v>
+        <v>1227404</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96443</v>
+        <v>96556</v>
       </c>
       <c r="D250" t="n">
-        <v>141312865</v>
+        <v>141480229</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65731</v>
+        <v>65842</v>
       </c>
       <c r="D253" t="n">
-        <v>95259938</v>
+        <v>95419882</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2422</v>
+        <v>2426</v>
       </c>
       <c r="D255" t="n">
-        <v>3414819</v>
+        <v>3420273</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4697</v>
+        <v>4715</v>
       </c>
       <c r="D258" t="n">
-        <v>6600605</v>
+        <v>6626760</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-27 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>324074</v>
+        <v>324535</v>
       </c>
       <c r="D2" t="n">
-        <v>412922472</v>
+        <v>413482458</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D4" t="n">
-        <v>464207</v>
+        <v>467692</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117874</v>
+        <v>118013</v>
       </c>
       <c r="D10" t="n">
-        <v>172715765</v>
+        <v>172917118</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60069</v>
+        <v>60152</v>
       </c>
       <c r="D12" t="n">
-        <v>86696408</v>
+        <v>86814505</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4025</v>
+        <v>4027</v>
       </c>
       <c r="D16" t="n">
-        <v>5712197</v>
+        <v>5715197</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6830</v>
+        <v>6863</v>
       </c>
       <c r="D20" t="n">
-        <v>9533037</v>
+        <v>9580704</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78190</v>
+        <v>78268</v>
       </c>
       <c r="D22" t="n">
-        <v>97445489</v>
+        <v>97545640</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32667</v>
+        <v>32688</v>
       </c>
       <c r="D28" t="n">
-        <v>47814776</v>
+        <v>47844999</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11577</v>
+        <v>11583</v>
       </c>
       <c r="D30" t="n">
-        <v>16653312</v>
+        <v>16661747</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1564</v>
+        <v>1568</v>
       </c>
       <c r="D33" t="n">
-        <v>2197281</v>
+        <v>2203281</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D34" t="n">
-        <v>19184</v>
+        <v>20684</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1880</v>
+        <v>1890</v>
       </c>
       <c r="D35" t="n">
-        <v>2655168</v>
+        <v>2670168</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98050</v>
+        <v>98146</v>
       </c>
       <c r="D36" t="n">
-        <v>123337544</v>
+        <v>123446064</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44611</v>
+        <v>44651</v>
       </c>
       <c r="D44" t="n">
-        <v>65380019</v>
+        <v>65437560</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9231</v>
+        <v>9245</v>
       </c>
       <c r="D46" t="n">
-        <v>13243911</v>
+        <v>13261108</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1414</v>
+        <v>1416</v>
       </c>
       <c r="D48" t="n">
-        <v>1963603</v>
+        <v>1966603</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2375</v>
+        <v>2393</v>
       </c>
       <c r="D51" t="n">
-        <v>3317952</v>
+        <v>3343402</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69681</v>
+        <v>69764</v>
       </c>
       <c r="D52" t="n">
-        <v>87396051</v>
+        <v>87497943</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28380</v>
+        <v>28415</v>
       </c>
       <c r="D59" t="n">
-        <v>41621428</v>
+        <v>41670204</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11236</v>
+        <v>11252</v>
       </c>
       <c r="D62" t="n">
-        <v>16247212</v>
+        <v>16271212</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D64" t="n">
-        <v>1907737</v>
+        <v>1909237</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1514</v>
+        <v>1526</v>
       </c>
       <c r="D68" t="n">
-        <v>2122704</v>
+        <v>2138114</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20678</v>
+        <v>20699</v>
       </c>
       <c r="D70" t="n">
-        <v>27080493</v>
+        <v>27107108</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7655</v>
+        <v>7660</v>
       </c>
       <c r="D74" t="n">
-        <v>11210276</v>
+        <v>11216856</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5168</v>
+        <v>5177</v>
       </c>
       <c r="D76" t="n">
-        <v>7504063</v>
+        <v>7517372</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D78" t="n">
-        <v>399083</v>
+        <v>400583</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>142179</v>
+        <v>142338</v>
       </c>
       <c r="D79" t="n">
-        <v>177218222</v>
+        <v>177403150</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>63966</v>
+        <v>64050</v>
       </c>
       <c r="D85" t="n">
-        <v>93751771</v>
+        <v>93870725</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30008</v>
+        <v>30047</v>
       </c>
       <c r="D88" t="n">
-        <v>43406845</v>
+        <v>43464983</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2746</v>
+        <v>2753</v>
       </c>
       <c r="D90" t="n">
-        <v>3953457</v>
+        <v>3963957</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2893</v>
+        <v>2902</v>
       </c>
       <c r="D91" t="n">
-        <v>4090360</v>
+        <v>4103847</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33679</v>
+        <v>33775</v>
       </c>
       <c r="D92" t="n">
-        <v>45646991</v>
+        <v>45777271</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8158</v>
+        <v>8196</v>
       </c>
       <c r="D96" t="n">
-        <v>11994580</v>
+        <v>12048402</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7509</v>
+        <v>7531</v>
       </c>
       <c r="D98" t="n">
-        <v>10893587</v>
+        <v>10926568</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D100" t="n">
-        <v>765151</v>
+        <v>766651</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D101" t="n">
-        <v>722891</v>
+        <v>725891</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10434</v>
+        <v>10515</v>
       </c>
       <c r="D102" t="n">
-        <v>15915355</v>
+        <v>16096474</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2573</v>
+        <v>2586</v>
       </c>
       <c r="D104" t="n">
-        <v>4195321</v>
+        <v>4228621</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3478</v>
+        <v>3504</v>
       </c>
       <c r="D106" t="n">
-        <v>5664690</v>
+        <v>5735573</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D108" t="n">
-        <v>262445</v>
+        <v>265445</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D109" t="n">
-        <v>308030</v>
+        <v>318530</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>142860</v>
+        <v>143033</v>
       </c>
       <c r="D110" t="n">
-        <v>176655196</v>
+        <v>176863546</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D113" t="n">
-        <v>8895</v>
+        <v>10395</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53104</v>
+        <v>53156</v>
       </c>
       <c r="D116" t="n">
-        <v>77837043</v>
+        <v>77912310</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D117" t="n">
-        <v>125959</v>
+        <v>127459</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27413</v>
+        <v>27466</v>
       </c>
       <c r="D118" t="n">
-        <v>39719852</v>
+        <v>39794034</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2317</v>
+        <v>2320</v>
       </c>
       <c r="D122" t="n">
-        <v>3257168</v>
+        <v>3260509</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>521312</v>
+        <v>522361</v>
       </c>
       <c r="D124" t="n">
-        <v>688532394</v>
+        <v>689896786</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1386</v>
+        <v>1388</v>
       </c>
       <c r="D129" t="n">
-        <v>2054182</v>
+        <v>2057182</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>210405</v>
+        <v>210770</v>
       </c>
       <c r="D131" t="n">
-        <v>309309006</v>
+        <v>309844471</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D132" t="n">
-        <v>607250</v>
+        <v>611750</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>185957</v>
+        <v>186400</v>
       </c>
       <c r="D134" t="n">
-        <v>270422504</v>
+        <v>271064958</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D136" t="n">
-        <v>46832</v>
+        <v>48332</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2863</v>
+        <v>2872</v>
       </c>
       <c r="D137" t="n">
-        <v>4021893</v>
+        <v>4032799</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6517</v>
+        <v>6538</v>
       </c>
       <c r="D139" t="n">
-        <v>9208214</v>
+        <v>9236919</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>45222</v>
+        <v>45326</v>
       </c>
       <c r="D142" t="n">
-        <v>60373149</v>
+        <v>60507242</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14209</v>
+        <v>14229</v>
       </c>
       <c r="D148" t="n">
-        <v>20831928</v>
+        <v>20861738</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3804</v>
+        <v>3808</v>
       </c>
       <c r="D149" t="n">
-        <v>5485240</v>
+        <v>5491240</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D154" t="n">
-        <v>558263</v>
+        <v>559763</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17825</v>
+        <v>17861</v>
       </c>
       <c r="D155" t="n">
-        <v>23559950</v>
+        <v>23606905</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7275</v>
+        <v>7285</v>
       </c>
       <c r="D159" t="n">
-        <v>10585075</v>
+        <v>10599404</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5074</v>
+        <v>5082</v>
       </c>
       <c r="D161" t="n">
-        <v>7303496</v>
+        <v>7315496</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D164" t="n">
-        <v>387864</v>
+        <v>389364</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18533</v>
+        <v>18714</v>
       </c>
       <c r="D166" t="n">
-        <v>30115202</v>
+        <v>30538370</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2030</v>
+        <v>2044</v>
       </c>
       <c r="D167" t="n">
-        <v>3326572</v>
+        <v>3361072</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D168" t="n">
-        <v>448101</v>
+        <v>454589</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D171" t="n">
-        <v>160449</v>
+        <v>181449</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88621</v>
+        <v>88709</v>
       </c>
       <c r="D172" t="n">
-        <v>110760198</v>
+        <v>110866653</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D177" t="n">
-        <v>949348</v>
+        <v>950588</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>34116</v>
+        <v>34138</v>
       </c>
       <c r="D179" t="n">
-        <v>50026949</v>
+        <v>50059477</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13168</v>
+        <v>13180</v>
       </c>
       <c r="D181" t="n">
-        <v>19024845</v>
+        <v>19042845</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D183" t="n">
-        <v>1749929</v>
+        <v>1751429</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1692</v>
+        <v>1700</v>
       </c>
       <c r="D185" t="n">
-        <v>2378192</v>
+        <v>2389005</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>240589</v>
+        <v>240882</v>
       </c>
       <c r="D187" t="n">
-        <v>298985378</v>
+        <v>299325312</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D189" t="n">
-        <v>243736</v>
+        <v>245236</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="D193" t="n">
-        <v>1297345</v>
+        <v>1298845</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>87174</v>
+        <v>87253</v>
       </c>
       <c r="D195" t="n">
-        <v>127783392</v>
+        <v>127897857</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33330</v>
+        <v>33367</v>
       </c>
       <c r="D198" t="n">
-        <v>47979310</v>
+        <v>48032595</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5150</v>
+        <v>5156</v>
       </c>
       <c r="D201" t="n">
-        <v>7333077</v>
+        <v>7339796</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5002</v>
+        <v>5017</v>
       </c>
       <c r="D204" t="n">
-        <v>6927484</v>
+        <v>6947378</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>266535</v>
+        <v>266897</v>
       </c>
       <c r="D207" t="n">
-        <v>329806749</v>
+        <v>330258895</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D209" t="n">
-        <v>365539</v>
+        <v>367039</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D214" t="n">
-        <v>902878</v>
+        <v>904378</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95808</v>
+        <v>95937</v>
       </c>
       <c r="D216" t="n">
-        <v>140163257</v>
+        <v>140349246</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>51981</v>
+        <v>52066</v>
       </c>
       <c r="D219" t="n">
-        <v>75127469</v>
+        <v>75250062</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4702</v>
+        <v>4709</v>
       </c>
       <c r="D222" t="n">
-        <v>6600691</v>
+        <v>6609823</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5916</v>
+        <v>5950</v>
       </c>
       <c r="D225" t="n">
-        <v>8189397</v>
+        <v>8236605</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>107378</v>
+        <v>107504</v>
       </c>
       <c r="D228" t="n">
-        <v>134233300</v>
+        <v>134392646</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49860</v>
+        <v>49912</v>
       </c>
       <c r="D235" t="n">
-        <v>73039747</v>
+        <v>73117543</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12582</v>
+        <v>12608</v>
       </c>
       <c r="D237" t="n">
-        <v>18089606</v>
+        <v>18127904</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="D239" t="n">
-        <v>2725382</v>
+        <v>2726882</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2576</v>
+        <v>2586</v>
       </c>
       <c r="D241" t="n">
-        <v>3604686</v>
+        <v>3619686</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>260526</v>
+        <v>260873</v>
       </c>
       <c r="D242" t="n">
-        <v>328954344</v>
+        <v>329377272</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D246" t="n">
-        <v>22500</v>
+        <v>24000</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="D248" t="n">
-        <v>1227404</v>
+        <v>1228904</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96556</v>
+        <v>96661</v>
       </c>
       <c r="D250" t="n">
-        <v>141480229</v>
+        <v>141635122</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65842</v>
+        <v>65973</v>
       </c>
       <c r="D253" t="n">
-        <v>95419882</v>
+        <v>95608796</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2426</v>
+        <v>2431</v>
       </c>
       <c r="D255" t="n">
-        <v>3420273</v>
+        <v>3427773</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4715</v>
+        <v>4748</v>
       </c>
       <c r="D258" t="n">
-        <v>6626760</v>
+        <v>6673279</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-28 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>324535</v>
+        <v>324987</v>
       </c>
       <c r="D2" t="n">
-        <v>413482458</v>
+        <v>414031423</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D3" t="n">
-        <v>311952</v>
+        <v>313452</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D8" t="n">
-        <v>1278295</v>
+        <v>1279795</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>118013</v>
+        <v>118155</v>
       </c>
       <c r="D10" t="n">
-        <v>172917118</v>
+        <v>173121141</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60152</v>
+        <v>60245</v>
       </c>
       <c r="D12" t="n">
-        <v>86814505</v>
+        <v>86947766</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4027</v>
+        <v>4031</v>
       </c>
       <c r="D16" t="n">
-        <v>5715197</v>
+        <v>5721197</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6863</v>
+        <v>6885</v>
       </c>
       <c r="D20" t="n">
-        <v>9580704</v>
+        <v>9610848</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78268</v>
+        <v>78348</v>
       </c>
       <c r="D22" t="n">
-        <v>97545640</v>
+        <v>97636176</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32688</v>
+        <v>32723</v>
       </c>
       <c r="D28" t="n">
-        <v>47844999</v>
+        <v>47895791</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11583</v>
+        <v>11600</v>
       </c>
       <c r="D30" t="n">
-        <v>16661747</v>
+        <v>16686097</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D33" t="n">
-        <v>2203281</v>
+        <v>2204781</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1890</v>
+        <v>1892</v>
       </c>
       <c r="D35" t="n">
-        <v>2670168</v>
+        <v>2673168</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98146</v>
+        <v>98240</v>
       </c>
       <c r="D36" t="n">
-        <v>123446064</v>
+        <v>123565614</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44651</v>
+        <v>44695</v>
       </c>
       <c r="D44" t="n">
-        <v>65437560</v>
+        <v>65501066</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9245</v>
+        <v>9255</v>
       </c>
       <c r="D46" t="n">
-        <v>13261108</v>
+        <v>13276108</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1416</v>
+        <v>1418</v>
       </c>
       <c r="D48" t="n">
-        <v>1966603</v>
+        <v>1969311</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2393</v>
+        <v>2407</v>
       </c>
       <c r="D51" t="n">
-        <v>3343402</v>
+        <v>3363848</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69764</v>
+        <v>69835</v>
       </c>
       <c r="D52" t="n">
-        <v>87497943</v>
+        <v>87585741</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28415</v>
+        <v>28446</v>
       </c>
       <c r="D59" t="n">
-        <v>41670204</v>
+        <v>41716704</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11252</v>
+        <v>11262</v>
       </c>
       <c r="D62" t="n">
-        <v>16271212</v>
+        <v>16285835</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1526</v>
+        <v>1531</v>
       </c>
       <c r="D68" t="n">
-        <v>2138114</v>
+        <v>2144417</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20699</v>
+        <v>20715</v>
       </c>
       <c r="D70" t="n">
-        <v>27107108</v>
+        <v>27127758</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7660</v>
+        <v>7669</v>
       </c>
       <c r="D74" t="n">
-        <v>11216856</v>
+        <v>11230356</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5177</v>
+        <v>5186</v>
       </c>
       <c r="D76" t="n">
-        <v>7517372</v>
+        <v>7529986</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>142338</v>
+        <v>142532</v>
       </c>
       <c r="D79" t="n">
-        <v>177403150</v>
+        <v>177627259</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64050</v>
+        <v>64128</v>
       </c>
       <c r="D85" t="n">
-        <v>93870725</v>
+        <v>93984195</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D86" t="n">
-        <v>120082</v>
+        <v>121582</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30047</v>
+        <v>30089</v>
       </c>
       <c r="D88" t="n">
-        <v>43464983</v>
+        <v>43524018</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2753</v>
+        <v>2755</v>
       </c>
       <c r="D90" t="n">
-        <v>3963957</v>
+        <v>3966957</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2902</v>
+        <v>2917</v>
       </c>
       <c r="D91" t="n">
-        <v>4103847</v>
+        <v>4124547</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33775</v>
+        <v>33857</v>
       </c>
       <c r="D92" t="n">
-        <v>45777271</v>
+        <v>45886126</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8196</v>
+        <v>8212</v>
       </c>
       <c r="D96" t="n">
-        <v>12048402</v>
+        <v>12072127</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7531</v>
+        <v>7549</v>
       </c>
       <c r="D98" t="n">
-        <v>10926568</v>
+        <v>10951980</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="D100" t="n">
-        <v>766651</v>
+        <v>771135</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10515</v>
+        <v>10635</v>
       </c>
       <c r="D102" t="n">
-        <v>16096474</v>
+        <v>16360661</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2586</v>
+        <v>2610</v>
       </c>
       <c r="D104" t="n">
-        <v>4228621</v>
+        <v>4285676</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3504</v>
+        <v>3539</v>
       </c>
       <c r="D106" t="n">
-        <v>5735573</v>
+        <v>5817151</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D109" t="n">
-        <v>318530</v>
+        <v>326860</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>143033</v>
+        <v>143179</v>
       </c>
       <c r="D110" t="n">
-        <v>176863546</v>
+        <v>177042076</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="D114" t="n">
-        <v>1395536</v>
+        <v>1399477</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53156</v>
+        <v>53212</v>
       </c>
       <c r="D116" t="n">
-        <v>77912310</v>
+        <v>77990734</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27466</v>
+        <v>27495</v>
       </c>
       <c r="D118" t="n">
-        <v>39794034</v>
+        <v>39835838</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2320</v>
+        <v>2328</v>
       </c>
       <c r="D122" t="n">
-        <v>3260509</v>
+        <v>3270699</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>522361</v>
+        <v>523430</v>
       </c>
       <c r="D124" t="n">
-        <v>689896786</v>
+        <v>691300140</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D126" t="n">
-        <v>321009</v>
+        <v>322509</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1388</v>
+        <v>1391</v>
       </c>
       <c r="D129" t="n">
-        <v>2057182</v>
+        <v>2061682</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>210770</v>
+        <v>211149</v>
       </c>
       <c r="D131" t="n">
-        <v>309844471</v>
+        <v>310392931</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D132" t="n">
-        <v>611750</v>
+        <v>613250</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>186400</v>
+        <v>186797</v>
       </c>
       <c r="D134" t="n">
-        <v>271064958</v>
+        <v>271646081</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2872</v>
+        <v>2873</v>
       </c>
       <c r="D137" t="n">
-        <v>4032799</v>
+        <v>4034299</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6538</v>
+        <v>6567</v>
       </c>
       <c r="D139" t="n">
-        <v>9236919</v>
+        <v>9278534</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>45326</v>
+        <v>45408</v>
       </c>
       <c r="D142" t="n">
-        <v>60507242</v>
+        <v>60617729</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14229</v>
+        <v>14244</v>
       </c>
       <c r="D148" t="n">
-        <v>20861738</v>
+        <v>20883723</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3808</v>
+        <v>3815</v>
       </c>
       <c r="D149" t="n">
-        <v>5491240</v>
+        <v>5501740</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D154" t="n">
-        <v>559763</v>
+        <v>562763</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17861</v>
+        <v>17900</v>
       </c>
       <c r="D155" t="n">
-        <v>23606905</v>
+        <v>23657680</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7285</v>
+        <v>7289</v>
       </c>
       <c r="D159" t="n">
-        <v>10599404</v>
+        <v>10605404</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5082</v>
+        <v>5095</v>
       </c>
       <c r="D161" t="n">
-        <v>7315496</v>
+        <v>7334996</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D163" t="n">
-        <v>388931</v>
+        <v>390239</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18714</v>
+        <v>18907</v>
       </c>
       <c r="D166" t="n">
-        <v>30538370</v>
+        <v>30982945</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2044</v>
+        <v>2054</v>
       </c>
       <c r="D167" t="n">
-        <v>3361072</v>
+        <v>3385072</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D171" t="n">
-        <v>181449</v>
+        <v>182949</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88709</v>
+        <v>88804</v>
       </c>
       <c r="D172" t="n">
-        <v>110866653</v>
+        <v>110979784</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D177" t="n">
-        <v>950588</v>
+        <v>952088</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>34138</v>
+        <v>34175</v>
       </c>
       <c r="D179" t="n">
-        <v>50059477</v>
+        <v>50112703</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13180</v>
+        <v>13193</v>
       </c>
       <c r="D181" t="n">
-        <v>19042845</v>
+        <v>19061357</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="D183" t="n">
-        <v>1751429</v>
+        <v>1754429</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1700</v>
+        <v>1707</v>
       </c>
       <c r="D185" t="n">
-        <v>2389005</v>
+        <v>2397239</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>240882</v>
+        <v>241175</v>
       </c>
       <c r="D187" t="n">
-        <v>299325312</v>
+        <v>299679902</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D189" t="n">
-        <v>245236</v>
+        <v>246736</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="D193" t="n">
-        <v>1298845</v>
+        <v>1300345</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>87253</v>
+        <v>87318</v>
       </c>
       <c r="D195" t="n">
-        <v>127897857</v>
+        <v>127993230</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33367</v>
+        <v>33420</v>
       </c>
       <c r="D198" t="n">
-        <v>48032595</v>
+        <v>48109725</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5156</v>
+        <v>5161</v>
       </c>
       <c r="D201" t="n">
-        <v>7339796</v>
+        <v>7347296</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5017</v>
+        <v>5038</v>
       </c>
       <c r="D204" t="n">
-        <v>6947378</v>
+        <v>6976710</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>266897</v>
+        <v>267233</v>
       </c>
       <c r="D207" t="n">
-        <v>330258895</v>
+        <v>330666003</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D209" t="n">
-        <v>367039</v>
+        <v>368539</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>95937</v>
+        <v>96065</v>
       </c>
       <c r="D216" t="n">
-        <v>140349246</v>
+        <v>140534619</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>52066</v>
+        <v>52144</v>
       </c>
       <c r="D219" t="n">
-        <v>75250062</v>
+        <v>75364853</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4709</v>
+        <v>4716</v>
       </c>
       <c r="D222" t="n">
-        <v>6609823</v>
+        <v>6620323</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5950</v>
+        <v>5985</v>
       </c>
       <c r="D225" t="n">
-        <v>8236605</v>
+        <v>8283726</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>107504</v>
+        <v>107639</v>
       </c>
       <c r="D228" t="n">
-        <v>134392646</v>
+        <v>134553886</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D230" t="n">
-        <v>106445</v>
+        <v>107513</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49912</v>
+        <v>49954</v>
       </c>
       <c r="D235" t="n">
-        <v>73117543</v>
+        <v>73179763</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12608</v>
+        <v>12626</v>
       </c>
       <c r="D237" t="n">
-        <v>18127904</v>
+        <v>18154490</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2586</v>
+        <v>2592</v>
       </c>
       <c r="D241" t="n">
-        <v>3619686</v>
+        <v>3628686</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>260873</v>
+        <v>261211</v>
       </c>
       <c r="D242" t="n">
-        <v>329377272</v>
+        <v>329794298</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D243" t="n">
-        <v>212933</v>
+        <v>214433</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96661</v>
+        <v>96780</v>
       </c>
       <c r="D250" t="n">
-        <v>141635122</v>
+        <v>141808870</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>65973</v>
+        <v>66067</v>
       </c>
       <c r="D253" t="n">
-        <v>95608796</v>
+        <v>95744711</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2431</v>
+        <v>2435</v>
       </c>
       <c r="D255" t="n">
-        <v>3427773</v>
+        <v>3433773</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4748</v>
+        <v>4760</v>
       </c>
       <c r="D258" t="n">
-        <v>6673279</v>
+        <v>6690137</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-31 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H258"/>
+  <dimension ref="A1:H259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>325370</v>
+        <v>326016</v>
       </c>
       <c r="D2" t="n">
-        <v>414484961</v>
+        <v>415284957</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D3" t="n">
-        <v>313452</v>
+        <v>314583</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D4" t="n">
-        <v>467692</v>
+        <v>469192</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D8" t="n">
-        <v>1279795</v>
+        <v>1281295</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>118238</v>
+        <v>118466</v>
       </c>
       <c r="D10" t="n">
-        <v>173244238</v>
+        <v>173575008</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60313</v>
+        <v>60457</v>
       </c>
       <c r="D12" t="n">
-        <v>87042626</v>
+        <v>87246374</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4032</v>
+        <v>4039</v>
       </c>
       <c r="D16" t="n">
-        <v>5722697</v>
+        <v>5733197</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6919</v>
+        <v>6970</v>
       </c>
       <c r="D20" t="n">
-        <v>9658932</v>
+        <v>9728468</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78403</v>
+        <v>78531</v>
       </c>
       <c r="D22" t="n">
-        <v>97695968</v>
+        <v>97847300</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32744</v>
+        <v>32791</v>
       </c>
       <c r="D28" t="n">
-        <v>47926911</v>
+        <v>47994984</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D29" t="n">
-        <v>40404</v>
+        <v>42154</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11612</v>
+        <v>11629</v>
       </c>
       <c r="D30" t="n">
-        <v>16703214</v>
+        <v>16728113</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D33" t="n">
-        <v>2204781</v>
+        <v>2206281</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1901</v>
+        <v>1911</v>
       </c>
       <c r="D35" t="n">
-        <v>2684626</v>
+        <v>2697092</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98315</v>
+        <v>98449</v>
       </c>
       <c r="D36" t="n">
-        <v>123653914</v>
+        <v>123808217</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44728</v>
+        <v>44781</v>
       </c>
       <c r="D44" t="n">
-        <v>65548733</v>
+        <v>65623445</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9269</v>
+        <v>9282</v>
       </c>
       <c r="D46" t="n">
-        <v>13294085</v>
+        <v>13311453</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1418</v>
+        <v>1423</v>
       </c>
       <c r="D48" t="n">
-        <v>1969311</v>
+        <v>1976811</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2417</v>
+        <v>2438</v>
       </c>
       <c r="D51" t="n">
-        <v>3377321</v>
+        <v>3407762</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>69882</v>
+        <v>70002</v>
       </c>
       <c r="D52" t="n">
-        <v>87639529</v>
+        <v>87785644</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D53" t="n">
-        <v>47883</v>
+        <v>49383</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D57" t="n">
-        <v>565730</v>
+        <v>566874</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28463</v>
+        <v>28489</v>
       </c>
       <c r="D59" t="n">
-        <v>41740846</v>
+        <v>41779554</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11279</v>
+        <v>11303</v>
       </c>
       <c r="D62" t="n">
-        <v>16309419</v>
+        <v>16343214</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1368</v>
+        <v>1370</v>
       </c>
       <c r="D64" t="n">
-        <v>1912237</v>
+        <v>1915237</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1534</v>
+        <v>1544</v>
       </c>
       <c r="D68" t="n">
-        <v>2147591</v>
+        <v>2162423</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20739</v>
+        <v>20775</v>
       </c>
       <c r="D70" t="n">
-        <v>27157590</v>
+        <v>27199801</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D73" t="n">
-        <v>87573</v>
+        <v>89073</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7672</v>
+        <v>7689</v>
       </c>
       <c r="D74" t="n">
-        <v>11234856</v>
+        <v>11260356</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5187</v>
+        <v>5194</v>
       </c>
       <c r="D76" t="n">
-        <v>7531486</v>
+        <v>7541986</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>142679</v>
+        <v>142897</v>
       </c>
       <c r="D79" t="n">
-        <v>177807291</v>
+        <v>178072668</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64194</v>
+        <v>64312</v>
       </c>
       <c r="D85" t="n">
-        <v>94080698</v>
+        <v>94251337</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30106</v>
+        <v>30163</v>
       </c>
       <c r="D88" t="n">
-        <v>43549256</v>
+        <v>43632190</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2757</v>
+        <v>2762</v>
       </c>
       <c r="D90" t="n">
-        <v>3969608</v>
+        <v>3977108</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2932</v>
+        <v>2948</v>
       </c>
       <c r="D91" t="n">
-        <v>4146126</v>
+        <v>4167678</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33925</v>
+        <v>33996</v>
       </c>
       <c r="D92" t="n">
-        <v>45982281</v>
+        <v>46078609</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8226</v>
+        <v>8241</v>
       </c>
       <c r="D96" t="n">
-        <v>12091517</v>
+        <v>12113758</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7571</v>
+        <v>7588</v>
       </c>
       <c r="D98" t="n">
-        <v>10984190</v>
+        <v>11008552</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D101" t="n">
-        <v>727391</v>
+        <v>733391</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10692</v>
+        <v>10753</v>
       </c>
       <c r="D102" t="n">
-        <v>16480189</v>
+        <v>16608986</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2627</v>
+        <v>2643</v>
       </c>
       <c r="D104" t="n">
-        <v>4329376</v>
+        <v>4367399</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3578</v>
+        <v>3594</v>
       </c>
       <c r="D106" t="n">
-        <v>5911207</v>
+        <v>5947427</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D109" t="n">
-        <v>326860</v>
+        <v>331360</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>143319</v>
+        <v>143528</v>
       </c>
       <c r="D110" t="n">
-        <v>177218080</v>
+        <v>177466718</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D112" t="n">
-        <v>104144</v>
+        <v>104557</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="D114" t="n">
-        <v>1399477</v>
+        <v>1406977</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53237</v>
+        <v>53319</v>
       </c>
       <c r="D116" t="n">
-        <v>78024109</v>
+        <v>78144709</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D117" t="n">
-        <v>127459</v>
+        <v>128959</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27520</v>
+        <v>27570</v>
       </c>
       <c r="D118" t="n">
-        <v>39870822</v>
+        <v>39941940</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="D119" t="n">
-        <v>1800981</v>
+        <v>1804931</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2331</v>
+        <v>2341</v>
       </c>
       <c r="D122" t="n">
-        <v>3275199</v>
+        <v>3290067</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>524648</v>
+        <v>525871</v>
       </c>
       <c r="D124" t="n">
-        <v>692891127</v>
+        <v>694426741</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1394</v>
+        <v>1397</v>
       </c>
       <c r="D129" t="n">
-        <v>2066182</v>
+        <v>2070682</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>211501</v>
+        <v>212011</v>
       </c>
       <c r="D131" t="n">
-        <v>310905529</v>
+        <v>311654615</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D132" t="n">
-        <v>616250</v>
+        <v>617750</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>187206</v>
+        <v>187715</v>
       </c>
       <c r="D134" t="n">
-        <v>272242172</v>
+        <v>272975742</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2875</v>
+        <v>2879</v>
       </c>
       <c r="D137" t="n">
-        <v>4036252</v>
+        <v>4042252</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D138" t="n">
-        <v>17722</v>
+        <v>4133</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5605,12 +5605,12 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Comité d'entreprise</t>
         </is>
       </c>
     </row>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6611</v>
+        <v>12</v>
       </c>
       <c r="D139" t="n">
-        <v>9342137</v>
+        <v>17722</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5643,12 +5643,12 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>4</v>
+        <v>6649</v>
       </c>
       <c r="D140" t="n">
-        <v>6000</v>
+        <v>9393269</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5681,12 +5681,12 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D141" t="n">
-        <v>24000</v>
+        <v>6000</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5719,12 +5719,12 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -5740,29 +5740,29 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>45474</v>
+        <v>16</v>
       </c>
       <c r="D142" t="n">
-        <v>60698389</v>
+        <v>24000</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>La Réunion</t>
+          <t>Île-de-France</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>29</v>
+        <v>45574</v>
       </c>
       <c r="D143" t="n">
-        <v>40262</v>
+        <v>60830189</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5795,12 +5795,12 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D144" t="n">
-        <v>34730</v>
+        <v>40262</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5833,12 +5833,12 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D145" t="n">
-        <v>9000</v>
+        <v>34730</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5871,12 +5871,12 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D146" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5909,12 +5909,12 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>452</v>
+        <v>5</v>
       </c>
       <c r="D147" t="n">
-        <v>677665</v>
+        <v>7500</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5947,12 +5947,12 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14260</v>
+        <v>452</v>
       </c>
       <c r="D148" t="n">
-        <v>20907241</v>
+        <v>677665</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -5985,12 +5985,12 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3819</v>
+        <v>14300</v>
       </c>
       <c r="D149" t="n">
-        <v>5507100</v>
+        <v>20964005</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6023,12 +6023,12 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>8</v>
+        <v>3830</v>
       </c>
       <c r="D150" t="n">
-        <v>12000</v>
+        <v>5523596</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6061,12 +6061,12 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D151" t="n">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6099,12 +6099,12 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>405</v>
+        <v>7</v>
       </c>
       <c r="D152" t="n">
-        <v>582716</v>
+        <v>10500</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6137,12 +6137,12 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3</v>
+        <v>406</v>
       </c>
       <c r="D153" t="n">
-        <v>4500</v>
+        <v>584216</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6175,12 +6175,12 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>399</v>
+        <v>3</v>
       </c>
       <c r="D154" t="n">
-        <v>564263</v>
+        <v>4500</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6213,12 +6213,12 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>91</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Syndicat de propriétaires</t>
         </is>
       </c>
     </row>
@@ -6234,29 +6234,29 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17938</v>
+        <v>404</v>
       </c>
       <c r="D155" t="n">
-        <v>23708075</v>
+        <v>570213</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Martinique</t>
+          <t>La Réunion</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>8</v>
+        <v>17953</v>
       </c>
       <c r="D156" t="n">
-        <v>10626</v>
+        <v>23728615</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6289,12 +6289,12 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D157" t="n">
-        <v>6000</v>
+        <v>10626</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6327,12 +6327,12 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D158" t="n">
-        <v>79406</v>
+        <v>6000</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6365,12 +6365,12 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7298</v>
+        <v>54</v>
       </c>
       <c r="D159" t="n">
-        <v>10618344</v>
+        <v>79406</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6403,12 +6403,12 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4</v>
+        <v>7310</v>
       </c>
       <c r="D160" t="n">
-        <v>6000</v>
+        <v>10635604</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6441,12 +6441,12 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5099</v>
+        <v>4</v>
       </c>
       <c r="D161" t="n">
-        <v>7340996</v>
+        <v>6000</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6479,12 +6479,12 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>4</v>
+        <v>5109</v>
       </c>
       <c r="D162" t="n">
-        <v>5310</v>
+        <v>7355524</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6517,12 +6517,12 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>282</v>
+        <v>4</v>
       </c>
       <c r="D163" t="n">
-        <v>390239</v>
+        <v>5310</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6555,12 +6555,12 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="D164" t="n">
-        <v>392364</v>
+        <v>393239</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6593,12 +6593,12 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>4</v>
+        <v>275</v>
       </c>
       <c r="D165" t="n">
-        <v>5750</v>
+        <v>392664</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6631,12 +6631,12 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6652,29 +6652,29 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>18987</v>
+        <v>4</v>
       </c>
       <c r="D166" t="n">
-        <v>31173397</v>
+        <v>5750</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>02</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Mayotte</t>
+          <t>Martinique</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2067</v>
+        <v>19139</v>
       </c>
       <c r="D167" t="n">
-        <v>3417822</v>
+        <v>31526600</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6707,12 +6707,12 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>278</v>
+        <v>2084</v>
       </c>
       <c r="D168" t="n">
-        <v>454589</v>
+        <v>3461722</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6745,12 +6745,12 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>4</v>
+        <v>280</v>
       </c>
       <c r="D169" t="n">
-        <v>6000</v>
+        <v>460589</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6783,12 +6783,12 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D170" t="n">
-        <v>110690</v>
+        <v>6000</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6821,12 +6821,12 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="D171" t="n">
-        <v>188949</v>
+        <v>110690</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6859,12 +6859,12 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6880,29 +6880,29 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>88870</v>
+        <v>109</v>
       </c>
       <c r="D172" t="n">
-        <v>111051119</v>
+        <v>188949</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>06</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Normandie</t>
+          <t>Mayotte</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>32</v>
+        <v>88978</v>
       </c>
       <c r="D173" t="n">
-        <v>37159</v>
+        <v>111177164</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6935,12 +6935,12 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="D174" t="n">
-        <v>124454</v>
+        <v>37159</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6973,12 +6973,12 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D175" t="n">
-        <v>3961</v>
+        <v>124454</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7011,12 +7011,12 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D176" t="n">
-        <v>20820</v>
+        <v>3961</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7049,12 +7049,12 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>646</v>
+        <v>14</v>
       </c>
       <c r="D177" t="n">
-        <v>952088</v>
+        <v>20820</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7087,12 +7087,12 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>4</v>
+        <v>646</v>
       </c>
       <c r="D178" t="n">
-        <v>6000</v>
+        <v>952088</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7125,12 +7125,12 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>34189</v>
+        <v>4</v>
       </c>
       <c r="D179" t="n">
-        <v>50133334</v>
+        <v>6000</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7163,12 +7163,12 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>27</v>
+        <v>34265</v>
       </c>
       <c r="D180" t="n">
-        <v>40500</v>
+        <v>50241866</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7201,12 +7201,12 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13199</v>
+        <v>27</v>
       </c>
       <c r="D181" t="n">
-        <v>19070357</v>
+        <v>40500</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7239,12 +7239,12 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>10</v>
+        <v>13226</v>
       </c>
       <c r="D182" t="n">
-        <v>13919</v>
+        <v>19107969</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7277,12 +7277,12 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1255</v>
+        <v>10</v>
       </c>
       <c r="D183" t="n">
-        <v>1757339</v>
+        <v>13919</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7315,12 +7315,12 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>4</v>
+        <v>1257</v>
       </c>
       <c r="D184" t="n">
-        <v>5839</v>
+        <v>1760339</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7353,12 +7353,12 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1712</v>
+        <v>4</v>
       </c>
       <c r="D185" t="n">
-        <v>2402871</v>
+        <v>5839</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7391,12 +7391,12 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>4</v>
+        <v>1720</v>
       </c>
       <c r="D186" t="n">
-        <v>6000</v>
+        <v>2413671</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7429,12 +7429,12 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -7450,29 +7450,29 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>241383</v>
+        <v>4</v>
       </c>
       <c r="D187" t="n">
-        <v>299920686</v>
+        <v>6000</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Nouvelle-Aquitaine</t>
+          <t>Normandie</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>136</v>
+        <v>241710</v>
       </c>
       <c r="D188" t="n">
-        <v>146087</v>
+        <v>300309828</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7505,12 +7505,12 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="D189" t="n">
-        <v>246736</v>
+        <v>147587</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7543,12 +7543,12 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="D190" t="n">
-        <v>6741</v>
+        <v>248236</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7581,12 +7581,12 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D191" t="n">
-        <v>13500</v>
+        <v>6741</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7619,12 +7619,12 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Paroisse hors zone concordataire</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D192" t="n">
-        <v>10795</v>
+        <v>13500</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7657,12 +7657,12 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Paroisse hors zone concordataire</t>
         </is>
       </c>
     </row>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>884</v>
+        <v>10</v>
       </c>
       <c r="D193" t="n">
-        <v>1300345</v>
+        <v>10795</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7695,12 +7695,12 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>7</v>
+        <v>884</v>
       </c>
       <c r="D194" t="n">
-        <v>9883</v>
+        <v>1300345</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7733,12 +7733,12 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>87371</v>
+        <v>7</v>
       </c>
       <c r="D195" t="n">
-        <v>128070825</v>
+        <v>9883</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7771,12 +7771,12 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>96</v>
+        <v>87492</v>
       </c>
       <c r="D196" t="n">
-        <v>139627</v>
+        <v>128242974</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7809,12 +7809,12 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D197" t="n">
-        <v>6000</v>
+        <v>139627</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7847,12 +7847,12 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>33455</v>
+        <v>4</v>
       </c>
       <c r="D198" t="n">
-        <v>48160920</v>
+        <v>6000</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7885,12 +7885,12 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>26</v>
+        <v>33516</v>
       </c>
       <c r="D199" t="n">
-        <v>39000</v>
+        <v>48251131</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7923,12 +7923,12 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D200" t="n">
-        <v>22108</v>
+        <v>39000</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7961,12 +7961,12 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5163</v>
+        <v>16</v>
       </c>
       <c r="D201" t="n">
-        <v>7349896</v>
+        <v>22108</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -7999,12 +7999,12 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>3</v>
+        <v>5169</v>
       </c>
       <c r="D202" t="n">
-        <v>4500</v>
+        <v>7358896</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8037,12 +8037,12 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Comité d'entreprise</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D203" t="n">
-        <v>15000</v>
+        <v>4500</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8075,12 +8075,12 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Comité d'entreprise</t>
         </is>
       </c>
     </row>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5056</v>
+        <v>10</v>
       </c>
       <c r="D204" t="n">
-        <v>7000250</v>
+        <v>15000</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8113,12 +8113,12 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>4</v>
+        <v>5082</v>
       </c>
       <c r="D205" t="n">
-        <v>6000</v>
+        <v>7037499</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8151,12 +8151,12 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D206" t="n">
-        <v>12679</v>
+        <v>6000</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8189,12 +8189,12 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -8210,29 +8210,29 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>267489</v>
+        <v>10</v>
       </c>
       <c r="D207" t="n">
-        <v>330968798</v>
+        <v>12679</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Occitanie</t>
+          <t>Nouvelle-Aquitaine</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>160</v>
+        <v>267889</v>
       </c>
       <c r="D208" t="n">
-        <v>176413</v>
+        <v>331438006</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8265,12 +8265,12 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="D209" t="n">
-        <v>368539</v>
+        <v>176413</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8303,12 +8303,12 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>17</v>
+        <v>258</v>
       </c>
       <c r="D210" t="n">
-        <v>23935</v>
+        <v>368539</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8341,12 +8341,12 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -8362,10 +8362,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D211" t="n">
-        <v>12731</v>
+        <v>23935</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -8379,12 +8379,12 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D212" t="n">
-        <v>4500</v>
+        <v>12731</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8417,12 +8417,12 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -8455,12 +8455,12 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>621</v>
+        <v>3</v>
       </c>
       <c r="D214" t="n">
-        <v>904378</v>
+        <v>4500</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8493,12 +8493,12 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>5</v>
+        <v>622</v>
       </c>
       <c r="D215" t="n">
-        <v>7500</v>
+        <v>905878</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8531,12 +8531,12 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>96127</v>
+        <v>5</v>
       </c>
       <c r="D216" t="n">
-        <v>140622357</v>
+        <v>7500</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8569,12 +8569,12 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>91</v>
+        <v>96308</v>
       </c>
       <c r="D217" t="n">
-        <v>135699</v>
+        <v>140883219</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8607,12 +8607,12 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D218" t="n">
-        <v>10500</v>
+        <v>140199</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8645,12 +8645,12 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>52192</v>
+        <v>7</v>
       </c>
       <c r="D219" t="n">
-        <v>75432161</v>
+        <v>10500</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8683,12 +8683,12 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>34</v>
+        <v>52335</v>
       </c>
       <c r="D220" t="n">
-        <v>48922</v>
+        <v>75638958</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8721,12 +8721,12 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D221" t="n">
-        <v>24160</v>
+        <v>48922</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8759,12 +8759,12 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4717</v>
+        <v>17</v>
       </c>
       <c r="D222" t="n">
-        <v>6620548</v>
+        <v>24160</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8797,12 +8797,12 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>7</v>
+        <v>4724</v>
       </c>
       <c r="D223" t="n">
-        <v>10500</v>
+        <v>6631048</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8835,12 +8835,12 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D224" t="n">
-        <v>26320</v>
+        <v>10500</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8873,12 +8873,12 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>69</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
         </is>
       </c>
     </row>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>6008</v>
+        <v>18</v>
       </c>
       <c r="D225" t="n">
-        <v>8316779</v>
+        <v>26320</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8911,12 +8911,12 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>8</v>
+        <v>6044</v>
       </c>
       <c r="D226" t="n">
-        <v>12000</v>
+        <v>8368542</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -8949,12 +8949,12 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D227" t="n">
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -8987,12 +8987,12 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -9008,29 +9008,29 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>107724</v>
+        <v>6</v>
       </c>
       <c r="D228" t="n">
-        <v>134651820</v>
+        <v>9000</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>76</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Pays de la Loire</t>
+          <t>Occitanie</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>76</v>
+        <v>107877</v>
       </c>
       <c r="D229" t="n">
-        <v>80550</v>
+        <v>134833076</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9063,12 +9063,12 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D230" t="n">
-        <v>107513</v>
+        <v>80550</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9101,12 +9101,12 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D231" t="n">
-        <v>12647</v>
+        <v>109013</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9139,12 +9139,12 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D232" t="n">
-        <v>3655</v>
+        <v>12647</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9177,12 +9177,12 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>567</v>
+        <v>3</v>
       </c>
       <c r="D233" t="n">
-        <v>828439</v>
+        <v>3655</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9215,12 +9215,12 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>4</v>
+        <v>567</v>
       </c>
       <c r="D234" t="n">
-        <v>2563</v>
+        <v>828439</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9253,12 +9253,12 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>49978</v>
+        <v>4</v>
       </c>
       <c r="D235" t="n">
-        <v>73215137</v>
+        <v>2563</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9291,12 +9291,12 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>35</v>
+        <v>50042</v>
       </c>
       <c r="D236" t="n">
-        <v>50211</v>
+        <v>73307397</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9329,12 +9329,12 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>12632</v>
+        <v>37</v>
       </c>
       <c r="D237" t="n">
-        <v>18163490</v>
+        <v>53211</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9367,12 +9367,12 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>13</v>
+        <v>12657</v>
       </c>
       <c r="D238" t="n">
-        <v>13183</v>
+        <v>18200990</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9405,12 +9405,12 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1902</v>
+        <v>13</v>
       </c>
       <c r="D239" t="n">
-        <v>2726882</v>
+        <v>13183</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9443,12 +9443,12 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>7</v>
+        <v>1906</v>
       </c>
       <c r="D240" t="n">
-        <v>8596</v>
+        <v>2732882</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9481,12 +9481,12 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2600</v>
+        <v>7</v>
       </c>
       <c r="D241" t="n">
-        <v>3640192</v>
+        <v>8596</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9519,12 +9519,12 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -9540,29 +9540,29 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>261549</v>
+        <v>2615</v>
       </c>
       <c r="D242" t="n">
-        <v>330197014</v>
+        <v>3659944</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>174</v>
+        <v>261988</v>
       </c>
       <c r="D243" t="n">
-        <v>215181</v>
+        <v>330743284</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9595,12 +9595,12 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>251</v>
+        <v>174</v>
       </c>
       <c r="D244" t="n">
-        <v>360312</v>
+        <v>215181</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9633,12 +9633,12 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="D245" t="n">
-        <v>22500</v>
+        <v>361812</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9671,12 +9671,12 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D246" t="n">
-        <v>24000</v>
+        <v>22500</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9709,12 +9709,12 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D247" t="n">
-        <v>17480</v>
+        <v>24000</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9747,12 +9747,12 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>837</v>
+        <v>12</v>
       </c>
       <c r="D248" t="n">
-        <v>1228904</v>
+        <v>17480</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9785,12 +9785,12 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>10</v>
+        <v>840</v>
       </c>
       <c r="D249" t="n">
-        <v>15000</v>
+        <v>1233404</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9823,12 +9823,12 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>96860</v>
+        <v>10</v>
       </c>
       <c r="D250" t="n">
-        <v>141927087</v>
+        <v>15000</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9861,12 +9861,12 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>77</v>
+        <v>97047</v>
       </c>
       <c r="D251" t="n">
-        <v>112661</v>
+        <v>142198206</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9899,12 +9899,12 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="D252" t="n">
-        <v>6000</v>
+        <v>112661</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9937,12 +9937,12 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>66155</v>
+        <v>4</v>
       </c>
       <c r="D253" t="n">
-        <v>95873681</v>
+        <v>6000</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9975,12 +9975,12 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>16</v>
+        <v>66311</v>
       </c>
       <c r="D254" t="n">
-        <v>23989</v>
+        <v>96103918</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10013,12 +10013,12 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2437</v>
+        <v>16</v>
       </c>
       <c r="D255" t="n">
-        <v>3436773</v>
+        <v>23989</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10051,12 +10051,12 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>10</v>
+        <v>2439</v>
       </c>
       <c r="D256" t="n">
-        <v>15000</v>
+        <v>3439573</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10089,12 +10089,12 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D257" t="n">
-        <v>10500</v>
+        <v>15000</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10127,12 +10127,12 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4787</v>
+        <v>7</v>
       </c>
       <c r="D258" t="n">
-        <v>6726683</v>
+        <v>10500</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10165,10 +10165,48 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>Syndicat de propriétaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>4815</v>
+      </c>
+      <c r="D259" t="n">
+        <v>6764014</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
           <t>92</t>
         </is>
       </c>
-      <c r="H258" t="inlineStr">
+      <c r="H259" t="inlineStr">
         <is>
           <t>Association loi 1901 ou assimilé</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-01 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>326016</v>
+        <v>327307</v>
       </c>
       <c r="D2" t="n">
-        <v>415284957</v>
+        <v>416903939</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D3" t="n">
-        <v>314583</v>
+        <v>316083</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D4" t="n">
-        <v>469192</v>
+        <v>470692</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="D8" t="n">
-        <v>1281295</v>
+        <v>1286899</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>118466</v>
+        <v>118799</v>
       </c>
       <c r="D10" t="n">
-        <v>173575008</v>
+        <v>174059813</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60457</v>
+        <v>60677</v>
       </c>
       <c r="D12" t="n">
-        <v>87246374</v>
+        <v>87562990</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" t="n">
-        <v>67543</v>
+        <v>69039</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4039</v>
+        <v>4046</v>
       </c>
       <c r="D16" t="n">
-        <v>5733197</v>
+        <v>5743697</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D19" t="n">
-        <v>103035</v>
+        <v>107535</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6970</v>
+        <v>7034</v>
       </c>
       <c r="D20" t="n">
-        <v>9728468</v>
+        <v>9819014</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78531</v>
+        <v>78799</v>
       </c>
       <c r="D22" t="n">
-        <v>97847300</v>
+        <v>98176338</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32791</v>
+        <v>32862</v>
       </c>
       <c r="D28" t="n">
-        <v>47994984</v>
+        <v>48096936</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11629</v>
+        <v>11676</v>
       </c>
       <c r="D30" t="n">
-        <v>16728113</v>
+        <v>16796116</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1570</v>
+        <v>1572</v>
       </c>
       <c r="D33" t="n">
-        <v>2206281</v>
+        <v>2208781</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1911</v>
+        <v>1935</v>
       </c>
       <c r="D35" t="n">
-        <v>2697092</v>
+        <v>2731421</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98449</v>
+        <v>98731</v>
       </c>
       <c r="D36" t="n">
-        <v>123808217</v>
+        <v>124153656</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="D42" t="n">
-        <v>1330685</v>
+        <v>1333685</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44781</v>
+        <v>44882</v>
       </c>
       <c r="D44" t="n">
-        <v>65623445</v>
+        <v>65771629</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9282</v>
+        <v>9314</v>
       </c>
       <c r="D46" t="n">
-        <v>13311453</v>
+        <v>13357668</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="D48" t="n">
-        <v>1976811</v>
+        <v>1979811</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2438</v>
+        <v>2462</v>
       </c>
       <c r="D51" t="n">
-        <v>3407762</v>
+        <v>3441802</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70002</v>
+        <v>70212</v>
       </c>
       <c r="D52" t="n">
-        <v>87785644</v>
+        <v>88044381</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28489</v>
+        <v>28575</v>
       </c>
       <c r="D59" t="n">
-        <v>41779554</v>
+        <v>41906493</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11303</v>
+        <v>11351</v>
       </c>
       <c r="D62" t="n">
-        <v>16343214</v>
+        <v>16410368</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D64" t="n">
-        <v>1915237</v>
+        <v>1916737</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1544</v>
+        <v>1562</v>
       </c>
       <c r="D68" t="n">
-        <v>2162423</v>
+        <v>2188581</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20775</v>
+        <v>20840</v>
       </c>
       <c r="D70" t="n">
-        <v>27199801</v>
+        <v>27287296</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7689</v>
+        <v>7705</v>
       </c>
       <c r="D74" t="n">
-        <v>11260356</v>
+        <v>11284101</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5194</v>
+        <v>5208</v>
       </c>
       <c r="D76" t="n">
-        <v>7541986</v>
+        <v>7562986</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D77" t="n">
-        <v>701239</v>
+        <v>702739</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>142897</v>
+        <v>143405</v>
       </c>
       <c r="D79" t="n">
-        <v>178072668</v>
+        <v>178706970</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="D83" t="n">
-        <v>629324</v>
+        <v>635324</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64312</v>
+        <v>64437</v>
       </c>
       <c r="D85" t="n">
-        <v>94251337</v>
+        <v>94431439</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30163</v>
+        <v>30268</v>
       </c>
       <c r="D88" t="n">
-        <v>43632190</v>
+        <v>43785165</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2762</v>
+        <v>2767</v>
       </c>
       <c r="D90" t="n">
-        <v>3977108</v>
+        <v>3984198</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2948</v>
+        <v>2971</v>
       </c>
       <c r="D91" t="n">
-        <v>4167678</v>
+        <v>4200764</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33996</v>
+        <v>34175</v>
       </c>
       <c r="D92" t="n">
-        <v>46078609</v>
+        <v>46334405</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8241</v>
+        <v>8270</v>
       </c>
       <c r="D96" t="n">
-        <v>12113758</v>
+        <v>12156583</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7588</v>
+        <v>7639</v>
       </c>
       <c r="D98" t="n">
-        <v>11008552</v>
+        <v>11083971</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="D100" t="n">
-        <v>771135</v>
+        <v>773406</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="D101" t="n">
-        <v>733391</v>
+        <v>742026</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>10753</v>
+        <v>11079</v>
       </c>
       <c r="D102" t="n">
-        <v>16608986</v>
+        <v>17392189</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2643</v>
+        <v>2716</v>
       </c>
       <c r="D104" t="n">
-        <v>4367399</v>
+        <v>4577049</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3594</v>
+        <v>3695</v>
       </c>
       <c r="D106" t="n">
-        <v>5947427</v>
+        <v>6211094</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D108" t="n">
-        <v>265445</v>
+        <v>271445</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D109" t="n">
-        <v>331360</v>
+        <v>339180</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>143528</v>
+        <v>144204</v>
       </c>
       <c r="D110" t="n">
-        <v>177466718</v>
+        <v>178353166</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D114" t="n">
-        <v>1406977</v>
+        <v>1408477</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53319</v>
+        <v>53457</v>
       </c>
       <c r="D116" t="n">
-        <v>78144709</v>
+        <v>78347067</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27570</v>
+        <v>27749</v>
       </c>
       <c r="D118" t="n">
-        <v>39941940</v>
+        <v>40203803</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="D119" t="n">
-        <v>1804931</v>
+        <v>1809431</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2341</v>
+        <v>2359</v>
       </c>
       <c r="D122" t="n">
-        <v>3290067</v>
+        <v>3316951</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>525871</v>
+        <v>531313</v>
       </c>
       <c r="D124" t="n">
-        <v>694426741</v>
+        <v>701911255</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D126" t="n">
-        <v>322509</v>
+        <v>325509</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D128" t="n">
-        <v>32998</v>
+        <v>35998</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1397</v>
+        <v>1401</v>
       </c>
       <c r="D129" t="n">
-        <v>2070682</v>
+        <v>2076682</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>212011</v>
+        <v>212945</v>
       </c>
       <c r="D131" t="n">
-        <v>311654615</v>
+        <v>313018040</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D132" t="n">
-        <v>617750</v>
+        <v>620710</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>187715</v>
+        <v>189756</v>
       </c>
       <c r="D134" t="n">
-        <v>272975742</v>
+        <v>275957706</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2879</v>
+        <v>2882</v>
       </c>
       <c r="D137" t="n">
-        <v>4042252</v>
+        <v>4046752</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6649</v>
+        <v>6707</v>
       </c>
       <c r="D140" t="n">
-        <v>9393269</v>
+        <v>9473603</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>45574</v>
+        <v>45815</v>
       </c>
       <c r="D143" t="n">
-        <v>60830189</v>
+        <v>61154904</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>14300</v>
+        <v>14345</v>
       </c>
       <c r="D149" t="n">
-        <v>20964005</v>
+        <v>21026910</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3830</v>
+        <v>3845</v>
       </c>
       <c r="D150" t="n">
-        <v>5523596</v>
+        <v>5543592</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D155" t="n">
-        <v>570213</v>
+        <v>577813</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>17953</v>
+        <v>18046</v>
       </c>
       <c r="D156" t="n">
-        <v>23728615</v>
+        <v>23858981</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7310</v>
+        <v>7355</v>
       </c>
       <c r="D160" t="n">
-        <v>10635604</v>
+        <v>10701429</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5109</v>
+        <v>5132</v>
       </c>
       <c r="D162" t="n">
-        <v>7355524</v>
+        <v>7389073</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D164" t="n">
-        <v>393239</v>
+        <v>394139</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D165" t="n">
-        <v>392664</v>
+        <v>395664</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>19139</v>
+        <v>19937</v>
       </c>
       <c r="D167" t="n">
-        <v>31526600</v>
+        <v>33722794</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2084</v>
+        <v>2147</v>
       </c>
       <c r="D168" t="n">
-        <v>3461722</v>
+        <v>3640234</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D169" t="n">
-        <v>460589</v>
+        <v>480089</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D171" t="n">
-        <v>110690</v>
+        <v>119690</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D172" t="n">
-        <v>188949</v>
+        <v>203949</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>88978</v>
+        <v>89256</v>
       </c>
       <c r="D173" t="n">
-        <v>111177164</v>
+        <v>111525245</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>34265</v>
+        <v>34334</v>
       </c>
       <c r="D180" t="n">
-        <v>50241866</v>
+        <v>50342558</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>13226</v>
+        <v>13279</v>
       </c>
       <c r="D182" t="n">
-        <v>19107969</v>
+        <v>19185092</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D184" t="n">
-        <v>1760339</v>
+        <v>1761839</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1720</v>
+        <v>1729</v>
       </c>
       <c r="D186" t="n">
-        <v>2413671</v>
+        <v>2426207</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>241710</v>
+        <v>242532</v>
       </c>
       <c r="D188" t="n">
-        <v>300309828</v>
+        <v>301328956</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="D194" t="n">
-        <v>1300345</v>
+        <v>1306345</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>87492</v>
+        <v>87688</v>
       </c>
       <c r="D196" t="n">
-        <v>128242974</v>
+        <v>128522041</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>33516</v>
+        <v>33636</v>
       </c>
       <c r="D199" t="n">
-        <v>48251131</v>
+        <v>48426042</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D201" t="n">
-        <v>22108</v>
+        <v>23608</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>5169</v>
+        <v>5174</v>
       </c>
       <c r="D202" t="n">
-        <v>7358896</v>
+        <v>7366396</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>5082</v>
+        <v>5122</v>
       </c>
       <c r="D205" t="n">
-        <v>7037499</v>
+        <v>7093246</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>267889</v>
+        <v>268856</v>
       </c>
       <c r="D208" t="n">
-        <v>331438006</v>
+        <v>332642480</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D209" t="n">
-        <v>176413</v>
+        <v>177913</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D215" t="n">
-        <v>905878</v>
+        <v>907378</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>96308</v>
+        <v>96538</v>
       </c>
       <c r="D217" t="n">
-        <v>140883219</v>
+        <v>141218029</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>52335</v>
+        <v>52572</v>
       </c>
       <c r="D220" t="n">
-        <v>75638958</v>
+        <v>75981869</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4724</v>
+        <v>4729</v>
       </c>
       <c r="D223" t="n">
-        <v>6631048</v>
+        <v>6637365</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D225" t="n">
-        <v>26320</v>
+        <v>29238</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>6044</v>
+        <v>6079</v>
       </c>
       <c r="D226" t="n">
-        <v>8368542</v>
+        <v>8420386</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>107877</v>
+        <v>108331</v>
       </c>
       <c r="D229" t="n">
-        <v>134833076</v>
+        <v>135409601</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D234" t="n">
-        <v>828439</v>
+        <v>829939</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>50042</v>
+        <v>50160</v>
       </c>
       <c r="D236" t="n">
-        <v>73307397</v>
+        <v>73477831</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D237" t="n">
-        <v>53211</v>
+        <v>54711</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>12657</v>
+        <v>12728</v>
       </c>
       <c r="D238" t="n">
-        <v>18200990</v>
+        <v>18306818</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1906</v>
+        <v>1907</v>
       </c>
       <c r="D240" t="n">
-        <v>2732882</v>
+        <v>2734382</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2615</v>
+        <v>2634</v>
       </c>
       <c r="D242" t="n">
-        <v>3659944</v>
+        <v>3688444</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>261988</v>
+        <v>263058</v>
       </c>
       <c r="D243" t="n">
-        <v>330743284</v>
+        <v>332122744</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D245" t="n">
-        <v>361812</v>
+        <v>363312</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D248" t="n">
-        <v>17480</v>
+        <v>20480</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="D249" t="n">
-        <v>1233404</v>
+        <v>1237904</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>97047</v>
+        <v>97313</v>
       </c>
       <c r="D251" t="n">
-        <v>142198206</v>
+        <v>142583196</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>66311</v>
+        <v>66620</v>
       </c>
       <c r="D254" t="n">
-        <v>96103918</v>
+        <v>96556577</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2439</v>
+        <v>2447</v>
       </c>
       <c r="D256" t="n">
-        <v>3439573</v>
+        <v>3451224</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4815</v>
+        <v>4862</v>
       </c>
       <c r="D259" t="n">
-        <v>6764014</v>
+        <v>6828926</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-02 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>327307</v>
+        <v>328210</v>
       </c>
       <c r="D2" t="n">
-        <v>416903939</v>
+        <v>418052235</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D4" t="n">
-        <v>470692</v>
+        <v>472192</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>118799</v>
+        <v>119020</v>
       </c>
       <c r="D10" t="n">
-        <v>174059813</v>
+        <v>174383802</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60677</v>
+        <v>60902</v>
       </c>
       <c r="D12" t="n">
-        <v>87562990</v>
+        <v>87886707</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4046</v>
+        <v>4047</v>
       </c>
       <c r="D16" t="n">
-        <v>5743697</v>
+        <v>5745197</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7034</v>
+        <v>7076</v>
       </c>
       <c r="D20" t="n">
-        <v>9819014</v>
+        <v>9881318</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78799</v>
+        <v>78986</v>
       </c>
       <c r="D22" t="n">
-        <v>98176338</v>
+        <v>98399880</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D23" t="n">
-        <v>71209</v>
+        <v>74209</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32862</v>
+        <v>32926</v>
       </c>
       <c r="D28" t="n">
-        <v>48096936</v>
+        <v>48189214</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11676</v>
+        <v>11712</v>
       </c>
       <c r="D30" t="n">
-        <v>16796116</v>
+        <v>16848427</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1935</v>
+        <v>1945</v>
       </c>
       <c r="D35" t="n">
-        <v>2731421</v>
+        <v>2745194</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98731</v>
+        <v>98954</v>
       </c>
       <c r="D36" t="n">
-        <v>124153656</v>
+        <v>124421860</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="D42" t="n">
-        <v>1333685</v>
+        <v>1336685</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44882</v>
+        <v>44965</v>
       </c>
       <c r="D44" t="n">
-        <v>65771629</v>
+        <v>65892848</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9314</v>
+        <v>9349</v>
       </c>
       <c r="D46" t="n">
-        <v>13357668</v>
+        <v>13408625</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D48" t="n">
-        <v>1979811</v>
+        <v>1981311</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2462</v>
+        <v>2474</v>
       </c>
       <c r="D51" t="n">
-        <v>3441802</v>
+        <v>3459602</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70212</v>
+        <v>70406</v>
       </c>
       <c r="D52" t="n">
-        <v>88044381</v>
+        <v>88281022</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D53" t="n">
-        <v>49383</v>
+        <v>50883</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28575</v>
+        <v>28627</v>
       </c>
       <c r="D59" t="n">
-        <v>41906493</v>
+        <v>41983766</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11351</v>
+        <v>11384</v>
       </c>
       <c r="D62" t="n">
-        <v>16410368</v>
+        <v>16458647</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="D64" t="n">
-        <v>1916737</v>
+        <v>1919497</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1562</v>
+        <v>1574</v>
       </c>
       <c r="D68" t="n">
-        <v>2188581</v>
+        <v>2206581</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20840</v>
+        <v>20885</v>
       </c>
       <c r="D70" t="n">
-        <v>27287296</v>
+        <v>27348823</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7705</v>
+        <v>7722</v>
       </c>
       <c r="D74" t="n">
-        <v>11284101</v>
+        <v>11309601</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5208</v>
+        <v>5214</v>
       </c>
       <c r="D76" t="n">
-        <v>7562986</v>
+        <v>7571499</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D77" t="n">
-        <v>702739</v>
+        <v>704239</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D78" t="n">
-        <v>405083</v>
+        <v>408083</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>143405</v>
+        <v>143721</v>
       </c>
       <c r="D79" t="n">
-        <v>178706970</v>
+        <v>179093809</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D80" t="n">
-        <v>84321</v>
+        <v>84766</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D81" t="n">
-        <v>123384</v>
+        <v>124884</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D83" t="n">
-        <v>635324</v>
+        <v>638324</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64437</v>
+        <v>64547</v>
       </c>
       <c r="D85" t="n">
-        <v>94431439</v>
+        <v>94593284</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30268</v>
+        <v>30321</v>
       </c>
       <c r="D88" t="n">
-        <v>43785165</v>
+        <v>43863090</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2767</v>
+        <v>2769</v>
       </c>
       <c r="D90" t="n">
-        <v>3984198</v>
+        <v>3987143</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2971</v>
+        <v>2988</v>
       </c>
       <c r="D91" t="n">
-        <v>4200764</v>
+        <v>4225334</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>34175</v>
+        <v>34335</v>
       </c>
       <c r="D92" t="n">
-        <v>46334405</v>
+        <v>46550683</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8270</v>
+        <v>8320</v>
       </c>
       <c r="D96" t="n">
-        <v>12156583</v>
+        <v>12230763</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7639</v>
+        <v>7676</v>
       </c>
       <c r="D98" t="n">
-        <v>11083971</v>
+        <v>11138362</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="D100" t="n">
-        <v>773406</v>
+        <v>779406</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="D101" t="n">
-        <v>742026</v>
+        <v>749050</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11079</v>
+        <v>11249</v>
       </c>
       <c r="D102" t="n">
-        <v>17392189</v>
+        <v>17824918</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2716</v>
+        <v>2754</v>
       </c>
       <c r="D104" t="n">
-        <v>4577049</v>
+        <v>4684854</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3695</v>
+        <v>3777</v>
       </c>
       <c r="D106" t="n">
-        <v>6211094</v>
+        <v>6448776</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D108" t="n">
-        <v>271445</v>
+        <v>280445</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D109" t="n">
-        <v>339180</v>
+        <v>356030</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>144204</v>
+        <v>144666</v>
       </c>
       <c r="D110" t="n">
-        <v>178353166</v>
+        <v>178919200</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53457</v>
+        <v>53576</v>
       </c>
       <c r="D116" t="n">
-        <v>78347067</v>
+        <v>78520350</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27749</v>
+        <v>27864</v>
       </c>
       <c r="D118" t="n">
-        <v>40203803</v>
+        <v>40372562</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="D119" t="n">
-        <v>1809431</v>
+        <v>1812194</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="D122" t="n">
-        <v>3316951</v>
+        <v>3341770</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>531313</v>
+        <v>535398</v>
       </c>
       <c r="D124" t="n">
-        <v>701911255</v>
+        <v>707450560</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D125" t="n">
-        <v>122289</v>
+        <v>123789</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1401</v>
+        <v>1403</v>
       </c>
       <c r="D129" t="n">
-        <v>2076682</v>
+        <v>2079682</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>212945</v>
+        <v>213701</v>
       </c>
       <c r="D131" t="n">
-        <v>313018040</v>
+        <v>314130371</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D132" t="n">
-        <v>620710</v>
+        <v>623710</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>189756</v>
+        <v>191244</v>
       </c>
       <c r="D134" t="n">
-        <v>275957706</v>
+        <v>278116760</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2882</v>
+        <v>2886</v>
       </c>
       <c r="D137" t="n">
-        <v>4046752</v>
+        <v>4052272</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6707</v>
+        <v>6751</v>
       </c>
       <c r="D140" t="n">
-        <v>9473603</v>
+        <v>9528706</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>45815</v>
+        <v>45963</v>
       </c>
       <c r="D143" t="n">
-        <v>61154904</v>
+        <v>61349800</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>14345</v>
+        <v>14375</v>
       </c>
       <c r="D149" t="n">
-        <v>21026910</v>
+        <v>21070307</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3845</v>
+        <v>3858</v>
       </c>
       <c r="D150" t="n">
-        <v>5543592</v>
+        <v>5563092</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="D155" t="n">
-        <v>577813</v>
+        <v>582313</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>18046</v>
+        <v>18111</v>
       </c>
       <c r="D156" t="n">
-        <v>23858981</v>
+        <v>23945906</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7355</v>
+        <v>7382</v>
       </c>
       <c r="D160" t="n">
-        <v>10701429</v>
+        <v>10742048</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5132</v>
+        <v>5157</v>
       </c>
       <c r="D162" t="n">
-        <v>7389073</v>
+        <v>7423474</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D165" t="n">
-        <v>395664</v>
+        <v>397164</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>19937</v>
+        <v>20587</v>
       </c>
       <c r="D167" t="n">
-        <v>33722794</v>
+        <v>35592563</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2147</v>
+        <v>2213</v>
       </c>
       <c r="D168" t="n">
-        <v>3640234</v>
+        <v>3830701</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="D169" t="n">
-        <v>480089</v>
+        <v>495089</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D171" t="n">
-        <v>119690</v>
+        <v>131690</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D172" t="n">
-        <v>203949</v>
+        <v>211449</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>89256</v>
+        <v>89496</v>
       </c>
       <c r="D173" t="n">
-        <v>111525245</v>
+        <v>111791414</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>34334</v>
+        <v>34407</v>
       </c>
       <c r="D180" t="n">
-        <v>50342558</v>
+        <v>50448058</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>13279</v>
+        <v>13321</v>
       </c>
       <c r="D182" t="n">
-        <v>19185092</v>
+        <v>19247992</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1258</v>
+        <v>1264</v>
       </c>
       <c r="D184" t="n">
-        <v>1761839</v>
+        <v>1768933</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1729</v>
+        <v>1740</v>
       </c>
       <c r="D186" t="n">
-        <v>2426207</v>
+        <v>2441487</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>242532</v>
+        <v>243132</v>
       </c>
       <c r="D188" t="n">
-        <v>301328956</v>
+        <v>302059535</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D190" t="n">
-        <v>248236</v>
+        <v>249736</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="D194" t="n">
-        <v>1306345</v>
+        <v>1309345</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>87688</v>
+        <v>87873</v>
       </c>
       <c r="D196" t="n">
-        <v>128522041</v>
+        <v>128793334</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>33636</v>
+        <v>33722</v>
       </c>
       <c r="D199" t="n">
-        <v>48426042</v>
+        <v>48549463</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>5174</v>
+        <v>5182</v>
       </c>
       <c r="D202" t="n">
-        <v>7366396</v>
+        <v>7377358</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>5122</v>
+        <v>5157</v>
       </c>
       <c r="D205" t="n">
-        <v>7093246</v>
+        <v>7140867</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>268856</v>
+        <v>269503</v>
       </c>
       <c r="D208" t="n">
-        <v>332642480</v>
+        <v>333455676</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>96538</v>
+        <v>96725</v>
       </c>
       <c r="D217" t="n">
-        <v>141218029</v>
+        <v>141493030</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D218" t="n">
-        <v>140199</v>
+        <v>141699</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>52572</v>
+        <v>52747</v>
       </c>
       <c r="D220" t="n">
-        <v>75981869</v>
+        <v>76233209</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4729</v>
+        <v>4732</v>
       </c>
       <c r="D223" t="n">
-        <v>6637365</v>
+        <v>6641035</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>6079</v>
+        <v>6112</v>
       </c>
       <c r="D226" t="n">
-        <v>8420386</v>
+        <v>8466100</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D228" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>108331</v>
+        <v>108657</v>
       </c>
       <c r="D229" t="n">
-        <v>135409601</v>
+        <v>135816647</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D232" t="n">
-        <v>12647</v>
+        <v>14147</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D234" t="n">
-        <v>829939</v>
+        <v>832939</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>50160</v>
+        <v>50251</v>
       </c>
       <c r="D236" t="n">
-        <v>73477831</v>
+        <v>73610986</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>12728</v>
+        <v>12765</v>
       </c>
       <c r="D238" t="n">
-        <v>18306818</v>
+        <v>18359767</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1907</v>
+        <v>1909</v>
       </c>
       <c r="D240" t="n">
-        <v>2734382</v>
+        <v>2737382</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2634</v>
+        <v>2645</v>
       </c>
       <c r="D242" t="n">
-        <v>3688444</v>
+        <v>3704384</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>263058</v>
+        <v>263879</v>
       </c>
       <c r="D243" t="n">
-        <v>332122744</v>
+        <v>333156164</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>97313</v>
+        <v>97521</v>
       </c>
       <c r="D251" t="n">
-        <v>142583196</v>
+        <v>142890737</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>66620</v>
+        <v>66868</v>
       </c>
       <c r="D254" t="n">
-        <v>96556577</v>
+        <v>96920073</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2447</v>
+        <v>2449</v>
       </c>
       <c r="D256" t="n">
-        <v>3451224</v>
+        <v>3454224</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4862</v>
+        <v>4892</v>
       </c>
       <c r="D259" t="n">
-        <v>6828926</v>
+        <v>6873294</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-03 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>328210</v>
+        <v>329058</v>
       </c>
       <c r="D2" t="n">
-        <v>418052235</v>
+        <v>419105950</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D8" t="n">
-        <v>1286899</v>
+        <v>1288399</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>119020</v>
+        <v>119243</v>
       </c>
       <c r="D10" t="n">
-        <v>174383802</v>
+        <v>174713253</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>60902</v>
+        <v>61080</v>
       </c>
       <c r="D12" t="n">
-        <v>87886707</v>
+        <v>88144701</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4047</v>
+        <v>4050</v>
       </c>
       <c r="D16" t="n">
-        <v>5745197</v>
+        <v>5749637</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7076</v>
+        <v>7109</v>
       </c>
       <c r="D20" t="n">
-        <v>9881318</v>
+        <v>9925961</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>78986</v>
+        <v>79172</v>
       </c>
       <c r="D22" t="n">
-        <v>98399880</v>
+        <v>98626700</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32926</v>
+        <v>32965</v>
       </c>
       <c r="D28" t="n">
-        <v>48189214</v>
+        <v>48247181</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11712</v>
+        <v>11737</v>
       </c>
       <c r="D30" t="n">
-        <v>16848427</v>
+        <v>16882730</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D33" t="n">
-        <v>2208781</v>
+        <v>2209891</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1945</v>
+        <v>1954</v>
       </c>
       <c r="D35" t="n">
-        <v>2745194</v>
+        <v>2757992</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>98954</v>
+        <v>99154</v>
       </c>
       <c r="D36" t="n">
-        <v>124421860</v>
+        <v>124657883</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44965</v>
+        <v>45048</v>
       </c>
       <c r="D44" t="n">
-        <v>65892848</v>
+        <v>66012119</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9349</v>
+        <v>9373</v>
       </c>
       <c r="D46" t="n">
-        <v>13408625</v>
+        <v>13441824</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1426</v>
+        <v>1430</v>
       </c>
       <c r="D48" t="n">
-        <v>1981311</v>
+        <v>1987311</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2474</v>
+        <v>2481</v>
       </c>
       <c r="D51" t="n">
-        <v>3459602</v>
+        <v>3468587</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70406</v>
+        <v>70548</v>
       </c>
       <c r="D52" t="n">
-        <v>88281022</v>
+        <v>88459159</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28627</v>
+        <v>28669</v>
       </c>
       <c r="D59" t="n">
-        <v>41983766</v>
+        <v>42045742</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11384</v>
+        <v>11407</v>
       </c>
       <c r="D62" t="n">
-        <v>16458647</v>
+        <v>16492001</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1574</v>
+        <v>1579</v>
       </c>
       <c r="D68" t="n">
-        <v>2206581</v>
+        <v>2213851</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20885</v>
+        <v>20929</v>
       </c>
       <c r="D70" t="n">
-        <v>27348823</v>
+        <v>27404826</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7722</v>
+        <v>7734</v>
       </c>
       <c r="D74" t="n">
-        <v>11309601</v>
+        <v>11326800</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5214</v>
+        <v>5228</v>
       </c>
       <c r="D76" t="n">
-        <v>7571499</v>
+        <v>7592494</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D78" t="n">
-        <v>408083</v>
+        <v>411083</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>143721</v>
+        <v>144006</v>
       </c>
       <c r="D79" t="n">
-        <v>179093809</v>
+        <v>179451635</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="D83" t="n">
-        <v>638324</v>
+        <v>642824</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64547</v>
+        <v>64648</v>
       </c>
       <c r="D85" t="n">
-        <v>94593284</v>
+        <v>94740475</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30321</v>
+        <v>30393</v>
       </c>
       <c r="D88" t="n">
-        <v>43863090</v>
+        <v>43967559</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2988</v>
+        <v>3000</v>
       </c>
       <c r="D91" t="n">
-        <v>4225334</v>
+        <v>4242243</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>34335</v>
+        <v>34481</v>
       </c>
       <c r="D92" t="n">
-        <v>46550683</v>
+        <v>46749197</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8320</v>
+        <v>8359</v>
       </c>
       <c r="D96" t="n">
-        <v>12230763</v>
+        <v>12288126</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7676</v>
+        <v>7729</v>
       </c>
       <c r="D98" t="n">
-        <v>11138362</v>
+        <v>11216237</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D100" t="n">
-        <v>779406</v>
+        <v>782406</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D101" t="n">
-        <v>749050</v>
+        <v>752050</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11249</v>
+        <v>11428</v>
       </c>
       <c r="D102" t="n">
-        <v>17824918</v>
+        <v>18274439</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2754</v>
+        <v>2792</v>
       </c>
       <c r="D104" t="n">
-        <v>4684854</v>
+        <v>4797354</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3777</v>
+        <v>3825</v>
       </c>
       <c r="D106" t="n">
-        <v>6448776</v>
+        <v>6581934</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D108" t="n">
-        <v>280445</v>
+        <v>285045</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D109" t="n">
-        <v>356030</v>
+        <v>359030</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>144666</v>
+        <v>145011</v>
       </c>
       <c r="D110" t="n">
-        <v>178919200</v>
+        <v>179340364</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="D114" t="n">
-        <v>1408477</v>
+        <v>1409977</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53576</v>
+        <v>53687</v>
       </c>
       <c r="D116" t="n">
-        <v>78520350</v>
+        <v>78682945</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27864</v>
+        <v>27947</v>
       </c>
       <c r="D118" t="n">
-        <v>40372562</v>
+        <v>40490219</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D119" t="n">
-        <v>1812194</v>
+        <v>1813694</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2377</v>
+        <v>2398</v>
       </c>
       <c r="D122" t="n">
-        <v>3341770</v>
+        <v>3372326</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>535398</v>
+        <v>538400</v>
       </c>
       <c r="D124" t="n">
-        <v>707450560</v>
+        <v>711455433</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1403</v>
+        <v>1409</v>
       </c>
       <c r="D129" t="n">
-        <v>2079682</v>
+        <v>2088214</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>213701</v>
+        <v>214404</v>
       </c>
       <c r="D131" t="n">
-        <v>314130371</v>
+        <v>315157910</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D132" t="n">
-        <v>623710</v>
+        <v>631210</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>191244</v>
+        <v>192284</v>
       </c>
       <c r="D134" t="n">
-        <v>278116760</v>
+        <v>279636318</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2886</v>
+        <v>2887</v>
       </c>
       <c r="D137" t="n">
-        <v>4052272</v>
+        <v>4053072</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6751</v>
+        <v>6792</v>
       </c>
       <c r="D140" t="n">
-        <v>9528706</v>
+        <v>9588568</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>45963</v>
+        <v>46095</v>
       </c>
       <c r="D143" t="n">
-        <v>61349800</v>
+        <v>61516197</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D145" t="n">
-        <v>34730</v>
+        <v>36230</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>14375</v>
+        <v>14409</v>
       </c>
       <c r="D149" t="n">
-        <v>21070307</v>
+        <v>21118939</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3858</v>
+        <v>3862</v>
       </c>
       <c r="D150" t="n">
-        <v>5563092</v>
+        <v>5569092</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D155" t="n">
-        <v>582313</v>
+        <v>583813</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>18111</v>
+        <v>18156</v>
       </c>
       <c r="D156" t="n">
-        <v>23945906</v>
+        <v>24002421</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7382</v>
+        <v>7407</v>
       </c>
       <c r="D160" t="n">
-        <v>10742048</v>
+        <v>10777403</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5157</v>
+        <v>5180</v>
       </c>
       <c r="D162" t="n">
-        <v>7423474</v>
+        <v>7455538</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>20587</v>
+        <v>21046</v>
       </c>
       <c r="D167" t="n">
-        <v>35592563</v>
+        <v>36877480</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2213</v>
+        <v>2256</v>
       </c>
       <c r="D168" t="n">
-        <v>3830701</v>
+        <v>3955071</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D169" t="n">
-        <v>495089</v>
+        <v>501089</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D172" t="n">
-        <v>211449</v>
+        <v>217449</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>89496</v>
+        <v>89714</v>
       </c>
       <c r="D173" t="n">
-        <v>111791414</v>
+        <v>112051640</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>34407</v>
+        <v>34471</v>
       </c>
       <c r="D180" t="n">
-        <v>50448058</v>
+        <v>50543665</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>13321</v>
+        <v>13356</v>
       </c>
       <c r="D182" t="n">
-        <v>19247992</v>
+        <v>19297802</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1740</v>
+        <v>1746</v>
       </c>
       <c r="D186" t="n">
-        <v>2441487</v>
+        <v>2450429</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>243132</v>
+        <v>243637</v>
       </c>
       <c r="D188" t="n">
-        <v>302059535</v>
+        <v>302682416</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="D194" t="n">
-        <v>1309345</v>
+        <v>1313845</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>87873</v>
+        <v>88011</v>
       </c>
       <c r="D196" t="n">
-        <v>128793334</v>
+        <v>128995603</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>33722</v>
+        <v>33795</v>
       </c>
       <c r="D199" t="n">
-        <v>48549463</v>
+        <v>48656175</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>5182</v>
+        <v>5190</v>
       </c>
       <c r="D202" t="n">
-        <v>7377358</v>
+        <v>7389358</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>5157</v>
+        <v>5185</v>
       </c>
       <c r="D205" t="n">
-        <v>7140867</v>
+        <v>7180301</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>269503</v>
+        <v>270055</v>
       </c>
       <c r="D208" t="n">
-        <v>333455676</v>
+        <v>334122123</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D215" t="n">
-        <v>907378</v>
+        <v>908878</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>96725</v>
+        <v>96883</v>
       </c>
       <c r="D217" t="n">
-        <v>141493030</v>
+        <v>141727250</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>52747</v>
+        <v>52882</v>
       </c>
       <c r="D220" t="n">
-        <v>76233209</v>
+        <v>76425479</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D222" t="n">
-        <v>24160</v>
+        <v>25660</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4732</v>
+        <v>4736</v>
       </c>
       <c r="D223" t="n">
-        <v>6641035</v>
+        <v>6647035</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>6112</v>
+        <v>6155</v>
       </c>
       <c r="D226" t="n">
-        <v>8466100</v>
+        <v>8528238</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>108657</v>
+        <v>108921</v>
       </c>
       <c r="D229" t="n">
-        <v>135816647</v>
+        <v>136144884</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D234" t="n">
-        <v>832939</v>
+        <v>834439</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>50251</v>
+        <v>50343</v>
       </c>
       <c r="D236" t="n">
-        <v>73610986</v>
+        <v>73744891</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>12765</v>
+        <v>12820</v>
       </c>
       <c r="D238" t="n">
-        <v>18359767</v>
+        <v>18439035</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2645</v>
+        <v>2662</v>
       </c>
       <c r="D242" t="n">
-        <v>3704384</v>
+        <v>3729013</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>263879</v>
+        <v>264596</v>
       </c>
       <c r="D243" t="n">
-        <v>333156164</v>
+        <v>334067782</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D249" t="n">
-        <v>1237904</v>
+        <v>1240904</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>97521</v>
+        <v>97722</v>
       </c>
       <c r="D251" t="n">
-        <v>142890737</v>
+        <v>143185763</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>66868</v>
+        <v>67095</v>
       </c>
       <c r="D254" t="n">
-        <v>96920073</v>
+        <v>97252397</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2449</v>
+        <v>2451</v>
       </c>
       <c r="D256" t="n">
-        <v>3454224</v>
+        <v>3457224</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4892</v>
+        <v>4920</v>
       </c>
       <c r="D259" t="n">
-        <v>6873294</v>
+        <v>6908304</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-04 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>329058</v>
+        <v>329747</v>
       </c>
       <c r="D2" t="n">
-        <v>419105950</v>
+        <v>419937615</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D4" t="n">
-        <v>472192</v>
+        <v>474987</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D8" t="n">
-        <v>1288399</v>
+        <v>1289899</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>119243</v>
+        <v>119395</v>
       </c>
       <c r="D10" t="n">
-        <v>174713253</v>
+        <v>174938243</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>61080</v>
+        <v>61237</v>
       </c>
       <c r="D12" t="n">
-        <v>88144701</v>
+        <v>88372499</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4050</v>
+        <v>4051</v>
       </c>
       <c r="D16" t="n">
-        <v>5749637</v>
+        <v>5751137</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7109</v>
+        <v>7153</v>
       </c>
       <c r="D20" t="n">
-        <v>9925961</v>
+        <v>9988435</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>79172</v>
+        <v>79301</v>
       </c>
       <c r="D22" t="n">
-        <v>98626700</v>
+        <v>98769465</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32965</v>
+        <v>33001</v>
       </c>
       <c r="D28" t="n">
-        <v>48247181</v>
+        <v>48301181</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11737</v>
+        <v>11761</v>
       </c>
       <c r="D30" t="n">
-        <v>16882730</v>
+        <v>16916106</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1954</v>
+        <v>1966</v>
       </c>
       <c r="D35" t="n">
-        <v>2757992</v>
+        <v>2775092</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>99154</v>
+        <v>99303</v>
       </c>
       <c r="D36" t="n">
-        <v>124657883</v>
+        <v>124833671</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>45048</v>
+        <v>45092</v>
       </c>
       <c r="D44" t="n">
-        <v>66012119</v>
+        <v>66075533</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9373</v>
+        <v>9388</v>
       </c>
       <c r="D46" t="n">
-        <v>13441824</v>
+        <v>13463729</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2481</v>
+        <v>2502</v>
       </c>
       <c r="D51" t="n">
-        <v>3468587</v>
+        <v>3497418</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70548</v>
+        <v>70656</v>
       </c>
       <c r="D52" t="n">
-        <v>88459159</v>
+        <v>88586409</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28669</v>
+        <v>28707</v>
       </c>
       <c r="D59" t="n">
-        <v>42045742</v>
+        <v>42102120</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11407</v>
+        <v>11429</v>
       </c>
       <c r="D62" t="n">
-        <v>16492001</v>
+        <v>16523918</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D64" t="n">
-        <v>1919497</v>
+        <v>1920997</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1579</v>
+        <v>1588</v>
       </c>
       <c r="D68" t="n">
-        <v>2213851</v>
+        <v>2227351</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20929</v>
+        <v>20946</v>
       </c>
       <c r="D70" t="n">
-        <v>27404826</v>
+        <v>27428748</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7734</v>
+        <v>7741</v>
       </c>
       <c r="D74" t="n">
-        <v>11326800</v>
+        <v>11337300</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5228</v>
+        <v>5236</v>
       </c>
       <c r="D76" t="n">
-        <v>7592494</v>
+        <v>7604494</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>144006</v>
+        <v>144262</v>
       </c>
       <c r="D79" t="n">
-        <v>179451635</v>
+        <v>179743613</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D83" t="n">
-        <v>642824</v>
+        <v>645824</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64648</v>
+        <v>64752</v>
       </c>
       <c r="D85" t="n">
-        <v>94740475</v>
+        <v>94894265</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30393</v>
+        <v>30454</v>
       </c>
       <c r="D88" t="n">
-        <v>43967559</v>
+        <v>44054104</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2769</v>
+        <v>2772</v>
       </c>
       <c r="D90" t="n">
-        <v>3987143</v>
+        <v>3990652</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3000</v>
+        <v>3011</v>
       </c>
       <c r="D91" t="n">
-        <v>4242243</v>
+        <v>4255668</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>34481</v>
+        <v>34624</v>
       </c>
       <c r="D92" t="n">
-        <v>46749197</v>
+        <v>46951793</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8359</v>
+        <v>8394</v>
       </c>
       <c r="D96" t="n">
-        <v>12288126</v>
+        <v>12339821</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7729</v>
+        <v>7779</v>
       </c>
       <c r="D98" t="n">
-        <v>11216237</v>
+        <v>11290347</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D100" t="n">
-        <v>782406</v>
+        <v>786156</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D101" t="n">
-        <v>752050</v>
+        <v>756550</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11428</v>
+        <v>11642</v>
       </c>
       <c r="D102" t="n">
-        <v>18274439</v>
+        <v>18764262</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2792</v>
+        <v>2827</v>
       </c>
       <c r="D104" t="n">
-        <v>4797354</v>
+        <v>4893970</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3825</v>
+        <v>3891</v>
       </c>
       <c r="D106" t="n">
-        <v>6581934</v>
+        <v>6764869</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D108" t="n">
-        <v>285045</v>
+        <v>294045</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D109" t="n">
-        <v>359030</v>
+        <v>364530</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>145011</v>
+        <v>145328</v>
       </c>
       <c r="D110" t="n">
-        <v>179340364</v>
+        <v>179733269</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="D114" t="n">
-        <v>1409977</v>
+        <v>1410815</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53687</v>
+        <v>53777</v>
       </c>
       <c r="D116" t="n">
-        <v>78682945</v>
+        <v>78809549</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D117" t="n">
-        <v>128959</v>
+        <v>131959</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>27947</v>
+        <v>28023</v>
       </c>
       <c r="D118" t="n">
-        <v>40490219</v>
+        <v>40600436</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2398</v>
+        <v>2412</v>
       </c>
       <c r="D122" t="n">
-        <v>3372326</v>
+        <v>3392994</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>538400</v>
+        <v>540898</v>
       </c>
       <c r="D124" t="n">
-        <v>711455433</v>
+        <v>714802948</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D125" t="n">
-        <v>123789</v>
+        <v>125071</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D126" t="n">
-        <v>325509</v>
+        <v>328509</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1409</v>
+        <v>1412</v>
       </c>
       <c r="D129" t="n">
-        <v>2088214</v>
+        <v>2092714</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>214404</v>
+        <v>215029</v>
       </c>
       <c r="D131" t="n">
-        <v>315157910</v>
+        <v>316067834</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D132" t="n">
-        <v>631210</v>
+        <v>634210</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>192284</v>
+        <v>193252</v>
       </c>
       <c r="D134" t="n">
-        <v>279636318</v>
+        <v>281033776</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D136" t="n">
-        <v>48332</v>
+        <v>51332</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2887</v>
+        <v>2890</v>
       </c>
       <c r="D137" t="n">
-        <v>4053072</v>
+        <v>4057572</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6792</v>
+        <v>6842</v>
       </c>
       <c r="D140" t="n">
-        <v>9588568</v>
+        <v>9654555</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>46095</v>
+        <v>46189</v>
       </c>
       <c r="D143" t="n">
-        <v>61516197</v>
+        <v>61642790</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>14409</v>
+        <v>14434</v>
       </c>
       <c r="D149" t="n">
-        <v>21118939</v>
+        <v>21156239</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3862</v>
+        <v>3873</v>
       </c>
       <c r="D150" t="n">
-        <v>5569092</v>
+        <v>5585482</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D155" t="n">
-        <v>583813</v>
+        <v>586813</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>18156</v>
+        <v>18205</v>
       </c>
       <c r="D156" t="n">
-        <v>24002421</v>
+        <v>24065567</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7407</v>
+        <v>7427</v>
       </c>
       <c r="D160" t="n">
-        <v>10777403</v>
+        <v>10808593</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5180</v>
+        <v>5196</v>
       </c>
       <c r="D162" t="n">
-        <v>7455538</v>
+        <v>7479538</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>21046</v>
+        <v>21301</v>
       </c>
       <c r="D167" t="n">
-        <v>36877480</v>
+        <v>37579924</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2256</v>
+        <v>2271</v>
       </c>
       <c r="D168" t="n">
-        <v>3955071</v>
+        <v>3998571</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D169" t="n">
-        <v>501089</v>
+        <v>510089</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D172" t="n">
-        <v>217449</v>
+        <v>218949</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>89714</v>
+        <v>89871</v>
       </c>
       <c r="D173" t="n">
-        <v>112051640</v>
+        <v>112236808</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>34471</v>
+        <v>34508</v>
       </c>
       <c r="D180" t="n">
-        <v>50543665</v>
+        <v>50597758</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>13356</v>
+        <v>13384</v>
       </c>
       <c r="D182" t="n">
-        <v>19297802</v>
+        <v>19337488</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1264</v>
+        <v>1268</v>
       </c>
       <c r="D184" t="n">
-        <v>1768933</v>
+        <v>1774527</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1746</v>
+        <v>1753</v>
       </c>
       <c r="D186" t="n">
-        <v>2450429</v>
+        <v>2460929</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>243637</v>
+        <v>244090</v>
       </c>
       <c r="D188" t="n">
-        <v>302682416</v>
+        <v>303223086</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>88011</v>
+        <v>88137</v>
       </c>
       <c r="D196" t="n">
-        <v>128995603</v>
+        <v>129178702</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>33795</v>
+        <v>33865</v>
       </c>
       <c r="D199" t="n">
-        <v>48656175</v>
+        <v>48754132</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>5190</v>
+        <v>5193</v>
       </c>
       <c r="D202" t="n">
-        <v>7389358</v>
+        <v>7393505</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>5185</v>
+        <v>5202</v>
       </c>
       <c r="D205" t="n">
-        <v>7180301</v>
+        <v>7205801</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>270055</v>
+        <v>270566</v>
       </c>
       <c r="D208" t="n">
-        <v>334122123</v>
+        <v>334738435</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D215" t="n">
-        <v>908878</v>
+        <v>911878</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>96883</v>
+        <v>97034</v>
       </c>
       <c r="D217" t="n">
-        <v>141727250</v>
+        <v>141949861</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>52882</v>
+        <v>52979</v>
       </c>
       <c r="D220" t="n">
-        <v>76425479</v>
+        <v>76565846</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4736</v>
+        <v>4739</v>
       </c>
       <c r="D223" t="n">
-        <v>6647035</v>
+        <v>6650835</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>6155</v>
+        <v>6193</v>
       </c>
       <c r="D226" t="n">
-        <v>8528238</v>
+        <v>8582999</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>108921</v>
+        <v>109106</v>
       </c>
       <c r="D229" t="n">
-        <v>136144884</v>
+        <v>136368209</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D231" t="n">
-        <v>109013</v>
+        <v>110513</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>50343</v>
+        <v>50420</v>
       </c>
       <c r="D236" t="n">
-        <v>73744891</v>
+        <v>73858454</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D237" t="n">
-        <v>54711</v>
+        <v>56211</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>12820</v>
+        <v>12851</v>
       </c>
       <c r="D238" t="n">
-        <v>18439035</v>
+        <v>18485535</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1909</v>
+        <v>1911</v>
       </c>
       <c r="D240" t="n">
-        <v>2737382</v>
+        <v>2740382</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2662</v>
+        <v>2671</v>
       </c>
       <c r="D242" t="n">
-        <v>3729013</v>
+        <v>3741506</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>264596</v>
+        <v>265132</v>
       </c>
       <c r="D243" t="n">
-        <v>334067782</v>
+        <v>334739703</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D249" t="n">
-        <v>1240904</v>
+        <v>1242404</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D250" t="n">
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>97722</v>
+        <v>97909</v>
       </c>
       <c r="D251" t="n">
-        <v>143185763</v>
+        <v>143454141</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D252" t="n">
-        <v>112661</v>
+        <v>114161</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>67095</v>
+        <v>67267</v>
       </c>
       <c r="D254" t="n">
-        <v>97252397</v>
+        <v>97506155</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2451</v>
+        <v>2452</v>
       </c>
       <c r="D256" t="n">
-        <v>3457224</v>
+        <v>3458724</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4920</v>
+        <v>4944</v>
       </c>
       <c r="D259" t="n">
-        <v>6908304</v>
+        <v>6943190</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-07 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H259"/>
+  <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>330296</v>
+        <v>331014</v>
       </c>
       <c r="D2" t="n">
-        <v>420628070</v>
+        <v>421514655</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D3" t="n">
-        <v>316083</v>
+        <v>317212</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D4" t="n">
-        <v>474987</v>
+        <v>479093</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="D8" t="n">
-        <v>1289899</v>
+        <v>1291399</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>119488</v>
+        <v>119690</v>
       </c>
       <c r="D10" t="n">
-        <v>175068467</v>
+        <v>175362277</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>61321</v>
+        <v>61481</v>
       </c>
       <c r="D12" t="n">
-        <v>88493445</v>
+        <v>88720715</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4052</v>
+        <v>4053</v>
       </c>
       <c r="D16" t="n">
-        <v>5752637</v>
+        <v>5754137</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7184</v>
+        <v>7219</v>
       </c>
       <c r="D20" t="n">
-        <v>10030422</v>
+        <v>10081884</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>79411</v>
+        <v>79564</v>
       </c>
       <c r="D22" t="n">
-        <v>98892614</v>
+        <v>99077086</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D27" t="n">
-        <v>416147</v>
+        <v>417647</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>33028</v>
+        <v>33079</v>
       </c>
       <c r="D28" t="n">
-        <v>48338559</v>
+        <v>48412393</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11789</v>
+        <v>11819</v>
       </c>
       <c r="D30" t="n">
-        <v>16957239</v>
+        <v>17001178</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1973</v>
+        <v>1981</v>
       </c>
       <c r="D35" t="n">
-        <v>2785592</v>
+        <v>2796551</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>99434</v>
+        <v>99610</v>
       </c>
       <c r="D36" t="n">
-        <v>124983216</v>
+        <v>125190018</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>45118</v>
+        <v>45189</v>
       </c>
       <c r="D44" t="n">
-        <v>66111143</v>
+        <v>66216474</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9406</v>
+        <v>9425</v>
       </c>
       <c r="D46" t="n">
-        <v>13487123</v>
+        <v>13514165</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1430</v>
+        <v>1432</v>
       </c>
       <c r="D48" t="n">
-        <v>1987311</v>
+        <v>1990311</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2506</v>
+        <v>2515</v>
       </c>
       <c r="D51" t="n">
-        <v>3503418</v>
+        <v>3515911</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70758</v>
+        <v>70884</v>
       </c>
       <c r="D52" t="n">
-        <v>88709482</v>
+        <v>88859442</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>28747</v>
+        <v>28789</v>
       </c>
       <c r="D59" t="n">
-        <v>42158657</v>
+        <v>42220415</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11437</v>
+        <v>11461</v>
       </c>
       <c r="D62" t="n">
-        <v>16534544</v>
+        <v>16568555</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1376</v>
+        <v>1382</v>
       </c>
       <c r="D64" t="n">
-        <v>1923997</v>
+        <v>1931101</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1591</v>
+        <v>1601</v>
       </c>
       <c r="D68" t="n">
-        <v>2231363</v>
+        <v>2245161</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>20970</v>
+        <v>20991</v>
       </c>
       <c r="D70" t="n">
-        <v>27458383</v>
+        <v>27487602</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7749</v>
+        <v>7767</v>
       </c>
       <c r="D74" t="n">
-        <v>11349148</v>
+        <v>11375744</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5244</v>
+        <v>5261</v>
       </c>
       <c r="D76" t="n">
-        <v>7615294</v>
+        <v>7640466</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D78" t="n">
-        <v>411083</v>
+        <v>412583</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>144456</v>
+        <v>144689</v>
       </c>
       <c r="D79" t="n">
-        <v>179976756</v>
+        <v>180248386</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D83" t="n">
-        <v>645824</v>
+        <v>647324</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>64793</v>
+        <v>64878</v>
       </c>
       <c r="D85" t="n">
-        <v>94954309</v>
+        <v>95073438</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>30492</v>
+        <v>30544</v>
       </c>
       <c r="D88" t="n">
-        <v>44108470</v>
+        <v>44185513</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3026</v>
+        <v>3039</v>
       </c>
       <c r="D91" t="n">
-        <v>4276010</v>
+        <v>4293280</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>34744</v>
+        <v>34821</v>
       </c>
       <c r="D92" t="n">
-        <v>47110522</v>
+        <v>47215432</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8419</v>
+        <v>8442</v>
       </c>
       <c r="D96" t="n">
-        <v>12376097</v>
+        <v>12410597</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7806</v>
+        <v>7818</v>
       </c>
       <c r="D98" t="n">
-        <v>11330807</v>
+        <v>11348455</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D101" t="n">
-        <v>758050</v>
+        <v>761050</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11789</v>
+        <v>11891</v>
       </c>
       <c r="D102" t="n">
-        <v>19125984</v>
+        <v>19383569</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2857</v>
+        <v>2883</v>
       </c>
       <c r="D104" t="n">
-        <v>4980170</v>
+        <v>5049526</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3937</v>
+        <v>3968</v>
       </c>
       <c r="D106" t="n">
-        <v>6892269</v>
+        <v>6977462</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D107" t="n">
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D108" t="n">
-        <v>294045</v>
+        <v>300345</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D109" t="n">
-        <v>370530</v>
+        <v>381205</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,29 +4524,29 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>145523</v>
+        <v>4</v>
       </c>
       <c r="D110" t="n">
-        <v>179972407</v>
+        <v>6000</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>03</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Hauts-de-France</t>
+          <t>Guyane</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>34</v>
+        <v>145782</v>
       </c>
       <c r="D111" t="n">
-        <v>44717</v>
+        <v>180284401</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4579,12 +4579,12 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="D112" t="n">
-        <v>104557</v>
+        <v>44717</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4617,12 +4617,12 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="D113" t="n">
-        <v>10395</v>
+        <v>104557</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4655,12 +4655,12 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>962</v>
+        <v>7</v>
       </c>
       <c r="D114" t="n">
-        <v>1410815</v>
+        <v>10395</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4693,12 +4693,12 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>5</v>
+        <v>962</v>
       </c>
       <c r="D115" t="n">
-        <v>7100</v>
+        <v>1410815</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4731,12 +4731,12 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>53812</v>
+        <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>78857461</v>
+        <v>7100</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4769,12 +4769,12 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>89</v>
+        <v>53903</v>
       </c>
       <c r="D117" t="n">
-        <v>131959</v>
+        <v>78985498</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4807,12 +4807,12 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>28073</v>
+        <v>89</v>
       </c>
       <c r="D118" t="n">
-        <v>40671950</v>
+        <v>131959</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4845,12 +4845,12 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1326</v>
+        <v>28145</v>
       </c>
       <c r="D119" t="n">
-        <v>1813694</v>
+        <v>40774131</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4883,12 +4883,12 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4</v>
+        <v>1326</v>
       </c>
       <c r="D120" t="n">
-        <v>6000</v>
+        <v>1813694</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4921,12 +4921,12 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Organisme mutualiste</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D121" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4959,12 +4959,12 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>82</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Organisme mutualiste</t>
         </is>
       </c>
     </row>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2414</v>
+        <v>3</v>
       </c>
       <c r="D122" t="n">
-        <v>3395994</v>
+        <v>4500</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -4997,12 +4997,12 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>11</v>
+        <v>2427</v>
       </c>
       <c r="D123" t="n">
-        <v>16500</v>
+        <v>3414954</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5035,12 +5035,12 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -5056,29 +5056,29 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>543135</v>
+        <v>11</v>
       </c>
       <c r="D124" t="n">
-        <v>717740829</v>
+        <v>16500</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>32</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Île-de-France</t>
+          <t>Hauts-de-France</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>94</v>
+        <v>545189</v>
       </c>
       <c r="D125" t="n">
-        <v>125071</v>
+        <v>720461684</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5111,12 +5111,12 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>223</v>
+        <v>94</v>
       </c>
       <c r="D126" t="n">
-        <v>328509</v>
+        <v>125071</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5149,12 +5149,12 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>8</v>
+        <v>224</v>
       </c>
       <c r="D127" t="n">
-        <v>12000</v>
+        <v>330009</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5187,12 +5187,12 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D128" t="n">
-        <v>35998</v>
+        <v>12000</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5225,12 +5225,12 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1415</v>
+        <v>24</v>
       </c>
       <c r="D129" t="n">
-        <v>2097214</v>
+        <v>35998</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5263,12 +5263,12 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>32</v>
+        <v>1422</v>
       </c>
       <c r="D130" t="n">
-        <v>42010</v>
+        <v>2105752</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5301,12 +5301,12 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>215477</v>
+        <v>32</v>
       </c>
       <c r="D131" t="n">
-        <v>316715341</v>
+        <v>42010</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5339,12 +5339,12 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>425</v>
+        <v>216060</v>
       </c>
       <c r="D132" t="n">
-        <v>634210</v>
+        <v>317568496</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5377,12 +5377,12 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>13</v>
+        <v>428</v>
       </c>
       <c r="D133" t="n">
-        <v>19500</v>
+        <v>638710</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5415,12 +5415,12 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>193946</v>
+        <v>13</v>
       </c>
       <c r="D134" t="n">
-        <v>282040188</v>
+        <v>19500</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5453,12 +5453,12 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>4</v>
+        <v>194695</v>
       </c>
       <c r="D135" t="n">
-        <v>6000</v>
+        <v>283133921</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5491,12 +5491,12 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Société européenne</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D136" t="n">
-        <v>51332</v>
+        <v>6000</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5529,12 +5529,12 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société européenne</t>
         </is>
       </c>
     </row>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2891</v>
+        <v>36</v>
       </c>
       <c r="D137" t="n">
-        <v>4059072</v>
+        <v>52832</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5567,12 +5567,12 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>3</v>
+        <v>2893</v>
       </c>
       <c r="D138" t="n">
-        <v>4133</v>
+        <v>4061096</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5605,12 +5605,12 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Comité d'entreprise</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D139" t="n">
-        <v>17722</v>
+        <v>4133</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5643,12 +5643,12 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Comité d'entreprise</t>
         </is>
       </c>
     </row>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6874</v>
+        <v>12</v>
       </c>
       <c r="D140" t="n">
-        <v>9698876</v>
+        <v>17722</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5681,12 +5681,12 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>4</v>
+        <v>6918</v>
       </c>
       <c r="D141" t="n">
-        <v>6000</v>
+        <v>9763471</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5719,12 +5719,12 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D142" t="n">
-        <v>24000</v>
+        <v>6000</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5757,12 +5757,12 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -5778,29 +5778,29 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>46259</v>
+        <v>16</v>
       </c>
       <c r="D143" t="n">
-        <v>61739950</v>
+        <v>24000</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>La Réunion</t>
+          <t>Île-de-France</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>29</v>
+        <v>46368</v>
       </c>
       <c r="D144" t="n">
-        <v>40262</v>
+        <v>61881593</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5833,12 +5833,12 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D145" t="n">
-        <v>36230</v>
+        <v>40262</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5871,12 +5871,12 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D146" t="n">
-        <v>9000</v>
+        <v>36230</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5909,12 +5909,12 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -5947,12 +5947,12 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>452</v>
+        <v>6</v>
       </c>
       <c r="D148" t="n">
-        <v>677665</v>
+        <v>9000</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -5985,12 +5985,12 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>14444</v>
+        <v>452</v>
       </c>
       <c r="D149" t="n">
-        <v>21170094</v>
+        <v>677665</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6023,12 +6023,12 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>3880</v>
+        <v>14468</v>
       </c>
       <c r="D150" t="n">
-        <v>5594931</v>
+        <v>21205116</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6061,12 +6061,12 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>8</v>
+        <v>3886</v>
       </c>
       <c r="D151" t="n">
-        <v>12000</v>
+        <v>5603931</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6099,12 +6099,12 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D152" t="n">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6137,12 +6137,12 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>407</v>
+        <v>7</v>
       </c>
       <c r="D153" t="n">
-        <v>585716</v>
+        <v>10500</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6175,12 +6175,12 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>3</v>
+        <v>407</v>
       </c>
       <c r="D154" t="n">
-        <v>4500</v>
+        <v>585716</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6213,12 +6213,12 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>417</v>
+        <v>3</v>
       </c>
       <c r="D155" t="n">
-        <v>588313</v>
+        <v>4500</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6251,12 +6251,12 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>91</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Syndicat de propriétaires</t>
         </is>
       </c>
     </row>
@@ -6272,29 +6272,29 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>18250</v>
+        <v>418</v>
       </c>
       <c r="D156" t="n">
-        <v>24130080</v>
+        <v>589813</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Martinique</t>
+          <t>La Réunion</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>8</v>
+        <v>18291</v>
       </c>
       <c r="D157" t="n">
-        <v>10626</v>
+        <v>24184953</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6327,12 +6327,12 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D158" t="n">
-        <v>6000</v>
+        <v>10626</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6365,12 +6365,12 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D159" t="n">
-        <v>79406</v>
+        <v>6000</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6403,12 +6403,12 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7452</v>
+        <v>54</v>
       </c>
       <c r="D160" t="n">
-        <v>10846728</v>
+        <v>79406</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6441,12 +6441,12 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4</v>
+        <v>7463</v>
       </c>
       <c r="D161" t="n">
-        <v>6000</v>
+        <v>10861708</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6479,12 +6479,12 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5214</v>
+        <v>4</v>
       </c>
       <c r="D162" t="n">
-        <v>7505821</v>
+        <v>6000</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6517,12 +6517,12 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>4</v>
+        <v>5230</v>
       </c>
       <c r="D163" t="n">
-        <v>5310</v>
+        <v>7529775</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6555,12 +6555,12 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>285</v>
+        <v>4</v>
       </c>
       <c r="D164" t="n">
-        <v>394139</v>
+        <v>5310</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6593,12 +6593,12 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D165" t="n">
-        <v>401664</v>
+        <v>394139</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6631,12 +6631,12 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>4</v>
+        <v>281</v>
       </c>
       <c r="D166" t="n">
-        <v>5750</v>
+        <v>401664</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6669,12 +6669,12 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6690,29 +6690,29 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>21587</v>
+        <v>4</v>
       </c>
       <c r="D167" t="n">
-        <v>38346680</v>
+        <v>5750</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>02</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Mayotte</t>
+          <t>Martinique</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2295</v>
+        <v>21772</v>
       </c>
       <c r="D168" t="n">
-        <v>4067571</v>
+        <v>38821584</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6745,12 +6745,12 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>301</v>
+        <v>2308</v>
       </c>
       <c r="D169" t="n">
-        <v>522089</v>
+        <v>4104071</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6783,12 +6783,12 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>4</v>
+        <v>305</v>
       </c>
       <c r="D170" t="n">
-        <v>6000</v>
+        <v>531089</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6821,12 +6821,12 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="D171" t="n">
-        <v>131690</v>
+        <v>6000</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6859,12 +6859,12 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="D172" t="n">
-        <v>218949</v>
+        <v>131690</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6897,12 +6897,12 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -6918,29 +6918,29 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>89977</v>
+        <v>122</v>
       </c>
       <c r="D173" t="n">
-        <v>112364889</v>
+        <v>224949</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>06</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>Normandie</t>
+          <t>Mayotte</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>32</v>
+        <v>90108</v>
       </c>
       <c r="D174" t="n">
-        <v>37159</v>
+        <v>112523253</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6973,12 +6973,12 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="D175" t="n">
-        <v>124454</v>
+        <v>37159</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7011,12 +7011,12 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D176" t="n">
-        <v>3961</v>
+        <v>124454</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7049,12 +7049,12 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D177" t="n">
-        <v>21889</v>
+        <v>3961</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7087,12 +7087,12 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>646</v>
+        <v>15</v>
       </c>
       <c r="D178" t="n">
-        <v>952088</v>
+        <v>21889</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7125,12 +7125,12 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>4</v>
+        <v>646</v>
       </c>
       <c r="D179" t="n">
-        <v>6000</v>
+        <v>952088</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7163,12 +7163,12 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>34532</v>
+        <v>4</v>
       </c>
       <c r="D180" t="n">
-        <v>50632229</v>
+        <v>6000</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7201,12 +7201,12 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>29</v>
+        <v>34602</v>
       </c>
       <c r="D181" t="n">
-        <v>43500</v>
+        <v>50734709</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7239,12 +7239,12 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>13410</v>
+        <v>29</v>
       </c>
       <c r="D182" t="n">
-        <v>19375414</v>
+        <v>43500</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7277,12 +7277,12 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>10</v>
+        <v>13432</v>
       </c>
       <c r="D183" t="n">
-        <v>13919</v>
+        <v>19406925</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7315,12 +7315,12 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1269</v>
+        <v>10</v>
       </c>
       <c r="D184" t="n">
-        <v>1776027</v>
+        <v>13919</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7353,12 +7353,12 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>4</v>
+        <v>1270</v>
       </c>
       <c r="D185" t="n">
-        <v>5839</v>
+        <v>1777527</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7391,12 +7391,12 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1755</v>
+        <v>4</v>
       </c>
       <c r="D186" t="n">
-        <v>2463929</v>
+        <v>5839</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7429,12 +7429,12 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>4</v>
+        <v>1767</v>
       </c>
       <c r="D187" t="n">
-        <v>6000</v>
+        <v>2480717</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7467,12 +7467,12 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -7488,29 +7488,29 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>244403</v>
+        <v>4</v>
       </c>
       <c r="D188" t="n">
-        <v>303594093</v>
+        <v>6000</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>Nouvelle-Aquitaine</t>
+          <t>Normandie</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>137</v>
+        <v>244780</v>
       </c>
       <c r="D189" t="n">
-        <v>147587</v>
+        <v>304043127</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7543,12 +7543,12 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="D190" t="n">
-        <v>251236</v>
+        <v>147587</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7581,12 +7581,12 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="D191" t="n">
-        <v>6741</v>
+        <v>251236</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7619,12 +7619,12 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D192" t="n">
-        <v>13500</v>
+        <v>6741</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7657,12 +7657,12 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>Paroisse hors zone concordataire</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D193" t="n">
-        <v>10795</v>
+        <v>13500</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7695,12 +7695,12 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Paroisse hors zone concordataire</t>
         </is>
       </c>
     </row>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>893</v>
+        <v>10</v>
       </c>
       <c r="D194" t="n">
-        <v>1313845</v>
+        <v>10795</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7733,12 +7733,12 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>7</v>
+        <v>893</v>
       </c>
       <c r="D195" t="n">
-        <v>9883</v>
+        <v>1313845</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7771,12 +7771,12 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>88215</v>
+        <v>7</v>
       </c>
       <c r="D196" t="n">
-        <v>129289770</v>
+        <v>9883</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7809,12 +7809,12 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>96</v>
+        <v>88345</v>
       </c>
       <c r="D197" t="n">
-        <v>139627</v>
+        <v>129476232</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7847,12 +7847,12 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D198" t="n">
-        <v>6000</v>
+        <v>139627</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7885,12 +7885,12 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>33911</v>
+        <v>4</v>
       </c>
       <c r="D199" t="n">
-        <v>48817678</v>
+        <v>6000</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7923,12 +7923,12 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>26</v>
+        <v>33987</v>
       </c>
       <c r="D200" t="n">
-        <v>39000</v>
+        <v>48924583</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7961,12 +7961,12 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D201" t="n">
-        <v>23608</v>
+        <v>39000</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -7999,12 +7999,12 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>5194</v>
+        <v>17</v>
       </c>
       <c r="D202" t="n">
-        <v>7395005</v>
+        <v>23608</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8037,12 +8037,12 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>3</v>
+        <v>5199</v>
       </c>
       <c r="D203" t="n">
-        <v>4500</v>
+        <v>7402505</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8075,12 +8075,12 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Comité d'entreprise</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D204" t="n">
-        <v>15000</v>
+        <v>4500</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8113,12 +8113,12 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Comité d'entreprise</t>
         </is>
       </c>
     </row>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>5212</v>
+        <v>10</v>
       </c>
       <c r="D205" t="n">
-        <v>7217775</v>
+        <v>15000</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8151,12 +8151,12 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8172,10 +8172,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>4</v>
+        <v>5230</v>
       </c>
       <c r="D206" t="n">
-        <v>6000</v>
+        <v>7238171</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -8189,12 +8189,12 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D207" t="n">
-        <v>12679</v>
+        <v>6000</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8227,12 +8227,12 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -8248,29 +8248,29 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>270954</v>
+        <v>10</v>
       </c>
       <c r="D208" t="n">
-        <v>335204816</v>
+        <v>12679</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Occitanie</t>
+          <t>Nouvelle-Aquitaine</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>161</v>
+        <v>271456</v>
       </c>
       <c r="D209" t="n">
-        <v>177913</v>
+        <v>335811602</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8303,12 +8303,12 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>259</v>
+        <v>161</v>
       </c>
       <c r="D210" t="n">
-        <v>370039</v>
+        <v>177913</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8341,12 +8341,12 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -8362,10 +8362,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>17</v>
+        <v>259</v>
       </c>
       <c r="D211" t="n">
-        <v>23935</v>
+        <v>370039</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -8379,12 +8379,12 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D212" t="n">
-        <v>12731</v>
+        <v>23935</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8417,12 +8417,12 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D213" t="n">
-        <v>4500</v>
+        <v>12731</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8455,12 +8455,12 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -8493,12 +8493,12 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>628</v>
+        <v>3</v>
       </c>
       <c r="D215" t="n">
-        <v>914878</v>
+        <v>4500</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8531,12 +8531,12 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>5</v>
+        <v>628</v>
       </c>
       <c r="D216" t="n">
-        <v>7500</v>
+        <v>914878</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8569,12 +8569,12 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>97125</v>
+        <v>5</v>
       </c>
       <c r="D217" t="n">
-        <v>142083087</v>
+        <v>7500</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8607,12 +8607,12 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>97</v>
+        <v>97303</v>
       </c>
       <c r="D218" t="n">
-        <v>144699</v>
+        <v>142338754</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8645,12 +8645,12 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="D219" t="n">
-        <v>10500</v>
+        <v>144699</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8683,12 +8683,12 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>53039</v>
+        <v>7</v>
       </c>
       <c r="D220" t="n">
-        <v>76653644</v>
+        <v>10500</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8721,12 +8721,12 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>34</v>
+        <v>53134</v>
       </c>
       <c r="D221" t="n">
-        <v>48922</v>
+        <v>76789540</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8759,12 +8759,12 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D222" t="n">
-        <v>25660</v>
+        <v>48922</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8797,12 +8797,12 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4739</v>
+        <v>18</v>
       </c>
       <c r="D223" t="n">
-        <v>6650835</v>
+        <v>25660</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8835,12 +8835,12 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>7</v>
+        <v>4742</v>
       </c>
       <c r="D224" t="n">
-        <v>10500</v>
+        <v>6655155</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8873,12 +8873,12 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D225" t="n">
-        <v>29238</v>
+        <v>10500</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8911,12 +8911,12 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>69</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Autre personne morale de droit privé inscrite au registre du commerce et des sociétés</t>
         </is>
       </c>
     </row>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>6216</v>
+        <v>20</v>
       </c>
       <c r="D226" t="n">
-        <v>8612618</v>
+        <v>29238</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -8949,12 +8949,12 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>8</v>
+        <v>6257</v>
       </c>
       <c r="D227" t="n">
-        <v>12000</v>
+        <v>8666861</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -8987,12 +8987,12 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D228" t="n">
-        <v>10500</v>
+        <v>12000</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9025,12 +9025,12 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>93</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Autre personne morale de droit privé</t>
+          <t>Fondation</t>
         </is>
       </c>
     </row>
@@ -9046,29 +9046,29 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>109243</v>
+        <v>7</v>
       </c>
       <c r="D229" t="n">
-        <v>136530613</v>
+        <v>10500</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>76</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Pays de la Loire</t>
+          <t>Occitanie</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Autre personne morale de droit privé</t>
         </is>
       </c>
     </row>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>76</v>
+        <v>109482</v>
       </c>
       <c r="D230" t="n">
-        <v>80550</v>
+        <v>136823900</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9101,12 +9101,12 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D231" t="n">
-        <v>112013</v>
+        <v>80550</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9139,12 +9139,12 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D232" t="n">
-        <v>14147</v>
+        <v>112013</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9177,12 +9177,12 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D233" t="n">
-        <v>3655</v>
+        <v>14147</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9215,12 +9215,12 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>571</v>
+        <v>3</v>
       </c>
       <c r="D234" t="n">
-        <v>834439</v>
+        <v>3655</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9253,12 +9253,12 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>4</v>
+        <v>571</v>
       </c>
       <c r="D235" t="n">
-        <v>2563</v>
+        <v>834439</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9291,12 +9291,12 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>50469</v>
+        <v>4</v>
       </c>
       <c r="D236" t="n">
-        <v>73928892</v>
+        <v>2563</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9329,12 +9329,12 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>40</v>
+        <v>50551</v>
       </c>
       <c r="D237" t="n">
-        <v>57711</v>
+        <v>74049228</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9367,12 +9367,12 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>12873</v>
+        <v>41</v>
       </c>
       <c r="D238" t="n">
-        <v>18517067</v>
+        <v>59211</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9405,12 +9405,12 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>13</v>
+        <v>12899</v>
       </c>
       <c r="D239" t="n">
-        <v>13183</v>
+        <v>18554363</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9443,12 +9443,12 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1911</v>
+        <v>13</v>
       </c>
       <c r="D240" t="n">
-        <v>2740382</v>
+        <v>13183</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9481,12 +9481,12 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>7</v>
+        <v>1911</v>
       </c>
       <c r="D241" t="n">
-        <v>8596</v>
+        <v>2740382</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9519,12 +9519,12 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2679</v>
+        <v>7</v>
       </c>
       <c r="D242" t="n">
-        <v>3753506</v>
+        <v>8596</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9557,12 +9557,12 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -9578,29 +9578,29 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>265590</v>
+        <v>2688</v>
       </c>
       <c r="D243" t="n">
-        <v>335314089</v>
+        <v>3766522</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>174</v>
+        <v>266089</v>
       </c>
       <c r="D244" t="n">
-        <v>215181</v>
+        <v>335938341</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9633,12 +9633,12 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>253</v>
+        <v>177</v>
       </c>
       <c r="D245" t="n">
-        <v>363312</v>
+        <v>219355</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9671,12 +9671,12 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="D246" t="n">
-        <v>22500</v>
+        <v>364812</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9709,12 +9709,12 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D247" t="n">
-        <v>24000</v>
+        <v>22500</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9747,12 +9747,12 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D248" t="n">
-        <v>20480</v>
+        <v>24000</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9785,12 +9785,12 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>846</v>
+        <v>14</v>
       </c>
       <c r="D249" t="n">
-        <v>1242404</v>
+        <v>20480</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9823,12 +9823,12 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>11</v>
+        <v>848</v>
       </c>
       <c r="D250" t="n">
-        <v>16500</v>
+        <v>1245404</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9861,12 +9861,12 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>98002</v>
+        <v>11</v>
       </c>
       <c r="D251" t="n">
-        <v>143590654</v>
+        <v>16500</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9899,12 +9899,12 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>78</v>
+        <v>98174</v>
       </c>
       <c r="D252" t="n">
-        <v>114161</v>
+        <v>143845890</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9937,12 +9937,12 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D253" t="n">
-        <v>7500</v>
+        <v>114161</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9975,12 +9975,12 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>67385</v>
+        <v>5</v>
       </c>
       <c r="D254" t="n">
-        <v>97677937</v>
+        <v>7500</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10013,12 +10013,12 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>16</v>
+        <v>67543</v>
       </c>
       <c r="D255" t="n">
-        <v>23989</v>
+        <v>97906499</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10051,12 +10051,12 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2453</v>
+        <v>16</v>
       </c>
       <c r="D256" t="n">
-        <v>3460224</v>
+        <v>23989</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10089,12 +10089,12 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>10</v>
+        <v>2455</v>
       </c>
       <c r="D257" t="n">
-        <v>15000</v>
+        <v>3462672</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10127,12 +10127,12 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D258" t="n">
-        <v>10500</v>
+        <v>16500</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10165,12 +10165,12 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4959</v>
+        <v>7</v>
       </c>
       <c r="D259" t="n">
-        <v>6963977</v>
+        <v>10500</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10203,10 +10203,48 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>Syndicat de propriétaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>4982</v>
+      </c>
+      <c r="D260" t="n">
+        <v>6996114</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
           <t>92</t>
         </is>
       </c>
-      <c r="H259" t="inlineStr">
+      <c r="H260" t="inlineStr">
         <is>
           <t>Association loi 1901 ou assimilé</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-20 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>333240</v>
+        <v>335634</v>
       </c>
       <c r="D2" t="n">
-        <v>424263660</v>
+        <v>427170753</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D3" t="n">
-        <v>322292</v>
+        <v>325292</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D4" t="n">
-        <v>485093</v>
+        <v>491093</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="D8" t="n">
-        <v>1291399</v>
+        <v>1298899</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>120327</v>
+        <v>121003</v>
       </c>
       <c r="D10" t="n">
-        <v>176276802</v>
+        <v>177252782</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>61973</v>
+        <v>62480</v>
       </c>
       <c r="D12" t="n">
-        <v>89446117</v>
+        <v>90170616</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4058</v>
+        <v>4077</v>
       </c>
       <c r="D16" t="n">
-        <v>5761637</v>
+        <v>5788399</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D19" t="n">
-        <v>107535</v>
+        <v>112035</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7383</v>
+        <v>7541</v>
       </c>
       <c r="D21" t="n">
-        <v>10317634</v>
+        <v>10536768</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>80024</v>
+        <v>80560</v>
       </c>
       <c r="D23" t="n">
-        <v>99601113</v>
+        <v>100229018</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D25" t="n">
-        <v>54234</v>
+        <v>55734</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D28" t="n">
-        <v>417647</v>
+        <v>419147</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>33228</v>
+        <v>33390</v>
       </c>
       <c r="D29" t="n">
-        <v>48629780</v>
+        <v>48865597</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11894</v>
+        <v>11968</v>
       </c>
       <c r="D31" t="n">
-        <v>17108101</v>
+        <v>17215877</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1581</v>
+        <v>1588</v>
       </c>
       <c r="D34" t="n">
-        <v>2221891</v>
+        <v>2231591</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2017</v>
+        <v>2050</v>
       </c>
       <c r="D36" t="n">
-        <v>2849070</v>
+        <v>2894384</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>100136</v>
+        <v>100727</v>
       </c>
       <c r="D37" t="n">
-        <v>125814027</v>
+        <v>126514597</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="D43" t="n">
-        <v>1336685</v>
+        <v>1341185</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>45392</v>
+        <v>45623</v>
       </c>
       <c r="D45" t="n">
-        <v>66509432</v>
+        <v>66842898</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D46" t="n">
-        <v>38950</v>
+        <v>40450</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>9486</v>
+        <v>9543</v>
       </c>
       <c r="D47" t="n">
-        <v>13600140</v>
+        <v>13682607</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D48" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1435</v>
+        <v>1447</v>
       </c>
       <c r="D49" t="n">
-        <v>1994129</v>
+        <v>2011327</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2577</v>
+        <v>2638</v>
       </c>
       <c r="D52" t="n">
-        <v>3603582</v>
+        <v>3690157</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>71317</v>
+        <v>71809</v>
       </c>
       <c r="D53" t="n">
-        <v>89374780</v>
+        <v>89957930</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D58" t="n">
-        <v>566874</v>
+        <v>568374</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>28934</v>
+        <v>29090</v>
       </c>
       <c r="D60" t="n">
-        <v>42433452</v>
+        <v>42655732</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>11539</v>
+        <v>11629</v>
       </c>
       <c r="D63" t="n">
-        <v>16681152</v>
+        <v>16804430</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1390</v>
+        <v>1396</v>
       </c>
       <c r="D65" t="n">
-        <v>1943080</v>
+        <v>1952080</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1644</v>
+        <v>1675</v>
       </c>
       <c r="D69" t="n">
-        <v>2304397</v>
+        <v>2348940</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>21192</v>
+        <v>21387</v>
       </c>
       <c r="D71" t="n">
-        <v>27749671</v>
+        <v>27995910</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D72" t="n">
-        <v>43781</v>
+        <v>44600</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D74" t="n">
-        <v>90573</v>
+        <v>93573</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>7834</v>
+        <v>7911</v>
       </c>
       <c r="D75" t="n">
-        <v>11474555</v>
+        <v>11587181</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>5321</v>
+        <v>5356</v>
       </c>
       <c r="D77" t="n">
-        <v>7730466</v>
+        <v>7781826</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D78" t="n">
-        <v>715560</v>
+        <v>721560</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="D79" t="n">
-        <v>423083</v>
+        <v>435083</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>145453</v>
+        <v>146395</v>
       </c>
       <c r="D80" t="n">
-        <v>181140906</v>
+        <v>182230400</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D81" t="n">
-        <v>84766</v>
+        <v>86266</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D83" t="n">
-        <v>29650</v>
+        <v>31610</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="D84" t="n">
-        <v>651583</v>
+        <v>660583</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>65180</v>
+        <v>65482</v>
       </c>
       <c r="D86" t="n">
-        <v>95506819</v>
+        <v>95942450</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D88" t="n">
-        <v>15000</v>
+        <v>19500</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>30695</v>
+        <v>30884</v>
       </c>
       <c r="D89" t="n">
-        <v>44403593</v>
+        <v>44673124</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2783</v>
+        <v>2808</v>
       </c>
       <c r="D91" t="n">
-        <v>4007152</v>
+        <v>4044652</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3085</v>
+        <v>3143</v>
       </c>
       <c r="D92" t="n">
-        <v>4356545</v>
+        <v>4434119</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>35154</v>
+        <v>35548</v>
       </c>
       <c r="D93" t="n">
-        <v>47668900</v>
+        <v>48207329</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8540</v>
+        <v>8655</v>
       </c>
       <c r="D97" t="n">
-        <v>12552955</v>
+        <v>12720584</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7903</v>
+        <v>8019</v>
       </c>
       <c r="D99" t="n">
-        <v>11468508</v>
+        <v>11636561</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D101" t="n">
-        <v>800083</v>
+        <v>809876</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="D102" t="n">
-        <v>769560</v>
+        <v>781560</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>12532</v>
+        <v>13088</v>
       </c>
       <c r="D103" t="n">
-        <v>20926306</v>
+        <v>22254511</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>3013</v>
+        <v>3117</v>
       </c>
       <c r="D105" t="n">
-        <v>5405521</v>
+        <v>5696059</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4158</v>
+        <v>4325</v>
       </c>
       <c r="D107" t="n">
-        <v>7484911</v>
+        <v>7925494</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D109" t="n">
-        <v>321120</v>
+        <v>336120</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="D110" t="n">
-        <v>408755</v>
+        <v>453673</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>146658</v>
+        <v>147587</v>
       </c>
       <c r="D112" t="n">
-        <v>181333858</v>
+        <v>182416420</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D114" t="n">
-        <v>104557</v>
+        <v>106057</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="D116" t="n">
-        <v>1413815</v>
+        <v>1416815</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>54248</v>
+        <v>54557</v>
       </c>
       <c r="D118" t="n">
-        <v>79482713</v>
+        <v>79920656</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D119" t="n">
-        <v>131959</v>
+        <v>134959</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>28382</v>
+        <v>28631</v>
       </c>
       <c r="D120" t="n">
-        <v>41121005</v>
+        <v>41473936</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1329</v>
+        <v>1338</v>
       </c>
       <c r="D121" t="n">
-        <v>1818194</v>
+        <v>1831694</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>2479</v>
+        <v>2531</v>
       </c>
       <c r="D124" t="n">
-        <v>3486952</v>
+        <v>3563495</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>551601</v>
+        <v>559071</v>
       </c>
       <c r="D126" t="n">
-        <v>728760072</v>
+        <v>738431919</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D127" t="n">
-        <v>128071</v>
+        <v>129755</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D128" t="n">
-        <v>334509</v>
+        <v>336009</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1429</v>
+        <v>1448</v>
       </c>
       <c r="D131" t="n">
-        <v>2115317</v>
+        <v>2143817</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>218055</v>
+        <v>220581</v>
       </c>
       <c r="D133" t="n">
-        <v>320462567</v>
+        <v>324138075</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="D134" t="n">
-        <v>655210</v>
+        <v>671710</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D135" t="n">
-        <v>19500</v>
+        <v>24000</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>197134</v>
+        <v>199895</v>
       </c>
       <c r="D136" t="n">
-        <v>286653425</v>
+        <v>290658537</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2911</v>
+        <v>2931</v>
       </c>
       <c r="D139" t="n">
-        <v>4087496</v>
+        <v>4116072</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>7060</v>
+        <v>7244</v>
       </c>
       <c r="D142" t="n">
-        <v>9962577</v>
+        <v>10221446</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>46747</v>
+        <v>47237</v>
       </c>
       <c r="D145" t="n">
-        <v>62364009</v>
+        <v>63016528</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D146" t="n">
-        <v>40262</v>
+        <v>41762</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>14548</v>
+        <v>14664</v>
       </c>
       <c r="D151" t="n">
-        <v>21320445</v>
+        <v>21492138</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>3908</v>
+        <v>3953</v>
       </c>
       <c r="D152" t="n">
-        <v>5636256</v>
+        <v>5701831</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D155" t="n">
-        <v>591716</v>
+        <v>596216</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="D157" t="n">
-        <v>603313</v>
+        <v>622813</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>18428</v>
+        <v>18598</v>
       </c>
       <c r="D158" t="n">
-        <v>24365042</v>
+        <v>24593529</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D161" t="n">
-        <v>79406</v>
+        <v>80906</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7552</v>
+        <v>7651</v>
       </c>
       <c r="D162" t="n">
-        <v>10991319</v>
+        <v>11134245</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>5286</v>
+        <v>5370</v>
       </c>
       <c r="D164" t="n">
-        <v>7611778</v>
+        <v>7734621</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D166" t="n">
-        <v>401639</v>
+        <v>411939</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D167" t="n">
-        <v>404664</v>
+        <v>410664</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>22589</v>
+        <v>23387</v>
       </c>
       <c r="D169" t="n">
-        <v>40952820</v>
+        <v>43069828</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>2376</v>
+        <v>2427</v>
       </c>
       <c r="D170" t="n">
-        <v>4290256</v>
+        <v>4424521</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="D171" t="n">
-        <v>549809</v>
+        <v>577440</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D173" t="n">
-        <v>145190</v>
+        <v>148190</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D174" t="n">
-        <v>227949</v>
+        <v>247449</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>90591</v>
+        <v>91170</v>
       </c>
       <c r="D175" t="n">
-        <v>113094275</v>
+        <v>113786839</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D176" t="n">
-        <v>38659</v>
+        <v>40159</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D180" t="n">
-        <v>952088</v>
+        <v>955088</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>34800</v>
+        <v>34993</v>
       </c>
       <c r="D182" t="n">
-        <v>51019719</v>
+        <v>51299183</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>13541</v>
+        <v>13649</v>
       </c>
       <c r="D184" t="n">
-        <v>19565093</v>
+        <v>19721055</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1277</v>
+        <v>1283</v>
       </c>
       <c r="D186" t="n">
-        <v>1788027</v>
+        <v>1795531</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1798</v>
+        <v>1830</v>
       </c>
       <c r="D188" t="n">
-        <v>2524492</v>
+        <v>2568086</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>246272</v>
+        <v>247848</v>
       </c>
       <c r="D190" t="n">
-        <v>305821221</v>
+        <v>307680371</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D191" t="n">
-        <v>150587</v>
+        <v>153587</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>899</v>
+        <v>910</v>
       </c>
       <c r="D196" t="n">
-        <v>1322601</v>
+        <v>1338519</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>88794</v>
+        <v>89266</v>
       </c>
       <c r="D198" t="n">
-        <v>130129995</v>
+        <v>130813818</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D199" t="n">
-        <v>139627</v>
+        <v>144127</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>34211</v>
+        <v>34503</v>
       </c>
       <c r="D201" t="n">
-        <v>49246757</v>
+        <v>49671462</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5228</v>
+        <v>5245</v>
       </c>
       <c r="D204" t="n">
-        <v>7445178</v>
+        <v>7470442</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5326</v>
+        <v>5413</v>
       </c>
       <c r="D207" t="n">
-        <v>7379199</v>
+        <v>7499144</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>273154</v>
+        <v>275104</v>
       </c>
       <c r="D210" t="n">
-        <v>337867296</v>
+        <v>340167948</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D212" t="n">
-        <v>370039</v>
+        <v>373039</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="D217" t="n">
-        <v>918798</v>
+        <v>926298</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>97803</v>
+        <v>98418</v>
       </c>
       <c r="D219" t="n">
-        <v>143061533</v>
+        <v>143950203</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D220" t="n">
-        <v>144699</v>
+        <v>147199</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>53511</v>
+        <v>53937</v>
       </c>
       <c r="D222" t="n">
-        <v>77328893</v>
+        <v>77946081</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D223" t="n">
-        <v>48922</v>
+        <v>51922</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>4766</v>
+        <v>4798</v>
       </c>
       <c r="D225" t="n">
-        <v>6688684</v>
+        <v>6733329</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>6402</v>
+        <v>6547</v>
       </c>
       <c r="D228" t="n">
-        <v>8873576</v>
+        <v>9075007</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>110195</v>
+        <v>110963</v>
       </c>
       <c r="D231" t="n">
-        <v>137674321</v>
+        <v>138569014</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D232" t="n">
-        <v>85050</v>
+        <v>88050</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D233" t="n">
-        <v>113513</v>
+        <v>114213</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="D236" t="n">
-        <v>841939</v>
+        <v>846439</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>50812</v>
+        <v>51095</v>
       </c>
       <c r="D238" t="n">
-        <v>74432823</v>
+        <v>74841645</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D239" t="n">
-        <v>59211</v>
+        <v>60711</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>13019</v>
+        <v>13139</v>
       </c>
       <c r="D240" t="n">
-        <v>18727388</v>
+        <v>18894544</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>1915</v>
+        <v>1921</v>
       </c>
       <c r="D242" t="n">
-        <v>2746382</v>
+        <v>2755382</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2731</v>
+        <v>2780</v>
       </c>
       <c r="D244" t="n">
-        <v>3827473</v>
+        <v>3893343</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>267871</v>
+        <v>269827</v>
       </c>
       <c r="D245" t="n">
-        <v>338160886</v>
+        <v>340568585</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D247" t="n">
-        <v>367812</v>
+        <v>370167</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D250" t="n">
-        <v>20480</v>
+        <v>21980</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>852</v>
+        <v>859</v>
       </c>
       <c r="D251" t="n">
-        <v>1251404</v>
+        <v>1261654</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>98773</v>
+        <v>99347</v>
       </c>
       <c r="D253" t="n">
-        <v>144718921</v>
+        <v>145548389</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>68041</v>
+        <v>68564</v>
       </c>
       <c r="D256" t="n">
-        <v>98630025</v>
+        <v>99386268</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>2466</v>
+        <v>2474</v>
       </c>
       <c r="D258" t="n">
-        <v>3477893</v>
+        <v>3487199</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>5073</v>
+        <v>5192</v>
       </c>
       <c r="D261" t="n">
-        <v>7127495</v>
+        <v>7287376</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>335634</v>
+        <v>336547</v>
       </c>
       <c r="D2" t="n">
-        <v>427170753</v>
+        <v>428299639</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D3" t="n">
-        <v>325292</v>
+        <v>326562</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="D4" t="n">
-        <v>491093</v>
+        <v>498593</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="D8" t="n">
-        <v>1298899</v>
+        <v>1303216</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
-        <v>25256</v>
+        <v>26756</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>121003</v>
+        <v>121334</v>
       </c>
       <c r="D10" t="n">
-        <v>177252782</v>
+        <v>177730392</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D11" t="n">
-        <v>216013</v>
+        <v>217513</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>62480</v>
+        <v>62667</v>
       </c>
       <c r="D12" t="n">
-        <v>90170616</v>
+        <v>90442256</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4077</v>
+        <v>4084</v>
       </c>
       <c r="D16" t="n">
-        <v>5788399</v>
+        <v>5798639</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7541</v>
+        <v>7633</v>
       </c>
       <c r="D21" t="n">
-        <v>10536768</v>
+        <v>10664915</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>80560</v>
+        <v>80748</v>
       </c>
       <c r="D23" t="n">
-        <v>100229018</v>
+        <v>100443899</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D28" t="n">
-        <v>419147</v>
+        <v>420647</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>33390</v>
+        <v>33466</v>
       </c>
       <c r="D29" t="n">
-        <v>48865597</v>
+        <v>48977224</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11968</v>
+        <v>12001</v>
       </c>
       <c r="D31" t="n">
-        <v>17215877</v>
+        <v>17262902</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2050</v>
+        <v>2075</v>
       </c>
       <c r="D36" t="n">
-        <v>2894384</v>
+        <v>2931253</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>100727</v>
+        <v>100937</v>
       </c>
       <c r="D37" t="n">
-        <v>126514597</v>
+        <v>126762577</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D43" t="n">
-        <v>1341185</v>
+        <v>1342685</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>45623</v>
+        <v>45730</v>
       </c>
       <c r="D45" t="n">
-        <v>66842898</v>
+        <v>66997807</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>9543</v>
+        <v>9565</v>
       </c>
       <c r="D47" t="n">
-        <v>13682607</v>
+        <v>13712510</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1447</v>
+        <v>1454</v>
       </c>
       <c r="D49" t="n">
-        <v>2011327</v>
+        <v>2021827</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2638</v>
+        <v>2653</v>
       </c>
       <c r="D52" t="n">
-        <v>3690157</v>
+        <v>3712037</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>71809</v>
+        <v>71992</v>
       </c>
       <c r="D53" t="n">
-        <v>89957930</v>
+        <v>90182009</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D55" t="n">
-        <v>63697</v>
+        <v>65197</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>29090</v>
+        <v>29162</v>
       </c>
       <c r="D60" t="n">
-        <v>42655732</v>
+        <v>42760166</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>11629</v>
+        <v>11658</v>
       </c>
       <c r="D63" t="n">
-        <v>16804430</v>
+        <v>16845520</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1396</v>
+        <v>1399</v>
       </c>
       <c r="D65" t="n">
-        <v>1952080</v>
+        <v>1955987</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1675</v>
+        <v>1689</v>
       </c>
       <c r="D69" t="n">
-        <v>2348940</v>
+        <v>2368948</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>21387</v>
+        <v>21457</v>
       </c>
       <c r="D71" t="n">
-        <v>27995910</v>
+        <v>28081952</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D74" t="n">
-        <v>93573</v>
+        <v>95073</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>7911</v>
+        <v>7933</v>
       </c>
       <c r="D75" t="n">
-        <v>11587181</v>
+        <v>11620181</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>5356</v>
+        <v>5387</v>
       </c>
       <c r="D77" t="n">
-        <v>7781826</v>
+        <v>7828091</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="D78" t="n">
-        <v>721560</v>
+        <v>729060</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D79" t="n">
-        <v>435083</v>
+        <v>438323</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>146395</v>
+        <v>146852</v>
       </c>
       <c r="D80" t="n">
-        <v>182230400</v>
+        <v>182785038</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D84" t="n">
-        <v>660583</v>
+        <v>662083</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>65482</v>
+        <v>65639</v>
       </c>
       <c r="D86" t="n">
-        <v>95942450</v>
+        <v>96166747</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>30884</v>
+        <v>30964</v>
       </c>
       <c r="D89" t="n">
-        <v>44673124</v>
+        <v>44789010</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2808</v>
+        <v>2834</v>
       </c>
       <c r="D91" t="n">
-        <v>4044652</v>
+        <v>4083652</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3143</v>
+        <v>3171</v>
       </c>
       <c r="D92" t="n">
-        <v>4434119</v>
+        <v>4475271</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>35548</v>
+        <v>35705</v>
       </c>
       <c r="D93" t="n">
-        <v>48207329</v>
+        <v>48425060</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8655</v>
+        <v>8684</v>
       </c>
       <c r="D97" t="n">
-        <v>12720584</v>
+        <v>12764473</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>8019</v>
+        <v>8056</v>
       </c>
       <c r="D99" t="n">
-        <v>11636561</v>
+        <v>11689931</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D101" t="n">
-        <v>809876</v>
+        <v>811376</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="D102" t="n">
-        <v>781560</v>
+        <v>786060</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>13088</v>
+        <v>13307</v>
       </c>
       <c r="D103" t="n">
-        <v>22254511</v>
+        <v>22764072</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D104" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>3117</v>
+        <v>3160</v>
       </c>
       <c r="D105" t="n">
-        <v>5696059</v>
+        <v>5811413</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4325</v>
+        <v>4402</v>
       </c>
       <c r="D107" t="n">
-        <v>7925494</v>
+        <v>8120756</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D109" t="n">
-        <v>336120</v>
+        <v>348120</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D110" t="n">
-        <v>453673</v>
+        <v>485173</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>147587</v>
+        <v>147962</v>
       </c>
       <c r="D112" t="n">
-        <v>182416420</v>
+        <v>182864725</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="D116" t="n">
-        <v>1416815</v>
+        <v>1418315</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>54557</v>
+        <v>54682</v>
       </c>
       <c r="D118" t="n">
-        <v>79920656</v>
+        <v>80097160</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>28631</v>
+        <v>28727</v>
       </c>
       <c r="D120" t="n">
-        <v>41473936</v>
+        <v>41611871</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="D121" t="n">
-        <v>1831694</v>
+        <v>1834694</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>2531</v>
+        <v>2547</v>
       </c>
       <c r="D124" t="n">
-        <v>3563495</v>
+        <v>3586295</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>559071</v>
+        <v>562229</v>
       </c>
       <c r="D126" t="n">
-        <v>738431919</v>
+        <v>742516843</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D128" t="n">
-        <v>336009</v>
+        <v>340509</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1448</v>
+        <v>1457</v>
       </c>
       <c r="D131" t="n">
-        <v>2143817</v>
+        <v>2157317</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>220581</v>
+        <v>221635</v>
       </c>
       <c r="D133" t="n">
-        <v>324138075</v>
+        <v>325678421</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D134" t="n">
-        <v>671710</v>
+        <v>674710</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>199895</v>
+        <v>201010</v>
       </c>
       <c r="D136" t="n">
-        <v>290658537</v>
+        <v>292275870</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D137" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2931</v>
+        <v>2935</v>
       </c>
       <c r="D139" t="n">
-        <v>4116072</v>
+        <v>4121462</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>7244</v>
+        <v>7331</v>
       </c>
       <c r="D142" t="n">
-        <v>10221446</v>
+        <v>10346147</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>47237</v>
+        <v>47424</v>
       </c>
       <c r="D145" t="n">
-        <v>63016528</v>
+        <v>63262755</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>14664</v>
+        <v>14699</v>
       </c>
       <c r="D151" t="n">
-        <v>21492138</v>
+        <v>21543565</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>3953</v>
+        <v>3971</v>
       </c>
       <c r="D152" t="n">
-        <v>5701831</v>
+        <v>5728075</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D155" t="n">
-        <v>596216</v>
+        <v>597716</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D157" t="n">
-        <v>622813</v>
+        <v>628813</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>18598</v>
+        <v>18677</v>
       </c>
       <c r="D158" t="n">
-        <v>24593529</v>
+        <v>24696207</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7651</v>
+        <v>7677</v>
       </c>
       <c r="D162" t="n">
-        <v>11134245</v>
+        <v>11171428</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>5370</v>
+        <v>5395</v>
       </c>
       <c r="D164" t="n">
-        <v>7734621</v>
+        <v>7771227</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D167" t="n">
-        <v>410664</v>
+        <v>412164</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>23387</v>
+        <v>23578</v>
       </c>
       <c r="D169" t="n">
-        <v>43069828</v>
+        <v>43531589</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>2427</v>
+        <v>2451</v>
       </c>
       <c r="D170" t="n">
-        <v>4424521</v>
+        <v>4490091</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D174" t="n">
-        <v>247449</v>
+        <v>250449</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>91170</v>
+        <v>91347</v>
       </c>
       <c r="D175" t="n">
-        <v>113786839</v>
+        <v>113991124</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>34993</v>
+        <v>35068</v>
       </c>
       <c r="D182" t="n">
-        <v>51299183</v>
+        <v>51405774</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>13649</v>
+        <v>13695</v>
       </c>
       <c r="D184" t="n">
-        <v>19721055</v>
+        <v>19785350</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D186" t="n">
-        <v>1795531</v>
+        <v>1797031</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1830</v>
+        <v>1840</v>
       </c>
       <c r="D188" t="n">
-        <v>2568086</v>
+        <v>2581946</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>247848</v>
+        <v>248464</v>
       </c>
       <c r="D190" t="n">
-        <v>307680371</v>
+        <v>308406991</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D192" t="n">
-        <v>251236</v>
+        <v>254236</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="D196" t="n">
-        <v>1338519</v>
+        <v>1340590</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>89266</v>
+        <v>89442</v>
       </c>
       <c r="D198" t="n">
-        <v>130813818</v>
+        <v>131068349</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>34503</v>
+        <v>34607</v>
       </c>
       <c r="D201" t="n">
-        <v>49671462</v>
+        <v>49817817</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5245</v>
+        <v>5259</v>
       </c>
       <c r="D204" t="n">
-        <v>7470442</v>
+        <v>7489683</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5413</v>
+        <v>5448</v>
       </c>
       <c r="D207" t="n">
-        <v>7499144</v>
+        <v>7550857</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>275104</v>
+        <v>275763</v>
       </c>
       <c r="D210" t="n">
-        <v>340167948</v>
+        <v>340941891</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8362,10 +8362,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D211" t="n">
-        <v>180913</v>
+        <v>182413</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D217" t="n">
-        <v>926298</v>
+        <v>927798</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>98418</v>
+        <v>98705</v>
       </c>
       <c r="D219" t="n">
-        <v>143950203</v>
+        <v>144370606</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>53937</v>
+        <v>54102</v>
       </c>
       <c r="D222" t="n">
-        <v>77946081</v>
+        <v>78179958</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D223" t="n">
-        <v>51922</v>
+        <v>53422</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>4798</v>
+        <v>4803</v>
       </c>
       <c r="D225" t="n">
-        <v>6733329</v>
+        <v>6740829</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>6547</v>
+        <v>6615</v>
       </c>
       <c r="D228" t="n">
-        <v>9075007</v>
+        <v>9166300</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>110963</v>
+        <v>111228</v>
       </c>
       <c r="D231" t="n">
-        <v>138569014</v>
+        <v>138872866</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D236" t="n">
-        <v>846439</v>
+        <v>847939</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>51095</v>
+        <v>51211</v>
       </c>
       <c r="D238" t="n">
-        <v>74841645</v>
+        <v>75011259</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>13139</v>
+        <v>13177</v>
       </c>
       <c r="D240" t="n">
-        <v>18894544</v>
+        <v>18950061</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>1921</v>
+        <v>1923</v>
       </c>
       <c r="D242" t="n">
-        <v>2755382</v>
+        <v>2758382</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2780</v>
+        <v>2798</v>
       </c>
       <c r="D244" t="n">
-        <v>3893343</v>
+        <v>3919743</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>269827</v>
+        <v>270572</v>
       </c>
       <c r="D245" t="n">
-        <v>340568585</v>
+        <v>341468254</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="D251" t="n">
-        <v>1261654</v>
+        <v>1267654</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>99347</v>
+        <v>99595</v>
       </c>
       <c r="D253" t="n">
-        <v>145548389</v>
+        <v>145904471</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>68564</v>
+        <v>68791</v>
       </c>
       <c r="D256" t="n">
-        <v>99386268</v>
+        <v>99710151</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>2474</v>
+        <v>2478</v>
       </c>
       <c r="D258" t="n">
-        <v>3487199</v>
+        <v>3492535</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>5192</v>
+        <v>5236</v>
       </c>
       <c r="D261" t="n">
-        <v>7287376</v>
+        <v>7347773</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-10-18 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>343034</v>
+        <v>346945</v>
       </c>
       <c r="D2" t="n">
-        <v>436369424</v>
+        <v>441228100</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D3" t="n">
-        <v>332562</v>
+        <v>334062</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D4" t="n">
-        <v>516593</v>
+        <v>527093</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>902</v>
+        <v>911</v>
       </c>
       <c r="D8" t="n">
-        <v>1326211</v>
+        <v>1339711</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>26756</v>
+        <v>28256</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>123113</v>
+        <v>124259</v>
       </c>
       <c r="D10" t="n">
-        <v>180318884</v>
+        <v>181980723</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>64039</v>
+        <v>64882</v>
       </c>
       <c r="D12" t="n">
-        <v>92430673</v>
+        <v>93649478</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4111</v>
+        <v>4130</v>
       </c>
       <c r="D16" t="n">
-        <v>5836271</v>
+        <v>5862322</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8018</v>
+        <v>8273</v>
       </c>
       <c r="D21" t="n">
-        <v>11196196</v>
+        <v>11548087</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>82015</v>
+        <v>82781</v>
       </c>
       <c r="D23" t="n">
-        <v>101976030</v>
+        <v>102871039</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27" t="n">
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D28" t="n">
-        <v>423647</v>
+        <v>428147</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>33856</v>
+        <v>34102</v>
       </c>
       <c r="D29" t="n">
-        <v>49548547</v>
+        <v>49907178</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12212</v>
+        <v>12345</v>
       </c>
       <c r="D32" t="n">
-        <v>17568245</v>
+        <v>17758320</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1597</v>
+        <v>1606</v>
       </c>
       <c r="D35" t="n">
-        <v>2243233</v>
+        <v>2256733</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2164</v>
+        <v>2202</v>
       </c>
       <c r="D37" t="n">
-        <v>3054043</v>
+        <v>3105586</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>102453</v>
+        <v>103422</v>
       </c>
       <c r="D38" t="n">
-        <v>128585886</v>
+        <v>129710617</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="D44" t="n">
-        <v>1351685</v>
+        <v>1353185</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>46262</v>
+        <v>46551</v>
       </c>
       <c r="D46" t="n">
-        <v>67765728</v>
+        <v>68186040</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9748</v>
+        <v>9855</v>
       </c>
       <c r="D48" t="n">
-        <v>13969887</v>
+        <v>14122379</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1461</v>
+        <v>1467</v>
       </c>
       <c r="D50" t="n">
-        <v>2032093</v>
+        <v>2041093</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2751</v>
+        <v>2812</v>
       </c>
       <c r="D53" t="n">
-        <v>3851820</v>
+        <v>3938188</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>73169</v>
+        <v>73899</v>
       </c>
       <c r="D54" t="n">
-        <v>91616730</v>
+        <v>92496450</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D59" t="n">
-        <v>568374</v>
+        <v>569874</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>29588</v>
+        <v>29860</v>
       </c>
       <c r="D61" t="n">
-        <v>43373028</v>
+        <v>43761424</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D62" t="n">
-        <v>36000</v>
+        <v>39000</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>11884</v>
+        <v>12045</v>
       </c>
       <c r="D64" t="n">
-        <v>17171991</v>
+        <v>17408794</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1410</v>
+        <v>1416</v>
       </c>
       <c r="D66" t="n">
-        <v>1972487</v>
+        <v>1980647</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1751</v>
+        <v>1796</v>
       </c>
       <c r="D70" t="n">
-        <v>2456024</v>
+        <v>2521026</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>21920</v>
+        <v>22157</v>
       </c>
       <c r="D72" t="n">
-        <v>28674822</v>
+        <v>28967556</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D73" t="n">
-        <v>44600</v>
+        <v>45419</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D74" t="n">
-        <v>36225</v>
+        <v>37725</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D75" t="n">
-        <v>98073</v>
+        <v>107073</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8091</v>
+        <v>8176</v>
       </c>
       <c r="D76" t="n">
-        <v>11847738</v>
+        <v>11971933</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5510</v>
+        <v>5574</v>
       </c>
       <c r="D78" t="n">
-        <v>8010816</v>
+        <v>8104552</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="D79" t="n">
-        <v>756347</v>
+        <v>765086</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D80" t="n">
-        <v>465783</v>
+        <v>485743</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>149500</v>
+        <v>150919</v>
       </c>
       <c r="D81" t="n">
-        <v>185955081</v>
+        <v>187619778</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D82" t="n">
-        <v>87766</v>
+        <v>88591</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D85" t="n">
-        <v>668083</v>
+        <v>671083</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>66449</v>
+        <v>66909</v>
       </c>
       <c r="D87" t="n">
-        <v>97349272</v>
+        <v>98025252</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D88" t="n">
-        <v>123082</v>
+        <v>126082</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>31498</v>
+        <v>31787</v>
       </c>
       <c r="D90" t="n">
-        <v>45556413</v>
+        <v>45978135</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2908</v>
+        <v>2929</v>
       </c>
       <c r="D92" t="n">
-        <v>4192698</v>
+        <v>4223347</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3333</v>
+        <v>3401</v>
       </c>
       <c r="D94" t="n">
-        <v>4707913</v>
+        <v>4807291</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>36668</v>
+        <v>37343</v>
       </c>
       <c r="D95" t="n">
-        <v>49749767</v>
+        <v>50661687</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D98" t="n">
-        <v>48004</v>
+        <v>51004</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>8975</v>
+        <v>9176</v>
       </c>
       <c r="D99" t="n">
-        <v>13188442</v>
+        <v>13478419</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8332</v>
+        <v>8568</v>
       </c>
       <c r="D101" t="n">
-        <v>12088407</v>
+        <v>12433762</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="D103" t="n">
-        <v>827760</v>
+        <v>834670</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="D104" t="n">
-        <v>804060</v>
+        <v>816060</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>14698</v>
+        <v>15717</v>
       </c>
       <c r="D105" t="n">
-        <v>26230800</v>
+        <v>28818869</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D106" t="n">
-        <v>9000</v>
+        <v>18000</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3456</v>
+        <v>3665</v>
       </c>
       <c r="D108" t="n">
-        <v>6628725</v>
+        <v>7234878</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4847</v>
+        <v>5171</v>
       </c>
       <c r="D110" t="n">
-        <v>9359305</v>
+        <v>10277027</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D111" t="n">
-        <v>12000</v>
+        <v>21000</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="D112" t="n">
-        <v>403170</v>
+        <v>443595</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="D113" t="n">
-        <v>549691</v>
+        <v>579650</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>150641</v>
+        <v>152112</v>
       </c>
       <c r="D115" t="n">
-        <v>186157257</v>
+        <v>187918151</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D117" t="n">
-        <v>107557</v>
+        <v>109057</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="D119" t="n">
-        <v>1426954</v>
+        <v>1431454</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>55487</v>
+        <v>55958</v>
       </c>
       <c r="D121" t="n">
-        <v>81263353</v>
+        <v>81952560</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D122" t="n">
-        <v>143959</v>
+        <v>145459</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>29470</v>
+        <v>29946</v>
       </c>
       <c r="D123" t="n">
-        <v>42694182</v>
+        <v>43379905</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1351</v>
+        <v>1358</v>
       </c>
       <c r="D124" t="n">
-        <v>1851194</v>
+        <v>1861694</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2659</v>
+        <v>2725</v>
       </c>
       <c r="D127" t="n">
-        <v>3745031</v>
+        <v>3837480</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>586280</v>
+        <v>600041</v>
       </c>
       <c r="D129" t="n">
-        <v>774696562</v>
+        <v>792879663</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D130" t="n">
-        <v>137324</v>
+        <v>138964</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D131" t="n">
-        <v>350520</v>
+        <v>357713</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D133" t="n">
-        <v>35998</v>
+        <v>37498</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1497</v>
+        <v>1537</v>
       </c>
       <c r="D134" t="n">
-        <v>2217317</v>
+        <v>2276020</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>227572</v>
+        <v>231459</v>
       </c>
       <c r="D136" t="n">
-        <v>334356279</v>
+        <v>340055932</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>476</v>
+        <v>498</v>
       </c>
       <c r="D137" t="n">
-        <v>710670</v>
+        <v>743670</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D138" t="n">
-        <v>24000</v>
+        <v>25500</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>209589</v>
+        <v>214686</v>
       </c>
       <c r="D139" t="n">
-        <v>304820803</v>
+        <v>312250779</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D141" t="n">
-        <v>57332</v>
+        <v>60332</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2965</v>
+        <v>2985</v>
       </c>
       <c r="D142" t="n">
-        <v>4165458</v>
+        <v>4194258</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>7794</v>
+        <v>8039</v>
       </c>
       <c r="D145" t="n">
-        <v>10993361</v>
+        <v>11334094</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D147" t="n">
-        <v>28500</v>
+        <v>30000</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>48463</v>
+        <v>49070</v>
       </c>
       <c r="D148" t="n">
-        <v>64639983</v>
+        <v>65422470</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D149" t="n">
-        <v>41762</v>
+        <v>43262</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D150" t="n">
-        <v>36230</v>
+        <v>37730</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>14932</v>
+        <v>15120</v>
       </c>
       <c r="D154" t="n">
-        <v>21884508</v>
+        <v>22156523</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>4047</v>
+        <v>4103</v>
       </c>
       <c r="D155" t="n">
-        <v>5836750</v>
+        <v>5919727</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D158" t="n">
-        <v>599087</v>
+        <v>603587</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>465</v>
+        <v>484</v>
       </c>
       <c r="D160" t="n">
-        <v>656773</v>
+        <v>684473</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>19092</v>
+        <v>19390</v>
       </c>
       <c r="D161" t="n">
-        <v>25242716</v>
+        <v>25647156</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>7839</v>
+        <v>7995</v>
       </c>
       <c r="D165" t="n">
-        <v>11404440</v>
+        <v>11630108</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5542</v>
+        <v>5648</v>
       </c>
       <c r="D167" t="n">
-        <v>7982012</v>
+        <v>8130016</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="D169" t="n">
-        <v>417171</v>
+        <v>424521</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D170" t="n">
-        <v>430164</v>
+        <v>438766</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>26296</v>
+        <v>27895</v>
       </c>
       <c r="D172" t="n">
-        <v>51018647</v>
+        <v>55559686</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2642</v>
+        <v>2780</v>
       </c>
       <c r="D173" t="n">
-        <v>5037416</v>
+        <v>5446655</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="D174" t="n">
-        <v>643430</v>
+        <v>684281</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D176" t="n">
-        <v>168516</v>
+        <v>177516</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D177" t="n">
-        <v>316949</v>
+        <v>353637</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>92776</v>
+        <v>93646</v>
       </c>
       <c r="D178" t="n">
-        <v>115677190</v>
+        <v>116707570</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D180" t="n">
-        <v>124454</v>
+        <v>125602</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D182" t="n">
-        <v>21889</v>
+        <v>22889</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="D183" t="n">
-        <v>956206</v>
+        <v>962206</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>35563</v>
+        <v>35834</v>
       </c>
       <c r="D185" t="n">
-        <v>52128849</v>
+        <v>52524907</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>13987</v>
+        <v>14184</v>
       </c>
       <c r="D187" t="n">
-        <v>20208666</v>
+        <v>20494194</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>1297</v>
+        <v>1301</v>
       </c>
       <c r="D189" t="n">
-        <v>1814903</v>
+        <v>1819862</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1924</v>
+        <v>1968</v>
       </c>
       <c r="D191" t="n">
-        <v>2701979</v>
+        <v>2764479</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>252712</v>
+        <v>255130</v>
       </c>
       <c r="D193" t="n">
-        <v>313481939</v>
+        <v>316354787</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D195" t="n">
-        <v>259479</v>
+        <v>260979</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="D199" t="n">
-        <v>1354090</v>
+        <v>1365779</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>90621</v>
+        <v>91432</v>
       </c>
       <c r="D201" t="n">
-        <v>132783842</v>
+        <v>133966134</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D202" t="n">
-        <v>147127</v>
+        <v>150127</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>35343</v>
+        <v>35754</v>
       </c>
       <c r="D204" t="n">
-        <v>50890779</v>
+        <v>51491832</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5334</v>
+        <v>5371</v>
       </c>
       <c r="D207" t="n">
-        <v>7597244</v>
+        <v>7652152</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>5676</v>
+        <v>5826</v>
       </c>
       <c r="D210" t="n">
-        <v>7873156</v>
+        <v>8069682</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>280621</v>
+        <v>283574</v>
       </c>
       <c r="D213" t="n">
-        <v>346905986</v>
+        <v>350332266</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D214" t="n">
-        <v>188314</v>
+        <v>191969</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D215" t="n">
-        <v>377384</v>
+        <v>380384</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="D220" t="n">
-        <v>931014</v>
+        <v>937014</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>100095</v>
+        <v>101066</v>
       </c>
       <c r="D222" t="n">
-        <v>146394701</v>
+        <v>147815192</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D223" t="n">
-        <v>151699</v>
+        <v>160699</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>55138</v>
+        <v>55884</v>
       </c>
       <c r="D225" t="n">
-        <v>79670827</v>
+        <v>80742569</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D226" t="n">
-        <v>53422</v>
+        <v>56422</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>4846</v>
+        <v>4880</v>
       </c>
       <c r="D228" t="n">
-        <v>6803553</v>
+        <v>6850109</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>7009</v>
+        <v>7226</v>
       </c>
       <c r="D231" t="n">
-        <v>9713113</v>
+        <v>10008617</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>113185</v>
+        <v>114359</v>
       </c>
       <c r="D234" t="n">
-        <v>141233865</v>
+        <v>142618474</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D235" t="n">
-        <v>88050</v>
+        <v>89550</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D236" t="n">
-        <v>119492</v>
+        <v>122492</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D237" t="n">
-        <v>14147</v>
+        <v>15647</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="D239" t="n">
-        <v>855439</v>
+        <v>861259</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>51838</v>
+        <v>52238</v>
       </c>
       <c r="D241" t="n">
-        <v>75926982</v>
+        <v>76509039</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D242" t="n">
-        <v>65211</v>
+        <v>66711</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>13475</v>
+        <v>13666</v>
       </c>
       <c r="D243" t="n">
-        <v>19379023</v>
+        <v>19655941</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>1941</v>
+        <v>1957</v>
       </c>
       <c r="D245" t="n">
-        <v>2782086</v>
+        <v>2805589</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>2918</v>
+        <v>2986</v>
       </c>
       <c r="D247" t="n">
-        <v>4087489</v>
+        <v>4182797</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>276332</v>
+        <v>279707</v>
       </c>
       <c r="D248" t="n">
-        <v>348746381</v>
+        <v>352923428</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D249" t="n">
-        <v>231751</v>
+        <v>237452</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D250" t="n">
-        <v>377053</v>
+        <v>382408</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D253" t="n">
-        <v>21980</v>
+        <v>23480</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>881</v>
+        <v>891</v>
       </c>
       <c r="D254" t="n">
-        <v>1294368</v>
+        <v>1309368</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D255" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>101434</v>
+        <v>102721</v>
       </c>
       <c r="D256" t="n">
-        <v>148587386</v>
+        <v>150471732</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D257" t="n">
-        <v>122564</v>
+        <v>128564</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>70656</v>
+        <v>71749</v>
       </c>
       <c r="D259" t="n">
-        <v>102421554</v>
+        <v>103980835</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>2509</v>
+        <v>2520</v>
       </c>
       <c r="D261" t="n">
-        <v>3535667</v>
+        <v>3550465</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>5528</v>
+        <v>5691</v>
       </c>
       <c r="D264" t="n">
-        <v>7759890</v>
+        <v>7987189</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-10-25 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H264"/>
+  <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>346945</v>
+        <v>348894</v>
       </c>
       <c r="D2" t="n">
-        <v>441228100</v>
+        <v>443573513</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D3" t="n">
-        <v>334062</v>
+        <v>334819</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="D4" t="n">
-        <v>527093</v>
+        <v>535359</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>911</v>
+        <v>918</v>
       </c>
       <c r="D8" t="n">
-        <v>1339711</v>
+        <v>1350096</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>124259</v>
+        <v>124903</v>
       </c>
       <c r="D10" t="n">
-        <v>181980723</v>
+        <v>182919890</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>64882</v>
+        <v>65320</v>
       </c>
       <c r="D12" t="n">
-        <v>93649478</v>
+        <v>94283062</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4130</v>
+        <v>4141</v>
       </c>
       <c r="D16" t="n">
-        <v>5862322</v>
+        <v>5878129</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8273</v>
+        <v>8447</v>
       </c>
       <c r="D21" t="n">
-        <v>11548087</v>
+        <v>11797510</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>82781</v>
+        <v>83159</v>
       </c>
       <c r="D23" t="n">
-        <v>102871039</v>
+        <v>103299725</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D28" t="n">
-        <v>428147</v>
+        <v>429647</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>34102</v>
+        <v>34224</v>
       </c>
       <c r="D29" t="n">
-        <v>49907178</v>
+        <v>50083235</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12345</v>
+        <v>12403</v>
       </c>
       <c r="D32" t="n">
-        <v>17758320</v>
+        <v>17841033</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="D35" t="n">
-        <v>2256733</v>
+        <v>2258233</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2202</v>
+        <v>2235</v>
       </c>
       <c r="D37" t="n">
-        <v>3105586</v>
+        <v>3150546</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>103422</v>
+        <v>103854</v>
       </c>
       <c r="D38" t="n">
-        <v>129710617</v>
+        <v>130190445</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D40" t="n">
-        <v>119397</v>
+        <v>120078</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>46551</v>
+        <v>46713</v>
       </c>
       <c r="D46" t="n">
-        <v>68186040</v>
+        <v>68419847</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9855</v>
+        <v>9895</v>
       </c>
       <c r="D48" t="n">
-        <v>14122379</v>
+        <v>14180007</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1467</v>
+        <v>1476</v>
       </c>
       <c r="D50" t="n">
-        <v>2041093</v>
+        <v>2054593</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2812</v>
+        <v>2848</v>
       </c>
       <c r="D53" t="n">
-        <v>3938188</v>
+        <v>3990357</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>73899</v>
+        <v>74211</v>
       </c>
       <c r="D54" t="n">
-        <v>92496450</v>
+        <v>92863995</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D56" t="n">
-        <v>66697</v>
+        <v>70163</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D59" t="n">
-        <v>569874</v>
+        <v>572874</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>29860</v>
+        <v>29974</v>
       </c>
       <c r="D61" t="n">
-        <v>43761424</v>
+        <v>43924014</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>12045</v>
+        <v>12103</v>
       </c>
       <c r="D64" t="n">
-        <v>17408794</v>
+        <v>17489732</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1416</v>
+        <v>1425</v>
       </c>
       <c r="D66" t="n">
-        <v>1980647</v>
+        <v>1993560</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1796</v>
+        <v>1838</v>
       </c>
       <c r="D70" t="n">
-        <v>2521026</v>
+        <v>2581579</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>22157</v>
+        <v>22299</v>
       </c>
       <c r="D72" t="n">
-        <v>28967556</v>
+        <v>29143144</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8176</v>
+        <v>8225</v>
       </c>
       <c r="D76" t="n">
-        <v>11971933</v>
+        <v>12044647</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5574</v>
+        <v>5611</v>
       </c>
       <c r="D78" t="n">
-        <v>8104552</v>
+        <v>8157054</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D79" t="n">
-        <v>765086</v>
+        <v>768062</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="D80" t="n">
-        <v>485743</v>
+        <v>496996</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>150919</v>
+        <v>151676</v>
       </c>
       <c r="D81" t="n">
-        <v>187619778</v>
+        <v>188486422</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D85" t="n">
-        <v>671083</v>
+        <v>672583</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>66909</v>
+        <v>67211</v>
       </c>
       <c r="D87" t="n">
-        <v>98025252</v>
+        <v>98466689</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D88" t="n">
-        <v>126082</v>
+        <v>127582</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>31787</v>
+        <v>31948</v>
       </c>
       <c r="D90" t="n">
-        <v>45978135</v>
+        <v>46211737</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2929</v>
+        <v>2960</v>
       </c>
       <c r="D92" t="n">
-        <v>4223347</v>
+        <v>4269847</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3401</v>
+        <v>3449</v>
       </c>
       <c r="D94" t="n">
-        <v>4807291</v>
+        <v>4875513</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>37343</v>
+        <v>37615</v>
       </c>
       <c r="D95" t="n">
-        <v>50661687</v>
+        <v>51033761</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D98" t="n">
-        <v>51004</v>
+        <v>52504</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9176</v>
+        <v>9270</v>
       </c>
       <c r="D99" t="n">
-        <v>13478419</v>
+        <v>13615717</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8568</v>
+        <v>8649</v>
       </c>
       <c r="D101" t="n">
-        <v>12433762</v>
+        <v>12549920</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D103" t="n">
-        <v>834670</v>
+        <v>836170</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="D104" t="n">
-        <v>816060</v>
+        <v>822060</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>15717</v>
+        <v>16232</v>
       </c>
       <c r="D105" t="n">
-        <v>28818869</v>
+        <v>30144975</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D107" t="n">
-        <v>7500</v>
+        <v>10500</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3665</v>
+        <v>3750</v>
       </c>
       <c r="D108" t="n">
-        <v>7234878</v>
+        <v>7468111</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>5171</v>
+        <v>5326</v>
       </c>
       <c r="D110" t="n">
-        <v>10277027</v>
+        <v>10724999</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D111" t="n">
-        <v>21000</v>
+        <v>30000</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="D112" t="n">
-        <v>443595</v>
+        <v>472750</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D113" t="n">
-        <v>579650</v>
+        <v>603650</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>152112</v>
+        <v>152783</v>
       </c>
       <c r="D115" t="n">
-        <v>187918151</v>
+        <v>188698791</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D117" t="n">
-        <v>109057</v>
+        <v>111614</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D119" t="n">
-        <v>1431454</v>
+        <v>1432954</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>55958</v>
+        <v>56229</v>
       </c>
       <c r="D121" t="n">
-        <v>81952560</v>
+        <v>82341310</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>29946</v>
+        <v>30147</v>
       </c>
       <c r="D123" t="n">
-        <v>43379905</v>
+        <v>43672287</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1358</v>
+        <v>1362</v>
       </c>
       <c r="D124" t="n">
-        <v>1861694</v>
+        <v>1866928</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2725</v>
+        <v>2753</v>
       </c>
       <c r="D127" t="n">
-        <v>3837480</v>
+        <v>3876443</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>600041</v>
+        <v>606428</v>
       </c>
       <c r="D129" t="n">
-        <v>792879663</v>
+        <v>801131527</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D130" t="n">
-        <v>138964</v>
+        <v>140464</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D131" t="n">
-        <v>357713</v>
+        <v>363713</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1537</v>
+        <v>1559</v>
       </c>
       <c r="D134" t="n">
-        <v>2276020</v>
+        <v>2308103</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>231459</v>
+        <v>233798</v>
       </c>
       <c r="D136" t="n">
-        <v>340055932</v>
+        <v>343460968</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>498</v>
+        <v>512</v>
       </c>
       <c r="D137" t="n">
-        <v>743670</v>
+        <v>764670</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>214686</v>
+        <v>217441</v>
       </c>
       <c r="D139" t="n">
-        <v>312250779</v>
+        <v>316211334</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2985</v>
+        <v>2999</v>
       </c>
       <c r="D142" t="n">
-        <v>4194258</v>
+        <v>4214408</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>8039</v>
+        <v>8213</v>
       </c>
       <c r="D145" t="n">
-        <v>11334094</v>
+        <v>11580406</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>49070</v>
+        <v>49316</v>
       </c>
       <c r="D148" t="n">
-        <v>65422470</v>
+        <v>65755456</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D149" t="n">
-        <v>43262</v>
+        <v>44762</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D152" t="n">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>15120</v>
+        <v>15206</v>
       </c>
       <c r="D154" t="n">
-        <v>22156523</v>
+        <v>22281267</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>4103</v>
+        <v>4128</v>
       </c>
       <c r="D155" t="n">
-        <v>5919727</v>
+        <v>5956326</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D158" t="n">
-        <v>603587</v>
+        <v>605087</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="D160" t="n">
-        <v>684473</v>
+        <v>693473</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>19390</v>
+        <v>19549</v>
       </c>
       <c r="D161" t="n">
-        <v>25647156</v>
+        <v>25859317</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>7995</v>
+        <v>8061</v>
       </c>
       <c r="D165" t="n">
-        <v>11630108</v>
+        <v>11722263</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5648</v>
+        <v>5714</v>
       </c>
       <c r="D167" t="n">
-        <v>8130016</v>
+        <v>8227781</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="D170" t="n">
-        <v>438766</v>
+        <v>455266</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>27895</v>
+        <v>28420</v>
       </c>
       <c r="D172" t="n">
-        <v>55559686</v>
+        <v>57008901</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2780</v>
+        <v>2825</v>
       </c>
       <c r="D173" t="n">
-        <v>5446655</v>
+        <v>5576937</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D174" t="n">
-        <v>684281</v>
+        <v>702800</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D177" t="n">
-        <v>353637</v>
+        <v>362637</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>93646</v>
+        <v>94067</v>
       </c>
       <c r="D178" t="n">
-        <v>116707570</v>
+        <v>117198557</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D180" t="n">
-        <v>125602</v>
+        <v>126520</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D183" t="n">
-        <v>962206</v>
+        <v>966706</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>35834</v>
+        <v>35989</v>
       </c>
       <c r="D185" t="n">
-        <v>52524907</v>
+        <v>52750330</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D186" t="n">
-        <v>43500</v>
+        <v>45000</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>14184</v>
+        <v>14278</v>
       </c>
       <c r="D187" t="n">
-        <v>20494194</v>
+        <v>20631292</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>1301</v>
+        <v>1305</v>
       </c>
       <c r="D189" t="n">
-        <v>1819862</v>
+        <v>1825862</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1968</v>
+        <v>2003</v>
       </c>
       <c r="D191" t="n">
-        <v>2764479</v>
+        <v>2812748</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>255130</v>
+        <v>256296</v>
       </c>
       <c r="D193" t="n">
-        <v>316354787</v>
+        <v>317718874</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D194" t="n">
-        <v>154051</v>
+        <v>158551</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D195" t="n">
-        <v>260979</v>
+        <v>263979</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="D199" t="n">
-        <v>1365779</v>
+        <v>1371779</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>91432</v>
+        <v>91868</v>
       </c>
       <c r="D201" t="n">
-        <v>133966134</v>
+        <v>134601329</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>35754</v>
+        <v>35960</v>
       </c>
       <c r="D204" t="n">
-        <v>51491832</v>
+        <v>51787310</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5371</v>
+        <v>5415</v>
       </c>
       <c r="D207" t="n">
-        <v>7652152</v>
+        <v>7716385</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>5826</v>
+        <v>5918</v>
       </c>
       <c r="D210" t="n">
-        <v>8069682</v>
+        <v>8194714</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>283574</v>
+        <v>284924</v>
       </c>
       <c r="D213" t="n">
-        <v>350332266</v>
+        <v>351877136</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8476,10 +8476,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D214" t="n">
-        <v>191969</v>
+        <v>193469</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>644</v>
+        <v>651</v>
       </c>
       <c r="D220" t="n">
-        <v>937014</v>
+        <v>947416</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>101066</v>
+        <v>101597</v>
       </c>
       <c r="D222" t="n">
-        <v>147815192</v>
+        <v>148581044</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>55884</v>
+        <v>56230</v>
       </c>
       <c r="D225" t="n">
-        <v>80742569</v>
+        <v>81239673</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D226" t="n">
-        <v>56422</v>
+        <v>57922</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>4880</v>
+        <v>4898</v>
       </c>
       <c r="D228" t="n">
-        <v>6850109</v>
+        <v>6876146</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D229" t="n">
-        <v>12000</v>
+        <v>13500</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>7226</v>
+        <v>7340</v>
       </c>
       <c r="D231" t="n">
-        <v>10008617</v>
+        <v>10166922</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>114359</v>
+        <v>114884</v>
       </c>
       <c r="D234" t="n">
-        <v>142618474</v>
+        <v>143223801</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D235" t="n">
-        <v>89550</v>
+        <v>91864</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="D239" t="n">
-        <v>861259</v>
+        <v>864259</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>52238</v>
+        <v>52462</v>
       </c>
       <c r="D241" t="n">
-        <v>76509039</v>
+        <v>76837490</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>13666</v>
+        <v>13757</v>
       </c>
       <c r="D243" t="n">
-        <v>19655941</v>
+        <v>19787799</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>1957</v>
+        <v>1960</v>
       </c>
       <c r="D245" t="n">
-        <v>2805589</v>
+        <v>2809244</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>2986</v>
+        <v>3027</v>
       </c>
       <c r="D247" t="n">
-        <v>4182797</v>
+        <v>4239477</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>279707</v>
+        <v>281313</v>
       </c>
       <c r="D248" t="n">
-        <v>352923428</v>
+        <v>354846866</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D250" t="n">
-        <v>382408</v>
+        <v>384469</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D253" t="n">
-        <v>23480</v>
+        <v>4500</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -9975,12 +9975,12 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>891</v>
+        <v>16</v>
       </c>
       <c r="D254" t="n">
-        <v>1309368</v>
+        <v>23480</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10013,12 +10013,12 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>12</v>
+        <v>898</v>
       </c>
       <c r="D255" t="n">
-        <v>18000</v>
+        <v>1319868</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10051,12 +10051,12 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -10072,10 +10072,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>102721</v>
+        <v>12</v>
       </c>
       <c r="D256" t="n">
-        <v>150471732</v>
+        <v>18000</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10089,12 +10089,12 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>89</v>
+        <v>103370</v>
       </c>
       <c r="D257" t="n">
-        <v>128564</v>
+        <v>151422064</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10127,12 +10127,12 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D258" t="n">
-        <v>7500</v>
+        <v>128564</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10165,12 +10165,12 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>71749</v>
+        <v>5</v>
       </c>
       <c r="D259" t="n">
-        <v>103980835</v>
+        <v>7500</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10203,12 +10203,12 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -10224,10 +10224,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>16</v>
+        <v>72394</v>
       </c>
       <c r="D260" t="n">
-        <v>23989</v>
+        <v>104909265</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -10241,12 +10241,12 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>2520</v>
+        <v>17</v>
       </c>
       <c r="D261" t="n">
-        <v>3550465</v>
+        <v>25489</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -10279,12 +10279,12 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -10300,10 +10300,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>11</v>
+        <v>2529</v>
       </c>
       <c r="D262" t="n">
-        <v>16500</v>
+        <v>3563065</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -10317,12 +10317,12 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -10338,10 +10338,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D263" t="n">
-        <v>10500</v>
+        <v>16500</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -10355,12 +10355,12 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>5691</v>
+        <v>7</v>
       </c>
       <c r="D264" t="n">
-        <v>7987189</v>
+        <v>10500</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10393,10 +10393,48 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>Syndicat de propriétaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>5801</v>
+      </c>
+      <c r="D265" t="n">
+        <v>8137964</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
           <t>92</t>
         </is>
       </c>
-      <c r="H264" t="inlineStr">
+      <c r="H265" t="inlineStr">
         <is>
           <t>Association loi 1901 ou assimilé</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-11-04 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>348894</v>
+        <v>350123</v>
       </c>
       <c r="D2" t="n">
-        <v>443573513</v>
+        <v>444980236</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D3" t="n">
-        <v>334819</v>
+        <v>341716</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D4" t="n">
-        <v>535359</v>
+        <v>538359</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D8" t="n">
-        <v>1350096</v>
+        <v>1353096</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>124903</v>
+        <v>125296</v>
       </c>
       <c r="D10" t="n">
-        <v>182919890</v>
+        <v>183490198</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>65320</v>
+        <v>65620</v>
       </c>
       <c r="D12" t="n">
-        <v>94283062</v>
+        <v>94717635</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4141</v>
+        <v>4147</v>
       </c>
       <c r="D16" t="n">
-        <v>5878129</v>
+        <v>5887129</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8447</v>
+        <v>8571</v>
       </c>
       <c r="D21" t="n">
-        <v>11797510</v>
+        <v>11967675</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>83159</v>
+        <v>83375</v>
       </c>
       <c r="D23" t="n">
-        <v>103299725</v>
+        <v>103525478</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>34224</v>
+        <v>34302</v>
       </c>
       <c r="D29" t="n">
-        <v>50083235</v>
+        <v>50199083</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D30" t="n">
-        <v>46937</v>
+        <v>51437</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12403</v>
+        <v>12452</v>
       </c>
       <c r="D32" t="n">
-        <v>17841033</v>
+        <v>17912328</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1607</v>
+        <v>1610</v>
       </c>
       <c r="D35" t="n">
-        <v>2258233</v>
+        <v>2262483</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2235</v>
+        <v>2266</v>
       </c>
       <c r="D37" t="n">
-        <v>3150546</v>
+        <v>3193473</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>103854</v>
+        <v>104185</v>
       </c>
       <c r="D38" t="n">
-        <v>130190445</v>
+        <v>130534703</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="D44" t="n">
-        <v>1353185</v>
+        <v>1357685</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>46713</v>
+        <v>46804</v>
       </c>
       <c r="D46" t="n">
-        <v>68419847</v>
+        <v>68553252</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9895</v>
+        <v>9929</v>
       </c>
       <c r="D48" t="n">
-        <v>14180007</v>
+        <v>14228962</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1476</v>
+        <v>1483</v>
       </c>
       <c r="D50" t="n">
-        <v>2054593</v>
+        <v>2064757</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2848</v>
+        <v>2877</v>
       </c>
       <c r="D53" t="n">
-        <v>3990357</v>
+        <v>4032931</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>74211</v>
+        <v>74437</v>
       </c>
       <c r="D54" t="n">
-        <v>92863995</v>
+        <v>93133618</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D59" t="n">
-        <v>572874</v>
+        <v>574374</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>29974</v>
+        <v>30051</v>
       </c>
       <c r="D61" t="n">
-        <v>43924014</v>
+        <v>44037363</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>12103</v>
+        <v>12149</v>
       </c>
       <c r="D64" t="n">
-        <v>17489732</v>
+        <v>17554377</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="D66" t="n">
-        <v>1993560</v>
+        <v>1997360</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1838</v>
+        <v>1856</v>
       </c>
       <c r="D70" t="n">
-        <v>2581579</v>
+        <v>2606327</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>22299</v>
+        <v>22388</v>
       </c>
       <c r="D72" t="n">
-        <v>29143144</v>
+        <v>29250777</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8225</v>
+        <v>8254</v>
       </c>
       <c r="D76" t="n">
-        <v>12044647</v>
+        <v>12085428</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5611</v>
+        <v>5652</v>
       </c>
       <c r="D78" t="n">
-        <v>8157054</v>
+        <v>8217431</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="D79" t="n">
-        <v>768062</v>
+        <v>771782</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D80" t="n">
-        <v>496996</v>
+        <v>502148</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>151676</v>
+        <v>152180</v>
       </c>
       <c r="D81" t="n">
-        <v>188486422</v>
+        <v>189012450</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D85" t="n">
-        <v>672583</v>
+        <v>675583</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>67211</v>
+        <v>67425</v>
       </c>
       <c r="D87" t="n">
-        <v>98466689</v>
+        <v>98763950</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>31948</v>
+        <v>32044</v>
       </c>
       <c r="D90" t="n">
-        <v>46211737</v>
+        <v>46351450</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2960</v>
+        <v>2973</v>
       </c>
       <c r="D92" t="n">
-        <v>4269847</v>
+        <v>4288182</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3449</v>
+        <v>3495</v>
       </c>
       <c r="D94" t="n">
-        <v>4875513</v>
+        <v>4937809</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>37615</v>
+        <v>37719</v>
       </c>
       <c r="D95" t="n">
-        <v>51033761</v>
+        <v>51166107</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9270</v>
+        <v>9305</v>
       </c>
       <c r="D99" t="n">
-        <v>13615717</v>
+        <v>13667118</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8649</v>
+        <v>8686</v>
       </c>
       <c r="D101" t="n">
-        <v>12549920</v>
+        <v>12601876</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>16232</v>
+        <v>16359</v>
       </c>
       <c r="D105" t="n">
-        <v>30144975</v>
+        <v>30477362</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D107" t="n">
-        <v>10500</v>
+        <v>13500</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3750</v>
+        <v>3766</v>
       </c>
       <c r="D108" t="n">
-        <v>7468111</v>
+        <v>7514801</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>5326</v>
+        <v>5369</v>
       </c>
       <c r="D110" t="n">
-        <v>10724999</v>
+        <v>10838494</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D112" t="n">
-        <v>472750</v>
+        <v>475750</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D113" t="n">
-        <v>603650</v>
+        <v>615650</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>152783</v>
+        <v>153266</v>
       </c>
       <c r="D115" t="n">
-        <v>188698791</v>
+        <v>189212382</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="D119" t="n">
-        <v>1432954</v>
+        <v>1443454</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>56229</v>
+        <v>56381</v>
       </c>
       <c r="D121" t="n">
-        <v>82341310</v>
+        <v>82559372</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>30147</v>
+        <v>30279</v>
       </c>
       <c r="D123" t="n">
-        <v>43672287</v>
+        <v>43859494</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1362</v>
+        <v>1367</v>
       </c>
       <c r="D124" t="n">
-        <v>1866928</v>
+        <v>1874428</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2753</v>
+        <v>2792</v>
       </c>
       <c r="D127" t="n">
-        <v>3876443</v>
+        <v>3931853</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>606428</v>
+        <v>610263</v>
       </c>
       <c r="D129" t="n">
-        <v>801131527</v>
+        <v>805914344</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D130" t="n">
-        <v>140464</v>
+        <v>141262</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1559</v>
+        <v>1573</v>
       </c>
       <c r="D134" t="n">
-        <v>2308103</v>
+        <v>2329103</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>233798</v>
+        <v>235221</v>
       </c>
       <c r="D136" t="n">
-        <v>343460968</v>
+        <v>345553299</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="D137" t="n">
-        <v>764670</v>
+        <v>778170</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D138" t="n">
-        <v>25500</v>
+        <v>26176</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>217441</v>
+        <v>219014</v>
       </c>
       <c r="D139" t="n">
-        <v>316211334</v>
+        <v>318478919</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2999</v>
+        <v>3008</v>
       </c>
       <c r="D142" t="n">
-        <v>4214408</v>
+        <v>4227398</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>8213</v>
+        <v>8353</v>
       </c>
       <c r="D145" t="n">
-        <v>11580406</v>
+        <v>11779054</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>49316</v>
+        <v>49414</v>
       </c>
       <c r="D148" t="n">
-        <v>65755456</v>
+        <v>65876806</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>15206</v>
+        <v>15239</v>
       </c>
       <c r="D154" t="n">
-        <v>22281267</v>
+        <v>22331826</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>4128</v>
+        <v>4139</v>
       </c>
       <c r="D155" t="n">
-        <v>5956326</v>
+        <v>5972826</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D157" t="n">
-        <v>10500</v>
+        <v>13500</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="D160" t="n">
-        <v>693473</v>
+        <v>702473</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>19549</v>
+        <v>19658</v>
       </c>
       <c r="D161" t="n">
-        <v>25859317</v>
+        <v>25993748</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6614,10 +6614,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>8061</v>
+        <v>8128</v>
       </c>
       <c r="D165" t="n">
-        <v>11722263</v>
+        <v>11822206</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5714</v>
+        <v>5771</v>
       </c>
       <c r="D167" t="n">
-        <v>8227781</v>
+        <v>8301874</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D170" t="n">
-        <v>455266</v>
+        <v>464266</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>28420</v>
+        <v>28581</v>
       </c>
       <c r="D172" t="n">
-        <v>57008901</v>
+        <v>57436650</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2825</v>
+        <v>2847</v>
       </c>
       <c r="D173" t="n">
-        <v>5576937</v>
+        <v>5642337</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D174" t="n">
-        <v>702800</v>
+        <v>714100</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D176" t="n">
-        <v>177516</v>
+        <v>183516</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D177" t="n">
-        <v>362637</v>
+        <v>365637</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>94067</v>
+        <v>94317</v>
       </c>
       <c r="D178" t="n">
-        <v>117198557</v>
+        <v>117462370</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>35989</v>
+        <v>36062</v>
       </c>
       <c r="D185" t="n">
-        <v>52750330</v>
+        <v>52856496</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>14278</v>
+        <v>14334</v>
       </c>
       <c r="D187" t="n">
-        <v>20631292</v>
+        <v>20706253</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>1305</v>
+        <v>1311</v>
       </c>
       <c r="D189" t="n">
-        <v>1825862</v>
+        <v>1833721</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>2003</v>
+        <v>2026</v>
       </c>
       <c r="D191" t="n">
-        <v>2812748</v>
+        <v>2846733</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>256296</v>
+        <v>257103</v>
       </c>
       <c r="D193" t="n">
-        <v>317718874</v>
+        <v>318574624</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D194" t="n">
-        <v>158551</v>
+        <v>160051</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D195" t="n">
-        <v>263979</v>
+        <v>266979</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="D199" t="n">
-        <v>1371779</v>
+        <v>1372781</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>91868</v>
+        <v>92097</v>
       </c>
       <c r="D201" t="n">
-        <v>134601329</v>
+        <v>134928515</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D202" t="n">
-        <v>150127</v>
+        <v>151627</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>35960</v>
+        <v>36104</v>
       </c>
       <c r="D204" t="n">
-        <v>51787310</v>
+        <v>51989618</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5415</v>
+        <v>5438</v>
       </c>
       <c r="D207" t="n">
-        <v>7716385</v>
+        <v>7747604</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>5918</v>
+        <v>5974</v>
       </c>
       <c r="D210" t="n">
-        <v>8194714</v>
+        <v>8271357</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>284924</v>
+        <v>285877</v>
       </c>
       <c r="D213" t="n">
-        <v>351877136</v>
+        <v>352899426</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D220" t="n">
-        <v>947416</v>
+        <v>950416</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>101597</v>
+        <v>101853</v>
       </c>
       <c r="D222" t="n">
-        <v>148581044</v>
+        <v>148955464</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>56230</v>
+        <v>56429</v>
       </c>
       <c r="D225" t="n">
-        <v>81239673</v>
+        <v>81528823</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>4898</v>
+        <v>4907</v>
       </c>
       <c r="D228" t="n">
-        <v>6876146</v>
+        <v>6887606</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>7340</v>
+        <v>7427</v>
       </c>
       <c r="D231" t="n">
-        <v>10166922</v>
+        <v>10280506</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>114884</v>
+        <v>115252</v>
       </c>
       <c r="D234" t="n">
-        <v>143223801</v>
+        <v>143634828</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9274,10 +9274,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D235" t="n">
-        <v>91864</v>
+        <v>95367</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D239" t="n">
-        <v>864259</v>
+        <v>867259</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>52462</v>
+        <v>52545</v>
       </c>
       <c r="D241" t="n">
-        <v>76837490</v>
+        <v>76955478</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>13757</v>
+        <v>13819</v>
       </c>
       <c r="D243" t="n">
-        <v>19787799</v>
+        <v>19877285</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>3027</v>
+        <v>3055</v>
       </c>
       <c r="D247" t="n">
-        <v>4239477</v>
+        <v>4276590</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>281313</v>
+        <v>282374</v>
       </c>
       <c r="D248" t="n">
-        <v>354846866</v>
+        <v>356067759</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D249" t="n">
-        <v>237452</v>
+        <v>240452</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>898</v>
+        <v>904</v>
       </c>
       <c r="D255" t="n">
-        <v>1319868</v>
+        <v>1328329</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>103370</v>
+        <v>103833</v>
       </c>
       <c r="D257" t="n">
-        <v>151422064</v>
+        <v>152111458</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10224,10 +10224,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>72394</v>
+        <v>72832</v>
       </c>
       <c r="D260" t="n">
-        <v>104909265</v>
+        <v>105544871</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -10300,10 +10300,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>2529</v>
+        <v>2542</v>
       </c>
       <c r="D262" t="n">
-        <v>3563065</v>
+        <v>3581108</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -10338,10 +10338,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D263" t="n">
-        <v>16500</v>
+        <v>18000</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>5801</v>
+        <v>5913</v>
       </c>
       <c r="D265" t="n">
-        <v>8137964</v>
+        <v>8292918</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-11-22 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>368418</v>
+        <v>371530</v>
       </c>
       <c r="D2" t="n">
-        <v>473340448</v>
+        <v>478438275</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D3" t="n">
-        <v>357855</v>
+        <v>358730</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D4" t="n">
-        <v>567985</v>
+        <v>575460</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>976</v>
+        <v>985</v>
       </c>
       <c r="D9" t="n">
-        <v>1493959</v>
+        <v>1523938</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="n">
-        <v>38256</v>
+        <v>48256</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>131126</v>
+        <v>132060</v>
       </c>
       <c r="D11" t="n">
-        <v>199611581</v>
+        <v>202599608</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D12" t="n">
-        <v>229177</v>
+        <v>230677</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>69424</v>
+        <v>70005</v>
       </c>
       <c r="D13" t="n">
-        <v>105260803</v>
+        <v>107202458</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4226</v>
+        <v>4234</v>
       </c>
       <c r="D17" t="n">
-        <v>6035522</v>
+        <v>6065494</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9205</v>
+        <v>9284</v>
       </c>
       <c r="D22" t="n">
-        <v>13299083</v>
+        <v>13521155</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>87208</v>
+        <v>87824</v>
       </c>
       <c r="D24" t="n">
-        <v>108568469</v>
+        <v>109419554</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D25" t="n">
-        <v>84209</v>
+        <v>94209</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D29" t="n">
-        <v>436753</v>
+        <v>440083</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>35642</v>
+        <v>35854</v>
       </c>
       <c r="D30" t="n">
-        <v>53120097</v>
+        <v>53581734</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>13010</v>
+        <v>13109</v>
       </c>
       <c r="D33" t="n">
-        <v>19252667</v>
+        <v>19521818</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1658</v>
+        <v>1663</v>
       </c>
       <c r="D36" t="n">
-        <v>2372583</v>
+        <v>2392578</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2409</v>
+        <v>2432</v>
       </c>
       <c r="D38" t="n">
-        <v>3440606</v>
+        <v>3490955</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>108335</v>
+        <v>108987</v>
       </c>
       <c r="D39" t="n">
-        <v>136030163</v>
+        <v>136858251</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D40" t="n">
-        <v>80868</v>
+        <v>82368</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D41" t="n">
-        <v>124578</v>
+        <v>126078</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="D45" t="n">
-        <v>1399938</v>
+        <v>1404517</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>48523</v>
+        <v>48847</v>
       </c>
       <c r="D47" t="n">
-        <v>72126096</v>
+        <v>72731871</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>10385</v>
+        <v>10455</v>
       </c>
       <c r="D49" t="n">
-        <v>15286956</v>
+        <v>15456034</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1507</v>
+        <v>1512</v>
       </c>
       <c r="D51" t="n">
-        <v>2105730</v>
+        <v>2111195</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3056</v>
+        <v>3078</v>
       </c>
       <c r="D54" t="n">
-        <v>4373978</v>
+        <v>4436798</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>77920</v>
+        <v>78465</v>
       </c>
       <c r="D55" t="n">
-        <v>98147558</v>
+        <v>99007845</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D57" t="n">
-        <v>81400</v>
+        <v>89637</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D60" t="n">
-        <v>593151</v>
+        <v>595015</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>31364</v>
+        <v>31588</v>
       </c>
       <c r="D62" t="n">
-        <v>46930822</v>
+        <v>47359833</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D63" t="n">
-        <v>42284</v>
+        <v>44450</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>12766</v>
+        <v>12882</v>
       </c>
       <c r="D65" t="n">
-        <v>18897907</v>
+        <v>19145030</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1463</v>
+        <v>1469</v>
       </c>
       <c r="D67" t="n">
-        <v>2049815</v>
+        <v>2058169</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1966</v>
+        <v>1982</v>
       </c>
       <c r="D71" t="n">
-        <v>2851978</v>
+        <v>2909419</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>23508</v>
+        <v>23648</v>
       </c>
       <c r="D73" t="n">
-        <v>30957696</v>
+        <v>31163970</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>8614</v>
+        <v>8660</v>
       </c>
       <c r="D77" t="n">
-        <v>13004665</v>
+        <v>13164204</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5938</v>
+        <v>5971</v>
       </c>
       <c r="D79" t="n">
-        <v>8951723</v>
+        <v>9022672</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D80" t="n">
-        <v>838391</v>
+        <v>839491</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D81" t="n">
-        <v>569028</v>
+        <v>572028</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>159382</v>
+        <v>160494</v>
       </c>
       <c r="D82" t="n">
-        <v>198924752</v>
+        <v>200523980</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D84" t="n">
-        <v>141059</v>
+        <v>143578</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D86" t="n">
-        <v>707270</v>
+        <v>709352</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>69878</v>
+        <v>70351</v>
       </c>
       <c r="D88" t="n">
-        <v>103922169</v>
+        <v>104907477</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>33464</v>
+        <v>33691</v>
       </c>
       <c r="D91" t="n">
-        <v>49571965</v>
+        <v>50157610</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>3059</v>
+        <v>3060</v>
       </c>
       <c r="D93" t="n">
-        <v>4467236</v>
+        <v>4477236</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>3719</v>
+        <v>3747</v>
       </c>
       <c r="D95" t="n">
-        <v>5381025</v>
+        <v>5466073</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>39123</v>
+        <v>39356</v>
       </c>
       <c r="D96" t="n">
-        <v>53609747</v>
+        <v>54054988</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>9738</v>
+        <v>9799</v>
       </c>
       <c r="D100" t="n">
-        <v>14737805</v>
+        <v>14925015</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9052</v>
+        <v>9098</v>
       </c>
       <c r="D102" t="n">
-        <v>13526673</v>
+        <v>13685471</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D104" t="n">
-        <v>869044</v>
+        <v>878127</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>17151</v>
+        <v>17206</v>
       </c>
       <c r="D106" t="n">
-        <v>32774515</v>
+        <v>32992757</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3941</v>
+        <v>3956</v>
       </c>
       <c r="D109" t="n">
-        <v>8078607</v>
+        <v>8140751</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>5639</v>
+        <v>5658</v>
       </c>
       <c r="D111" t="n">
-        <v>11720603</v>
+        <v>11823621</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D114" t="n">
-        <v>666578</v>
+        <v>675578</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>161635</v>
+        <v>163083</v>
       </c>
       <c r="D116" t="n">
-        <v>201531290</v>
+        <v>203707585</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1030</v>
+        <v>1041</v>
       </c>
       <c r="D120" t="n">
-        <v>1549192</v>
+        <v>1578470</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>59023</v>
+        <v>59463</v>
       </c>
       <c r="D122" t="n">
-        <v>89595237</v>
+        <v>90839555</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D123" t="n">
-        <v>169671</v>
+        <v>171171</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>32079</v>
+        <v>32378</v>
       </c>
       <c r="D124" t="n">
-        <v>48600223</v>
+        <v>49490443</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1404</v>
+        <v>1406</v>
       </c>
       <c r="D125" t="n">
-        <v>1954795</v>
+        <v>1961480</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3047</v>
+        <v>3073</v>
       </c>
       <c r="D129" t="n">
-        <v>4443688</v>
+        <v>4526822</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>663222</v>
+        <v>672564</v>
       </c>
       <c r="D131" t="n">
-        <v>904356216</v>
+        <v>924790001</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D132" t="n">
-        <v>157262</v>
+        <v>167262</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D133" t="n">
-        <v>427901</v>
+        <v>447901</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1730</v>
+        <v>1753</v>
       </c>
       <c r="D136" t="n">
-        <v>2862774</v>
+        <v>2940143</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D137" t="n">
-        <v>69510</v>
+        <v>79510</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>250551</v>
+        <v>253040</v>
       </c>
       <c r="D138" t="n">
-        <v>392346793</v>
+        <v>401749785</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="D139" t="n">
-        <v>1127693</v>
+        <v>1182549</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D140" t="n">
-        <v>44974</v>
+        <v>53957</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>238120</v>
+        <v>241101</v>
       </c>
       <c r="D141" t="n">
-        <v>374479186</v>
+        <v>385332368</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>3138</v>
+        <v>3153</v>
       </c>
       <c r="D144" t="n">
-        <v>4511714</v>
+        <v>4548870</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>9192</v>
+        <v>9273</v>
       </c>
       <c r="D147" t="n">
-        <v>13606385</v>
+        <v>13863695</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>51273</v>
+        <v>51456</v>
       </c>
       <c r="D150" t="n">
-        <v>68851418</v>
+        <v>69206237</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D154" t="n">
-        <v>14809</v>
+        <v>19118</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>15691</v>
+        <v>15731</v>
       </c>
       <c r="D156" t="n">
-        <v>23271588</v>
+        <v>23403390</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4283</v>
+        <v>4295</v>
       </c>
       <c r="D157" t="n">
-        <v>6247165</v>
+        <v>6281513</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6500,10 +6500,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="D162" t="n">
-        <v>784081</v>
+        <v>791921</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -6538,10 +6538,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>20534</v>
+        <v>20664</v>
       </c>
       <c r="D163" t="n">
-        <v>27321758</v>
+        <v>27545267</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>8525</v>
+        <v>8588</v>
       </c>
       <c r="D167" t="n">
-        <v>12717422</v>
+        <v>12914262</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>6086</v>
+        <v>6122</v>
       </c>
       <c r="D169" t="n">
-        <v>9016339</v>
+        <v>9136021</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D172" t="n">
-        <v>516444</v>
+        <v>519444</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>29595</v>
+        <v>29719</v>
       </c>
       <c r="D174" t="n">
-        <v>60652344</v>
+        <v>61277131</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>2983</v>
+        <v>3000</v>
       </c>
       <c r="D176" t="n">
-        <v>6116252</v>
+        <v>6200380</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D177" t="n">
-        <v>804159</v>
+        <v>825982</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D179" t="n">
-        <v>194523</v>
+        <v>199530</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D180" t="n">
-        <v>410487</v>
+        <v>415887</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>98636</v>
+        <v>99350</v>
       </c>
       <c r="D181" t="n">
-        <v>123425161</v>
+        <v>124412865</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="D186" t="n">
-        <v>1007119</v>
+        <v>1017500</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>37606</v>
+        <v>37876</v>
       </c>
       <c r="D188" t="n">
-        <v>56599653</v>
+        <v>57267264</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>15128</v>
+        <v>15252</v>
       </c>
       <c r="D190" t="n">
-        <v>22748540</v>
+        <v>23127385</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D192" t="n">
-        <v>1885554</v>
+        <v>1887054</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>2174</v>
+        <v>2188</v>
       </c>
       <c r="D194" t="n">
-        <v>3148319</v>
+        <v>3183099</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>268097</v>
+        <v>269725</v>
       </c>
       <c r="D196" t="n">
-        <v>333478799</v>
+        <v>335896009</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D198" t="n">
-        <v>278155</v>
+        <v>281155</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="D202" t="n">
-        <v>1451026</v>
+        <v>1470026</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>95648</v>
+        <v>96156</v>
       </c>
       <c r="D204" t="n">
-        <v>142757191</v>
+        <v>143794046</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>37811</v>
+        <v>38064</v>
       </c>
       <c r="D207" t="n">
-        <v>55783864</v>
+        <v>56437565</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>5576</v>
+        <v>5582</v>
       </c>
       <c r="D210" t="n">
-        <v>8030982</v>
+        <v>8047721</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>6385</v>
+        <v>6423</v>
       </c>
       <c r="D213" t="n">
-        <v>8984958</v>
+        <v>9090951</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>300610</v>
+        <v>302985</v>
       </c>
       <c r="D216" t="n">
-        <v>374377231</v>
+        <v>378000974</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="D223" t="n">
-        <v>1033447</v>
+        <v>1057023</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>106524</v>
+        <v>107201</v>
       </c>
       <c r="D225" t="n">
-        <v>161794836</v>
+        <v>163869518</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>59483</v>
+        <v>59916</v>
       </c>
       <c r="D228" t="n">
-        <v>89651369</v>
+        <v>90949260</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>5029</v>
+        <v>5042</v>
       </c>
       <c r="D231" t="n">
-        <v>7101378</v>
+        <v>7124092</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>8043</v>
+        <v>8099</v>
       </c>
       <c r="D234" t="n">
-        <v>11495720</v>
+        <v>11638662</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>120397</v>
+        <v>121145</v>
       </c>
       <c r="D237" t="n">
-        <v>150555437</v>
+        <v>151574078</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D239" t="n">
-        <v>130401</v>
+        <v>131901</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D240" t="n">
-        <v>17147</v>
+        <v>18647</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="D242" t="n">
-        <v>882966</v>
+        <v>888837</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9616,10 +9616,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>54663</v>
+        <v>55050</v>
       </c>
       <c r="D244" t="n">
-        <v>81080113</v>
+        <v>81774514</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>14568</v>
+        <v>14683</v>
       </c>
       <c r="D246" t="n">
-        <v>21471994</v>
+        <v>21777042</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>1992</v>
+        <v>1997</v>
       </c>
       <c r="D248" t="n">
-        <v>2887401</v>
+        <v>2903697</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>3247</v>
+        <v>3263</v>
       </c>
       <c r="D250" t="n">
-        <v>4627210</v>
+        <v>4672030</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>298889</v>
+        <v>301566</v>
       </c>
       <c r="D251" t="n">
-        <v>382413075</v>
+        <v>386977432</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D252" t="n">
-        <v>261483</v>
+        <v>266658</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D253" t="n">
-        <v>400849</v>
+        <v>402541</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="D258" t="n">
-        <v>1502512</v>
+        <v>1524245</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10224,10 +10224,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>109828</v>
+        <v>110620</v>
       </c>
       <c r="D260" t="n">
-        <v>169149978</v>
+        <v>171715362</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -10338,10 +10338,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>78284</v>
+        <v>78981</v>
       </c>
       <c r="D263" t="n">
-        <v>120540492</v>
+        <v>122830034</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>2648</v>
+        <v>2662</v>
       </c>
       <c r="D265" t="n">
-        <v>3784800</v>
+        <v>3832416</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>6472</v>
+        <v>6535</v>
       </c>
       <c r="D268" t="n">
-        <v>9464309</v>
+        <v>9640490</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-06 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>406517</v>
+        <v>401914</v>
       </c>
       <c r="D2" t="n">
-        <v>563443264</v>
+        <v>548370962</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D3" t="n">
-        <v>429654</v>
+        <v>404666</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D4" t="n">
-        <v>771901</v>
+        <v>739056</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1205</v>
+        <v>1180</v>
       </c>
       <c r="D9" t="n">
-        <v>2445633</v>
+        <v>2258931</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>152485</v>
+        <v>149971</v>
       </c>
       <c r="D11" t="n">
-        <v>298236107</v>
+        <v>279649567</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D12" t="n">
-        <v>502302</v>
+        <v>468873</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>80320</v>
+        <v>78975</v>
       </c>
       <c r="D13" t="n">
-        <v>156159623</v>
+        <v>146774176</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4418</v>
+        <v>4396</v>
       </c>
       <c r="D17" t="n">
-        <v>6800849</v>
+        <v>6667785</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>10262</v>
+        <v>10155</v>
       </c>
       <c r="D22" t="n">
-        <v>17412866</v>
+        <v>16851101</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>96750</v>
+        <v>95487</v>
       </c>
       <c r="D24" t="n">
-        <v>130094120</v>
+        <v>125913996</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="D29" t="n">
-        <v>705351</v>
+        <v>625455</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>41501</v>
+        <v>40778</v>
       </c>
       <c r="D30" t="n">
-        <v>78178917</v>
+        <v>72748095</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" t="n">
-        <v>115964</v>
+        <v>106812</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>38166</v>
+        <v>28166</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>15088</v>
+        <v>14814</v>
       </c>
       <c r="D33" t="n">
-        <v>28257517</v>
+        <v>26391462</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1754</v>
+        <v>1748</v>
       </c>
       <c r="D36" t="n">
-        <v>2682924</v>
+        <v>2655361</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2650</v>
+        <v>2625</v>
       </c>
       <c r="D38" t="n">
-        <v>4311957</v>
+        <v>4159120</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>119274</v>
+        <v>117767</v>
       </c>
       <c r="D39" t="n">
-        <v>161654290</v>
+        <v>156394411</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" t="n">
-        <v>155334</v>
+        <v>153834</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1232</v>
+        <v>1206</v>
       </c>
       <c r="D45" t="n">
-        <v>2229632</v>
+        <v>2030510</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>57472</v>
+        <v>56231</v>
       </c>
       <c r="D47" t="n">
-        <v>109686001</v>
+        <v>100388271</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D48" t="n">
-        <v>119662</v>
+        <v>99662</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>12212</v>
+        <v>11959</v>
       </c>
       <c r="D49" t="n">
-        <v>23363002</v>
+        <v>21538578</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1570</v>
+        <v>1564</v>
       </c>
       <c r="D51" t="n">
-        <v>2319882</v>
+        <v>2288387</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3374</v>
+        <v>3346</v>
       </c>
       <c r="D54" t="n">
-        <v>5390098</v>
+        <v>5259172</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>86179</v>
+        <v>85033</v>
       </c>
       <c r="D55" t="n">
-        <v>119042368</v>
+        <v>114868078</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D57" t="n">
-        <v>103636</v>
+        <v>93636</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D60" t="n">
-        <v>24500</v>
+        <v>14500</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="D61" t="n">
-        <v>940484</v>
+        <v>875740</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>36496</v>
+        <v>35803</v>
       </c>
       <c r="D63" t="n">
-        <v>69948838</v>
+        <v>64874249</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D64" t="n">
-        <v>135614</v>
+        <v>104948</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>14742</v>
+        <v>14458</v>
       </c>
       <c r="D66" t="n">
-        <v>27945319</v>
+        <v>25985505</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1557</v>
+        <v>1550</v>
       </c>
       <c r="D68" t="n">
-        <v>2398863</v>
+        <v>2371074</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2179</v>
+        <v>2154</v>
       </c>
       <c r="D72" t="n">
-        <v>3595616</v>
+        <v>3486270</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>25835</v>
+        <v>25572</v>
       </c>
       <c r="D74" t="n">
-        <v>36852221</v>
+        <v>35891209</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D76" t="n">
-        <v>69891</v>
+        <v>59891</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D77" t="n">
-        <v>146431</v>
+        <v>136431</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>10094</v>
+        <v>9897</v>
       </c>
       <c r="D78" t="n">
-        <v>20279964</v>
+        <v>18819532</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6903</v>
+        <v>6780</v>
       </c>
       <c r="D80" t="n">
-        <v>13614295</v>
+        <v>12709567</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D81" t="n">
-        <v>985956</v>
+        <v>961532</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D82" t="n">
-        <v>730182</v>
+        <v>719274</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>175817</v>
+        <v>173721</v>
       </c>
       <c r="D83" t="n">
-        <v>238593187</v>
+        <v>231486719</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D84" t="n">
-        <v>212662</v>
+        <v>197081</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D85" t="n">
-        <v>231384</v>
+        <v>197840</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="D87" t="n">
-        <v>1208040</v>
+        <v>1129749</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>80649</v>
+        <v>79320</v>
       </c>
       <c r="D89" t="n">
-        <v>149792381</v>
+        <v>139968188</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D90" t="n">
-        <v>358732</v>
+        <v>319015</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>38366</v>
+        <v>37707</v>
       </c>
       <c r="D92" t="n">
-        <v>70796576</v>
+        <v>65986948</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3712</v>
+        <v>3661</v>
       </c>
       <c r="D94" t="n">
-        <v>8713636</v>
+        <v>8337782</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4074</v>
+        <v>4047</v>
       </c>
       <c r="D96" t="n">
-        <v>6664877</v>
+        <v>6501885</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>41704</v>
+        <v>41510</v>
       </c>
       <c r="D97" t="n">
-        <v>59697247</v>
+        <v>58965133</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>10401</v>
+        <v>10339</v>
       </c>
       <c r="D101" t="n">
-        <v>17090943</v>
+        <v>16730430</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>9687</v>
+        <v>9644</v>
       </c>
       <c r="D103" t="n">
-        <v>15386046</v>
+        <v>15197282</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D105" t="n">
-        <v>944682</v>
+        <v>934682</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D106" t="n">
-        <v>983952</v>
+        <v>982452</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>17836</v>
+        <v>17775</v>
       </c>
       <c r="D107" t="n">
-        <v>35867577</v>
+        <v>35467766</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4067</v>
+        <v>4060</v>
       </c>
       <c r="D110" t="n">
-        <v>8743566</v>
+        <v>8688326</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5856</v>
+        <v>5841</v>
       </c>
       <c r="D112" t="n">
-        <v>12866808</v>
+        <v>12744979</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D115" t="n">
-        <v>733125</v>
+        <v>723125</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>179735</v>
+        <v>177338</v>
       </c>
       <c r="D117" t="n">
-        <v>245145049</v>
+        <v>236925142</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D118" t="n">
-        <v>53833</v>
+        <v>52233</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D119" t="n">
-        <v>141041</v>
+        <v>131041</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1330</v>
+        <v>1297</v>
       </c>
       <c r="D121" t="n">
-        <v>2761420</v>
+        <v>2515289</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>68689</v>
+        <v>67458</v>
       </c>
       <c r="D123" t="n">
-        <v>132732507</v>
+        <v>123546423</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D124" t="n">
-        <v>391077</v>
+        <v>342379</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>37178</v>
+        <v>36543</v>
       </c>
       <c r="D126" t="n">
-        <v>71681485</v>
+        <v>67171728</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1505</v>
+        <v>1496</v>
       </c>
       <c r="D127" t="n">
-        <v>2426794</v>
+        <v>2359029</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>3402</v>
+        <v>3372</v>
       </c>
       <c r="D131" t="n">
-        <v>5757952</v>
+        <v>5608572</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>734493</v>
+        <v>725898</v>
       </c>
       <c r="D133" t="n">
-        <v>1117516473</v>
+        <v>1084747691</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D134" t="n">
-        <v>198665</v>
+        <v>188665</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D135" t="n">
-        <v>617782</v>
+        <v>586542</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D137" t="n">
-        <v>61164</v>
+        <v>51164</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>2198</v>
+        <v>2149</v>
       </c>
       <c r="D138" t="n">
-        <v>5496668</v>
+        <v>5094614</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D139" t="n">
-        <v>166681</v>
+        <v>156681</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>285693</v>
+        <v>281725</v>
       </c>
       <c r="D140" t="n">
-        <v>565955359</v>
+        <v>536835956</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>803</v>
+        <v>781</v>
       </c>
       <c r="D141" t="n">
-        <v>2609747</v>
+        <v>2405527</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D142" t="n">
-        <v>210140</v>
+        <v>180140</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>270288</v>
+        <v>266629</v>
       </c>
       <c r="D143" t="n">
-        <v>528676920</v>
+        <v>503860762</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D145" t="n">
-        <v>139620</v>
+        <v>129620</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>3373</v>
+        <v>3347</v>
       </c>
       <c r="D146" t="n">
-        <v>5308990</v>
+        <v>5192473</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D147" t="n">
-        <v>24133</v>
+        <v>14133</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>10309</v>
+        <v>10217</v>
       </c>
       <c r="D149" t="n">
-        <v>18027183</v>
+        <v>17477392</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>52919</v>
+        <v>52757</v>
       </c>
       <c r="D152" t="n">
-        <v>72594051</v>
+        <v>72119232</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D154" t="n">
-        <v>72619</v>
+        <v>62619</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>16090</v>
+        <v>16060</v>
       </c>
       <c r="D158" t="n">
-        <v>24954548</v>
+        <v>24793760</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4426</v>
+        <v>4416</v>
       </c>
       <c r="D160" t="n">
-        <v>6747281</v>
+        <v>6693402</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>22343</v>
+        <v>22179</v>
       </c>
       <c r="D166" t="n">
-        <v>31731512</v>
+        <v>31191988</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>9438</v>
+        <v>9324</v>
       </c>
       <c r="D170" t="n">
-        <v>16594695</v>
+        <v>15847758</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6880,10 +6880,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>6738</v>
+        <v>6671</v>
       </c>
       <c r="D172" t="n">
-        <v>11575198</v>
+        <v>11181777</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D174" t="n">
-        <v>481434</v>
+        <v>471434</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D175" t="n">
-        <v>656442</v>
+        <v>638175</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7070,10 +7070,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>31357</v>
+        <v>31246</v>
       </c>
       <c r="D177" t="n">
-        <v>70497431</v>
+        <v>69637134</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>3133</v>
+        <v>3124</v>
       </c>
       <c r="D179" t="n">
-        <v>7015840</v>
+        <v>6944881</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D180" t="n">
-        <v>920679</v>
+        <v>910679</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D183" t="n">
-        <v>451087</v>
+        <v>441087</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>109988</v>
+        <v>108412</v>
       </c>
       <c r="D184" t="n">
-        <v>151178803</v>
+        <v>145380630</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D186" t="n">
-        <v>184148</v>
+        <v>160610</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>872</v>
+        <v>857</v>
       </c>
       <c r="D189" t="n">
-        <v>1697888</v>
+        <v>1593987</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>44457</v>
+        <v>43487</v>
       </c>
       <c r="D191" t="n">
-        <v>87616313</v>
+        <v>80179336</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>17762</v>
+        <v>17375</v>
       </c>
       <c r="D193" t="n">
-        <v>34693045</v>
+        <v>32009244</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D194" t="n">
-        <v>16725</v>
+        <v>15322</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>1414</v>
+        <v>1404</v>
       </c>
       <c r="D195" t="n">
-        <v>2131685</v>
+        <v>2070988</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>2403</v>
+        <v>2373</v>
       </c>
       <c r="D197" t="n">
-        <v>3957414</v>
+        <v>3801888</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>294051</v>
+        <v>290407</v>
       </c>
       <c r="D199" t="n">
-        <v>396021123</v>
+        <v>384491088</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D200" t="n">
-        <v>178194</v>
+        <v>176916</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D201" t="n">
-        <v>367685</v>
+        <v>337562</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1178</v>
+        <v>1152</v>
       </c>
       <c r="D205" t="n">
-        <v>2216366</v>
+        <v>2033117</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>110827</v>
+        <v>108622</v>
       </c>
       <c r="D207" t="n">
-        <v>210537236</v>
+        <v>194289839</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D208" t="n">
-        <v>323687</v>
+        <v>292112</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>43649</v>
+        <v>42799</v>
       </c>
       <c r="D210" t="n">
-        <v>82121595</v>
+        <v>76174365</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D212" t="n">
-        <v>26454</v>
+        <v>26114</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8438,10 +8438,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>5927</v>
+        <v>5888</v>
       </c>
       <c r="D213" t="n">
-        <v>9474186</v>
+        <v>9271944</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>7084</v>
+        <v>7015</v>
       </c>
       <c r="D216" t="n">
-        <v>11315073</v>
+        <v>10965617</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>332095</v>
+        <v>328218</v>
       </c>
       <c r="D219" t="n">
-        <v>444457472</v>
+        <v>432384436</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D220" t="n">
-        <v>236374</v>
+        <v>234375</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D221" t="n">
-        <v>485576</v>
+        <v>475946</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8932,10 +8932,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>825</v>
+        <v>812</v>
       </c>
       <c r="D226" t="n">
-        <v>1596858</v>
+        <v>1513638</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>123300</v>
+        <v>121202</v>
       </c>
       <c r="D228" t="n">
-        <v>236542812</v>
+        <v>221354347</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9046,10 +9046,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D229" t="n">
-        <v>378947</v>
+        <v>328947</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>68552</v>
+        <v>67401</v>
       </c>
       <c r="D231" t="n">
-        <v>130818482</v>
+        <v>122717941</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9160,10 +9160,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D232" t="n">
-        <v>109313</v>
+        <v>106985</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D233" t="n">
-        <v>28660</v>
+        <v>27160</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>5359</v>
+        <v>5325</v>
       </c>
       <c r="D234" t="n">
-        <v>8223100</v>
+        <v>8037821</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D236" t="n">
-        <v>24078</v>
+        <v>14078</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>8971</v>
+        <v>8896</v>
       </c>
       <c r="D238" t="n">
-        <v>14677372</v>
+        <v>14294550</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>132256</v>
+        <v>130597</v>
       </c>
       <c r="D241" t="n">
-        <v>180037136</v>
+        <v>174416879</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D243" t="n">
-        <v>190050</v>
+        <v>184307</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="D246" t="n">
-        <v>1503040</v>
+        <v>1338222</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>63850</v>
+        <v>62551</v>
       </c>
       <c r="D248" t="n">
-        <v>122141064</v>
+        <v>112357328</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>16865</v>
+        <v>16529</v>
       </c>
       <c r="D250" t="n">
-        <v>31896873</v>
+        <v>29540884</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D251" t="n">
-        <v>21529</v>
+        <v>18335</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>2103</v>
+        <v>2086</v>
       </c>
       <c r="D252" t="n">
-        <v>3273259</v>
+        <v>3196363</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9996,10 +9996,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>3544</v>
+        <v>3517</v>
       </c>
       <c r="D254" t="n">
-        <v>5637837</v>
+        <v>5505520</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>332347</v>
+        <v>328162</v>
       </c>
       <c r="D255" t="n">
-        <v>460392856</v>
+        <v>447109432</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D257" t="n">
-        <v>547192</v>
+        <v>523747</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D258" t="n">
-        <v>78455</v>
+        <v>69705</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10300,10 +10300,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>1270</v>
+        <v>1242</v>
       </c>
       <c r="D262" t="n">
-        <v>2996083</v>
+        <v>2758276</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>128391</v>
+        <v>126031</v>
       </c>
       <c r="D264" t="n">
-        <v>257954385</v>
+        <v>240500456</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D265" t="n">
-        <v>439104</v>
+        <v>371986</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D266" t="n">
-        <v>50500</v>
+        <v>40500</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10490,10 +10490,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>91427</v>
+        <v>89810</v>
       </c>
       <c r="D267" t="n">
-        <v>181572799</v>
+        <v>170623232</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -10566,10 +10566,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>2861</v>
+        <v>2835</v>
       </c>
       <c r="D269" t="n">
-        <v>4506467</v>
+        <v>4398764</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -10642,10 +10642,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D271" t="n">
-        <v>45234</v>
+        <v>36730</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -10680,10 +10680,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>7322</v>
+        <v>7248</v>
       </c>
       <c r="D272" t="n">
-        <v>12470578</v>
+        <v>12078393</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Correct 2020-12-06 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -711,10 +711,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>395522</v>
+        <v>401914</v>
       </c>
       <c r="D2">
-        <v>528589981</v>
+        <v>548370962</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -737,10 +737,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D3">
-        <v>394997</v>
+        <v>404666</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -763,10 +763,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D4">
-        <v>705778</v>
+        <v>739056</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -893,10 +893,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1160</v>
+        <v>1180</v>
       </c>
       <c r="D9">
-        <v>2090906</v>
+        <v>2258931</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -919,10 +919,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>50451</v>
+        <v>70451</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -945,10 +945,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>146965</v>
+        <v>149971</v>
       </c>
       <c r="D11">
-        <v>258087643</v>
+        <v>279649567</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -971,10 +971,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D12">
-        <v>447373</v>
+        <v>468873</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -997,10 +997,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>77506</v>
+        <v>78975</v>
       </c>
       <c r="D13">
-        <v>136849817</v>
+        <v>146774176</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1049,10 +1049,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>96835</v>
+        <v>98071</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1101,10 +1101,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>4378</v>
+        <v>4396</v>
       </c>
       <c r="D17">
-        <v>6573398</v>
+        <v>6667785</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1179,10 +1179,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D20">
-        <v>131035</v>
+        <v>151035</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1231,10 +1231,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>10065</v>
+        <v>10155</v>
       </c>
       <c r="D22">
-        <v>16391951</v>
+        <v>16851101</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1283,10 +1283,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>93745</v>
+        <v>95487</v>
       </c>
       <c r="D24">
-        <v>120623251</v>
+        <v>125913996</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1413,10 +1413,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="D29">
-        <v>598184</v>
+        <v>625455</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -1439,10 +1439,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>39976</v>
+        <v>40778</v>
       </c>
       <c r="D30">
-        <v>67041497</v>
+        <v>72748095</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1465,10 +1465,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D31">
-        <v>86812</v>
+        <v>106812</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1517,10 +1517,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>14506</v>
+        <v>14814</v>
       </c>
       <c r="D33">
-        <v>24300618</v>
+        <v>26391462</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1595,10 +1595,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>1727</v>
+        <v>1748</v>
       </c>
       <c r="D36">
-        <v>2571436</v>
+        <v>2655361</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1647,10 +1647,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>2605</v>
+        <v>2625</v>
       </c>
       <c r="D38">
-        <v>4067659</v>
+        <v>4159120</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1673,10 +1673,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>115734</v>
+        <v>117767</v>
       </c>
       <c r="D39">
-        <v>149913504</v>
+        <v>156394411</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1699,10 +1699,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D40">
-        <v>81534</v>
+        <v>82981</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1725,10 +1725,10 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D41">
-        <v>143168</v>
+        <v>153834</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1829,10 +1829,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>1184</v>
+        <v>1206</v>
       </c>
       <c r="D45">
-        <v>1892932</v>
+        <v>2030510</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1881,10 +1881,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>54988</v>
+        <v>56231</v>
       </c>
       <c r="D47">
-        <v>91508101</v>
+        <v>100388271</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1907,10 +1907,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D48">
-        <v>98162</v>
+        <v>99662</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1933,10 +1933,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>11694</v>
+        <v>11959</v>
       </c>
       <c r="D49">
-        <v>19721606</v>
+        <v>21538578</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1985,10 +1985,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>1556</v>
+        <v>1564</v>
       </c>
       <c r="D51">
-        <v>2250887</v>
+        <v>2288387</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2011,10 +2011,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52">
-        <v>4500</v>
+        <v>8125</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2063,10 +2063,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>3307</v>
+        <v>3346</v>
       </c>
       <c r="D54">
-        <v>5076105</v>
+        <v>5259172</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2089,10 +2089,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>83507</v>
+        <v>85033</v>
       </c>
       <c r="D55">
-        <v>110041162</v>
+        <v>114868078</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -2245,10 +2245,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="D61">
-        <v>812485</v>
+        <v>875740</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2297,10 +2297,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>34983</v>
+        <v>35803</v>
       </c>
       <c r="D63">
-        <v>58934777</v>
+        <v>64874249</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2375,10 +2375,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>14164</v>
+        <v>14458</v>
       </c>
       <c r="D66">
-        <v>24026406</v>
+        <v>25985505</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -2427,10 +2427,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>1537</v>
+        <v>1550</v>
       </c>
       <c r="D68">
-        <v>2288972</v>
+        <v>2371074</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2531,10 +2531,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>2131</v>
+        <v>2154</v>
       </c>
       <c r="D72">
-        <v>3373991</v>
+        <v>3486270</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -2583,10 +2583,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>25196</v>
+        <v>25572</v>
       </c>
       <c r="D74">
-        <v>34738013</v>
+        <v>35891209</v>
       </c>
       <c r="E74" t="s">
         <v>14</v>
@@ -2609,10 +2609,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D75">
-        <v>51437</v>
+        <v>52256</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
@@ -2687,10 +2687,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>9714</v>
+        <v>9897</v>
       </c>
       <c r="D78">
-        <v>17473705</v>
+        <v>18819532</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -2713,10 +2713,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D79">
-        <v>6000</v>
+        <v>16000</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -2739,10 +2739,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>6613</v>
+        <v>6780</v>
       </c>
       <c r="D80">
-        <v>11632182</v>
+        <v>12709567</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -2765,10 +2765,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="D81">
-        <v>947907</v>
+        <v>961532</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -2791,10 +2791,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="D82">
-        <v>676843</v>
+        <v>719274</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2817,10 +2817,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>170697</v>
+        <v>173721</v>
       </c>
       <c r="D83">
-        <v>222495805</v>
+        <v>231486719</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -2843,10 +2843,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D84">
-        <v>188306</v>
+        <v>197081</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -2869,10 +2869,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D85">
-        <v>184762</v>
+        <v>197840</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -2895,10 +2895,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D86">
-        <v>36956</v>
+        <v>38806</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -2921,10 +2921,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>570</v>
+        <v>585</v>
       </c>
       <c r="D87">
-        <v>1007533</v>
+        <v>1129749</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -2947,10 +2947,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D88">
-        <v>19021</v>
+        <v>19104</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -2973,10 +2973,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>77851</v>
+        <v>79320</v>
       </c>
       <c r="D89">
-        <v>129458758</v>
+        <v>139968188</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -2999,10 +2999,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D90">
-        <v>309015</v>
+        <v>319015</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -3051,10 +3051,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>37038</v>
+        <v>37707</v>
       </c>
       <c r="D92">
-        <v>61498302</v>
+        <v>65986948</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3103,10 +3103,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>3600</v>
+        <v>3661</v>
       </c>
       <c r="D94">
-        <v>7890902</v>
+        <v>8337782</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3155,10 +3155,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>4007</v>
+        <v>4047</v>
       </c>
       <c r="D96">
-        <v>6300773</v>
+        <v>6501885</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -3181,10 +3181,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>41165</v>
+        <v>41510</v>
       </c>
       <c r="D97">
-        <v>57974001</v>
+        <v>58965133</v>
       </c>
       <c r="E97" t="s">
         <v>16</v>
@@ -3259,10 +3259,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D100">
-        <v>62960</v>
+        <v>67182</v>
       </c>
       <c r="E100" t="s">
         <v>16</v>
@@ -3285,10 +3285,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>10264</v>
+        <v>10339</v>
       </c>
       <c r="D101">
-        <v>16322616</v>
+        <v>16730430</v>
       </c>
       <c r="E101" t="s">
         <v>16</v>
@@ -3311,10 +3311,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D102">
-        <v>17500</v>
+        <v>19000</v>
       </c>
       <c r="E102" t="s">
         <v>16</v>
@@ -3337,10 +3337,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>9578</v>
+        <v>9644</v>
       </c>
       <c r="D103">
-        <v>14901166</v>
+        <v>15197282</v>
       </c>
       <c r="E103" t="s">
         <v>16</v>
@@ -3389,10 +3389,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D105">
-        <v>933972</v>
+        <v>934682</v>
       </c>
       <c r="E105" t="s">
         <v>16</v>
@@ -3415,10 +3415,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="D106">
-        <v>932480</v>
+        <v>982452</v>
       </c>
       <c r="E106" t="s">
         <v>16</v>
@@ -3441,10 +3441,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>17694</v>
+        <v>17775</v>
       </c>
       <c r="D107">
-        <v>35082069</v>
+        <v>35467766</v>
       </c>
       <c r="E107" t="s">
         <v>17</v>
@@ -3519,10 +3519,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>4052</v>
+        <v>4060</v>
       </c>
       <c r="D110">
-        <v>8634976</v>
+        <v>8688326</v>
       </c>
       <c r="E110" t="s">
         <v>17</v>
@@ -3571,10 +3571,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>5818</v>
+        <v>5841</v>
       </c>
       <c r="D112">
-        <v>12618498</v>
+        <v>12744979</v>
       </c>
       <c r="E112" t="s">
         <v>17</v>
@@ -3701,10 +3701,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>174087</v>
+        <v>177338</v>
       </c>
       <c r="D117">
-        <v>227314511</v>
+        <v>236925142</v>
       </c>
       <c r="E117" t="s">
         <v>18</v>
@@ -3727,10 +3727,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D118">
-        <v>46317</v>
+        <v>52233</v>
       </c>
       <c r="E118" t="s">
         <v>18</v>
@@ -3805,10 +3805,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>1272</v>
+        <v>1297</v>
       </c>
       <c r="D121">
-        <v>2322522</v>
+        <v>2515289</v>
       </c>
       <c r="E121" t="s">
         <v>18</v>
@@ -3857,10 +3857,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>66136</v>
+        <v>67458</v>
       </c>
       <c r="D123">
-        <v>114298555</v>
+        <v>123546423</v>
       </c>
       <c r="E123" t="s">
         <v>18</v>
@@ -3883,10 +3883,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D124">
-        <v>312379</v>
+        <v>342379</v>
       </c>
       <c r="E124" t="s">
         <v>18</v>
@@ -3935,10 +3935,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>35764</v>
+        <v>36543</v>
       </c>
       <c r="D126">
-        <v>61785084</v>
+        <v>67171728</v>
       </c>
       <c r="E126" t="s">
         <v>18</v>
@@ -3961,10 +3961,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>1480</v>
+        <v>1496</v>
       </c>
       <c r="D127">
-        <v>2280577</v>
+        <v>2359029</v>
       </c>
       <c r="E127" t="s">
         <v>18</v>
@@ -4013,10 +4013,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D129">
-        <v>17500</v>
+        <v>27500</v>
       </c>
       <c r="E129" t="s">
         <v>18</v>
@@ -4065,10 +4065,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>3326</v>
+        <v>3372</v>
       </c>
       <c r="D131">
-        <v>5386501</v>
+        <v>5608572</v>
       </c>
       <c r="E131" t="s">
         <v>18</v>
@@ -4091,10 +4091,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D132">
-        <v>23269</v>
+        <v>25695</v>
       </c>
       <c r="E132" t="s">
         <v>18</v>
@@ -4117,10 +4117,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>713997</v>
+        <v>725898</v>
       </c>
       <c r="D133">
-        <v>1042316616</v>
+        <v>1084747691</v>
       </c>
       <c r="E133" t="s">
         <v>19</v>
@@ -4169,10 +4169,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D135">
-        <v>561741</v>
+        <v>586542</v>
       </c>
       <c r="E135" t="s">
         <v>19</v>
@@ -4247,10 +4247,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>2114</v>
+        <v>2149</v>
       </c>
       <c r="D138">
-        <v>4806194</v>
+        <v>5094614</v>
       </c>
       <c r="E138" t="s">
         <v>19</v>
@@ -4273,10 +4273,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D139">
-        <v>126681</v>
+        <v>156681</v>
       </c>
       <c r="E139" t="s">
         <v>19</v>
@@ -4299,10 +4299,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>276960</v>
+        <v>281725</v>
       </c>
       <c r="D140">
-        <v>502758280</v>
+        <v>536835956</v>
       </c>
       <c r="E140" t="s">
         <v>19</v>
@@ -4325,10 +4325,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>763</v>
+        <v>781</v>
       </c>
       <c r="D141">
-        <v>2242702</v>
+        <v>2405527</v>
       </c>
       <c r="E141" t="s">
         <v>19</v>
@@ -4351,10 +4351,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D142">
-        <v>169474</v>
+        <v>180140</v>
       </c>
       <c r="E142" t="s">
         <v>19</v>
@@ -4377,10 +4377,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>261934</v>
+        <v>266629</v>
       </c>
       <c r="D143">
-        <v>474559760</v>
+        <v>503860762</v>
       </c>
       <c r="E143" t="s">
         <v>19</v>
@@ -4403,10 +4403,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D144">
-        <v>17823</v>
+        <v>27823</v>
       </c>
       <c r="E144" t="s">
         <v>19</v>
@@ -4429,10 +4429,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D145">
-        <v>105878</v>
+        <v>129620</v>
       </c>
       <c r="E145" t="s">
         <v>19</v>
@@ -4455,10 +4455,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>3328</v>
+        <v>3347</v>
       </c>
       <c r="D146">
-        <v>5106471</v>
+        <v>5192473</v>
       </c>
       <c r="E146" t="s">
         <v>19</v>
@@ -4533,10 +4533,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>10103</v>
+        <v>10217</v>
       </c>
       <c r="D149">
-        <v>16819856</v>
+        <v>17477392</v>
       </c>
       <c r="E149" t="s">
         <v>19</v>
@@ -4611,10 +4611,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>52519</v>
+        <v>52757</v>
       </c>
       <c r="D152">
-        <v>71433726</v>
+        <v>72119232</v>
       </c>
       <c r="E152" t="s">
         <v>20</v>
@@ -4663,10 +4663,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D154">
-        <v>61551</v>
+        <v>62619</v>
       </c>
       <c r="E154" t="s">
         <v>20</v>
@@ -4767,10 +4767,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>16024</v>
+        <v>16060</v>
       </c>
       <c r="D158">
-        <v>24598406</v>
+        <v>24793760</v>
       </c>
       <c r="E158" t="s">
         <v>20</v>
@@ -4793,10 +4793,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D159">
-        <v>31823</v>
+        <v>41823</v>
       </c>
       <c r="E159" t="s">
         <v>20</v>
@@ -4819,10 +4819,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>4400</v>
+        <v>4416</v>
       </c>
       <c r="D160">
-        <v>6610560</v>
+        <v>6693402</v>
       </c>
       <c r="E160" t="s">
         <v>20</v>
@@ -4897,10 +4897,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D163">
-        <v>638927</v>
+        <v>643507</v>
       </c>
       <c r="E163" t="s">
         <v>20</v>
@@ -4949,10 +4949,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="D165">
-        <v>834280</v>
+        <v>840680</v>
       </c>
       <c r="E165" t="s">
         <v>20</v>
@@ -4975,10 +4975,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>21738</v>
+        <v>22179</v>
       </c>
       <c r="D166">
-        <v>29655261</v>
+        <v>31191988</v>
       </c>
       <c r="E166" t="s">
         <v>21</v>
@@ -5079,10 +5079,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>9146</v>
+        <v>9324</v>
       </c>
       <c r="D170">
-        <v>14705497</v>
+        <v>15847758</v>
       </c>
       <c r="E170" t="s">
         <v>21</v>
@@ -5131,10 +5131,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>6571</v>
+        <v>6671</v>
       </c>
       <c r="D172">
-        <v>10568333</v>
+        <v>11181777</v>
       </c>
       <c r="E172" t="s">
         <v>21</v>
@@ -5157,10 +5157,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D173">
-        <v>5310</v>
+        <v>15310</v>
       </c>
       <c r="E173" t="s">
         <v>21</v>
@@ -5183,10 +5183,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D174">
-        <v>469446</v>
+        <v>471434</v>
       </c>
       <c r="E174" t="s">
         <v>21</v>
@@ -5209,10 +5209,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="D175">
-        <v>620690</v>
+        <v>638175</v>
       </c>
       <c r="E175" t="s">
         <v>21</v>
@@ -5261,10 +5261,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>31047</v>
+        <v>31246</v>
       </c>
       <c r="D177">
-        <v>68261921</v>
+        <v>69637134</v>
       </c>
       <c r="E177" t="s">
         <v>22</v>
@@ -5313,10 +5313,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>3108</v>
+        <v>3124</v>
       </c>
       <c r="D179">
-        <v>6825281</v>
+        <v>6944881</v>
       </c>
       <c r="E179" t="s">
         <v>22</v>
@@ -5339,10 +5339,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="D180">
-        <v>880679</v>
+        <v>910679</v>
       </c>
       <c r="E180" t="s">
         <v>22</v>
@@ -5417,10 +5417,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D183">
-        <v>431087</v>
+        <v>441087</v>
       </c>
       <c r="E183" t="s">
         <v>22</v>
@@ -5443,10 +5443,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>106299</v>
+        <v>108412</v>
       </c>
       <c r="D184">
-        <v>138482615</v>
+        <v>145380630</v>
       </c>
       <c r="E184" t="s">
         <v>23</v>
@@ -5495,10 +5495,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D186">
-        <v>154769</v>
+        <v>160610</v>
       </c>
       <c r="E186" t="s">
         <v>23</v>
@@ -5573,10 +5573,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>827</v>
+        <v>857</v>
       </c>
       <c r="D189">
-        <v>1377763</v>
+        <v>1593987</v>
       </c>
       <c r="E189" t="s">
         <v>23</v>
@@ -5625,10 +5625,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>42549</v>
+        <v>43487</v>
       </c>
       <c r="D191">
-        <v>73353981</v>
+        <v>80179336</v>
       </c>
       <c r="E191" t="s">
         <v>23</v>
@@ -5651,10 +5651,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D192">
-        <v>82299</v>
+        <v>92299</v>
       </c>
       <c r="E192" t="s">
         <v>23</v>
@@ -5677,10 +5677,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>17018</v>
+        <v>17375</v>
       </c>
       <c r="D193">
-        <v>29598852</v>
+        <v>32009244</v>
       </c>
       <c r="E193" t="s">
         <v>23</v>
@@ -5729,10 +5729,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>1393</v>
+        <v>1404</v>
       </c>
       <c r="D195">
-        <v>2040346</v>
+        <v>2070988</v>
       </c>
       <c r="E195" t="s">
         <v>23</v>
@@ -5781,10 +5781,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>2348</v>
+        <v>2373</v>
       </c>
       <c r="D197">
-        <v>3679049</v>
+        <v>3801888</v>
       </c>
       <c r="E197" t="s">
         <v>23</v>
@@ -5833,10 +5833,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>285470</v>
+        <v>290407</v>
       </c>
       <c r="D199">
-        <v>369990934</v>
+        <v>384491088</v>
       </c>
       <c r="E199" t="s">
         <v>24</v>
@@ -5885,10 +5885,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D201">
-        <v>328102</v>
+        <v>337562</v>
       </c>
       <c r="E201" t="s">
         <v>24</v>
@@ -5989,10 +5989,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>1123</v>
+        <v>1152</v>
       </c>
       <c r="D205">
-        <v>1859781</v>
+        <v>2033117</v>
       </c>
       <c r="E205" t="s">
         <v>24</v>
@@ -6041,10 +6041,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>106391</v>
+        <v>108622</v>
       </c>
       <c r="D207">
-        <v>178690743</v>
+        <v>194289839</v>
       </c>
       <c r="E207" t="s">
         <v>24</v>
@@ -6067,10 +6067,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D208">
-        <v>272112</v>
+        <v>292112</v>
       </c>
       <c r="E208" t="s">
         <v>24</v>
@@ -6119,10 +6119,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>41947</v>
+        <v>42799</v>
       </c>
       <c r="D210">
-        <v>70569708</v>
+        <v>76174365</v>
       </c>
       <c r="E210" t="s">
         <v>24</v>
@@ -6197,10 +6197,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>5843</v>
+        <v>5888</v>
       </c>
       <c r="D213">
-        <v>9005811</v>
+        <v>9271944</v>
       </c>
       <c r="E213" t="s">
         <v>24</v>
@@ -6275,10 +6275,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>6936</v>
+        <v>7015</v>
       </c>
       <c r="D216">
-        <v>10540964</v>
+        <v>10965617</v>
       </c>
       <c r="E216" t="s">
         <v>24</v>
@@ -6353,10 +6353,10 @@
         <v>9</v>
       </c>
       <c r="C219">
-        <v>322909</v>
+        <v>328218</v>
       </c>
       <c r="D219">
-        <v>417788216</v>
+        <v>432384436</v>
       </c>
       <c r="E219" t="s">
         <v>25</v>
@@ -6379,10 +6379,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D220">
-        <v>228573</v>
+        <v>234375</v>
       </c>
       <c r="E220" t="s">
         <v>25</v>
@@ -6405,10 +6405,10 @@
         <v>9</v>
       </c>
       <c r="C221">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D221">
-        <v>460506</v>
+        <v>475946</v>
       </c>
       <c r="E221" t="s">
         <v>25</v>
@@ -6535,10 +6535,10 @@
         <v>9</v>
       </c>
       <c r="C226">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="D226">
-        <v>1384016</v>
+        <v>1513638</v>
       </c>
       <c r="E226" t="s">
         <v>25</v>
@@ -6587,10 +6587,10 @@
         <v>9</v>
       </c>
       <c r="C228">
-        <v>119086</v>
+        <v>121202</v>
       </c>
       <c r="D228">
-        <v>206489900</v>
+        <v>221354347</v>
       </c>
       <c r="E228" t="s">
         <v>25</v>
@@ -6613,10 +6613,10 @@
         <v>9</v>
       </c>
       <c r="C229">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D229">
-        <v>298947</v>
+        <v>328947</v>
       </c>
       <c r="E229" t="s">
         <v>25</v>
@@ -6665,10 +6665,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>66199</v>
+        <v>67401</v>
       </c>
       <c r="D231">
-        <v>114708466</v>
+        <v>122717941</v>
       </c>
       <c r="E231" t="s">
         <v>25</v>
@@ -6743,10 +6743,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>5288</v>
+        <v>5325</v>
       </c>
       <c r="D234">
-        <v>7886360</v>
+        <v>8037821</v>
       </c>
       <c r="E234" t="s">
         <v>25</v>
@@ -6769,10 +6769,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D235">
-        <v>18327</v>
+        <v>19422</v>
       </c>
       <c r="E235" t="s">
         <v>25</v>
@@ -6795,10 +6795,10 @@
         <v>9</v>
       </c>
       <c r="C236">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D236">
-        <v>13000</v>
+        <v>14078</v>
       </c>
       <c r="E236" t="s">
         <v>25</v>
@@ -6847,10 +6847,10 @@
         <v>9</v>
       </c>
       <c r="C238">
-        <v>8808</v>
+        <v>8896</v>
       </c>
       <c r="D238">
-        <v>13862763</v>
+        <v>14294550</v>
       </c>
       <c r="E238" t="s">
         <v>25</v>
@@ -6925,10 +6925,10 @@
         <v>9</v>
       </c>
       <c r="C241">
-        <v>128365</v>
+        <v>130597</v>
       </c>
       <c r="D241">
-        <v>167334326</v>
+        <v>174416879</v>
       </c>
       <c r="E241" t="s">
         <v>26</v>
@@ -6977,10 +6977,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D243">
-        <v>148966</v>
+        <v>184307</v>
       </c>
       <c r="E243" t="s">
         <v>26</v>
@@ -7003,10 +7003,10 @@
         <v>9</v>
       </c>
       <c r="C244">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D244">
-        <v>17147</v>
+        <v>22128</v>
       </c>
       <c r="E244" t="s">
         <v>26</v>
@@ -7055,10 +7055,10 @@
         <v>9</v>
       </c>
       <c r="C246">
-        <v>737</v>
+        <v>753</v>
       </c>
       <c r="D246">
-        <v>1226584</v>
+        <v>1338222</v>
       </c>
       <c r="E246" t="s">
         <v>26</v>
@@ -7107,10 +7107,10 @@
         <v>9</v>
       </c>
       <c r="C248">
-        <v>61223</v>
+        <v>62551</v>
       </c>
       <c r="D248">
-        <v>102320529</v>
+        <v>112357328</v>
       </c>
       <c r="E248" t="s">
         <v>26</v>
@@ -7133,10 +7133,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D249">
-        <v>76377</v>
+        <v>86377</v>
       </c>
       <c r="E249" t="s">
         <v>26</v>
@@ -7159,10 +7159,10 @@
         <v>9</v>
       </c>
       <c r="C250">
-        <v>16148</v>
+        <v>16529</v>
       </c>
       <c r="D250">
-        <v>27172767</v>
+        <v>29540884</v>
       </c>
       <c r="E250" t="s">
         <v>26</v>
@@ -7211,10 +7211,10 @@
         <v>9</v>
       </c>
       <c r="C252">
-        <v>2070</v>
+        <v>2086</v>
       </c>
       <c r="D252">
-        <v>3141523</v>
+        <v>3196363</v>
       </c>
       <c r="E252" t="s">
         <v>26</v>
@@ -7263,10 +7263,10 @@
         <v>9</v>
       </c>
       <c r="C254">
-        <v>3487</v>
+        <v>3517</v>
       </c>
       <c r="D254">
-        <v>5344351</v>
+        <v>5505520</v>
       </c>
       <c r="E254" t="s">
         <v>26</v>
@@ -7289,10 +7289,10 @@
         <v>9</v>
       </c>
       <c r="C255">
-        <v>322421</v>
+        <v>328162</v>
       </c>
       <c r="D255">
-        <v>431131122</v>
+        <v>447109432</v>
       </c>
       <c r="E255" t="s">
         <v>27</v>
@@ -7315,10 +7315,10 @@
         <v>9</v>
       </c>
       <c r="C256">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D256">
-        <v>288811</v>
+        <v>311290</v>
       </c>
       <c r="E256" t="s">
         <v>27</v>
@@ -7341,10 +7341,10 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D257">
-        <v>488805</v>
+        <v>523747</v>
       </c>
       <c r="E257" t="s">
         <v>27</v>
@@ -7445,10 +7445,10 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D261">
-        <v>23480</v>
+        <v>24980</v>
       </c>
       <c r="E261" t="s">
         <v>27</v>
@@ -7471,10 +7471,10 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <v>1200</v>
+        <v>1242</v>
       </c>
       <c r="D262">
-        <v>2425423</v>
+        <v>2758276</v>
       </c>
       <c r="E262" t="s">
         <v>27</v>
@@ -7523,10 +7523,10 @@
         <v>9</v>
       </c>
       <c r="C264">
-        <v>123652</v>
+        <v>126031</v>
       </c>
       <c r="D264">
-        <v>223993880</v>
+        <v>240500456</v>
       </c>
       <c r="E264" t="s">
         <v>27</v>
@@ -7549,10 +7549,10 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D265">
-        <v>351986</v>
+        <v>371986</v>
       </c>
       <c r="E265" t="s">
         <v>27</v>
@@ -7601,10 +7601,10 @@
         <v>9</v>
       </c>
       <c r="C267">
-        <v>88093</v>
+        <v>89810</v>
       </c>
       <c r="D267">
-        <v>159482571</v>
+        <v>170623232</v>
       </c>
       <c r="E267" t="s">
         <v>27</v>
@@ -7653,10 +7653,10 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <v>2815</v>
+        <v>2835</v>
       </c>
       <c r="D269">
-        <v>4291185</v>
+        <v>4398764</v>
       </c>
       <c r="E269" t="s">
         <v>27</v>
@@ -7679,10 +7679,10 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D270">
-        <v>21240</v>
+        <v>31240</v>
       </c>
       <c r="E270" t="s">
         <v>27</v>
@@ -7731,10 +7731,10 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <v>7136</v>
+        <v>7248</v>
       </c>
       <c r="D272">
-        <v>11595647</v>
+        <v>12078393</v>
       </c>
       <c r="E272" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-09 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>417440</v>
+        <v>422296</v>
       </c>
       <c r="D2" t="n">
-        <v>593871671</v>
+        <v>609351049</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D3" t="n">
-        <v>435130</v>
+        <v>454588</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D4" t="n">
-        <v>853162</v>
+        <v>867191</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>34500</v>
+        <v>44500</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1251</v>
+        <v>1280</v>
       </c>
       <c r="D9" t="n">
-        <v>2711516</v>
+        <v>2874303</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>158889</v>
+        <v>162330</v>
       </c>
       <c r="D11" t="n">
-        <v>339664915</v>
+        <v>362622615</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="D12" t="n">
-        <v>708535</v>
+        <v>839201</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>83223</v>
+        <v>84917</v>
       </c>
       <c r="D13" t="n">
-        <v>172829135</v>
+        <v>183160739</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D15" t="n">
-        <v>115856</v>
+        <v>128799</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4496</v>
+        <v>4540</v>
       </c>
       <c r="D17" t="n">
-        <v>7037200</v>
+        <v>7194334</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>10561</v>
+        <v>10701</v>
       </c>
       <c r="D22" t="n">
-        <v>18702426</v>
+        <v>19340775</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D23" t="n">
-        <v>17706</v>
+        <v>27912</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>99543</v>
+        <v>100774</v>
       </c>
       <c r="D24" t="n">
-        <v>138633550</v>
+        <v>142699084</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" t="n">
-        <v>100904</v>
+        <v>108572</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D27" t="n">
-        <v>16527</v>
+        <v>22205</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>44000</v>
+        <v>64000</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="D29" t="n">
-        <v>835410</v>
+        <v>930747</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>43294</v>
+        <v>44275</v>
       </c>
       <c r="D30" t="n">
-        <v>89679660</v>
+        <v>96227521</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D31" t="n">
-        <v>136920</v>
+        <v>149053</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>38166</v>
+        <v>48166</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>15641</v>
+        <v>15935</v>
       </c>
       <c r="D33" t="n">
-        <v>31655384</v>
+        <v>33538235</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1793</v>
+        <v>1811</v>
       </c>
       <c r="D36" t="n">
-        <v>2871455</v>
+        <v>2958160</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D37" t="n">
-        <v>33426</v>
+        <v>43168</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2726</v>
+        <v>2763</v>
       </c>
       <c r="D38" t="n">
-        <v>4585792</v>
+        <v>4748430</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>122910</v>
+        <v>124634</v>
       </c>
       <c r="D39" t="n">
-        <v>173380493</v>
+        <v>179386458</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D41" t="n">
-        <v>216482</v>
+        <v>262024</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1343</v>
+        <v>1410</v>
       </c>
       <c r="D45" t="n">
-        <v>2954392</v>
+        <v>3401875</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>60520</v>
+        <v>62301</v>
       </c>
       <c r="D47" t="n">
-        <v>129768013</v>
+        <v>141710877</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D48" t="n">
-        <v>110328</v>
+        <v>120994</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>12767</v>
+        <v>13078</v>
       </c>
       <c r="D49" t="n">
-        <v>26611555</v>
+        <v>28533910</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1602</v>
+        <v>1616</v>
       </c>
       <c r="D51" t="n">
-        <v>2434825</v>
+        <v>2516629</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3476</v>
+        <v>3531</v>
       </c>
       <c r="D54" t="n">
-        <v>5931805</v>
+        <v>6245889</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>88595</v>
+        <v>89686</v>
       </c>
       <c r="D55" t="n">
-        <v>126164117</v>
+        <v>129754347</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D57" t="n">
-        <v>110530</v>
+        <v>117695</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>535</v>
+        <v>559</v>
       </c>
       <c r="D61" t="n">
-        <v>1159335</v>
+        <v>1318149</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>37861</v>
+        <v>38605</v>
       </c>
       <c r="D63" t="n">
-        <v>78626105</v>
+        <v>83540236</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D64" t="n">
-        <v>177114</v>
+        <v>198614</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D65" t="n">
-        <v>18166</v>
+        <v>18832</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>15207</v>
+        <v>15439</v>
       </c>
       <c r="D66" t="n">
-        <v>30655509</v>
+        <v>32026805</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1590</v>
+        <v>1600</v>
       </c>
       <c r="D68" t="n">
-        <v>2550702</v>
+        <v>2603575</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2239</v>
+        <v>2272</v>
       </c>
       <c r="D72" t="n">
-        <v>3854887</v>
+        <v>4016021</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>26403</v>
+        <v>26681</v>
       </c>
       <c r="D74" t="n">
-        <v>38506590</v>
+        <v>39561216</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D76" t="n">
-        <v>62710</v>
+        <v>65529</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>10471</v>
+        <v>10722</v>
       </c>
       <c r="D78" t="n">
-        <v>22936287</v>
+        <v>24750590</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D79" t="n">
-        <v>22860</v>
+        <v>29720</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>7200</v>
+        <v>7341</v>
       </c>
       <c r="D80" t="n">
-        <v>15224388</v>
+        <v>16012947</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="D81" t="n">
-        <v>1021569</v>
+        <v>1069270</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="D82" t="n">
-        <v>786792</v>
+        <v>795332</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>180893</v>
+        <v>183286</v>
       </c>
       <c r="D83" t="n">
-        <v>254195161</v>
+        <v>262027892</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D84" t="n">
-        <v>211074</v>
+        <v>224022</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D85" t="n">
-        <v>239115</v>
+        <v>277808</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>637</v>
+        <v>659</v>
       </c>
       <c r="D87" t="n">
-        <v>1449688</v>
+        <v>1550190</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D88" t="n">
-        <v>30687</v>
+        <v>32187</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>84405</v>
+        <v>86477</v>
       </c>
       <c r="D89" t="n">
-        <v>173584655</v>
+        <v>186876957</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D90" t="n">
-        <v>414805</v>
+        <v>429596</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D91" t="n">
-        <v>50586</v>
+        <v>60586</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>39940</v>
+        <v>40812</v>
       </c>
       <c r="D92" t="n">
-        <v>79970124</v>
+        <v>85327618</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D93" t="n">
-        <v>28603</v>
+        <v>29962</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4019</v>
+        <v>4209</v>
       </c>
       <c r="D94" t="n">
-        <v>10695321</v>
+        <v>11975261</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4191</v>
+        <v>4243</v>
       </c>
       <c r="D96" t="n">
-        <v>7181482</v>
+        <v>7435939</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>42432</v>
+        <v>42744</v>
       </c>
       <c r="D97" t="n">
-        <v>61052014</v>
+        <v>61688212</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>10494</v>
+        <v>10550</v>
       </c>
       <c r="D101" t="n">
-        <v>17460141</v>
+        <v>17712180</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>9780</v>
+        <v>9829</v>
       </c>
       <c r="D103" t="n">
-        <v>15664549</v>
+        <v>15826202</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="D105" t="n">
-        <v>955712</v>
+        <v>960752</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="D106" t="n">
-        <v>1018270</v>
+        <v>1044094</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>17974</v>
+        <v>18031</v>
       </c>
       <c r="D107" t="n">
-        <v>36307350</v>
+        <v>36542404</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4086</v>
+        <v>4094</v>
       </c>
       <c r="D110" t="n">
-        <v>8767747</v>
+        <v>8788247</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5888</v>
+        <v>5910</v>
       </c>
       <c r="D112" t="n">
-        <v>13042093</v>
+        <v>13181374</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D115" t="n">
-        <v>737625</v>
+        <v>747625</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>184365</v>
+        <v>186635</v>
       </c>
       <c r="D117" t="n">
-        <v>258123588</v>
+        <v>265370732</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D119" t="n">
-        <v>161662</v>
+        <v>173162</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1399</v>
+        <v>1438</v>
       </c>
       <c r="D121" t="n">
-        <v>3175351</v>
+        <v>3415893</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>71399</v>
+        <v>72937</v>
       </c>
       <c r="D123" t="n">
-        <v>150011856</v>
+        <v>160076755</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D124" t="n">
-        <v>478734</v>
+        <v>538124</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>38333</v>
+        <v>39016</v>
       </c>
       <c r="D126" t="n">
-        <v>78216349</v>
+        <v>82348800</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D127" t="n">
-        <v>6926</v>
+        <v>10852</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1540</v>
+        <v>1556</v>
       </c>
       <c r="D128" t="n">
-        <v>2615173</v>
+        <v>2717252</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>3532</v>
+        <v>3594</v>
       </c>
       <c r="D132" t="n">
-        <v>6338156</v>
+        <v>6604717</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>751121</v>
+        <v>758347</v>
       </c>
       <c r="D134" t="n">
-        <v>1161360696</v>
+        <v>1182731541</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D135" t="n">
-        <v>230222</v>
+        <v>257054</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D136" t="n">
-        <v>678922</v>
+        <v>718907</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D138" t="n">
-        <v>51777</v>
+        <v>52390</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2328</v>
+        <v>2410</v>
       </c>
       <c r="D139" t="n">
-        <v>6420761</v>
+        <v>6997806</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D140" t="n">
-        <v>208679</v>
+        <v>218679</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>295584</v>
+        <v>300880</v>
       </c>
       <c r="D141" t="n">
-        <v>627923523</v>
+        <v>662697306</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>880</v>
+        <v>918</v>
       </c>
       <c r="D142" t="n">
-        <v>3215252</v>
+        <v>3494238</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D143" t="n">
-        <v>227961</v>
+        <v>246944</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>278026</v>
+        <v>282095</v>
       </c>
       <c r="D144" t="n">
-        <v>571249835</v>
+        <v>595364789</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D146" t="n">
-        <v>166714</v>
+        <v>168777</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>3420</v>
+        <v>3443</v>
       </c>
       <c r="D147" t="n">
-        <v>5497910</v>
+        <v>5586131</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>10678</v>
+        <v>10847</v>
       </c>
       <c r="D150" t="n">
-        <v>19654459</v>
+        <v>20519430</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D151" t="n">
-        <v>16000</v>
+        <v>26000</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>53337</v>
+        <v>53505</v>
       </c>
       <c r="D153" t="n">
-        <v>73353609</v>
+        <v>73682133</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>16200</v>
+        <v>16252</v>
       </c>
       <c r="D159" t="n">
-        <v>25492397</v>
+        <v>25727579</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D160" t="n">
-        <v>51823</v>
+        <v>61823</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4457</v>
+        <v>4471</v>
       </c>
       <c r="D161" t="n">
-        <v>6854690</v>
+        <v>6912249</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6576,10 +6576,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D164" t="n">
-        <v>654468</v>
+        <v>657468</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D166" t="n">
-        <v>851181</v>
+        <v>854664</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>22968</v>
+        <v>23231</v>
       </c>
       <c r="D167" t="n">
-        <v>33412839</v>
+        <v>34136920</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D170" t="n">
-        <v>91124</v>
+        <v>99842</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>9695</v>
+        <v>9830</v>
       </c>
       <c r="D171" t="n">
-        <v>18020820</v>
+        <v>18804055</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6918,10 +6918,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>6897</v>
+        <v>6975</v>
       </c>
       <c r="D173" t="n">
-        <v>12300989</v>
+        <v>12731635</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D175" t="n">
-        <v>481509</v>
+        <v>486517</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D176" t="n">
-        <v>691978</v>
+        <v>707478</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>31853</v>
+        <v>32005</v>
       </c>
       <c r="D178" t="n">
-        <v>73645099</v>
+        <v>74550325</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>3169</v>
+        <v>3185</v>
       </c>
       <c r="D180" t="n">
-        <v>7232063</v>
+        <v>7341293</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D181" t="n">
-        <v>948179</v>
+        <v>949679</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D184" t="n">
-        <v>458264</v>
+        <v>461255</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>113185</v>
+        <v>114613</v>
       </c>
       <c r="D185" t="n">
-        <v>160881505</v>
+        <v>165755099</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D189" t="n">
-        <v>27389</v>
+        <v>28889</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7564,10 +7564,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D190" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -7602,10 +7602,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>958</v>
+        <v>1018</v>
       </c>
       <c r="D191" t="n">
-        <v>2262799</v>
+        <v>2679301</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>46357</v>
+        <v>47405</v>
       </c>
       <c r="D193" t="n">
-        <v>99770886</v>
+        <v>107021919</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7716,10 +7716,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D194" t="n">
-        <v>124187</v>
+        <v>144575</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>18318</v>
+        <v>18666</v>
       </c>
       <c r="D195" t="n">
-        <v>38105505</v>
+        <v>40415595</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D196" t="n">
-        <v>18514</v>
+        <v>21706</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1444</v>
+        <v>1456</v>
       </c>
       <c r="D197" t="n">
-        <v>2255343</v>
+        <v>2311537</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>2483</v>
+        <v>2524</v>
       </c>
       <c r="D199" t="n">
-        <v>4328693</v>
+        <v>4515004</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>301735</v>
+        <v>305181</v>
       </c>
       <c r="D201" t="n">
-        <v>417387353</v>
+        <v>427928432</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D202" t="n">
-        <v>211833</v>
+        <v>232449</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D203" t="n">
-        <v>407167</v>
+        <v>427089</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D204" t="n">
-        <v>11413</v>
+        <v>12913</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>1237</v>
+        <v>1275</v>
       </c>
       <c r="D207" t="n">
-        <v>2535367</v>
+        <v>2756717</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>115293</v>
+        <v>117983</v>
       </c>
       <c r="D209" t="n">
-        <v>238352049</v>
+        <v>256066589</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="D210" t="n">
-        <v>386284</v>
+        <v>431684</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>45280</v>
+        <v>46214</v>
       </c>
       <c r="D212" t="n">
-        <v>91363833</v>
+        <v>97067371</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8514,10 +8514,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>6041</v>
+        <v>6107</v>
       </c>
       <c r="D215" t="n">
-        <v>10061493</v>
+        <v>10416067</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>7343</v>
+        <v>7457</v>
       </c>
       <c r="D218" t="n">
-        <v>12310666</v>
+        <v>12774223</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>340801</v>
+        <v>344631</v>
       </c>
       <c r="D221" t="n">
-        <v>465963478</v>
+        <v>476755916</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8818,10 +8818,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D223" t="n">
-        <v>566267</v>
+        <v>595916</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>872</v>
+        <v>904</v>
       </c>
       <c r="D228" t="n">
-        <v>1936048</v>
+        <v>2169177</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>127823</v>
+        <v>130444</v>
       </c>
       <c r="D230" t="n">
-        <v>264959341</v>
+        <v>281711108</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D231" t="n">
-        <v>459220</v>
+        <v>520665</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>70922</v>
+        <v>72351</v>
       </c>
       <c r="D233" t="n">
-        <v>143907708</v>
+        <v>152371501</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9236,10 +9236,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D234" t="n">
-        <v>121484</v>
+        <v>131484</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>5460</v>
+        <v>5511</v>
       </c>
       <c r="D236" t="n">
-        <v>8521106</v>
+        <v>8757686</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D239" t="n">
-        <v>75978</v>
+        <v>85978</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>9274</v>
+        <v>9422</v>
       </c>
       <c r="D240" t="n">
-        <v>15828029</v>
+        <v>16430553</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>136020</v>
+        <v>137607</v>
       </c>
       <c r="D243" t="n">
-        <v>192240349</v>
+        <v>197812984</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9730,10 +9730,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D247" t="n">
-        <v>9980</v>
+        <v>16305</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>822</v>
+        <v>852</v>
       </c>
       <c r="D248" t="n">
-        <v>1782296</v>
+        <v>1982975</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>66763</v>
+        <v>68413</v>
       </c>
       <c r="D250" t="n">
-        <v>140927411</v>
+        <v>151595197</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9882,10 +9882,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D251" t="n">
-        <v>126377</v>
+        <v>146377</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D252" t="n">
-        <v>21332</v>
+        <v>41332</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>17519</v>
+        <v>17909</v>
       </c>
       <c r="D253" t="n">
-        <v>35740006</v>
+        <v>38227021</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10034,10 +10034,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2145</v>
+        <v>2168</v>
       </c>
       <c r="D255" t="n">
-        <v>3446064</v>
+        <v>3547152</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>3654</v>
+        <v>3698</v>
       </c>
       <c r="D257" t="n">
-        <v>6132614</v>
+        <v>6341353</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>340796</v>
+        <v>344613</v>
       </c>
       <c r="D258" t="n">
-        <v>481219475</v>
+        <v>491970595</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D259" t="n">
-        <v>342097</v>
+        <v>347631</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10224,10 +10224,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="D260" t="n">
-        <v>587938</v>
+        <v>625701</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>1346</v>
+        <v>1394</v>
       </c>
       <c r="D265" t="n">
-        <v>3444391</v>
+        <v>3760096</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D266" t="n">
-        <v>54498</v>
+        <v>74498</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10490,10 +10490,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>133138</v>
+        <v>135959</v>
       </c>
       <c r="D267" t="n">
-        <v>287288058</v>
+        <v>305736439</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D268" t="n">
-        <v>492156</v>
+        <v>543656</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -10566,10 +10566,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D269" t="n">
-        <v>58339</v>
+        <v>68339</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -10604,10 +10604,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>94513</v>
+        <v>96298</v>
       </c>
       <c r="D270" t="n">
-        <v>199209080</v>
+        <v>210063960</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -10680,10 +10680,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>2925</v>
+        <v>2965</v>
       </c>
       <c r="D272" t="n">
-        <v>4726493</v>
+        <v>4903996</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -10794,10 +10794,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>7579</v>
+        <v>7716</v>
       </c>
       <c r="D275" t="n">
-        <v>13651618</v>
+        <v>14285809</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-27 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>455202</v>
+        <v>456350</v>
       </c>
       <c r="D2" t="n">
-        <v>675449789</v>
+        <v>677856754</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1503</v>
+        <v>1508</v>
       </c>
       <c r="D9" t="n">
-        <v>4125259</v>
+        <v>4141244</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>177155</v>
+        <v>177423</v>
       </c>
       <c r="D11" t="n">
-        <v>434785834</v>
+        <v>436090543</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>92099</v>
+        <v>92265</v>
       </c>
       <c r="D14" t="n">
-        <v>215916327</v>
+        <v>216652328</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4948</v>
+        <v>4957</v>
       </c>
       <c r="D18" t="n">
-        <v>8426754</v>
+        <v>8446401</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D21" t="n">
-        <v>220464</v>
+        <v>223464</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11803</v>
+        <v>11846</v>
       </c>
       <c r="D23" t="n">
-        <v>24238405</v>
+        <v>24379328</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>108470</v>
+        <v>108660</v>
       </c>
       <c r="D25" t="n">
-        <v>158237629</v>
+        <v>158592060</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>47911</v>
+        <v>47972</v>
       </c>
       <c r="D31" t="n">
-        <v>114239377</v>
+        <v>114528453</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17402</v>
+        <v>17421</v>
       </c>
       <c r="D34" t="n">
-        <v>40148972</v>
+        <v>40227622</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="D37" t="n">
-        <v>3529329</v>
+        <v>3540829</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3031</v>
+        <v>3038</v>
       </c>
       <c r="D39" t="n">
-        <v>5928859</v>
+        <v>5940586</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>133654</v>
+        <v>133837</v>
       </c>
       <c r="D40" t="n">
-        <v>198494498</v>
+        <v>198856387</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>67172</v>
+        <v>67221</v>
       </c>
       <c r="D48" t="n">
-        <v>165535217</v>
+        <v>165768659</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>14253</v>
+        <v>14277</v>
       </c>
       <c r="D51" t="n">
-        <v>34013117</v>
+        <v>34107664</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1726</v>
+        <v>1730</v>
       </c>
       <c r="D53" t="n">
-        <v>2829897</v>
+        <v>2844397</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3817</v>
+        <v>3822</v>
       </c>
       <c r="D56" t="n">
-        <v>7564972</v>
+        <v>7588638</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>96106</v>
+        <v>96247</v>
       </c>
       <c r="D57" t="n">
-        <v>142452027</v>
+        <v>142767023</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>41463</v>
+        <v>41515</v>
       </c>
       <c r="D65" t="n">
-        <v>96769930</v>
+        <v>96999551</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>16608</v>
+        <v>16633</v>
       </c>
       <c r="D68" t="n">
-        <v>37281180</v>
+        <v>37401413</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="D70" t="n">
-        <v>3161980</v>
+        <v>3167178</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2493</v>
+        <v>2502</v>
       </c>
       <c r="D74" t="n">
-        <v>4950257</v>
+        <v>4972370</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>28601</v>
+        <v>28646</v>
       </c>
       <c r="D76" t="n">
-        <v>44076646</v>
+        <v>44149632</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11844</v>
+        <v>11862</v>
       </c>
       <c r="D80" t="n">
-        <v>31302048</v>
+        <v>31414048</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8014</v>
+        <v>8023</v>
       </c>
       <c r="D82" t="n">
-        <v>19457247</v>
+        <v>19503578</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="D85" t="n">
-        <v>975486</v>
+        <v>983098</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>199776</v>
+        <v>200153</v>
       </c>
       <c r="D86" t="n">
-        <v>300811184</v>
+        <v>301579474</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D87" t="n">
-        <v>415519</v>
+        <v>418519</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>94029</v>
+        <v>94142</v>
       </c>
       <c r="D92" t="n">
-        <v>221073137</v>
+        <v>221516178</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44458</v>
+        <v>44534</v>
       </c>
       <c r="D95" t="n">
-        <v>101079320</v>
+        <v>101452882</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6906</v>
+        <v>6945</v>
       </c>
       <c r="D98" t="n">
-        <v>26100778</v>
+        <v>26295361</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4671</v>
+        <v>4682</v>
       </c>
       <c r="D100" t="n">
-        <v>9356466</v>
+        <v>9384119</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>44392</v>
+        <v>44478</v>
       </c>
       <c r="D102" t="n">
-        <v>65719461</v>
+        <v>65968613</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>10816</v>
+        <v>10830</v>
       </c>
       <c r="D106" t="n">
-        <v>18739157</v>
+        <v>18768471</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>10120</v>
+        <v>10136</v>
       </c>
       <c r="D108" t="n">
-        <v>16788184</v>
+        <v>16858490</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="D111" t="n">
-        <v>1061746</v>
+        <v>1074746</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>18547</v>
+        <v>18570</v>
       </c>
       <c r="D112" t="n">
-        <v>37843191</v>
+        <v>37898062</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4171</v>
+        <v>4176</v>
       </c>
       <c r="D115" t="n">
-        <v>9091448</v>
+        <v>9104278</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6053</v>
+        <v>6057</v>
       </c>
       <c r="D117" t="n">
-        <v>13611656</v>
+        <v>13643156</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>199974</v>
+        <v>200296</v>
       </c>
       <c r="D122" t="n">
-        <v>290828810</v>
+        <v>291366130</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="D127" t="n">
-        <v>4454183</v>
+        <v>4457750</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>78212</v>
+        <v>78315</v>
       </c>
       <c r="D129" t="n">
-        <v>184506145</v>
+        <v>184915781</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>41910</v>
+        <v>41993</v>
       </c>
       <c r="D132" t="n">
-        <v>95230853</v>
+        <v>95563597</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1788</v>
+        <v>1802</v>
       </c>
       <c r="D135" t="n">
-        <v>3644678</v>
+        <v>3674301</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>3876</v>
+        <v>3894</v>
       </c>
       <c r="D139" t="n">
-        <v>7847502</v>
+        <v>7920845</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>799515</v>
+        <v>801177</v>
       </c>
       <c r="D141" t="n">
-        <v>1272880137</v>
+        <v>1276930730</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D142" t="n">
-        <v>244965</v>
+        <v>250663</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>2756</v>
+        <v>2782</v>
       </c>
       <c r="D146" t="n">
-        <v>9381721</v>
+        <v>9619112</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>323364</v>
+        <v>323956</v>
       </c>
       <c r="D148" t="n">
-        <v>773829120</v>
+        <v>776604998</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1067</v>
+        <v>1072</v>
       </c>
       <c r="D149" t="n">
-        <v>4605741</v>
+        <v>4647241</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>300159</v>
+        <v>300789</v>
       </c>
       <c r="D151" t="n">
-        <v>674492394</v>
+        <v>677141237</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>3796</v>
+        <v>3807</v>
       </c>
       <c r="D154" t="n">
-        <v>6373207</v>
+        <v>6409069</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>11825</v>
+        <v>11864</v>
       </c>
       <c r="D157" t="n">
-        <v>24506088</v>
+        <v>24680597</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>54724</v>
+        <v>54776</v>
       </c>
       <c r="D160" t="n">
-        <v>76005226</v>
+        <v>76109114</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>16476</v>
+        <v>16487</v>
       </c>
       <c r="D166" t="n">
-        <v>26598477</v>
+        <v>26617558</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>4560</v>
+        <v>4563</v>
       </c>
       <c r="D168" t="n">
-        <v>7226595</v>
+        <v>7233389</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>24571</v>
+        <v>24626</v>
       </c>
       <c r="D174" t="n">
-        <v>36614233</v>
+        <v>36710816</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>10343</v>
+        <v>10359</v>
       </c>
       <c r="D178" t="n">
-        <v>21103427</v>
+        <v>21141376</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>7288</v>
+        <v>7295</v>
       </c>
       <c r="D180" t="n">
-        <v>13774707</v>
+        <v>13785766</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D183" t="n">
-        <v>785867</v>
+        <v>795867</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>33268</v>
+        <v>33336</v>
       </c>
       <c r="D185" t="n">
-        <v>80640727</v>
+        <v>80996378</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>3258</v>
+        <v>3259</v>
       </c>
       <c r="D187" t="n">
-        <v>7639574</v>
+        <v>7642574</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>123343</v>
+        <v>123484</v>
       </c>
       <c r="D192" t="n">
-        <v>184567769</v>
+        <v>184886253</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="D198" t="n">
-        <v>3476136</v>
+        <v>3488298</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>51186</v>
+        <v>51230</v>
       </c>
       <c r="D200" t="n">
-        <v>125559028</v>
+        <v>125769618</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D201" t="n">
-        <v>185879</v>
+        <v>196545</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>20190</v>
+        <v>20226</v>
       </c>
       <c r="D202" t="n">
-        <v>47436090</v>
+        <v>47575830</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>1588</v>
+        <v>1590</v>
       </c>
       <c r="D204" t="n">
-        <v>2732761</v>
+        <v>2736019</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>2804</v>
+        <v>2820</v>
       </c>
       <c r="D207" t="n">
-        <v>5677904</v>
+        <v>5750340</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>326360</v>
+        <v>326777</v>
       </c>
       <c r="D209" t="n">
-        <v>469103219</v>
+        <v>470052629</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>126615</v>
+        <v>126742</v>
       </c>
       <c r="D218" t="n">
-        <v>296032568</v>
+        <v>296742418</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>49809</v>
+        <v>49874</v>
       </c>
       <c r="D221" t="n">
-        <v>112715728</v>
+        <v>113021934</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>6545</v>
+        <v>6551</v>
       </c>
       <c r="D224" t="n">
-        <v>11891107</v>
+        <v>11917591</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>8135</v>
+        <v>8152</v>
       </c>
       <c r="D227" t="n">
-        <v>15504740</v>
+        <v>15562073</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>370371</v>
+        <v>371016</v>
       </c>
       <c r="D230" t="n">
-        <v>523310178</v>
+        <v>524585758</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D231" t="n">
-        <v>310823</v>
+        <v>312823</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>140928</v>
+        <v>141065</v>
       </c>
       <c r="D239" t="n">
-        <v>329008435</v>
+        <v>329543755</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>77893</v>
+        <v>78010</v>
       </c>
       <c r="D242" t="n">
-        <v>175223695</v>
+        <v>175722191</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>5987</v>
+        <v>5992</v>
       </c>
       <c r="D245" t="n">
-        <v>9908835</v>
+        <v>9920235</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D248" t="n">
-        <v>165197</v>
+        <v>179640</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>10270</v>
+        <v>10288</v>
       </c>
       <c r="D249" t="n">
-        <v>19779968</v>
+        <v>19854337</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>147541</v>
+        <v>147757</v>
       </c>
       <c r="D252" t="n">
-        <v>217441607</v>
+        <v>217919617</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="D257" t="n">
-        <v>2949389</v>
+        <v>2986745</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>73301</v>
+        <v>73366</v>
       </c>
       <c r="D259" t="n">
-        <v>174923739</v>
+        <v>175252784</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10300,10 +10300,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>19293</v>
+        <v>19317</v>
       </c>
       <c r="D262" t="n">
-        <v>44083532</v>
+        <v>44189892</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>2371</v>
+        <v>2372</v>
       </c>
       <c r="D264" t="n">
-        <v>4270980</v>
+        <v>4271392</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>4048</v>
+        <v>4057</v>
       </c>
       <c r="D266" t="n">
-        <v>8054540</v>
+        <v>8098295</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10490,10 +10490,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>370854</v>
+        <v>371616</v>
       </c>
       <c r="D267" t="n">
-        <v>541046312</v>
+        <v>542505211</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D268" t="n">
-        <v>387280</v>
+        <v>389001</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -10756,10 +10756,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>1582</v>
+        <v>1585</v>
       </c>
       <c r="D274" t="n">
-        <v>4916081</v>
+        <v>4942000</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -10832,10 +10832,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>146963</v>
+        <v>147111</v>
       </c>
       <c r="D276" t="n">
-        <v>356488220</v>
+        <v>357189169</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -10946,10 +10946,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>103951</v>
+        <v>104113</v>
       </c>
       <c r="D279" t="n">
-        <v>241258654</v>
+        <v>241943196</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -11060,10 +11060,10 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>3261</v>
+        <v>3265</v>
       </c>
       <c r="D282" t="n">
-        <v>5618025</v>
+        <v>5629994</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -11174,10 +11174,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>8372</v>
+        <v>8396</v>
       </c>
       <c r="D285" t="n">
-        <v>16888139</v>
+        <v>16973801</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-28 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H287"/>
+  <dimension ref="A1:H288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>456350</v>
+        <v>457239</v>
       </c>
       <c r="D2" t="n">
-        <v>677856754</v>
+        <v>679719220</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D3" t="n">
-        <v>501925</v>
+        <v>505232</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D4" t="n">
-        <v>1092300</v>
+        <v>1098739</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D9" t="n">
-        <v>4141244</v>
+        <v>4142744</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>177423</v>
+        <v>177761</v>
       </c>
       <c r="D11" t="n">
-        <v>436090543</v>
+        <v>437675865</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D12" t="n">
-        <v>1284804</v>
+        <v>1315470</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>92265</v>
+        <v>92487</v>
       </c>
       <c r="D14" t="n">
-        <v>216652328</v>
+        <v>217600160</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="n">
-        <v>123853</v>
+        <v>130726</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4957</v>
+        <v>4969</v>
       </c>
       <c r="D18" t="n">
-        <v>8446401</v>
+        <v>8467277</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11846</v>
+        <v>11885</v>
       </c>
       <c r="D23" t="n">
-        <v>24379328</v>
+        <v>24538956</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>108660</v>
+        <v>108821</v>
       </c>
       <c r="D25" t="n">
-        <v>158592060</v>
+        <v>158892297</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D30" t="n">
-        <v>1214569</v>
+        <v>1217569</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>47972</v>
+        <v>48050</v>
       </c>
       <c r="D31" t="n">
-        <v>114528453</v>
+        <v>114892664</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17421</v>
+        <v>17455</v>
       </c>
       <c r="D34" t="n">
-        <v>40227622</v>
+        <v>40387801</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2001</v>
+        <v>2009</v>
       </c>
       <c r="D37" t="n">
-        <v>3540829</v>
+        <v>3572571</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3038</v>
+        <v>3049</v>
       </c>
       <c r="D39" t="n">
-        <v>5940586</v>
+        <v>5985515</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>133837</v>
+        <v>134043</v>
       </c>
       <c r="D40" t="n">
-        <v>198856387</v>
+        <v>199248499</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1682</v>
+        <v>1689</v>
       </c>
       <c r="D46" t="n">
-        <v>5088999</v>
+        <v>5123653</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>67221</v>
+        <v>67316</v>
       </c>
       <c r="D48" t="n">
-        <v>165768659</v>
+        <v>166230121</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>14277</v>
+        <v>14307</v>
       </c>
       <c r="D51" t="n">
-        <v>34107664</v>
+        <v>34221035</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="D53" t="n">
-        <v>2844397</v>
+        <v>2845063</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3822</v>
+        <v>3840</v>
       </c>
       <c r="D56" t="n">
-        <v>7588638</v>
+        <v>7683005</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>96247</v>
+        <v>96406</v>
       </c>
       <c r="D57" t="n">
-        <v>142767023</v>
+        <v>143098985</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D63" t="n">
-        <v>1700228</v>
+        <v>1707966</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>41515</v>
+        <v>41580</v>
       </c>
       <c r="D65" t="n">
-        <v>96999551</v>
+        <v>97292018</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D66" t="n">
-        <v>297762</v>
+        <v>298428</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>16633</v>
+        <v>16678</v>
       </c>
       <c r="D68" t="n">
-        <v>37401413</v>
+        <v>37560491</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1768</v>
+        <v>1774</v>
       </c>
       <c r="D70" t="n">
-        <v>3167178</v>
+        <v>3178702</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2502</v>
+        <v>2518</v>
       </c>
       <c r="D74" t="n">
-        <v>4972370</v>
+        <v>5062625</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>28646</v>
+        <v>28699</v>
       </c>
       <c r="D76" t="n">
-        <v>44149632</v>
+        <v>44273508</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11862</v>
+        <v>11884</v>
       </c>
       <c r="D80" t="n">
-        <v>31414048</v>
+        <v>31518567</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D81" t="n">
-        <v>52860</v>
+        <v>54360</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8023</v>
+        <v>8047</v>
       </c>
       <c r="D82" t="n">
-        <v>19503578</v>
+        <v>19612266</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="D84" t="n">
-        <v>1214288</v>
+        <v>1229768</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D85" t="n">
-        <v>983098</v>
+        <v>984598</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>200153</v>
+        <v>200638</v>
       </c>
       <c r="D86" t="n">
-        <v>301579474</v>
+        <v>302866497</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D87" t="n">
-        <v>418519</v>
+        <v>445047</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="D90" t="n">
-        <v>2051127</v>
+        <v>2072164</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>94142</v>
+        <v>94344</v>
       </c>
       <c r="D92" t="n">
-        <v>221516178</v>
+        <v>222291672</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D93" t="n">
-        <v>724165</v>
+        <v>734165</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44534</v>
+        <v>44627</v>
       </c>
       <c r="D95" t="n">
-        <v>101452882</v>
+        <v>101884105</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6945</v>
+        <v>7063</v>
       </c>
       <c r="D98" t="n">
-        <v>26295361</v>
+        <v>26818899</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4682</v>
+        <v>4703</v>
       </c>
       <c r="D100" t="n">
-        <v>9384119</v>
+        <v>9468753</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>44478</v>
+        <v>44520</v>
       </c>
       <c r="D102" t="n">
-        <v>65968613</v>
+        <v>66078657</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>10830</v>
+        <v>10833</v>
       </c>
       <c r="D106" t="n">
-        <v>18768471</v>
+        <v>18781471</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>10136</v>
+        <v>10143</v>
       </c>
       <c r="D108" t="n">
-        <v>16858490</v>
+        <v>16879194</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D111" t="n">
-        <v>1074746</v>
+        <v>1077746</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>18570</v>
+        <v>18601</v>
       </c>
       <c r="D112" t="n">
-        <v>37898062</v>
+        <v>38005577</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4176</v>
+        <v>4179</v>
       </c>
       <c r="D115" t="n">
-        <v>9104278</v>
+        <v>9114950</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6057</v>
+        <v>6062</v>
       </c>
       <c r="D117" t="n">
-        <v>13643156</v>
+        <v>13664435</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>200296</v>
+        <v>200626</v>
       </c>
       <c r="D122" t="n">
-        <v>291366130</v>
+        <v>291993322</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1610</v>
+        <v>1614</v>
       </c>
       <c r="D127" t="n">
-        <v>4457750</v>
+        <v>4467127</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>78315</v>
+        <v>78467</v>
       </c>
       <c r="D129" t="n">
-        <v>184915781</v>
+        <v>185717518</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D130" t="n">
-        <v>674942</v>
+        <v>681182</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>41993</v>
+        <v>42085</v>
       </c>
       <c r="D132" t="n">
-        <v>95563597</v>
+        <v>95901240</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1802</v>
+        <v>1813</v>
       </c>
       <c r="D135" t="n">
-        <v>3674301</v>
+        <v>3690688</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>3894</v>
+        <v>3900</v>
       </c>
       <c r="D139" t="n">
-        <v>7920845</v>
+        <v>7944113</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>801177</v>
+        <v>802419</v>
       </c>
       <c r="D141" t="n">
-        <v>1276930730</v>
+        <v>1279826527</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>2782</v>
+        <v>2794</v>
       </c>
       <c r="D146" t="n">
-        <v>9619112</v>
+        <v>9685711</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>323956</v>
+        <v>324726</v>
       </c>
       <c r="D148" t="n">
-        <v>776604998</v>
+        <v>780355379</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="D149" t="n">
-        <v>4647241</v>
+        <v>4671741</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>300789</v>
+        <v>301493</v>
       </c>
       <c r="D151" t="n">
-        <v>677141237</v>
+        <v>680141817</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>3807</v>
+        <v>3825</v>
       </c>
       <c r="D154" t="n">
-        <v>6409069</v>
+        <v>6434107</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>11864</v>
+        <v>11908</v>
       </c>
       <c r="D157" t="n">
-        <v>24680597</v>
+        <v>24866789</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>54776</v>
+        <v>54844</v>
       </c>
       <c r="D160" t="n">
-        <v>76109114</v>
+        <v>76227038</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -6652,10 +6652,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>16487</v>
+        <v>16496</v>
       </c>
       <c r="D166" t="n">
-        <v>26617558</v>
+        <v>26647258</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -6728,10 +6728,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>4563</v>
+        <v>4569</v>
       </c>
       <c r="D168" t="n">
-        <v>7233389</v>
+        <v>7245609</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6842,10 +6842,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D171" t="n">
-        <v>681610</v>
+        <v>683110</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -6956,10 +6956,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>24626</v>
+        <v>24665</v>
       </c>
       <c r="D174" t="n">
-        <v>36710816</v>
+        <v>36772358</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -7108,10 +7108,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>10359</v>
+        <v>10366</v>
       </c>
       <c r="D178" t="n">
-        <v>21141376</v>
+        <v>21170229</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>7295</v>
+        <v>7298</v>
       </c>
       <c r="D180" t="n">
-        <v>13785766</v>
+        <v>13794926</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -7260,10 +7260,10 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D182" t="n">
-        <v>560430</v>
+        <v>561930</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D183" t="n">
-        <v>795867</v>
+        <v>801337</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -7374,10 +7374,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>33336</v>
+        <v>33389</v>
       </c>
       <c r="D185" t="n">
-        <v>80996378</v>
+        <v>81190143</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -7450,10 +7450,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>3259</v>
+        <v>3261</v>
       </c>
       <c r="D187" t="n">
-        <v>7642574</v>
+        <v>7647181</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>123484</v>
+        <v>123663</v>
       </c>
       <c r="D192" t="n">
-        <v>184886253</v>
+        <v>185216010</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -7792,10 +7792,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D196" t="n">
-        <v>27389</v>
+        <v>28889</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7868,10 +7868,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>1163</v>
+        <v>1168</v>
       </c>
       <c r="D198" t="n">
-        <v>3488298</v>
+        <v>3521770</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -7944,10 +7944,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>51230</v>
+        <v>51309</v>
       </c>
       <c r="D200" t="n">
-        <v>125769618</v>
+        <v>126102856</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D201" t="n">
-        <v>196545</v>
+        <v>198045</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8020,10 +8020,10 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>20226</v>
+        <v>20262</v>
       </c>
       <c r="D202" t="n">
-        <v>47575830</v>
+        <v>47767828</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -8096,10 +8096,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D204" t="n">
-        <v>2736019</v>
+        <v>2746019</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -8210,10 +8210,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>2820</v>
+        <v>2834</v>
       </c>
       <c r="D207" t="n">
-        <v>5750340</v>
+        <v>5823500</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -8286,10 +8286,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>326777</v>
+        <v>327332</v>
       </c>
       <c r="D209" t="n">
-        <v>470052629</v>
+        <v>471152649</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D210" t="n">
-        <v>227169</v>
+        <v>227211</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8552,10 +8552,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>1439</v>
+        <v>1448</v>
       </c>
       <c r="D216" t="n">
-        <v>3735709</v>
+        <v>3775748</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -8628,10 +8628,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>126742</v>
+        <v>126932</v>
       </c>
       <c r="D218" t="n">
-        <v>296742418</v>
+        <v>297710402</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>49874</v>
+        <v>49978</v>
       </c>
       <c r="D221" t="n">
-        <v>113021934</v>
+        <v>113443751</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8856,10 +8856,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>6551</v>
+        <v>6574</v>
       </c>
       <c r="D224" t="n">
-        <v>11917591</v>
+        <v>12003304</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>8152</v>
+        <v>8189</v>
       </c>
       <c r="D227" t="n">
-        <v>15562073</v>
+        <v>15685449</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -9084,10 +9084,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>371016</v>
+        <v>371594</v>
       </c>
       <c r="D230" t="n">
-        <v>524585758</v>
+        <v>525636691</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -9312,10 +9312,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D236" t="n">
-        <v>19580</v>
+        <v>39580</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -9350,10 +9350,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D237" t="n">
-        <v>2587006</v>
+        <v>2597006</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -9426,10 +9426,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>141065</v>
+        <v>141249</v>
       </c>
       <c r="D239" t="n">
-        <v>329543755</v>
+        <v>330429759</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D240" t="n">
-        <v>766106</v>
+        <v>779106</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9540,10 +9540,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>78010</v>
+        <v>78169</v>
       </c>
       <c r="D242" t="n">
-        <v>175722191</v>
+        <v>176427392</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -9654,10 +9654,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>5992</v>
+        <v>6002</v>
       </c>
       <c r="D245" t="n">
-        <v>9920235</v>
+        <v>9953236</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -9768,10 +9768,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D248" t="n">
-        <v>179640</v>
+        <v>189963</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>10288</v>
+        <v>10319</v>
       </c>
       <c r="D249" t="n">
-        <v>19854337</v>
+        <v>19965436</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9920,10 +9920,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>147757</v>
+        <v>147982</v>
       </c>
       <c r="D252" t="n">
-        <v>217919617</v>
+        <v>218398393</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -10075,7 +10075,7 @@
         <v>4</v>
       </c>
       <c r="D256" t="n">
-        <v>9980</v>
+        <v>8979</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -10089,12 +10089,12 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - immatriculée au RCS</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -10110,10 +10110,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>1035</v>
+        <v>4</v>
       </c>
       <c r="D257" t="n">
-        <v>2986745</v>
+        <v>9980</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -10127,12 +10127,12 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Personne morale de droit étranger - immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -10148,10 +10148,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>5</v>
+        <v>1037</v>
       </c>
       <c r="D258" t="n">
-        <v>2880</v>
+        <v>3006745</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -10165,12 +10165,12 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>73366</v>
+        <v>5</v>
       </c>
       <c r="D259" t="n">
-        <v>175252784</v>
+        <v>2880</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10203,12 +10203,12 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -10224,10 +10224,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>79</v>
+        <v>73490</v>
       </c>
       <c r="D260" t="n">
-        <v>270179</v>
+        <v>175888407</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -10241,12 +10241,12 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="D261" t="n">
-        <v>31332</v>
+        <v>270179</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -10279,12 +10279,12 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -10300,10 +10300,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>19317</v>
+        <v>5</v>
       </c>
       <c r="D262" t="n">
-        <v>44189892</v>
+        <v>31332</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -10317,12 +10317,12 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -10338,10 +10338,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>20</v>
+        <v>19356</v>
       </c>
       <c r="D263" t="n">
-        <v>40068</v>
+        <v>44410296</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -10355,12 +10355,12 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>2372</v>
+        <v>20</v>
       </c>
       <c r="D264" t="n">
-        <v>4271392</v>
+        <v>40068</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10393,12 +10393,12 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>7</v>
+        <v>2381</v>
       </c>
       <c r="D265" t="n">
-        <v>8596</v>
+        <v>4311915</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -10431,12 +10431,12 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>4057</v>
+        <v>7</v>
       </c>
       <c r="D266" t="n">
-        <v>8098295</v>
+        <v>8596</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10469,12 +10469,12 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -10490,29 +10490,29 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>371616</v>
+        <v>4075</v>
       </c>
       <c r="D267" t="n">
-        <v>542505211</v>
+        <v>8161439</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>Entrepreneur individuel</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>242</v>
+        <v>372334</v>
       </c>
       <c r="D268" t="n">
-        <v>389001</v>
+        <v>543919173</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -10545,12 +10545,12 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>Indivision</t>
+          <t>Entrepreneur individuel</t>
         </is>
       </c>
     </row>
@@ -10566,10 +10566,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>374</v>
+        <v>243</v>
       </c>
       <c r="D269" t="n">
-        <v>807312</v>
+        <v>390985</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -10583,12 +10583,12 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>Société créée de fait</t>
+          <t>Indivision</t>
         </is>
       </c>
     </row>
@@ -10604,10 +10604,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>23</v>
+        <v>374</v>
       </c>
       <c r="D270" t="n">
-        <v>89705</v>
+        <v>807312</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -10621,12 +10621,12 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>Société en participation</t>
+          <t>Société créée de fait</t>
         </is>
       </c>
     </row>
@@ -10642,10 +10642,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D271" t="n">
-        <v>30536</v>
+        <v>89705</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -10659,12 +10659,12 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
+          <t>Société en participation</t>
         </is>
       </c>
     </row>
@@ -10680,10 +10680,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D272" t="n">
-        <v>9395</v>
+        <v>30536</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -10697,12 +10697,12 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
+          <t>Autre groupement de droit privé non doté de la personnalité morale</t>
         </is>
       </c>
     </row>
@@ -10718,10 +10718,10 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D273" t="n">
-        <v>37146</v>
+        <v>9395</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -10735,12 +10735,12 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
+          <t>Personne morale de droit étranger - non immatriculée au RCS</t>
         </is>
       </c>
     </row>
@@ -10756,10 +10756,10 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>1585</v>
+        <v>20</v>
       </c>
       <c r="D274" t="n">
-        <v>4942000</v>
+        <v>37146</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -10773,12 +10773,12 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>Société en nom collectif</t>
+          <t>Etablissement public ou régie à caractère industriel ou commercial</t>
         </is>
       </c>
     </row>
@@ -10794,10 +10794,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>27</v>
+        <v>1587</v>
       </c>
       <c r="D275" t="n">
-        <v>105998</v>
+        <v>4962000</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -10811,12 +10811,12 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
         <is>
-          <t>Société en commandite</t>
+          <t>Société en nom collectif</t>
         </is>
       </c>
     </row>
@@ -10832,10 +10832,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>147111</v>
+        <v>27</v>
       </c>
       <c r="D276" t="n">
-        <v>357189169</v>
+        <v>105998</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -10849,12 +10849,12 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>Société à responsabilité limitée (SARL)</t>
+          <t>Société en commandite</t>
         </is>
       </c>
     </row>
@@ -10870,10 +10870,10 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>189</v>
+        <v>147355</v>
       </c>
       <c r="D277" t="n">
-        <v>794560</v>
+        <v>358338268</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -10887,12 +10887,12 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>Société anonyme à conseil d'administration</t>
+          <t>Société à responsabilité limitée (SARL)</t>
         </is>
       </c>
     </row>
@@ -10908,10 +10908,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="D278" t="n">
-        <v>80505</v>
+        <v>794560</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -10925,12 +10925,12 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>Société anonyme à directoire</t>
+          <t>Société anonyme à conseil d'administration</t>
         </is>
       </c>
     </row>
@@ -10946,10 +10946,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>104113</v>
+        <v>16</v>
       </c>
       <c r="D279" t="n">
-        <v>241943196</v>
+        <v>80505</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -10963,12 +10963,12 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>Société par actions simplifiée</t>
+          <t>Société anonyme à directoire</t>
         </is>
       </c>
     </row>
@@ -10984,10 +10984,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>21</v>
+        <v>104310</v>
       </c>
       <c r="D280" t="n">
-        <v>42504</v>
+        <v>242750170</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -11001,12 +11001,12 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>57</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>Groupement d'intérêt économique</t>
+          <t>Société par actions simplifiée</t>
         </is>
       </c>
     </row>
@@ -11022,10 +11022,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D281" t="n">
-        <v>20500</v>
+        <v>42504</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -11039,12 +11039,12 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>62</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>Société coopérative agricole</t>
+          <t>Groupement d'intérêt économique</t>
         </is>
       </c>
     </row>
@@ -11060,10 +11060,10 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>3265</v>
+        <v>8</v>
       </c>
       <c r="D282" t="n">
-        <v>5629994</v>
+        <v>20500</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -11077,12 +11077,12 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
         <is>
-          <t>Société civile</t>
+          <t>Société coopérative agricole</t>
         </is>
       </c>
     </row>
@@ -11098,10 +11098,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>16</v>
+        <v>3279</v>
       </c>
       <c r="D283" t="n">
-        <v>42740</v>
+        <v>5664655</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -11115,12 +11115,12 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>Organisme professionnel</t>
+          <t>Société civile</t>
         </is>
       </c>
     </row>
@@ -11136,10 +11136,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D284" t="n">
-        <v>36730</v>
+        <v>47740</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -11153,12 +11153,12 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>84</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>Syndicat de propriétaires</t>
+          <t>Organisme professionnel</t>
         </is>
       </c>
     </row>
@@ -11174,10 +11174,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>8396</v>
+        <v>11</v>
       </c>
       <c r="D285" t="n">
-        <v>16973801</v>
+        <v>36730</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -11191,12 +11191,12 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>91</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>Association loi 1901 ou assimilé</t>
+          <t>Syndicat de propriétaires</t>
         </is>
       </c>
     </row>
@@ -11212,10 +11212,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3</v>
+        <v>8430</v>
       </c>
       <c r="D286" t="n">
-        <v>20666</v>
+        <v>17078228</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -11229,12 +11229,12 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>92</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>Fondation</t>
+          <t>Association loi 1901 ou assimilé</t>
         </is>
       </c>
     </row>
@@ -11250,27 +11250,65 @@
         </is>
       </c>
       <c r="C287" t="n">
+        <v>3</v>
+      </c>
+      <c r="D287" t="n">
+        <v>20666</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>Fondation</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
         <v>4</v>
       </c>
-      <c r="D287" t="n">
+      <c r="D288" t="n">
         <v>11970</v>
       </c>
-      <c r="E287" t="inlineStr">
+      <c r="E288" t="inlineStr">
         <is>
           <t>93</t>
         </is>
       </c>
-      <c r="F287" t="inlineStr">
+      <c r="F288" t="inlineStr">
         <is>
           <t>Provence-Alpes-Côte d'Azur</t>
         </is>
       </c>
-      <c r="G287" t="inlineStr">
+      <c r="G288" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="H287" t="inlineStr">
+      <c r="H288" t="inlineStr">
         <is>
           <t>Autre personne morale de droit privé</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>458262</v>
+        <v>459278</v>
       </c>
       <c r="D2" t="n">
-        <v>681788747</v>
+        <v>683735850</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D3" t="n">
-        <v>516500</v>
+        <v>517629</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="D4" t="n">
-        <v>1109607</v>
+        <v>1131452</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1513</v>
+        <v>1522</v>
       </c>
       <c r="D9" t="n">
-        <v>4169947</v>
+        <v>4226770</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>178173</v>
+        <v>178519</v>
       </c>
       <c r="D11" t="n">
-        <v>439894006</v>
+        <v>441484115</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D12" t="n">
-        <v>1337636</v>
+        <v>1350318</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>92748</v>
+        <v>92979</v>
       </c>
       <c r="D14" t="n">
-        <v>218791366</v>
+        <v>219793018</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>6000</v>
+        <v>24400</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4981</v>
+        <v>5004</v>
       </c>
       <c r="D18" t="n">
-        <v>8506500</v>
+        <v>8555008</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D21" t="n">
-        <v>269596</v>
+        <v>312596</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11932</v>
+        <v>11997</v>
       </c>
       <c r="D23" t="n">
-        <v>24727938</v>
+        <v>24952950</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>108983</v>
+        <v>109165</v>
       </c>
       <c r="D25" t="n">
-        <v>159213495</v>
+        <v>159647931</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D30" t="n">
-        <v>1229894</v>
+        <v>1234182</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>48156</v>
+        <v>48257</v>
       </c>
       <c r="D31" t="n">
-        <v>115392606</v>
+        <v>115868070</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17494</v>
+        <v>17529</v>
       </c>
       <c r="D34" t="n">
-        <v>40536867</v>
+        <v>40647229</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D37" t="n">
-        <v>3582341</v>
+        <v>3604221</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3066</v>
+        <v>3076</v>
       </c>
       <c r="D39" t="n">
-        <v>6050445</v>
+        <v>6088474</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>134286</v>
+        <v>134529</v>
       </c>
       <c r="D40" t="n">
-        <v>199748128</v>
+        <v>200217214</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D42" t="n">
-        <v>218166</v>
+        <v>229456</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D43" t="n">
-        <v>4500</v>
+        <v>14868</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="D46" t="n">
-        <v>5169691</v>
+        <v>5172691</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>67426</v>
+        <v>67515</v>
       </c>
       <c r="D48" t="n">
-        <v>166804333</v>
+        <v>167238661</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>14338</v>
+        <v>14381</v>
       </c>
       <c r="D51" t="n">
-        <v>34357837</v>
+        <v>34546791</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3853</v>
+        <v>3870</v>
       </c>
       <c r="D56" t="n">
-        <v>7753242</v>
+        <v>7815439</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>96613</v>
+        <v>96797</v>
       </c>
       <c r="D57" t="n">
-        <v>143585621</v>
+        <v>143906612</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D63" t="n">
-        <v>1707966</v>
+        <v>1714410</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>41674</v>
+        <v>41760</v>
       </c>
       <c r="D65" t="n">
-        <v>97772414</v>
+        <v>98231139</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>16748</v>
+        <v>16792</v>
       </c>
       <c r="D68" t="n">
-        <v>37919855</v>
+        <v>38123207</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1785</v>
+        <v>1788</v>
       </c>
       <c r="D70" t="n">
-        <v>3224183</v>
+        <v>3240506</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2529</v>
+        <v>2546</v>
       </c>
       <c r="D74" t="n">
-        <v>5087201</v>
+        <v>5151630</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>28772</v>
+        <v>28823</v>
       </c>
       <c r="D76" t="n">
-        <v>44469428</v>
+        <v>44573604</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11902</v>
+        <v>11942</v>
       </c>
       <c r="D80" t="n">
-        <v>31617970</v>
+        <v>31821555</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8074</v>
+        <v>8095</v>
       </c>
       <c r="D82" t="n">
-        <v>19729020</v>
+        <v>19853112</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="D84" t="n">
-        <v>1229768</v>
+        <v>1240215</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D85" t="n">
-        <v>984598</v>
+        <v>996098</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>201135</v>
+        <v>201598</v>
       </c>
       <c r="D86" t="n">
-        <v>304079629</v>
+        <v>305127766</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D87" t="n">
-        <v>450228</v>
+        <v>473724</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D90" t="n">
-        <v>2100617</v>
+        <v>2112117</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>94550</v>
+        <v>94786</v>
       </c>
       <c r="D92" t="n">
-        <v>223112399</v>
+        <v>224070573</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D93" t="n">
-        <v>734165</v>
+        <v>735665</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D94" t="n">
-        <v>115419</v>
+        <v>116085</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44742</v>
+        <v>44853</v>
       </c>
       <c r="D95" t="n">
-        <v>102279638</v>
+        <v>102697147</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D96" t="n">
-        <v>37459</v>
+        <v>40459</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D97" t="n">
-        <v>269812</v>
+        <v>280034</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7170</v>
+        <v>7275</v>
       </c>
       <c r="D98" t="n">
-        <v>27195305</v>
+        <v>27541302</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4729</v>
+        <v>4749</v>
       </c>
       <c r="D100" t="n">
-        <v>9535022</v>
+        <v>9634911</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>44598</v>
+        <v>44646</v>
       </c>
       <c r="D102" t="n">
-        <v>66251443</v>
+        <v>66359480</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>10845</v>
+        <v>10852</v>
       </c>
       <c r="D106" t="n">
-        <v>18841795</v>
+        <v>18880583</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>10157</v>
+        <v>10163</v>
       </c>
       <c r="D108" t="n">
-        <v>16917950</v>
+        <v>16933245</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D110" t="n">
-        <v>1007785</v>
+        <v>1008635</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>18612</v>
+        <v>18648</v>
       </c>
       <c r="D112" t="n">
-        <v>38043886</v>
+        <v>38146477</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4181</v>
+        <v>4188</v>
       </c>
       <c r="D115" t="n">
-        <v>9117950</v>
+        <v>9152634</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6074</v>
+        <v>6078</v>
       </c>
       <c r="D117" t="n">
-        <v>13702849</v>
+        <v>13721950</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D119" t="n">
-        <v>548640</v>
+        <v>553097</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D120" t="n">
-        <v>770889</v>
+        <v>779409</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>201040</v>
+        <v>201369</v>
       </c>
       <c r="D122" t="n">
-        <v>292930980</v>
+        <v>293589909</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1626</v>
+        <v>1630</v>
       </c>
       <c r="D128" t="n">
-        <v>4527576</v>
+        <v>4558565</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>78650</v>
+        <v>78823</v>
       </c>
       <c r="D130" t="n">
-        <v>186617829</v>
+        <v>187549044</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D131" t="n">
-        <v>682682</v>
+        <v>684182</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>42205</v>
+        <v>42317</v>
       </c>
       <c r="D133" t="n">
-        <v>96404083</v>
+        <v>96888140</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1827</v>
+        <v>1835</v>
       </c>
       <c r="D136" t="n">
-        <v>3728600</v>
+        <v>3740600</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3929</v>
+        <v>3947</v>
       </c>
       <c r="D140" t="n">
-        <v>8046895</v>
+        <v>8105217</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>803770</v>
+        <v>805159</v>
       </c>
       <c r="D142" t="n">
-        <v>1283013131</v>
+        <v>1286093512</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D143" t="n">
-        <v>250663</v>
+        <v>252163</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="D144" t="n">
-        <v>829635</v>
+        <v>855743</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>2803</v>
+        <v>2814</v>
       </c>
       <c r="D147" t="n">
-        <v>9747044</v>
+        <v>9840431</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>325618</v>
+        <v>326504</v>
       </c>
       <c r="D149" t="n">
-        <v>784813771</v>
+        <v>788797478</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1088</v>
+        <v>1097</v>
       </c>
       <c r="D150" t="n">
-        <v>4761604</v>
+        <v>4809104</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6082,10 +6082,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D151" t="n">
-        <v>359850</v>
+        <v>369850</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>302225</v>
+        <v>302922</v>
       </c>
       <c r="D152" t="n">
-        <v>683234832</v>
+        <v>686201697</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D154" t="n">
-        <v>169784</v>
+        <v>177144</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3843</v>
+        <v>3858</v>
       </c>
       <c r="D155" t="n">
-        <v>6467984</v>
+        <v>6514918</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>11951</v>
+        <v>12024</v>
       </c>
       <c r="D158" t="n">
-        <v>25018619</v>
+        <v>25352020</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>54916</v>
+        <v>54980</v>
       </c>
       <c r="D161" t="n">
-        <v>76359189</v>
+        <v>76486671</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>16510</v>
+        <v>16518</v>
       </c>
       <c r="D167" t="n">
-        <v>26721756</v>
+        <v>26763496</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>4572</v>
+        <v>4573</v>
       </c>
       <c r="D169" t="n">
-        <v>7248914</v>
+        <v>7250554</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>24729</v>
+        <v>24784</v>
       </c>
       <c r="D175" t="n">
-        <v>36896187</v>
+        <v>37015452</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7032,10 +7032,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D176" t="n">
-        <v>11316</v>
+        <v>12233</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>10396</v>
+        <v>10419</v>
       </c>
       <c r="D179" t="n">
-        <v>21310210</v>
+        <v>21406803</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>7314</v>
+        <v>7327</v>
       </c>
       <c r="D181" t="n">
-        <v>13847126</v>
+        <v>13894514</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>33432</v>
+        <v>33483</v>
       </c>
       <c r="D186" t="n">
-        <v>81343798</v>
+        <v>81678710</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7488,10 +7488,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3261</v>
+        <v>3263</v>
       </c>
       <c r="D188" t="n">
-        <v>7647181</v>
+        <v>7653181</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -7526,10 +7526,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D189" t="n">
-        <v>1008068</v>
+        <v>1011068</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>123905</v>
+        <v>124100</v>
       </c>
       <c r="D193" t="n">
-        <v>185669966</v>
+        <v>186077918</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7830,10 +7830,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D197" t="n">
-        <v>28889</v>
+        <v>30389</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>1174</v>
+        <v>1179</v>
       </c>
       <c r="D199" t="n">
-        <v>3553768</v>
+        <v>3572341</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>51422</v>
+        <v>51516</v>
       </c>
       <c r="D201" t="n">
-        <v>126618653</v>
+        <v>127033589</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>20331</v>
+        <v>20371</v>
       </c>
       <c r="D203" t="n">
-        <v>48091464</v>
+        <v>48275232</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1593</v>
+        <v>1598</v>
       </c>
       <c r="D205" t="n">
-        <v>2753544</v>
+        <v>2768894</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2847</v>
+        <v>2855</v>
       </c>
       <c r="D208" t="n">
-        <v>5861985</v>
+        <v>5888660</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>327989</v>
+        <v>328601</v>
       </c>
       <c r="D210" t="n">
-        <v>472580215</v>
+        <v>473817336</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D212" t="n">
-        <v>482710</v>
+        <v>490223</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D217" t="n">
-        <v>3795991</v>
+        <v>3796657</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>127186</v>
+        <v>127367</v>
       </c>
       <c r="D219" t="n">
-        <v>299021336</v>
+        <v>299889658</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D220" t="n">
-        <v>673207</v>
+        <v>687707</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>50103</v>
+        <v>50216</v>
       </c>
       <c r="D222" t="n">
-        <v>114080303</v>
+        <v>114642338</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>6599</v>
+        <v>6614</v>
       </c>
       <c r="D225" t="n">
-        <v>12062027</v>
+        <v>12099267</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>8214</v>
+        <v>8252</v>
       </c>
       <c r="D228" t="n">
-        <v>15759045</v>
+        <v>15904822</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>372234</v>
+        <v>372820</v>
       </c>
       <c r="D231" t="n">
-        <v>526792775</v>
+        <v>527844260</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9388,10 +9388,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>978</v>
+        <v>985</v>
       </c>
       <c r="D238" t="n">
-        <v>2615845</v>
+        <v>2647935</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>141468</v>
+        <v>141732</v>
       </c>
       <c r="D240" t="n">
-        <v>331447747</v>
+        <v>332661823</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>78369</v>
+        <v>78535</v>
       </c>
       <c r="D243" t="n">
-        <v>177252845</v>
+        <v>177957899</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>6024</v>
+        <v>6039</v>
       </c>
       <c r="D246" t="n">
-        <v>9996967</v>
+        <v>10046699</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D249" t="n">
-        <v>191463</v>
+        <v>197022</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>10376</v>
+        <v>10405</v>
       </c>
       <c r="D250" t="n">
-        <v>20152317</v>
+        <v>20251612</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>148251</v>
+        <v>148506</v>
       </c>
       <c r="D253" t="n">
-        <v>218994210</v>
+        <v>219513962</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="D259" t="n">
-        <v>3014254</v>
+        <v>3045586</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>73622</v>
+        <v>73752</v>
       </c>
       <c r="D261" t="n">
-        <v>176516165</v>
+        <v>177153531</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>19394</v>
+        <v>19456</v>
       </c>
       <c r="D264" t="n">
-        <v>44584345</v>
+        <v>44901083</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>2386</v>
+        <v>2397</v>
       </c>
       <c r="D266" t="n">
-        <v>4344008</v>
+        <v>4386023</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>4088</v>
+        <v>4114</v>
       </c>
       <c r="D268" t="n">
-        <v>8195784</v>
+        <v>8310781</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -10566,10 +10566,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>373150</v>
+        <v>373825</v>
       </c>
       <c r="D269" t="n">
-        <v>545471165</v>
+        <v>546796016</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -10832,10 +10832,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>1593</v>
+        <v>1596</v>
       </c>
       <c r="D276" t="n">
-        <v>4995948</v>
+        <v>5007866</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -10908,10 +10908,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>147621</v>
+        <v>147839</v>
       </c>
       <c r="D278" t="n">
-        <v>359503305</v>
+        <v>360532682</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -11022,10 +11022,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>104542</v>
+        <v>104741</v>
       </c>
       <c r="D281" t="n">
-        <v>243648315</v>
+        <v>244480512</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -11136,10 +11136,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>3296</v>
+        <v>3309</v>
       </c>
       <c r="D284" t="n">
-        <v>5719425</v>
+        <v>5745668</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -11250,10 +11250,10 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>8481</v>
+        <v>8528</v>
       </c>
       <c r="D287" t="n">
-        <v>17318008</v>
+        <v>17531275</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-31 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>459278</v>
+        <v>460129</v>
       </c>
       <c r="D2" t="n">
-        <v>683735850</v>
+        <v>685402007</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D3" t="n">
-        <v>517629</v>
+        <v>520577</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="D9" t="n">
-        <v>4226770</v>
+        <v>4243491</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>178519</v>
+        <v>178912</v>
       </c>
       <c r="D11" t="n">
-        <v>441484115</v>
+        <v>443288343</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D12" t="n">
-        <v>1350318</v>
+        <v>1380601</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>92979</v>
+        <v>93162</v>
       </c>
       <c r="D14" t="n">
-        <v>219793018</v>
+        <v>220558115</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5004</v>
+        <v>5009</v>
       </c>
       <c r="D18" t="n">
-        <v>8555008</v>
+        <v>8572122</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D21" t="n">
-        <v>312596</v>
+        <v>332596</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11997</v>
+        <v>12045</v>
       </c>
       <c r="D23" t="n">
-        <v>24952950</v>
+        <v>25110145</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>109165</v>
+        <v>109297</v>
       </c>
       <c r="D25" t="n">
-        <v>159647931</v>
+        <v>159899794</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>48257</v>
+        <v>48316</v>
       </c>
       <c r="D31" t="n">
-        <v>115868070</v>
+        <v>116108254</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D32" t="n">
-        <v>309905</v>
+        <v>310571</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17529</v>
+        <v>17565</v>
       </c>
       <c r="D34" t="n">
-        <v>40647229</v>
+        <v>40828266</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2021</v>
+        <v>2035</v>
       </c>
       <c r="D37" t="n">
-        <v>3604221</v>
+        <v>3645047</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3076</v>
+        <v>3087</v>
       </c>
       <c r="D39" t="n">
-        <v>6088474</v>
+        <v>6122992</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>134529</v>
+        <v>134670</v>
       </c>
       <c r="D40" t="n">
-        <v>200217214</v>
+        <v>200458382</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D42" t="n">
-        <v>229456</v>
+        <v>229620</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1699</v>
+        <v>1702</v>
       </c>
       <c r="D46" t="n">
-        <v>5172691</v>
+        <v>5194022</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>67515</v>
+        <v>67620</v>
       </c>
       <c r="D48" t="n">
-        <v>167238661</v>
+        <v>167756838</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>14381</v>
+        <v>14416</v>
       </c>
       <c r="D51" t="n">
-        <v>34546791</v>
+        <v>34752051</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1737</v>
+        <v>1739</v>
       </c>
       <c r="D53" t="n">
-        <v>2862505</v>
+        <v>2869497</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3870</v>
+        <v>3880</v>
       </c>
       <c r="D56" t="n">
-        <v>7815439</v>
+        <v>7873477</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>96797</v>
+        <v>96948</v>
       </c>
       <c r="D57" t="n">
-        <v>143906612</v>
+        <v>144158120</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D63" t="n">
-        <v>1714410</v>
+        <v>1715076</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>41760</v>
+        <v>41797</v>
       </c>
       <c r="D65" t="n">
-        <v>98231139</v>
+        <v>98378526</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D66" t="n">
-        <v>308428</v>
+        <v>309094</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>16792</v>
+        <v>16825</v>
       </c>
       <c r="D68" t="n">
-        <v>38123207</v>
+        <v>38248020</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1788</v>
+        <v>1790</v>
       </c>
       <c r="D70" t="n">
-        <v>3240506</v>
+        <v>3242260</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2546</v>
+        <v>2555</v>
       </c>
       <c r="D74" t="n">
-        <v>5151630</v>
+        <v>5183363</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>28823</v>
+        <v>28844</v>
       </c>
       <c r="D76" t="n">
-        <v>44573604</v>
+        <v>44630124</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11942</v>
+        <v>11966</v>
       </c>
       <c r="D80" t="n">
-        <v>31821555</v>
+        <v>31940052</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>54360</v>
+        <v>64360</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8095</v>
+        <v>8113</v>
       </c>
       <c r="D82" t="n">
-        <v>19853112</v>
+        <v>19944131</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D85" t="n">
-        <v>996098</v>
+        <v>1000132</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>201598</v>
+        <v>201948</v>
       </c>
       <c r="D86" t="n">
-        <v>305127766</v>
+        <v>305942269</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="D90" t="n">
-        <v>2112117</v>
+        <v>2117774</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D91" t="n">
-        <v>52853</v>
+        <v>53852</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>94786</v>
+        <v>94963</v>
       </c>
       <c r="D92" t="n">
-        <v>224070573</v>
+        <v>224743764</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44853</v>
+        <v>44950</v>
       </c>
       <c r="D95" t="n">
-        <v>102697147</v>
+        <v>103113227</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D97" t="n">
-        <v>280034</v>
+        <v>281534</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7275</v>
+        <v>7339</v>
       </c>
       <c r="D98" t="n">
-        <v>27541302</v>
+        <v>27724507</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4749</v>
+        <v>4769</v>
       </c>
       <c r="D100" t="n">
-        <v>9634911</v>
+        <v>9699285</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>44646</v>
+        <v>44706</v>
       </c>
       <c r="D102" t="n">
-        <v>66359480</v>
+        <v>66498231</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>10852</v>
+        <v>10870</v>
       </c>
       <c r="D106" t="n">
-        <v>18880583</v>
+        <v>18968334</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>10163</v>
+        <v>10176</v>
       </c>
       <c r="D108" t="n">
-        <v>16933245</v>
+        <v>16992399</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>18648</v>
+        <v>18661</v>
       </c>
       <c r="D112" t="n">
-        <v>38146477</v>
+        <v>38177287</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4188</v>
+        <v>4190</v>
       </c>
       <c r="D115" t="n">
-        <v>9152634</v>
+        <v>9157134</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6078</v>
+        <v>6083</v>
       </c>
       <c r="D117" t="n">
-        <v>13721950</v>
+        <v>13730950</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>201369</v>
+        <v>201688</v>
       </c>
       <c r="D122" t="n">
-        <v>293589909</v>
+        <v>294195230</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D123" t="n">
-        <v>85060</v>
+        <v>87813</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1630</v>
+        <v>1637</v>
       </c>
       <c r="D128" t="n">
-        <v>4558565</v>
+        <v>4579279</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>78823</v>
+        <v>78979</v>
       </c>
       <c r="D130" t="n">
-        <v>187549044</v>
+        <v>188268229</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D131" t="n">
-        <v>684182</v>
+        <v>694182</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>42317</v>
+        <v>42413</v>
       </c>
       <c r="D133" t="n">
-        <v>96888140</v>
+        <v>97332975</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1835</v>
+        <v>1846</v>
       </c>
       <c r="D136" t="n">
-        <v>3740600</v>
+        <v>3780460</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3947</v>
+        <v>3961</v>
       </c>
       <c r="D140" t="n">
-        <v>8105217</v>
+        <v>8134997</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>805159</v>
+        <v>806347</v>
       </c>
       <c r="D142" t="n">
-        <v>1286093512</v>
+        <v>1288770553</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>2814</v>
+        <v>2828</v>
       </c>
       <c r="D147" t="n">
-        <v>9840431</v>
+        <v>9942002</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>326504</v>
+        <v>327305</v>
       </c>
       <c r="D149" t="n">
-        <v>788797478</v>
+        <v>792478746</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6044,10 +6044,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1097</v>
+        <v>1103</v>
       </c>
       <c r="D150" t="n">
-        <v>4809104</v>
+        <v>4852104</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>302922</v>
+        <v>303598</v>
       </c>
       <c r="D152" t="n">
-        <v>686201697</v>
+        <v>688853702</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3858</v>
+        <v>3866</v>
       </c>
       <c r="D155" t="n">
-        <v>6514918</v>
+        <v>6531082</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>12024</v>
+        <v>12070</v>
       </c>
       <c r="D158" t="n">
-        <v>25352020</v>
+        <v>25545550</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>54980</v>
+        <v>55027</v>
       </c>
       <c r="D161" t="n">
-        <v>76486671</v>
+        <v>76563928</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6690,10 +6690,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>16518</v>
+        <v>16525</v>
       </c>
       <c r="D167" t="n">
-        <v>26763496</v>
+        <v>26794546</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>4573</v>
+        <v>4580</v>
       </c>
       <c r="D169" t="n">
-        <v>7250554</v>
+        <v>7320554</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -6994,10 +6994,10 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>24784</v>
+        <v>24813</v>
       </c>
       <c r="D175" t="n">
-        <v>37015452</v>
+        <v>37061954</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -7146,10 +7146,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>10419</v>
+        <v>10426</v>
       </c>
       <c r="D179" t="n">
-        <v>21406803</v>
+        <v>21450148</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -7222,10 +7222,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>7327</v>
+        <v>7331</v>
       </c>
       <c r="D181" t="n">
-        <v>13894514</v>
+        <v>13909730</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -7336,10 +7336,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D184" t="n">
-        <v>802837</v>
+        <v>812837</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>33483</v>
+        <v>33529</v>
       </c>
       <c r="D186" t="n">
-        <v>81678710</v>
+        <v>81892829</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>124100</v>
+        <v>124237</v>
       </c>
       <c r="D193" t="n">
-        <v>186077918</v>
+        <v>186302967</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -7906,10 +7906,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>1179</v>
+        <v>1183</v>
       </c>
       <c r="D199" t="n">
-        <v>3572341</v>
+        <v>3591053</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7982,10 +7982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>51516</v>
+        <v>51589</v>
       </c>
       <c r="D201" t="n">
-        <v>127033589</v>
+        <v>127351624</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -8058,10 +8058,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>20371</v>
+        <v>20414</v>
       </c>
       <c r="D203" t="n">
-        <v>48275232</v>
+        <v>48433760</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -8134,10 +8134,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1598</v>
+        <v>1606</v>
       </c>
       <c r="D205" t="n">
-        <v>2768894</v>
+        <v>2806647</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2855</v>
+        <v>2861</v>
       </c>
       <c r="D208" t="n">
-        <v>5888660</v>
+        <v>5906761</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8324,10 +8324,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>328601</v>
+        <v>329076</v>
       </c>
       <c r="D210" t="n">
-        <v>473817336</v>
+        <v>474706029</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -8400,10 +8400,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D212" t="n">
-        <v>490223</v>
+        <v>493588</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D217" t="n">
-        <v>3796657</v>
+        <v>3804563</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -8666,10 +8666,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>127367</v>
+        <v>127556</v>
       </c>
       <c r="D219" t="n">
-        <v>299889658</v>
+        <v>300624876</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -8704,10 +8704,10 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D220" t="n">
-        <v>687707</v>
+        <v>688706</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -8742,10 +8742,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D221" t="n">
-        <v>53332</v>
+        <v>63332</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -8780,10 +8780,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>50216</v>
+        <v>50313</v>
       </c>
       <c r="D222" t="n">
-        <v>114642338</v>
+        <v>115088924</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>6614</v>
+        <v>6637</v>
       </c>
       <c r="D225" t="n">
-        <v>12099267</v>
+        <v>12222419</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -9008,10 +9008,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>8252</v>
+        <v>8286</v>
       </c>
       <c r="D228" t="n">
-        <v>15904822</v>
+        <v>16011441</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -9122,10 +9122,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>372820</v>
+        <v>373372</v>
       </c>
       <c r="D231" t="n">
-        <v>527844260</v>
+        <v>528840476</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -9198,10 +9198,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D233" t="n">
-        <v>672767</v>
+        <v>684198</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -9464,10 +9464,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>141732</v>
+        <v>141969</v>
       </c>
       <c r="D240" t="n">
-        <v>332661823</v>
+        <v>333620170</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D241" t="n">
-        <v>780606</v>
+        <v>792439</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -9578,10 +9578,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>78535</v>
+        <v>78681</v>
       </c>
       <c r="D243" t="n">
-        <v>177957899</v>
+        <v>178600684</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -9692,10 +9692,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>6039</v>
+        <v>6050</v>
       </c>
       <c r="D246" t="n">
-        <v>10046699</v>
+        <v>10073618</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -9806,10 +9806,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D249" t="n">
-        <v>197022</v>
+        <v>198522</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -9844,10 +9844,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>10405</v>
+        <v>10458</v>
       </c>
       <c r="D250" t="n">
-        <v>20251612</v>
+        <v>20394533</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -9958,10 +9958,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>148506</v>
+        <v>148681</v>
       </c>
       <c r="D253" t="n">
-        <v>219513962</v>
+        <v>219873282</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -10186,10 +10186,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>1046</v>
+        <v>1054</v>
       </c>
       <c r="D259" t="n">
-        <v>3045586</v>
+        <v>3083395</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -10262,10 +10262,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>73752</v>
+        <v>73822</v>
       </c>
       <c r="D261" t="n">
-        <v>177153531</v>
+        <v>177491783</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -10376,10 +10376,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>19456</v>
+        <v>19481</v>
       </c>
       <c r="D264" t="n">
-        <v>44901083</v>
+        <v>45015251</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -10452,10 +10452,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>2397</v>
+        <v>2407</v>
       </c>
       <c r="D266" t="n">
-        <v>4386023</v>
+        <v>4428091</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -10528,10 +10528,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>4114</v>
+        <v>4126</v>
       </c>
       <c r="D268" t="n">
-        <v>8310781</v>
+        <v>8350140</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -10566,10 +10566,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>373825</v>
+        <v>374375</v>
       </c>
       <c r="D269" t="n">
-        <v>546796016</v>
+        <v>547839253</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -10642,10 +10642,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D271" t="n">
-        <v>807312</v>
+        <v>813870</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -10832,10 +10832,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>1596</v>
+        <v>1600</v>
       </c>
       <c r="D276" t="n">
-        <v>5007866</v>
+        <v>5027305</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -10908,10 +10908,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>147839</v>
+        <v>148078</v>
       </c>
       <c r="D278" t="n">
-        <v>360532682</v>
+        <v>361530919</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -10984,10 +10984,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D280" t="n">
-        <v>80505</v>
+        <v>87065</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -11022,10 +11022,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>104741</v>
+        <v>104940</v>
       </c>
       <c r="D281" t="n">
-        <v>244480512</v>
+        <v>245217315</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -11098,10 +11098,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D283" t="n">
-        <v>23500</v>
+        <v>26500</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -11136,10 +11136,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>3309</v>
+        <v>3319</v>
       </c>
       <c r="D284" t="n">
-        <v>5745668</v>
+        <v>5772451</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -11250,10 +11250,10 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>8528</v>
+        <v>8558</v>
       </c>
       <c r="D287" t="n">
-        <v>17531275</v>
+        <v>17647194</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-14 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -425,13 +425,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>501459</v>
+        <v>504271</v>
       </c>
       <c r="D2" t="n">
-        <v>150523</v>
+        <v>150682</v>
       </c>
       <c r="E2" t="n">
-        <v>776404164</v>
+        <v>783068210</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D3" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" t="n">
-        <v>637158</v>
+        <v>640423</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D4" t="n">
         <v>161</v>
       </c>
       <c r="E4" t="n">
-        <v>1569235</v>
+        <v>1587302</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1842</v>
+        <v>1864</v>
       </c>
       <c r="D8" t="n">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="E8" t="n">
-        <v>7077528</v>
+        <v>7197164</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9" t="n">
         <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>303223</v>
+        <v>323223</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>198196</v>
+        <v>199693</v>
       </c>
       <c r="D10" t="n">
-        <v>60977</v>
+        <v>61119</v>
       </c>
       <c r="E10" t="n">
-        <v>585495029</v>
+        <v>593435703</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="D11" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E11" t="n">
-        <v>3344179</v>
+        <v>3388511</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>149572</v>
+        <v>170238</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>104187</v>
+        <v>104855</v>
       </c>
       <c r="D13" t="n">
-        <v>30754</v>
+        <v>30842</v>
       </c>
       <c r="E13" t="n">
-        <v>305810419</v>
+        <v>309302023</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5750</v>
+        <v>5786</v>
       </c>
       <c r="D15" t="n">
-        <v>2536</v>
+        <v>2540</v>
       </c>
       <c r="E15" t="n">
-        <v>10555286</v>
+        <v>10663147</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -999,13 +999,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D16" t="n">
         <v>61</v>
       </c>
       <c r="E16" t="n">
-        <v>853883</v>
+        <v>860126</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>13550</v>
+        <v>13647</v>
       </c>
       <c r="D17" t="n">
-        <v>3601</v>
+        <v>3611</v>
       </c>
       <c r="E17" t="n">
-        <v>32904461</v>
+        <v>33257408</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>118465</v>
+        <v>119133</v>
       </c>
       <c r="D19" t="n">
-        <v>36853</v>
+        <v>36901</v>
       </c>
       <c r="E19" t="n">
-        <v>181707815</v>
+        <v>183417352</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1163,13 +1163,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D20" t="n">
         <v>22</v>
       </c>
       <c r="E20" t="n">
-        <v>157221</v>
+        <v>161101</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1204,13 +1204,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D21" t="n">
         <v>22</v>
       </c>
       <c r="E21" t="n">
-        <v>121755</v>
+        <v>127198</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1327,13 +1327,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="D24" t="n">
         <v>157</v>
       </c>
       <c r="E24" t="n">
-        <v>1834130</v>
+        <v>1867387</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>53253</v>
+        <v>53645</v>
       </c>
       <c r="D25" t="n">
-        <v>16771</v>
+        <v>16824</v>
       </c>
       <c r="E25" t="n">
-        <v>153249300</v>
+        <v>155345711</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1409,13 +1409,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D26" t="n">
         <v>46</v>
       </c>
       <c r="E26" t="n">
-        <v>1007840</v>
+        <v>1010840</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1491,13 +1491,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19811</v>
+        <v>19961</v>
       </c>
       <c r="D28" t="n">
-        <v>6084</v>
+        <v>6101</v>
       </c>
       <c r="E28" t="n">
-        <v>56738232</v>
+        <v>57527506</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1573,13 +1573,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2325</v>
+        <v>2345</v>
       </c>
       <c r="D30" t="n">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="E30" t="n">
-        <v>4683311</v>
+        <v>4738040</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1655,13 +1655,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3489</v>
+        <v>3522</v>
       </c>
       <c r="D32" t="n">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E32" t="n">
-        <v>8215534</v>
+        <v>8353762</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1696,13 +1696,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>144422</v>
+        <v>145178</v>
       </c>
       <c r="D33" t="n">
-        <v>46927</v>
+        <v>46994</v>
       </c>
       <c r="E33" t="n">
-        <v>226136568</v>
+        <v>228013611</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1737,13 +1737,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D34" t="n">
         <v>31</v>
       </c>
       <c r="E34" t="n">
-        <v>117071</v>
+        <v>127071</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1819,13 +1819,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2119</v>
+        <v>2136</v>
       </c>
       <c r="D36" t="n">
         <v>591</v>
       </c>
       <c r="E36" t="n">
-        <v>8665577</v>
+        <v>8770871</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1901,13 +1901,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>74393</v>
+        <v>74942</v>
       </c>
       <c r="D38" t="n">
-        <v>23328</v>
+        <v>23384</v>
       </c>
       <c r="E38" t="n">
-        <v>222423554</v>
+        <v>225377854</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1942,13 +1942,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D39" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E39" t="n">
-        <v>830852</v>
+        <v>863541</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1983,13 +1983,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E40" t="n">
-        <v>37500</v>
+        <v>39000</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2024,13 +2024,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>16155</v>
+        <v>16256</v>
       </c>
       <c r="D41" t="n">
-        <v>5112</v>
+        <v>5130</v>
       </c>
       <c r="E41" t="n">
-        <v>50376297</v>
+        <v>50902601</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2106,13 +2106,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1922</v>
+        <v>1936</v>
       </c>
       <c r="D43" t="n">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="E43" t="n">
-        <v>3465544</v>
+        <v>3522898</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2147,13 +2147,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4393</v>
+        <v>4421</v>
       </c>
       <c r="D44" t="n">
-        <v>1226</v>
+        <v>1231</v>
       </c>
       <c r="E44" t="n">
-        <v>10825371</v>
+        <v>10954548</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2188,13 +2188,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>104116</v>
+        <v>104614</v>
       </c>
       <c r="D45" t="n">
-        <v>32644</v>
+        <v>32676</v>
       </c>
       <c r="E45" t="n">
-        <v>161296596</v>
+        <v>162687263</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2270,13 +2270,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D47" t="n">
         <v>19</v>
       </c>
       <c r="E47" t="n">
-        <v>179477</v>
+        <v>188737</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2352,13 +2352,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>762</v>
+        <v>769</v>
       </c>
       <c r="D49" t="n">
         <v>234</v>
       </c>
       <c r="E49" t="n">
-        <v>2718973</v>
+        <v>2750137</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2393,13 +2393,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>45687</v>
+        <v>45971</v>
       </c>
       <c r="D50" t="n">
-        <v>14367</v>
+        <v>14389</v>
       </c>
       <c r="E50" t="n">
-        <v>127215675</v>
+        <v>128874362</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2434,13 +2434,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D51" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E51" t="n">
-        <v>652907</v>
+        <v>673573</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2516,13 +2516,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>18575</v>
+        <v>18681</v>
       </c>
       <c r="D53" t="n">
-        <v>5607</v>
+        <v>5624</v>
       </c>
       <c r="E53" t="n">
-        <v>50747230</v>
+        <v>51246795</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2557,13 +2557,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1957</v>
+        <v>1967</v>
       </c>
       <c r="D54" t="n">
         <v>776</v>
       </c>
       <c r="E54" t="n">
-        <v>3788058</v>
+        <v>3821300</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2639,13 +2639,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2905</v>
+        <v>2925</v>
       </c>
       <c r="D56" t="n">
-        <v>842</v>
+        <v>848</v>
       </c>
       <c r="E56" t="n">
-        <v>6733716</v>
+        <v>6840921</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2721,13 +2721,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>31432</v>
+        <v>31561</v>
       </c>
       <c r="D58" t="n">
-        <v>9197</v>
+        <v>9204</v>
       </c>
       <c r="E58" t="n">
-        <v>51920671</v>
+        <v>52315737</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2885,13 +2885,13 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>13791</v>
+        <v>13914</v>
       </c>
       <c r="D62" t="n">
-        <v>3986</v>
+        <v>4002</v>
       </c>
       <c r="E62" t="n">
-        <v>46636551</v>
+        <v>47360205</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2967,13 +2967,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>9187</v>
+        <v>9252</v>
       </c>
       <c r="D64" t="n">
-        <v>2641</v>
+        <v>2652</v>
       </c>
       <c r="E64" t="n">
-        <v>27962015</v>
+        <v>28309900</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -3008,13 +3008,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="D65" t="n">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E65" t="n">
-        <v>1467844</v>
+        <v>1473800</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -3049,13 +3049,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D66" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E66" t="n">
-        <v>1212558</v>
+        <v>1223686</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -3090,13 +3090,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>218433</v>
+        <v>219905</v>
       </c>
       <c r="D67" t="n">
-        <v>68811</v>
+        <v>69054</v>
       </c>
       <c r="E67" t="n">
-        <v>346955065</v>
+        <v>351192233</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -3131,13 +3131,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D68" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E68" t="n">
-        <v>661420</v>
+        <v>717874</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -3172,13 +3172,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D69" t="n">
         <v>44</v>
       </c>
       <c r="E69" t="n">
-        <v>389847</v>
+        <v>392847</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -3254,13 +3254,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>941</v>
+        <v>957</v>
       </c>
       <c r="D71" t="n">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E71" t="n">
-        <v>3329297</v>
+        <v>3418356</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -3336,13 +3336,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>104370</v>
+        <v>105313</v>
       </c>
       <c r="D73" t="n">
-        <v>33095</v>
+        <v>33216</v>
       </c>
       <c r="E73" t="n">
-        <v>297248024</v>
+        <v>302252012</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -3377,13 +3377,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D74" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E74" t="n">
-        <v>2472039</v>
+        <v>2500725</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -3418,13 +3418,13 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D75" t="n">
         <v>15</v>
       </c>
       <c r="E75" t="n">
-        <v>235241</v>
+        <v>245241</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -3459,13 +3459,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>49868</v>
+        <v>50288</v>
       </c>
       <c r="D76" t="n">
-        <v>15463</v>
+        <v>15518</v>
       </c>
       <c r="E76" t="n">
-        <v>142306770</v>
+        <v>144568628</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -3500,13 +3500,13 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D77" t="n">
         <v>19</v>
       </c>
       <c r="E77" t="n">
-        <v>56302</v>
+        <v>57940</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -3541,13 +3541,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D78" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E78" t="n">
-        <v>622648</v>
+        <v>635648</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -3582,13 +3582,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>9195</v>
+        <v>9503</v>
       </c>
       <c r="D79" t="n">
-        <v>5104</v>
+        <v>5275</v>
       </c>
       <c r="E79" t="n">
-        <v>36108223</v>
+        <v>37989222</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -3623,13 +3623,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5413</v>
+        <v>5462</v>
       </c>
       <c r="D80" t="n">
-        <v>1487</v>
+        <v>1491</v>
       </c>
       <c r="E80" t="n">
-        <v>13264581</v>
+        <v>13480359</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -3664,13 +3664,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>46871</v>
+        <v>47046</v>
       </c>
       <c r="D81" t="n">
-        <v>11933</v>
+        <v>11939</v>
       </c>
       <c r="E81" t="n">
-        <v>71543154</v>
+        <v>71847263</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -3787,13 +3787,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>11256</v>
+        <v>11295</v>
       </c>
       <c r="D84" t="n">
-        <v>3154</v>
+        <v>3157</v>
       </c>
       <c r="E84" t="n">
-        <v>21182834</v>
+        <v>21342527</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -3869,13 +3869,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>10554</v>
+        <v>10582</v>
       </c>
       <c r="D86" t="n">
         <v>2652</v>
       </c>
       <c r="E86" t="n">
-        <v>18580453</v>
+        <v>18702087</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -3951,13 +3951,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D88" t="n">
         <v>188</v>
       </c>
       <c r="E88" t="n">
-        <v>1161593</v>
+        <v>1163093</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3992,13 +3992,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>19280</v>
+        <v>19306</v>
       </c>
       <c r="D89" t="n">
-        <v>3634</v>
+        <v>3636</v>
       </c>
       <c r="E89" t="n">
-        <v>39585066</v>
+        <v>39659369</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -4033,13 +4033,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4346</v>
+        <v>4350</v>
       </c>
       <c r="D90" t="n">
         <v>882</v>
       </c>
       <c r="E90" t="n">
-        <v>9847977</v>
+        <v>9871477</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -4115,13 +4115,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6285</v>
+        <v>6291</v>
       </c>
       <c r="D92" t="n">
         <v>1217</v>
       </c>
       <c r="E92" t="n">
-        <v>14341479</v>
+        <v>14350479</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -4279,13 +4279,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>216291</v>
+        <v>217296</v>
       </c>
       <c r="D96" t="n">
-        <v>66105</v>
+        <v>66197</v>
       </c>
       <c r="E96" t="n">
-        <v>327471684</v>
+        <v>330021675</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -4484,13 +4484,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2009</v>
+        <v>2035</v>
       </c>
       <c r="D101" t="n">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E101" t="n">
-        <v>7188620</v>
+        <v>7377137</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -4566,13 +4566,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>86168</v>
+        <v>86676</v>
       </c>
       <c r="D103" t="n">
-        <v>26704</v>
+        <v>26758</v>
       </c>
       <c r="E103" t="n">
-        <v>241065476</v>
+        <v>243727921</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -4607,13 +4607,13 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D104" t="n">
         <v>90</v>
       </c>
       <c r="E104" t="n">
-        <v>1770324</v>
+        <v>1800324</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -4648,13 +4648,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D105" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E105" t="n">
-        <v>157690</v>
+        <v>159190</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -4689,13 +4689,13 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>46625</v>
+        <v>46929</v>
       </c>
       <c r="D106" t="n">
-        <v>13485</v>
+        <v>13517</v>
       </c>
       <c r="E106" t="n">
-        <v>128519964</v>
+        <v>129846223</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -4771,13 +4771,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2158</v>
+        <v>2184</v>
       </c>
       <c r="D108" t="n">
-        <v>914</v>
+        <v>922</v>
       </c>
       <c r="E108" t="n">
-        <v>4852822</v>
+        <v>5022860</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -4812,13 +4812,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4418</v>
+        <v>4452</v>
       </c>
       <c r="D109" t="n">
-        <v>1233</v>
+        <v>1236</v>
       </c>
       <c r="E109" t="n">
-        <v>10419243</v>
+        <v>10543033</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -4853,13 +4853,13 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D110" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E110" t="n">
-        <v>29766</v>
+        <v>31266</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -4894,13 +4894,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>865230</v>
+        <v>868807</v>
       </c>
       <c r="D111" t="n">
-        <v>213404</v>
+        <v>213575</v>
       </c>
       <c r="E111" t="n">
-        <v>1416773466</v>
+        <v>1425199155</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -4935,13 +4935,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D112" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E112" t="n">
-        <v>318271</v>
+        <v>321271</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -4976,13 +4976,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E113" t="n">
-        <v>1232643</v>
+        <v>1282075</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -5099,13 +5099,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>3557</v>
+        <v>3593</v>
       </c>
       <c r="D116" t="n">
-        <v>1120</v>
+        <v>1126</v>
       </c>
       <c r="E116" t="n">
-        <v>19803599</v>
+        <v>20081093</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -5181,13 +5181,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>359473</v>
+        <v>361639</v>
       </c>
       <c r="D118" t="n">
-        <v>99554</v>
+        <v>99777</v>
       </c>
       <c r="E118" t="n">
-        <v>1033426638</v>
+        <v>1045141026</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -5222,13 +5222,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1369</v>
+        <v>1387</v>
       </c>
       <c r="D119" t="n">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="E119" t="n">
-        <v>10925327</v>
+        <v>11070378</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -5263,13 +5263,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D120" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E120" t="n">
-        <v>1485177</v>
+        <v>1521904</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -5304,13 +5304,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>332478</v>
+        <v>334269</v>
       </c>
       <c r="D121" t="n">
-        <v>83867</v>
+        <v>84052</v>
       </c>
       <c r="E121" t="n">
-        <v>897523841</v>
+        <v>906401896</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -5386,13 +5386,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>4285</v>
+        <v>4306</v>
       </c>
       <c r="D123" t="n">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="E123" t="n">
-        <v>7542312</v>
+        <v>7585283</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
@@ -5468,13 +5468,13 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>13527</v>
+        <v>13619</v>
       </c>
       <c r="D125" t="n">
-        <v>3609</v>
+        <v>3619</v>
       </c>
       <c r="E125" t="n">
-        <v>33162717</v>
+        <v>33545110</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -5591,13 +5591,13 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>56898</v>
+        <v>57013</v>
       </c>
       <c r="D128" t="n">
-        <v>17195</v>
+        <v>17198</v>
       </c>
       <c r="E128" t="n">
-        <v>80000762</v>
+        <v>80252010</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>16959</v>
+        <v>16987</v>
       </c>
       <c r="D132" t="n">
-        <v>5875</v>
+        <v>5876</v>
       </c>
       <c r="E132" t="n">
-        <v>29636137</v>
+        <v>29771406</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -5837,13 +5837,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>4716</v>
+        <v>4728</v>
       </c>
       <c r="D134" t="n">
         <v>1516</v>
       </c>
       <c r="E134" t="n">
-        <v>7917466</v>
+        <v>7942309</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -6001,13 +6001,13 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D138" t="n">
         <v>164</v>
       </c>
       <c r="E138" t="n">
-        <v>1014739</v>
+        <v>1026239</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -6042,13 +6042,13 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>26048</v>
+        <v>26141</v>
       </c>
       <c r="D139" t="n">
-        <v>6972</v>
+        <v>6973</v>
       </c>
       <c r="E139" t="n">
-        <v>39481249</v>
+        <v>39787170</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -6165,13 +6165,13 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>10871</v>
+        <v>10913</v>
       </c>
       <c r="D142" t="n">
-        <v>3100</v>
+        <v>3107</v>
       </c>
       <c r="E142" t="n">
-        <v>23976013</v>
+        <v>24163657</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -6247,13 +6247,13 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>7699</v>
+        <v>7730</v>
       </c>
       <c r="D144" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="E144" t="n">
-        <v>15476601</v>
+        <v>15601193</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>34823</v>
+        <v>34917</v>
       </c>
       <c r="D147" t="n">
-        <v>5350</v>
+        <v>5351</v>
       </c>
       <c r="E147" t="n">
-        <v>86239238</v>
+        <v>86717999</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -6411,13 +6411,13 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3360</v>
+        <v>3368</v>
       </c>
       <c r="D148" t="n">
         <v>657</v>
       </c>
       <c r="E148" t="n">
-        <v>8155229</v>
+        <v>8207403</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -6452,13 +6452,13 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D149" t="n">
         <v>86</v>
       </c>
       <c r="E149" t="n">
-        <v>1084152</v>
+        <v>1104152</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -6575,13 +6575,13 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>133162</v>
+        <v>134027</v>
       </c>
       <c r="D152" t="n">
-        <v>41450</v>
+        <v>41522</v>
       </c>
       <c r="E152" t="n">
-        <v>209412481</v>
+        <v>211850518</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -6616,13 +6616,13 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D153" t="n">
         <v>15</v>
       </c>
       <c r="E153" t="n">
-        <v>79574</v>
+        <v>87569</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -6739,13 +6739,13 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1482</v>
+        <v>1497</v>
       </c>
       <c r="D156" t="n">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E156" t="n">
-        <v>6013800</v>
+        <v>6111805</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -6821,13 +6821,13 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>56466</v>
+        <v>56915</v>
       </c>
       <c r="D158" t="n">
-        <v>17614</v>
+        <v>17659</v>
       </c>
       <c r="E158" t="n">
-        <v>165785957</v>
+        <v>168437669</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -6862,13 +6862,13 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D159" t="n">
         <v>31</v>
       </c>
       <c r="E159" t="n">
-        <v>666540</v>
+        <v>668040</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -6903,13 +6903,13 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>22621</v>
+        <v>22782</v>
       </c>
       <c r="D160" t="n">
-        <v>6696</v>
+        <v>6719</v>
       </c>
       <c r="E160" t="n">
-        <v>66756757</v>
+        <v>67583142</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -6985,13 +6985,13 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1735</v>
+        <v>1745</v>
       </c>
       <c r="D162" t="n">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E162" t="n">
-        <v>3243861</v>
+        <v>3283476</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -7026,13 +7026,13 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3283</v>
+        <v>3307</v>
       </c>
       <c r="D163" t="n">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="E163" t="n">
-        <v>7782998</v>
+        <v>7846279</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -7067,13 +7067,13 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>354045</v>
+        <v>355649</v>
       </c>
       <c r="D164" t="n">
-        <v>111793</v>
+        <v>111901</v>
       </c>
       <c r="E164" t="n">
-        <v>528548497</v>
+        <v>532470811</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -7313,13 +7313,13 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1714</v>
+        <v>1721</v>
       </c>
       <c r="D170" t="n">
         <v>515</v>
       </c>
       <c r="E170" t="n">
-        <v>5995872</v>
+        <v>6022469</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -7395,13 +7395,13 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>140144</v>
+        <v>141048</v>
       </c>
       <c r="D172" t="n">
-        <v>44407</v>
+        <v>44497</v>
       </c>
       <c r="E172" t="n">
-        <v>397471021</v>
+        <v>402528775</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
@@ -7436,13 +7436,13 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D173" t="n">
         <v>93</v>
       </c>
       <c r="E173" t="n">
-        <v>1758850</v>
+        <v>1774829</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -7518,13 +7518,13 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>56074</v>
+        <v>56428</v>
       </c>
       <c r="D175" t="n">
-        <v>17004</v>
+        <v>17054</v>
       </c>
       <c r="E175" t="n">
-        <v>158846229</v>
+        <v>160583955</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -7641,13 +7641,13 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>7415</v>
+        <v>7459</v>
       </c>
       <c r="D178" t="n">
-        <v>3096</v>
+        <v>3106</v>
       </c>
       <c r="E178" t="n">
-        <v>15271470</v>
+        <v>15452244</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -7723,13 +7723,13 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>9298</v>
+        <v>9370</v>
       </c>
       <c r="D180" t="n">
-        <v>2569</v>
+        <v>2575</v>
       </c>
       <c r="E180" t="n">
-        <v>20733120</v>
+        <v>21028323</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -7805,13 +7805,13 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>403571</v>
+        <v>405754</v>
       </c>
       <c r="D182" t="n">
-        <v>123321</v>
+        <v>123480</v>
       </c>
       <c r="E182" t="n">
-        <v>589586785</v>
+        <v>594234809</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -7846,13 +7846,13 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D183" t="n">
         <v>70</v>
       </c>
       <c r="E183" t="n">
-        <v>352422</v>
+        <v>353505</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -7887,13 +7887,13 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D184" t="n">
         <v>127</v>
       </c>
       <c r="E184" t="n">
-        <v>856798</v>
+        <v>879852</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -8051,13 +8051,13 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1131</v>
+        <v>1148</v>
       </c>
       <c r="D188" t="n">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E188" t="n">
-        <v>3895338</v>
+        <v>4001936</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -8133,13 +8133,13 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>156851</v>
+        <v>157943</v>
       </c>
       <c r="D190" t="n">
-        <v>47764</v>
+        <v>47848</v>
       </c>
       <c r="E190" t="n">
-        <v>439357731</v>
+        <v>445094762</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -8174,13 +8174,13 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="D191" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E191" t="n">
-        <v>1922450</v>
+        <v>1976116</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -8256,13 +8256,13 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>87646</v>
+        <v>88195</v>
       </c>
       <c r="D193" t="n">
-        <v>25454</v>
+        <v>25505</v>
       </c>
       <c r="E193" t="n">
-        <v>237547522</v>
+        <v>240352966</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -8297,13 +8297,13 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D194" t="n">
         <v>17</v>
       </c>
       <c r="E194" t="n">
-        <v>160861</v>
+        <v>170861</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -8379,13 +8379,13 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>6723</v>
+        <v>6754</v>
       </c>
       <c r="D196" t="n">
-        <v>2697</v>
+        <v>2701</v>
       </c>
       <c r="E196" t="n">
-        <v>12181835</v>
+        <v>12275837</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -8461,13 +8461,13 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D198" t="n">
         <v>24</v>
       </c>
       <c r="E198" t="n">
-        <v>241522</v>
+        <v>251522</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -8502,13 +8502,13 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>11782</v>
+        <v>11878</v>
       </c>
       <c r="D199" t="n">
-        <v>3075</v>
+        <v>3083</v>
       </c>
       <c r="E199" t="n">
-        <v>26216025</v>
+        <v>26607254</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -8584,13 +8584,13 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>159178</v>
+        <v>160003</v>
       </c>
       <c r="D201" t="n">
-        <v>51021</v>
+        <v>51091</v>
       </c>
       <c r="E201" t="n">
-        <v>244421066</v>
+        <v>246363024</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -8748,13 +8748,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1331</v>
+        <v>1347</v>
       </c>
       <c r="D205" t="n">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E205" t="n">
-        <v>5518764</v>
+        <v>5607052</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -8789,13 +8789,13 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>80763</v>
+        <v>81352</v>
       </c>
       <c r="D206" t="n">
-        <v>26167</v>
+        <v>26238</v>
       </c>
       <c r="E206" t="n">
-        <v>232791795</v>
+        <v>236077599</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -8830,13 +8830,13 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D207" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E207" t="n">
-        <v>961035</v>
+        <v>981701</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -8912,13 +8912,13 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>21747</v>
+        <v>21885</v>
       </c>
       <c r="D209" t="n">
-        <v>6645</v>
+        <v>6673</v>
       </c>
       <c r="E209" t="n">
-        <v>65158994</v>
+        <v>65869339</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -8994,13 +8994,13 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>2620</v>
+        <v>2632</v>
       </c>
       <c r="D211" t="n">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="E211" t="n">
-        <v>5257450</v>
+        <v>5286908</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -9076,13 +9076,13 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>4685</v>
+        <v>4718</v>
       </c>
       <c r="D213" t="n">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="E213" t="n">
-        <v>11272080</v>
+        <v>11392939</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -9117,13 +9117,13 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>406365</v>
+        <v>408505</v>
       </c>
       <c r="D214" t="n">
-        <v>117438</v>
+        <v>117592</v>
       </c>
       <c r="E214" t="n">
-        <v>613655013</v>
+        <v>618228838</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>
@@ -9158,13 +9158,13 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D215" t="n">
         <v>81</v>
       </c>
       <c r="E215" t="n">
-        <v>464594</v>
+        <v>467731</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>
@@ -9199,13 +9199,13 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D216" t="n">
         <v>126</v>
       </c>
       <c r="E216" t="n">
-        <v>1052683</v>
+        <v>1071639</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -9240,13 +9240,13 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D217" t="n">
         <v>11</v>
       </c>
       <c r="E217" t="n">
-        <v>127553</v>
+        <v>137553</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
@@ -9363,13 +9363,13 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>1910</v>
+        <v>1920</v>
       </c>
       <c r="D220" t="n">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E220" t="n">
-        <v>8030162</v>
+        <v>8076944</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -9445,13 +9445,13 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>163629</v>
+        <v>164712</v>
       </c>
       <c r="D222" t="n">
-        <v>47696</v>
+        <v>47804</v>
       </c>
       <c r="E222" t="n">
-        <v>474209494</v>
+        <v>479925068</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
@@ -9486,13 +9486,13 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D223" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E223" t="n">
-        <v>1665995</v>
+        <v>1710209</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -9568,13 +9568,13 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>116514</v>
+        <v>117264</v>
       </c>
       <c r="D225" t="n">
-        <v>31929</v>
+        <v>32020</v>
       </c>
       <c r="E225" t="n">
-        <v>325312192</v>
+        <v>328944793</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
@@ -9691,13 +9691,13 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>3734</v>
+        <v>3755</v>
       </c>
       <c r="D228" t="n">
-        <v>1421</v>
+        <v>1423</v>
       </c>
       <c r="E228" t="n">
-        <v>6992030</v>
+        <v>7108596</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -9814,13 +9814,13 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>9530</v>
+        <v>9590</v>
       </c>
       <c r="D231" t="n">
-        <v>2415</v>
+        <v>2421</v>
       </c>
       <c r="E231" t="n">
-        <v>22208463</v>
+        <v>22456566</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-16 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -425,13 +425,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>504271</v>
+        <v>505810</v>
       </c>
       <c r="D2" t="n">
-        <v>150682</v>
+        <v>150810</v>
       </c>
       <c r="E2" t="n">
-        <v>783068210</v>
+        <v>786524177</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="D4" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E4" t="n">
-        <v>1587302</v>
+        <v>1597794</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1864</v>
+        <v>1877</v>
       </c>
       <c r="D8" t="n">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E8" t="n">
-        <v>7197164</v>
+        <v>7268424</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>199693</v>
+        <v>200425</v>
       </c>
       <c r="D10" t="n">
-        <v>61119</v>
+        <v>61191</v>
       </c>
       <c r="E10" t="n">
-        <v>593435703</v>
+        <v>597645007</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D11" t="n">
         <v>171</v>
       </c>
       <c r="E11" t="n">
-        <v>3388511</v>
+        <v>3401511</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>104855</v>
+        <v>105238</v>
       </c>
       <c r="D13" t="n">
-        <v>30842</v>
+        <v>30893</v>
       </c>
       <c r="E13" t="n">
-        <v>309302023</v>
+        <v>311138520</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -917,13 +917,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" t="n">
         <v>26</v>
       </c>
       <c r="E14" t="n">
-        <v>148693</v>
+        <v>149993</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5786</v>
+        <v>5820</v>
       </c>
       <c r="D15" t="n">
-        <v>2540</v>
+        <v>2546</v>
       </c>
       <c r="E15" t="n">
-        <v>10663147</v>
+        <v>10774582</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>13647</v>
+        <v>13707</v>
       </c>
       <c r="D17" t="n">
-        <v>3611</v>
+        <v>3621</v>
       </c>
       <c r="E17" t="n">
-        <v>33257408</v>
+        <v>33491309</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>119133</v>
+        <v>119489</v>
       </c>
       <c r="D19" t="n">
-        <v>36901</v>
+        <v>36935</v>
       </c>
       <c r="E19" t="n">
-        <v>183417352</v>
+        <v>184273019</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1327,13 +1327,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="D24" t="n">
         <v>157</v>
       </c>
       <c r="E24" t="n">
-        <v>1867387</v>
+        <v>1874053</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>53645</v>
+        <v>53850</v>
       </c>
       <c r="D25" t="n">
-        <v>16824</v>
+        <v>16846</v>
       </c>
       <c r="E25" t="n">
-        <v>155345711</v>
+        <v>156448501</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1491,13 +1491,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19961</v>
+        <v>20050</v>
       </c>
       <c r="D28" t="n">
-        <v>6101</v>
+        <v>6112</v>
       </c>
       <c r="E28" t="n">
-        <v>57527506</v>
+        <v>57923319</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1573,13 +1573,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2345</v>
+        <v>2360</v>
       </c>
       <c r="D30" t="n">
-        <v>1018</v>
+        <v>1025</v>
       </c>
       <c r="E30" t="n">
-        <v>4738040</v>
+        <v>4771938</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1655,13 +1655,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3522</v>
+        <v>3541</v>
       </c>
       <c r="D32" t="n">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="E32" t="n">
-        <v>8353762</v>
+        <v>8446235</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1696,13 +1696,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>145178</v>
+        <v>145564</v>
       </c>
       <c r="D33" t="n">
-        <v>46994</v>
+        <v>47032</v>
       </c>
       <c r="E33" t="n">
-        <v>228013611</v>
+        <v>229025255</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1819,13 +1819,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2136</v>
+        <v>2149</v>
       </c>
       <c r="D36" t="n">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="E36" t="n">
-        <v>8770871</v>
+        <v>8853852</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1901,13 +1901,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>74942</v>
+        <v>75196</v>
       </c>
       <c r="D38" t="n">
-        <v>23384</v>
+        <v>23424</v>
       </c>
       <c r="E38" t="n">
-        <v>225377854</v>
+        <v>226873730</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2024,13 +2024,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>16256</v>
+        <v>16330</v>
       </c>
       <c r="D41" t="n">
-        <v>5130</v>
+        <v>5140</v>
       </c>
       <c r="E41" t="n">
-        <v>50902601</v>
+        <v>51300718</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2106,13 +2106,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1936</v>
+        <v>1944</v>
       </c>
       <c r="D43" t="n">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="E43" t="n">
-        <v>3522898</v>
+        <v>3543356</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2147,13 +2147,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4421</v>
+        <v>4438</v>
       </c>
       <c r="D44" t="n">
-        <v>1231</v>
+        <v>1236</v>
       </c>
       <c r="E44" t="n">
-        <v>10954548</v>
+        <v>11008638</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2188,13 +2188,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>104614</v>
+        <v>104903</v>
       </c>
       <c r="D45" t="n">
-        <v>32676</v>
+        <v>32703</v>
       </c>
       <c r="E45" t="n">
-        <v>162687263</v>
+        <v>163387842</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2352,13 +2352,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="D49" t="n">
         <v>234</v>
       </c>
       <c r="E49" t="n">
-        <v>2750137</v>
+        <v>2777280</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2393,13 +2393,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>45971</v>
+        <v>46128</v>
       </c>
       <c r="D50" t="n">
-        <v>14389</v>
+        <v>14401</v>
       </c>
       <c r="E50" t="n">
-        <v>128874362</v>
+        <v>129791908</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2516,13 +2516,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>18681</v>
+        <v>18775</v>
       </c>
       <c r="D53" t="n">
-        <v>5624</v>
+        <v>5642</v>
       </c>
       <c r="E53" t="n">
-        <v>51246795</v>
+        <v>51633557</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2557,13 +2557,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1967</v>
+        <v>1980</v>
       </c>
       <c r="D54" t="n">
         <v>776</v>
       </c>
       <c r="E54" t="n">
-        <v>3821300</v>
+        <v>3880436</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2639,13 +2639,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2925</v>
+        <v>2940</v>
       </c>
       <c r="D56" t="n">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="E56" t="n">
-        <v>6840921</v>
+        <v>6917228</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2721,13 +2721,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>31561</v>
+        <v>31681</v>
       </c>
       <c r="D58" t="n">
-        <v>9204</v>
+        <v>9207</v>
       </c>
       <c r="E58" t="n">
-        <v>52315737</v>
+        <v>52607053</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2844,13 +2844,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D61" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E61" t="n">
-        <v>344036</v>
+        <v>356700</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2885,13 +2885,13 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>13914</v>
+        <v>14002</v>
       </c>
       <c r="D62" t="n">
-        <v>4002</v>
+        <v>4009</v>
       </c>
       <c r="E62" t="n">
-        <v>47360205</v>
+        <v>47848639</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2967,13 +2967,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>9252</v>
+        <v>9292</v>
       </c>
       <c r="D64" t="n">
-        <v>2652</v>
+        <v>2661</v>
       </c>
       <c r="E64" t="n">
-        <v>28309900</v>
+        <v>28503440</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -3008,13 +3008,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D65" t="n">
         <v>241</v>
       </c>
       <c r="E65" t="n">
-        <v>1473800</v>
+        <v>1476900</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -3049,13 +3049,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D66" t="n">
         <v>135</v>
       </c>
       <c r="E66" t="n">
-        <v>1223686</v>
+        <v>1244783</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -3090,13 +3090,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>219905</v>
+        <v>220757</v>
       </c>
       <c r="D67" t="n">
-        <v>69054</v>
+        <v>69170</v>
       </c>
       <c r="E67" t="n">
-        <v>351192233</v>
+        <v>353211235</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -3131,13 +3131,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D68" t="n">
         <v>91</v>
       </c>
       <c r="E68" t="n">
-        <v>717874</v>
+        <v>720874</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -3172,13 +3172,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D69" t="n">
         <v>44</v>
       </c>
       <c r="E69" t="n">
-        <v>392847</v>
+        <v>402847</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -3254,13 +3254,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="D71" t="n">
         <v>288</v>
       </c>
       <c r="E71" t="n">
-        <v>3418356</v>
+        <v>3428356</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -3336,13 +3336,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>105313</v>
+        <v>105746</v>
       </c>
       <c r="D73" t="n">
-        <v>33216</v>
+        <v>33280</v>
       </c>
       <c r="E73" t="n">
-        <v>302252012</v>
+        <v>304366742</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -3377,13 +3377,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D74" t="n">
         <v>102</v>
       </c>
       <c r="E74" t="n">
-        <v>2500725</v>
+        <v>2502225</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -3418,13 +3418,13 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D75" t="n">
         <v>15</v>
       </c>
       <c r="E75" t="n">
-        <v>245241</v>
+        <v>255907</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -3459,13 +3459,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>50288</v>
+        <v>50499</v>
       </c>
       <c r="D76" t="n">
-        <v>15518</v>
+        <v>15558</v>
       </c>
       <c r="E76" t="n">
-        <v>144568628</v>
+        <v>145482380</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -3541,13 +3541,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D78" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E78" t="n">
-        <v>635648</v>
+        <v>645648</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -3582,13 +3582,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>9503</v>
+        <v>9680</v>
       </c>
       <c r="D79" t="n">
-        <v>5275</v>
+        <v>5378</v>
       </c>
       <c r="E79" t="n">
-        <v>37989222</v>
+        <v>39006875</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -3623,13 +3623,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5462</v>
+        <v>5489</v>
       </c>
       <c r="D80" t="n">
-        <v>1491</v>
+        <v>1494</v>
       </c>
       <c r="E80" t="n">
-        <v>13480359</v>
+        <v>13595350</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -3664,13 +3664,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>47046</v>
+        <v>47192</v>
       </c>
       <c r="D81" t="n">
-        <v>11939</v>
+        <v>11943</v>
       </c>
       <c r="E81" t="n">
-        <v>71847263</v>
+        <v>72192915</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -3787,13 +3787,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>11295</v>
+        <v>11320</v>
       </c>
       <c r="D84" t="n">
         <v>3157</v>
       </c>
       <c r="E84" t="n">
-        <v>21342527</v>
+        <v>21400424</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -3869,13 +3869,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>10582</v>
+        <v>10598</v>
       </c>
       <c r="D86" t="n">
-        <v>2652</v>
+        <v>2654</v>
       </c>
       <c r="E86" t="n">
-        <v>18702087</v>
+        <v>18774221</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -3910,13 +3910,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="D87" t="n">
         <v>196</v>
       </c>
       <c r="E87" t="n">
-        <v>1102220</v>
+        <v>1109720</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -3951,13 +3951,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="D88" t="n">
         <v>188</v>
       </c>
       <c r="E88" t="n">
-        <v>1163093</v>
+        <v>1167593</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3992,13 +3992,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>19306</v>
+        <v>19353</v>
       </c>
       <c r="D89" t="n">
-        <v>3636</v>
+        <v>3639</v>
       </c>
       <c r="E89" t="n">
-        <v>39659369</v>
+        <v>39759790</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -4033,13 +4033,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4350</v>
+        <v>4361</v>
       </c>
       <c r="D90" t="n">
         <v>882</v>
       </c>
       <c r="E90" t="n">
-        <v>9871477</v>
+        <v>9897303</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -4115,13 +4115,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6291</v>
+        <v>6300</v>
       </c>
       <c r="D92" t="n">
         <v>1217</v>
       </c>
       <c r="E92" t="n">
-        <v>14350479</v>
+        <v>14376350</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -4238,13 +4238,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D95" t="n">
         <v>76</v>
       </c>
       <c r="E95" t="n">
-        <v>829749</v>
+        <v>834249</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -4279,13 +4279,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>217296</v>
+        <v>217932</v>
       </c>
       <c r="D96" t="n">
-        <v>66197</v>
+        <v>66246</v>
       </c>
       <c r="E96" t="n">
-        <v>330021675</v>
+        <v>331377919</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -4484,13 +4484,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2035</v>
+        <v>2052</v>
       </c>
       <c r="D101" t="n">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E101" t="n">
-        <v>7377137</v>
+        <v>7484980</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -4566,13 +4566,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>86676</v>
+        <v>87003</v>
       </c>
       <c r="D103" t="n">
-        <v>26758</v>
+        <v>26793</v>
       </c>
       <c r="E103" t="n">
-        <v>243727921</v>
+        <v>245526729</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -4607,13 +4607,13 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D104" t="n">
         <v>90</v>
       </c>
       <c r="E104" t="n">
-        <v>1800324</v>
+        <v>1810324</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -4648,13 +4648,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D105" t="n">
         <v>10</v>
       </c>
       <c r="E105" t="n">
-        <v>159190</v>
+        <v>169190</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -4689,13 +4689,13 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>46929</v>
+        <v>47083</v>
       </c>
       <c r="D106" t="n">
-        <v>13517</v>
+        <v>13533</v>
       </c>
       <c r="E106" t="n">
-        <v>129846223</v>
+        <v>130540436</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -4771,13 +4771,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2184</v>
+        <v>2198</v>
       </c>
       <c r="D108" t="n">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="E108" t="n">
-        <v>5022860</v>
+        <v>5071877</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -4812,13 +4812,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4452</v>
+        <v>4476</v>
       </c>
       <c r="D109" t="n">
-        <v>1236</v>
+        <v>1239</v>
       </c>
       <c r="E109" t="n">
-        <v>10543033</v>
+        <v>10615440</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -4894,13 +4894,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>868807</v>
+        <v>870834</v>
       </c>
       <c r="D111" t="n">
-        <v>213575</v>
+        <v>213685</v>
       </c>
       <c r="E111" t="n">
-        <v>1425199155</v>
+        <v>1430311155</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -4935,13 +4935,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D112" t="n">
         <v>42</v>
       </c>
       <c r="E112" t="n">
-        <v>321271</v>
+        <v>331937</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -4976,13 +4976,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D113" t="n">
         <v>117</v>
       </c>
       <c r="E113" t="n">
-        <v>1282075</v>
+        <v>1292075</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -5099,13 +5099,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>3593</v>
+        <v>3619</v>
       </c>
       <c r="D116" t="n">
-        <v>1126</v>
+        <v>1130</v>
       </c>
       <c r="E116" t="n">
-        <v>20081093</v>
+        <v>20301483</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -5181,13 +5181,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>361639</v>
+        <v>363023</v>
       </c>
       <c r="D118" t="n">
-        <v>99777</v>
+        <v>99908</v>
       </c>
       <c r="E118" t="n">
-        <v>1045141026</v>
+        <v>1052780794</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -5222,13 +5222,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1387</v>
+        <v>1394</v>
       </c>
       <c r="D119" t="n">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E119" t="n">
-        <v>11070378</v>
+        <v>11130759</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -5304,13 +5304,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>334269</v>
+        <v>335396</v>
       </c>
       <c r="D121" t="n">
-        <v>84052</v>
+        <v>84157</v>
       </c>
       <c r="E121" t="n">
-        <v>906401896</v>
+        <v>912007927</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -5386,13 +5386,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>4306</v>
+        <v>4317</v>
       </c>
       <c r="D123" t="n">
-        <v>1499</v>
+        <v>1501</v>
       </c>
       <c r="E123" t="n">
-        <v>7585283</v>
+        <v>7613136</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
@@ -5468,13 +5468,13 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>13619</v>
+        <v>13666</v>
       </c>
       <c r="D125" t="n">
-        <v>3619</v>
+        <v>3628</v>
       </c>
       <c r="E125" t="n">
-        <v>33545110</v>
+        <v>33728946</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -5591,13 +5591,13 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>57013</v>
+        <v>57073</v>
       </c>
       <c r="D128" t="n">
-        <v>17198</v>
+        <v>17199</v>
       </c>
       <c r="E128" t="n">
-        <v>80252010</v>
+        <v>80354591</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -5755,13 +5755,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>16987</v>
+        <v>17010</v>
       </c>
       <c r="D132" t="n">
         <v>5876</v>
       </c>
       <c r="E132" t="n">
-        <v>29771406</v>
+        <v>29882059</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -5837,13 +5837,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>4728</v>
+        <v>4733</v>
       </c>
       <c r="D134" t="n">
         <v>1516</v>
       </c>
       <c r="E134" t="n">
-        <v>7942309</v>
+        <v>7949545</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -5960,13 +5960,13 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D137" t="n">
         <v>166</v>
       </c>
       <c r="E137" t="n">
-        <v>711133</v>
+        <v>712504</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -6042,13 +6042,13 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>26141</v>
+        <v>26243</v>
       </c>
       <c r="D139" t="n">
-        <v>6973</v>
+        <v>6975</v>
       </c>
       <c r="E139" t="n">
-        <v>39787170</v>
+        <v>40013963</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -6124,13 +6124,13 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D141" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E141" t="n">
-        <v>122020</v>
+        <v>132020</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -6165,13 +6165,13 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>10913</v>
+        <v>10952</v>
       </c>
       <c r="D142" t="n">
-        <v>3107</v>
+        <v>3114</v>
       </c>
       <c r="E142" t="n">
-        <v>24163657</v>
+        <v>24356755</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -6247,13 +6247,13 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>7730</v>
+        <v>7756</v>
       </c>
       <c r="D144" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="E144" t="n">
-        <v>15601193</v>
+        <v>15716399</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -6288,13 +6288,13 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D145" t="n">
         <v>123</v>
       </c>
       <c r="E145" t="n">
-        <v>618952</v>
+        <v>620363</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -6329,13 +6329,13 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D146" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E146" t="n">
-        <v>942251</v>
+        <v>945251</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>34917</v>
+        <v>35002</v>
       </c>
       <c r="D147" t="n">
-        <v>5351</v>
+        <v>5353</v>
       </c>
       <c r="E147" t="n">
-        <v>86717999</v>
+        <v>87259622</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -6411,13 +6411,13 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3368</v>
+        <v>3372</v>
       </c>
       <c r="D148" t="n">
         <v>657</v>
       </c>
       <c r="E148" t="n">
-        <v>8207403</v>
+        <v>8236403</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -6493,13 +6493,13 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D150" t="n">
         <v>17</v>
       </c>
       <c r="E150" t="n">
-        <v>265095</v>
+        <v>275095</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -6534,13 +6534,13 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D151" t="n">
         <v>37</v>
       </c>
       <c r="E151" t="n">
-        <v>520986</v>
+        <v>523986</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -6575,13 +6575,13 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>134027</v>
+        <v>134465</v>
       </c>
       <c r="D152" t="n">
-        <v>41522</v>
+        <v>41566</v>
       </c>
       <c r="E152" t="n">
-        <v>211850518</v>
+        <v>212888506</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -6616,13 +6616,13 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D153" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E153" t="n">
-        <v>87569</v>
+        <v>88687</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -6739,13 +6739,13 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1497</v>
+        <v>1509</v>
       </c>
       <c r="D156" t="n">
         <v>459</v>
       </c>
       <c r="E156" t="n">
-        <v>6111805</v>
+        <v>6198274</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -6821,13 +6821,13 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>56915</v>
+        <v>57153</v>
       </c>
       <c r="D158" t="n">
-        <v>17659</v>
+        <v>17690</v>
       </c>
       <c r="E158" t="n">
-        <v>168437669</v>
+        <v>169758026</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -6903,13 +6903,13 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>22782</v>
+        <v>22852</v>
       </c>
       <c r="D160" t="n">
-        <v>6719</v>
+        <v>6728</v>
       </c>
       <c r="E160" t="n">
-        <v>67583142</v>
+        <v>67947264</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -6985,13 +6985,13 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1745</v>
+        <v>1752</v>
       </c>
       <c r="D162" t="n">
         <v>644</v>
       </c>
       <c r="E162" t="n">
-        <v>3283476</v>
+        <v>3302095</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -7026,13 +7026,13 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3307</v>
+        <v>3324</v>
       </c>
       <c r="D163" t="n">
-        <v>969</v>
+        <v>974</v>
       </c>
       <c r="E163" t="n">
-        <v>7846279</v>
+        <v>7890843</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -7067,13 +7067,13 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>355649</v>
+        <v>356626</v>
       </c>
       <c r="D164" t="n">
-        <v>111901</v>
+        <v>111995</v>
       </c>
       <c r="E164" t="n">
-        <v>532470811</v>
+        <v>534728812</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -7313,13 +7313,13 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1721</v>
+        <v>1726</v>
       </c>
       <c r="D170" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E170" t="n">
-        <v>6022469</v>
+        <v>6046969</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -7395,13 +7395,13 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>141048</v>
+        <v>141567</v>
       </c>
       <c r="D172" t="n">
-        <v>44497</v>
+        <v>44556</v>
       </c>
       <c r="E172" t="n">
-        <v>402528775</v>
+        <v>405239001</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
@@ -7436,13 +7436,13 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D173" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E173" t="n">
-        <v>1774829</v>
+        <v>1804829</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -7518,13 +7518,13 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>56428</v>
+        <v>56600</v>
       </c>
       <c r="D175" t="n">
-        <v>17054</v>
+        <v>17081</v>
       </c>
       <c r="E175" t="n">
-        <v>160583955</v>
+        <v>161467640</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -7641,13 +7641,13 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>7459</v>
+        <v>7487</v>
       </c>
       <c r="D178" t="n">
-        <v>3106</v>
+        <v>3112</v>
       </c>
       <c r="E178" t="n">
-        <v>15452244</v>
+        <v>15589341</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -7723,13 +7723,13 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>9370</v>
+        <v>9396</v>
       </c>
       <c r="D180" t="n">
-        <v>2575</v>
+        <v>2576</v>
       </c>
       <c r="E180" t="n">
-        <v>21028323</v>
+        <v>21138204</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -7805,13 +7805,13 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>405754</v>
+        <v>406927</v>
       </c>
       <c r="D182" t="n">
-        <v>123480</v>
+        <v>123577</v>
       </c>
       <c r="E182" t="n">
-        <v>594234809</v>
+        <v>596726163</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -7846,13 +7846,13 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D183" t="n">
         <v>70</v>
       </c>
       <c r="E183" t="n">
-        <v>353505</v>
+        <v>359125</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -8051,13 +8051,13 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="D188" t="n">
         <v>336</v>
       </c>
       <c r="E188" t="n">
-        <v>4001936</v>
+        <v>4011936</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -8133,13 +8133,13 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>157943</v>
+        <v>158486</v>
       </c>
       <c r="D190" t="n">
-        <v>47848</v>
+        <v>47899</v>
       </c>
       <c r="E190" t="n">
-        <v>445094762</v>
+        <v>447953954</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -8174,13 +8174,13 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D191" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E191" t="n">
-        <v>1976116</v>
+        <v>1995032</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -8256,13 +8256,13 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>88195</v>
+        <v>88515</v>
       </c>
       <c r="D193" t="n">
-        <v>25505</v>
+        <v>25543</v>
       </c>
       <c r="E193" t="n">
-        <v>240352966</v>
+        <v>241844450</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -8379,13 +8379,13 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>6754</v>
+        <v>6789</v>
       </c>
       <c r="D196" t="n">
-        <v>2701</v>
+        <v>2706</v>
       </c>
       <c r="E196" t="n">
-        <v>12275837</v>
+        <v>12372863</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -8502,13 +8502,13 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>11878</v>
+        <v>11926</v>
       </c>
       <c r="D199" t="n">
-        <v>3083</v>
+        <v>3091</v>
       </c>
       <c r="E199" t="n">
-        <v>26607254</v>
+        <v>26802760</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -8584,13 +8584,13 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>160003</v>
+        <v>160424</v>
       </c>
       <c r="D201" t="n">
-        <v>51091</v>
+        <v>51126</v>
       </c>
       <c r="E201" t="n">
-        <v>246363024</v>
+        <v>247345914</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -8748,13 +8748,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1347</v>
+        <v>1354</v>
       </c>
       <c r="D205" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E205" t="n">
-        <v>5607052</v>
+        <v>5643577</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -8789,13 +8789,13 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>81352</v>
+        <v>81620</v>
       </c>
       <c r="D206" t="n">
-        <v>26238</v>
+        <v>26286</v>
       </c>
       <c r="E206" t="n">
-        <v>236077599</v>
+        <v>237499170</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -8830,13 +8830,13 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D207" t="n">
         <v>40</v>
       </c>
       <c r="E207" t="n">
-        <v>981701</v>
+        <v>991701</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -8912,13 +8912,13 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>21885</v>
+        <v>21976</v>
       </c>
       <c r="D209" t="n">
-        <v>6673</v>
+        <v>6693</v>
       </c>
       <c r="E209" t="n">
-        <v>65869339</v>
+        <v>66371836</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -8994,13 +8994,13 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>2632</v>
+        <v>2649</v>
       </c>
       <c r="D211" t="n">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="E211" t="n">
-        <v>5286908</v>
+        <v>5352995</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -9076,13 +9076,13 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>4718</v>
+        <v>4740</v>
       </c>
       <c r="D213" t="n">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="E213" t="n">
-        <v>11392939</v>
+        <v>11505714</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -9117,13 +9117,13 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>408505</v>
+        <v>409802</v>
       </c>
       <c r="D214" t="n">
-        <v>117592</v>
+        <v>117693</v>
       </c>
       <c r="E214" t="n">
-        <v>618228838</v>
+        <v>620972635</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>
@@ -9158,13 +9158,13 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D215" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E215" t="n">
-        <v>467731</v>
+        <v>474938</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>
@@ -9199,13 +9199,13 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D216" t="n">
         <v>126</v>
       </c>
       <c r="E216" t="n">
-        <v>1071639</v>
+        <v>1086034</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -9363,13 +9363,13 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>1920</v>
+        <v>1934</v>
       </c>
       <c r="D220" t="n">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E220" t="n">
-        <v>8076944</v>
+        <v>8182542</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -9445,13 +9445,13 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>164712</v>
+        <v>165326</v>
       </c>
       <c r="D222" t="n">
-        <v>47804</v>
+        <v>47874</v>
       </c>
       <c r="E222" t="n">
-        <v>479925068</v>
+        <v>483133639</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
@@ -9486,13 +9486,13 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D223" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E223" t="n">
-        <v>1710209</v>
+        <v>1720209</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -9568,13 +9568,13 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>117264</v>
+        <v>117685</v>
       </c>
       <c r="D225" t="n">
-        <v>32020</v>
+        <v>32069</v>
       </c>
       <c r="E225" t="n">
-        <v>328944793</v>
+        <v>331031589</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
@@ -9691,13 +9691,13 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>3755</v>
+        <v>3766</v>
       </c>
       <c r="D228" t="n">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="E228" t="n">
-        <v>7108596</v>
+        <v>7137948</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -9732,13 +9732,13 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D229" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E229" t="n">
-        <v>155559</v>
+        <v>163831</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
@@ -9773,13 +9773,13 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D230" t="n">
         <v>4</v>
       </c>
       <c r="E230" t="n">
-        <v>39842</v>
+        <v>40846</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
@@ -9814,13 +9814,13 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>9590</v>
+        <v>9627</v>
       </c>
       <c r="D231" t="n">
-        <v>2421</v>
+        <v>2427</v>
       </c>
       <c r="E231" t="n">
-        <v>22456566</v>
+        <v>22643615</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2021-01-19 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-categorie-juridique-latest.xlsx
@@ -425,13 +425,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>505810</v>
+        <v>509465</v>
       </c>
       <c r="D2" t="n">
-        <v>150810</v>
+        <v>150951</v>
       </c>
       <c r="E2" t="n">
-        <v>786524177</v>
+        <v>795210352</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D3" t="n">
         <v>126</v>
       </c>
       <c r="E3" t="n">
-        <v>640423</v>
+        <v>666565</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D4" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E4" t="n">
-        <v>1597794</v>
+        <v>1651293</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
         <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>339092</v>
+        <v>348826</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1877</v>
+        <v>1909</v>
       </c>
       <c r="D8" t="n">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E8" t="n">
-        <v>7268424</v>
+        <v>7521773</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>323223</v>
+        <v>415439</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>200425</v>
+        <v>202445</v>
       </c>
       <c r="D10" t="n">
-        <v>61191</v>
+        <v>61317</v>
       </c>
       <c r="E10" t="n">
-        <v>597645007</v>
+        <v>614001439</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="D11" t="n">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E11" t="n">
-        <v>3401511</v>
+        <v>3548687</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" t="n">
-        <v>170238</v>
+        <v>296778</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>105238</v>
+        <v>106032</v>
       </c>
       <c r="D13" t="n">
-        <v>30893</v>
+        <v>30953</v>
       </c>
       <c r="E13" t="n">
-        <v>311138520</v>
+        <v>317144337</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -917,13 +917,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D14" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" t="n">
-        <v>149993</v>
+        <v>181493</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5820</v>
+        <v>5864</v>
       </c>
       <c r="D15" t="n">
-        <v>2546</v>
+        <v>2553</v>
       </c>
       <c r="E15" t="n">
-        <v>10774582</v>
+        <v>10855301</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>